<commit_message>
Code updated 23-04-24 11:30:57
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:I118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,6 +426,16 @@
           <t>04-22_0</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>04-23_A</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>04-23_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -452,9 +462,15 @@
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -483,7 +499,13 @@
       <c r="F3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -514,7 +536,13 @@
       <c r="F4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -545,9 +573,15 @@
       <c r="F5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2866</t>
+      <c r="G5" t="n">
+        <v>2866</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -576,9 +610,15 @@
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2562</t>
+      <c r="G6" t="n">
+        <v>2562</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -607,9 +647,15 @@
       <c r="F7" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>2911</t>
+      <c r="G7" t="n">
+        <v>2911</v>
+      </c>
+      <c r="H7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -638,9 +684,15 @@
       <c r="F8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>2595</t>
+      <c r="G8" t="n">
+        <v>2595</v>
+      </c>
+      <c r="H8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -669,7 +721,13 @@
       <c r="F9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -700,9 +758,15 @@
       <c r="F10" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>3047</t>
+      <c r="G10" t="n">
+        <v>3047</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2610</t>
         </is>
       </c>
     </row>
@@ -731,7 +795,13 @@
       <c r="F11" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -762,7 +832,13 @@
       <c r="F12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -793,7 +869,13 @@
       <c r="F13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -824,9 +906,15 @@
       <c r="F14" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>1496</t>
+      <c r="G14" t="n">
+        <v>1496</v>
+      </c>
+      <c r="H14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>1400</t>
         </is>
       </c>
     </row>
@@ -855,9 +943,15 @@
       <c r="F15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>1454</t>
+      <c r="G15" t="n">
+        <v>1454</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -886,9 +980,15 @@
       <c r="F16" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>1742</t>
+      <c r="G16" t="n">
+        <v>1742</v>
+      </c>
+      <c r="H16" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>1783</t>
         </is>
       </c>
     </row>
@@ -917,9 +1017,15 @@
       <c r="F17" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>1624</t>
+      <c r="G17" t="n">
+        <v>1624</v>
+      </c>
+      <c r="H17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -948,9 +1054,15 @@
       <c r="F18" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>4091</t>
+      <c r="G18" t="n">
+        <v>4091</v>
+      </c>
+      <c r="H18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2510</t>
         </is>
       </c>
     </row>
@@ -979,9 +1091,15 @@
       <c r="F19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>2854</t>
+      <c r="G19" t="n">
+        <v>2854</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1010,9 +1128,15 @@
       <c r="F20" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>4724</t>
+      <c r="G20" t="n">
+        <v>4724</v>
+      </c>
+      <c r="H20" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>2723</t>
         </is>
       </c>
     </row>
@@ -1041,9 +1165,15 @@
       <c r="F21" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>5413</t>
+      <c r="G21" t="n">
+        <v>5413</v>
+      </c>
+      <c r="H21" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>3034</t>
         </is>
       </c>
     </row>
@@ -1072,9 +1202,15 @@
       <c r="F22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>5579</t>
+      <c r="G22" t="n">
+        <v>5579</v>
+      </c>
+      <c r="H22" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2834</t>
         </is>
       </c>
     </row>
@@ -1103,9 +1239,15 @@
       <c r="F23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>6485</t>
+      <c r="G23" t="n">
+        <v>6485</v>
+      </c>
+      <c r="H23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2921</t>
         </is>
       </c>
     </row>
@@ -1134,9 +1276,15 @@
       <c r="F24" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>5736</t>
+      <c r="G24" t="n">
+        <v>5736</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>3015</t>
         </is>
       </c>
     </row>
@@ -1165,9 +1313,15 @@
       <c r="F25" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>6147</t>
+      <c r="G25" t="n">
+        <v>6147</v>
+      </c>
+      <c r="H25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>2910</t>
         </is>
       </c>
     </row>
@@ -1196,9 +1350,15 @@
       <c r="F26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>4193</t>
+      <c r="G26" t="n">
+        <v>4193</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1227,9 +1387,15 @@
       <c r="F27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -1258,11 +1424,11 @@
       <c r="F28" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="4" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1289,9 +1455,15 @@
       <c r="F29" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>5221</t>
+      <c r="G29" t="n">
+        <v>5221</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1320,9 +1492,15 @@
       <c r="F30" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="G30" t="inlineStr">
-        <is>
-          <t>5542</t>
+      <c r="G30" t="n">
+        <v>5542</v>
+      </c>
+      <c r="H30" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>3065</t>
         </is>
       </c>
     </row>
@@ -1351,9 +1529,15 @@
       <c r="F31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>5505</t>
+      <c r="G31" t="n">
+        <v>5505</v>
+      </c>
+      <c r="H31" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>2965</t>
         </is>
       </c>
     </row>
@@ -1382,9 +1566,15 @@
       <c r="F32" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>5015</t>
+      <c r="G32" t="n">
+        <v>5015</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -1413,9 +1603,15 @@
       <c r="F33" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>4556</t>
+      <c r="G33" t="n">
+        <v>4556</v>
+      </c>
+      <c r="H33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1444,9 +1640,15 @@
       <c r="F34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -1475,9 +1677,15 @@
       <c r="F35" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>5358</t>
+      <c r="G35" t="n">
+        <v>5358</v>
+      </c>
+      <c r="H35" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>2771</t>
         </is>
       </c>
     </row>
@@ -1506,9 +1714,15 @@
       <c r="F36" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>4673</t>
+      <c r="G36" t="n">
+        <v>4673</v>
+      </c>
+      <c r="H36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>2518</t>
         </is>
       </c>
     </row>
@@ -1537,9 +1751,15 @@
       <c r="F37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>5216</t>
+      <c r="G37" t="n">
+        <v>5216</v>
+      </c>
+      <c r="H37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>2913</t>
         </is>
       </c>
     </row>
@@ -1568,9 +1788,15 @@
       <c r="F38" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>5849</t>
+      <c r="G38" t="n">
+        <v>5849</v>
+      </c>
+      <c r="H38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -1599,9 +1825,15 @@
       <c r="F39" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>4755</t>
+      <c r="G39" t="n">
+        <v>4755</v>
+      </c>
+      <c r="H39" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>2853</t>
         </is>
       </c>
     </row>
@@ -1630,9 +1862,15 @@
       <c r="F40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>2731</t>
+      <c r="G40" t="n">
+        <v>2731</v>
+      </c>
+      <c r="H40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1661,9 +1899,15 @@
       <c r="F41" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>4700</t>
+      <c r="G41" t="n">
+        <v>4700</v>
+      </c>
+      <c r="H41" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>2892</t>
         </is>
       </c>
     </row>
@@ -1692,9 +1936,15 @@
       <c r="F42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>3600</t>
+      <c r="G42" t="n">
+        <v>3600</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1723,9 +1973,15 @@
       <c r="F43" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>5787</t>
+      <c r="G43" t="n">
+        <v>5787</v>
+      </c>
+      <c r="H43" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>2868</t>
         </is>
       </c>
     </row>
@@ -1754,9 +2010,15 @@
       <c r="F44" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>6019</t>
+      <c r="G44" t="n">
+        <v>6019</v>
+      </c>
+      <c r="H44" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>2949</t>
         </is>
       </c>
     </row>
@@ -1785,9 +2047,15 @@
       <c r="F45" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>4271</t>
+      <c r="G45" t="n">
+        <v>4271</v>
+      </c>
+      <c r="H45" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>2759</t>
         </is>
       </c>
     </row>
@@ -1816,9 +2084,15 @@
       <c r="F46" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>4050</t>
+      <c r="G46" t="n">
+        <v>4050</v>
+      </c>
+      <c r="H46" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>2689</t>
         </is>
       </c>
     </row>
@@ -1847,9 +2121,15 @@
       <c r="F47" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>6077</t>
+      <c r="G47" t="n">
+        <v>6077</v>
+      </c>
+      <c r="H47" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>2968</t>
         </is>
       </c>
     </row>
@@ -1878,9 +2158,15 @@
       <c r="F48" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>5739</t>
+      <c r="G48" t="n">
+        <v>5739</v>
+      </c>
+      <c r="H48" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>3010</t>
         </is>
       </c>
     </row>
@@ -1909,9 +2195,15 @@
       <c r="F49" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>5212</t>
+      <c r="G49" t="n">
+        <v>5212</v>
+      </c>
+      <c r="H49" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>3063</t>
         </is>
       </c>
     </row>
@@ -1940,9 +2232,15 @@
       <c r="F50" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>5545</t>
+      <c r="G50" t="n">
+        <v>5545</v>
+      </c>
+      <c r="H50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>2978</t>
         </is>
       </c>
     </row>
@@ -1971,9 +2269,15 @@
       <c r="F51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>5049</t>
+      <c r="G51" t="n">
+        <v>5049</v>
+      </c>
+      <c r="H51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2002,9 +2306,15 @@
       <c r="F52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>5526</t>
+      <c r="G52" t="n">
+        <v>5526</v>
+      </c>
+      <c r="H52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>2988</t>
         </is>
       </c>
     </row>
@@ -2033,9 +2343,15 @@
       <c r="F53" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>4145</t>
+      <c r="G53" t="n">
+        <v>4145</v>
+      </c>
+      <c r="H53" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>2719</t>
         </is>
       </c>
     </row>
@@ -2064,9 +2380,15 @@
       <c r="F54" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>5247</t>
+      <c r="G54" t="n">
+        <v>5247</v>
+      </c>
+      <c r="H54" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>2835</t>
         </is>
       </c>
     </row>
@@ -2095,9 +2417,15 @@
       <c r="F55" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>4947</t>
+      <c r="G55" t="n">
+        <v>4947</v>
+      </c>
+      <c r="H55" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>2708</t>
         </is>
       </c>
     </row>
@@ -2126,9 +2454,15 @@
       <c r="F56" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>5577</t>
+      <c r="G56" t="n">
+        <v>5577</v>
+      </c>
+      <c r="H56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>3161</t>
         </is>
       </c>
     </row>
@@ -2157,9 +2491,15 @@
       <c r="F57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>4535</t>
+      <c r="G57" t="n">
+        <v>4535</v>
+      </c>
+      <c r="H57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>2759</t>
         </is>
       </c>
     </row>
@@ -2188,9 +2528,15 @@
       <c r="F58" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>4492</t>
+      <c r="G58" t="n">
+        <v>4492</v>
+      </c>
+      <c r="H58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>2874</t>
         </is>
       </c>
     </row>
@@ -2219,9 +2565,15 @@
       <c r="F59" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>4449</t>
+      <c r="G59" t="n">
+        <v>4449</v>
+      </c>
+      <c r="H59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>2818</t>
         </is>
       </c>
     </row>
@@ -2250,9 +2602,15 @@
       <c r="F60" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>4594</t>
+      <c r="G60" t="n">
+        <v>4594</v>
+      </c>
+      <c r="H60" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>2855</t>
         </is>
       </c>
     </row>
@@ -2281,11 +2639,11 @@
       <c r="F61" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>4095</t>
-        </is>
-      </c>
+      <c r="G61" t="n">
+        <v>4095</v>
+      </c>
+      <c r="H61" s="4" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -2312,9 +2670,15 @@
       <c r="F62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>4204</t>
+      <c r="G62" t="n">
+        <v>4204</v>
+      </c>
+      <c r="H62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>2781</t>
         </is>
       </c>
     </row>
@@ -2343,9 +2707,15 @@
       <c r="F63" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>4259</t>
+      <c r="G63" t="n">
+        <v>4259</v>
+      </c>
+      <c r="H63" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>2884</t>
         </is>
       </c>
     </row>
@@ -2374,9 +2744,15 @@
       <c r="F64" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>4594</t>
+      <c r="G64" t="n">
+        <v>4594</v>
+      </c>
+      <c r="H64" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>2914</t>
         </is>
       </c>
     </row>
@@ -2405,9 +2781,15 @@
       <c r="F65" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>4007</t>
+      <c r="G65" t="n">
+        <v>4007</v>
+      </c>
+      <c r="H65" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>2621</t>
         </is>
       </c>
     </row>
@@ -2436,7 +2818,13 @@
       <c r="F66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G66" t="inlineStr">
+      <c r="G66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2467,9 +2855,15 @@
       <c r="F67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>2993</t>
+      <c r="G67" t="n">
+        <v>2993</v>
+      </c>
+      <c r="H67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2498,9 +2892,15 @@
       <c r="F68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>2502</t>
+      <c r="G68" t="n">
+        <v>2502</v>
+      </c>
+      <c r="H68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2529,9 +2929,15 @@
       <c r="F69" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>4437</t>
+      <c r="G69" t="n">
+        <v>4437</v>
+      </c>
+      <c r="H69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -2560,7 +2966,13 @@
       <c r="F70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G70" t="inlineStr">
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2591,7 +3003,13 @@
       <c r="F71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G71" t="inlineStr">
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2622,7 +3040,13 @@
       <c r="F72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G72" t="inlineStr">
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2653,9 +3077,15 @@
       <c r="F73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>2964</t>
+      <c r="G73" t="n">
+        <v>2964</v>
+      </c>
+      <c r="H73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2684,9 +3114,15 @@
       <c r="F74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>2752</t>
+      <c r="G74" t="n">
+        <v>2752</v>
+      </c>
+      <c r="H74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2715,7 +3151,13 @@
       <c r="F75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G75" t="inlineStr">
+      <c r="G75" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2746,9 +3188,15 @@
       <c r="F76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>4652</t>
+      <c r="G76" t="n">
+        <v>4652</v>
+      </c>
+      <c r="H76" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>2637</t>
         </is>
       </c>
     </row>
@@ -2777,9 +3225,15 @@
       <c r="F77" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>3621</t>
+      <c r="G77" t="n">
+        <v>3621</v>
+      </c>
+      <c r="H77" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>2669</t>
         </is>
       </c>
     </row>
@@ -2808,7 +3262,13 @@
       <c r="F78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G78" t="inlineStr">
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2839,9 +3299,15 @@
       <c r="F79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>1225</t>
+      <c r="G79" t="n">
+        <v>1225</v>
+      </c>
+      <c r="H79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2870,7 +3336,13 @@
       <c r="F80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G80" t="inlineStr">
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2901,9 +3373,15 @@
       <c r="F81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>3126</t>
+      <c r="G81" t="n">
+        <v>3126</v>
+      </c>
+      <c r="H81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2932,7 +3410,13 @@
       <c r="F82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G82" t="inlineStr">
+      <c r="G82" t="n">
+        <v>0</v>
+      </c>
+      <c r="H82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2963,7 +3447,13 @@
       <c r="F83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G83" t="inlineStr">
+      <c r="G83" t="n">
+        <v>0</v>
+      </c>
+      <c r="H83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2994,9 +3484,15 @@
       <c r="F84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>1525</t>
+      <c r="G84" t="n">
+        <v>1525</v>
+      </c>
+      <c r="H84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3025,7 +3521,13 @@
       <c r="F85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G85" t="inlineStr">
+      <c r="G85" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3056,7 +3558,13 @@
       <c r="F86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G86" t="inlineStr">
+      <c r="G86" t="n">
+        <v>0</v>
+      </c>
+      <c r="H86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3087,7 +3595,13 @@
       <c r="F87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G87" t="inlineStr">
+      <c r="G87" t="n">
+        <v>0</v>
+      </c>
+      <c r="H87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3118,7 +3632,13 @@
       <c r="F88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G88" t="inlineStr">
+      <c r="G88" t="n">
+        <v>0</v>
+      </c>
+      <c r="H88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3149,7 +3669,13 @@
       <c r="F89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G89" t="inlineStr">
+      <c r="G89" t="n">
+        <v>0</v>
+      </c>
+      <c r="H89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3180,7 +3706,13 @@
       <c r="F90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G90" t="inlineStr">
+      <c r="G90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3211,7 +3743,13 @@
       <c r="F91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G91" t="inlineStr">
+      <c r="G91" t="n">
+        <v>0</v>
+      </c>
+      <c r="H91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3242,7 +3780,13 @@
       <c r="F92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G92" t="inlineStr">
+      <c r="G92" t="n">
+        <v>0</v>
+      </c>
+      <c r="H92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3273,7 +3817,13 @@
       <c r="F93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G93" t="inlineStr">
+      <c r="G93" t="n">
+        <v>0</v>
+      </c>
+      <c r="H93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3304,7 +3854,13 @@
       <c r="F94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G94" t="inlineStr">
+      <c r="G94" t="n">
+        <v>0</v>
+      </c>
+      <c r="H94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3335,7 +3891,13 @@
       <c r="F95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G95" t="inlineStr">
+      <c r="G95" t="n">
+        <v>0</v>
+      </c>
+      <c r="H95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3366,9 +3928,15 @@
       <c r="F96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>3713</t>
+      <c r="G96" t="n">
+        <v>3713</v>
+      </c>
+      <c r="H96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>2494</t>
         </is>
       </c>
     </row>
@@ -3397,7 +3965,13 @@
       <c r="F97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G97" t="inlineStr">
+      <c r="G97" t="n">
+        <v>0</v>
+      </c>
+      <c r="H97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3428,7 +4002,13 @@
       <c r="F98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G98" t="inlineStr">
+      <c r="G98" t="n">
+        <v>0</v>
+      </c>
+      <c r="H98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3459,7 +4039,13 @@
       <c r="F99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G99" t="inlineStr">
+      <c r="G99" t="n">
+        <v>0</v>
+      </c>
+      <c r="H99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3490,7 +4076,13 @@
       <c r="F100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G100" t="inlineStr">
+      <c r="G100" t="n">
+        <v>0</v>
+      </c>
+      <c r="H100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3521,7 +4113,13 @@
       <c r="F101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G101" t="inlineStr">
+      <c r="G101" t="n">
+        <v>0</v>
+      </c>
+      <c r="H101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3552,7 +4150,13 @@
       <c r="F102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G102" t="inlineStr">
+      <c r="G102" t="n">
+        <v>0</v>
+      </c>
+      <c r="H102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3583,7 +4187,13 @@
       <c r="F103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G103" t="inlineStr">
+      <c r="G103" t="n">
+        <v>0</v>
+      </c>
+      <c r="H103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3614,7 +4224,13 @@
       <c r="F104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G104" t="inlineStr">
+      <c r="G104" t="n">
+        <v>0</v>
+      </c>
+      <c r="H104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3645,7 +4261,13 @@
       <c r="F105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G105" t="inlineStr">
+      <c r="G105" t="n">
+        <v>0</v>
+      </c>
+      <c r="H105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3671,6 +4293,8 @@
       <c r="E106" t="inlineStr"/>
       <c r="F106" s="4" t="inlineStr"/>
       <c r="G106" t="inlineStr"/>
+      <c r="H106" s="4" t="inlineStr"/>
+      <c r="I106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -3692,6 +4316,8 @@
       <c r="E107" t="inlineStr"/>
       <c r="F107" s="4" t="inlineStr"/>
       <c r="G107" t="inlineStr"/>
+      <c r="H107" s="4" t="inlineStr"/>
+      <c r="I107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -3713,6 +4339,8 @@
       <c r="E108" t="inlineStr"/>
       <c r="F108" s="4" t="inlineStr"/>
       <c r="G108" t="inlineStr"/>
+      <c r="H108" s="4" t="inlineStr"/>
+      <c r="I108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -3734,6 +4362,8 @@
       <c r="E109" t="inlineStr"/>
       <c r="F109" s="4" t="inlineStr"/>
       <c r="G109" t="inlineStr"/>
+      <c r="H109" s="4" t="inlineStr"/>
+      <c r="I109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -3755,6 +4385,8 @@
       <c r="E110" t="inlineStr"/>
       <c r="F110" s="4" t="inlineStr"/>
       <c r="G110" t="inlineStr"/>
+      <c r="H110" s="4" t="inlineStr"/>
+      <c r="I110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -3776,6 +4408,8 @@
       <c r="E111" t="inlineStr"/>
       <c r="F111" s="4" t="inlineStr"/>
       <c r="G111" t="inlineStr"/>
+      <c r="H111" s="4" t="inlineStr"/>
+      <c r="I111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -3797,6 +4431,8 @@
       <c r="E112" t="inlineStr"/>
       <c r="F112" s="4" t="inlineStr"/>
       <c r="G112" t="inlineStr"/>
+      <c r="H112" s="4" t="inlineStr"/>
+      <c r="I112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -3818,6 +4454,8 @@
       <c r="E113" t="inlineStr"/>
       <c r="F113" s="4" t="inlineStr"/>
       <c r="G113" t="inlineStr"/>
+      <c r="H113" s="4" t="inlineStr"/>
+      <c r="I113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -3839,6 +4477,124 @@
       <c r="E114" t="inlineStr"/>
       <c r="F114" s="4" t="inlineStr"/>
       <c r="G114" t="inlineStr"/>
+      <c r="H114" s="4" t="inlineStr"/>
+      <c r="I114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>20199374</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>RuanFan</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr"/>
+      <c r="D115" t="inlineStr"/>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F115" s="4" t="inlineStr"/>
+      <c r="G115" t="inlineStr"/>
+      <c r="H115" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>3159</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>26280580</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>AOW全体工作人员吃屎交易大厅</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr"/>
+      <c r="D116" t="inlineStr"/>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F116" s="4" t="inlineStr"/>
+      <c r="G116" t="inlineStr"/>
+      <c r="H116" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>3019</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>26588375</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>何苦僧ᶻᵍˣ</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr"/>
+      <c r="D117" t="inlineStr"/>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F117" s="4" t="inlineStr"/>
+      <c r="G117" t="inlineStr"/>
+      <c r="H117" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>2807</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>35114520</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>13lur¹³</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr"/>
+      <c r="D118" t="inlineStr"/>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F118" s="4" t="inlineStr"/>
+      <c r="G118" t="inlineStr"/>
+      <c r="H118" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>2911</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Code updated 23-04-26 11:30:56
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I118"/>
+  <dimension ref="A1:K118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,16 @@
           <t>04-23_0</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>04-25_A</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>04-25_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -468,9 +478,15 @@
       <c r="H2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="I2" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -505,7 +521,13 @@
       <c r="H3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -542,7 +564,13 @@
       <c r="H4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -579,9 +607,15 @@
       <c r="H5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -616,9 +650,15 @@
       <c r="H6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>2495</t>
         </is>
       </c>
     </row>
@@ -653,11 +693,11 @@
       <c r="H7" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="4" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -690,11 +730,11 @@
       <c r="H8" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="4" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -727,11 +767,11 @@
       <c r="H9" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="4" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -764,11 +804,11 @@
       <c r="H10" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>2610</t>
-        </is>
-      </c>
+      <c r="I10" t="n">
+        <v>2610</v>
+      </c>
+      <c r="J10" s="4" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -801,11 +841,11 @@
       <c r="H11" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="4" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -838,11 +878,11 @@
       <c r="H12" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="4" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -875,11 +915,11 @@
       <c r="H13" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="4" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -912,11 +952,11 @@
       <c r="H14" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>1400</t>
-        </is>
-      </c>
+      <c r="I14" t="n">
+        <v>1400</v>
+      </c>
+      <c r="J14" s="4" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -949,11 +989,11 @@
       <c r="H15" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -986,11 +1026,11 @@
       <c r="H16" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>1783</t>
-        </is>
-      </c>
+      <c r="I16" t="n">
+        <v>1783</v>
+      </c>
+      <c r="J16" s="4" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1023,11 +1063,11 @@
       <c r="H17" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="I17" t="n">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1060,9 +1100,15 @@
       <c r="H18" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>2510</t>
+      <c r="I18" t="n">
+        <v>2510</v>
+      </c>
+      <c r="J18" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>2799</t>
         </is>
       </c>
     </row>
@@ -1097,7 +1143,13 @@
       <c r="H19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1134,9 +1186,15 @@
       <c r="H20" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>2723</t>
+      <c r="I20" t="n">
+        <v>2723</v>
+      </c>
+      <c r="J20" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>3241</t>
         </is>
       </c>
     </row>
@@ -1171,9 +1229,15 @@
       <c r="H21" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>3034</t>
+      <c r="I21" t="n">
+        <v>3034</v>
+      </c>
+      <c r="J21" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>3824</t>
         </is>
       </c>
     </row>
@@ -1208,9 +1272,15 @@
       <c r="H22" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>2834</t>
+      <c r="I22" t="n">
+        <v>2834</v>
+      </c>
+      <c r="J22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>3461</t>
         </is>
       </c>
     </row>
@@ -1245,9 +1315,15 @@
       <c r="H23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>2921</t>
+      <c r="I23" t="n">
+        <v>2921</v>
+      </c>
+      <c r="J23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>3682</t>
         </is>
       </c>
     </row>
@@ -1282,9 +1358,15 @@
       <c r="H24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>3015</t>
+      <c r="I24" t="n">
+        <v>3015</v>
+      </c>
+      <c r="J24" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>3702</t>
         </is>
       </c>
     </row>
@@ -1319,9 +1401,15 @@
       <c r="H25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>2910</t>
+      <c r="I25" t="n">
+        <v>2910</v>
+      </c>
+      <c r="J25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>3799</t>
         </is>
       </c>
     </row>
@@ -1356,9 +1444,15 @@
       <c r="H26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>2560</t>
         </is>
       </c>
     </row>
@@ -1393,7 +1487,13 @@
       <c r="H27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I27" t="inlineStr">
+      <c r="I27" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1429,6 +1529,8 @@
       </c>
       <c r="H28" s="4" t="inlineStr"/>
       <c r="I28" t="inlineStr"/>
+      <c r="J28" s="4" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1461,9 +1563,15 @@
       <c r="H29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>2516</t>
         </is>
       </c>
     </row>
@@ -1498,9 +1606,15 @@
       <c r="H30" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>3065</t>
+      <c r="I30" t="n">
+        <v>3065</v>
+      </c>
+      <c r="J30" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>3782</t>
         </is>
       </c>
     </row>
@@ -1535,9 +1649,15 @@
       <c r="H31" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>2965</t>
+      <c r="I31" t="n">
+        <v>2965</v>
+      </c>
+      <c r="J31" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>3816</t>
         </is>
       </c>
     </row>
@@ -1572,9 +1692,15 @@
       <c r="H32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="I32" t="n">
+        <v>2498</v>
+      </c>
+      <c r="J32" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>2554</t>
         </is>
       </c>
     </row>
@@ -1609,7 +1735,13 @@
       <c r="H33" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I33" t="inlineStr">
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1646,7 +1778,13 @@
       <c r="H34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I34" t="inlineStr">
+      <c r="I34" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1683,9 +1821,15 @@
       <c r="H35" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>2771</t>
+      <c r="I35" t="n">
+        <v>2771</v>
+      </c>
+      <c r="J35" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>3471</t>
         </is>
       </c>
     </row>
@@ -1720,9 +1864,15 @@
       <c r="H36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>2518</t>
+      <c r="I36" t="n">
+        <v>2518</v>
+      </c>
+      <c r="J36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>2595</t>
         </is>
       </c>
     </row>
@@ -1757,9 +1907,15 @@
       <c r="H37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>2913</t>
+      <c r="I37" t="n">
+        <v>2913</v>
+      </c>
+      <c r="J37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>3592</t>
         </is>
       </c>
     </row>
@@ -1794,9 +1950,15 @@
       <c r="H38" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="I38" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J38" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>3410</t>
         </is>
       </c>
     </row>
@@ -1831,9 +1993,15 @@
       <c r="H39" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>2853</t>
+      <c r="I39" t="n">
+        <v>2853</v>
+      </c>
+      <c r="J39" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>3452</t>
         </is>
       </c>
     </row>
@@ -1868,7 +2036,13 @@
       <c r="H40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I40" t="inlineStr">
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1905,9 +2079,15 @@
       <c r="H41" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>2892</t>
+      <c r="I41" t="n">
+        <v>2892</v>
+      </c>
+      <c r="J41" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>3422</t>
         </is>
       </c>
     </row>
@@ -1942,9 +2122,15 @@
       <c r="H42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I42" t="n">
+        <v>0</v>
+      </c>
+      <c r="J42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>2625</t>
         </is>
       </c>
     </row>
@@ -1979,11 +2165,11 @@
       <c r="H43" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>2868</t>
-        </is>
-      </c>
+      <c r="I43" t="n">
+        <v>2868</v>
+      </c>
+      <c r="J43" s="4" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2016,9 +2202,15 @@
       <c r="H44" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>2949</t>
+      <c r="I44" t="n">
+        <v>2949</v>
+      </c>
+      <c r="J44" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>3946</t>
         </is>
       </c>
     </row>
@@ -2053,9 +2245,15 @@
       <c r="H45" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>2759</t>
+      <c r="I45" t="n">
+        <v>2759</v>
+      </c>
+      <c r="J45" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>3061</t>
         </is>
       </c>
     </row>
@@ -2090,9 +2288,15 @@
       <c r="H46" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>2689</t>
+      <c r="I46" t="n">
+        <v>2689</v>
+      </c>
+      <c r="J46" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>2988</t>
         </is>
       </c>
     </row>
@@ -2127,9 +2331,15 @@
       <c r="H47" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>2968</t>
+      <c r="I47" t="n">
+        <v>2968</v>
+      </c>
+      <c r="J47" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>3996</t>
         </is>
       </c>
     </row>
@@ -2164,9 +2374,15 @@
       <c r="H48" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>3010</t>
+      <c r="I48" t="n">
+        <v>3010</v>
+      </c>
+      <c r="J48" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>3991</t>
         </is>
       </c>
     </row>
@@ -2201,9 +2417,15 @@
       <c r="H49" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>3063</t>
+      <c r="I49" t="n">
+        <v>3063</v>
+      </c>
+      <c r="J49" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>3732</t>
         </is>
       </c>
     </row>
@@ -2238,9 +2460,15 @@
       <c r="H50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>2978</t>
+      <c r="I50" t="n">
+        <v>2978</v>
+      </c>
+      <c r="J50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>3822</t>
         </is>
       </c>
     </row>
@@ -2275,9 +2503,15 @@
       <c r="H51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>2965</t>
         </is>
       </c>
     </row>
@@ -2312,9 +2546,15 @@
       <c r="H52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>2988</t>
+      <c r="I52" t="n">
+        <v>2988</v>
+      </c>
+      <c r="J52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>3897</t>
         </is>
       </c>
     </row>
@@ -2349,9 +2589,15 @@
       <c r="H53" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>2719</t>
+      <c r="I53" t="n">
+        <v>2719</v>
+      </c>
+      <c r="J53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>2934</t>
         </is>
       </c>
     </row>
@@ -2386,9 +2632,15 @@
       <c r="H54" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>2835</t>
+      <c r="I54" t="n">
+        <v>2835</v>
+      </c>
+      <c r="J54" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>3428</t>
         </is>
       </c>
     </row>
@@ -2423,9 +2675,15 @@
       <c r="H55" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>2708</t>
+      <c r="I55" t="n">
+        <v>2708</v>
+      </c>
+      <c r="J55" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>3002</t>
         </is>
       </c>
     </row>
@@ -2460,9 +2718,15 @@
       <c r="H56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>3161</t>
+      <c r="I56" t="n">
+        <v>3161</v>
+      </c>
+      <c r="J56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>3992</t>
         </is>
       </c>
     </row>
@@ -2497,9 +2761,15 @@
       <c r="H57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>2759</t>
+      <c r="I57" t="n">
+        <v>2759</v>
+      </c>
+      <c r="J57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>3263</t>
         </is>
       </c>
     </row>
@@ -2534,9 +2804,15 @@
       <c r="H58" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>2874</t>
+      <c r="I58" t="n">
+        <v>2874</v>
+      </c>
+      <c r="J58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>3248</t>
         </is>
       </c>
     </row>
@@ -2571,9 +2847,15 @@
       <c r="H59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>2818</t>
+      <c r="I59" t="n">
+        <v>2818</v>
+      </c>
+      <c r="J59" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>3197</t>
         </is>
       </c>
     </row>
@@ -2608,9 +2890,15 @@
       <c r="H60" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>2855</t>
+      <c r="I60" t="n">
+        <v>2855</v>
+      </c>
+      <c r="J60" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>3458</t>
         </is>
       </c>
     </row>
@@ -2644,6 +2932,8 @@
       </c>
       <c r="H61" s="4" t="inlineStr"/>
       <c r="I61" t="inlineStr"/>
+      <c r="J61" s="4" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -2676,9 +2966,15 @@
       <c r="H62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>2781</t>
+      <c r="I62" t="n">
+        <v>2781</v>
+      </c>
+      <c r="J62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>3122</t>
         </is>
       </c>
     </row>
@@ -2713,9 +3009,15 @@
       <c r="H63" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>2884</t>
+      <c r="I63" t="n">
+        <v>2884</v>
+      </c>
+      <c r="J63" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>3194</t>
         </is>
       </c>
     </row>
@@ -2750,9 +3052,15 @@
       <c r="H64" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>2914</t>
+      <c r="I64" t="n">
+        <v>2914</v>
+      </c>
+      <c r="J64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>3407</t>
         </is>
       </c>
     </row>
@@ -2787,9 +3095,15 @@
       <c r="H65" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>2621</t>
+      <c r="I65" t="n">
+        <v>2621</v>
+      </c>
+      <c r="J65" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>2919</t>
         </is>
       </c>
     </row>
@@ -2824,7 +3138,13 @@
       <c r="H66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I66" t="inlineStr">
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2861,7 +3181,13 @@
       <c r="H67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I67" t="inlineStr">
+      <c r="I67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2898,7 +3224,13 @@
       <c r="H68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I68" t="inlineStr">
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2935,7 +3267,13 @@
       <c r="H69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I69" t="inlineStr">
+      <c r="I69" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K69" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2972,7 +3310,13 @@
       <c r="H70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I70" t="inlineStr">
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3009,7 +3353,13 @@
       <c r="H71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I71" t="inlineStr">
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
+      <c r="J71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3046,7 +3396,13 @@
       <c r="H72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I72" t="inlineStr">
+      <c r="I72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3083,9 +3439,15 @@
       <c r="H73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I73" t="n">
+        <v>0</v>
+      </c>
+      <c r="J73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>2567</t>
         </is>
       </c>
     </row>
@@ -3120,7 +3482,13 @@
       <c r="H74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I74" t="inlineStr">
+      <c r="I74" t="n">
+        <v>0</v>
+      </c>
+      <c r="J74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3157,7 +3525,13 @@
       <c r="H75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I75" t="inlineStr">
+      <c r="I75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3194,9 +3568,15 @@
       <c r="H76" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t>2637</t>
+      <c r="I76" t="n">
+        <v>2637</v>
+      </c>
+      <c r="J76" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>3129</t>
         </is>
       </c>
     </row>
@@ -3231,9 +3611,15 @@
       <c r="H77" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>2669</t>
+      <c r="I77" t="n">
+        <v>2669</v>
+      </c>
+      <c r="J77" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>3133</t>
         </is>
       </c>
     </row>
@@ -3268,9 +3654,15 @@
       <c r="H78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I78" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>2497</t>
         </is>
       </c>
     </row>
@@ -3305,7 +3697,13 @@
       <c r="H79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I79" t="inlineStr">
+      <c r="I79" t="n">
+        <v>0</v>
+      </c>
+      <c r="J79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3342,7 +3740,13 @@
       <c r="H80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I80" t="inlineStr">
+      <c r="I80" t="n">
+        <v>0</v>
+      </c>
+      <c r="J80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3379,9 +3783,15 @@
       <c r="H81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I81" t="n">
+        <v>0</v>
+      </c>
+      <c r="J81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -3416,7 +3826,13 @@
       <c r="H82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I82" t="inlineStr">
+      <c r="I82" t="n">
+        <v>0</v>
+      </c>
+      <c r="J82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3453,7 +3869,13 @@
       <c r="H83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I83" t="inlineStr">
+      <c r="I83" t="n">
+        <v>0</v>
+      </c>
+      <c r="J83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3490,9 +3912,15 @@
       <c r="H84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I84" t="n">
+        <v>0</v>
+      </c>
+      <c r="J84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>1527</t>
         </is>
       </c>
     </row>
@@ -3527,7 +3955,13 @@
       <c r="H85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I85" t="inlineStr">
+      <c r="I85" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3564,7 +3998,13 @@
       <c r="H86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I86" t="inlineStr">
+      <c r="I86" t="n">
+        <v>0</v>
+      </c>
+      <c r="J86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3601,7 +4041,13 @@
       <c r="H87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I87" t="inlineStr">
+      <c r="I87" t="n">
+        <v>0</v>
+      </c>
+      <c r="J87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3638,7 +4084,13 @@
       <c r="H88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I88" t="inlineStr">
+      <c r="I88" t="n">
+        <v>0</v>
+      </c>
+      <c r="J88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3675,7 +4127,13 @@
       <c r="H89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I89" t="inlineStr">
+      <c r="I89" t="n">
+        <v>0</v>
+      </c>
+      <c r="J89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3712,7 +4170,13 @@
       <c r="H90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I90" t="inlineStr">
+      <c r="I90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3749,7 +4213,13 @@
       <c r="H91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I91" t="inlineStr">
+      <c r="I91" t="n">
+        <v>0</v>
+      </c>
+      <c r="J91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3786,7 +4256,13 @@
       <c r="H92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I92" t="inlineStr">
+      <c r="I92" t="n">
+        <v>0</v>
+      </c>
+      <c r="J92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3823,7 +4299,13 @@
       <c r="H93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I93" t="inlineStr">
+      <c r="I93" t="n">
+        <v>0</v>
+      </c>
+      <c r="J93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3860,7 +4342,13 @@
       <c r="H94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I94" t="inlineStr">
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
+      <c r="J94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3897,7 +4385,13 @@
       <c r="H95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I95" t="inlineStr">
+      <c r="I95" t="n">
+        <v>0</v>
+      </c>
+      <c r="J95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3934,9 +4428,15 @@
       <c r="H96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>2494</t>
+      <c r="I96" t="n">
+        <v>2494</v>
+      </c>
+      <c r="J96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>2834</t>
         </is>
       </c>
     </row>
@@ -3971,7 +4471,13 @@
       <c r="H97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I97" t="inlineStr">
+      <c r="I97" t="n">
+        <v>0</v>
+      </c>
+      <c r="J97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4008,7 +4514,13 @@
       <c r="H98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I98" t="inlineStr">
+      <c r="I98" t="n">
+        <v>0</v>
+      </c>
+      <c r="J98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4045,7 +4557,13 @@
       <c r="H99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I99" t="inlineStr">
+      <c r="I99" t="n">
+        <v>0</v>
+      </c>
+      <c r="J99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4082,7 +4600,13 @@
       <c r="H100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I100" t="inlineStr">
+      <c r="I100" t="n">
+        <v>0</v>
+      </c>
+      <c r="J100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4119,7 +4643,13 @@
       <c r="H101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I101" t="inlineStr">
+      <c r="I101" t="n">
+        <v>0</v>
+      </c>
+      <c r="J101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4156,7 +4686,13 @@
       <c r="H102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I102" t="inlineStr">
+      <c r="I102" t="n">
+        <v>0</v>
+      </c>
+      <c r="J102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4193,7 +4729,13 @@
       <c r="H103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I103" t="inlineStr">
+      <c r="I103" t="n">
+        <v>0</v>
+      </c>
+      <c r="J103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4230,7 +4772,13 @@
       <c r="H104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I104" t="inlineStr">
+      <c r="I104" t="n">
+        <v>0</v>
+      </c>
+      <c r="J104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4267,7 +4815,13 @@
       <c r="H105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I105" t="inlineStr">
+      <c r="I105" t="n">
+        <v>0</v>
+      </c>
+      <c r="J105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4295,6 +4849,8 @@
       <c r="G106" t="inlineStr"/>
       <c r="H106" s="4" t="inlineStr"/>
       <c r="I106" t="inlineStr"/>
+      <c r="J106" s="4" t="inlineStr"/>
+      <c r="K106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -4318,6 +4874,8 @@
       <c r="G107" t="inlineStr"/>
       <c r="H107" s="4" t="inlineStr"/>
       <c r="I107" t="inlineStr"/>
+      <c r="J107" s="4" t="inlineStr"/>
+      <c r="K107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -4341,6 +4899,8 @@
       <c r="G108" t="inlineStr"/>
       <c r="H108" s="4" t="inlineStr"/>
       <c r="I108" t="inlineStr"/>
+      <c r="J108" s="4" t="inlineStr"/>
+      <c r="K108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -4364,6 +4924,8 @@
       <c r="G109" t="inlineStr"/>
       <c r="H109" s="4" t="inlineStr"/>
       <c r="I109" t="inlineStr"/>
+      <c r="J109" s="4" t="inlineStr"/>
+      <c r="K109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -4387,6 +4949,8 @@
       <c r="G110" t="inlineStr"/>
       <c r="H110" s="4" t="inlineStr"/>
       <c r="I110" t="inlineStr"/>
+      <c r="J110" s="4" t="inlineStr"/>
+      <c r="K110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -4410,6 +4974,8 @@
       <c r="G111" t="inlineStr"/>
       <c r="H111" s="4" t="inlineStr"/>
       <c r="I111" t="inlineStr"/>
+      <c r="J111" s="4" t="inlineStr"/>
+      <c r="K111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -4433,6 +4999,8 @@
       <c r="G112" t="inlineStr"/>
       <c r="H112" s="4" t="inlineStr"/>
       <c r="I112" t="inlineStr"/>
+      <c r="J112" s="4" t="inlineStr"/>
+      <c r="K112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -4456,6 +5024,8 @@
       <c r="G113" t="inlineStr"/>
       <c r="H113" s="4" t="inlineStr"/>
       <c r="I113" t="inlineStr"/>
+      <c r="J113" s="4" t="inlineStr"/>
+      <c r="K113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -4479,12 +5049,12 @@
       <c r="G114" t="inlineStr"/>
       <c r="H114" s="4" t="inlineStr"/>
       <c r="I114" t="inlineStr"/>
+      <c r="J114" s="4" t="inlineStr"/>
+      <c r="K114" t="inlineStr"/>
     </row>
     <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>20199374</t>
-        </is>
+      <c r="A115" t="n">
+        <v>20199374</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -4503,21 +5073,25 @@
       <c r="H115" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>3159</t>
+      <c r="I115" t="n">
+        <v>3159</v>
+      </c>
+      <c r="J115" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>4227</t>
         </is>
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>26280580</t>
-        </is>
+      <c r="A116" t="n">
+        <v>26280580</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>AOW全体工作人员吃屎交易大厅</t>
+          <t>꧁SSS.TIGRESS꧂ᶻᵍˣ</t>
         </is>
       </c>
       <c r="C116" t="inlineStr"/>
@@ -4532,17 +5106,21 @@
       <c r="H116" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>3019</t>
+      <c r="I116" t="n">
+        <v>3019</v>
+      </c>
+      <c r="J116" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>3789</t>
         </is>
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>26588375</t>
-        </is>
+      <c r="A117" t="n">
+        <v>26588375</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
@@ -4561,17 +5139,21 @@
       <c r="H117" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="I117" t="inlineStr">
-        <is>
-          <t>2807</t>
+      <c r="I117" t="n">
+        <v>2807</v>
+      </c>
+      <c r="J117" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>3494</t>
         </is>
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>35114520</t>
-        </is>
+      <c r="A118" t="n">
+        <v>35114520</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -4590,9 +5172,15 @@
       <c r="H118" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="I118" t="inlineStr">
-        <is>
-          <t>2911</t>
+      <c r="I118" t="n">
+        <v>2911</v>
+      </c>
+      <c r="J118" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>3654</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-27 11:30:55
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K118"/>
+  <dimension ref="A1:M118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,16 @@
           <t>04-25_0</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>04-26_A</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>04-26_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -484,9 +494,15 @@
       <c r="J2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="K2" t="n">
+        <v>2499</v>
+      </c>
+      <c r="L2" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>3067</t>
         </is>
       </c>
     </row>
@@ -527,7 +543,13 @@
       <c r="J3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -570,7 +592,13 @@
       <c r="J4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -613,9 +641,15 @@
       <c r="J5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="K5" t="n">
+        <v>2499</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>2515</t>
         </is>
       </c>
     </row>
@@ -656,9 +690,15 @@
       <c r="J6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>2495</t>
+      <c r="K6" t="n">
+        <v>2495</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>2534</t>
         </is>
       </c>
     </row>
@@ -698,6 +738,8 @@
       </c>
       <c r="J7" s="4" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
+      <c r="L7" s="4" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -735,6 +777,8 @@
       </c>
       <c r="J8" s="4" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
+      <c r="L8" s="4" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -772,6 +816,8 @@
       </c>
       <c r="J9" s="4" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
+      <c r="L9" s="4" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -809,6 +855,8 @@
       </c>
       <c r="J10" s="4" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
+      <c r="L10" s="4" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -846,6 +894,8 @@
       </c>
       <c r="J11" s="4" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
+      <c r="L11" s="4" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -883,6 +933,8 @@
       </c>
       <c r="J12" s="4" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
+      <c r="L12" s="4" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -920,6 +972,8 @@
       </c>
       <c r="J13" s="4" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
+      <c r="L13" s="4" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -957,6 +1011,8 @@
       </c>
       <c r="J14" s="4" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
+      <c r="L14" s="4" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -994,6 +1050,8 @@
       </c>
       <c r="J15" s="4" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
+      <c r="L15" s="4" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1031,6 +1089,8 @@
       </c>
       <c r="J16" s="4" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
+      <c r="L16" s="4" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1068,6 +1128,8 @@
       </c>
       <c r="J17" s="4" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
+      <c r="L17" s="4" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1106,9 +1168,15 @@
       <c r="J18" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>2799</t>
+      <c r="K18" t="n">
+        <v>2799</v>
+      </c>
+      <c r="L18" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>2893</t>
         </is>
       </c>
     </row>
@@ -1149,9 +1217,15 @@
       <c r="J19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>2516</t>
         </is>
       </c>
     </row>
@@ -1192,9 +1266,15 @@
       <c r="J20" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>3241</t>
+      <c r="K20" t="n">
+        <v>3241</v>
+      </c>
+      <c r="L20" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>3252</t>
         </is>
       </c>
     </row>
@@ -1235,9 +1315,15 @@
       <c r="J21" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>3824</t>
+      <c r="K21" t="n">
+        <v>3824</v>
+      </c>
+      <c r="L21" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>3989</t>
         </is>
       </c>
     </row>
@@ -1278,9 +1364,15 @@
       <c r="J22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>3461</t>
+      <c r="K22" t="n">
+        <v>3461</v>
+      </c>
+      <c r="L22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>3767</t>
         </is>
       </c>
     </row>
@@ -1321,9 +1413,15 @@
       <c r="J23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>3682</t>
+      <c r="K23" t="n">
+        <v>3682</v>
+      </c>
+      <c r="L23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>4053</t>
         </is>
       </c>
     </row>
@@ -1364,9 +1462,15 @@
       <c r="J24" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>3702</t>
+      <c r="K24" t="n">
+        <v>3702</v>
+      </c>
+      <c r="L24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>3989</t>
         </is>
       </c>
     </row>
@@ -1407,9 +1511,15 @@
       <c r="J25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>3799</t>
+      <c r="K25" t="n">
+        <v>3799</v>
+      </c>
+      <c r="L25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>4195</t>
         </is>
       </c>
     </row>
@@ -1450,7 +1560,13 @@
       <c r="J26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K26" t="inlineStr">
+      <c r="K26" t="n">
+        <v>2560</v>
+      </c>
+      <c r="L26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="inlineStr">
         <is>
           <t>2560</t>
         </is>
@@ -1493,7 +1609,13 @@
       <c r="J27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K27" t="inlineStr">
+      <c r="K27" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1531,6 +1653,8 @@
       <c r="I28" t="inlineStr"/>
       <c r="J28" s="4" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
+      <c r="L28" s="4" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1569,7 +1693,13 @@
       <c r="J29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K29" t="inlineStr">
+      <c r="K29" t="n">
+        <v>2516</v>
+      </c>
+      <c r="L29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M29" t="inlineStr">
         <is>
           <t>2516</t>
         </is>
@@ -1612,9 +1742,15 @@
       <c r="J30" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="K30" t="inlineStr">
-        <is>
-          <t>3782</t>
+      <c r="K30" t="n">
+        <v>3782</v>
+      </c>
+      <c r="L30" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>3996</t>
         </is>
       </c>
     </row>
@@ -1655,9 +1791,15 @@
       <c r="J31" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>3816</t>
+      <c r="K31" t="n">
+        <v>3816</v>
+      </c>
+      <c r="L31" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>3989</t>
         </is>
       </c>
     </row>
@@ -1698,9 +1840,15 @@
       <c r="J32" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>2554</t>
+      <c r="K32" t="n">
+        <v>2554</v>
+      </c>
+      <c r="L32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>2581</t>
         </is>
       </c>
     </row>
@@ -1741,7 +1889,13 @@
       <c r="J33" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K33" t="inlineStr">
+      <c r="K33" t="n">
+        <v>0</v>
+      </c>
+      <c r="L33" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M33" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1784,7 +1938,13 @@
       <c r="J34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K34" t="inlineStr">
+      <c r="K34" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1827,9 +1987,15 @@
       <c r="J35" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>3471</t>
+      <c r="K35" t="n">
+        <v>3471</v>
+      </c>
+      <c r="L35" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>3830</t>
         </is>
       </c>
     </row>
@@ -1870,9 +2036,15 @@
       <c r="J36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>2595</t>
+      <c r="K36" t="n">
+        <v>2595</v>
+      </c>
+      <c r="L36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>2633</t>
         </is>
       </c>
     </row>
@@ -1913,9 +2085,15 @@
       <c r="J37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>3592</t>
+      <c r="K37" t="n">
+        <v>3592</v>
+      </c>
+      <c r="L37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>3930</t>
         </is>
       </c>
     </row>
@@ -1956,9 +2134,15 @@
       <c r="J38" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>3410</t>
+      <c r="K38" t="n">
+        <v>3410</v>
+      </c>
+      <c r="L38" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>3829</t>
         </is>
       </c>
     </row>
@@ -1999,9 +2183,15 @@
       <c r="J39" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>3452</t>
+      <c r="K39" t="n">
+        <v>3452</v>
+      </c>
+      <c r="L39" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>3755</t>
         </is>
       </c>
     </row>
@@ -2042,7 +2232,13 @@
       <c r="J40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K40" t="inlineStr">
+      <c r="K40" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2085,9 +2281,15 @@
       <c r="J41" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>3422</t>
+      <c r="K41" t="n">
+        <v>3422</v>
+      </c>
+      <c r="L41" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>3609</t>
         </is>
       </c>
     </row>
@@ -2128,9 +2330,15 @@
       <c r="J42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>2625</t>
+      <c r="K42" t="n">
+        <v>2625</v>
+      </c>
+      <c r="L42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>2651</t>
         </is>
       </c>
     </row>
@@ -2170,6 +2378,8 @@
       </c>
       <c r="J43" s="4" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
+      <c r="L43" s="4" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2208,9 +2418,15 @@
       <c r="J44" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="K44" t="inlineStr">
-        <is>
-          <t>3946</t>
+      <c r="K44" t="n">
+        <v>3946</v>
+      </c>
+      <c r="L44" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>4083</t>
         </is>
       </c>
     </row>
@@ -2251,9 +2467,15 @@
       <c r="J45" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>3061</t>
+      <c r="K45" t="n">
+        <v>3061</v>
+      </c>
+      <c r="L45" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>3388</t>
         </is>
       </c>
     </row>
@@ -2294,9 +2516,15 @@
       <c r="J46" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>2988</t>
+      <c r="K46" t="n">
+        <v>2988</v>
+      </c>
+      <c r="L46" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>3103</t>
         </is>
       </c>
     </row>
@@ -2337,9 +2565,15 @@
       <c r="J47" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>3996</t>
+      <c r="K47" t="n">
+        <v>3996</v>
+      </c>
+      <c r="L47" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>4157</t>
         </is>
       </c>
     </row>
@@ -2380,9 +2614,15 @@
       <c r="J48" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>3991</t>
+      <c r="K48" t="n">
+        <v>3991</v>
+      </c>
+      <c r="L48" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>4007</t>
         </is>
       </c>
     </row>
@@ -2423,9 +2663,15 @@
       <c r="J49" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>3732</t>
+      <c r="K49" t="n">
+        <v>3732</v>
+      </c>
+      <c r="L49" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>3856</t>
         </is>
       </c>
     </row>
@@ -2466,9 +2712,15 @@
       <c r="J50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>3822</t>
+      <c r="K50" t="n">
+        <v>3822</v>
+      </c>
+      <c r="L50" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -2509,9 +2761,15 @@
       <c r="J51" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>2965</t>
+      <c r="K51" t="n">
+        <v>2965</v>
+      </c>
+      <c r="L51" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>3255</t>
         </is>
       </c>
     </row>
@@ -2552,9 +2810,15 @@
       <c r="J52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>3897</t>
+      <c r="K52" t="n">
+        <v>3897</v>
+      </c>
+      <c r="L52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>3990</t>
         </is>
       </c>
     </row>
@@ -2595,9 +2859,15 @@
       <c r="J53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>2934</t>
+      <c r="K53" t="n">
+        <v>2934</v>
+      </c>
+      <c r="L53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>3031</t>
         </is>
       </c>
     </row>
@@ -2638,9 +2908,15 @@
       <c r="J54" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>3428</t>
+      <c r="K54" t="n">
+        <v>3428</v>
+      </c>
+      <c r="L54" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>3771</t>
         </is>
       </c>
     </row>
@@ -2681,9 +2957,15 @@
       <c r="J55" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>3002</t>
+      <c r="K55" t="n">
+        <v>3002</v>
+      </c>
+      <c r="L55" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>3283</t>
         </is>
       </c>
     </row>
@@ -2724,9 +3006,15 @@
       <c r="J56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>3992</t>
+      <c r="K56" t="n">
+        <v>3992</v>
+      </c>
+      <c r="L56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>4172</t>
         </is>
       </c>
     </row>
@@ -2767,9 +3055,15 @@
       <c r="J57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>3263</t>
+      <c r="K57" t="n">
+        <v>3263</v>
+      </c>
+      <c r="L57" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>3528</t>
         </is>
       </c>
     </row>
@@ -2810,9 +3104,15 @@
       <c r="J58" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>3248</t>
+      <c r="K58" t="n">
+        <v>3248</v>
+      </c>
+      <c r="L58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>3549</t>
         </is>
       </c>
     </row>
@@ -2853,9 +3153,15 @@
       <c r="J59" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>3197</t>
+      <c r="K59" t="n">
+        <v>3197</v>
+      </c>
+      <c r="L59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>3470</t>
         </is>
       </c>
     </row>
@@ -2896,9 +3202,15 @@
       <c r="J60" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>3458</t>
+      <c r="K60" t="n">
+        <v>3458</v>
+      </c>
+      <c r="L60" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>3711</t>
         </is>
       </c>
     </row>
@@ -2934,6 +3246,8 @@
       <c r="I61" t="inlineStr"/>
       <c r="J61" s="4" t="inlineStr"/>
       <c r="K61" t="inlineStr"/>
+      <c r="L61" s="4" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -2972,9 +3286,15 @@
       <c r="J62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>3122</t>
+      <c r="K62" t="n">
+        <v>3122</v>
+      </c>
+      <c r="L62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>3268</t>
         </is>
       </c>
     </row>
@@ -3015,9 +3335,15 @@
       <c r="J63" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>3194</t>
+      <c r="K63" t="n">
+        <v>3194</v>
+      </c>
+      <c r="L63" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>3469</t>
         </is>
       </c>
     </row>
@@ -3058,9 +3384,15 @@
       <c r="J64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>3407</t>
+      <c r="K64" t="n">
+        <v>3407</v>
+      </c>
+      <c r="L64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>3599</t>
         </is>
       </c>
     </row>
@@ -3101,9 +3433,15 @@
       <c r="J65" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>2919</t>
+      <c r="K65" t="n">
+        <v>2919</v>
+      </c>
+      <c r="L65" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>3074</t>
         </is>
       </c>
     </row>
@@ -3144,7 +3482,13 @@
       <c r="J66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K66" t="inlineStr">
+      <c r="K66" t="n">
+        <v>0</v>
+      </c>
+      <c r="L66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3187,7 +3531,13 @@
       <c r="J67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K67" t="inlineStr">
+      <c r="K67" t="n">
+        <v>0</v>
+      </c>
+      <c r="L67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3230,9 +3580,15 @@
       <c r="J68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K68" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K68" t="n">
+        <v>0</v>
+      </c>
+      <c r="L68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -3273,7 +3629,13 @@
       <c r="J69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K69" t="inlineStr">
+      <c r="K69" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M69" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3316,7 +3678,13 @@
       <c r="J70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K70" t="inlineStr">
+      <c r="K70" t="n">
+        <v>0</v>
+      </c>
+      <c r="L70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3359,7 +3727,13 @@
       <c r="J71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K71" t="inlineStr">
+      <c r="K71" t="n">
+        <v>0</v>
+      </c>
+      <c r="L71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3402,7 +3776,13 @@
       <c r="J72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K72" t="inlineStr">
+      <c r="K72" t="n">
+        <v>0</v>
+      </c>
+      <c r="L72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3445,9 +3825,15 @@
       <c r="J73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K73" t="inlineStr">
-        <is>
-          <t>2567</t>
+      <c r="K73" t="n">
+        <v>2567</v>
+      </c>
+      <c r="L73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>2606</t>
         </is>
       </c>
     </row>
@@ -3488,7 +3874,13 @@
       <c r="J74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K74" t="inlineStr">
+      <c r="K74" t="n">
+        <v>0</v>
+      </c>
+      <c r="L74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3531,7 +3923,13 @@
       <c r="J75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K75" t="inlineStr">
+      <c r="K75" t="n">
+        <v>0</v>
+      </c>
+      <c r="L75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3574,9 +3972,15 @@
       <c r="J76" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="K76" t="inlineStr">
-        <is>
-          <t>3129</t>
+      <c r="K76" t="n">
+        <v>3129</v>
+      </c>
+      <c r="L76" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>3306</t>
         </is>
       </c>
     </row>
@@ -3617,9 +4021,15 @@
       <c r="J77" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="K77" t="inlineStr">
-        <is>
-          <t>3133</t>
+      <c r="K77" t="n">
+        <v>3133</v>
+      </c>
+      <c r="L77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>3140</t>
         </is>
       </c>
     </row>
@@ -3660,9 +4070,15 @@
       <c r="J78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K78" t="inlineStr">
-        <is>
-          <t>2497</t>
+      <c r="K78" t="n">
+        <v>2497</v>
+      </c>
+      <c r="L78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>2537</t>
         </is>
       </c>
     </row>
@@ -3703,9 +4119,15 @@
       <c r="J79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K79" t="n">
+        <v>0</v>
+      </c>
+      <c r="L79" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>1284</t>
         </is>
       </c>
     </row>
@@ -3746,7 +4168,13 @@
       <c r="J80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K80" t="inlineStr">
+      <c r="K80" t="n">
+        <v>0</v>
+      </c>
+      <c r="L80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3789,9 +4217,15 @@
       <c r="J81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="K81" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L81" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>2571</t>
         </is>
       </c>
     </row>
@@ -3832,7 +4266,13 @@
       <c r="J82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K82" t="inlineStr">
+      <c r="K82" t="n">
+        <v>0</v>
+      </c>
+      <c r="L82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3875,7 +4315,13 @@
       <c r="J83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K83" t="inlineStr">
+      <c r="K83" t="n">
+        <v>0</v>
+      </c>
+      <c r="L83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3918,9 +4364,15 @@
       <c r="J84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>1527</t>
+      <c r="K84" t="n">
+        <v>1527</v>
+      </c>
+      <c r="L84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>1523</t>
         </is>
       </c>
     </row>
@@ -3961,7 +4413,13 @@
       <c r="J85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K85" t="inlineStr">
+      <c r="K85" t="n">
+        <v>0</v>
+      </c>
+      <c r="L85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4004,7 +4462,13 @@
       <c r="J86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K86" t="inlineStr">
+      <c r="K86" t="n">
+        <v>0</v>
+      </c>
+      <c r="L86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4047,7 +4511,13 @@
       <c r="J87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K87" t="inlineStr">
+      <c r="K87" t="n">
+        <v>0</v>
+      </c>
+      <c r="L87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4090,7 +4560,13 @@
       <c r="J88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K88" t="inlineStr">
+      <c r="K88" t="n">
+        <v>0</v>
+      </c>
+      <c r="L88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4133,7 +4609,13 @@
       <c r="J89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K89" t="inlineStr">
+      <c r="K89" t="n">
+        <v>0</v>
+      </c>
+      <c r="L89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4176,7 +4658,13 @@
       <c r="J90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K90" t="inlineStr">
+      <c r="K90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4219,7 +4707,13 @@
       <c r="J91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K91" t="inlineStr">
+      <c r="K91" t="n">
+        <v>0</v>
+      </c>
+      <c r="L91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4262,7 +4756,13 @@
       <c r="J92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K92" t="inlineStr">
+      <c r="K92" t="n">
+        <v>0</v>
+      </c>
+      <c r="L92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4305,7 +4805,13 @@
       <c r="J93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K93" t="inlineStr">
+      <c r="K93" t="n">
+        <v>0</v>
+      </c>
+      <c r="L93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4348,7 +4854,13 @@
       <c r="J94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K94" t="inlineStr">
+      <c r="K94" t="n">
+        <v>0</v>
+      </c>
+      <c r="L94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4391,7 +4903,13 @@
       <c r="J95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K95" t="inlineStr">
+      <c r="K95" t="n">
+        <v>0</v>
+      </c>
+      <c r="L95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4434,9 +4952,15 @@
       <c r="J96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>2834</t>
+      <c r="K96" t="n">
+        <v>2834</v>
+      </c>
+      <c r="L96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>2821</t>
         </is>
       </c>
     </row>
@@ -4477,7 +5001,13 @@
       <c r="J97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K97" t="inlineStr">
+      <c r="K97" t="n">
+        <v>0</v>
+      </c>
+      <c r="L97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4520,7 +5050,13 @@
       <c r="J98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K98" t="inlineStr">
+      <c r="K98" t="n">
+        <v>0</v>
+      </c>
+      <c r="L98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4563,7 +5099,13 @@
       <c r="J99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K99" t="inlineStr">
+      <c r="K99" t="n">
+        <v>0</v>
+      </c>
+      <c r="L99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4606,7 +5148,13 @@
       <c r="J100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K100" t="inlineStr">
+      <c r="K100" t="n">
+        <v>0</v>
+      </c>
+      <c r="L100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4649,7 +5197,13 @@
       <c r="J101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K101" t="inlineStr">
+      <c r="K101" t="n">
+        <v>0</v>
+      </c>
+      <c r="L101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4692,7 +5246,13 @@
       <c r="J102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K102" t="inlineStr">
+      <c r="K102" t="n">
+        <v>0</v>
+      </c>
+      <c r="L102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4735,7 +5295,13 @@
       <c r="J103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K103" t="inlineStr">
+      <c r="K103" t="n">
+        <v>0</v>
+      </c>
+      <c r="L103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4778,7 +5344,13 @@
       <c r="J104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K104" t="inlineStr">
+      <c r="K104" t="n">
+        <v>0</v>
+      </c>
+      <c r="L104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4821,7 +5393,13 @@
       <c r="J105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K105" t="inlineStr">
+      <c r="K105" t="n">
+        <v>0</v>
+      </c>
+      <c r="L105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4851,6 +5429,8 @@
       <c r="I106" t="inlineStr"/>
       <c r="J106" s="4" t="inlineStr"/>
       <c r="K106" t="inlineStr"/>
+      <c r="L106" s="4" t="inlineStr"/>
+      <c r="M106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -4876,6 +5456,8 @@
       <c r="I107" t="inlineStr"/>
       <c r="J107" s="4" t="inlineStr"/>
       <c r="K107" t="inlineStr"/>
+      <c r="L107" s="4" t="inlineStr"/>
+      <c r="M107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -4901,6 +5483,8 @@
       <c r="I108" t="inlineStr"/>
       <c r="J108" s="4" t="inlineStr"/>
       <c r="K108" t="inlineStr"/>
+      <c r="L108" s="4" t="inlineStr"/>
+      <c r="M108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -4926,6 +5510,8 @@
       <c r="I109" t="inlineStr"/>
       <c r="J109" s="4" t="inlineStr"/>
       <c r="K109" t="inlineStr"/>
+      <c r="L109" s="4" t="inlineStr"/>
+      <c r="M109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -4951,6 +5537,8 @@
       <c r="I110" t="inlineStr"/>
       <c r="J110" s="4" t="inlineStr"/>
       <c r="K110" t="inlineStr"/>
+      <c r="L110" s="4" t="inlineStr"/>
+      <c r="M110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -4976,6 +5564,8 @@
       <c r="I111" t="inlineStr"/>
       <c r="J111" s="4" t="inlineStr"/>
       <c r="K111" t="inlineStr"/>
+      <c r="L111" s="4" t="inlineStr"/>
+      <c r="M111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -5001,6 +5591,8 @@
       <c r="I112" t="inlineStr"/>
       <c r="J112" s="4" t="inlineStr"/>
       <c r="K112" t="inlineStr"/>
+      <c r="L112" s="4" t="inlineStr"/>
+      <c r="M112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -5026,6 +5618,8 @@
       <c r="I113" t="inlineStr"/>
       <c r="J113" s="4" t="inlineStr"/>
       <c r="K113" t="inlineStr"/>
+      <c r="L113" s="4" t="inlineStr"/>
+      <c r="M113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -5051,6 +5645,8 @@
       <c r="I114" t="inlineStr"/>
       <c r="J114" s="4" t="inlineStr"/>
       <c r="K114" t="inlineStr"/>
+      <c r="L114" s="4" t="inlineStr"/>
+      <c r="M114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -5079,9 +5675,15 @@
       <c r="J115" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="K115" t="inlineStr">
-        <is>
-          <t>4227</t>
+      <c r="K115" t="n">
+        <v>4227</v>
+      </c>
+      <c r="L115" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>4591</t>
         </is>
       </c>
     </row>
@@ -5112,9 +5714,15 @@
       <c r="J116" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="K116" t="inlineStr">
-        <is>
-          <t>3789</t>
+      <c r="K116" t="n">
+        <v>3789</v>
+      </c>
+      <c r="L116" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>3993</t>
         </is>
       </c>
     </row>
@@ -5145,9 +5753,15 @@
       <c r="J117" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="K117" t="inlineStr">
-        <is>
-          <t>3494</t>
+      <c r="K117" t="n">
+        <v>3494</v>
+      </c>
+      <c r="L117" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="M117" t="inlineStr">
+        <is>
+          <t>3859</t>
         </is>
       </c>
     </row>
@@ -5178,9 +5792,15 @@
       <c r="J118" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="K118" t="inlineStr">
-        <is>
-          <t>3654</t>
+      <c r="K118" t="n">
+        <v>3654</v>
+      </c>
+      <c r="L118" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="M118" t="inlineStr">
+        <is>
+          <t>4026</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-28 11:31:02
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M118"/>
+  <dimension ref="A1:O119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,16 @@
           <t>04-26_0</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>04-27_A</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>04-27_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -500,7 +510,13 @@
       <c r="L2" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="M2" t="n">
+        <v>3067</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="inlineStr">
         <is>
           <t>3067</t>
         </is>
@@ -549,7 +565,13 @@
       <c r="L3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -598,7 +620,13 @@
       <c r="L4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -647,9 +675,15 @@
       <c r="L5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>2515</t>
+      <c r="M5" t="n">
+        <v>2515</v>
+      </c>
+      <c r="N5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>2530</t>
         </is>
       </c>
     </row>
@@ -696,9 +730,15 @@
       <c r="L6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>2534</t>
+      <c r="M6" t="n">
+        <v>2534</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>2556</t>
         </is>
       </c>
     </row>
@@ -740,6 +780,8 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" s="4" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
+      <c r="N7" s="4" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -779,6 +821,8 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" s="4" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
+      <c r="N8" s="4" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -818,6 +862,8 @@
       <c r="K9" t="inlineStr"/>
       <c r="L9" s="4" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
+      <c r="N9" s="4" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -857,6 +903,8 @@
       <c r="K10" t="inlineStr"/>
       <c r="L10" s="4" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
+      <c r="N10" s="4" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -896,6 +944,8 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" s="4" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
+      <c r="N11" s="4" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -935,6 +985,8 @@
       <c r="K12" t="inlineStr"/>
       <c r="L12" s="4" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
+      <c r="N12" s="4" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -974,6 +1026,8 @@
       <c r="K13" t="inlineStr"/>
       <c r="L13" s="4" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
+      <c r="N13" s="4" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1013,6 +1067,8 @@
       <c r="K14" t="inlineStr"/>
       <c r="L14" s="4" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
+      <c r="N14" s="4" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1052,6 +1108,8 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" s="4" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
+      <c r="N15" s="4" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1091,6 +1149,8 @@
       <c r="K16" t="inlineStr"/>
       <c r="L16" s="4" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
+      <c r="N16" s="4" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1130,6 +1190,8 @@
       <c r="K17" t="inlineStr"/>
       <c r="L17" s="4" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
+      <c r="N17" s="4" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1174,9 +1236,15 @@
       <c r="L18" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>2893</t>
+      <c r="M18" t="n">
+        <v>2893</v>
+      </c>
+      <c r="N18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>2885</t>
         </is>
       </c>
     </row>
@@ -1223,7 +1291,13 @@
       <c r="L19" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="M19" t="inlineStr">
+      <c r="M19" t="n">
+        <v>2516</v>
+      </c>
+      <c r="N19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="inlineStr">
         <is>
           <t>2516</t>
         </is>
@@ -1272,9 +1346,15 @@
       <c r="L20" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>3252</t>
+      <c r="M20" t="n">
+        <v>3252</v>
+      </c>
+      <c r="N20" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>3604</t>
         </is>
       </c>
     </row>
@@ -1321,9 +1401,15 @@
       <c r="L21" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>3989</t>
+      <c r="M21" t="n">
+        <v>3989</v>
+      </c>
+      <c r="N21" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>4078</t>
         </is>
       </c>
     </row>
@@ -1370,9 +1456,15 @@
       <c r="L22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>3767</t>
+      <c r="M22" t="n">
+        <v>3767</v>
+      </c>
+      <c r="N22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>4044</t>
         </is>
       </c>
     </row>
@@ -1419,9 +1511,15 @@
       <c r="L23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>4053</t>
+      <c r="M23" t="n">
+        <v>4053</v>
+      </c>
+      <c r="N23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>4412</t>
         </is>
       </c>
     </row>
@@ -1468,9 +1566,15 @@
       <c r="L24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>3989</t>
+      <c r="M24" t="n">
+        <v>3989</v>
+      </c>
+      <c r="N24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>4077</t>
         </is>
       </c>
     </row>
@@ -1517,9 +1621,15 @@
       <c r="L25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>4195</t>
+      <c r="M25" t="n">
+        <v>4195</v>
+      </c>
+      <c r="N25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>4431</t>
         </is>
       </c>
     </row>
@@ -1566,9 +1676,15 @@
       <c r="L26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M26" t="inlineStr">
-        <is>
-          <t>2560</t>
+      <c r="M26" t="n">
+        <v>2560</v>
+      </c>
+      <c r="N26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>2589</t>
         </is>
       </c>
     </row>
@@ -1615,7 +1731,13 @@
       <c r="L27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M27" t="inlineStr">
+      <c r="M27" t="n">
+        <v>2500</v>
+      </c>
+      <c r="N27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1655,6 +1777,8 @@
       <c r="K28" t="inlineStr"/>
       <c r="L28" s="4" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
+      <c r="N28" s="4" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1699,7 +1823,13 @@
       <c r="L29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M29" t="inlineStr">
+      <c r="M29" t="n">
+        <v>2516</v>
+      </c>
+      <c r="N29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" t="inlineStr">
         <is>
           <t>2516</t>
         </is>
@@ -1748,9 +1878,15 @@
       <c r="L30" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="M30" t="inlineStr">
-        <is>
-          <t>3996</t>
+      <c r="M30" t="n">
+        <v>3996</v>
+      </c>
+      <c r="N30" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>4258</t>
         </is>
       </c>
     </row>
@@ -1797,9 +1933,15 @@
       <c r="L31" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>3989</t>
+      <c r="M31" t="n">
+        <v>3989</v>
+      </c>
+      <c r="N31" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>4180</t>
         </is>
       </c>
     </row>
@@ -1846,9 +1988,15 @@
       <c r="L32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>2581</t>
+      <c r="M32" t="n">
+        <v>2581</v>
+      </c>
+      <c r="N32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>2609</t>
         </is>
       </c>
     </row>
@@ -1895,11 +2043,11 @@
       <c r="L33" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M33" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="M33" t="n">
+        <v>0</v>
+      </c>
+      <c r="N33" s="4" t="inlineStr"/>
+      <c r="O33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1944,7 +2092,13 @@
       <c r="L34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M34" t="inlineStr">
+      <c r="M34" t="n">
+        <v>2500</v>
+      </c>
+      <c r="N34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1993,9 +2147,15 @@
       <c r="L35" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="M35" t="inlineStr">
-        <is>
-          <t>3830</t>
+      <c r="M35" t="n">
+        <v>3830</v>
+      </c>
+      <c r="N35" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>4073</t>
         </is>
       </c>
     </row>
@@ -2042,7 +2202,13 @@
       <c r="L36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M36" t="inlineStr">
+      <c r="M36" t="n">
+        <v>2633</v>
+      </c>
+      <c r="N36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O36" t="inlineStr">
         <is>
           <t>2633</t>
         </is>
@@ -2091,9 +2257,15 @@
       <c r="L37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>3930</t>
+      <c r="M37" t="n">
+        <v>3930</v>
+      </c>
+      <c r="N37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>3988</t>
         </is>
       </c>
     </row>
@@ -2140,9 +2312,15 @@
       <c r="L38" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>3829</t>
+      <c r="M38" t="n">
+        <v>3829</v>
+      </c>
+      <c r="N38" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>4209</t>
         </is>
       </c>
     </row>
@@ -2189,9 +2367,15 @@
       <c r="L39" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>3755</t>
+      <c r="M39" t="n">
+        <v>3755</v>
+      </c>
+      <c r="N39" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>3989</t>
         </is>
       </c>
     </row>
@@ -2238,7 +2422,13 @@
       <c r="L40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M40" t="inlineStr">
+      <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2287,9 +2477,15 @@
       <c r="L41" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>3609</t>
+      <c r="M41" t="n">
+        <v>3609</v>
+      </c>
+      <c r="N41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>3785</t>
         </is>
       </c>
     </row>
@@ -2336,9 +2532,15 @@
       <c r="L42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>2651</t>
+      <c r="M42" t="n">
+        <v>2651</v>
+      </c>
+      <c r="N42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>2710</t>
         </is>
       </c>
     </row>
@@ -2380,6 +2582,8 @@
       <c r="K43" t="inlineStr"/>
       <c r="L43" s="4" t="inlineStr"/>
       <c r="M43" t="inlineStr"/>
+      <c r="N43" s="4" t="inlineStr"/>
+      <c r="O43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2424,9 +2628,15 @@
       <c r="L44" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="M44" t="inlineStr">
-        <is>
-          <t>4083</t>
+      <c r="M44" t="n">
+        <v>4083</v>
+      </c>
+      <c r="N44" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>4332</t>
         </is>
       </c>
     </row>
@@ -2473,9 +2683,15 @@
       <c r="L45" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>3388</t>
+      <c r="M45" t="n">
+        <v>3388</v>
+      </c>
+      <c r="N45" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>3586</t>
         </is>
       </c>
     </row>
@@ -2522,9 +2738,15 @@
       <c r="L46" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>3103</t>
+      <c r="M46" t="n">
+        <v>3103</v>
+      </c>
+      <c r="N46" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>3310</t>
         </is>
       </c>
     </row>
@@ -2571,9 +2793,15 @@
       <c r="L47" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>4157</t>
+      <c r="M47" t="n">
+        <v>4157</v>
+      </c>
+      <c r="N47" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>4383</t>
         </is>
       </c>
     </row>
@@ -2620,9 +2848,15 @@
       <c r="L48" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>4007</t>
+      <c r="M48" t="n">
+        <v>4007</v>
+      </c>
+      <c r="N48" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>4290</t>
         </is>
       </c>
     </row>
@@ -2669,9 +2903,15 @@
       <c r="L49" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>3856</t>
+      <c r="M49" t="n">
+        <v>3856</v>
+      </c>
+      <c r="N49" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>3996</t>
         </is>
       </c>
     </row>
@@ -2718,9 +2958,15 @@
       <c r="L50" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>3995</t>
+      <c r="M50" t="n">
+        <v>3995</v>
+      </c>
+      <c r="N50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>4118</t>
         </is>
       </c>
     </row>
@@ -2767,9 +3013,15 @@
       <c r="L51" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>3255</t>
+      <c r="M51" t="n">
+        <v>3255</v>
+      </c>
+      <c r="N51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>3280</t>
         </is>
       </c>
     </row>
@@ -2816,9 +3068,15 @@
       <c r="L52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>3990</t>
+      <c r="M52" t="n">
+        <v>3990</v>
+      </c>
+      <c r="N52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>4183</t>
         </is>
       </c>
     </row>
@@ -2865,9 +3123,15 @@
       <c r="L53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>3031</t>
+      <c r="M53" t="n">
+        <v>3031</v>
+      </c>
+      <c r="N53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>3106</t>
         </is>
       </c>
     </row>
@@ -2914,9 +3178,15 @@
       <c r="L54" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>3771</t>
+      <c r="M54" t="n">
+        <v>3771</v>
+      </c>
+      <c r="N54" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>3987</t>
         </is>
       </c>
     </row>
@@ -2963,9 +3233,15 @@
       <c r="L55" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>3283</t>
+      <c r="M55" t="n">
+        <v>3283</v>
+      </c>
+      <c r="N55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>3307</t>
         </is>
       </c>
     </row>
@@ -3012,9 +3288,15 @@
       <c r="L56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>4172</t>
+      <c r="M56" t="n">
+        <v>4172</v>
+      </c>
+      <c r="N56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>4367</t>
         </is>
       </c>
     </row>
@@ -3061,9 +3343,15 @@
       <c r="L57" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>3528</t>
+      <c r="M57" t="n">
+        <v>3528</v>
+      </c>
+      <c r="N57" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>3756</t>
         </is>
       </c>
     </row>
@@ -3110,9 +3398,15 @@
       <c r="L58" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="M58" t="inlineStr">
-        <is>
-          <t>3549</t>
+      <c r="M58" t="n">
+        <v>3549</v>
+      </c>
+      <c r="N58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>3760</t>
         </is>
       </c>
     </row>
@@ -3159,9 +3453,15 @@
       <c r="L59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="M59" t="inlineStr">
-        <is>
-          <t>3470</t>
+      <c r="M59" t="n">
+        <v>3470</v>
+      </c>
+      <c r="N59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>3673</t>
         </is>
       </c>
     </row>
@@ -3208,9 +3508,15 @@
       <c r="L60" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="M60" t="inlineStr">
-        <is>
-          <t>3711</t>
+      <c r="M60" t="n">
+        <v>3711</v>
+      </c>
+      <c r="N60" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>3988</t>
         </is>
       </c>
     </row>
@@ -3248,6 +3554,8 @@
       <c r="K61" t="inlineStr"/>
       <c r="L61" s="4" t="inlineStr"/>
       <c r="M61" t="inlineStr"/>
+      <c r="N61" s="4" t="inlineStr"/>
+      <c r="O61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -3292,9 +3600,15 @@
       <c r="L62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="M62" t="inlineStr">
-        <is>
-          <t>3268</t>
+      <c r="M62" t="n">
+        <v>3268</v>
+      </c>
+      <c r="N62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>3435</t>
         </is>
       </c>
     </row>
@@ -3341,9 +3655,15 @@
       <c r="L63" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="M63" t="inlineStr">
-        <is>
-          <t>3469</t>
+      <c r="M63" t="n">
+        <v>3469</v>
+      </c>
+      <c r="N63" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>3656</t>
         </is>
       </c>
     </row>
@@ -3390,9 +3710,15 @@
       <c r="L64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="M64" t="inlineStr">
-        <is>
-          <t>3599</t>
+      <c r="M64" t="n">
+        <v>3599</v>
+      </c>
+      <c r="N64" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>3960</t>
         </is>
       </c>
     </row>
@@ -3439,9 +3765,15 @@
       <c r="L65" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="M65" t="inlineStr">
-        <is>
-          <t>3074</t>
+      <c r="M65" t="n">
+        <v>3074</v>
+      </c>
+      <c r="N65" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>3264</t>
         </is>
       </c>
     </row>
@@ -3488,7 +3820,13 @@
       <c r="L66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M66" t="inlineStr">
+      <c r="M66" t="n">
+        <v>0</v>
+      </c>
+      <c r="N66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3537,7 +3875,13 @@
       <c r="L67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M67" t="inlineStr">
+      <c r="M67" t="n">
+        <v>0</v>
+      </c>
+      <c r="N67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3586,9 +3930,15 @@
       <c r="L68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M68" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="M68" t="n">
+        <v>2499</v>
+      </c>
+      <c r="N68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -3635,7 +3985,13 @@
       <c r="L69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M69" t="inlineStr">
+      <c r="M69" t="n">
+        <v>2500</v>
+      </c>
+      <c r="N69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O69" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3684,7 +4040,13 @@
       <c r="L70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M70" t="inlineStr">
+      <c r="M70" t="n">
+        <v>0</v>
+      </c>
+      <c r="N70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3733,7 +4095,13 @@
       <c r="L71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M71" t="inlineStr">
+      <c r="M71" t="n">
+        <v>0</v>
+      </c>
+      <c r="N71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3782,7 +4150,13 @@
       <c r="L72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M72" t="inlineStr">
+      <c r="M72" t="n">
+        <v>0</v>
+      </c>
+      <c r="N72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3831,9 +4205,15 @@
       <c r="L73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M73" t="inlineStr">
-        <is>
-          <t>2606</t>
+      <c r="M73" t="n">
+        <v>2606</v>
+      </c>
+      <c r="N73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>2601</t>
         </is>
       </c>
     </row>
@@ -3880,7 +4260,13 @@
       <c r="L74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M74" t="inlineStr">
+      <c r="M74" t="n">
+        <v>0</v>
+      </c>
+      <c r="N74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3929,7 +4315,13 @@
       <c r="L75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M75" t="inlineStr">
+      <c r="M75" t="n">
+        <v>0</v>
+      </c>
+      <c r="N75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3978,9 +4370,15 @@
       <c r="L76" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="M76" t="inlineStr">
-        <is>
-          <t>3306</t>
+      <c r="M76" t="n">
+        <v>3306</v>
+      </c>
+      <c r="N76" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>3706</t>
         </is>
       </c>
     </row>
@@ -4027,9 +4425,15 @@
       <c r="L77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M77" t="inlineStr">
-        <is>
-          <t>3140</t>
+      <c r="M77" t="n">
+        <v>3140</v>
+      </c>
+      <c r="N77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>3130</t>
         </is>
       </c>
     </row>
@@ -4076,9 +4480,15 @@
       <c r="L78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M78" t="inlineStr">
-        <is>
-          <t>2537</t>
+      <c r="M78" t="n">
+        <v>2537</v>
+      </c>
+      <c r="N78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>2551</t>
         </is>
       </c>
     </row>
@@ -4125,9 +4535,15 @@
       <c r="L79" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="M79" t="inlineStr">
-        <is>
-          <t>1284</t>
+      <c r="M79" t="n">
+        <v>1284</v>
+      </c>
+      <c r="N79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4174,7 +4590,13 @@
       <c r="L80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M80" t="inlineStr">
+      <c r="M80" t="n">
+        <v>0</v>
+      </c>
+      <c r="N80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4223,9 +4645,15 @@
       <c r="L81" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="M81" t="inlineStr">
-        <is>
-          <t>2571</t>
+      <c r="M81" t="n">
+        <v>2571</v>
+      </c>
+      <c r="N81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>2568</t>
         </is>
       </c>
     </row>
@@ -4272,7 +4700,13 @@
       <c r="L82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M82" t="inlineStr">
+      <c r="M82" t="n">
+        <v>0</v>
+      </c>
+      <c r="N82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4321,7 +4755,13 @@
       <c r="L83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M83" t="inlineStr">
+      <c r="M83" t="n">
+        <v>0</v>
+      </c>
+      <c r="N83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4370,9 +4810,15 @@
       <c r="L84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M84" t="inlineStr">
-        <is>
-          <t>1523</t>
+      <c r="M84" t="n">
+        <v>1523</v>
+      </c>
+      <c r="N84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>1518</t>
         </is>
       </c>
     </row>
@@ -4419,7 +4865,13 @@
       <c r="L85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M85" t="inlineStr">
+      <c r="M85" t="n">
+        <v>0</v>
+      </c>
+      <c r="N85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4468,7 +4920,13 @@
       <c r="L86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M86" t="inlineStr">
+      <c r="M86" t="n">
+        <v>0</v>
+      </c>
+      <c r="N86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4517,7 +4975,13 @@
       <c r="L87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M87" t="inlineStr">
+      <c r="M87" t="n">
+        <v>0</v>
+      </c>
+      <c r="N87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4566,7 +5030,13 @@
       <c r="L88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M88" t="inlineStr">
+      <c r="M88" t="n">
+        <v>0</v>
+      </c>
+      <c r="N88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4615,7 +5085,13 @@
       <c r="L89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M89" t="inlineStr">
+      <c r="M89" t="n">
+        <v>0</v>
+      </c>
+      <c r="N89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4664,7 +5140,13 @@
       <c r="L90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M90" t="inlineStr">
+      <c r="M90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4713,7 +5195,13 @@
       <c r="L91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M91" t="inlineStr">
+      <c r="M91" t="n">
+        <v>0</v>
+      </c>
+      <c r="N91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4762,7 +5250,13 @@
       <c r="L92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M92" t="inlineStr">
+      <c r="M92" t="n">
+        <v>0</v>
+      </c>
+      <c r="N92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4811,7 +5305,13 @@
       <c r="L93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M93" t="inlineStr">
+      <c r="M93" t="n">
+        <v>0</v>
+      </c>
+      <c r="N93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4860,7 +5360,13 @@
       <c r="L94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M94" t="inlineStr">
+      <c r="M94" t="n">
+        <v>0</v>
+      </c>
+      <c r="N94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4909,7 +5415,13 @@
       <c r="L95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M95" t="inlineStr">
+      <c r="M95" t="n">
+        <v>0</v>
+      </c>
+      <c r="N95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4958,9 +5470,15 @@
       <c r="L96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M96" t="inlineStr">
-        <is>
-          <t>2821</t>
+      <c r="M96" t="n">
+        <v>2821</v>
+      </c>
+      <c r="N96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>2803</t>
         </is>
       </c>
     </row>
@@ -5007,7 +5525,13 @@
       <c r="L97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M97" t="inlineStr">
+      <c r="M97" t="n">
+        <v>0</v>
+      </c>
+      <c r="N97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5056,7 +5580,13 @@
       <c r="L98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M98" t="inlineStr">
+      <c r="M98" t="n">
+        <v>0</v>
+      </c>
+      <c r="N98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5105,7 +5635,13 @@
       <c r="L99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M99" t="inlineStr">
+      <c r="M99" t="n">
+        <v>0</v>
+      </c>
+      <c r="N99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5154,7 +5690,13 @@
       <c r="L100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M100" t="inlineStr">
+      <c r="M100" t="n">
+        <v>0</v>
+      </c>
+      <c r="N100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5203,7 +5745,13 @@
       <c r="L101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M101" t="inlineStr">
+      <c r="M101" t="n">
+        <v>0</v>
+      </c>
+      <c r="N101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5252,7 +5800,13 @@
       <c r="L102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M102" t="inlineStr">
+      <c r="M102" t="n">
+        <v>0</v>
+      </c>
+      <c r="N102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5301,7 +5855,13 @@
       <c r="L103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M103" t="inlineStr">
+      <c r="M103" t="n">
+        <v>0</v>
+      </c>
+      <c r="N103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5350,7 +5910,13 @@
       <c r="L104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M104" t="inlineStr">
+      <c r="M104" t="n">
+        <v>0</v>
+      </c>
+      <c r="N104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5399,7 +5965,13 @@
       <c r="L105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M105" t="inlineStr">
+      <c r="M105" t="n">
+        <v>0</v>
+      </c>
+      <c r="N105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5431,6 +6003,8 @@
       <c r="K106" t="inlineStr"/>
       <c r="L106" s="4" t="inlineStr"/>
       <c r="M106" t="inlineStr"/>
+      <c r="N106" s="4" t="inlineStr"/>
+      <c r="O106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -5458,6 +6032,8 @@
       <c r="K107" t="inlineStr"/>
       <c r="L107" s="4" t="inlineStr"/>
       <c r="M107" t="inlineStr"/>
+      <c r="N107" s="4" t="inlineStr"/>
+      <c r="O107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -5485,6 +6061,8 @@
       <c r="K108" t="inlineStr"/>
       <c r="L108" s="4" t="inlineStr"/>
       <c r="M108" t="inlineStr"/>
+      <c r="N108" s="4" t="inlineStr"/>
+      <c r="O108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -5512,6 +6090,8 @@
       <c r="K109" t="inlineStr"/>
       <c r="L109" s="4" t="inlineStr"/>
       <c r="M109" t="inlineStr"/>
+      <c r="N109" s="4" t="inlineStr"/>
+      <c r="O109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -5539,6 +6119,8 @@
       <c r="K110" t="inlineStr"/>
       <c r="L110" s="4" t="inlineStr"/>
       <c r="M110" t="inlineStr"/>
+      <c r="N110" s="4" t="inlineStr"/>
+      <c r="O110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -5566,6 +6148,8 @@
       <c r="K111" t="inlineStr"/>
       <c r="L111" s="4" t="inlineStr"/>
       <c r="M111" t="inlineStr"/>
+      <c r="N111" s="4" t="inlineStr"/>
+      <c r="O111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -5593,6 +6177,8 @@
       <c r="K112" t="inlineStr"/>
       <c r="L112" s="4" t="inlineStr"/>
       <c r="M112" t="inlineStr"/>
+      <c r="N112" s="4" t="inlineStr"/>
+      <c r="O112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -5620,6 +6206,8 @@
       <c r="K113" t="inlineStr"/>
       <c r="L113" s="4" t="inlineStr"/>
       <c r="M113" t="inlineStr"/>
+      <c r="N113" s="4" t="inlineStr"/>
+      <c r="O113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -5647,6 +6235,8 @@
       <c r="K114" t="inlineStr"/>
       <c r="L114" s="4" t="inlineStr"/>
       <c r="M114" t="inlineStr"/>
+      <c r="N114" s="4" t="inlineStr"/>
+      <c r="O114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -5681,9 +6271,15 @@
       <c r="L115" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M115" t="inlineStr">
-        <is>
-          <t>4591</t>
+      <c r="M115" t="n">
+        <v>4591</v>
+      </c>
+      <c r="N115" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O115" t="inlineStr">
+        <is>
+          <t>4997</t>
         </is>
       </c>
     </row>
@@ -5720,9 +6316,15 @@
       <c r="L116" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="M116" t="inlineStr">
-        <is>
-          <t>3993</t>
+      <c r="M116" t="n">
+        <v>3993</v>
+      </c>
+      <c r="N116" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="O116" t="inlineStr">
+        <is>
+          <t>4065</t>
         </is>
       </c>
     </row>
@@ -5759,9 +6361,15 @@
       <c r="L117" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="M117" t="inlineStr">
-        <is>
-          <t>3859</t>
+      <c r="M117" t="n">
+        <v>3859</v>
+      </c>
+      <c r="N117" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="O117" t="inlineStr">
+        <is>
+          <t>4065</t>
         </is>
       </c>
     </row>
@@ -5798,9 +6406,50 @@
       <c r="L118" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="M118" t="inlineStr">
-        <is>
-          <t>4026</t>
+      <c r="M118" t="n">
+        <v>4026</v>
+      </c>
+      <c r="N118" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>4315</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>8666978</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>FierceRocket</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr"/>
+      <c r="D119" t="inlineStr"/>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F119" s="4" t="inlineStr"/>
+      <c r="G119" t="inlineStr"/>
+      <c r="H119" s="4" t="inlineStr"/>
+      <c r="I119" t="inlineStr"/>
+      <c r="J119" s="4" t="inlineStr"/>
+      <c r="K119" t="inlineStr"/>
+      <c r="L119" s="4" t="inlineStr"/>
+      <c r="M119" t="inlineStr"/>
+      <c r="N119" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>1141</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-29 11:30:59
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O119"/>
+  <dimension ref="A1:Q119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,16 @@
           <t>04-27_0</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>04-28_A</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>04-28_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -516,7 +526,13 @@
       <c r="N2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="O2" t="n">
+        <v>3067</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="inlineStr">
         <is>
           <t>3067</t>
         </is>
@@ -571,7 +587,13 @@
       <c r="N3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -626,7 +648,13 @@
       <c r="N4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -681,9 +709,15 @@
       <c r="N5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>2530</t>
+      <c r="O5" t="n">
+        <v>2530</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>2526</t>
         </is>
       </c>
     </row>
@@ -736,9 +770,15 @@
       <c r="N6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>2556</t>
+      <c r="O6" t="n">
+        <v>2556</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>2569</t>
         </is>
       </c>
     </row>
@@ -782,6 +822,8 @@
       <c r="M7" t="inlineStr"/>
       <c r="N7" s="4" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
+      <c r="P7" s="4" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -823,6 +865,8 @@
       <c r="M8" t="inlineStr"/>
       <c r="N8" s="4" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
+      <c r="P8" s="4" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -864,6 +908,8 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" s="4" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
+      <c r="P9" s="4" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -905,6 +951,8 @@
       <c r="M10" t="inlineStr"/>
       <c r="N10" s="4" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
+      <c r="P10" s="4" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -946,6 +994,8 @@
       <c r="M11" t="inlineStr"/>
       <c r="N11" s="4" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
+      <c r="P11" s="4" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -987,6 +1037,8 @@
       <c r="M12" t="inlineStr"/>
       <c r="N12" s="4" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
+      <c r="P12" s="4" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1028,6 +1080,8 @@
       <c r="M13" t="inlineStr"/>
       <c r="N13" s="4" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
+      <c r="P13" s="4" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1069,6 +1123,8 @@
       <c r="M14" t="inlineStr"/>
       <c r="N14" s="4" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
+      <c r="P14" s="4" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1110,6 +1166,8 @@
       <c r="M15" t="inlineStr"/>
       <c r="N15" s="4" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
+      <c r="P15" s="4" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1151,6 +1209,8 @@
       <c r="M16" t="inlineStr"/>
       <c r="N16" s="4" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
+      <c r="P16" s="4" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1192,6 +1252,8 @@
       <c r="M17" t="inlineStr"/>
       <c r="N17" s="4" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
+      <c r="P17" s="4" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1242,9 +1304,15 @@
       <c r="N18" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>2885</t>
+      <c r="O18" t="n">
+        <v>2885</v>
+      </c>
+      <c r="P18" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>3189</t>
         </is>
       </c>
     </row>
@@ -1297,9 +1365,15 @@
       <c r="N19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>2516</t>
+      <c r="O19" t="n">
+        <v>2516</v>
+      </c>
+      <c r="P19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>2574</t>
         </is>
       </c>
     </row>
@@ -1352,9 +1426,15 @@
       <c r="N20" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>3604</t>
+      <c r="O20" t="n">
+        <v>3604</v>
+      </c>
+      <c r="P20" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>3872</t>
         </is>
       </c>
     </row>
@@ -1407,9 +1487,15 @@
       <c r="N21" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>4078</t>
+      <c r="O21" t="n">
+        <v>4078</v>
+      </c>
+      <c r="P21" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>4046</t>
         </is>
       </c>
     </row>
@@ -1462,9 +1548,15 @@
       <c r="N22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>4044</t>
+      <c r="O22" t="n">
+        <v>4044</v>
+      </c>
+      <c r="P22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>4292</t>
         </is>
       </c>
     </row>
@@ -1517,9 +1609,15 @@
       <c r="N23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>4412</t>
+      <c r="O23" t="n">
+        <v>4412</v>
+      </c>
+      <c r="P23" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>4579</t>
         </is>
       </c>
     </row>
@@ -1572,9 +1670,15 @@
       <c r="N24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>4077</t>
+      <c r="O24" t="n">
+        <v>4077</v>
+      </c>
+      <c r="P24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>4253</t>
         </is>
       </c>
     </row>
@@ -1627,9 +1731,15 @@
       <c r="N25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>4431</t>
+      <c r="O25" t="n">
+        <v>4431</v>
+      </c>
+      <c r="P25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>4545</t>
         </is>
       </c>
     </row>
@@ -1682,7 +1792,13 @@
       <c r="N26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O26" t="inlineStr">
+      <c r="O26" t="n">
+        <v>2589</v>
+      </c>
+      <c r="P26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="inlineStr">
         <is>
           <t>2589</t>
         </is>
@@ -1737,7 +1853,13 @@
       <c r="N27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O27" t="inlineStr">
+      <c r="O27" t="n">
+        <v>2500</v>
+      </c>
+      <c r="P27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1779,6 +1901,8 @@
       <c r="M28" t="inlineStr"/>
       <c r="N28" s="4" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
+      <c r="P28" s="4" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1829,9 +1953,15 @@
       <c r="N29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O29" t="inlineStr">
-        <is>
-          <t>2516</t>
+      <c r="O29" t="n">
+        <v>2516</v>
+      </c>
+      <c r="P29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>2557</t>
         </is>
       </c>
     </row>
@@ -1884,9 +2014,15 @@
       <c r="N30" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O30" t="inlineStr">
-        <is>
-          <t>4258</t>
+      <c r="O30" t="n">
+        <v>4258</v>
+      </c>
+      <c r="P30" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>4446</t>
         </is>
       </c>
     </row>
@@ -1939,9 +2075,15 @@
       <c r="N31" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>4180</t>
+      <c r="O31" t="n">
+        <v>4180</v>
+      </c>
+      <c r="P31" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>4360</t>
         </is>
       </c>
     </row>
@@ -1994,7 +2136,13 @@
       <c r="N32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O32" t="inlineStr">
+      <c r="O32" t="n">
+        <v>2609</v>
+      </c>
+      <c r="P32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="inlineStr">
         <is>
           <t>2609</t>
         </is>
@@ -2048,6 +2196,8 @@
       </c>
       <c r="N33" s="4" t="inlineStr"/>
       <c r="O33" t="inlineStr"/>
+      <c r="P33" s="4" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2098,7 +2248,13 @@
       <c r="N34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O34" t="inlineStr">
+      <c r="O34" t="n">
+        <v>2500</v>
+      </c>
+      <c r="P34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2153,9 +2309,15 @@
       <c r="N35" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>4073</t>
+      <c r="O35" t="n">
+        <v>4073</v>
+      </c>
+      <c r="P35" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>4188</t>
         </is>
       </c>
     </row>
@@ -2208,9 +2370,15 @@
       <c r="N36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>2633</t>
+      <c r="O36" t="n">
+        <v>2633</v>
+      </c>
+      <c r="P36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>2660</t>
         </is>
       </c>
     </row>
@@ -2263,9 +2431,15 @@
       <c r="N37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>3988</t>
+      <c r="O37" t="n">
+        <v>3988</v>
+      </c>
+      <c r="P37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>4115</t>
         </is>
       </c>
     </row>
@@ -2318,9 +2492,15 @@
       <c r="N38" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>4209</t>
+      <c r="O38" t="n">
+        <v>4209</v>
+      </c>
+      <c r="P38" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>4498</t>
         </is>
       </c>
     </row>
@@ -2373,9 +2553,15 @@
       <c r="N39" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>3989</t>
+      <c r="O39" t="n">
+        <v>3989</v>
+      </c>
+      <c r="P39" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>4089</t>
         </is>
       </c>
     </row>
@@ -2428,7 +2614,13 @@
       <c r="N40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O40" t="inlineStr">
+      <c r="O40" t="n">
+        <v>0</v>
+      </c>
+      <c r="P40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2483,9 +2675,15 @@
       <c r="N41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>3785</t>
+      <c r="O41" t="n">
+        <v>3785</v>
+      </c>
+      <c r="P41" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>4068</t>
         </is>
       </c>
     </row>
@@ -2538,9 +2736,15 @@
       <c r="N42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>2710</t>
+      <c r="O42" t="n">
+        <v>2710</v>
+      </c>
+      <c r="P42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>2740</t>
         </is>
       </c>
     </row>
@@ -2584,6 +2788,8 @@
       <c r="M43" t="inlineStr"/>
       <c r="N43" s="4" t="inlineStr"/>
       <c r="O43" t="inlineStr"/>
+      <c r="P43" s="4" t="inlineStr"/>
+      <c r="Q43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2634,9 +2840,15 @@
       <c r="N44" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>4332</t>
+      <c r="O44" t="n">
+        <v>4332</v>
+      </c>
+      <c r="P44" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>4514</t>
         </is>
       </c>
     </row>
@@ -2689,9 +2901,15 @@
       <c r="N45" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>3586</t>
+      <c r="O45" t="n">
+        <v>3586</v>
+      </c>
+      <c r="P45" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>3757</t>
         </is>
       </c>
     </row>
@@ -2744,9 +2962,15 @@
       <c r="N46" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>3310</t>
+      <c r="O46" t="n">
+        <v>3310</v>
+      </c>
+      <c r="P46" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>3446</t>
         </is>
       </c>
     </row>
@@ -2799,9 +3023,15 @@
       <c r="N47" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>4383</t>
+      <c r="O47" t="n">
+        <v>4383</v>
+      </c>
+      <c r="P47" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>4688</t>
         </is>
       </c>
     </row>
@@ -2854,9 +3084,15 @@
       <c r="N48" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>4290</t>
+      <c r="O48" t="n">
+        <v>4290</v>
+      </c>
+      <c r="P48" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>4546</t>
         </is>
       </c>
     </row>
@@ -2909,9 +3145,15 @@
       <c r="N49" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>3996</t>
+      <c r="O49" t="n">
+        <v>3996</v>
+      </c>
+      <c r="P49" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>4172</t>
         </is>
       </c>
     </row>
@@ -2964,9 +3206,15 @@
       <c r="N50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>4118</t>
+      <c r="O50" t="n">
+        <v>4118</v>
+      </c>
+      <c r="P50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>4390</t>
         </is>
       </c>
     </row>
@@ -3019,9 +3267,15 @@
       <c r="N51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>3280</t>
+      <c r="O51" t="n">
+        <v>3280</v>
+      </c>
+      <c r="P51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>3351</t>
         </is>
       </c>
     </row>
@@ -3074,9 +3328,15 @@
       <c r="N52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>4183</t>
+      <c r="O52" t="n">
+        <v>4183</v>
+      </c>
+      <c r="P52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>4413</t>
         </is>
       </c>
     </row>
@@ -3129,9 +3389,15 @@
       <c r="N53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>3106</t>
+      <c r="O53" t="n">
+        <v>3106</v>
+      </c>
+      <c r="P53" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>3294</t>
         </is>
       </c>
     </row>
@@ -3184,9 +3450,15 @@
       <c r="N54" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>3987</t>
+      <c r="O54" t="n">
+        <v>3987</v>
+      </c>
+      <c r="P54" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>4128</t>
         </is>
       </c>
     </row>
@@ -3239,9 +3511,15 @@
       <c r="N55" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>3307</t>
+      <c r="O55" t="n">
+        <v>3307</v>
+      </c>
+      <c r="P55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>3314</t>
         </is>
       </c>
     </row>
@@ -3294,9 +3572,15 @@
       <c r="N56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>4367</t>
+      <c r="O56" t="n">
+        <v>4367</v>
+      </c>
+      <c r="P56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>4433</t>
         </is>
       </c>
     </row>
@@ -3349,9 +3633,15 @@
       <c r="N57" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>3756</t>
+      <c r="O57" t="n">
+        <v>3756</v>
+      </c>
+      <c r="P57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>3992</t>
         </is>
       </c>
     </row>
@@ -3404,9 +3694,15 @@
       <c r="N58" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>3760</t>
+      <c r="O58" t="n">
+        <v>3760</v>
+      </c>
+      <c r="P58" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>3958</t>
         </is>
       </c>
     </row>
@@ -3459,9 +3755,15 @@
       <c r="N59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>3673</t>
+      <c r="O59" t="n">
+        <v>3673</v>
+      </c>
+      <c r="P59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>3895</t>
         </is>
       </c>
     </row>
@@ -3514,9 +3816,15 @@
       <c r="N60" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="O60" t="inlineStr">
-        <is>
-          <t>3988</t>
+      <c r="O60" t="n">
+        <v>3988</v>
+      </c>
+      <c r="P60" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>4019</t>
         </is>
       </c>
     </row>
@@ -3556,6 +3864,8 @@
       <c r="M61" t="inlineStr"/>
       <c r="N61" s="4" t="inlineStr"/>
       <c r="O61" t="inlineStr"/>
+      <c r="P61" s="4" t="inlineStr"/>
+      <c r="Q61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -3606,9 +3916,15 @@
       <c r="N62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>3435</t>
+      <c r="O62" t="n">
+        <v>3435</v>
+      </c>
+      <c r="P62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>3621</t>
         </is>
       </c>
     </row>
@@ -3661,9 +3977,15 @@
       <c r="N63" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>3656</t>
+      <c r="O63" t="n">
+        <v>3656</v>
+      </c>
+      <c r="P63" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>3945</t>
         </is>
       </c>
     </row>
@@ -3716,9 +4038,15 @@
       <c r="N64" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>3960</t>
+      <c r="O64" t="n">
+        <v>3960</v>
+      </c>
+      <c r="P64" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>3993</t>
         </is>
       </c>
     </row>
@@ -3771,9 +4099,15 @@
       <c r="N65" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="O65" t="inlineStr">
-        <is>
-          <t>3264</t>
+      <c r="O65" t="n">
+        <v>3264</v>
+      </c>
+      <c r="P65" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>3424</t>
         </is>
       </c>
     </row>
@@ -3826,7 +4160,13 @@
       <c r="N66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O66" t="inlineStr">
+      <c r="O66" t="n">
+        <v>0</v>
+      </c>
+      <c r="P66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3881,7 +4221,13 @@
       <c r="N67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O67" t="inlineStr">
+      <c r="O67" t="n">
+        <v>0</v>
+      </c>
+      <c r="P67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3936,9 +4282,15 @@
       <c r="N68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O68" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="O68" t="n">
+        <v>2498</v>
+      </c>
+      <c r="P68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>2495</t>
         </is>
       </c>
     </row>
@@ -3991,9 +4343,15 @@
       <c r="N69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="O69" t="n">
+        <v>2500</v>
+      </c>
+      <c r="P69" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>2934</t>
         </is>
       </c>
     </row>
@@ -4046,7 +4404,13 @@
       <c r="N70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O70" t="inlineStr">
+      <c r="O70" t="n">
+        <v>0</v>
+      </c>
+      <c r="P70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4101,7 +4465,13 @@
       <c r="N71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O71" t="inlineStr">
+      <c r="O71" t="n">
+        <v>0</v>
+      </c>
+      <c r="P71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4156,7 +4526,13 @@
       <c r="N72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O72" t="inlineStr">
+      <c r="O72" t="n">
+        <v>0</v>
+      </c>
+      <c r="P72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4211,9 +4587,15 @@
       <c r="N73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O73" t="inlineStr">
-        <is>
-          <t>2601</t>
+      <c r="O73" t="n">
+        <v>2601</v>
+      </c>
+      <c r="P73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>2600</t>
         </is>
       </c>
     </row>
@@ -4266,7 +4648,13 @@
       <c r="N74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O74" t="inlineStr">
+      <c r="O74" t="n">
+        <v>0</v>
+      </c>
+      <c r="P74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4321,7 +4709,13 @@
       <c r="N75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O75" t="inlineStr">
+      <c r="O75" t="n">
+        <v>0</v>
+      </c>
+      <c r="P75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4376,9 +4770,15 @@
       <c r="N76" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="O76" t="inlineStr">
-        <is>
-          <t>3706</t>
+      <c r="O76" t="n">
+        <v>3706</v>
+      </c>
+      <c r="P76" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>3871</t>
         </is>
       </c>
     </row>
@@ -4431,9 +4831,15 @@
       <c r="N77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>3130</t>
+      <c r="O77" t="n">
+        <v>3130</v>
+      </c>
+      <c r="P77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>3123</t>
         </is>
       </c>
     </row>
@@ -4486,9 +4892,15 @@
       <c r="N78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O78" t="inlineStr">
-        <is>
-          <t>2551</t>
+      <c r="O78" t="n">
+        <v>2551</v>
+      </c>
+      <c r="P78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>2614</t>
         </is>
       </c>
     </row>
@@ -4541,9 +4953,15 @@
       <c r="N79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="O79" t="n">
+        <v>0</v>
+      </c>
+      <c r="P79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>1280</t>
         </is>
       </c>
     </row>
@@ -4596,7 +5014,13 @@
       <c r="N80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O80" t="inlineStr">
+      <c r="O80" t="n">
+        <v>0</v>
+      </c>
+      <c r="P80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4651,9 +5075,15 @@
       <c r="N81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>2568</t>
+      <c r="O81" t="n">
+        <v>2568</v>
+      </c>
+      <c r="P81" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>2612</t>
         </is>
       </c>
     </row>
@@ -4706,7 +5136,13 @@
       <c r="N82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O82" t="inlineStr">
+      <c r="O82" t="n">
+        <v>0</v>
+      </c>
+      <c r="P82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4761,7 +5197,13 @@
       <c r="N83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O83" t="inlineStr">
+      <c r="O83" t="n">
+        <v>0</v>
+      </c>
+      <c r="P83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4816,9 +5258,15 @@
       <c r="N84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>1518</t>
+      <c r="O84" t="n">
+        <v>1518</v>
+      </c>
+      <c r="P84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>1512</t>
         </is>
       </c>
     </row>
@@ -4871,7 +5319,13 @@
       <c r="N85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O85" t="inlineStr">
+      <c r="O85" t="n">
+        <v>0</v>
+      </c>
+      <c r="P85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4926,7 +5380,13 @@
       <c r="N86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O86" t="inlineStr">
+      <c r="O86" t="n">
+        <v>0</v>
+      </c>
+      <c r="P86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4981,7 +5441,13 @@
       <c r="N87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O87" t="inlineStr">
+      <c r="O87" t="n">
+        <v>0</v>
+      </c>
+      <c r="P87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5036,7 +5502,13 @@
       <c r="N88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O88" t="inlineStr">
+      <c r="O88" t="n">
+        <v>0</v>
+      </c>
+      <c r="P88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5091,7 +5563,13 @@
       <c r="N89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O89" t="inlineStr">
+      <c r="O89" t="n">
+        <v>0</v>
+      </c>
+      <c r="P89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5146,7 +5624,13 @@
       <c r="N90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O90" t="inlineStr">
+      <c r="O90" t="n">
+        <v>0</v>
+      </c>
+      <c r="P90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5201,7 +5685,13 @@
       <c r="N91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O91" t="inlineStr">
+      <c r="O91" t="n">
+        <v>0</v>
+      </c>
+      <c r="P91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5256,7 +5746,13 @@
       <c r="N92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O92" t="inlineStr">
+      <c r="O92" t="n">
+        <v>0</v>
+      </c>
+      <c r="P92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5311,7 +5807,13 @@
       <c r="N93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O93" t="inlineStr">
+      <c r="O93" t="n">
+        <v>0</v>
+      </c>
+      <c r="P93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5366,7 +5868,13 @@
       <c r="N94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O94" t="inlineStr">
+      <c r="O94" t="n">
+        <v>0</v>
+      </c>
+      <c r="P94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5421,7 +5929,13 @@
       <c r="N95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O95" t="inlineStr">
+      <c r="O95" t="n">
+        <v>0</v>
+      </c>
+      <c r="P95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5476,9 +5990,15 @@
       <c r="N96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>2803</t>
+      <c r="O96" t="n">
+        <v>2803</v>
+      </c>
+      <c r="P96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q96" t="inlineStr">
+        <is>
+          <t>2800</t>
         </is>
       </c>
     </row>
@@ -5531,9 +6051,15 @@
       <c r="N97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O97" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="O97" t="n">
+        <v>0</v>
+      </c>
+      <c r="P97" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>1020</t>
         </is>
       </c>
     </row>
@@ -5586,7 +6112,13 @@
       <c r="N98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O98" t="inlineStr">
+      <c r="O98" t="n">
+        <v>0</v>
+      </c>
+      <c r="P98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5641,7 +6173,13 @@
       <c r="N99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O99" t="inlineStr">
+      <c r="O99" t="n">
+        <v>0</v>
+      </c>
+      <c r="P99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5696,7 +6234,13 @@
       <c r="N100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O100" t="inlineStr">
+      <c r="O100" t="n">
+        <v>0</v>
+      </c>
+      <c r="P100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5751,7 +6295,13 @@
       <c r="N101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O101" t="inlineStr">
+      <c r="O101" t="n">
+        <v>0</v>
+      </c>
+      <c r="P101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5806,7 +6356,13 @@
       <c r="N102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O102" t="inlineStr">
+      <c r="O102" t="n">
+        <v>0</v>
+      </c>
+      <c r="P102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5861,7 +6417,13 @@
       <c r="N103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O103" t="inlineStr">
+      <c r="O103" t="n">
+        <v>0</v>
+      </c>
+      <c r="P103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5916,7 +6478,13 @@
       <c r="N104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O104" t="inlineStr">
+      <c r="O104" t="n">
+        <v>0</v>
+      </c>
+      <c r="P104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5971,7 +6539,13 @@
       <c r="N105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O105" t="inlineStr">
+      <c r="O105" t="n">
+        <v>0</v>
+      </c>
+      <c r="P105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6005,6 +6579,8 @@
       <c r="M106" t="inlineStr"/>
       <c r="N106" s="4" t="inlineStr"/>
       <c r="O106" t="inlineStr"/>
+      <c r="P106" s="4" t="inlineStr"/>
+      <c r="Q106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -6034,6 +6610,8 @@
       <c r="M107" t="inlineStr"/>
       <c r="N107" s="4" t="inlineStr"/>
       <c r="O107" t="inlineStr"/>
+      <c r="P107" s="4" t="inlineStr"/>
+      <c r="Q107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -6063,6 +6641,8 @@
       <c r="M108" t="inlineStr"/>
       <c r="N108" s="4" t="inlineStr"/>
       <c r="O108" t="inlineStr"/>
+      <c r="P108" s="4" t="inlineStr"/>
+      <c r="Q108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -6092,6 +6672,8 @@
       <c r="M109" t="inlineStr"/>
       <c r="N109" s="4" t="inlineStr"/>
       <c r="O109" t="inlineStr"/>
+      <c r="P109" s="4" t="inlineStr"/>
+      <c r="Q109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -6121,6 +6703,8 @@
       <c r="M110" t="inlineStr"/>
       <c r="N110" s="4" t="inlineStr"/>
       <c r="O110" t="inlineStr"/>
+      <c r="P110" s="4" t="inlineStr"/>
+      <c r="Q110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -6150,6 +6734,8 @@
       <c r="M111" t="inlineStr"/>
       <c r="N111" s="4" t="inlineStr"/>
       <c r="O111" t="inlineStr"/>
+      <c r="P111" s="4" t="inlineStr"/>
+      <c r="Q111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -6179,6 +6765,8 @@
       <c r="M112" t="inlineStr"/>
       <c r="N112" s="4" t="inlineStr"/>
       <c r="O112" t="inlineStr"/>
+      <c r="P112" s="4" t="inlineStr"/>
+      <c r="Q112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -6208,6 +6796,8 @@
       <c r="M113" t="inlineStr"/>
       <c r="N113" s="4" t="inlineStr"/>
       <c r="O113" t="inlineStr"/>
+      <c r="P113" s="4" t="inlineStr"/>
+      <c r="Q113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -6237,6 +6827,8 @@
       <c r="M114" t="inlineStr"/>
       <c r="N114" s="4" t="inlineStr"/>
       <c r="O114" t="inlineStr"/>
+      <c r="P114" s="4" t="inlineStr"/>
+      <c r="Q114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -6277,9 +6869,15 @@
       <c r="N115" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O115" t="inlineStr">
-        <is>
-          <t>4997</t>
+      <c r="O115" t="n">
+        <v>4997</v>
+      </c>
+      <c r="P115" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q115" t="inlineStr">
+        <is>
+          <t>5347</t>
         </is>
       </c>
     </row>
@@ -6322,9 +6920,15 @@
       <c r="N116" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="O116" t="inlineStr">
-        <is>
-          <t>4065</t>
+      <c r="O116" t="n">
+        <v>4065</v>
+      </c>
+      <c r="P116" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q116" t="inlineStr">
+        <is>
+          <t>4251</t>
         </is>
       </c>
     </row>
@@ -6367,9 +6971,15 @@
       <c r="N117" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="O117" t="inlineStr">
-        <is>
-          <t>4065</t>
+      <c r="O117" t="n">
+        <v>4065</v>
+      </c>
+      <c r="P117" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q117" t="inlineStr">
+        <is>
+          <t>4287</t>
         </is>
       </c>
     </row>
@@ -6412,17 +7022,21 @@
       <c r="N118" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="O118" t="inlineStr">
-        <is>
-          <t>4315</t>
+      <c r="O118" t="n">
+        <v>4315</v>
+      </c>
+      <c r="P118" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q118" t="inlineStr">
+        <is>
+          <t>4602</t>
         </is>
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>8666978</t>
-        </is>
+      <c r="A119" t="n">
+        <v>8666978</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -6447,9 +7061,15 @@
       <c r="N119" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="O119" t="inlineStr">
-        <is>
-          <t>1141</t>
+      <c r="O119" t="n">
+        <v>1141</v>
+      </c>
+      <c r="P119" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q119" t="inlineStr">
+        <is>
+          <t>1154</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-04-30 08:03:35
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q119"/>
+  <dimension ref="A1:S119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,16 @@
           <t>04-28_0</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>04-29_A</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>04-29_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -532,7 +542,13 @@
       <c r="P2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="Q2" t="n">
+        <v>3067</v>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="inlineStr">
         <is>
           <t>3067</t>
         </is>
@@ -593,7 +609,13 @@
       <c r="P3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -654,7 +676,13 @@
       <c r="P4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -715,7 +743,13 @@
       <c r="P5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q5" t="inlineStr">
+      <c r="Q5" t="n">
+        <v>2526</v>
+      </c>
+      <c r="R5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="inlineStr">
         <is>
           <t>2526</t>
         </is>
@@ -776,7 +810,13 @@
       <c r="P6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q6" t="inlineStr">
+      <c r="Q6" t="n">
+        <v>2569</v>
+      </c>
+      <c r="R6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="inlineStr">
         <is>
           <t>2569</t>
         </is>
@@ -824,6 +864,8 @@
       <c r="O7" t="inlineStr"/>
       <c r="P7" s="4" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
+      <c r="R7" s="4" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -867,6 +909,8 @@
       <c r="O8" t="inlineStr"/>
       <c r="P8" s="4" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
+      <c r="R8" s="4" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -910,6 +954,8 @@
       <c r="O9" t="inlineStr"/>
       <c r="P9" s="4" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
+      <c r="R9" s="4" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -953,6 +999,8 @@
       <c r="O10" t="inlineStr"/>
       <c r="P10" s="4" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
+      <c r="R10" s="4" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -996,6 +1044,8 @@
       <c r="O11" t="inlineStr"/>
       <c r="P11" s="4" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
+      <c r="R11" s="4" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1039,6 +1089,8 @@
       <c r="O12" t="inlineStr"/>
       <c r="P12" s="4" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
+      <c r="R12" s="4" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1082,6 +1134,8 @@
       <c r="O13" t="inlineStr"/>
       <c r="P13" s="4" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
+      <c r="R13" s="4" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1125,6 +1179,8 @@
       <c r="O14" t="inlineStr"/>
       <c r="P14" s="4" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
+      <c r="R14" s="4" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1168,6 +1224,8 @@
       <c r="O15" t="inlineStr"/>
       <c r="P15" s="4" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
+      <c r="R15" s="4" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1211,6 +1269,8 @@
       <c r="O16" t="inlineStr"/>
       <c r="P16" s="4" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
+      <c r="R16" s="4" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1254,6 +1314,8 @@
       <c r="O17" t="inlineStr"/>
       <c r="P17" s="4" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
+      <c r="R17" s="4" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1310,7 +1372,13 @@
       <c r="P18" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Q18" t="inlineStr">
+      <c r="Q18" t="n">
+        <v>3189</v>
+      </c>
+      <c r="R18" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="S18" t="inlineStr">
         <is>
           <t>3189</t>
         </is>
@@ -1371,7 +1439,13 @@
       <c r="P19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q19" t="inlineStr">
+      <c r="Q19" t="n">
+        <v>2574</v>
+      </c>
+      <c r="R19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="inlineStr">
         <is>
           <t>2574</t>
         </is>
@@ -1432,7 +1506,13 @@
       <c r="P20" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="Q20" t="inlineStr">
+      <c r="Q20" t="n">
+        <v>3872</v>
+      </c>
+      <c r="R20" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="S20" t="inlineStr">
         <is>
           <t>3872</t>
         </is>
@@ -1493,7 +1573,13 @@
       <c r="P21" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="Q21" t="inlineStr">
+      <c r="Q21" t="n">
+        <v>4046</v>
+      </c>
+      <c r="R21" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="S21" t="inlineStr">
         <is>
           <t>4046</t>
         </is>
@@ -1554,7 +1640,13 @@
       <c r="P22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Q22" t="inlineStr">
+      <c r="Q22" t="n">
+        <v>4292</v>
+      </c>
+      <c r="R22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="S22" t="inlineStr">
         <is>
           <t>4292</t>
         </is>
@@ -1615,7 +1707,13 @@
       <c r="P23" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="Q23" t="inlineStr">
+      <c r="Q23" t="n">
+        <v>4579</v>
+      </c>
+      <c r="R23" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="S23" t="inlineStr">
         <is>
           <t>4579</t>
         </is>
@@ -1676,7 +1774,13 @@
       <c r="P24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Q24" t="inlineStr">
+      <c r="Q24" t="n">
+        <v>4253</v>
+      </c>
+      <c r="R24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S24" t="inlineStr">
         <is>
           <t>4253</t>
         </is>
@@ -1737,7 +1841,13 @@
       <c r="P25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Q25" t="inlineStr">
+      <c r="Q25" t="n">
+        <v>4545</v>
+      </c>
+      <c r="R25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="S25" t="inlineStr">
         <is>
           <t>4545</t>
         </is>
@@ -1798,7 +1908,13 @@
       <c r="P26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q26" t="inlineStr">
+      <c r="Q26" t="n">
+        <v>2589</v>
+      </c>
+      <c r="R26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" t="inlineStr">
         <is>
           <t>2589</t>
         </is>
@@ -1859,7 +1975,13 @@
       <c r="P27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q27" t="inlineStr">
+      <c r="Q27" t="n">
+        <v>2500</v>
+      </c>
+      <c r="R27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1903,6 +2025,8 @@
       <c r="O28" t="inlineStr"/>
       <c r="P28" s="4" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
+      <c r="R28" s="4" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1959,7 +2083,13 @@
       <c r="P29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q29" t="inlineStr">
+      <c r="Q29" t="n">
+        <v>2557</v>
+      </c>
+      <c r="R29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S29" t="inlineStr">
         <is>
           <t>2557</t>
         </is>
@@ -2020,7 +2150,13 @@
       <c r="P30" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="Q30" t="inlineStr">
+      <c r="Q30" t="n">
+        <v>4446</v>
+      </c>
+      <c r="R30" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="S30" t="inlineStr">
         <is>
           <t>4446</t>
         </is>
@@ -2081,7 +2217,13 @@
       <c r="P31" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="Q31" t="inlineStr">
+      <c r="Q31" t="n">
+        <v>4360</v>
+      </c>
+      <c r="R31" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="S31" t="inlineStr">
         <is>
           <t>4360</t>
         </is>
@@ -2142,7 +2284,13 @@
       <c r="P32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q32" t="inlineStr">
+      <c r="Q32" t="n">
+        <v>2609</v>
+      </c>
+      <c r="R32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="inlineStr">
         <is>
           <t>2609</t>
         </is>
@@ -2198,6 +2346,8 @@
       <c r="O33" t="inlineStr"/>
       <c r="P33" s="4" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
+      <c r="R33" s="4" t="inlineStr"/>
+      <c r="S33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2254,7 +2404,13 @@
       <c r="P34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q34" t="inlineStr">
+      <c r="Q34" t="n">
+        <v>2500</v>
+      </c>
+      <c r="R34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S34" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2315,7 +2471,13 @@
       <c r="P35" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Q35" t="inlineStr">
+      <c r="Q35" t="n">
+        <v>4188</v>
+      </c>
+      <c r="R35" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="S35" t="inlineStr">
         <is>
           <t>4188</t>
         </is>
@@ -2376,7 +2538,13 @@
       <c r="P36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q36" t="inlineStr">
+      <c r="Q36" t="n">
+        <v>2660</v>
+      </c>
+      <c r="R36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S36" t="inlineStr">
         <is>
           <t>2660</t>
         </is>
@@ -2437,7 +2605,13 @@
       <c r="P37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Q37" t="inlineStr">
+      <c r="Q37" t="n">
+        <v>4115</v>
+      </c>
+      <c r="R37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="S37" t="inlineStr">
         <is>
           <t>4115</t>
         </is>
@@ -2498,7 +2672,13 @@
       <c r="P38" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="Q38" t="inlineStr">
+      <c r="Q38" t="n">
+        <v>4498</v>
+      </c>
+      <c r="R38" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="S38" t="inlineStr">
         <is>
           <t>4498</t>
         </is>
@@ -2559,7 +2739,13 @@
       <c r="P39" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Q39" t="inlineStr">
+      <c r="Q39" t="n">
+        <v>4089</v>
+      </c>
+      <c r="R39" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="S39" t="inlineStr">
         <is>
           <t>4089</t>
         </is>
@@ -2620,7 +2806,13 @@
       <c r="P40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q40" t="inlineStr">
+      <c r="Q40" t="n">
+        <v>0</v>
+      </c>
+      <c r="R40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2681,7 +2873,13 @@
       <c r="P41" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="Q41" t="inlineStr">
+      <c r="Q41" t="n">
+        <v>4068</v>
+      </c>
+      <c r="R41" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="S41" t="inlineStr">
         <is>
           <t>4068</t>
         </is>
@@ -2742,7 +2940,13 @@
       <c r="P42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q42" t="inlineStr">
+      <c r="Q42" t="n">
+        <v>2740</v>
+      </c>
+      <c r="R42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S42" t="inlineStr">
         <is>
           <t>2740</t>
         </is>
@@ -2790,6 +2994,8 @@
       <c r="O43" t="inlineStr"/>
       <c r="P43" s="4" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
+      <c r="R43" s="4" t="inlineStr"/>
+      <c r="S43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2846,7 +3052,13 @@
       <c r="P44" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Q44" t="inlineStr">
+      <c r="Q44" t="n">
+        <v>4514</v>
+      </c>
+      <c r="R44" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="S44" t="inlineStr">
         <is>
           <t>4514</t>
         </is>
@@ -2907,7 +3119,13 @@
       <c r="P45" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Q45" t="inlineStr">
+      <c r="Q45" t="n">
+        <v>3757</v>
+      </c>
+      <c r="R45" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="S45" t="inlineStr">
         <is>
           <t>3757</t>
         </is>
@@ -2968,7 +3186,13 @@
       <c r="P46" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="Q46" t="inlineStr">
+      <c r="Q46" t="n">
+        <v>3446</v>
+      </c>
+      <c r="R46" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="S46" t="inlineStr">
         <is>
           <t>3446</t>
         </is>
@@ -3029,7 +3253,13 @@
       <c r="P47" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Q47" t="inlineStr">
+      <c r="Q47" t="n">
+        <v>4688</v>
+      </c>
+      <c r="R47" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="S47" t="inlineStr">
         <is>
           <t>4688</t>
         </is>
@@ -3090,7 +3320,13 @@
       <c r="P48" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="Q48" t="inlineStr">
+      <c r="Q48" t="n">
+        <v>4546</v>
+      </c>
+      <c r="R48" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="S48" t="inlineStr">
         <is>
           <t>4546</t>
         </is>
@@ -3151,7 +3387,13 @@
       <c r="P49" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Q49" t="inlineStr">
+      <c r="Q49" t="n">
+        <v>4172</v>
+      </c>
+      <c r="R49" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="S49" t="inlineStr">
         <is>
           <t>4172</t>
         </is>
@@ -3212,7 +3454,13 @@
       <c r="P50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="Q50" t="inlineStr">
+      <c r="Q50" t="n">
+        <v>4390</v>
+      </c>
+      <c r="R50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="S50" t="inlineStr">
         <is>
           <t>4390</t>
         </is>
@@ -3273,7 +3521,13 @@
       <c r="P51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q51" t="inlineStr">
+      <c r="Q51" t="n">
+        <v>3351</v>
+      </c>
+      <c r="R51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S51" t="inlineStr">
         <is>
           <t>3351</t>
         </is>
@@ -3334,7 +3588,13 @@
       <c r="P52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Q52" t="inlineStr">
+      <c r="Q52" t="n">
+        <v>4413</v>
+      </c>
+      <c r="R52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="S52" t="inlineStr">
         <is>
           <t>4413</t>
         </is>
@@ -3395,7 +3655,13 @@
       <c r="P53" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="Q53" t="inlineStr">
+      <c r="Q53" t="n">
+        <v>3294</v>
+      </c>
+      <c r="R53" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="S53" t="inlineStr">
         <is>
           <t>3294</t>
         </is>
@@ -3456,7 +3722,13 @@
       <c r="P54" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Q54" t="inlineStr">
+      <c r="Q54" t="n">
+        <v>4128</v>
+      </c>
+      <c r="R54" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="S54" t="inlineStr">
         <is>
           <t>4128</t>
         </is>
@@ -3517,7 +3789,13 @@
       <c r="P55" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q55" t="inlineStr">
+      <c r="Q55" t="n">
+        <v>3314</v>
+      </c>
+      <c r="R55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S55" t="inlineStr">
         <is>
           <t>3314</t>
         </is>
@@ -3578,7 +3856,13 @@
       <c r="P56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Q56" t="inlineStr">
+      <c r="Q56" t="n">
+        <v>4433</v>
+      </c>
+      <c r="R56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="S56" t="inlineStr">
         <is>
           <t>4433</t>
         </is>
@@ -3639,7 +3923,13 @@
       <c r="P57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Q57" t="inlineStr">
+      <c r="Q57" t="n">
+        <v>3992</v>
+      </c>
+      <c r="R57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="S57" t="inlineStr">
         <is>
           <t>3992</t>
         </is>
@@ -3700,7 +3990,13 @@
       <c r="P58" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="Q58" t="inlineStr">
+      <c r="Q58" t="n">
+        <v>3958</v>
+      </c>
+      <c r="R58" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="S58" t="inlineStr">
         <is>
           <t>3958</t>
         </is>
@@ -3761,7 +4057,13 @@
       <c r="P59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Q59" t="inlineStr">
+      <c r="Q59" t="n">
+        <v>3895</v>
+      </c>
+      <c r="R59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="S59" t="inlineStr">
         <is>
           <t>3895</t>
         </is>
@@ -3822,7 +4124,13 @@
       <c r="P60" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="Q60" t="inlineStr">
+      <c r="Q60" t="n">
+        <v>4019</v>
+      </c>
+      <c r="R60" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="S60" t="inlineStr">
         <is>
           <t>4019</t>
         </is>
@@ -3866,6 +4174,8 @@
       <c r="O61" t="inlineStr"/>
       <c r="P61" s="4" t="inlineStr"/>
       <c r="Q61" t="inlineStr"/>
+      <c r="R61" s="4" t="inlineStr"/>
+      <c r="S61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -3922,7 +4232,13 @@
       <c r="P62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Q62" t="inlineStr">
+      <c r="Q62" t="n">
+        <v>3621</v>
+      </c>
+      <c r="R62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="S62" t="inlineStr">
         <is>
           <t>3621</t>
         </is>
@@ -3983,7 +4299,13 @@
       <c r="P63" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="Q63" t="inlineStr">
+      <c r="Q63" t="n">
+        <v>3945</v>
+      </c>
+      <c r="R63" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="S63" t="inlineStr">
         <is>
           <t>3945</t>
         </is>
@@ -4044,7 +4366,13 @@
       <c r="P64" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="Q64" t="inlineStr">
+      <c r="Q64" t="n">
+        <v>3993</v>
+      </c>
+      <c r="R64" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="S64" t="inlineStr">
         <is>
           <t>3993</t>
         </is>
@@ -4105,7 +4433,13 @@
       <c r="P65" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="Q65" t="inlineStr">
+      <c r="Q65" t="n">
+        <v>3424</v>
+      </c>
+      <c r="R65" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="S65" t="inlineStr">
         <is>
           <t>3424</t>
         </is>
@@ -4166,7 +4500,13 @@
       <c r="P66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q66" t="inlineStr">
+      <c r="Q66" t="n">
+        <v>0</v>
+      </c>
+      <c r="R66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4227,7 +4567,13 @@
       <c r="P67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q67" t="inlineStr">
+      <c r="Q67" t="n">
+        <v>0</v>
+      </c>
+      <c r="R67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4288,7 +4634,13 @@
       <c r="P68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q68" t="inlineStr">
+      <c r="Q68" t="n">
+        <v>2495</v>
+      </c>
+      <c r="R68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S68" t="inlineStr">
         <is>
           <t>2495</t>
         </is>
@@ -4349,7 +4701,13 @@
       <c r="P69" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="Q69" t="inlineStr">
+      <c r="Q69" t="n">
+        <v>2934</v>
+      </c>
+      <c r="R69" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="S69" t="inlineStr">
         <is>
           <t>2934</t>
         </is>
@@ -4410,7 +4768,13 @@
       <c r="P70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q70" t="inlineStr">
+      <c r="Q70" t="n">
+        <v>0</v>
+      </c>
+      <c r="R70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4471,7 +4835,13 @@
       <c r="P71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q71" t="inlineStr">
+      <c r="Q71" t="n">
+        <v>0</v>
+      </c>
+      <c r="R71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4532,7 +4902,13 @@
       <c r="P72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q72" t="inlineStr">
+      <c r="Q72" t="n">
+        <v>0</v>
+      </c>
+      <c r="R72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4593,7 +4969,13 @@
       <c r="P73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q73" t="inlineStr">
+      <c r="Q73" t="n">
+        <v>2600</v>
+      </c>
+      <c r="R73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S73" t="inlineStr">
         <is>
           <t>2600</t>
         </is>
@@ -4654,7 +5036,13 @@
       <c r="P74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q74" t="inlineStr">
+      <c r="Q74" t="n">
+        <v>0</v>
+      </c>
+      <c r="R74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4715,7 +5103,13 @@
       <c r="P75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q75" t="inlineStr">
+      <c r="Q75" t="n">
+        <v>0</v>
+      </c>
+      <c r="R75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4776,7 +5170,13 @@
       <c r="P76" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="Q76" t="inlineStr">
+      <c r="Q76" t="n">
+        <v>3871</v>
+      </c>
+      <c r="R76" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="S76" t="inlineStr">
         <is>
           <t>3871</t>
         </is>
@@ -4837,7 +5237,13 @@
       <c r="P77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q77" t="inlineStr">
+      <c r="Q77" t="n">
+        <v>3123</v>
+      </c>
+      <c r="R77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S77" t="inlineStr">
         <is>
           <t>3123</t>
         </is>
@@ -4898,7 +5304,13 @@
       <c r="P78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q78" t="inlineStr">
+      <c r="Q78" t="n">
+        <v>2614</v>
+      </c>
+      <c r="R78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S78" t="inlineStr">
         <is>
           <t>2614</t>
         </is>
@@ -4959,7 +5371,13 @@
       <c r="P79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q79" t="inlineStr">
+      <c r="Q79" t="n">
+        <v>1280</v>
+      </c>
+      <c r="R79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S79" t="inlineStr">
         <is>
           <t>1280</t>
         </is>
@@ -5020,7 +5438,13 @@
       <c r="P80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q80" t="inlineStr">
+      <c r="Q80" t="n">
+        <v>0</v>
+      </c>
+      <c r="R80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5081,7 +5505,13 @@
       <c r="P81" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="Q81" t="inlineStr">
+      <c r="Q81" t="n">
+        <v>2612</v>
+      </c>
+      <c r="R81" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="S81" t="inlineStr">
         <is>
           <t>2612</t>
         </is>
@@ -5142,7 +5572,13 @@
       <c r="P82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q82" t="inlineStr">
+      <c r="Q82" t="n">
+        <v>0</v>
+      </c>
+      <c r="R82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5203,7 +5639,13 @@
       <c r="P83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q83" t="inlineStr">
+      <c r="Q83" t="n">
+        <v>0</v>
+      </c>
+      <c r="R83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5264,7 +5706,13 @@
       <c r="P84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q84" t="inlineStr">
+      <c r="Q84" t="n">
+        <v>1512</v>
+      </c>
+      <c r="R84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S84" t="inlineStr">
         <is>
           <t>1512</t>
         </is>
@@ -5325,7 +5773,13 @@
       <c r="P85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q85" t="inlineStr">
+      <c r="Q85" t="n">
+        <v>0</v>
+      </c>
+      <c r="R85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5386,7 +5840,13 @@
       <c r="P86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q86" t="inlineStr">
+      <c r="Q86" t="n">
+        <v>0</v>
+      </c>
+      <c r="R86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5447,7 +5907,13 @@
       <c r="P87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q87" t="inlineStr">
+      <c r="Q87" t="n">
+        <v>0</v>
+      </c>
+      <c r="R87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5508,7 +5974,13 @@
       <c r="P88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q88" t="inlineStr">
+      <c r="Q88" t="n">
+        <v>0</v>
+      </c>
+      <c r="R88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5569,7 +6041,13 @@
       <c r="P89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q89" t="inlineStr">
+      <c r="Q89" t="n">
+        <v>0</v>
+      </c>
+      <c r="R89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5630,7 +6108,13 @@
       <c r="P90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q90" t="inlineStr">
+      <c r="Q90" t="n">
+        <v>0</v>
+      </c>
+      <c r="R90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5691,7 +6175,13 @@
       <c r="P91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q91" t="inlineStr">
+      <c r="Q91" t="n">
+        <v>0</v>
+      </c>
+      <c r="R91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5752,7 +6242,13 @@
       <c r="P92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q92" t="inlineStr">
+      <c r="Q92" t="n">
+        <v>0</v>
+      </c>
+      <c r="R92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5813,7 +6309,13 @@
       <c r="P93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q93" t="inlineStr">
+      <c r="Q93" t="n">
+        <v>0</v>
+      </c>
+      <c r="R93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5874,7 +6376,13 @@
       <c r="P94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q94" t="inlineStr">
+      <c r="Q94" t="n">
+        <v>0</v>
+      </c>
+      <c r="R94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5935,7 +6443,13 @@
       <c r="P95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q95" t="inlineStr">
+      <c r="Q95" t="n">
+        <v>0</v>
+      </c>
+      <c r="R95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5996,7 +6510,13 @@
       <c r="P96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q96" t="inlineStr">
+      <c r="Q96" t="n">
+        <v>2800</v>
+      </c>
+      <c r="R96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S96" t="inlineStr">
         <is>
           <t>2800</t>
         </is>
@@ -6057,7 +6577,13 @@
       <c r="P97" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="Q97" t="inlineStr">
+      <c r="Q97" t="n">
+        <v>1020</v>
+      </c>
+      <c r="R97" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="S97" t="inlineStr">
         <is>
           <t>1020</t>
         </is>
@@ -6118,7 +6644,13 @@
       <c r="P98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q98" t="inlineStr">
+      <c r="Q98" t="n">
+        <v>0</v>
+      </c>
+      <c r="R98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6179,7 +6711,13 @@
       <c r="P99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q99" t="inlineStr">
+      <c r="Q99" t="n">
+        <v>0</v>
+      </c>
+      <c r="R99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6240,7 +6778,13 @@
       <c r="P100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q100" t="inlineStr">
+      <c r="Q100" t="n">
+        <v>0</v>
+      </c>
+      <c r="R100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6301,7 +6845,13 @@
       <c r="P101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q101" t="inlineStr">
+      <c r="Q101" t="n">
+        <v>0</v>
+      </c>
+      <c r="R101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6362,7 +6912,13 @@
       <c r="P102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q102" t="inlineStr">
+      <c r="Q102" t="n">
+        <v>0</v>
+      </c>
+      <c r="R102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6423,7 +6979,13 @@
       <c r="P103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q103" t="inlineStr">
+      <c r="Q103" t="n">
+        <v>0</v>
+      </c>
+      <c r="R103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6484,7 +7046,13 @@
       <c r="P104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q104" t="inlineStr">
+      <c r="Q104" t="n">
+        <v>0</v>
+      </c>
+      <c r="R104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6545,7 +7113,13 @@
       <c r="P105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q105" t="inlineStr">
+      <c r="Q105" t="n">
+        <v>0</v>
+      </c>
+      <c r="R105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6581,6 +7155,8 @@
       <c r="O106" t="inlineStr"/>
       <c r="P106" s="4" t="inlineStr"/>
       <c r="Q106" t="inlineStr"/>
+      <c r="R106" s="4" t="inlineStr"/>
+      <c r="S106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -6612,6 +7188,8 @@
       <c r="O107" t="inlineStr"/>
       <c r="P107" s="4" t="inlineStr"/>
       <c r="Q107" t="inlineStr"/>
+      <c r="R107" s="4" t="inlineStr"/>
+      <c r="S107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -6643,6 +7221,8 @@
       <c r="O108" t="inlineStr"/>
       <c r="P108" s="4" t="inlineStr"/>
       <c r="Q108" t="inlineStr"/>
+      <c r="R108" s="4" t="inlineStr"/>
+      <c r="S108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -6674,6 +7254,8 @@
       <c r="O109" t="inlineStr"/>
       <c r="P109" s="4" t="inlineStr"/>
       <c r="Q109" t="inlineStr"/>
+      <c r="R109" s="4" t="inlineStr"/>
+      <c r="S109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -6705,6 +7287,8 @@
       <c r="O110" t="inlineStr"/>
       <c r="P110" s="4" t="inlineStr"/>
       <c r="Q110" t="inlineStr"/>
+      <c r="R110" s="4" t="inlineStr"/>
+      <c r="S110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -6736,6 +7320,8 @@
       <c r="O111" t="inlineStr"/>
       <c r="P111" s="4" t="inlineStr"/>
       <c r="Q111" t="inlineStr"/>
+      <c r="R111" s="4" t="inlineStr"/>
+      <c r="S111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -6767,6 +7353,8 @@
       <c r="O112" t="inlineStr"/>
       <c r="P112" s="4" t="inlineStr"/>
       <c r="Q112" t="inlineStr"/>
+      <c r="R112" s="4" t="inlineStr"/>
+      <c r="S112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -6798,6 +7386,8 @@
       <c r="O113" t="inlineStr"/>
       <c r="P113" s="4" t="inlineStr"/>
       <c r="Q113" t="inlineStr"/>
+      <c r="R113" s="4" t="inlineStr"/>
+      <c r="S113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -6829,6 +7419,8 @@
       <c r="O114" t="inlineStr"/>
       <c r="P114" s="4" t="inlineStr"/>
       <c r="Q114" t="inlineStr"/>
+      <c r="R114" s="4" t="inlineStr"/>
+      <c r="S114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -6875,7 +7467,13 @@
       <c r="P115" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Q115" t="inlineStr">
+      <c r="Q115" t="n">
+        <v>5347</v>
+      </c>
+      <c r="R115" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S115" t="inlineStr">
         <is>
           <t>5347</t>
         </is>
@@ -6926,7 +7524,13 @@
       <c r="P116" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="Q116" t="inlineStr">
+      <c r="Q116" t="n">
+        <v>4251</v>
+      </c>
+      <c r="R116" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="S116" t="inlineStr">
         <is>
           <t>4251</t>
         </is>
@@ -6977,7 +7581,13 @@
       <c r="P117" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="Q117" t="inlineStr">
+      <c r="Q117" t="n">
+        <v>4287</v>
+      </c>
+      <c r="R117" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="S117" t="inlineStr">
         <is>
           <t>4287</t>
         </is>
@@ -7028,7 +7638,13 @@
       <c r="P118" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="Q118" t="inlineStr">
+      <c r="Q118" t="n">
+        <v>4602</v>
+      </c>
+      <c r="R118" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="S118" t="inlineStr">
         <is>
           <t>4602</t>
         </is>
@@ -7067,7 +7683,13 @@
       <c r="P119" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="Q119" t="inlineStr">
+      <c r="Q119" t="n">
+        <v>1154</v>
+      </c>
+      <c r="R119" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="S119" t="inlineStr">
         <is>
           <t>1154</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-05-01 11:30:54
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S119"/>
+  <dimension ref="A1:U119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +486,16 @@
           <t>04-29_0</t>
         </is>
       </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>04-30_A</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>04-30_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -548,9 +558,15 @@
       <c r="R2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>3067</t>
+      <c r="S2" t="n">
+        <v>3067</v>
+      </c>
+      <c r="T2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>3083</t>
         </is>
       </c>
     </row>
@@ -615,7 +631,13 @@
       <c r="R3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -682,7 +704,13 @@
       <c r="R4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -749,9 +777,15 @@
       <c r="R5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>2526</t>
+      <c r="S5" t="n">
+        <v>2526</v>
+      </c>
+      <c r="T5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>2512</t>
         </is>
       </c>
     </row>
@@ -816,9 +850,15 @@
       <c r="R6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>2569</t>
+      <c r="S6" t="n">
+        <v>2569</v>
+      </c>
+      <c r="T6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>2646</t>
         </is>
       </c>
     </row>
@@ -866,6 +906,8 @@
       <c r="Q7" t="inlineStr"/>
       <c r="R7" s="4" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
+      <c r="T7" s="4" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -911,6 +953,8 @@
       <c r="Q8" t="inlineStr"/>
       <c r="R8" s="4" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
+      <c r="T8" s="4" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -956,6 +1000,8 @@
       <c r="Q9" t="inlineStr"/>
       <c r="R9" s="4" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
+      <c r="T9" s="4" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1001,6 +1047,8 @@
       <c r="Q10" t="inlineStr"/>
       <c r="R10" s="4" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
+      <c r="T10" s="4" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1046,6 +1094,8 @@
       <c r="Q11" t="inlineStr"/>
       <c r="R11" s="4" t="inlineStr"/>
       <c r="S11" t="inlineStr"/>
+      <c r="T11" s="4" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1091,6 +1141,8 @@
       <c r="Q12" t="inlineStr"/>
       <c r="R12" s="4" t="inlineStr"/>
       <c r="S12" t="inlineStr"/>
+      <c r="T12" s="4" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1136,6 +1188,8 @@
       <c r="Q13" t="inlineStr"/>
       <c r="R13" s="4" t="inlineStr"/>
       <c r="S13" t="inlineStr"/>
+      <c r="T13" s="4" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1181,6 +1235,8 @@
       <c r="Q14" t="inlineStr"/>
       <c r="R14" s="4" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
+      <c r="T14" s="4" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1226,6 +1282,8 @@
       <c r="Q15" t="inlineStr"/>
       <c r="R15" s="4" t="inlineStr"/>
       <c r="S15" t="inlineStr"/>
+      <c r="T15" s="4" t="inlineStr"/>
+      <c r="U15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1271,6 +1329,8 @@
       <c r="Q16" t="inlineStr"/>
       <c r="R16" s="4" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
+      <c r="T16" s="4" t="inlineStr"/>
+      <c r="U16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1316,6 +1376,8 @@
       <c r="Q17" t="inlineStr"/>
       <c r="R17" s="4" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
+      <c r="T17" s="4" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1378,9 +1440,15 @@
       <c r="R18" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>3189</t>
+      <c r="S18" t="n">
+        <v>3189</v>
+      </c>
+      <c r="T18" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>3753</t>
         </is>
       </c>
     </row>
@@ -1445,9 +1513,15 @@
       <c r="R19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>2574</t>
+      <c r="S19" t="n">
+        <v>2574</v>
+      </c>
+      <c r="T19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>2605</t>
         </is>
       </c>
     </row>
@@ -1512,9 +1586,15 @@
       <c r="R20" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>3872</t>
+      <c r="S20" t="n">
+        <v>3872</v>
+      </c>
+      <c r="T20" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>4080</t>
         </is>
       </c>
     </row>
@@ -1579,9 +1659,15 @@
       <c r="R21" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>4046</t>
+      <c r="S21" t="n">
+        <v>4046</v>
+      </c>
+      <c r="T21" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>4577</t>
         </is>
       </c>
     </row>
@@ -1646,9 +1732,15 @@
       <c r="R22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>4292</t>
+      <c r="S22" t="n">
+        <v>4292</v>
+      </c>
+      <c r="T22" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>4541</t>
         </is>
       </c>
     </row>
@@ -1713,9 +1805,15 @@
       <c r="R23" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>4579</t>
+      <c r="S23" t="n">
+        <v>4579</v>
+      </c>
+      <c r="T23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>5008</t>
         </is>
       </c>
     </row>
@@ -1780,9 +1878,15 @@
       <c r="R24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>4253</t>
+      <c r="S24" t="n">
+        <v>4253</v>
+      </c>
+      <c r="T24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>4596</t>
         </is>
       </c>
     </row>
@@ -1847,9 +1951,15 @@
       <c r="R25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>4545</t>
+      <c r="S25" t="n">
+        <v>4545</v>
+      </c>
+      <c r="T25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>4960</t>
         </is>
       </c>
     </row>
@@ -1914,9 +2024,15 @@
       <c r="R26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>2589</t>
+      <c r="S26" t="n">
+        <v>2589</v>
+      </c>
+      <c r="T26" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>2778</t>
         </is>
       </c>
     </row>
@@ -1981,7 +2097,13 @@
       <c r="R27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S27" t="inlineStr">
+      <c r="S27" t="n">
+        <v>2500</v>
+      </c>
+      <c r="T27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U27" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2027,6 +2149,8 @@
       <c r="Q28" t="inlineStr"/>
       <c r="R28" s="4" t="inlineStr"/>
       <c r="S28" t="inlineStr"/>
+      <c r="T28" s="4" t="inlineStr"/>
+      <c r="U28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2089,7 +2213,13 @@
       <c r="R29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S29" t="inlineStr">
+      <c r="S29" t="n">
+        <v>2557</v>
+      </c>
+      <c r="T29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U29" t="inlineStr">
         <is>
           <t>2557</t>
         </is>
@@ -2156,9 +2286,15 @@
       <c r="R30" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>4446</t>
+      <c r="S30" t="n">
+        <v>4446</v>
+      </c>
+      <c r="T30" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>4832</t>
         </is>
       </c>
     </row>
@@ -2223,9 +2359,15 @@
       <c r="R31" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>4360</t>
+      <c r="S31" t="n">
+        <v>4360</v>
+      </c>
+      <c r="T31" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>4782</t>
         </is>
       </c>
     </row>
@@ -2290,9 +2432,15 @@
       <c r="R32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>2609</t>
+      <c r="S32" t="n">
+        <v>2609</v>
+      </c>
+      <c r="T32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>2640</t>
         </is>
       </c>
     </row>
@@ -2348,6 +2496,8 @@
       <c r="Q33" t="inlineStr"/>
       <c r="R33" s="4" t="inlineStr"/>
       <c r="S33" t="inlineStr"/>
+      <c r="T33" s="4" t="inlineStr"/>
+      <c r="U33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2410,7 +2560,13 @@
       <c r="R34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S34" t="inlineStr">
+      <c r="S34" t="n">
+        <v>2500</v>
+      </c>
+      <c r="T34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U34" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2477,9 +2633,15 @@
       <c r="R35" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="S35" t="inlineStr">
-        <is>
-          <t>4188</t>
+      <c r="S35" t="n">
+        <v>4188</v>
+      </c>
+      <c r="T35" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>4489</t>
         </is>
       </c>
     </row>
@@ -2544,9 +2706,15 @@
       <c r="R36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S36" t="inlineStr">
-        <is>
-          <t>2660</t>
+      <c r="S36" t="n">
+        <v>2660</v>
+      </c>
+      <c r="T36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>2731</t>
         </is>
       </c>
     </row>
@@ -2611,9 +2779,15 @@
       <c r="R37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>4115</t>
+      <c r="S37" t="n">
+        <v>4115</v>
+      </c>
+      <c r="T37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>4364</t>
         </is>
       </c>
     </row>
@@ -2678,9 +2852,15 @@
       <c r="R38" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="S38" t="inlineStr">
-        <is>
-          <t>4498</t>
+      <c r="S38" t="n">
+        <v>4498</v>
+      </c>
+      <c r="T38" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>4925</t>
         </is>
       </c>
     </row>
@@ -2745,9 +2925,15 @@
       <c r="R39" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="S39" t="inlineStr">
-        <is>
-          <t>4089</t>
+      <c r="S39" t="n">
+        <v>4089</v>
+      </c>
+      <c r="T39" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>4446</t>
         </is>
       </c>
     </row>
@@ -2812,7 +2998,13 @@
       <c r="R40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S40" t="inlineStr">
+      <c r="S40" t="n">
+        <v>0</v>
+      </c>
+      <c r="T40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2879,9 +3071,15 @@
       <c r="R41" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="S41" t="inlineStr">
-        <is>
-          <t>4068</t>
+      <c r="S41" t="n">
+        <v>4068</v>
+      </c>
+      <c r="T41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>4191</t>
         </is>
       </c>
     </row>
@@ -2946,9 +3144,15 @@
       <c r="R42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S42" t="inlineStr">
-        <is>
-          <t>2740</t>
+      <c r="S42" t="n">
+        <v>2740</v>
+      </c>
+      <c r="T42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>2900</t>
         </is>
       </c>
     </row>
@@ -2996,6 +3200,8 @@
       <c r="Q43" t="inlineStr"/>
       <c r="R43" s="4" t="inlineStr"/>
       <c r="S43" t="inlineStr"/>
+      <c r="T43" s="4" t="inlineStr"/>
+      <c r="U43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3058,9 +3264,15 @@
       <c r="R44" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="S44" t="inlineStr">
-        <is>
-          <t>4514</t>
+      <c r="S44" t="n">
+        <v>4514</v>
+      </c>
+      <c r="T44" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>4860</t>
         </is>
       </c>
     </row>
@@ -3125,9 +3337,15 @@
       <c r="R45" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="S45" t="inlineStr">
-        <is>
-          <t>3757</t>
+      <c r="S45" t="n">
+        <v>3757</v>
+      </c>
+      <c r="T45" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>3982</t>
         </is>
       </c>
     </row>
@@ -3192,9 +3410,15 @@
       <c r="R46" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="S46" t="inlineStr">
-        <is>
-          <t>3446</t>
+      <c r="S46" t="n">
+        <v>3446</v>
+      </c>
+      <c r="T46" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>3767</t>
         </is>
       </c>
     </row>
@@ -3259,9 +3483,15 @@
       <c r="R47" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="S47" t="inlineStr">
-        <is>
-          <t>4688</t>
+      <c r="S47" t="n">
+        <v>4688</v>
+      </c>
+      <c r="T47" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>5050</t>
         </is>
       </c>
     </row>
@@ -3326,9 +3556,15 @@
       <c r="R48" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="S48" t="inlineStr">
-        <is>
-          <t>4546</t>
+      <c r="S48" t="n">
+        <v>4546</v>
+      </c>
+      <c r="T48" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>4658</t>
         </is>
       </c>
     </row>
@@ -3393,9 +3629,15 @@
       <c r="R49" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="S49" t="inlineStr">
-        <is>
-          <t>4172</t>
+      <c r="S49" t="n">
+        <v>4172</v>
+      </c>
+      <c r="T49" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>4454</t>
         </is>
       </c>
     </row>
@@ -3460,9 +3702,15 @@
       <c r="R50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="S50" t="inlineStr">
-        <is>
-          <t>4390</t>
+      <c r="S50" t="n">
+        <v>4390</v>
+      </c>
+      <c r="T50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>4598</t>
         </is>
       </c>
     </row>
@@ -3527,9 +3775,15 @@
       <c r="R51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S51" t="inlineStr">
-        <is>
-          <t>3351</t>
+      <c r="S51" t="n">
+        <v>3351</v>
+      </c>
+      <c r="T51" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>3562</t>
         </is>
       </c>
     </row>
@@ -3594,9 +3848,15 @@
       <c r="R52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="S52" t="inlineStr">
-        <is>
-          <t>4413</t>
+      <c r="S52" t="n">
+        <v>4413</v>
+      </c>
+      <c r="T52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>4720</t>
         </is>
       </c>
     </row>
@@ -3661,9 +3921,15 @@
       <c r="R53" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="S53" t="inlineStr">
-        <is>
-          <t>3294</t>
+      <c r="S53" t="n">
+        <v>3294</v>
+      </c>
+      <c r="T53" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>3419</t>
         </is>
       </c>
     </row>
@@ -3728,9 +3994,15 @@
       <c r="R54" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="S54" t="inlineStr">
-        <is>
-          <t>4128</t>
+      <c r="S54" t="n">
+        <v>4128</v>
+      </c>
+      <c r="T54" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="U54" t="inlineStr">
+        <is>
+          <t>4517</t>
         </is>
       </c>
     </row>
@@ -3795,9 +4067,15 @@
       <c r="R55" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S55" t="inlineStr">
-        <is>
-          <t>3314</t>
+      <c r="S55" t="n">
+        <v>3314</v>
+      </c>
+      <c r="T55" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>3487</t>
         </is>
       </c>
     </row>
@@ -3862,9 +4140,15 @@
       <c r="R56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="S56" t="inlineStr">
-        <is>
-          <t>4433</t>
+      <c r="S56" t="n">
+        <v>4433</v>
+      </c>
+      <c r="T56" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t>4909</t>
         </is>
       </c>
     </row>
@@ -3929,9 +4213,15 @@
       <c r="R57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="S57" t="inlineStr">
-        <is>
-          <t>3992</t>
+      <c r="S57" t="n">
+        <v>3992</v>
+      </c>
+      <c r="T57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="U57" t="inlineStr">
+        <is>
+          <t>4118</t>
         </is>
       </c>
     </row>
@@ -3996,9 +4286,15 @@
       <c r="R58" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="S58" t="inlineStr">
-        <is>
-          <t>3958</t>
+      <c r="S58" t="n">
+        <v>3958</v>
+      </c>
+      <c r="T58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="U58" t="inlineStr">
+        <is>
+          <t>4086</t>
         </is>
       </c>
     </row>
@@ -4063,9 +4359,15 @@
       <c r="R59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="S59" t="inlineStr">
-        <is>
-          <t>3895</t>
+      <c r="S59" t="n">
+        <v>3895</v>
+      </c>
+      <c r="T59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="U59" t="inlineStr">
+        <is>
+          <t>3992</t>
         </is>
       </c>
     </row>
@@ -4130,9 +4432,15 @@
       <c r="R60" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="S60" t="inlineStr">
-        <is>
-          <t>4019</t>
+      <c r="S60" t="n">
+        <v>4019</v>
+      </c>
+      <c r="T60" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>4127</t>
         </is>
       </c>
     </row>
@@ -4176,6 +4484,8 @@
       <c r="Q61" t="inlineStr"/>
       <c r="R61" s="4" t="inlineStr"/>
       <c r="S61" t="inlineStr"/>
+      <c r="T61" s="4" t="inlineStr"/>
+      <c r="U61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -4238,9 +4548,15 @@
       <c r="R62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="S62" t="inlineStr">
-        <is>
-          <t>3621</t>
+      <c r="S62" t="n">
+        <v>3621</v>
+      </c>
+      <c r="T62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>3917</t>
         </is>
       </c>
     </row>
@@ -4305,9 +4621,15 @@
       <c r="R63" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="S63" t="inlineStr">
-        <is>
-          <t>3945</t>
+      <c r="S63" t="n">
+        <v>3945</v>
+      </c>
+      <c r="T63" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>3998</t>
         </is>
       </c>
     </row>
@@ -4372,9 +4694,15 @@
       <c r="R64" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="S64" t="inlineStr">
-        <is>
-          <t>3993</t>
+      <c r="S64" t="n">
+        <v>3993</v>
+      </c>
+      <c r="T64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U64" t="inlineStr">
+        <is>
+          <t>4001</t>
         </is>
       </c>
     </row>
@@ -4439,9 +4767,15 @@
       <c r="R65" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="S65" t="inlineStr">
-        <is>
-          <t>3424</t>
+      <c r="S65" t="n">
+        <v>3424</v>
+      </c>
+      <c r="T65" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="U65" t="inlineStr">
+        <is>
+          <t>3693</t>
         </is>
       </c>
     </row>
@@ -4506,7 +4840,13 @@
       <c r="R66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S66" t="inlineStr">
+      <c r="S66" t="n">
+        <v>0</v>
+      </c>
+      <c r="T66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4573,7 +4913,13 @@
       <c r="R67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S67" t="inlineStr">
+      <c r="S67" t="n">
+        <v>0</v>
+      </c>
+      <c r="T67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4640,9 +4986,15 @@
       <c r="R68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S68" t="inlineStr">
-        <is>
-          <t>2495</t>
+      <c r="S68" t="n">
+        <v>2495</v>
+      </c>
+      <c r="T68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U68" t="inlineStr">
+        <is>
+          <t>2502</t>
         </is>
       </c>
     </row>
@@ -4707,9 +5059,15 @@
       <c r="R69" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="S69" t="inlineStr">
-        <is>
-          <t>2934</t>
+      <c r="S69" t="n">
+        <v>2934</v>
+      </c>
+      <c r="T69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U69" t="inlineStr">
+        <is>
+          <t>2957</t>
         </is>
       </c>
     </row>
@@ -4774,9 +5132,15 @@
       <c r="R70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S70" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="S70" t="n">
+        <v>0</v>
+      </c>
+      <c r="T70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U70" t="inlineStr">
+        <is>
+          <t>1523</t>
         </is>
       </c>
     </row>
@@ -4841,7 +5205,13 @@
       <c r="R71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S71" t="inlineStr">
+      <c r="S71" t="n">
+        <v>0</v>
+      </c>
+      <c r="T71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4908,7 +5278,13 @@
       <c r="R72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S72" t="inlineStr">
+      <c r="S72" t="n">
+        <v>0</v>
+      </c>
+      <c r="T72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4975,9 +5351,15 @@
       <c r="R73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S73" t="inlineStr">
-        <is>
-          <t>2600</t>
+      <c r="S73" t="n">
+        <v>2600</v>
+      </c>
+      <c r="T73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U73" t="inlineStr">
+        <is>
+          <t>2582</t>
         </is>
       </c>
     </row>
@@ -5042,7 +5424,13 @@
       <c r="R74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S74" t="inlineStr">
+      <c r="S74" t="n">
+        <v>0</v>
+      </c>
+      <c r="T74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5109,7 +5497,13 @@
       <c r="R75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S75" t="inlineStr">
+      <c r="S75" t="n">
+        <v>0</v>
+      </c>
+      <c r="T75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5176,9 +5570,15 @@
       <c r="R76" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="S76" t="inlineStr">
-        <is>
-          <t>3871</t>
+      <c r="S76" t="n">
+        <v>3871</v>
+      </c>
+      <c r="T76" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="U76" t="inlineStr">
+        <is>
+          <t>4114</t>
         </is>
       </c>
     </row>
@@ -5243,9 +5643,15 @@
       <c r="R77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S77" t="inlineStr">
-        <is>
-          <t>3123</t>
+      <c r="S77" t="n">
+        <v>3123</v>
+      </c>
+      <c r="T77" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="U77" t="inlineStr">
+        <is>
+          <t>3448</t>
         </is>
       </c>
     </row>
@@ -5310,9 +5716,15 @@
       <c r="R78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S78" t="inlineStr">
-        <is>
-          <t>2614</t>
+      <c r="S78" t="n">
+        <v>2614</v>
+      </c>
+      <c r="T78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U78" t="inlineStr">
+        <is>
+          <t>2727</t>
         </is>
       </c>
     </row>
@@ -5377,9 +5789,15 @@
       <c r="R79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S79" t="inlineStr">
-        <is>
-          <t>1280</t>
+      <c r="S79" t="n">
+        <v>1280</v>
+      </c>
+      <c r="T79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U79" t="inlineStr">
+        <is>
+          <t>1276</t>
         </is>
       </c>
     </row>
@@ -5444,7 +5862,13 @@
       <c r="R80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S80" t="inlineStr">
+      <c r="S80" t="n">
+        <v>0</v>
+      </c>
+      <c r="T80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5511,9 +5935,15 @@
       <c r="R81" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="S81" t="inlineStr">
-        <is>
-          <t>2612</t>
+      <c r="S81" t="n">
+        <v>2612</v>
+      </c>
+      <c r="T81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U81" t="inlineStr">
+        <is>
+          <t>2606</t>
         </is>
       </c>
     </row>
@@ -5578,7 +6008,13 @@
       <c r="R82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S82" t="inlineStr">
+      <c r="S82" t="n">
+        <v>0</v>
+      </c>
+      <c r="T82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5645,7 +6081,13 @@
       <c r="R83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S83" t="inlineStr">
+      <c r="S83" t="n">
+        <v>0</v>
+      </c>
+      <c r="T83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5712,9 +6154,15 @@
       <c r="R84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S84" t="inlineStr">
-        <is>
-          <t>1512</t>
+      <c r="S84" t="n">
+        <v>1512</v>
+      </c>
+      <c r="T84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U84" t="inlineStr">
+        <is>
+          <t>1528</t>
         </is>
       </c>
     </row>
@@ -5779,7 +6227,13 @@
       <c r="R85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S85" t="inlineStr">
+      <c r="S85" t="n">
+        <v>0</v>
+      </c>
+      <c r="T85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5846,7 +6300,13 @@
       <c r="R86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S86" t="inlineStr">
+      <c r="S86" t="n">
+        <v>0</v>
+      </c>
+      <c r="T86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5913,7 +6373,13 @@
       <c r="R87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S87" t="inlineStr">
+      <c r="S87" t="n">
+        <v>0</v>
+      </c>
+      <c r="T87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5980,7 +6446,13 @@
       <c r="R88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S88" t="inlineStr">
+      <c r="S88" t="n">
+        <v>0</v>
+      </c>
+      <c r="T88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6047,7 +6519,13 @@
       <c r="R89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S89" t="inlineStr">
+      <c r="S89" t="n">
+        <v>0</v>
+      </c>
+      <c r="T89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6114,7 +6592,13 @@
       <c r="R90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S90" t="inlineStr">
+      <c r="S90" t="n">
+        <v>0</v>
+      </c>
+      <c r="T90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6181,7 +6665,13 @@
       <c r="R91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S91" t="inlineStr">
+      <c r="S91" t="n">
+        <v>0</v>
+      </c>
+      <c r="T91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6248,7 +6738,13 @@
       <c r="R92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S92" t="inlineStr">
+      <c r="S92" t="n">
+        <v>0</v>
+      </c>
+      <c r="T92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6315,7 +6811,13 @@
       <c r="R93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S93" t="inlineStr">
+      <c r="S93" t="n">
+        <v>0</v>
+      </c>
+      <c r="T93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6382,7 +6884,13 @@
       <c r="R94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S94" t="inlineStr">
+      <c r="S94" t="n">
+        <v>0</v>
+      </c>
+      <c r="T94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6449,7 +6957,13 @@
       <c r="R95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S95" t="inlineStr">
+      <c r="S95" t="n">
+        <v>0</v>
+      </c>
+      <c r="T95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6516,9 +7030,15 @@
       <c r="R96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S96" t="inlineStr">
-        <is>
-          <t>2800</t>
+      <c r="S96" t="n">
+        <v>2800</v>
+      </c>
+      <c r="T96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U96" t="inlineStr">
+        <is>
+          <t>2798</t>
         </is>
       </c>
     </row>
@@ -6583,9 +7103,15 @@
       <c r="R97" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="S97" t="inlineStr">
-        <is>
-          <t>1020</t>
+      <c r="S97" t="n">
+        <v>1020</v>
+      </c>
+      <c r="T97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U97" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -6650,7 +7176,13 @@
       <c r="R98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S98" t="inlineStr">
+      <c r="S98" t="n">
+        <v>0</v>
+      </c>
+      <c r="T98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6717,7 +7249,13 @@
       <c r="R99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S99" t="inlineStr">
+      <c r="S99" t="n">
+        <v>0</v>
+      </c>
+      <c r="T99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6784,7 +7322,13 @@
       <c r="R100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S100" t="inlineStr">
+      <c r="S100" t="n">
+        <v>0</v>
+      </c>
+      <c r="T100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6851,7 +7395,13 @@
       <c r="R101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S101" t="inlineStr">
+      <c r="S101" t="n">
+        <v>0</v>
+      </c>
+      <c r="T101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6918,7 +7468,13 @@
       <c r="R102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S102" t="inlineStr">
+      <c r="S102" t="n">
+        <v>0</v>
+      </c>
+      <c r="T102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6985,7 +7541,13 @@
       <c r="R103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S103" t="inlineStr">
+      <c r="S103" t="n">
+        <v>0</v>
+      </c>
+      <c r="T103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7052,7 +7614,13 @@
       <c r="R104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S104" t="inlineStr">
+      <c r="S104" t="n">
+        <v>0</v>
+      </c>
+      <c r="T104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7119,7 +7687,13 @@
       <c r="R105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S105" t="inlineStr">
+      <c r="S105" t="n">
+        <v>0</v>
+      </c>
+      <c r="T105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7157,6 +7731,8 @@
       <c r="Q106" t="inlineStr"/>
       <c r="R106" s="4" t="inlineStr"/>
       <c r="S106" t="inlineStr"/>
+      <c r="T106" s="4" t="inlineStr"/>
+      <c r="U106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -7190,6 +7766,8 @@
       <c r="Q107" t="inlineStr"/>
       <c r="R107" s="4" t="inlineStr"/>
       <c r="S107" t="inlineStr"/>
+      <c r="T107" s="4" t="inlineStr"/>
+      <c r="U107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -7223,6 +7801,8 @@
       <c r="Q108" t="inlineStr"/>
       <c r="R108" s="4" t="inlineStr"/>
       <c r="S108" t="inlineStr"/>
+      <c r="T108" s="4" t="inlineStr"/>
+      <c r="U108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -7256,6 +7836,8 @@
       <c r="Q109" t="inlineStr"/>
       <c r="R109" s="4" t="inlineStr"/>
       <c r="S109" t="inlineStr"/>
+      <c r="T109" s="4" t="inlineStr"/>
+      <c r="U109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -7289,6 +7871,8 @@
       <c r="Q110" t="inlineStr"/>
       <c r="R110" s="4" t="inlineStr"/>
       <c r="S110" t="inlineStr"/>
+      <c r="T110" s="4" t="inlineStr"/>
+      <c r="U110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -7322,6 +7906,8 @@
       <c r="Q111" t="inlineStr"/>
       <c r="R111" s="4" t="inlineStr"/>
       <c r="S111" t="inlineStr"/>
+      <c r="T111" s="4" t="inlineStr"/>
+      <c r="U111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -7355,6 +7941,8 @@
       <c r="Q112" t="inlineStr"/>
       <c r="R112" s="4" t="inlineStr"/>
       <c r="S112" t="inlineStr"/>
+      <c r="T112" s="4" t="inlineStr"/>
+      <c r="U112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -7388,6 +7976,8 @@
       <c r="Q113" t="inlineStr"/>
       <c r="R113" s="4" t="inlineStr"/>
       <c r="S113" t="inlineStr"/>
+      <c r="T113" s="4" t="inlineStr"/>
+      <c r="U113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -7421,6 +8011,8 @@
       <c r="Q114" t="inlineStr"/>
       <c r="R114" s="4" t="inlineStr"/>
       <c r="S114" t="inlineStr"/>
+      <c r="T114" s="4" t="inlineStr"/>
+      <c r="U114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -7473,9 +8065,15 @@
       <c r="R115" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="S115" t="inlineStr">
-        <is>
-          <t>5347</t>
+      <c r="S115" t="n">
+        <v>5347</v>
+      </c>
+      <c r="T115" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="U115" t="inlineStr">
+        <is>
+          <t>6011</t>
         </is>
       </c>
     </row>
@@ -7530,9 +8128,15 @@
       <c r="R116" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="S116" t="inlineStr">
-        <is>
-          <t>4251</t>
+      <c r="S116" t="n">
+        <v>4251</v>
+      </c>
+      <c r="T116" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="U116" t="inlineStr">
+        <is>
+          <t>4944</t>
         </is>
       </c>
     </row>
@@ -7587,9 +8191,15 @@
       <c r="R117" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="S117" t="inlineStr">
-        <is>
-          <t>4287</t>
+      <c r="S117" t="n">
+        <v>4287</v>
+      </c>
+      <c r="T117" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="U117" t="inlineStr">
+        <is>
+          <t>4672</t>
         </is>
       </c>
     </row>
@@ -7644,9 +8254,15 @@
       <c r="R118" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="S118" t="inlineStr">
-        <is>
-          <t>4602</t>
+      <c r="S118" t="n">
+        <v>4602</v>
+      </c>
+      <c r="T118" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="U118" t="inlineStr">
+        <is>
+          <t>5083</t>
         </is>
       </c>
     </row>
@@ -7689,9 +8305,15 @@
       <c r="R119" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="S119" t="inlineStr">
-        <is>
-          <t>1154</t>
+      <c r="S119" t="n">
+        <v>1154</v>
+      </c>
+      <c r="T119" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="U119" t="inlineStr">
+        <is>
+          <t>1574</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-02 04:31:20
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U119"/>
+  <dimension ref="A1:W119"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,6 +496,16 @@
           <t>04-30_0</t>
         </is>
       </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>05-01_A</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>05-01_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -564,7 +574,13 @@
       <c r="T2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="U2" t="n">
+        <v>3083</v>
+      </c>
+      <c r="V2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="inlineStr">
         <is>
           <t>3083</t>
         </is>
@@ -637,7 +653,13 @@
       <c r="T3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -710,7 +732,13 @@
       <c r="T4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U4" t="inlineStr">
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -783,7 +811,13 @@
       <c r="T5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U5" t="inlineStr">
+      <c r="U5" t="n">
+        <v>2512</v>
+      </c>
+      <c r="V5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" t="inlineStr">
         <is>
           <t>2512</t>
         </is>
@@ -856,7 +890,13 @@
       <c r="T6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U6" t="inlineStr">
+      <c r="U6" t="n">
+        <v>2646</v>
+      </c>
+      <c r="V6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="inlineStr">
         <is>
           <t>2646</t>
         </is>
@@ -908,6 +948,8 @@
       <c r="S7" t="inlineStr"/>
       <c r="T7" s="4" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
+      <c r="V7" s="4" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -955,6 +997,8 @@
       <c r="S8" t="inlineStr"/>
       <c r="T8" s="4" t="inlineStr"/>
       <c r="U8" t="inlineStr"/>
+      <c r="V8" s="4" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1002,6 +1046,8 @@
       <c r="S9" t="inlineStr"/>
       <c r="T9" s="4" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
+      <c r="V9" s="4" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1049,6 +1095,8 @@
       <c r="S10" t="inlineStr"/>
       <c r="T10" s="4" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
+      <c r="V10" s="4" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1096,6 +1144,8 @@
       <c r="S11" t="inlineStr"/>
       <c r="T11" s="4" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
+      <c r="V11" s="4" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1143,6 +1193,8 @@
       <c r="S12" t="inlineStr"/>
       <c r="T12" s="4" t="inlineStr"/>
       <c r="U12" t="inlineStr"/>
+      <c r="V12" s="4" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1190,6 +1242,8 @@
       <c r="S13" t="inlineStr"/>
       <c r="T13" s="4" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
+      <c r="V13" s="4" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1237,6 +1291,8 @@
       <c r="S14" t="inlineStr"/>
       <c r="T14" s="4" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
+      <c r="V14" s="4" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1284,6 +1340,8 @@
       <c r="S15" t="inlineStr"/>
       <c r="T15" s="4" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
+      <c r="V15" s="4" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1331,6 +1389,8 @@
       <c r="S16" t="inlineStr"/>
       <c r="T16" s="4" t="inlineStr"/>
       <c r="U16" t="inlineStr"/>
+      <c r="V16" s="4" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1378,6 +1438,8 @@
       <c r="S17" t="inlineStr"/>
       <c r="T17" s="4" t="inlineStr"/>
       <c r="U17" t="inlineStr"/>
+      <c r="V17" s="4" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1446,7 +1508,13 @@
       <c r="T18" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="U18" t="inlineStr">
+      <c r="U18" t="n">
+        <v>3753</v>
+      </c>
+      <c r="V18" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="W18" t="inlineStr">
         <is>
           <t>3753</t>
         </is>
@@ -1519,7 +1587,13 @@
       <c r="T19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U19" t="inlineStr">
+      <c r="U19" t="n">
+        <v>2605</v>
+      </c>
+      <c r="V19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W19" t="inlineStr">
         <is>
           <t>2605</t>
         </is>
@@ -1592,7 +1666,13 @@
       <c r="T20" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="U20" t="inlineStr">
+      <c r="U20" t="n">
+        <v>4080</v>
+      </c>
+      <c r="V20" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="W20" t="inlineStr">
         <is>
           <t>4080</t>
         </is>
@@ -1665,7 +1745,13 @@
       <c r="T21" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="U21" t="inlineStr">
+      <c r="U21" t="n">
+        <v>4577</v>
+      </c>
+      <c r="V21" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="W21" t="inlineStr">
         <is>
           <t>4577</t>
         </is>
@@ -1738,7 +1824,13 @@
       <c r="T22" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="U22" t="inlineStr">
+      <c r="U22" t="n">
+        <v>4541</v>
+      </c>
+      <c r="V22" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="W22" t="inlineStr">
         <is>
           <t>4541</t>
         </is>
@@ -1811,7 +1903,13 @@
       <c r="T23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="U23" t="inlineStr">
+      <c r="U23" t="n">
+        <v>5008</v>
+      </c>
+      <c r="V23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="W23" t="inlineStr">
         <is>
           <t>5008</t>
         </is>
@@ -1884,7 +1982,13 @@
       <c r="T24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="U24" t="inlineStr">
+      <c r="U24" t="n">
+        <v>4596</v>
+      </c>
+      <c r="V24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="W24" t="inlineStr">
         <is>
           <t>4596</t>
         </is>
@@ -1957,7 +2061,13 @@
       <c r="T25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="U25" t="inlineStr">
+      <c r="U25" t="n">
+        <v>4960</v>
+      </c>
+      <c r="V25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="W25" t="inlineStr">
         <is>
           <t>4960</t>
         </is>
@@ -2030,7 +2140,13 @@
       <c r="T26" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="U26" t="inlineStr">
+      <c r="U26" t="n">
+        <v>2778</v>
+      </c>
+      <c r="V26" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="W26" t="inlineStr">
         <is>
           <t>2778</t>
         </is>
@@ -2103,7 +2219,13 @@
       <c r="T27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U27" t="inlineStr">
+      <c r="U27" t="n">
+        <v>2500</v>
+      </c>
+      <c r="V27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2151,6 +2273,8 @@
       <c r="S28" t="inlineStr"/>
       <c r="T28" s="4" t="inlineStr"/>
       <c r="U28" t="inlineStr"/>
+      <c r="V28" s="4" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2219,7 +2343,13 @@
       <c r="T29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U29" t="inlineStr">
+      <c r="U29" t="n">
+        <v>2557</v>
+      </c>
+      <c r="V29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W29" t="inlineStr">
         <is>
           <t>2557</t>
         </is>
@@ -2292,7 +2422,13 @@
       <c r="T30" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="U30" t="inlineStr">
+      <c r="U30" t="n">
+        <v>4832</v>
+      </c>
+      <c r="V30" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="W30" t="inlineStr">
         <is>
           <t>4832</t>
         </is>
@@ -2365,7 +2501,13 @@
       <c r="T31" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="U31" t="inlineStr">
+      <c r="U31" t="n">
+        <v>4782</v>
+      </c>
+      <c r="V31" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="W31" t="inlineStr">
         <is>
           <t>4782</t>
         </is>
@@ -2438,7 +2580,13 @@
       <c r="T32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U32" t="inlineStr">
+      <c r="U32" t="n">
+        <v>2640</v>
+      </c>
+      <c r="V32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" t="inlineStr">
         <is>
           <t>2640</t>
         </is>
@@ -2498,6 +2646,8 @@
       <c r="S33" t="inlineStr"/>
       <c r="T33" s="4" t="inlineStr"/>
       <c r="U33" t="inlineStr"/>
+      <c r="V33" s="4" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2566,7 +2716,13 @@
       <c r="T34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U34" t="inlineStr">
+      <c r="U34" t="n">
+        <v>2500</v>
+      </c>
+      <c r="V34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W34" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2639,7 +2795,13 @@
       <c r="T35" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="U35" t="inlineStr">
+      <c r="U35" t="n">
+        <v>4489</v>
+      </c>
+      <c r="V35" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="W35" t="inlineStr">
         <is>
           <t>4489</t>
         </is>
@@ -2712,7 +2874,13 @@
       <c r="T36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U36" t="inlineStr">
+      <c r="U36" t="n">
+        <v>2731</v>
+      </c>
+      <c r="V36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W36" t="inlineStr">
         <is>
           <t>2731</t>
         </is>
@@ -2785,7 +2953,13 @@
       <c r="T37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="U37" t="inlineStr">
+      <c r="U37" t="n">
+        <v>4364</v>
+      </c>
+      <c r="V37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="W37" t="inlineStr">
         <is>
           <t>4364</t>
         </is>
@@ -2858,7 +3032,13 @@
       <c r="T38" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="U38" t="inlineStr">
+      <c r="U38" t="n">
+        <v>4925</v>
+      </c>
+      <c r="V38" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="W38" t="inlineStr">
         <is>
           <t>4925</t>
         </is>
@@ -2931,7 +3111,13 @@
       <c r="T39" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="U39" t="inlineStr">
+      <c r="U39" t="n">
+        <v>4446</v>
+      </c>
+      <c r="V39" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="W39" t="inlineStr">
         <is>
           <t>4446</t>
         </is>
@@ -3004,7 +3190,13 @@
       <c r="T40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U40" t="inlineStr">
+      <c r="U40" t="n">
+        <v>0</v>
+      </c>
+      <c r="V40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3077,7 +3269,13 @@
       <c r="T41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U41" t="inlineStr">
+      <c r="U41" t="n">
+        <v>4191</v>
+      </c>
+      <c r="V41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W41" t="inlineStr">
         <is>
           <t>4191</t>
         </is>
@@ -3150,7 +3348,13 @@
       <c r="T42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U42" t="inlineStr">
+      <c r="U42" t="n">
+        <v>2900</v>
+      </c>
+      <c r="V42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W42" t="inlineStr">
         <is>
           <t>2900</t>
         </is>
@@ -3202,6 +3406,8 @@
       <c r="S43" t="inlineStr"/>
       <c r="T43" s="4" t="inlineStr"/>
       <c r="U43" t="inlineStr"/>
+      <c r="V43" s="4" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3270,7 +3476,13 @@
       <c r="T44" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="U44" t="inlineStr">
+      <c r="U44" t="n">
+        <v>4860</v>
+      </c>
+      <c r="V44" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="W44" t="inlineStr">
         <is>
           <t>4860</t>
         </is>
@@ -3343,7 +3555,13 @@
       <c r="T45" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="U45" t="inlineStr">
+      <c r="U45" t="n">
+        <v>3982</v>
+      </c>
+      <c r="V45" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="W45" t="inlineStr">
         <is>
           <t>3982</t>
         </is>
@@ -3416,7 +3634,13 @@
       <c r="T46" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="U46" t="inlineStr">
+      <c r="U46" t="n">
+        <v>3767</v>
+      </c>
+      <c r="V46" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="W46" t="inlineStr">
         <is>
           <t>3767</t>
         </is>
@@ -3489,7 +3713,13 @@
       <c r="T47" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="U47" t="inlineStr">
+      <c r="U47" t="n">
+        <v>5050</v>
+      </c>
+      <c r="V47" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="W47" t="inlineStr">
         <is>
           <t>5050</t>
         </is>
@@ -3562,7 +3792,13 @@
       <c r="T48" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="U48" t="inlineStr">
+      <c r="U48" t="n">
+        <v>4658</v>
+      </c>
+      <c r="V48" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="W48" t="inlineStr">
         <is>
           <t>4658</t>
         </is>
@@ -3635,7 +3871,13 @@
       <c r="T49" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="U49" t="inlineStr">
+      <c r="U49" t="n">
+        <v>4454</v>
+      </c>
+      <c r="V49" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="W49" t="inlineStr">
         <is>
           <t>4454</t>
         </is>
@@ -3708,7 +3950,13 @@
       <c r="T50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="U50" t="inlineStr">
+      <c r="U50" t="n">
+        <v>4598</v>
+      </c>
+      <c r="V50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="W50" t="inlineStr">
         <is>
           <t>4598</t>
         </is>
@@ -3781,7 +4029,13 @@
       <c r="T51" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="U51" t="inlineStr">
+      <c r="U51" t="n">
+        <v>3562</v>
+      </c>
+      <c r="V51" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="W51" t="inlineStr">
         <is>
           <t>3562</t>
         </is>
@@ -3854,7 +4108,13 @@
       <c r="T52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="U52" t="inlineStr">
+      <c r="U52" t="n">
+        <v>4720</v>
+      </c>
+      <c r="V52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="W52" t="inlineStr">
         <is>
           <t>4720</t>
         </is>
@@ -3927,7 +4187,13 @@
       <c r="T53" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="U53" t="inlineStr">
+      <c r="U53" t="n">
+        <v>3419</v>
+      </c>
+      <c r="V53" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="W53" t="inlineStr">
         <is>
           <t>3419</t>
         </is>
@@ -4000,7 +4266,13 @@
       <c r="T54" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="U54" t="inlineStr">
+      <c r="U54" t="n">
+        <v>4517</v>
+      </c>
+      <c r="V54" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="W54" t="inlineStr">
         <is>
           <t>4517</t>
         </is>
@@ -4073,7 +4345,13 @@
       <c r="T55" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="U55" t="inlineStr">
+      <c r="U55" t="n">
+        <v>3487</v>
+      </c>
+      <c r="V55" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="W55" t="inlineStr">
         <is>
           <t>3487</t>
         </is>
@@ -4146,7 +4424,13 @@
       <c r="T56" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="U56" t="inlineStr">
+      <c r="U56" t="n">
+        <v>4909</v>
+      </c>
+      <c r="V56" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="W56" t="inlineStr">
         <is>
           <t>4909</t>
         </is>
@@ -4219,7 +4503,13 @@
       <c r="T57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="U57" t="inlineStr">
+      <c r="U57" t="n">
+        <v>4118</v>
+      </c>
+      <c r="V57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="W57" t="inlineStr">
         <is>
           <t>4118</t>
         </is>
@@ -4292,7 +4582,13 @@
       <c r="T58" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="U58" t="inlineStr">
+      <c r="U58" t="n">
+        <v>4086</v>
+      </c>
+      <c r="V58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="W58" t="inlineStr">
         <is>
           <t>4086</t>
         </is>
@@ -4365,7 +4661,13 @@
       <c r="T59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="U59" t="inlineStr">
+      <c r="U59" t="n">
+        <v>3992</v>
+      </c>
+      <c r="V59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="W59" t="inlineStr">
         <is>
           <t>3992</t>
         </is>
@@ -4438,7 +4740,13 @@
       <c r="T60" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="U60" t="inlineStr">
+      <c r="U60" t="n">
+        <v>4127</v>
+      </c>
+      <c r="V60" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="W60" t="inlineStr">
         <is>
           <t>4127</t>
         </is>
@@ -4486,6 +4794,8 @@
       <c r="S61" t="inlineStr"/>
       <c r="T61" s="4" t="inlineStr"/>
       <c r="U61" t="inlineStr"/>
+      <c r="V61" s="4" t="inlineStr"/>
+      <c r="W61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -4554,7 +4864,13 @@
       <c r="T62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="U62" t="inlineStr">
+      <c r="U62" t="n">
+        <v>3917</v>
+      </c>
+      <c r="V62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="W62" t="inlineStr">
         <is>
           <t>3917</t>
         </is>
@@ -4627,7 +4943,13 @@
       <c r="T63" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="U63" t="inlineStr">
+      <c r="U63" t="n">
+        <v>3998</v>
+      </c>
+      <c r="V63" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="W63" t="inlineStr">
         <is>
           <t>3998</t>
         </is>
@@ -4700,7 +5022,13 @@
       <c r="T64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U64" t="inlineStr">
+      <c r="U64" t="n">
+        <v>4001</v>
+      </c>
+      <c r="V64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W64" t="inlineStr">
         <is>
           <t>4001</t>
         </is>
@@ -4773,7 +5101,13 @@
       <c r="T65" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="U65" t="inlineStr">
+      <c r="U65" t="n">
+        <v>3693</v>
+      </c>
+      <c r="V65" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="W65" t="inlineStr">
         <is>
           <t>3693</t>
         </is>
@@ -4846,7 +5180,13 @@
       <c r="T66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U66" t="inlineStr">
+      <c r="U66" t="n">
+        <v>0</v>
+      </c>
+      <c r="V66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4919,7 +5259,13 @@
       <c r="T67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U67" t="inlineStr">
+      <c r="U67" t="n">
+        <v>0</v>
+      </c>
+      <c r="V67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4992,7 +5338,13 @@
       <c r="T68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U68" t="inlineStr">
+      <c r="U68" t="n">
+        <v>2502</v>
+      </c>
+      <c r="V68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W68" t="inlineStr">
         <is>
           <t>2502</t>
         </is>
@@ -5065,7 +5417,13 @@
       <c r="T69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U69" t="inlineStr">
+      <c r="U69" t="n">
+        <v>2957</v>
+      </c>
+      <c r="V69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W69" t="inlineStr">
         <is>
           <t>2957</t>
         </is>
@@ -5138,7 +5496,13 @@
       <c r="T70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U70" t="inlineStr">
+      <c r="U70" t="n">
+        <v>1523</v>
+      </c>
+      <c r="V70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W70" t="inlineStr">
         <is>
           <t>1523</t>
         </is>
@@ -5211,7 +5575,13 @@
       <c r="T71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U71" t="inlineStr">
+      <c r="U71" t="n">
+        <v>0</v>
+      </c>
+      <c r="V71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5284,7 +5654,13 @@
       <c r="T72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U72" t="inlineStr">
+      <c r="U72" t="n">
+        <v>0</v>
+      </c>
+      <c r="V72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5357,7 +5733,13 @@
       <c r="T73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U73" t="inlineStr">
+      <c r="U73" t="n">
+        <v>2582</v>
+      </c>
+      <c r="V73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W73" t="inlineStr">
         <is>
           <t>2582</t>
         </is>
@@ -5430,7 +5812,13 @@
       <c r="T74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U74" t="inlineStr">
+      <c r="U74" t="n">
+        <v>0</v>
+      </c>
+      <c r="V74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5503,7 +5891,13 @@
       <c r="T75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U75" t="inlineStr">
+      <c r="U75" t="n">
+        <v>0</v>
+      </c>
+      <c r="V75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5576,7 +5970,13 @@
       <c r="T76" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="U76" t="inlineStr">
+      <c r="U76" t="n">
+        <v>4114</v>
+      </c>
+      <c r="V76" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="W76" t="inlineStr">
         <is>
           <t>4114</t>
         </is>
@@ -5649,7 +6049,13 @@
       <c r="T77" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="U77" t="inlineStr">
+      <c r="U77" t="n">
+        <v>3448</v>
+      </c>
+      <c r="V77" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="W77" t="inlineStr">
         <is>
           <t>3448</t>
         </is>
@@ -5722,7 +6128,13 @@
       <c r="T78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U78" t="inlineStr">
+      <c r="U78" t="n">
+        <v>2727</v>
+      </c>
+      <c r="V78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W78" t="inlineStr">
         <is>
           <t>2727</t>
         </is>
@@ -5795,7 +6207,13 @@
       <c r="T79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U79" t="inlineStr">
+      <c r="U79" t="n">
+        <v>1276</v>
+      </c>
+      <c r="V79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W79" t="inlineStr">
         <is>
           <t>1276</t>
         </is>
@@ -5868,7 +6286,13 @@
       <c r="T80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U80" t="inlineStr">
+      <c r="U80" t="n">
+        <v>0</v>
+      </c>
+      <c r="V80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5941,7 +6365,13 @@
       <c r="T81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U81" t="inlineStr">
+      <c r="U81" t="n">
+        <v>2606</v>
+      </c>
+      <c r="V81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W81" t="inlineStr">
         <is>
           <t>2606</t>
         </is>
@@ -6014,7 +6444,13 @@
       <c r="T82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U82" t="inlineStr">
+      <c r="U82" t="n">
+        <v>0</v>
+      </c>
+      <c r="V82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6087,7 +6523,13 @@
       <c r="T83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U83" t="inlineStr">
+      <c r="U83" t="n">
+        <v>0</v>
+      </c>
+      <c r="V83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6160,7 +6602,13 @@
       <c r="T84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U84" t="inlineStr">
+      <c r="U84" t="n">
+        <v>1528</v>
+      </c>
+      <c r="V84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W84" t="inlineStr">
         <is>
           <t>1528</t>
         </is>
@@ -6233,7 +6681,13 @@
       <c r="T85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U85" t="inlineStr">
+      <c r="U85" t="n">
+        <v>0</v>
+      </c>
+      <c r="V85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6306,7 +6760,13 @@
       <c r="T86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U86" t="inlineStr">
+      <c r="U86" t="n">
+        <v>0</v>
+      </c>
+      <c r="V86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6379,7 +6839,13 @@
       <c r="T87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U87" t="inlineStr">
+      <c r="U87" t="n">
+        <v>0</v>
+      </c>
+      <c r="V87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6452,7 +6918,13 @@
       <c r="T88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U88" t="inlineStr">
+      <c r="U88" t="n">
+        <v>0</v>
+      </c>
+      <c r="V88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6525,7 +6997,13 @@
       <c r="T89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U89" t="inlineStr">
+      <c r="U89" t="n">
+        <v>0</v>
+      </c>
+      <c r="V89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6598,7 +7076,13 @@
       <c r="T90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U90" t="inlineStr">
+      <c r="U90" t="n">
+        <v>0</v>
+      </c>
+      <c r="V90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6671,7 +7155,13 @@
       <c r="T91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U91" t="inlineStr">
+      <c r="U91" t="n">
+        <v>0</v>
+      </c>
+      <c r="V91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6744,7 +7234,13 @@
       <c r="T92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U92" t="inlineStr">
+      <c r="U92" t="n">
+        <v>0</v>
+      </c>
+      <c r="V92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6817,7 +7313,13 @@
       <c r="T93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U93" t="inlineStr">
+      <c r="U93" t="n">
+        <v>0</v>
+      </c>
+      <c r="V93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6890,7 +7392,13 @@
       <c r="T94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U94" t="inlineStr">
+      <c r="U94" t="n">
+        <v>0</v>
+      </c>
+      <c r="V94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6963,7 +7471,13 @@
       <c r="T95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U95" t="inlineStr">
+      <c r="U95" t="n">
+        <v>0</v>
+      </c>
+      <c r="V95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7036,7 +7550,13 @@
       <c r="T96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U96" t="inlineStr">
+      <c r="U96" t="n">
+        <v>2798</v>
+      </c>
+      <c r="V96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W96" t="inlineStr">
         <is>
           <t>2798</t>
         </is>
@@ -7109,7 +7629,13 @@
       <c r="T97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U97" t="inlineStr">
+      <c r="U97" t="n">
+        <v>0</v>
+      </c>
+      <c r="V97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7182,7 +7708,13 @@
       <c r="T98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U98" t="inlineStr">
+      <c r="U98" t="n">
+        <v>0</v>
+      </c>
+      <c r="V98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7255,7 +7787,13 @@
       <c r="T99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U99" t="inlineStr">
+      <c r="U99" t="n">
+        <v>0</v>
+      </c>
+      <c r="V99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7328,7 +7866,13 @@
       <c r="T100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U100" t="inlineStr">
+      <c r="U100" t="n">
+        <v>0</v>
+      </c>
+      <c r="V100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7401,7 +7945,13 @@
       <c r="T101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U101" t="inlineStr">
+      <c r="U101" t="n">
+        <v>0</v>
+      </c>
+      <c r="V101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7474,7 +8024,13 @@
       <c r="T102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U102" t="inlineStr">
+      <c r="U102" t="n">
+        <v>0</v>
+      </c>
+      <c r="V102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7547,7 +8103,13 @@
       <c r="T103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U103" t="inlineStr">
+      <c r="U103" t="n">
+        <v>0</v>
+      </c>
+      <c r="V103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7620,7 +8182,13 @@
       <c r="T104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U104" t="inlineStr">
+      <c r="U104" t="n">
+        <v>0</v>
+      </c>
+      <c r="V104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7693,7 +8261,13 @@
       <c r="T105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U105" t="inlineStr">
+      <c r="U105" t="n">
+        <v>0</v>
+      </c>
+      <c r="V105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7733,6 +8307,8 @@
       <c r="S106" t="inlineStr"/>
       <c r="T106" s="4" t="inlineStr"/>
       <c r="U106" t="inlineStr"/>
+      <c r="V106" s="4" t="inlineStr"/>
+      <c r="W106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -7768,6 +8344,8 @@
       <c r="S107" t="inlineStr"/>
       <c r="T107" s="4" t="inlineStr"/>
       <c r="U107" t="inlineStr"/>
+      <c r="V107" s="4" t="inlineStr"/>
+      <c r="W107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -7803,6 +8381,8 @@
       <c r="S108" t="inlineStr"/>
       <c r="T108" s="4" t="inlineStr"/>
       <c r="U108" t="inlineStr"/>
+      <c r="V108" s="4" t="inlineStr"/>
+      <c r="W108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -7838,6 +8418,8 @@
       <c r="S109" t="inlineStr"/>
       <c r="T109" s="4" t="inlineStr"/>
       <c r="U109" t="inlineStr"/>
+      <c r="V109" s="4" t="inlineStr"/>
+      <c r="W109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -7873,6 +8455,8 @@
       <c r="S110" t="inlineStr"/>
       <c r="T110" s="4" t="inlineStr"/>
       <c r="U110" t="inlineStr"/>
+      <c r="V110" s="4" t="inlineStr"/>
+      <c r="W110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -7908,6 +8492,8 @@
       <c r="S111" t="inlineStr"/>
       <c r="T111" s="4" t="inlineStr"/>
       <c r="U111" t="inlineStr"/>
+      <c r="V111" s="4" t="inlineStr"/>
+      <c r="W111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -7943,6 +8529,8 @@
       <c r="S112" t="inlineStr"/>
       <c r="T112" s="4" t="inlineStr"/>
       <c r="U112" t="inlineStr"/>
+      <c r="V112" s="4" t="inlineStr"/>
+      <c r="W112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -7978,6 +8566,8 @@
       <c r="S113" t="inlineStr"/>
       <c r="T113" s="4" t="inlineStr"/>
       <c r="U113" t="inlineStr"/>
+      <c r="V113" s="4" t="inlineStr"/>
+      <c r="W113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -8013,6 +8603,8 @@
       <c r="S114" t="inlineStr"/>
       <c r="T114" s="4" t="inlineStr"/>
       <c r="U114" t="inlineStr"/>
+      <c r="V114" s="4" t="inlineStr"/>
+      <c r="W114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -8071,7 +8663,13 @@
       <c r="T115" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="U115" t="inlineStr">
+      <c r="U115" t="n">
+        <v>6011</v>
+      </c>
+      <c r="V115" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="W115" t="inlineStr">
         <is>
           <t>6011</t>
         </is>
@@ -8134,7 +8732,13 @@
       <c r="T116" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="U116" t="inlineStr">
+      <c r="U116" t="n">
+        <v>4944</v>
+      </c>
+      <c r="V116" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="W116" t="inlineStr">
         <is>
           <t>4944</t>
         </is>
@@ -8197,7 +8801,13 @@
       <c r="T117" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="U117" t="inlineStr">
+      <c r="U117" t="n">
+        <v>4672</v>
+      </c>
+      <c r="V117" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="W117" t="inlineStr">
         <is>
           <t>4672</t>
         </is>
@@ -8260,7 +8870,13 @@
       <c r="T118" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="U118" t="inlineStr">
+      <c r="U118" t="n">
+        <v>5083</v>
+      </c>
+      <c r="V118" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="W118" t="inlineStr">
         <is>
           <t>5083</t>
         </is>
@@ -8311,7 +8927,13 @@
       <c r="T119" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="U119" t="inlineStr">
+      <c r="U119" t="n">
+        <v>1574</v>
+      </c>
+      <c r="V119" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="W119" t="inlineStr">
         <is>
           <t>1574</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-05-02 11:30:55
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -819,7 +819,7 @@
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>2512</t>
+          <t>2506</t>
         </is>
       </c>
     </row>
@@ -898,7 +898,7 @@
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>2646</t>
+          <t>2720</t>
         </is>
       </c>
     </row>
@@ -1511,12 +1511,12 @@
       <c r="U18" t="n">
         <v>3753</v>
       </c>
-      <c r="V18" s="4" t="n">
-        <v>20</v>
+      <c r="V18" s="3" t="n">
+        <v>19</v>
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>3753</t>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="W19" t="inlineStr">
         <is>
-          <t>2605</t>
+          <t>2636</t>
         </is>
       </c>
     </row>
@@ -1670,11 +1670,11 @@
         <v>4080</v>
       </c>
       <c r="V20" s="4" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="W20" t="inlineStr">
         <is>
-          <t>4080</t>
+          <t>4213</t>
         </is>
       </c>
     </row>
@@ -1749,11 +1749,11 @@
         <v>4577</v>
       </c>
       <c r="V21" s="5" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="W21" t="inlineStr">
         <is>
-          <t>4577</t>
+          <t>4708</t>
         </is>
       </c>
     </row>
@@ -1828,11 +1828,11 @@
         <v>4541</v>
       </c>
       <c r="V22" s="4" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="W22" t="inlineStr">
         <is>
-          <t>4541</t>
+          <t>4681</t>
         </is>
       </c>
     </row>
@@ -1911,7 +1911,7 @@
       </c>
       <c r="W23" t="inlineStr">
         <is>
-          <t>5008</t>
+          <t>5283</t>
         </is>
       </c>
     </row>
@@ -1990,7 +1990,7 @@
       </c>
       <c r="W24" t="inlineStr">
         <is>
-          <t>4596</t>
+          <t>4832</t>
         </is>
       </c>
     </row>
@@ -2069,7 +2069,7 @@
       </c>
       <c r="W25" t="inlineStr">
         <is>
-          <t>4960</t>
+          <t>5118</t>
         </is>
       </c>
     </row>
@@ -2143,8 +2143,8 @@
       <c r="U26" t="n">
         <v>2778</v>
       </c>
-      <c r="V26" s="3" t="n">
-        <v>3</v>
+      <c r="V26" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="W26" t="inlineStr">
         <is>
@@ -2346,12 +2346,12 @@
       <c r="U29" t="n">
         <v>2557</v>
       </c>
-      <c r="V29" s="2" t="n">
-        <v>0</v>
+      <c r="V29" s="3" t="n">
+        <v>16</v>
       </c>
       <c r="W29" t="inlineStr">
         <is>
-          <t>2557</t>
+          <t>3050</t>
         </is>
       </c>
     </row>
@@ -2425,12 +2425,12 @@
       <c r="U30" t="n">
         <v>4832</v>
       </c>
-      <c r="V30" s="4" t="n">
-        <v>30</v>
+      <c r="V30" s="5" t="n">
+        <v>33</v>
       </c>
       <c r="W30" t="inlineStr">
         <is>
-          <t>4832</t>
+          <t>4956</t>
         </is>
       </c>
     </row>
@@ -2505,11 +2505,11 @@
         <v>4782</v>
       </c>
       <c r="V31" s="5" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W31" t="inlineStr">
         <is>
-          <t>4782</t>
+          <t>4862</t>
         </is>
       </c>
     </row>
@@ -2583,12 +2583,12 @@
       <c r="U32" t="n">
         <v>2640</v>
       </c>
-      <c r="V32" s="2" t="n">
-        <v>0</v>
+      <c r="V32" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="W32" t="inlineStr">
         <is>
-          <t>2640</t>
+          <t>2696</t>
         </is>
       </c>
     </row>
@@ -2803,7 +2803,7 @@
       </c>
       <c r="W35" t="inlineStr">
         <is>
-          <t>4489</t>
+          <t>4601</t>
         </is>
       </c>
     </row>
@@ -2882,7 +2882,7 @@
       </c>
       <c r="W36" t="inlineStr">
         <is>
-          <t>2731</t>
+          <t>2727</t>
         </is>
       </c>
     </row>
@@ -2961,7 +2961,7 @@
       </c>
       <c r="W37" t="inlineStr">
         <is>
-          <t>4364</t>
+          <t>4541</t>
         </is>
       </c>
     </row>
@@ -3035,12 +3035,12 @@
       <c r="U38" t="n">
         <v>4925</v>
       </c>
-      <c r="V38" s="4" t="n">
-        <v>28</v>
+      <c r="V38" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="W38" t="inlineStr">
         <is>
-          <t>4925</t>
+          <t>4918</t>
         </is>
       </c>
     </row>
@@ -3119,7 +3119,7 @@
       </c>
       <c r="W39" t="inlineStr">
         <is>
-          <t>4446</t>
+          <t>4575</t>
         </is>
       </c>
     </row>
@@ -3277,7 +3277,7 @@
       </c>
       <c r="W41" t="inlineStr">
         <is>
-          <t>4191</t>
+          <t>4281</t>
         </is>
       </c>
     </row>
@@ -3356,7 +3356,7 @@
       </c>
       <c r="W42" t="inlineStr">
         <is>
-          <t>2900</t>
+          <t>3044</t>
         </is>
       </c>
     </row>
@@ -3482,10 +3482,8 @@
       <c r="V44" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="W44" t="inlineStr">
-        <is>
-          <t>4860</t>
-        </is>
+      <c r="W44" t="n">
+        <v>4860</v>
       </c>
     </row>
     <row r="45">
@@ -3559,11 +3557,11 @@
         <v>3982</v>
       </c>
       <c r="V45" s="4" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="W45" t="inlineStr">
         <is>
-          <t>3982</t>
+          <t>3987</t>
         </is>
       </c>
     </row>
@@ -3642,7 +3640,7 @@
       </c>
       <c r="W46" t="inlineStr">
         <is>
-          <t>3767</t>
+          <t>3915</t>
         </is>
       </c>
     </row>
@@ -3717,11 +3715,11 @@
         <v>5050</v>
       </c>
       <c r="V47" s="5" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W47" t="inlineStr">
         <is>
-          <t>5050</t>
+          <t>5226</t>
         </is>
       </c>
     </row>
@@ -3795,12 +3793,12 @@
       <c r="U48" t="n">
         <v>4658</v>
       </c>
-      <c r="V48" s="3" t="n">
-        <v>5</v>
+      <c r="V48" s="4" t="n">
+        <v>30</v>
       </c>
       <c r="W48" t="inlineStr">
         <is>
-          <t>4658</t>
+          <t>4817</t>
         </is>
       </c>
     </row>
@@ -3879,7 +3877,7 @@
       </c>
       <c r="W49" t="inlineStr">
         <is>
-          <t>4454</t>
+          <t>4695</t>
         </is>
       </c>
     </row>
@@ -3958,7 +3956,7 @@
       </c>
       <c r="W50" t="inlineStr">
         <is>
-          <t>4598</t>
+          <t>4777</t>
         </is>
       </c>
     </row>
@@ -4033,11 +4031,11 @@
         <v>3562</v>
       </c>
       <c r="V51" s="3" t="n">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="W51" t="inlineStr">
         <is>
-          <t>3562</t>
+          <t>3875</t>
         </is>
       </c>
     </row>
@@ -4116,7 +4114,7 @@
       </c>
       <c r="W52" t="inlineStr">
         <is>
-          <t>4720</t>
+          <t>4949</t>
         </is>
       </c>
     </row>
@@ -4191,11 +4189,11 @@
         <v>3419</v>
       </c>
       <c r="V53" s="3" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="W53" t="inlineStr">
         <is>
-          <t>3419</t>
+          <t>3635</t>
         </is>
       </c>
     </row>
@@ -4274,7 +4272,7 @@
       </c>
       <c r="W54" t="inlineStr">
         <is>
-          <t>4517</t>
+          <t>4623</t>
         </is>
       </c>
     </row>
@@ -4349,11 +4347,11 @@
         <v>3487</v>
       </c>
       <c r="V55" s="3" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="W55" t="inlineStr">
         <is>
-          <t>3487</t>
+          <t>3705</t>
         </is>
       </c>
     </row>
@@ -4428,11 +4426,11 @@
         <v>4909</v>
       </c>
       <c r="V56" s="4" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="W56" t="inlineStr">
         <is>
-          <t>4909</t>
+          <t>5165</t>
         </is>
       </c>
     </row>
@@ -4506,12 +4504,12 @@
       <c r="U57" t="n">
         <v>4118</v>
       </c>
-      <c r="V57" s="4" t="n">
-        <v>20</v>
+      <c r="V57" s="3" t="n">
+        <v>18</v>
       </c>
       <c r="W57" t="inlineStr">
         <is>
-          <t>4118</t>
+          <t>4203</t>
         </is>
       </c>
     </row>
@@ -4590,7 +4588,7 @@
       </c>
       <c r="W58" t="inlineStr">
         <is>
-          <t>4086</t>
+          <t>4106</t>
         </is>
       </c>
     </row>
@@ -4664,12 +4662,12 @@
       <c r="U59" t="n">
         <v>3992</v>
       </c>
-      <c r="V59" s="4" t="n">
-        <v>20</v>
+      <c r="V59" s="3" t="n">
+        <v>18</v>
       </c>
       <c r="W59" t="inlineStr">
         <is>
-          <t>3992</t>
+          <t>4074</t>
         </is>
       </c>
     </row>
@@ -4748,7 +4746,7 @@
       </c>
       <c r="W60" t="inlineStr">
         <is>
-          <t>4127</t>
+          <t>4206</t>
         </is>
       </c>
     </row>
@@ -4872,7 +4870,7 @@
       </c>
       <c r="W62" t="inlineStr">
         <is>
-          <t>3917</t>
+          <t>3988</t>
         </is>
       </c>
     </row>
@@ -4947,11 +4945,11 @@
         <v>3998</v>
       </c>
       <c r="V63" s="4" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="W63" t="inlineStr">
         <is>
-          <t>3998</t>
+          <t>4035</t>
         </is>
       </c>
     </row>
@@ -5025,12 +5023,12 @@
       <c r="U64" t="n">
         <v>4001</v>
       </c>
-      <c r="V64" s="2" t="n">
-        <v>0</v>
+      <c r="V64" s="3" t="n">
+        <v>11</v>
       </c>
       <c r="W64" t="inlineStr">
         <is>
-          <t>4001</t>
+          <t>4143</t>
         </is>
       </c>
     </row>
@@ -5105,11 +5103,11 @@
         <v>3693</v>
       </c>
       <c r="V65" s="4" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="W65" t="inlineStr">
         <is>
-          <t>3693</t>
+          <t>3888</t>
         </is>
       </c>
     </row>
@@ -5425,7 +5423,7 @@
       </c>
       <c r="W69" t="inlineStr">
         <is>
-          <t>2957</t>
+          <t>2956</t>
         </is>
       </c>
     </row>
@@ -5504,7 +5502,7 @@
       </c>
       <c r="W70" t="inlineStr">
         <is>
-          <t>1523</t>
+          <t>1518</t>
         </is>
       </c>
     </row>
@@ -5741,7 +5739,7 @@
       </c>
       <c r="W73" t="inlineStr">
         <is>
-          <t>2582</t>
+          <t>2605</t>
         </is>
       </c>
     </row>
@@ -5976,10 +5974,8 @@
       <c r="V76" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="W76" t="inlineStr">
-        <is>
-          <t>4114</t>
-        </is>
+      <c r="W76" t="n">
+        <v>4114</v>
       </c>
     </row>
     <row r="77">
@@ -6057,7 +6053,7 @@
       </c>
       <c r="W77" t="inlineStr">
         <is>
-          <t>3448</t>
+          <t>3675</t>
         </is>
       </c>
     </row>
@@ -6136,7 +6132,7 @@
       </c>
       <c r="W78" t="inlineStr">
         <is>
-          <t>2727</t>
+          <t>2862</t>
         </is>
       </c>
     </row>
@@ -6215,7 +6211,7 @@
       </c>
       <c r="W79" t="inlineStr">
         <is>
-          <t>1276</t>
+          <t>1306</t>
         </is>
       </c>
     </row>
@@ -6373,7 +6369,7 @@
       </c>
       <c r="W81" t="inlineStr">
         <is>
-          <t>2606</t>
+          <t>2647</t>
         </is>
       </c>
     </row>
@@ -6610,7 +6606,7 @@
       </c>
       <c r="W84" t="inlineStr">
         <is>
-          <t>1528</t>
+          <t>1524</t>
         </is>
       </c>
     </row>
@@ -7558,7 +7554,7 @@
       </c>
       <c r="W96" t="inlineStr">
         <is>
-          <t>2798</t>
+          <t>2790</t>
         </is>
       </c>
     </row>
@@ -8669,10 +8665,8 @@
       <c r="V115" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="W115" t="inlineStr">
-        <is>
-          <t>6011</t>
-        </is>
+      <c r="W115" t="n">
+        <v>6011</v>
       </c>
     </row>
     <row r="116">
@@ -8738,10 +8732,8 @@
       <c r="V116" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="W116" t="inlineStr">
-        <is>
-          <t>4944</t>
-        </is>
+      <c r="W116" t="n">
+        <v>4944</v>
       </c>
     </row>
     <row r="117">
@@ -8807,10 +8799,8 @@
       <c r="V117" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="W117" t="inlineStr">
-        <is>
-          <t>4672</t>
-        </is>
+      <c r="W117" t="n">
+        <v>4672</v>
       </c>
     </row>
     <row r="118">
@@ -8874,11 +8864,11 @@
         <v>5083</v>
       </c>
       <c r="V118" s="4" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="W118" t="inlineStr">
         <is>
-          <t>5083</t>
+          <t>5403</t>
         </is>
       </c>
     </row>
@@ -8930,12 +8920,12 @@
       <c r="U119" t="n">
         <v>1574</v>
       </c>
-      <c r="V119" s="4" t="n">
-        <v>21</v>
+      <c r="V119" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="W119" t="inlineStr">
         <is>
-          <t>1574</t>
+          <t>1609</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-03 18:54:27
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W119"/>
+  <dimension ref="A1:Y120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,6 +506,16 @@
           <t>05-01_0</t>
         </is>
       </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>05-02_A</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>05-02_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -580,7 +590,13 @@
       <c r="V2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="W2" t="n">
+        <v>3083</v>
+      </c>
+      <c r="X2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="inlineStr">
         <is>
           <t>3083</t>
         </is>
@@ -659,7 +675,13 @@
       <c r="V3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W3" t="inlineStr">
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -738,7 +760,13 @@
       <c r="V4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W4" t="inlineStr">
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -817,9 +845,15 @@
       <c r="V5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>2506</t>
+      <c r="W5" t="n">
+        <v>2506</v>
+      </c>
+      <c r="X5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -896,9 +930,15 @@
       <c r="V6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>2720</t>
+      <c r="W6" t="n">
+        <v>2720</v>
+      </c>
+      <c r="X6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>2772</t>
         </is>
       </c>
     </row>
@@ -950,6 +990,8 @@
       <c r="U7" t="inlineStr"/>
       <c r="V7" s="4" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
+      <c r="X7" s="4" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -999,6 +1041,8 @@
       <c r="U8" t="inlineStr"/>
       <c r="V8" s="4" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
+      <c r="X8" s="4" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1048,6 +1092,8 @@
       <c r="U9" t="inlineStr"/>
       <c r="V9" s="4" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
+      <c r="X9" s="4" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1097,6 +1143,8 @@
       <c r="U10" t="inlineStr"/>
       <c r="V10" s="4" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
+      <c r="X10" s="4" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1146,6 +1194,8 @@
       <c r="U11" t="inlineStr"/>
       <c r="V11" s="4" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
+      <c r="X11" s="4" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1195,6 +1245,8 @@
       <c r="U12" t="inlineStr"/>
       <c r="V12" s="4" t="inlineStr"/>
       <c r="W12" t="inlineStr"/>
+      <c r="X12" s="4" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1244,6 +1296,8 @@
       <c r="U13" t="inlineStr"/>
       <c r="V13" s="4" t="inlineStr"/>
       <c r="W13" t="inlineStr"/>
+      <c r="X13" s="4" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1293,6 +1347,8 @@
       <c r="U14" t="inlineStr"/>
       <c r="V14" s="4" t="inlineStr"/>
       <c r="W14" t="inlineStr"/>
+      <c r="X14" s="4" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1342,6 +1398,8 @@
       <c r="U15" t="inlineStr"/>
       <c r="V15" s="4" t="inlineStr"/>
       <c r="W15" t="inlineStr"/>
+      <c r="X15" s="4" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1391,6 +1449,8 @@
       <c r="U16" t="inlineStr"/>
       <c r="V16" s="4" t="inlineStr"/>
       <c r="W16" t="inlineStr"/>
+      <c r="X16" s="4" t="inlineStr"/>
+      <c r="Y16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1440,6 +1500,8 @@
       <c r="U17" t="inlineStr"/>
       <c r="V17" s="4" t="inlineStr"/>
       <c r="W17" t="inlineStr"/>
+      <c r="X17" s="4" t="inlineStr"/>
+      <c r="Y17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1514,9 +1576,15 @@
       <c r="V18" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="W18" t="inlineStr">
-        <is>
-          <t>3995</t>
+      <c r="W18" t="n">
+        <v>3995</v>
+      </c>
+      <c r="X18" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>4066</t>
         </is>
       </c>
     </row>
@@ -1593,9 +1661,15 @@
       <c r="V19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W19" t="inlineStr">
-        <is>
-          <t>2636</t>
+      <c r="W19" t="n">
+        <v>2636</v>
+      </c>
+      <c r="X19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>2652</t>
         </is>
       </c>
     </row>
@@ -1672,9 +1746,15 @@
       <c r="V20" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="W20" t="inlineStr">
-        <is>
-          <t>4213</t>
+      <c r="W20" t="n">
+        <v>4213</v>
+      </c>
+      <c r="X20" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>4365</t>
         </is>
       </c>
     </row>
@@ -1751,9 +1831,15 @@
       <c r="V21" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="W21" t="inlineStr">
-        <is>
-          <t>4708</t>
+      <c r="W21" t="n">
+        <v>4708</v>
+      </c>
+      <c r="X21" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>4912</t>
         </is>
       </c>
     </row>
@@ -1830,9 +1916,15 @@
       <c r="V22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="W22" t="inlineStr">
-        <is>
-          <t>4681</t>
+      <c r="W22" t="n">
+        <v>4681</v>
+      </c>
+      <c r="X22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>4863</t>
         </is>
       </c>
     </row>
@@ -1909,9 +2001,15 @@
       <c r="V23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="W23" t="inlineStr">
-        <is>
-          <t>5283</t>
+      <c r="W23" t="n">
+        <v>5283</v>
+      </c>
+      <c r="X23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>5537</t>
         </is>
       </c>
     </row>
@@ -1988,9 +2086,15 @@
       <c r="V24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="W24" t="inlineStr">
-        <is>
-          <t>4832</t>
+      <c r="W24" t="n">
+        <v>4832</v>
+      </c>
+      <c r="X24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y24" t="inlineStr">
+        <is>
+          <t>4974</t>
         </is>
       </c>
     </row>
@@ -2067,9 +2171,15 @@
       <c r="V25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="W25" t="inlineStr">
-        <is>
-          <t>5118</t>
+      <c r="W25" t="n">
+        <v>5118</v>
+      </c>
+      <c r="X25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y25" t="inlineStr">
+        <is>
+          <t>5288</t>
         </is>
       </c>
     </row>
@@ -2146,9 +2256,15 @@
       <c r="V26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W26" t="inlineStr">
-        <is>
-          <t>2778</t>
+      <c r="W26" t="n">
+        <v>2778</v>
+      </c>
+      <c r="X26" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>2934</t>
         </is>
       </c>
     </row>
@@ -2225,7 +2341,13 @@
       <c r="V27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W27" t="inlineStr">
+      <c r="W27" t="n">
+        <v>2500</v>
+      </c>
+      <c r="X27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y27" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2275,6 +2397,8 @@
       <c r="U28" t="inlineStr"/>
       <c r="V28" s="4" t="inlineStr"/>
       <c r="W28" t="inlineStr"/>
+      <c r="X28" s="4" t="inlineStr"/>
+      <c r="Y28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2349,9 +2473,15 @@
       <c r="V29" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="W29" t="inlineStr">
-        <is>
-          <t>3050</t>
+      <c r="W29" t="n">
+        <v>3050</v>
+      </c>
+      <c r="X29" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>3623</t>
         </is>
       </c>
     </row>
@@ -2428,9 +2558,15 @@
       <c r="V30" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="W30" t="inlineStr">
-        <is>
-          <t>4956</t>
+      <c r="W30" t="n">
+        <v>4956</v>
+      </c>
+      <c r="X30" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>5010</t>
         </is>
       </c>
     </row>
@@ -2507,9 +2643,15 @@
       <c r="V31" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="W31" t="inlineStr">
-        <is>
-          <t>4862</t>
+      <c r="W31" t="n">
+        <v>4862</v>
+      </c>
+      <c r="X31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>4990</t>
         </is>
       </c>
     </row>
@@ -2586,7 +2728,13 @@
       <c r="V32" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="W32" t="inlineStr">
+      <c r="W32" t="n">
+        <v>2696</v>
+      </c>
+      <c r="X32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y32" t="inlineStr">
         <is>
           <t>2696</t>
         </is>
@@ -2648,6 +2796,8 @@
       <c r="U33" t="inlineStr"/>
       <c r="V33" s="4" t="inlineStr"/>
       <c r="W33" t="inlineStr"/>
+      <c r="X33" s="4" t="inlineStr"/>
+      <c r="Y33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2722,7 +2872,13 @@
       <c r="V34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W34" t="inlineStr">
+      <c r="W34" t="n">
+        <v>2500</v>
+      </c>
+      <c r="X34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y34" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2801,9 +2957,15 @@
       <c r="V35" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="W35" t="inlineStr">
-        <is>
-          <t>4601</t>
+      <c r="W35" t="n">
+        <v>4601</v>
+      </c>
+      <c r="X35" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y35" t="inlineStr">
+        <is>
+          <t>4840</t>
         </is>
       </c>
     </row>
@@ -2880,9 +3042,15 @@
       <c r="V36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W36" t="inlineStr">
-        <is>
-          <t>2727</t>
+      <c r="W36" t="n">
+        <v>2727</v>
+      </c>
+      <c r="X36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y36" t="inlineStr">
+        <is>
+          <t>2722</t>
         </is>
       </c>
     </row>
@@ -2959,9 +3127,15 @@
       <c r="V37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="W37" t="inlineStr">
-        <is>
-          <t>4541</t>
+      <c r="W37" t="n">
+        <v>4541</v>
+      </c>
+      <c r="X37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y37" t="inlineStr">
+        <is>
+          <t>4731</t>
         </is>
       </c>
     </row>
@@ -3038,9 +3212,15 @@
       <c r="V38" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W38" t="inlineStr">
-        <is>
-          <t>4918</t>
+      <c r="W38" t="n">
+        <v>4918</v>
+      </c>
+      <c r="X38" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y38" t="inlineStr">
+        <is>
+          <t>5177</t>
         </is>
       </c>
     </row>
@@ -3117,9 +3297,15 @@
       <c r="V39" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="W39" t="inlineStr">
-        <is>
-          <t>4575</t>
+      <c r="W39" t="n">
+        <v>4575</v>
+      </c>
+      <c r="X39" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="Y39" t="inlineStr">
+        <is>
+          <t>4683</t>
         </is>
       </c>
     </row>
@@ -3196,7 +3382,13 @@
       <c r="V40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W40" t="inlineStr">
+      <c r="W40" t="n">
+        <v>0</v>
+      </c>
+      <c r="X40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3275,9 +3467,15 @@
       <c r="V41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W41" t="inlineStr">
-        <is>
-          <t>4281</t>
+      <c r="W41" t="n">
+        <v>4281</v>
+      </c>
+      <c r="X41" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y41" t="inlineStr">
+        <is>
+          <t>4432</t>
         </is>
       </c>
     </row>
@@ -3354,9 +3552,15 @@
       <c r="V42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W42" t="inlineStr">
-        <is>
-          <t>3044</t>
+      <c r="W42" t="n">
+        <v>3044</v>
+      </c>
+      <c r="X42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y42" t="inlineStr">
+        <is>
+          <t>3149</t>
         </is>
       </c>
     </row>
@@ -3408,6 +3612,8 @@
       <c r="U43" t="inlineStr"/>
       <c r="V43" s="4" t="inlineStr"/>
       <c r="W43" t="inlineStr"/>
+      <c r="X43" s="4" t="inlineStr"/>
+      <c r="Y43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3485,6 +3691,8 @@
       <c r="W44" t="n">
         <v>4860</v>
       </c>
+      <c r="X44" s="4" t="inlineStr"/>
+      <c r="Y44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3559,9 +3767,15 @@
       <c r="V45" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="W45" t="inlineStr">
-        <is>
-          <t>3987</t>
+      <c r="W45" t="n">
+        <v>3987</v>
+      </c>
+      <c r="X45" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="Y45" t="inlineStr">
+        <is>
+          <t>4083</t>
         </is>
       </c>
     </row>
@@ -3638,9 +3852,15 @@
       <c r="V46" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="W46" t="inlineStr">
-        <is>
-          <t>3915</t>
+      <c r="W46" t="n">
+        <v>3915</v>
+      </c>
+      <c r="X46" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="Y46" t="inlineStr">
+        <is>
+          <t>4061</t>
         </is>
       </c>
     </row>
@@ -3717,9 +3937,15 @@
       <c r="V47" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="W47" t="inlineStr">
-        <is>
-          <t>5226</t>
+      <c r="W47" t="n">
+        <v>5226</v>
+      </c>
+      <c r="X47" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y47" t="inlineStr">
+        <is>
+          <t>5398</t>
         </is>
       </c>
     </row>
@@ -3796,9 +4022,15 @@
       <c r="V48" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="W48" t="inlineStr">
-        <is>
-          <t>4817</t>
+      <c r="W48" t="n">
+        <v>4817</v>
+      </c>
+      <c r="X48" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y48" t="inlineStr">
+        <is>
+          <t>5246</t>
         </is>
       </c>
     </row>
@@ -3875,9 +4107,15 @@
       <c r="V49" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="W49" t="inlineStr">
-        <is>
-          <t>4695</t>
+      <c r="W49" t="n">
+        <v>4695</v>
+      </c>
+      <c r="X49" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y49" t="inlineStr">
+        <is>
+          <t>4743</t>
         </is>
       </c>
     </row>
@@ -3954,9 +4192,15 @@
       <c r="V50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="W50" t="inlineStr">
-        <is>
-          <t>4777</t>
+      <c r="W50" t="n">
+        <v>4777</v>
+      </c>
+      <c r="X50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y50" t="inlineStr">
+        <is>
+          <t>4982</t>
         </is>
       </c>
     </row>
@@ -4033,9 +4277,15 @@
       <c r="V51" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="W51" t="inlineStr">
-        <is>
-          <t>3875</t>
+      <c r="W51" t="n">
+        <v>3875</v>
+      </c>
+      <c r="X51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y51" t="inlineStr">
+        <is>
+          <t>3922</t>
         </is>
       </c>
     </row>
@@ -4112,9 +4362,15 @@
       <c r="V52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="W52" t="inlineStr">
-        <is>
-          <t>4949</t>
+      <c r="W52" t="n">
+        <v>4949</v>
+      </c>
+      <c r="X52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y52" t="inlineStr">
+        <is>
+          <t>5055</t>
         </is>
       </c>
     </row>
@@ -4191,9 +4447,15 @@
       <c r="V53" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="W53" t="inlineStr">
-        <is>
-          <t>3635</t>
+      <c r="W53" t="n">
+        <v>3635</v>
+      </c>
+      <c r="X53" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y53" t="inlineStr">
+        <is>
+          <t>3751</t>
         </is>
       </c>
     </row>
@@ -4270,9 +4532,15 @@
       <c r="V54" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="W54" t="inlineStr">
-        <is>
-          <t>4623</t>
+      <c r="W54" t="n">
+        <v>4623</v>
+      </c>
+      <c r="X54" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y54" t="inlineStr">
+        <is>
+          <t>4733</t>
         </is>
       </c>
     </row>
@@ -4349,9 +4617,15 @@
       <c r="V55" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="W55" t="inlineStr">
-        <is>
-          <t>3705</t>
+      <c r="W55" t="n">
+        <v>3705</v>
+      </c>
+      <c r="X55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y55" t="inlineStr">
+        <is>
+          <t>3701</t>
         </is>
       </c>
     </row>
@@ -4428,9 +4702,15 @@
       <c r="V56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="W56" t="inlineStr">
-        <is>
-          <t>5165</t>
+      <c r="W56" t="n">
+        <v>5165</v>
+      </c>
+      <c r="X56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y56" t="inlineStr">
+        <is>
+          <t>5232</t>
         </is>
       </c>
     </row>
@@ -4507,9 +4787,15 @@
       <c r="V57" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="W57" t="inlineStr">
-        <is>
-          <t>4203</t>
+      <c r="W57" t="n">
+        <v>4203</v>
+      </c>
+      <c r="X57" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="Y57" t="inlineStr">
+        <is>
+          <t>4201</t>
         </is>
       </c>
     </row>
@@ -4586,9 +4872,15 @@
       <c r="V58" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="W58" t="inlineStr">
-        <is>
-          <t>4106</t>
+      <c r="W58" t="n">
+        <v>4106</v>
+      </c>
+      <c r="X58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y58" t="inlineStr">
+        <is>
+          <t>4186</t>
         </is>
       </c>
     </row>
@@ -4665,9 +4957,15 @@
       <c r="V59" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="W59" t="inlineStr">
-        <is>
-          <t>4074</t>
+      <c r="W59" t="n">
+        <v>4074</v>
+      </c>
+      <c r="X59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y59" t="inlineStr">
+        <is>
+          <t>4131</t>
         </is>
       </c>
     </row>
@@ -4744,9 +5042,15 @@
       <c r="V60" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="W60" t="inlineStr">
-        <is>
-          <t>4206</t>
+      <c r="W60" t="n">
+        <v>4206</v>
+      </c>
+      <c r="X60" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y60" t="inlineStr">
+        <is>
+          <t>4262</t>
         </is>
       </c>
     </row>
@@ -4794,6 +5098,8 @@
       <c r="U61" t="inlineStr"/>
       <c r="V61" s="4" t="inlineStr"/>
       <c r="W61" t="inlineStr"/>
+      <c r="X61" s="4" t="inlineStr"/>
+      <c r="Y61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -4868,9 +5174,15 @@
       <c r="V62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="W62" t="inlineStr">
-        <is>
-          <t>3988</t>
+      <c r="W62" t="n">
+        <v>3988</v>
+      </c>
+      <c r="X62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y62" t="inlineStr">
+        <is>
+          <t>4027</t>
         </is>
       </c>
     </row>
@@ -4947,9 +5259,15 @@
       <c r="V63" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="W63" t="inlineStr">
-        <is>
-          <t>4035</t>
+      <c r="W63" t="n">
+        <v>4035</v>
+      </c>
+      <c r="X63" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y63" t="inlineStr">
+        <is>
+          <t>4105</t>
         </is>
       </c>
     </row>
@@ -5026,9 +5344,15 @@
       <c r="V64" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="W64" t="inlineStr">
-        <is>
-          <t>4143</t>
+      <c r="W64" t="n">
+        <v>4143</v>
+      </c>
+      <c r="X64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y64" t="inlineStr">
+        <is>
+          <t>4133</t>
         </is>
       </c>
     </row>
@@ -5105,9 +5429,15 @@
       <c r="V65" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="W65" t="inlineStr">
-        <is>
-          <t>3888</t>
+      <c r="W65" t="n">
+        <v>3888</v>
+      </c>
+      <c r="X65" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y65" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -5184,7 +5514,13 @@
       <c r="V66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W66" t="inlineStr">
+      <c r="W66" t="n">
+        <v>0</v>
+      </c>
+      <c r="X66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5263,7 +5599,13 @@
       <c r="V67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W67" t="inlineStr">
+      <c r="W67" t="n">
+        <v>0</v>
+      </c>
+      <c r="X67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5342,9 +5684,15 @@
       <c r="V68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W68" t="inlineStr">
-        <is>
-          <t>2502</t>
+      <c r="W68" t="n">
+        <v>2502</v>
+      </c>
+      <c r="X68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y68" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -5421,9 +5769,15 @@
       <c r="V69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W69" t="inlineStr">
-        <is>
-          <t>2956</t>
+      <c r="W69" t="n">
+        <v>2956</v>
+      </c>
+      <c r="X69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y69" t="inlineStr">
+        <is>
+          <t>2963</t>
         </is>
       </c>
     </row>
@@ -5500,9 +5854,15 @@
       <c r="V70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W70" t="inlineStr">
-        <is>
-          <t>1518</t>
+      <c r="W70" t="n">
+        <v>1518</v>
+      </c>
+      <c r="X70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y70" t="inlineStr">
+        <is>
+          <t>1510</t>
         </is>
       </c>
     </row>
@@ -5579,7 +5939,13 @@
       <c r="V71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W71" t="inlineStr">
+      <c r="W71" t="n">
+        <v>0</v>
+      </c>
+      <c r="X71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5658,7 +6024,13 @@
       <c r="V72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W72" t="inlineStr">
+      <c r="W72" t="n">
+        <v>0</v>
+      </c>
+      <c r="X72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5737,9 +6109,15 @@
       <c r="V73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W73" t="inlineStr">
-        <is>
-          <t>2605</t>
+      <c r="W73" t="n">
+        <v>2605</v>
+      </c>
+      <c r="X73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y73" t="inlineStr">
+        <is>
+          <t>2628</t>
         </is>
       </c>
     </row>
@@ -5816,7 +6194,13 @@
       <c r="V74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W74" t="inlineStr">
+      <c r="W74" t="n">
+        <v>0</v>
+      </c>
+      <c r="X74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5895,7 +6279,13 @@
       <c r="V75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W75" t="inlineStr">
+      <c r="W75" t="n">
+        <v>0</v>
+      </c>
+      <c r="X75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5920,7 +6310,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>二馆</t>
+          <t>一馆</t>
         </is>
       </c>
       <c r="F76" s="2" t="n">
@@ -5976,6 +6366,14 @@
       </c>
       <c r="W76" t="n">
         <v>4114</v>
+      </c>
+      <c r="X76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y76" t="inlineStr">
+        <is>
+          <t>4510</t>
+        </is>
       </c>
     </row>
     <row r="77">
@@ -6051,9 +6449,15 @@
       <c r="V77" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="W77" t="inlineStr">
-        <is>
-          <t>3675</t>
+      <c r="W77" t="n">
+        <v>3675</v>
+      </c>
+      <c r="X77" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y77" t="inlineStr">
+        <is>
+          <t>3929</t>
         </is>
       </c>
     </row>
@@ -6130,9 +6534,15 @@
       <c r="V78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W78" t="inlineStr">
-        <is>
-          <t>2862</t>
+      <c r="W78" t="n">
+        <v>2862</v>
+      </c>
+      <c r="X78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y78" t="inlineStr">
+        <is>
+          <t>2909</t>
         </is>
       </c>
     </row>
@@ -6209,9 +6619,15 @@
       <c r="V79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W79" t="inlineStr">
-        <is>
-          <t>1306</t>
+      <c r="W79" t="n">
+        <v>1306</v>
+      </c>
+      <c r="X79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y79" t="inlineStr">
+        <is>
+          <t>1305</t>
         </is>
       </c>
     </row>
@@ -6288,7 +6704,13 @@
       <c r="V80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W80" t="inlineStr">
+      <c r="W80" t="n">
+        <v>0</v>
+      </c>
+      <c r="X80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6367,9 +6789,15 @@
       <c r="V81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W81" t="inlineStr">
-        <is>
-          <t>2647</t>
+      <c r="W81" t="n">
+        <v>2647</v>
+      </c>
+      <c r="X81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y81" t="inlineStr">
+        <is>
+          <t>2642</t>
         </is>
       </c>
     </row>
@@ -6446,7 +6874,13 @@
       <c r="V82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W82" t="inlineStr">
+      <c r="W82" t="n">
+        <v>0</v>
+      </c>
+      <c r="X82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6525,7 +6959,13 @@
       <c r="V83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W83" t="inlineStr">
+      <c r="W83" t="n">
+        <v>0</v>
+      </c>
+      <c r="X83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6604,9 +7044,15 @@
       <c r="V84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W84" t="inlineStr">
-        <is>
-          <t>1524</t>
+      <c r="W84" t="n">
+        <v>1524</v>
+      </c>
+      <c r="X84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y84" t="inlineStr">
+        <is>
+          <t>1515</t>
         </is>
       </c>
     </row>
@@ -6683,7 +7129,13 @@
       <c r="V85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W85" t="inlineStr">
+      <c r="W85" t="n">
+        <v>0</v>
+      </c>
+      <c r="X85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6762,7 +7214,13 @@
       <c r="V86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W86" t="inlineStr">
+      <c r="W86" t="n">
+        <v>0</v>
+      </c>
+      <c r="X86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6841,7 +7299,13 @@
       <c r="V87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W87" t="inlineStr">
+      <c r="W87" t="n">
+        <v>0</v>
+      </c>
+      <c r="X87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6920,7 +7384,13 @@
       <c r="V88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W88" t="inlineStr">
+      <c r="W88" t="n">
+        <v>0</v>
+      </c>
+      <c r="X88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6999,7 +7469,13 @@
       <c r="V89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W89" t="inlineStr">
+      <c r="W89" t="n">
+        <v>0</v>
+      </c>
+      <c r="X89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7078,7 +7554,13 @@
       <c r="V90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W90" t="inlineStr">
+      <c r="W90" t="n">
+        <v>0</v>
+      </c>
+      <c r="X90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7157,7 +7639,13 @@
       <c r="V91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W91" t="inlineStr">
+      <c r="W91" t="n">
+        <v>0</v>
+      </c>
+      <c r="X91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7236,7 +7724,13 @@
       <c r="V92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W92" t="inlineStr">
+      <c r="W92" t="n">
+        <v>0</v>
+      </c>
+      <c r="X92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7315,7 +7809,13 @@
       <c r="V93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W93" t="inlineStr">
+      <c r="W93" t="n">
+        <v>0</v>
+      </c>
+      <c r="X93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7394,7 +7894,13 @@
       <c r="V94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W94" t="inlineStr">
+      <c r="W94" t="n">
+        <v>0</v>
+      </c>
+      <c r="X94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7473,7 +7979,13 @@
       <c r="V95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W95" t="inlineStr">
+      <c r="W95" t="n">
+        <v>0</v>
+      </c>
+      <c r="X95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7552,9 +8064,15 @@
       <c r="V96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W96" t="inlineStr">
-        <is>
-          <t>2790</t>
+      <c r="W96" t="n">
+        <v>2790</v>
+      </c>
+      <c r="X96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y96" t="inlineStr">
+        <is>
+          <t>2785</t>
         </is>
       </c>
     </row>
@@ -7631,7 +8149,13 @@
       <c r="V97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W97" t="inlineStr">
+      <c r="W97" t="n">
+        <v>0</v>
+      </c>
+      <c r="X97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7710,7 +8234,13 @@
       <c r="V98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W98" t="inlineStr">
+      <c r="W98" t="n">
+        <v>0</v>
+      </c>
+      <c r="X98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7789,7 +8319,13 @@
       <c r="V99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W99" t="inlineStr">
+      <c r="W99" t="n">
+        <v>0</v>
+      </c>
+      <c r="X99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7868,7 +8404,13 @@
       <c r="V100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W100" t="inlineStr">
+      <c r="W100" t="n">
+        <v>0</v>
+      </c>
+      <c r="X100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7947,7 +8489,13 @@
       <c r="V101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W101" t="inlineStr">
+      <c r="W101" t="n">
+        <v>0</v>
+      </c>
+      <c r="X101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8026,7 +8574,13 @@
       <c r="V102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W102" t="inlineStr">
+      <c r="W102" t="n">
+        <v>0</v>
+      </c>
+      <c r="X102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8105,7 +8659,13 @@
       <c r="V103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W103" t="inlineStr">
+      <c r="W103" t="n">
+        <v>0</v>
+      </c>
+      <c r="X103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8184,7 +8744,13 @@
       <c r="V104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W104" t="inlineStr">
+      <c r="W104" t="n">
+        <v>0</v>
+      </c>
+      <c r="X104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8263,7 +8829,13 @@
       <c r="V105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W105" t="inlineStr">
+      <c r="W105" t="n">
+        <v>0</v>
+      </c>
+      <c r="X105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8305,6 +8877,8 @@
       <c r="U106" t="inlineStr"/>
       <c r="V106" s="4" t="inlineStr"/>
       <c r="W106" t="inlineStr"/>
+      <c r="X106" s="4" t="inlineStr"/>
+      <c r="Y106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -8342,6 +8916,8 @@
       <c r="U107" t="inlineStr"/>
       <c r="V107" s="4" t="inlineStr"/>
       <c r="W107" t="inlineStr"/>
+      <c r="X107" s="4" t="inlineStr"/>
+      <c r="Y107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -8379,6 +8955,8 @@
       <c r="U108" t="inlineStr"/>
       <c r="V108" s="4" t="inlineStr"/>
       <c r="W108" t="inlineStr"/>
+      <c r="X108" s="4" t="inlineStr"/>
+      <c r="Y108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -8416,6 +8994,8 @@
       <c r="U109" t="inlineStr"/>
       <c r="V109" s="4" t="inlineStr"/>
       <c r="W109" t="inlineStr"/>
+      <c r="X109" s="4" t="inlineStr"/>
+      <c r="Y109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -8453,6 +9033,8 @@
       <c r="U110" t="inlineStr"/>
       <c r="V110" s="4" t="inlineStr"/>
       <c r="W110" t="inlineStr"/>
+      <c r="X110" s="4" t="inlineStr"/>
+      <c r="Y110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -8490,6 +9072,8 @@
       <c r="U111" t="inlineStr"/>
       <c r="V111" s="4" t="inlineStr"/>
       <c r="W111" t="inlineStr"/>
+      <c r="X111" s="4" t="inlineStr"/>
+      <c r="Y111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -8527,6 +9111,8 @@
       <c r="U112" t="inlineStr"/>
       <c r="V112" s="4" t="inlineStr"/>
       <c r="W112" t="inlineStr"/>
+      <c r="X112" s="4" t="inlineStr"/>
+      <c r="Y112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -8564,6 +9150,8 @@
       <c r="U113" t="inlineStr"/>
       <c r="V113" s="4" t="inlineStr"/>
       <c r="W113" t="inlineStr"/>
+      <c r="X113" s="4" t="inlineStr"/>
+      <c r="Y113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -8601,6 +9189,8 @@
       <c r="U114" t="inlineStr"/>
       <c r="V114" s="4" t="inlineStr"/>
       <c r="W114" t="inlineStr"/>
+      <c r="X114" s="4" t="inlineStr"/>
+      <c r="Y114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -8668,6 +9258,8 @@
       <c r="W115" t="n">
         <v>6011</v>
       </c>
+      <c r="X115" s="4" t="inlineStr"/>
+      <c r="Y115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -8735,6 +9327,8 @@
       <c r="W116" t="n">
         <v>4944</v>
       </c>
+      <c r="X116" s="4" t="inlineStr"/>
+      <c r="Y116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -8802,6 +9396,8 @@
       <c r="W117" t="n">
         <v>4672</v>
       </c>
+      <c r="X117" s="4" t="inlineStr"/>
+      <c r="Y117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -8866,9 +9462,15 @@
       <c r="V118" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="W118" t="inlineStr">
-        <is>
-          <t>5403</t>
+      <c r="W118" t="n">
+        <v>5403</v>
+      </c>
+      <c r="X118" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y118" t="inlineStr">
+        <is>
+          <t>5578</t>
         </is>
       </c>
     </row>
@@ -8923,9 +9525,60 @@
       <c r="V119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W119" t="inlineStr">
-        <is>
-          <t>1609</t>
+      <c r="W119" t="n">
+        <v>1609</v>
+      </c>
+      <c r="X119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y119" t="inlineStr">
+        <is>
+          <t>1641</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>59304163</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>Hong</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr"/>
+      <c r="D120" t="inlineStr"/>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F120" s="4" t="inlineStr"/>
+      <c r="G120" t="inlineStr"/>
+      <c r="H120" s="4" t="inlineStr"/>
+      <c r="I120" t="inlineStr"/>
+      <c r="J120" s="4" t="inlineStr"/>
+      <c r="K120" t="inlineStr"/>
+      <c r="L120" s="4" t="inlineStr"/>
+      <c r="M120" t="inlineStr"/>
+      <c r="N120" s="4" t="inlineStr"/>
+      <c r="O120" t="inlineStr"/>
+      <c r="P120" s="4" t="inlineStr"/>
+      <c r="Q120" t="inlineStr"/>
+      <c r="R120" s="4" t="inlineStr"/>
+      <c r="S120" t="inlineStr"/>
+      <c r="T120" s="4" t="inlineStr"/>
+      <c r="U120" t="inlineStr"/>
+      <c r="V120" s="4" t="inlineStr"/>
+      <c r="W120" t="inlineStr"/>
+      <c r="X120" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="Y120" t="inlineStr">
+        <is>
+          <t>1851</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-04 11:02:53
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y120"/>
+  <dimension ref="A1:AA120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,6 +516,16 @@
           <t>05-02_0</t>
         </is>
       </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>05-03_A</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>05-03_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -596,9 +606,15 @@
       <c r="X2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>3083</t>
+      <c r="Y2" t="n">
+        <v>3083</v>
+      </c>
+      <c r="Z2" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>3130</t>
         </is>
       </c>
     </row>
@@ -681,7 +697,13 @@
       <c r="X3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -766,7 +788,13 @@
       <c r="X4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y4" t="inlineStr">
+      <c r="Y4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -851,9 +879,15 @@
       <c r="X5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="Y5" t="n">
+        <v>2499</v>
+      </c>
+      <c r="Z5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>2512</t>
         </is>
       </c>
     </row>
@@ -936,9 +970,15 @@
       <c r="X6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>2772</t>
+      <c r="Y6" t="n">
+        <v>2772</v>
+      </c>
+      <c r="Z6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>2793</t>
         </is>
       </c>
     </row>
@@ -992,6 +1032,8 @@
       <c r="W7" t="inlineStr"/>
       <c r="X7" s="4" t="inlineStr"/>
       <c r="Y7" t="inlineStr"/>
+      <c r="Z7" s="4" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1043,6 +1085,8 @@
       <c r="W8" t="inlineStr"/>
       <c r="X8" s="4" t="inlineStr"/>
       <c r="Y8" t="inlineStr"/>
+      <c r="Z8" s="4" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1094,6 +1138,8 @@
       <c r="W9" t="inlineStr"/>
       <c r="X9" s="4" t="inlineStr"/>
       <c r="Y9" t="inlineStr"/>
+      <c r="Z9" s="4" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1145,6 +1191,8 @@
       <c r="W10" t="inlineStr"/>
       <c r="X10" s="4" t="inlineStr"/>
       <c r="Y10" t="inlineStr"/>
+      <c r="Z10" s="4" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1196,6 +1244,8 @@
       <c r="W11" t="inlineStr"/>
       <c r="X11" s="4" t="inlineStr"/>
       <c r="Y11" t="inlineStr"/>
+      <c r="Z11" s="4" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1247,6 +1297,8 @@
       <c r="W12" t="inlineStr"/>
       <c r="X12" s="4" t="inlineStr"/>
       <c r="Y12" t="inlineStr"/>
+      <c r="Z12" s="4" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1298,6 +1350,8 @@
       <c r="W13" t="inlineStr"/>
       <c r="X13" s="4" t="inlineStr"/>
       <c r="Y13" t="inlineStr"/>
+      <c r="Z13" s="4" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1349,6 +1403,8 @@
       <c r="W14" t="inlineStr"/>
       <c r="X14" s="4" t="inlineStr"/>
       <c r="Y14" t="inlineStr"/>
+      <c r="Z14" s="4" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1400,6 +1456,8 @@
       <c r="W15" t="inlineStr"/>
       <c r="X15" s="4" t="inlineStr"/>
       <c r="Y15" t="inlineStr"/>
+      <c r="Z15" s="4" t="inlineStr"/>
+      <c r="AA15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1451,6 +1509,8 @@
       <c r="W16" t="inlineStr"/>
       <c r="X16" s="4" t="inlineStr"/>
       <c r="Y16" t="inlineStr"/>
+      <c r="Z16" s="4" t="inlineStr"/>
+      <c r="AA16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1502,6 +1562,8 @@
       <c r="W17" t="inlineStr"/>
       <c r="X17" s="4" t="inlineStr"/>
       <c r="Y17" t="inlineStr"/>
+      <c r="Z17" s="4" t="inlineStr"/>
+      <c r="AA17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1582,9 +1644,15 @@
       <c r="X18" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="Y18" t="inlineStr">
-        <is>
-          <t>4066</t>
+      <c r="Y18" t="n">
+        <v>4066</v>
+      </c>
+      <c r="Z18" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>4058</t>
         </is>
       </c>
     </row>
@@ -1667,9 +1735,15 @@
       <c r="X19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y19" t="inlineStr">
-        <is>
-          <t>2652</t>
+      <c r="Y19" t="n">
+        <v>2652</v>
+      </c>
+      <c r="Z19" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>2710</t>
         </is>
       </c>
     </row>
@@ -1752,9 +1826,15 @@
       <c r="X20" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="Y20" t="inlineStr">
-        <is>
-          <t>4365</t>
+      <c r="Y20" t="n">
+        <v>4365</v>
+      </c>
+      <c r="Z20" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>4474</t>
         </is>
       </c>
     </row>
@@ -1837,9 +1917,15 @@
       <c r="X21" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Y21" t="inlineStr">
-        <is>
-          <t>4912</t>
+      <c r="Y21" t="n">
+        <v>4912</v>
+      </c>
+      <c r="Z21" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>5064</t>
         </is>
       </c>
     </row>
@@ -1922,9 +2008,15 @@
       <c r="X22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Y22" t="inlineStr">
-        <is>
-          <t>4863</t>
+      <c r="Y22" t="n">
+        <v>4863</v>
+      </c>
+      <c r="Z22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA22" t="inlineStr">
+        <is>
+          <t>4993</t>
         </is>
       </c>
     </row>
@@ -2007,9 +2099,15 @@
       <c r="X23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="Y23" t="inlineStr">
-        <is>
-          <t>5537</t>
+      <c r="Y23" t="n">
+        <v>5537</v>
+      </c>
+      <c r="Z23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>5742</t>
         </is>
       </c>
     </row>
@@ -2092,9 +2190,15 @@
       <c r="X24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Y24" t="inlineStr">
-        <is>
-          <t>4974</t>
+      <c r="Y24" t="n">
+        <v>4974</v>
+      </c>
+      <c r="Z24" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AA24" t="inlineStr">
+        <is>
+          <t>5289</t>
         </is>
       </c>
     </row>
@@ -2177,9 +2281,15 @@
       <c r="X25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Y25" t="inlineStr">
-        <is>
-          <t>5288</t>
+      <c r="Y25" t="n">
+        <v>5288</v>
+      </c>
+      <c r="Z25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA25" t="inlineStr">
+        <is>
+          <t>5482</t>
         </is>
       </c>
     </row>
@@ -2262,9 +2372,15 @@
       <c r="X26" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="Y26" t="inlineStr">
-        <is>
-          <t>2934</t>
+      <c r="Y26" t="n">
+        <v>2934</v>
+      </c>
+      <c r="Z26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA26" t="inlineStr">
+        <is>
+          <t>2950</t>
         </is>
       </c>
     </row>
@@ -2347,7 +2463,13 @@
       <c r="X27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y27" t="inlineStr">
+      <c r="Y27" t="n">
+        <v>2500</v>
+      </c>
+      <c r="Z27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA27" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -2399,6 +2521,8 @@
       <c r="W28" t="inlineStr"/>
       <c r="X28" s="4" t="inlineStr"/>
       <c r="Y28" t="inlineStr"/>
+      <c r="Z28" s="4" t="inlineStr"/>
+      <c r="AA28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2479,9 +2603,15 @@
       <c r="X29" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="Y29" t="inlineStr">
-        <is>
-          <t>3623</t>
+      <c r="Y29" t="n">
+        <v>3623</v>
+      </c>
+      <c r="Z29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA29" t="inlineStr">
+        <is>
+          <t>3624</t>
         </is>
       </c>
     </row>
@@ -2564,9 +2694,15 @@
       <c r="X30" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="Y30" t="inlineStr">
-        <is>
-          <t>5010</t>
+      <c r="Y30" t="n">
+        <v>5010</v>
+      </c>
+      <c r="Z30" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AA30" t="inlineStr">
+        <is>
+          <t>5134</t>
         </is>
       </c>
     </row>
@@ -2649,9 +2785,15 @@
       <c r="X31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Y31" t="inlineStr">
-        <is>
-          <t>4990</t>
+      <c r="Y31" t="n">
+        <v>4990</v>
+      </c>
+      <c r="Z31" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA31" t="inlineStr">
+        <is>
+          <t>5119</t>
         </is>
       </c>
     </row>
@@ -2734,9 +2876,15 @@
       <c r="X32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y32" t="inlineStr">
-        <is>
-          <t>2696</t>
+      <c r="Y32" t="n">
+        <v>2696</v>
+      </c>
+      <c r="Z32" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA32" t="inlineStr">
+        <is>
+          <t>3337</t>
         </is>
       </c>
     </row>
@@ -2798,6 +2946,8 @@
       <c r="W33" t="inlineStr"/>
       <c r="X33" s="4" t="inlineStr"/>
       <c r="Y33" t="inlineStr"/>
+      <c r="Z33" s="4" t="inlineStr"/>
+      <c r="AA33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2878,9 +3028,15 @@
       <c r="X34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y34" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="Y34" t="n">
+        <v>2500</v>
+      </c>
+      <c r="Z34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA34" t="inlineStr">
+        <is>
+          <t>2530</t>
         </is>
       </c>
     </row>
@@ -2963,9 +3119,15 @@
       <c r="X35" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Y35" t="inlineStr">
-        <is>
-          <t>4840</t>
+      <c r="Y35" t="n">
+        <v>4840</v>
+      </c>
+      <c r="Z35" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA35" t="inlineStr">
+        <is>
+          <t>4981</t>
         </is>
       </c>
     </row>
@@ -3048,9 +3210,15 @@
       <c r="X36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y36" t="inlineStr">
-        <is>
-          <t>2722</t>
+      <c r="Y36" t="n">
+        <v>2722</v>
+      </c>
+      <c r="Z36" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA36" t="inlineStr">
+        <is>
+          <t>3273</t>
         </is>
       </c>
     </row>
@@ -3133,9 +3301,15 @@
       <c r="X37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Y37" t="inlineStr">
-        <is>
-          <t>4731</t>
+      <c r="Y37" t="n">
+        <v>4731</v>
+      </c>
+      <c r="Z37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA37" t="inlineStr">
+        <is>
+          <t>4856</t>
         </is>
       </c>
     </row>
@@ -3218,9 +3392,15 @@
       <c r="X38" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="Y38" t="inlineStr">
-        <is>
-          <t>5177</t>
+      <c r="Y38" t="n">
+        <v>5177</v>
+      </c>
+      <c r="Z38" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA38" t="inlineStr">
+        <is>
+          <t>5399</t>
         </is>
       </c>
     </row>
@@ -3303,9 +3483,15 @@
       <c r="X39" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="Y39" t="inlineStr">
-        <is>
-          <t>4683</t>
+      <c r="Y39" t="n">
+        <v>4683</v>
+      </c>
+      <c r="Z39" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA39" t="inlineStr">
+        <is>
+          <t>4765</t>
         </is>
       </c>
     </row>
@@ -3388,7 +3574,13 @@
       <c r="X40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y40" t="inlineStr">
+      <c r="Y40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3473,9 +3665,15 @@
       <c r="X41" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Y41" t="inlineStr">
-        <is>
-          <t>4432</t>
+      <c r="Y41" t="n">
+        <v>4432</v>
+      </c>
+      <c r="Z41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA41" t="inlineStr">
+        <is>
+          <t>4419</t>
         </is>
       </c>
     </row>
@@ -3558,9 +3756,15 @@
       <c r="X42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y42" t="inlineStr">
-        <is>
-          <t>3149</t>
+      <c r="Y42" t="n">
+        <v>3149</v>
+      </c>
+      <c r="Z42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA42" t="inlineStr">
+        <is>
+          <t>3174</t>
         </is>
       </c>
     </row>
@@ -3614,6 +3818,8 @@
       <c r="W43" t="inlineStr"/>
       <c r="X43" s="4" t="inlineStr"/>
       <c r="Y43" t="inlineStr"/>
+      <c r="Z43" s="4" t="inlineStr"/>
+      <c r="AA43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3693,6 +3899,8 @@
       </c>
       <c r="X44" s="4" t="inlineStr"/>
       <c r="Y44" t="inlineStr"/>
+      <c r="Z44" s="4" t="inlineStr"/>
+      <c r="AA44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3773,9 +3981,15 @@
       <c r="X45" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="Y45" t="inlineStr">
-        <is>
-          <t>4083</t>
+      <c r="Y45" t="n">
+        <v>4083</v>
+      </c>
+      <c r="Z45" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA45" t="inlineStr">
+        <is>
+          <t>4135</t>
         </is>
       </c>
     </row>
@@ -3858,9 +4072,15 @@
       <c r="X46" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="Y46" t="inlineStr">
-        <is>
-          <t>4061</t>
+      <c r="Y46" t="n">
+        <v>4061</v>
+      </c>
+      <c r="Z46" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA46" t="inlineStr">
+        <is>
+          <t>4281</t>
         </is>
       </c>
     </row>
@@ -3943,9 +4163,15 @@
       <c r="X47" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Y47" t="inlineStr">
-        <is>
-          <t>5398</t>
+      <c r="Y47" t="n">
+        <v>5398</v>
+      </c>
+      <c r="Z47" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA47" t="inlineStr">
+        <is>
+          <t>5572</t>
         </is>
       </c>
     </row>
@@ -4028,9 +4254,15 @@
       <c r="X48" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Y48" t="inlineStr">
-        <is>
-          <t>5246</t>
+      <c r="Y48" t="n">
+        <v>5246</v>
+      </c>
+      <c r="Z48" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA48" t="inlineStr">
+        <is>
+          <t>5350</t>
         </is>
       </c>
     </row>
@@ -4113,9 +4345,15 @@
       <c r="X49" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Y49" t="inlineStr">
-        <is>
-          <t>4743</t>
+      <c r="Y49" t="n">
+        <v>4743</v>
+      </c>
+      <c r="Z49" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA49" t="inlineStr">
+        <is>
+          <t>4835</t>
         </is>
       </c>
     </row>
@@ -4198,9 +4436,15 @@
       <c r="X50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="Y50" t="inlineStr">
-        <is>
-          <t>4982</t>
+      <c r="Y50" t="n">
+        <v>4982</v>
+      </c>
+      <c r="Z50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA50" t="inlineStr">
+        <is>
+          <t>5115</t>
         </is>
       </c>
     </row>
@@ -4283,9 +4527,15 @@
       <c r="X51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y51" t="inlineStr">
-        <is>
-          <t>3922</t>
+      <c r="Y51" t="n">
+        <v>3922</v>
+      </c>
+      <c r="Z51" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA51" t="inlineStr">
+        <is>
+          <t>4390</t>
         </is>
       </c>
     </row>
@@ -4368,9 +4618,15 @@
       <c r="X52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Y52" t="inlineStr">
-        <is>
-          <t>5055</t>
+      <c r="Y52" t="n">
+        <v>5055</v>
+      </c>
+      <c r="Z52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA52" t="inlineStr">
+        <is>
+          <t>5345</t>
         </is>
       </c>
     </row>
@@ -4453,9 +4709,15 @@
       <c r="X53" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="Y53" t="inlineStr">
-        <is>
-          <t>3751</t>
+      <c r="Y53" t="n">
+        <v>3751</v>
+      </c>
+      <c r="Z53" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA53" t="inlineStr">
+        <is>
+          <t>3959</t>
         </is>
       </c>
     </row>
@@ -4538,9 +4800,15 @@
       <c r="X54" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Y54" t="inlineStr">
-        <is>
-          <t>4733</t>
+      <c r="Y54" t="n">
+        <v>4733</v>
+      </c>
+      <c r="Z54" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA54" t="inlineStr">
+        <is>
+          <t>4884</t>
         </is>
       </c>
     </row>
@@ -4623,9 +4891,15 @@
       <c r="X55" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y55" t="inlineStr">
-        <is>
-          <t>3701</t>
+      <c r="Y55" t="n">
+        <v>3701</v>
+      </c>
+      <c r="Z55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA55" t="inlineStr">
+        <is>
+          <t>3703</t>
         </is>
       </c>
     </row>
@@ -4708,9 +4982,15 @@
       <c r="X56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Y56" t="inlineStr">
-        <is>
-          <t>5232</t>
+      <c r="Y56" t="n">
+        <v>5232</v>
+      </c>
+      <c r="Z56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA56" t="inlineStr">
+        <is>
+          <t>5366</t>
         </is>
       </c>
     </row>
@@ -4793,9 +5073,15 @@
       <c r="X57" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="Y57" t="inlineStr">
-        <is>
-          <t>4201</t>
+      <c r="Y57" t="n">
+        <v>4201</v>
+      </c>
+      <c r="Z57" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="AA57" t="inlineStr">
+        <is>
+          <t>4298</t>
         </is>
       </c>
     </row>
@@ -4878,9 +5164,15 @@
       <c r="X58" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="Y58" t="inlineStr">
-        <is>
-          <t>4186</t>
+      <c r="Y58" t="n">
+        <v>4186</v>
+      </c>
+      <c r="Z58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA58" t="inlineStr">
+        <is>
+          <t>4391</t>
         </is>
       </c>
     </row>
@@ -4963,9 +5255,15 @@
       <c r="X59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Y59" t="inlineStr">
-        <is>
-          <t>4131</t>
+      <c r="Y59" t="n">
+        <v>4131</v>
+      </c>
+      <c r="Z59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA59" t="inlineStr">
+        <is>
+          <t>4256</t>
         </is>
       </c>
     </row>
@@ -5048,9 +5346,15 @@
       <c r="X60" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Y60" t="inlineStr">
-        <is>
-          <t>4262</t>
+      <c r="Y60" t="n">
+        <v>4262</v>
+      </c>
+      <c r="Z60" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA60" t="inlineStr">
+        <is>
+          <t>4328</t>
         </is>
       </c>
     </row>
@@ -5100,6 +5404,8 @@
       <c r="W61" t="inlineStr"/>
       <c r="X61" s="4" t="inlineStr"/>
       <c r="Y61" t="inlineStr"/>
+      <c r="Z61" s="4" t="inlineStr"/>
+      <c r="AA61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -5180,9 +5486,15 @@
       <c r="X62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Y62" t="inlineStr">
-        <is>
-          <t>4027</t>
+      <c r="Y62" t="n">
+        <v>4027</v>
+      </c>
+      <c r="Z62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA62" t="inlineStr">
+        <is>
+          <t>3994</t>
         </is>
       </c>
     </row>
@@ -5265,9 +5577,15 @@
       <c r="X63" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Y63" t="inlineStr">
-        <is>
-          <t>4105</t>
+      <c r="Y63" t="n">
+        <v>4105</v>
+      </c>
+      <c r="Z63" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA63" t="inlineStr">
+        <is>
+          <t>4146</t>
         </is>
       </c>
     </row>
@@ -5350,9 +5668,15 @@
       <c r="X64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y64" t="inlineStr">
-        <is>
-          <t>4133</t>
+      <c r="Y64" t="n">
+        <v>4133</v>
+      </c>
+      <c r="Z64" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="AA64" t="inlineStr">
+        <is>
+          <t>4267</t>
         </is>
       </c>
     </row>
@@ -5435,9 +5759,15 @@
       <c r="X65" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="Y65" t="inlineStr">
-        <is>
-          <t>3995</t>
+      <c r="Y65" t="n">
+        <v>3995</v>
+      </c>
+      <c r="Z65" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA65" t="inlineStr">
+        <is>
+          <t>3996</t>
         </is>
       </c>
     </row>
@@ -5520,7 +5850,13 @@
       <c r="X66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y66" t="inlineStr">
+      <c r="Y66" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5605,7 +5941,13 @@
       <c r="X67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y67" t="inlineStr">
+      <c r="Y67" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5690,9 +6032,15 @@
       <c r="X68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y68" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="Y68" t="n">
+        <v>2499</v>
+      </c>
+      <c r="Z68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA68" t="inlineStr">
+        <is>
+          <t>2496</t>
         </is>
       </c>
     </row>
@@ -5775,9 +6123,15 @@
       <c r="X69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y69" t="inlineStr">
-        <is>
-          <t>2963</t>
+      <c r="Y69" t="n">
+        <v>2963</v>
+      </c>
+      <c r="Z69" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AA69" t="inlineStr">
+        <is>
+          <t>3034</t>
         </is>
       </c>
     </row>
@@ -5860,9 +6214,15 @@
       <c r="X70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y70" t="inlineStr">
-        <is>
-          <t>1510</t>
+      <c r="Y70" t="n">
+        <v>1510</v>
+      </c>
+      <c r="Z70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA70" t="inlineStr">
+        <is>
+          <t>1504</t>
         </is>
       </c>
     </row>
@@ -5945,7 +6305,13 @@
       <c r="X71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y71" t="inlineStr">
+      <c r="Y71" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6030,7 +6396,13 @@
       <c r="X72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y72" t="inlineStr">
+      <c r="Y72" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6115,9 +6487,15 @@
       <c r="X73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y73" t="inlineStr">
-        <is>
-          <t>2628</t>
+      <c r="Y73" t="n">
+        <v>2628</v>
+      </c>
+      <c r="Z73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA73" t="inlineStr">
+        <is>
+          <t>2625</t>
         </is>
       </c>
     </row>
@@ -6200,7 +6578,13 @@
       <c r="X74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y74" t="inlineStr">
+      <c r="Y74" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6285,7 +6669,13 @@
       <c r="X75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y75" t="inlineStr">
+      <c r="Y75" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6370,9 +6760,15 @@
       <c r="X76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y76" t="inlineStr">
-        <is>
-          <t>4510</t>
+      <c r="Y76" t="n">
+        <v>4510</v>
+      </c>
+      <c r="Z76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA76" t="inlineStr">
+        <is>
+          <t>4514</t>
         </is>
       </c>
     </row>
@@ -6455,9 +6851,15 @@
       <c r="X77" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Y77" t="inlineStr">
-        <is>
-          <t>3929</t>
+      <c r="Y77" t="n">
+        <v>3929</v>
+      </c>
+      <c r="Z77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA77" t="inlineStr">
+        <is>
+          <t>3947</t>
         </is>
       </c>
     </row>
@@ -6540,9 +6942,15 @@
       <c r="X78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y78" t="inlineStr">
-        <is>
-          <t>2909</t>
+      <c r="Y78" t="n">
+        <v>2909</v>
+      </c>
+      <c r="Z78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA78" t="inlineStr">
+        <is>
+          <t>3004</t>
         </is>
       </c>
     </row>
@@ -6625,9 +7033,15 @@
       <c r="X79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y79" t="inlineStr">
-        <is>
-          <t>1305</t>
+      <c r="Y79" t="n">
+        <v>1305</v>
+      </c>
+      <c r="Z79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA79" t="inlineStr">
+        <is>
+          <t>1302</t>
         </is>
       </c>
     </row>
@@ -6710,9 +7124,15 @@
       <c r="X80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y80" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="Y80" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA80" t="inlineStr">
+        <is>
+          <t>1428</t>
         </is>
       </c>
     </row>
@@ -6795,9 +7215,15 @@
       <c r="X81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y81" t="inlineStr">
-        <is>
-          <t>2642</t>
+      <c r="Y81" t="n">
+        <v>2642</v>
+      </c>
+      <c r="Z81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA81" t="inlineStr">
+        <is>
+          <t>2687</t>
         </is>
       </c>
     </row>
@@ -6880,7 +7306,13 @@
       <c r="X82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y82" t="inlineStr">
+      <c r="Y82" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6965,7 +7397,13 @@
       <c r="X83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y83" t="inlineStr">
+      <c r="Y83" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7050,9 +7488,15 @@
       <c r="X84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y84" t="inlineStr">
-        <is>
-          <t>1515</t>
+      <c r="Y84" t="n">
+        <v>1515</v>
+      </c>
+      <c r="Z84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA84" t="inlineStr">
+        <is>
+          <t>1507</t>
         </is>
       </c>
     </row>
@@ -7135,7 +7579,13 @@
       <c r="X85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y85" t="inlineStr">
+      <c r="Y85" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7220,7 +7670,13 @@
       <c r="X86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y86" t="inlineStr">
+      <c r="Y86" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7305,7 +7761,13 @@
       <c r="X87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y87" t="inlineStr">
+      <c r="Y87" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7390,7 +7852,13 @@
       <c r="X88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y88" t="inlineStr">
+      <c r="Y88" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7475,7 +7943,13 @@
       <c r="X89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y89" t="inlineStr">
+      <c r="Y89" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7560,7 +8034,13 @@
       <c r="X90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y90" t="inlineStr">
+      <c r="Y90" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7645,7 +8125,13 @@
       <c r="X91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y91" t="inlineStr">
+      <c r="Y91" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7730,7 +8216,13 @@
       <c r="X92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y92" t="inlineStr">
+      <c r="Y92" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7815,7 +8307,13 @@
       <c r="X93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y93" t="inlineStr">
+      <c r="Y93" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7900,7 +8398,13 @@
       <c r="X94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y94" t="inlineStr">
+      <c r="Y94" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7985,7 +8489,13 @@
       <c r="X95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y95" t="inlineStr">
+      <c r="Y95" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8070,9 +8580,15 @@
       <c r="X96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y96" t="inlineStr">
-        <is>
-          <t>2785</t>
+      <c r="Y96" t="n">
+        <v>2785</v>
+      </c>
+      <c r="Z96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA96" t="inlineStr">
+        <is>
+          <t>2798</t>
         </is>
       </c>
     </row>
@@ -8155,7 +8671,13 @@
       <c r="X97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y97" t="inlineStr">
+      <c r="Y97" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8240,7 +8762,13 @@
       <c r="X98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y98" t="inlineStr">
+      <c r="Y98" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8325,7 +8853,13 @@
       <c r="X99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y99" t="inlineStr">
+      <c r="Y99" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8410,7 +8944,13 @@
       <c r="X100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y100" t="inlineStr">
+      <c r="Y100" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8495,7 +9035,13 @@
       <c r="X101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y101" t="inlineStr">
+      <c r="Y101" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8580,7 +9126,13 @@
       <c r="X102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y102" t="inlineStr">
+      <c r="Y102" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8665,7 +9217,13 @@
       <c r="X103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y103" t="inlineStr">
+      <c r="Y103" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8750,7 +9308,13 @@
       <c r="X104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y104" t="inlineStr">
+      <c r="Y104" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8835,7 +9399,13 @@
       <c r="X105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y105" t="inlineStr">
+      <c r="Y105" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8879,6 +9449,8 @@
       <c r="W106" t="inlineStr"/>
       <c r="X106" s="4" t="inlineStr"/>
       <c r="Y106" t="inlineStr"/>
+      <c r="Z106" s="4" t="inlineStr"/>
+      <c r="AA106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -8918,6 +9490,8 @@
       <c r="W107" t="inlineStr"/>
       <c r="X107" s="4" t="inlineStr"/>
       <c r="Y107" t="inlineStr"/>
+      <c r="Z107" s="4" t="inlineStr"/>
+      <c r="AA107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -8957,6 +9531,8 @@
       <c r="W108" t="inlineStr"/>
       <c r="X108" s="4" t="inlineStr"/>
       <c r="Y108" t="inlineStr"/>
+      <c r="Z108" s="4" t="inlineStr"/>
+      <c r="AA108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -8996,6 +9572,8 @@
       <c r="W109" t="inlineStr"/>
       <c r="X109" s="4" t="inlineStr"/>
       <c r="Y109" t="inlineStr"/>
+      <c r="Z109" s="4" t="inlineStr"/>
+      <c r="AA109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -9035,6 +9613,8 @@
       <c r="W110" t="inlineStr"/>
       <c r="X110" s="4" t="inlineStr"/>
       <c r="Y110" t="inlineStr"/>
+      <c r="Z110" s="4" t="inlineStr"/>
+      <c r="AA110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -9074,6 +9654,8 @@
       <c r="W111" t="inlineStr"/>
       <c r="X111" s="4" t="inlineStr"/>
       <c r="Y111" t="inlineStr"/>
+      <c r="Z111" s="4" t="inlineStr"/>
+      <c r="AA111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -9113,6 +9695,8 @@
       <c r="W112" t="inlineStr"/>
       <c r="X112" s="4" t="inlineStr"/>
       <c r="Y112" t="inlineStr"/>
+      <c r="Z112" s="4" t="inlineStr"/>
+      <c r="AA112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -9152,6 +9736,8 @@
       <c r="W113" t="inlineStr"/>
       <c r="X113" s="4" t="inlineStr"/>
       <c r="Y113" t="inlineStr"/>
+      <c r="Z113" s="4" t="inlineStr"/>
+      <c r="AA113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -9191,6 +9777,8 @@
       <c r="W114" t="inlineStr"/>
       <c r="X114" s="4" t="inlineStr"/>
       <c r="Y114" t="inlineStr"/>
+      <c r="Z114" s="4" t="inlineStr"/>
+      <c r="AA114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -9260,6 +9848,8 @@
       </c>
       <c r="X115" s="4" t="inlineStr"/>
       <c r="Y115" t="inlineStr"/>
+      <c r="Z115" s="4" t="inlineStr"/>
+      <c r="AA115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -9329,6 +9919,8 @@
       </c>
       <c r="X116" s="4" t="inlineStr"/>
       <c r="Y116" t="inlineStr"/>
+      <c r="Z116" s="4" t="inlineStr"/>
+      <c r="AA116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -9398,6 +9990,8 @@
       </c>
       <c r="X117" s="4" t="inlineStr"/>
       <c r="Y117" t="inlineStr"/>
+      <c r="Z117" s="4" t="inlineStr"/>
+      <c r="AA117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -9468,9 +10062,15 @@
       <c r="X118" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Y118" t="inlineStr">
-        <is>
-          <t>5578</t>
+      <c r="Y118" t="n">
+        <v>5578</v>
+      </c>
+      <c r="Z118" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA118" t="inlineStr">
+        <is>
+          <t>5815</t>
         </is>
       </c>
     </row>
@@ -9531,17 +10131,21 @@
       <c r="X119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y119" t="inlineStr">
-        <is>
-          <t>1641</t>
+      <c r="Y119" t="n">
+        <v>1641</v>
+      </c>
+      <c r="Z119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA119" t="inlineStr">
+        <is>
+          <t>1636</t>
         </is>
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>59304163</t>
-        </is>
+      <c r="A120" t="n">
+        <v>59304163</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
@@ -9576,9 +10180,15 @@
       <c r="X120" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="Y120" t="inlineStr">
-        <is>
-          <t>1851</t>
+      <c r="Y120" t="n">
+        <v>1851</v>
+      </c>
+      <c r="Z120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA120" t="inlineStr">
+        <is>
+          <t>1862</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-05 11:30:54
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA120"/>
+  <dimension ref="A1:AC120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,6 +526,16 @@
           <t>05-03_0</t>
         </is>
       </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>05-04_A</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>05-04_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -612,7 +622,13 @@
       <c r="Z2" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="AA2" t="inlineStr">
+      <c r="AA2" t="n">
+        <v>3130</v>
+      </c>
+      <c r="AB2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="inlineStr">
         <is>
           <t>3130</t>
         </is>
@@ -703,7 +719,13 @@
       <c r="Z3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA3" t="inlineStr">
+      <c r="AA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -794,7 +816,13 @@
       <c r="Z4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA4" t="inlineStr">
+      <c r="AA4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -885,9 +913,15 @@
       <c r="Z5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>2512</t>
+      <c r="AA5" t="n">
+        <v>2512</v>
+      </c>
+      <c r="AB5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>2528</t>
         </is>
       </c>
     </row>
@@ -976,9 +1010,15 @@
       <c r="Z6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>2793</t>
+      <c r="AA6" t="n">
+        <v>2793</v>
+      </c>
+      <c r="AB6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>2792</t>
         </is>
       </c>
     </row>
@@ -1034,6 +1074,8 @@
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" s="4" t="inlineStr"/>
       <c r="AA7" t="inlineStr"/>
+      <c r="AB7" s="4" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1087,6 +1129,8 @@
       <c r="Y8" t="inlineStr"/>
       <c r="Z8" s="4" t="inlineStr"/>
       <c r="AA8" t="inlineStr"/>
+      <c r="AB8" s="4" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1140,6 +1184,8 @@
       <c r="Y9" t="inlineStr"/>
       <c r="Z9" s="4" t="inlineStr"/>
       <c r="AA9" t="inlineStr"/>
+      <c r="AB9" s="4" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1193,6 +1239,8 @@
       <c r="Y10" t="inlineStr"/>
       <c r="Z10" s="4" t="inlineStr"/>
       <c r="AA10" t="inlineStr"/>
+      <c r="AB10" s="4" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1246,6 +1294,8 @@
       <c r="Y11" t="inlineStr"/>
       <c r="Z11" s="4" t="inlineStr"/>
       <c r="AA11" t="inlineStr"/>
+      <c r="AB11" s="4" t="inlineStr"/>
+      <c r="AC11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1299,6 +1349,8 @@
       <c r="Y12" t="inlineStr"/>
       <c r="Z12" s="4" t="inlineStr"/>
       <c r="AA12" t="inlineStr"/>
+      <c r="AB12" s="4" t="inlineStr"/>
+      <c r="AC12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1352,6 +1404,8 @@
       <c r="Y13" t="inlineStr"/>
       <c r="Z13" s="4" t="inlineStr"/>
       <c r="AA13" t="inlineStr"/>
+      <c r="AB13" s="4" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1405,6 +1459,8 @@
       <c r="Y14" t="inlineStr"/>
       <c r="Z14" s="4" t="inlineStr"/>
       <c r="AA14" t="inlineStr"/>
+      <c r="AB14" s="4" t="inlineStr"/>
+      <c r="AC14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1458,6 +1514,8 @@
       <c r="Y15" t="inlineStr"/>
       <c r="Z15" s="4" t="inlineStr"/>
       <c r="AA15" t="inlineStr"/>
+      <c r="AB15" s="4" t="inlineStr"/>
+      <c r="AC15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1511,6 +1569,8 @@
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" s="4" t="inlineStr"/>
       <c r="AA16" t="inlineStr"/>
+      <c r="AB16" s="4" t="inlineStr"/>
+      <c r="AC16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1564,6 +1624,8 @@
       <c r="Y17" t="inlineStr"/>
       <c r="Z17" s="4" t="inlineStr"/>
       <c r="AA17" t="inlineStr"/>
+      <c r="AB17" s="4" t="inlineStr"/>
+      <c r="AC17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1650,9 +1712,15 @@
       <c r="Z18" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="AA18" t="inlineStr">
-        <is>
-          <t>4058</t>
+      <c r="AA18" t="n">
+        <v>4058</v>
+      </c>
+      <c r="AB18" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>4116</t>
         </is>
       </c>
     </row>
@@ -1741,9 +1809,15 @@
       <c r="Z19" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="AA19" t="inlineStr">
-        <is>
-          <t>2710</t>
+      <c r="AA19" t="n">
+        <v>2710</v>
+      </c>
+      <c r="AB19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>2758</t>
         </is>
       </c>
     </row>
@@ -1832,9 +1906,15 @@
       <c r="Z20" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AA20" t="inlineStr">
-        <is>
-          <t>4474</t>
+      <c r="AA20" t="n">
+        <v>4474</v>
+      </c>
+      <c r="AB20" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>4565</t>
         </is>
       </c>
     </row>
@@ -1923,9 +2003,15 @@
       <c r="Z21" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA21" t="inlineStr">
-        <is>
-          <t>5064</t>
+      <c r="AA21" t="n">
+        <v>5064</v>
+      </c>
+      <c r="AB21" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC21" t="inlineStr">
+        <is>
+          <t>5201</t>
         </is>
       </c>
     </row>
@@ -2014,9 +2100,15 @@
       <c r="Z22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AA22" t="inlineStr">
-        <is>
-          <t>4993</t>
+      <c r="AA22" t="n">
+        <v>4993</v>
+      </c>
+      <c r="AB22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC22" t="inlineStr">
+        <is>
+          <t>5169</t>
         </is>
       </c>
     </row>
@@ -2105,9 +2197,15 @@
       <c r="Z23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AA23" t="inlineStr">
-        <is>
-          <t>5742</t>
+      <c r="AA23" t="n">
+        <v>5742</v>
+      </c>
+      <c r="AB23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC23" t="inlineStr">
+        <is>
+          <t>5917</t>
         </is>
       </c>
     </row>
@@ -2196,9 +2294,15 @@
       <c r="Z24" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AA24" t="inlineStr">
-        <is>
-          <t>5289</t>
+      <c r="AA24" t="n">
+        <v>5289</v>
+      </c>
+      <c r="AB24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC24" t="inlineStr">
+        <is>
+          <t>5401</t>
         </is>
       </c>
     </row>
@@ -2287,9 +2391,15 @@
       <c r="Z25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AA25" t="inlineStr">
-        <is>
-          <t>5482</t>
+      <c r="AA25" t="n">
+        <v>5482</v>
+      </c>
+      <c r="AB25" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC25" t="inlineStr">
+        <is>
+          <t>5564</t>
         </is>
       </c>
     </row>
@@ -2378,9 +2488,15 @@
       <c r="Z26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA26" t="inlineStr">
-        <is>
-          <t>2950</t>
+      <c r="AA26" t="n">
+        <v>2950</v>
+      </c>
+      <c r="AB26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC26" t="inlineStr">
+        <is>
+          <t>2949</t>
         </is>
       </c>
     </row>
@@ -2469,9 +2585,15 @@
       <c r="Z27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA27" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="AA27" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AB27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC27" t="inlineStr">
+        <is>
+          <t>2532</t>
         </is>
       </c>
     </row>
@@ -2523,6 +2645,8 @@
       <c r="Y28" t="inlineStr"/>
       <c r="Z28" s="4" t="inlineStr"/>
       <c r="AA28" t="inlineStr"/>
+      <c r="AB28" s="4" t="inlineStr"/>
+      <c r="AC28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2609,7 +2733,13 @@
       <c r="Z29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA29" t="inlineStr">
+      <c r="AA29" t="n">
+        <v>3624</v>
+      </c>
+      <c r="AB29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC29" t="inlineStr">
         <is>
           <t>3624</t>
         </is>
@@ -2700,9 +2830,15 @@
       <c r="Z30" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AA30" t="inlineStr">
-        <is>
-          <t>5134</t>
+      <c r="AA30" t="n">
+        <v>5134</v>
+      </c>
+      <c r="AB30" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AC30" t="inlineStr">
+        <is>
+          <t>5290</t>
         </is>
       </c>
     </row>
@@ -2791,9 +2927,15 @@
       <c r="Z31" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA31" t="inlineStr">
-        <is>
-          <t>5119</t>
+      <c r="AA31" t="n">
+        <v>5119</v>
+      </c>
+      <c r="AB31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC31" t="inlineStr">
+        <is>
+          <t>5252</t>
         </is>
       </c>
     </row>
@@ -2882,9 +3024,15 @@
       <c r="Z32" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AA32" t="inlineStr">
-        <is>
-          <t>3337</t>
+      <c r="AA32" t="n">
+        <v>3337</v>
+      </c>
+      <c r="AB32" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC32" t="inlineStr">
+        <is>
+          <t>3908</t>
         </is>
       </c>
     </row>
@@ -2948,6 +3096,8 @@
       <c r="Y33" t="inlineStr"/>
       <c r="Z33" s="4" t="inlineStr"/>
       <c r="AA33" t="inlineStr"/>
+      <c r="AB33" s="4" t="inlineStr"/>
+      <c r="AC33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3034,7 +3184,13 @@
       <c r="Z34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA34" t="inlineStr">
+      <c r="AA34" t="n">
+        <v>2530</v>
+      </c>
+      <c r="AB34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC34" t="inlineStr">
         <is>
           <t>2530</t>
         </is>
@@ -3125,9 +3281,15 @@
       <c r="Z35" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AA35" t="inlineStr">
-        <is>
-          <t>4981</t>
+      <c r="AA35" t="n">
+        <v>4981</v>
+      </c>
+      <c r="AB35" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC35" t="inlineStr">
+        <is>
+          <t>5129</t>
         </is>
       </c>
     </row>
@@ -3216,9 +3378,15 @@
       <c r="Z36" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AA36" t="inlineStr">
-        <is>
-          <t>3273</t>
+      <c r="AA36" t="n">
+        <v>3273</v>
+      </c>
+      <c r="AB36" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC36" t="inlineStr">
+        <is>
+          <t>3925</t>
         </is>
       </c>
     </row>
@@ -3307,9 +3475,15 @@
       <c r="Z37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AA37" t="inlineStr">
-        <is>
-          <t>4856</t>
+      <c r="AA37" t="n">
+        <v>4856</v>
+      </c>
+      <c r="AB37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC37" t="inlineStr">
+        <is>
+          <t>4994</t>
         </is>
       </c>
     </row>
@@ -3398,9 +3572,15 @@
       <c r="Z38" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AA38" t="inlineStr">
-        <is>
-          <t>5399</t>
+      <c r="AA38" t="n">
+        <v>5399</v>
+      </c>
+      <c r="AB38" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC38" t="inlineStr">
+        <is>
+          <t>5590</t>
         </is>
       </c>
     </row>
@@ -3489,9 +3669,15 @@
       <c r="Z39" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AA39" t="inlineStr">
-        <is>
-          <t>4765</t>
+      <c r="AA39" t="n">
+        <v>4765</v>
+      </c>
+      <c r="AB39" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC39" t="inlineStr">
+        <is>
+          <t>4844</t>
         </is>
       </c>
     </row>
@@ -3580,7 +3766,13 @@
       <c r="Z40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA40" t="inlineStr">
+      <c r="AA40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3671,9 +3863,15 @@
       <c r="Z41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA41" t="inlineStr">
-        <is>
-          <t>4419</t>
+      <c r="AA41" t="n">
+        <v>4419</v>
+      </c>
+      <c r="AB41" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC41" t="inlineStr">
+        <is>
+          <t>4502</t>
         </is>
       </c>
     </row>
@@ -3762,9 +3960,15 @@
       <c r="Z42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA42" t="inlineStr">
-        <is>
-          <t>3174</t>
+      <c r="AA42" t="n">
+        <v>3174</v>
+      </c>
+      <c r="AB42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC42" t="inlineStr">
+        <is>
+          <t>3231</t>
         </is>
       </c>
     </row>
@@ -3820,6 +4024,8 @@
       <c r="Y43" t="inlineStr"/>
       <c r="Z43" s="4" t="inlineStr"/>
       <c r="AA43" t="inlineStr"/>
+      <c r="AB43" s="4" t="inlineStr"/>
+      <c r="AC43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3901,6 +4107,8 @@
       <c r="Y44" t="inlineStr"/>
       <c r="Z44" s="4" t="inlineStr"/>
       <c r="AA44" t="inlineStr"/>
+      <c r="AB44" s="4" t="inlineStr"/>
+      <c r="AC44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3987,9 +4195,15 @@
       <c r="Z45" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AA45" t="inlineStr">
-        <is>
-          <t>4135</t>
+      <c r="AA45" t="n">
+        <v>4135</v>
+      </c>
+      <c r="AB45" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AC45" t="inlineStr">
+        <is>
+          <t>4133</t>
         </is>
       </c>
     </row>
@@ -4078,9 +4292,15 @@
       <c r="Z46" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="AA46" t="inlineStr">
-        <is>
-          <t>4281</t>
+      <c r="AA46" t="n">
+        <v>4281</v>
+      </c>
+      <c r="AB46" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="AC46" t="inlineStr">
+        <is>
+          <t>4397</t>
         </is>
       </c>
     </row>
@@ -4169,9 +4389,15 @@
       <c r="Z47" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA47" t="inlineStr">
-        <is>
-          <t>5572</t>
+      <c r="AA47" t="n">
+        <v>5572</v>
+      </c>
+      <c r="AB47" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC47" t="inlineStr">
+        <is>
+          <t>5740</t>
         </is>
       </c>
     </row>
@@ -4260,9 +4486,15 @@
       <c r="Z48" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AA48" t="inlineStr">
-        <is>
-          <t>5350</t>
+      <c r="AA48" t="n">
+        <v>5350</v>
+      </c>
+      <c r="AB48" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC48" t="inlineStr">
+        <is>
+          <t>5486</t>
         </is>
       </c>
     </row>
@@ -4351,9 +4583,15 @@
       <c r="Z49" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="AA49" t="inlineStr">
-        <is>
-          <t>4835</t>
+      <c r="AA49" t="n">
+        <v>4835</v>
+      </c>
+      <c r="AB49" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC49" t="inlineStr">
+        <is>
+          <t>5004</t>
         </is>
       </c>
     </row>
@@ -4442,9 +4680,15 @@
       <c r="Z50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AA50" t="inlineStr">
-        <is>
-          <t>5115</t>
+      <c r="AA50" t="n">
+        <v>5115</v>
+      </c>
+      <c r="AB50" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC50" t="inlineStr">
+        <is>
+          <t>5256</t>
         </is>
       </c>
     </row>
@@ -4533,9 +4777,15 @@
       <c r="Z51" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AA51" t="inlineStr">
-        <is>
-          <t>4390</t>
+      <c r="AA51" t="n">
+        <v>4390</v>
+      </c>
+      <c r="AB51" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC51" t="inlineStr">
+        <is>
+          <t>4556</t>
         </is>
       </c>
     </row>
@@ -4624,9 +4874,15 @@
       <c r="Z52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AA52" t="inlineStr">
-        <is>
-          <t>5345</t>
+      <c r="AA52" t="n">
+        <v>5345</v>
+      </c>
+      <c r="AB52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC52" t="inlineStr">
+        <is>
+          <t>5646</t>
         </is>
       </c>
     </row>
@@ -4715,9 +4971,15 @@
       <c r="Z53" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="AA53" t="inlineStr">
-        <is>
-          <t>3959</t>
+      <c r="AA53" t="n">
+        <v>3959</v>
+      </c>
+      <c r="AB53" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC53" t="inlineStr">
+        <is>
+          <t>4109</t>
         </is>
       </c>
     </row>
@@ -4806,9 +5068,15 @@
       <c r="Z54" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AA54" t="inlineStr">
-        <is>
-          <t>4884</t>
+      <c r="AA54" t="n">
+        <v>4884</v>
+      </c>
+      <c r="AB54" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="AC54" t="inlineStr">
+        <is>
+          <t>4993</t>
         </is>
       </c>
     </row>
@@ -4897,9 +5165,15 @@
       <c r="Z55" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA55" t="inlineStr">
-        <is>
-          <t>3703</t>
+      <c r="AA55" t="n">
+        <v>3703</v>
+      </c>
+      <c r="AB55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC55" t="inlineStr">
+        <is>
+          <t>3729</t>
         </is>
       </c>
     </row>
@@ -4988,9 +5262,15 @@
       <c r="Z56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AA56" t="inlineStr">
-        <is>
-          <t>5366</t>
+      <c r="AA56" t="n">
+        <v>5366</v>
+      </c>
+      <c r="AB56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC56" t="inlineStr">
+        <is>
+          <t>5518</t>
         </is>
       </c>
     </row>
@@ -5079,9 +5359,15 @@
       <c r="Z57" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="AA57" t="inlineStr">
-        <is>
-          <t>4298</t>
+      <c r="AA57" t="n">
+        <v>4298</v>
+      </c>
+      <c r="AB57" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="AC57" t="inlineStr">
+        <is>
+          <t>4384</t>
         </is>
       </c>
     </row>
@@ -5170,9 +5456,15 @@
       <c r="Z58" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AA58" t="inlineStr">
-        <is>
-          <t>4391</t>
+      <c r="AA58" t="n">
+        <v>4391</v>
+      </c>
+      <c r="AB58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC58" t="inlineStr">
+        <is>
+          <t>4437</t>
         </is>
       </c>
     </row>
@@ -5261,9 +5553,15 @@
       <c r="Z59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AA59" t="inlineStr">
-        <is>
-          <t>4256</t>
+      <c r="AA59" t="n">
+        <v>4256</v>
+      </c>
+      <c r="AB59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC59" t="inlineStr">
+        <is>
+          <t>4331</t>
         </is>
       </c>
     </row>
@@ -5352,9 +5650,15 @@
       <c r="Z60" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AA60" t="inlineStr">
-        <is>
-          <t>4328</t>
+      <c r="AA60" t="n">
+        <v>4328</v>
+      </c>
+      <c r="AB60" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC60" t="inlineStr">
+        <is>
+          <t>4464</t>
         </is>
       </c>
     </row>
@@ -5406,6 +5710,8 @@
       <c r="Y61" t="inlineStr"/>
       <c r="Z61" s="4" t="inlineStr"/>
       <c r="AA61" t="inlineStr"/>
+      <c r="AB61" s="4" t="inlineStr"/>
+      <c r="AC61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -5492,9 +5798,15 @@
       <c r="Z62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AA62" t="inlineStr">
-        <is>
-          <t>3994</t>
+      <c r="AA62" t="n">
+        <v>3994</v>
+      </c>
+      <c r="AB62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC62" t="inlineStr">
+        <is>
+          <t>4059</t>
         </is>
       </c>
     </row>
@@ -5583,9 +5895,15 @@
       <c r="Z63" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AA63" t="inlineStr">
-        <is>
-          <t>4146</t>
+      <c r="AA63" t="n">
+        <v>4146</v>
+      </c>
+      <c r="AB63" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC63" t="inlineStr">
+        <is>
+          <t>4123</t>
         </is>
       </c>
     </row>
@@ -5674,9 +5992,15 @@
       <c r="Z64" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="AA64" t="inlineStr">
-        <is>
-          <t>4267</t>
+      <c r="AA64" t="n">
+        <v>4267</v>
+      </c>
+      <c r="AB64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC64" t="inlineStr">
+        <is>
+          <t>4490</t>
         </is>
       </c>
     </row>
@@ -5765,9 +6089,15 @@
       <c r="Z65" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AA65" t="inlineStr">
-        <is>
-          <t>3996</t>
+      <c r="AA65" t="n">
+        <v>3996</v>
+      </c>
+      <c r="AB65" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC65" t="inlineStr">
+        <is>
+          <t>3993</t>
         </is>
       </c>
     </row>
@@ -5856,7 +6186,13 @@
       <c r="Z66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA66" t="inlineStr">
+      <c r="AA66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5947,7 +6283,13 @@
       <c r="Z67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA67" t="inlineStr">
+      <c r="AA67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6038,9 +6380,15 @@
       <c r="Z68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA68" t="inlineStr">
-        <is>
-          <t>2496</t>
+      <c r="AA68" t="n">
+        <v>2496</v>
+      </c>
+      <c r="AB68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC68" t="inlineStr">
+        <is>
+          <t>2522</t>
         </is>
       </c>
     </row>
@@ -6129,9 +6477,15 @@
       <c r="Z69" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="AA69" t="inlineStr">
-        <is>
-          <t>3034</t>
+      <c r="AA69" t="n">
+        <v>3034</v>
+      </c>
+      <c r="AB69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC69" t="inlineStr">
+        <is>
+          <t>3080</t>
         </is>
       </c>
     </row>
@@ -6220,9 +6574,15 @@
       <c r="Z70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA70" t="inlineStr">
-        <is>
-          <t>1504</t>
+      <c r="AA70" t="n">
+        <v>1504</v>
+      </c>
+      <c r="AB70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC70" t="inlineStr">
+        <is>
+          <t>1500</t>
         </is>
       </c>
     </row>
@@ -6311,7 +6671,13 @@
       <c r="Z71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA71" t="inlineStr">
+      <c r="AA71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6402,7 +6768,13 @@
       <c r="Z72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA72" t="inlineStr">
+      <c r="AA72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6493,9 +6865,15 @@
       <c r="Z73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA73" t="inlineStr">
-        <is>
-          <t>2625</t>
+      <c r="AA73" t="n">
+        <v>2625</v>
+      </c>
+      <c r="AB73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC73" t="inlineStr">
+        <is>
+          <t>2650</t>
         </is>
       </c>
     </row>
@@ -6584,7 +6962,13 @@
       <c r="Z74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA74" t="inlineStr">
+      <c r="AA74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6675,7 +7059,13 @@
       <c r="Z75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA75" t="inlineStr">
+      <c r="AA75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6766,9 +7156,15 @@
       <c r="Z76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA76" t="inlineStr">
-        <is>
-          <t>4514</t>
+      <c r="AA76" t="n">
+        <v>4514</v>
+      </c>
+      <c r="AB76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC76" t="inlineStr">
+        <is>
+          <t>4559</t>
         </is>
       </c>
     </row>
@@ -6857,9 +7253,15 @@
       <c r="Z77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA77" t="inlineStr">
-        <is>
-          <t>3947</t>
+      <c r="AA77" t="n">
+        <v>3947</v>
+      </c>
+      <c r="AB77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC77" t="inlineStr">
+        <is>
+          <t>3945</t>
         </is>
       </c>
     </row>
@@ -6948,9 +7350,15 @@
       <c r="Z78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA78" t="inlineStr">
-        <is>
-          <t>3004</t>
+      <c r="AA78" t="n">
+        <v>3004</v>
+      </c>
+      <c r="AB78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC78" t="inlineStr">
+        <is>
+          <t>3088</t>
         </is>
       </c>
     </row>
@@ -7039,9 +7447,15 @@
       <c r="Z79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA79" t="inlineStr">
-        <is>
-          <t>1302</t>
+      <c r="AA79" t="n">
+        <v>1302</v>
+      </c>
+      <c r="AB79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC79" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -7130,9 +7544,15 @@
       <c r="Z80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA80" t="inlineStr">
-        <is>
-          <t>1428</t>
+      <c r="AA80" t="n">
+        <v>1428</v>
+      </c>
+      <c r="AB80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC80" t="inlineStr">
+        <is>
+          <t>1470</t>
         </is>
       </c>
     </row>
@@ -7221,9 +7641,15 @@
       <c r="Z81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA81" t="inlineStr">
-        <is>
-          <t>2687</t>
+      <c r="AA81" t="n">
+        <v>2687</v>
+      </c>
+      <c r="AB81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC81" t="inlineStr">
+        <is>
+          <t>2734</t>
         </is>
       </c>
     </row>
@@ -7312,7 +7738,13 @@
       <c r="Z82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA82" t="inlineStr">
+      <c r="AA82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7403,7 +7835,13 @@
       <c r="Z83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA83" t="inlineStr">
+      <c r="AA83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7494,9 +7932,15 @@
       <c r="Z84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA84" t="inlineStr">
-        <is>
-          <t>1507</t>
+      <c r="AA84" t="n">
+        <v>1507</v>
+      </c>
+      <c r="AB84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC84" t="inlineStr">
+        <is>
+          <t>1503</t>
         </is>
       </c>
     </row>
@@ -7585,7 +8029,13 @@
       <c r="Z85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA85" t="inlineStr">
+      <c r="AA85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7676,7 +8126,13 @@
       <c r="Z86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA86" t="inlineStr">
+      <c r="AA86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7767,7 +8223,13 @@
       <c r="Z87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA87" t="inlineStr">
+      <c r="AA87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7858,7 +8320,13 @@
       <c r="Z88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA88" t="inlineStr">
+      <c r="AA88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7949,7 +8417,13 @@
       <c r="Z89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA89" t="inlineStr">
+      <c r="AA89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8040,7 +8514,13 @@
       <c r="Z90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA90" t="inlineStr">
+      <c r="AA90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8131,7 +8611,13 @@
       <c r="Z91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA91" t="inlineStr">
+      <c r="AA91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8222,7 +8708,13 @@
       <c r="Z92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA92" t="inlineStr">
+      <c r="AA92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8313,7 +8805,13 @@
       <c r="Z93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA93" t="inlineStr">
+      <c r="AA93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8404,7 +8902,13 @@
       <c r="Z94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA94" t="inlineStr">
+      <c r="AA94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8495,7 +8999,13 @@
       <c r="Z95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA95" t="inlineStr">
+      <c r="AA95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8586,9 +9096,15 @@
       <c r="Z96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA96" t="inlineStr">
-        <is>
-          <t>2798</t>
+      <c r="AA96" t="n">
+        <v>2798</v>
+      </c>
+      <c r="AB96" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC96" t="inlineStr">
+        <is>
+          <t>3128</t>
         </is>
       </c>
     </row>
@@ -8677,7 +9193,13 @@
       <c r="Z97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA97" t="inlineStr">
+      <c r="AA97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8768,7 +9290,13 @@
       <c r="Z98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA98" t="inlineStr">
+      <c r="AA98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8859,7 +9387,13 @@
       <c r="Z99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA99" t="inlineStr">
+      <c r="AA99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8950,7 +9484,13 @@
       <c r="Z100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA100" t="inlineStr">
+      <c r="AA100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9041,7 +9581,13 @@
       <c r="Z101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA101" t="inlineStr">
+      <c r="AA101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9132,7 +9678,13 @@
       <c r="Z102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA102" t="inlineStr">
+      <c r="AA102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9223,7 +9775,13 @@
       <c r="Z103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA103" t="inlineStr">
+      <c r="AA103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9314,7 +9872,13 @@
       <c r="Z104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA104" t="inlineStr">
+      <c r="AA104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9405,7 +9969,13 @@
       <c r="Z105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA105" t="inlineStr">
+      <c r="AA105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9451,6 +10021,8 @@
       <c r="Y106" t="inlineStr"/>
       <c r="Z106" s="4" t="inlineStr"/>
       <c r="AA106" t="inlineStr"/>
+      <c r="AB106" s="4" t="inlineStr"/>
+      <c r="AC106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -9492,6 +10064,8 @@
       <c r="Y107" t="inlineStr"/>
       <c r="Z107" s="4" t="inlineStr"/>
       <c r="AA107" t="inlineStr"/>
+      <c r="AB107" s="4" t="inlineStr"/>
+      <c r="AC107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -9533,6 +10107,8 @@
       <c r="Y108" t="inlineStr"/>
       <c r="Z108" s="4" t="inlineStr"/>
       <c r="AA108" t="inlineStr"/>
+      <c r="AB108" s="4" t="inlineStr"/>
+      <c r="AC108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -9574,6 +10150,8 @@
       <c r="Y109" t="inlineStr"/>
       <c r="Z109" s="4" t="inlineStr"/>
       <c r="AA109" t="inlineStr"/>
+      <c r="AB109" s="4" t="inlineStr"/>
+      <c r="AC109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -9615,6 +10193,8 @@
       <c r="Y110" t="inlineStr"/>
       <c r="Z110" s="4" t="inlineStr"/>
       <c r="AA110" t="inlineStr"/>
+      <c r="AB110" s="4" t="inlineStr"/>
+      <c r="AC110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -9656,6 +10236,8 @@
       <c r="Y111" t="inlineStr"/>
       <c r="Z111" s="4" t="inlineStr"/>
       <c r="AA111" t="inlineStr"/>
+      <c r="AB111" s="4" t="inlineStr"/>
+      <c r="AC111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -9697,6 +10279,8 @@
       <c r="Y112" t="inlineStr"/>
       <c r="Z112" s="4" t="inlineStr"/>
       <c r="AA112" t="inlineStr"/>
+      <c r="AB112" s="4" t="inlineStr"/>
+      <c r="AC112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -9738,6 +10322,8 @@
       <c r="Y113" t="inlineStr"/>
       <c r="Z113" s="4" t="inlineStr"/>
       <c r="AA113" t="inlineStr"/>
+      <c r="AB113" s="4" t="inlineStr"/>
+      <c r="AC113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -9779,6 +10365,8 @@
       <c r="Y114" t="inlineStr"/>
       <c r="Z114" s="4" t="inlineStr"/>
       <c r="AA114" t="inlineStr"/>
+      <c r="AB114" s="4" t="inlineStr"/>
+      <c r="AC114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -9850,6 +10438,8 @@
       <c r="Y115" t="inlineStr"/>
       <c r="Z115" s="4" t="inlineStr"/>
       <c r="AA115" t="inlineStr"/>
+      <c r="AB115" s="4" t="inlineStr"/>
+      <c r="AC115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -9921,6 +10511,8 @@
       <c r="Y116" t="inlineStr"/>
       <c r="Z116" s="4" t="inlineStr"/>
       <c r="AA116" t="inlineStr"/>
+      <c r="AB116" s="4" t="inlineStr"/>
+      <c r="AC116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -9992,6 +10584,8 @@
       <c r="Y117" t="inlineStr"/>
       <c r="Z117" s="4" t="inlineStr"/>
       <c r="AA117" t="inlineStr"/>
+      <c r="AB117" s="4" t="inlineStr"/>
+      <c r="AC117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -10068,9 +10662,15 @@
       <c r="Z118" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AA118" t="inlineStr">
-        <is>
-          <t>5815</t>
+      <c r="AA118" t="n">
+        <v>5815</v>
+      </c>
+      <c r="AB118" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC118" t="inlineStr">
+        <is>
+          <t>5992</t>
         </is>
       </c>
     </row>
@@ -10137,9 +10737,15 @@
       <c r="Z119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA119" t="inlineStr">
-        <is>
-          <t>1636</t>
+      <c r="AA119" t="n">
+        <v>1636</v>
+      </c>
+      <c r="AB119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC119" t="inlineStr">
+        <is>
+          <t>1635</t>
         </is>
       </c>
     </row>
@@ -10186,9 +10792,15 @@
       <c r="Z120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA120" t="inlineStr">
-        <is>
-          <t>1862</t>
+      <c r="AA120" t="n">
+        <v>1862</v>
+      </c>
+      <c r="AB120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC120" t="inlineStr">
+        <is>
+          <t>1875</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-06 11:30:56
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC120"/>
+  <dimension ref="A1:AE120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,6 +536,16 @@
           <t>05-04_0</t>
         </is>
       </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>05-05_A</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>05-05_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -628,7 +638,13 @@
       <c r="AB2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC2" t="inlineStr">
+      <c r="AC2" t="n">
+        <v>3130</v>
+      </c>
+      <c r="AD2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="inlineStr">
         <is>
           <t>3130</t>
         </is>
@@ -725,7 +741,13 @@
       <c r="AB3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC3" t="inlineStr">
+      <c r="AC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -822,7 +844,13 @@
       <c r="AB4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC4" t="inlineStr">
+      <c r="AC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -919,9 +947,15 @@
       <c r="AB5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>2528</t>
+      <c r="AC5" t="n">
+        <v>2528</v>
+      </c>
+      <c r="AD5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>2579</t>
         </is>
       </c>
     </row>
@@ -1016,9 +1050,15 @@
       <c r="AB6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>2792</t>
+      <c r="AC6" t="n">
+        <v>2792</v>
+      </c>
+      <c r="AD6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>2802</t>
         </is>
       </c>
     </row>
@@ -1076,6 +1116,8 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" s="4" t="inlineStr"/>
       <c r="AC7" t="inlineStr"/>
+      <c r="AD7" s="4" t="inlineStr"/>
+      <c r="AE7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1131,6 +1173,8 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" s="4" t="inlineStr"/>
       <c r="AC8" t="inlineStr"/>
+      <c r="AD8" s="4" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1186,6 +1230,8 @@
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" s="4" t="inlineStr"/>
       <c r="AC9" t="inlineStr"/>
+      <c r="AD9" s="4" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1241,6 +1287,8 @@
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" s="4" t="inlineStr"/>
       <c r="AC10" t="inlineStr"/>
+      <c r="AD10" s="4" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1296,6 +1344,8 @@
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" s="4" t="inlineStr"/>
       <c r="AC11" t="inlineStr"/>
+      <c r="AD11" s="4" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1351,6 +1401,8 @@
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" s="4" t="inlineStr"/>
       <c r="AC12" t="inlineStr"/>
+      <c r="AD12" s="4" t="inlineStr"/>
+      <c r="AE12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1406,6 +1458,8 @@
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" s="4" t="inlineStr"/>
       <c r="AC13" t="inlineStr"/>
+      <c r="AD13" s="4" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1461,6 +1515,8 @@
       <c r="AA14" t="inlineStr"/>
       <c r="AB14" s="4" t="inlineStr"/>
       <c r="AC14" t="inlineStr"/>
+      <c r="AD14" s="4" t="inlineStr"/>
+      <c r="AE14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1516,6 +1572,8 @@
       <c r="AA15" t="inlineStr"/>
       <c r="AB15" s="4" t="inlineStr"/>
       <c r="AC15" t="inlineStr"/>
+      <c r="AD15" s="4" t="inlineStr"/>
+      <c r="AE15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1571,6 +1629,8 @@
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" s="4" t="inlineStr"/>
       <c r="AC16" t="inlineStr"/>
+      <c r="AD16" s="4" t="inlineStr"/>
+      <c r="AE16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1626,6 +1686,8 @@
       <c r="AA17" t="inlineStr"/>
       <c r="AB17" s="4" t="inlineStr"/>
       <c r="AC17" t="inlineStr"/>
+      <c r="AD17" s="4" t="inlineStr"/>
+      <c r="AE17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1718,9 +1780,15 @@
       <c r="AB18" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="AC18" t="inlineStr">
-        <is>
-          <t>4116</t>
+      <c r="AC18" t="n">
+        <v>4116</v>
+      </c>
+      <c r="AD18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>4071</t>
         </is>
       </c>
     </row>
@@ -1815,9 +1883,15 @@
       <c r="AB19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC19" t="inlineStr">
-        <is>
-          <t>2758</t>
+      <c r="AC19" t="n">
+        <v>2758</v>
+      </c>
+      <c r="AD19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>2821</t>
         </is>
       </c>
     </row>
@@ -1912,9 +1986,15 @@
       <c r="AB20" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AC20" t="inlineStr">
-        <is>
-          <t>4565</t>
+      <c r="AC20" t="n">
+        <v>4565</v>
+      </c>
+      <c r="AD20" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>4589</t>
         </is>
       </c>
     </row>
@@ -2009,9 +2089,15 @@
       <c r="AB21" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AC21" t="inlineStr">
-        <is>
-          <t>5201</t>
+      <c r="AC21" t="n">
+        <v>5201</v>
+      </c>
+      <c r="AD21" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="AE21" t="inlineStr">
+        <is>
+          <t>5188</t>
         </is>
       </c>
     </row>
@@ -2106,9 +2192,15 @@
       <c r="AB22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AC22" t="inlineStr">
-        <is>
-          <t>5169</t>
+      <c r="AC22" t="n">
+        <v>5169</v>
+      </c>
+      <c r="AD22" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AE22" t="inlineStr">
+        <is>
+          <t>5316</t>
         </is>
       </c>
     </row>
@@ -2203,9 +2295,15 @@
       <c r="AB23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AC23" t="inlineStr">
-        <is>
-          <t>5917</t>
+      <c r="AC23" t="n">
+        <v>5917</v>
+      </c>
+      <c r="AD23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE23" t="inlineStr">
+        <is>
+          <t>6064</t>
         </is>
       </c>
     </row>
@@ -2300,9 +2398,15 @@
       <c r="AB24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AC24" t="inlineStr">
-        <is>
-          <t>5401</t>
+      <c r="AC24" t="n">
+        <v>5401</v>
+      </c>
+      <c r="AD24" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AE24" t="inlineStr">
+        <is>
+          <t>5498</t>
         </is>
       </c>
     </row>
@@ -2397,9 +2501,15 @@
       <c r="AB25" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="AC25" t="inlineStr">
-        <is>
-          <t>5564</t>
+      <c r="AC25" t="n">
+        <v>5564</v>
+      </c>
+      <c r="AD25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE25" t="inlineStr">
+        <is>
+          <t>5940</t>
         </is>
       </c>
     </row>
@@ -2494,9 +2604,15 @@
       <c r="AB26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC26" t="inlineStr">
-        <is>
-          <t>2949</t>
+      <c r="AC26" t="n">
+        <v>2949</v>
+      </c>
+      <c r="AD26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE26" t="inlineStr">
+        <is>
+          <t>2965</t>
         </is>
       </c>
     </row>
@@ -2591,7 +2707,13 @@
       <c r="AB27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC27" t="inlineStr">
+      <c r="AC27" t="n">
+        <v>2532</v>
+      </c>
+      <c r="AD27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE27" t="inlineStr">
         <is>
           <t>2532</t>
         </is>
@@ -2647,6 +2769,8 @@
       <c r="AA28" t="inlineStr"/>
       <c r="AB28" s="4" t="inlineStr"/>
       <c r="AC28" t="inlineStr"/>
+      <c r="AD28" s="4" t="inlineStr"/>
+      <c r="AE28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2739,9 +2863,15 @@
       <c r="AB29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC29" t="inlineStr">
-        <is>
-          <t>3624</t>
+      <c r="AC29" t="n">
+        <v>3624</v>
+      </c>
+      <c r="AD29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE29" t="inlineStr">
+        <is>
+          <t>3625</t>
         </is>
       </c>
     </row>
@@ -2836,9 +2966,15 @@
       <c r="AB30" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AC30" t="inlineStr">
-        <is>
-          <t>5290</t>
+      <c r="AC30" t="n">
+        <v>5290</v>
+      </c>
+      <c r="AD30" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AE30" t="inlineStr">
+        <is>
+          <t>5398</t>
         </is>
       </c>
     </row>
@@ -2933,9 +3069,15 @@
       <c r="AB31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AC31" t="inlineStr">
-        <is>
-          <t>5252</t>
+      <c r="AC31" t="n">
+        <v>5252</v>
+      </c>
+      <c r="AD31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE31" t="inlineStr">
+        <is>
+          <t>5421</t>
         </is>
       </c>
     </row>
@@ -3030,9 +3172,15 @@
       <c r="AB32" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AC32" t="inlineStr">
-        <is>
-          <t>3908</t>
+      <c r="AC32" t="n">
+        <v>3908</v>
+      </c>
+      <c r="AD32" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE32" t="inlineStr">
+        <is>
+          <t>4377</t>
         </is>
       </c>
     </row>
@@ -3098,6 +3246,8 @@
       <c r="AA33" t="inlineStr"/>
       <c r="AB33" s="4" t="inlineStr"/>
       <c r="AC33" t="inlineStr"/>
+      <c r="AD33" s="4" t="inlineStr"/>
+      <c r="AE33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3190,9 +3340,15 @@
       <c r="AB34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC34" t="inlineStr">
-        <is>
-          <t>2530</t>
+      <c r="AC34" t="n">
+        <v>2530</v>
+      </c>
+      <c r="AD34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE34" t="inlineStr">
+        <is>
+          <t>2546</t>
         </is>
       </c>
     </row>
@@ -3287,9 +3443,15 @@
       <c r="AB35" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AC35" t="inlineStr">
-        <is>
-          <t>5129</t>
+      <c r="AC35" t="n">
+        <v>5129</v>
+      </c>
+      <c r="AD35" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE35" t="inlineStr">
+        <is>
+          <t>5205</t>
         </is>
       </c>
     </row>
@@ -3384,9 +3546,15 @@
       <c r="AB36" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AC36" t="inlineStr">
-        <is>
-          <t>3925</t>
+      <c r="AC36" t="n">
+        <v>3925</v>
+      </c>
+      <c r="AD36" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE36" t="inlineStr">
+        <is>
+          <t>4480</t>
         </is>
       </c>
     </row>
@@ -3481,9 +3649,15 @@
       <c r="AB37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AC37" t="inlineStr">
-        <is>
-          <t>4994</t>
+      <c r="AC37" t="n">
+        <v>4994</v>
+      </c>
+      <c r="AD37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE37" t="inlineStr">
+        <is>
+          <t>5120</t>
         </is>
       </c>
     </row>
@@ -3578,9 +3752,15 @@
       <c r="AB38" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="AC38" t="inlineStr">
-        <is>
-          <t>5590</t>
+      <c r="AC38" t="n">
+        <v>5590</v>
+      </c>
+      <c r="AD38" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE38" t="inlineStr">
+        <is>
+          <t>5779</t>
         </is>
       </c>
     </row>
@@ -3675,9 +3855,15 @@
       <c r="AB39" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AC39" t="inlineStr">
-        <is>
-          <t>4844</t>
+      <c r="AC39" t="n">
+        <v>4844</v>
+      </c>
+      <c r="AD39" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE39" t="inlineStr">
+        <is>
+          <t>4919</t>
         </is>
       </c>
     </row>
@@ -3772,7 +3958,13 @@
       <c r="AB40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC40" t="inlineStr">
+      <c r="AC40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3869,9 +4061,15 @@
       <c r="AB41" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="AC41" t="inlineStr">
-        <is>
-          <t>4502</t>
+      <c r="AC41" t="n">
+        <v>4502</v>
+      </c>
+      <c r="AD41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE41" t="inlineStr">
+        <is>
+          <t>4603</t>
         </is>
       </c>
     </row>
@@ -3966,9 +4164,15 @@
       <c r="AB42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC42" t="inlineStr">
-        <is>
-          <t>3231</t>
+      <c r="AC42" t="n">
+        <v>3231</v>
+      </c>
+      <c r="AD42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE42" t="inlineStr">
+        <is>
+          <t>3291</t>
         </is>
       </c>
     </row>
@@ -4026,6 +4230,8 @@
       <c r="AA43" t="inlineStr"/>
       <c r="AB43" s="4" t="inlineStr"/>
       <c r="AC43" t="inlineStr"/>
+      <c r="AD43" s="4" t="inlineStr"/>
+      <c r="AE43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -4109,6 +4315,8 @@
       <c r="AA44" t="inlineStr"/>
       <c r="AB44" s="4" t="inlineStr"/>
       <c r="AC44" t="inlineStr"/>
+      <c r="AD44" s="4" t="inlineStr"/>
+      <c r="AE44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -4201,9 +4409,15 @@
       <c r="AB45" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="AC45" t="inlineStr">
-        <is>
-          <t>4133</t>
+      <c r="AC45" t="n">
+        <v>4133</v>
+      </c>
+      <c r="AD45" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE45" t="inlineStr">
+        <is>
+          <t>4194</t>
         </is>
       </c>
     </row>
@@ -4298,9 +4512,15 @@
       <c r="AB46" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="AC46" t="inlineStr">
-        <is>
-          <t>4397</t>
+      <c r="AC46" t="n">
+        <v>4397</v>
+      </c>
+      <c r="AD46" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="AE46" t="inlineStr">
+        <is>
+          <t>4455</t>
         </is>
       </c>
     </row>
@@ -4395,9 +4615,15 @@
       <c r="AB47" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AC47" t="inlineStr">
-        <is>
-          <t>5740</t>
+      <c r="AC47" t="n">
+        <v>5740</v>
+      </c>
+      <c r="AD47" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AE47" t="inlineStr">
+        <is>
+          <t>5883</t>
         </is>
       </c>
     </row>
@@ -4492,9 +4718,15 @@
       <c r="AB48" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AC48" t="inlineStr">
-        <is>
-          <t>5486</t>
+      <c r="AC48" t="n">
+        <v>5486</v>
+      </c>
+      <c r="AD48" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE48" t="inlineStr">
+        <is>
+          <t>5636</t>
         </is>
       </c>
     </row>
@@ -4589,9 +4821,15 @@
       <c r="AB49" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AC49" t="inlineStr">
-        <is>
-          <t>5004</t>
+      <c r="AC49" t="n">
+        <v>5004</v>
+      </c>
+      <c r="AD49" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE49" t="inlineStr">
+        <is>
+          <t>5082</t>
         </is>
       </c>
     </row>
@@ -4686,9 +4924,15 @@
       <c r="AB50" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AC50" t="inlineStr">
-        <is>
-          <t>5256</t>
+      <c r="AC50" t="n">
+        <v>5256</v>
+      </c>
+      <c r="AD50" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AE50" t="inlineStr">
+        <is>
+          <t>5386</t>
         </is>
       </c>
     </row>
@@ -4783,9 +5027,15 @@
       <c r="AB51" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="AC51" t="inlineStr">
-        <is>
-          <t>4556</t>
+      <c r="AC51" t="n">
+        <v>4556</v>
+      </c>
+      <c r="AD51" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE51" t="inlineStr">
+        <is>
+          <t>4584</t>
         </is>
       </c>
     </row>
@@ -4880,9 +5130,15 @@
       <c r="AB52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AC52" t="inlineStr">
-        <is>
-          <t>5646</t>
+      <c r="AC52" t="n">
+        <v>5646</v>
+      </c>
+      <c r="AD52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE52" t="inlineStr">
+        <is>
+          <t>5681</t>
         </is>
       </c>
     </row>
@@ -4977,9 +5233,15 @@
       <c r="AB53" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="AC53" t="inlineStr">
-        <is>
-          <t>4109</t>
+      <c r="AC53" t="n">
+        <v>4109</v>
+      </c>
+      <c r="AD53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE53" t="inlineStr">
+        <is>
+          <t>4158</t>
         </is>
       </c>
     </row>
@@ -5074,9 +5336,15 @@
       <c r="AB54" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="AC54" t="inlineStr">
-        <is>
-          <t>4993</t>
+      <c r="AC54" t="n">
+        <v>4993</v>
+      </c>
+      <c r="AD54" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE54" t="inlineStr">
+        <is>
+          <t>5101</t>
         </is>
       </c>
     </row>
@@ -5171,9 +5439,15 @@
       <c r="AB55" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC55" t="inlineStr">
-        <is>
-          <t>3729</t>
+      <c r="AC55" t="n">
+        <v>3729</v>
+      </c>
+      <c r="AD55" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE55" t="inlineStr">
+        <is>
+          <t>4230</t>
         </is>
       </c>
     </row>
@@ -5268,9 +5542,15 @@
       <c r="AB56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AC56" t="inlineStr">
-        <is>
-          <t>5518</t>
+      <c r="AC56" t="n">
+        <v>5518</v>
+      </c>
+      <c r="AD56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE56" t="inlineStr">
+        <is>
+          <t>5755</t>
         </is>
       </c>
     </row>
@@ -5365,9 +5645,15 @@
       <c r="AB57" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="AC57" t="inlineStr">
-        <is>
-          <t>4384</t>
+      <c r="AC57" t="n">
+        <v>4384</v>
+      </c>
+      <c r="AD57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE57" t="inlineStr">
+        <is>
+          <t>4458</t>
         </is>
       </c>
     </row>
@@ -5462,9 +5748,15 @@
       <c r="AB58" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AC58" t="inlineStr">
-        <is>
-          <t>4437</t>
+      <c r="AC58" t="n">
+        <v>4437</v>
+      </c>
+      <c r="AD58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE58" t="inlineStr">
+        <is>
+          <t>4577</t>
         </is>
       </c>
     </row>
@@ -5559,9 +5851,15 @@
       <c r="AB59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AC59" t="inlineStr">
-        <is>
-          <t>4331</t>
+      <c r="AC59" t="n">
+        <v>4331</v>
+      </c>
+      <c r="AD59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE59" t="inlineStr">
+        <is>
+          <t>4450</t>
         </is>
       </c>
     </row>
@@ -5656,9 +5954,15 @@
       <c r="AB60" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AC60" t="inlineStr">
-        <is>
-          <t>4464</t>
+      <c r="AC60" t="n">
+        <v>4464</v>
+      </c>
+      <c r="AD60" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE60" t="inlineStr">
+        <is>
+          <t>4520</t>
         </is>
       </c>
     </row>
@@ -5712,6 +6016,8 @@
       <c r="AA61" t="inlineStr"/>
       <c r="AB61" s="4" t="inlineStr"/>
       <c r="AC61" t="inlineStr"/>
+      <c r="AD61" s="4" t="inlineStr"/>
+      <c r="AE61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -5804,9 +6110,15 @@
       <c r="AB62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AC62" t="inlineStr">
-        <is>
-          <t>4059</t>
+      <c r="AC62" t="n">
+        <v>4059</v>
+      </c>
+      <c r="AD62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE62" t="inlineStr">
+        <is>
+          <t>4091</t>
         </is>
       </c>
     </row>
@@ -5901,9 +6213,15 @@
       <c r="AB63" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AC63" t="inlineStr">
-        <is>
-          <t>4123</t>
+      <c r="AC63" t="n">
+        <v>4123</v>
+      </c>
+      <c r="AD63" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE63" t="inlineStr">
+        <is>
+          <t>4184</t>
         </is>
       </c>
     </row>
@@ -5998,9 +6316,15 @@
       <c r="AB64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AC64" t="inlineStr">
-        <is>
-          <t>4490</t>
+      <c r="AC64" t="n">
+        <v>4490</v>
+      </c>
+      <c r="AD64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE64" t="inlineStr">
+        <is>
+          <t>4583</t>
         </is>
       </c>
     </row>
@@ -6095,9 +6419,15 @@
       <c r="AB65" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AC65" t="inlineStr">
-        <is>
-          <t>3993</t>
+      <c r="AC65" t="n">
+        <v>3993</v>
+      </c>
+      <c r="AD65" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE65" t="inlineStr">
+        <is>
+          <t>4061</t>
         </is>
       </c>
     </row>
@@ -6192,7 +6522,13 @@
       <c r="AB66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC66" t="inlineStr">
+      <c r="AC66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6289,7 +6625,13 @@
       <c r="AB67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC67" t="inlineStr">
+      <c r="AC67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6386,9 +6728,15 @@
       <c r="AB68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC68" t="inlineStr">
-        <is>
-          <t>2522</t>
+      <c r="AC68" t="n">
+        <v>2522</v>
+      </c>
+      <c r="AD68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE68" t="inlineStr">
+        <is>
+          <t>2520</t>
         </is>
       </c>
     </row>
@@ -6483,9 +6831,15 @@
       <c r="AB69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC69" t="inlineStr">
-        <is>
-          <t>3080</t>
+      <c r="AC69" t="n">
+        <v>3080</v>
+      </c>
+      <c r="AD69" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE69" t="inlineStr">
+        <is>
+          <t>3497</t>
         </is>
       </c>
     </row>
@@ -6580,9 +6934,15 @@
       <c r="AB70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC70" t="inlineStr">
-        <is>
-          <t>1500</t>
+      <c r="AC70" t="n">
+        <v>1500</v>
+      </c>
+      <c r="AD70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE70" t="inlineStr">
+        <is>
+          <t>1499</t>
         </is>
       </c>
     </row>
@@ -6677,7 +7037,13 @@
       <c r="AB71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC71" t="inlineStr">
+      <c r="AC71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6774,7 +7140,13 @@
       <c r="AB72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC72" t="inlineStr">
+      <c r="AC72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6871,9 +7243,15 @@
       <c r="AB73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC73" t="inlineStr">
-        <is>
-          <t>2650</t>
+      <c r="AC73" t="n">
+        <v>2650</v>
+      </c>
+      <c r="AD73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE73" t="inlineStr">
+        <is>
+          <t>2662</t>
         </is>
       </c>
     </row>
@@ -6968,7 +7346,13 @@
       <c r="AB74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC74" t="inlineStr">
+      <c r="AC74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7065,7 +7449,13 @@
       <c r="AB75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC75" t="inlineStr">
+      <c r="AC75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7162,9 +7552,15 @@
       <c r="AB76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC76" t="inlineStr">
-        <is>
-          <t>4559</t>
+      <c r="AC76" t="n">
+        <v>4559</v>
+      </c>
+      <c r="AD76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE76" t="inlineStr">
+        <is>
+          <t>4657</t>
         </is>
       </c>
     </row>
@@ -7259,9 +7655,15 @@
       <c r="AB77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC77" t="inlineStr">
-        <is>
-          <t>3945</t>
+      <c r="AC77" t="n">
+        <v>3945</v>
+      </c>
+      <c r="AD77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE77" t="inlineStr">
+        <is>
+          <t>3982</t>
         </is>
       </c>
     </row>
@@ -7356,9 +7758,15 @@
       <c r="AB78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC78" t="inlineStr">
-        <is>
-          <t>3088</t>
+      <c r="AC78" t="n">
+        <v>3088</v>
+      </c>
+      <c r="AD78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE78" t="inlineStr">
+        <is>
+          <t>3181</t>
         </is>
       </c>
     </row>
@@ -7453,9 +7861,15 @@
       <c r="AB79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC79" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AC79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE79" t="inlineStr">
+        <is>
+          <t>1300</t>
         </is>
       </c>
     </row>
@@ -7550,9 +7964,15 @@
       <c r="AB80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC80" t="inlineStr">
-        <is>
-          <t>1470</t>
+      <c r="AC80" t="n">
+        <v>1470</v>
+      </c>
+      <c r="AD80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE80" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -7647,9 +8067,15 @@
       <c r="AB81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC81" t="inlineStr">
-        <is>
-          <t>2734</t>
+      <c r="AC81" t="n">
+        <v>2734</v>
+      </c>
+      <c r="AD81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE81" t="inlineStr">
+        <is>
+          <t>2729</t>
         </is>
       </c>
     </row>
@@ -7744,7 +8170,13 @@
       <c r="AB82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC82" t="inlineStr">
+      <c r="AC82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7841,7 +8273,13 @@
       <c r="AB83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC83" t="inlineStr">
+      <c r="AC83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7938,9 +8376,15 @@
       <c r="AB84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC84" t="inlineStr">
-        <is>
-          <t>1503</t>
+      <c r="AC84" t="n">
+        <v>1503</v>
+      </c>
+      <c r="AD84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE84" t="inlineStr">
+        <is>
+          <t>1498</t>
         </is>
       </c>
     </row>
@@ -8035,7 +8479,13 @@
       <c r="AB85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC85" t="inlineStr">
+      <c r="AC85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8132,7 +8582,13 @@
       <c r="AB86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC86" t="inlineStr">
+      <c r="AC86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8229,7 +8685,13 @@
       <c r="AB87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC87" t="inlineStr">
+      <c r="AC87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8326,7 +8788,13 @@
       <c r="AB88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC88" t="inlineStr">
+      <c r="AC88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8423,7 +8891,13 @@
       <c r="AB89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC89" t="inlineStr">
+      <c r="AC89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8520,7 +8994,13 @@
       <c r="AB90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC90" t="inlineStr">
+      <c r="AC90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8617,7 +9097,13 @@
       <c r="AB91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC91" t="inlineStr">
+      <c r="AC91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8714,7 +9200,13 @@
       <c r="AB92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC92" t="inlineStr">
+      <c r="AC92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8811,7 +9303,13 @@
       <c r="AB93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC93" t="inlineStr">
+      <c r="AC93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8908,7 +9406,13 @@
       <c r="AB94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC94" t="inlineStr">
+      <c r="AC94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9005,7 +9509,13 @@
       <c r="AB95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC95" t="inlineStr">
+      <c r="AC95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9102,9 +9612,15 @@
       <c r="AB96" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AC96" t="inlineStr">
-        <is>
-          <t>3128</t>
+      <c r="AC96" t="n">
+        <v>3128</v>
+      </c>
+      <c r="AD96" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE96" t="inlineStr">
+        <is>
+          <t>3521</t>
         </is>
       </c>
     </row>
@@ -9199,7 +9715,13 @@
       <c r="AB97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC97" t="inlineStr">
+      <c r="AC97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9296,7 +9818,13 @@
       <c r="AB98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC98" t="inlineStr">
+      <c r="AC98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9393,7 +9921,13 @@
       <c r="AB99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC99" t="inlineStr">
+      <c r="AC99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9490,7 +10024,13 @@
       <c r="AB100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC100" t="inlineStr">
+      <c r="AC100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9587,7 +10127,13 @@
       <c r="AB101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC101" t="inlineStr">
+      <c r="AC101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9684,7 +10230,13 @@
       <c r="AB102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC102" t="inlineStr">
+      <c r="AC102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9781,7 +10333,13 @@
       <c r="AB103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC103" t="inlineStr">
+      <c r="AC103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9878,7 +10436,13 @@
       <c r="AB104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC104" t="inlineStr">
+      <c r="AC104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9975,7 +10539,13 @@
       <c r="AB105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC105" t="inlineStr">
+      <c r="AC105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10023,6 +10593,8 @@
       <c r="AA106" t="inlineStr"/>
       <c r="AB106" s="4" t="inlineStr"/>
       <c r="AC106" t="inlineStr"/>
+      <c r="AD106" s="4" t="inlineStr"/>
+      <c r="AE106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -10066,6 +10638,8 @@
       <c r="AA107" t="inlineStr"/>
       <c r="AB107" s="4" t="inlineStr"/>
       <c r="AC107" t="inlineStr"/>
+      <c r="AD107" s="4" t="inlineStr"/>
+      <c r="AE107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -10109,6 +10683,8 @@
       <c r="AA108" t="inlineStr"/>
       <c r="AB108" s="4" t="inlineStr"/>
       <c r="AC108" t="inlineStr"/>
+      <c r="AD108" s="4" t="inlineStr"/>
+      <c r="AE108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -10152,6 +10728,8 @@
       <c r="AA109" t="inlineStr"/>
       <c r="AB109" s="4" t="inlineStr"/>
       <c r="AC109" t="inlineStr"/>
+      <c r="AD109" s="4" t="inlineStr"/>
+      <c r="AE109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -10195,6 +10773,8 @@
       <c r="AA110" t="inlineStr"/>
       <c r="AB110" s="4" t="inlineStr"/>
       <c r="AC110" t="inlineStr"/>
+      <c r="AD110" s="4" t="inlineStr"/>
+      <c r="AE110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -10238,6 +10818,8 @@
       <c r="AA111" t="inlineStr"/>
       <c r="AB111" s="4" t="inlineStr"/>
       <c r="AC111" t="inlineStr"/>
+      <c r="AD111" s="4" t="inlineStr"/>
+      <c r="AE111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -10281,6 +10863,8 @@
       <c r="AA112" t="inlineStr"/>
       <c r="AB112" s="4" t="inlineStr"/>
       <c r="AC112" t="inlineStr"/>
+      <c r="AD112" s="4" t="inlineStr"/>
+      <c r="AE112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -10324,6 +10908,8 @@
       <c r="AA113" t="inlineStr"/>
       <c r="AB113" s="4" t="inlineStr"/>
       <c r="AC113" t="inlineStr"/>
+      <c r="AD113" s="4" t="inlineStr"/>
+      <c r="AE113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -10367,6 +10953,8 @@
       <c r="AA114" t="inlineStr"/>
       <c r="AB114" s="4" t="inlineStr"/>
       <c r="AC114" t="inlineStr"/>
+      <c r="AD114" s="4" t="inlineStr"/>
+      <c r="AE114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -10440,6 +11028,8 @@
       <c r="AA115" t="inlineStr"/>
       <c r="AB115" s="4" t="inlineStr"/>
       <c r="AC115" t="inlineStr"/>
+      <c r="AD115" s="4" t="inlineStr"/>
+      <c r="AE115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -10513,6 +11103,8 @@
       <c r="AA116" t="inlineStr"/>
       <c r="AB116" s="4" t="inlineStr"/>
       <c r="AC116" t="inlineStr"/>
+      <c r="AD116" s="4" t="inlineStr"/>
+      <c r="AE116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -10586,6 +11178,8 @@
       <c r="AA117" t="inlineStr"/>
       <c r="AB117" s="4" t="inlineStr"/>
       <c r="AC117" t="inlineStr"/>
+      <c r="AD117" s="4" t="inlineStr"/>
+      <c r="AE117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -10668,9 +11262,15 @@
       <c r="AB118" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AC118" t="inlineStr">
-        <is>
-          <t>5992</t>
+      <c r="AC118" t="n">
+        <v>5992</v>
+      </c>
+      <c r="AD118" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE118" t="inlineStr">
+        <is>
+          <t>6133</t>
         </is>
       </c>
     </row>
@@ -10743,7 +11343,13 @@
       <c r="AB119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC119" t="inlineStr">
+      <c r="AC119" t="n">
+        <v>1635</v>
+      </c>
+      <c r="AD119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE119" t="inlineStr">
         <is>
           <t>1635</t>
         </is>
@@ -10798,9 +11404,15 @@
       <c r="AB120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC120" t="inlineStr">
-        <is>
-          <t>1875</t>
+      <c r="AC120" t="n">
+        <v>1875</v>
+      </c>
+      <c r="AD120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE120" t="inlineStr">
+        <is>
+          <t>1913</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-07 11:50:41
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE120"/>
+  <dimension ref="A1:AG120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,6 +546,16 @@
           <t>05-05_0</t>
         </is>
       </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>05-06_A</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>05-06_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -644,9 +654,15 @@
       <c r="AD2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>3130</t>
+      <c r="AE2" t="n">
+        <v>3130</v>
+      </c>
+      <c r="AF2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -747,7 +763,13 @@
       <c r="AD3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE3" t="inlineStr">
+      <c r="AE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -850,7 +872,13 @@
       <c r="AD4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE4" t="inlineStr">
+      <c r="AE4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -953,9 +981,15 @@
       <c r="AD5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t>2579</t>
+      <c r="AE5" t="n">
+        <v>2579</v>
+      </c>
+      <c r="AF5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>2592</t>
         </is>
       </c>
     </row>
@@ -1056,9 +1090,15 @@
       <c r="AD6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE6" t="inlineStr">
-        <is>
-          <t>2802</t>
+      <c r="AE6" t="n">
+        <v>2802</v>
+      </c>
+      <c r="AF6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>2801</t>
         </is>
       </c>
     </row>
@@ -1118,6 +1158,8 @@
       <c r="AC7" t="inlineStr"/>
       <c r="AD7" s="4" t="inlineStr"/>
       <c r="AE7" t="inlineStr"/>
+      <c r="AF7" s="4" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1175,6 +1217,8 @@
       <c r="AC8" t="inlineStr"/>
       <c r="AD8" s="4" t="inlineStr"/>
       <c r="AE8" t="inlineStr"/>
+      <c r="AF8" s="4" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1232,6 +1276,8 @@
       <c r="AC9" t="inlineStr"/>
       <c r="AD9" s="4" t="inlineStr"/>
       <c r="AE9" t="inlineStr"/>
+      <c r="AF9" s="4" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1289,6 +1335,8 @@
       <c r="AC10" t="inlineStr"/>
       <c r="AD10" s="4" t="inlineStr"/>
       <c r="AE10" t="inlineStr"/>
+      <c r="AF10" s="4" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1346,6 +1394,8 @@
       <c r="AC11" t="inlineStr"/>
       <c r="AD11" s="4" t="inlineStr"/>
       <c r="AE11" t="inlineStr"/>
+      <c r="AF11" s="4" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1403,6 +1453,8 @@
       <c r="AC12" t="inlineStr"/>
       <c r="AD12" s="4" t="inlineStr"/>
       <c r="AE12" t="inlineStr"/>
+      <c r="AF12" s="4" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1460,6 +1512,8 @@
       <c r="AC13" t="inlineStr"/>
       <c r="AD13" s="4" t="inlineStr"/>
       <c r="AE13" t="inlineStr"/>
+      <c r="AF13" s="4" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1517,6 +1571,8 @@
       <c r="AC14" t="inlineStr"/>
       <c r="AD14" s="4" t="inlineStr"/>
       <c r="AE14" t="inlineStr"/>
+      <c r="AF14" s="4" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1574,6 +1630,8 @@
       <c r="AC15" t="inlineStr"/>
       <c r="AD15" s="4" t="inlineStr"/>
       <c r="AE15" t="inlineStr"/>
+      <c r="AF15" s="4" t="inlineStr"/>
+      <c r="AG15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1631,6 +1689,8 @@
       <c r="AC16" t="inlineStr"/>
       <c r="AD16" s="4" t="inlineStr"/>
       <c r="AE16" t="inlineStr"/>
+      <c r="AF16" s="4" t="inlineStr"/>
+      <c r="AG16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1688,6 +1748,8 @@
       <c r="AC17" t="inlineStr"/>
       <c r="AD17" s="4" t="inlineStr"/>
       <c r="AE17" t="inlineStr"/>
+      <c r="AF17" s="4" t="inlineStr"/>
+      <c r="AG17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1786,9 +1848,15 @@
       <c r="AD18" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE18" t="inlineStr">
-        <is>
-          <t>4071</t>
+      <c r="AE18" t="n">
+        <v>4071</v>
+      </c>
+      <c r="AF18" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AG18" t="inlineStr">
+        <is>
+          <t>4150</t>
         </is>
       </c>
     </row>
@@ -1889,9 +1957,15 @@
       <c r="AD19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE19" t="inlineStr">
-        <is>
-          <t>2821</t>
+      <c r="AE19" t="n">
+        <v>2821</v>
+      </c>
+      <c r="AF19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG19" t="inlineStr">
+        <is>
+          <t>2853</t>
         </is>
       </c>
     </row>
@@ -1992,9 +2066,15 @@
       <c r="AD20" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="AE20" t="inlineStr">
-        <is>
-          <t>4589</t>
+      <c r="AE20" t="n">
+        <v>4589</v>
+      </c>
+      <c r="AF20" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AG20" t="inlineStr">
+        <is>
+          <t>4692</t>
         </is>
       </c>
     </row>
@@ -2095,9 +2175,15 @@
       <c r="AD21" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="AE21" t="inlineStr">
-        <is>
-          <t>5188</t>
+      <c r="AE21" t="n">
+        <v>5188</v>
+      </c>
+      <c r="AF21" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AG21" t="inlineStr">
+        <is>
+          <t>5315</t>
         </is>
       </c>
     </row>
@@ -2198,9 +2284,15 @@
       <c r="AD22" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="AE22" t="inlineStr">
-        <is>
-          <t>5316</t>
+      <c r="AE22" t="n">
+        <v>5316</v>
+      </c>
+      <c r="AF22" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AG22" t="inlineStr">
+        <is>
+          <t>5499</t>
         </is>
       </c>
     </row>
@@ -2301,9 +2393,15 @@
       <c r="AD23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AE23" t="inlineStr">
-        <is>
-          <t>6064</t>
+      <c r="AE23" t="n">
+        <v>6064</v>
+      </c>
+      <c r="AF23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AG23" t="inlineStr">
+        <is>
+          <t>6225</t>
         </is>
       </c>
     </row>
@@ -2404,9 +2502,15 @@
       <c r="AD24" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AE24" t="inlineStr">
-        <is>
-          <t>5498</t>
+      <c r="AE24" t="n">
+        <v>5498</v>
+      </c>
+      <c r="AF24" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AG24" t="inlineStr">
+        <is>
+          <t>5621</t>
         </is>
       </c>
     </row>
@@ -2507,9 +2611,15 @@
       <c r="AD25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AE25" t="inlineStr">
-        <is>
-          <t>5940</t>
+      <c r="AE25" t="n">
+        <v>5940</v>
+      </c>
+      <c r="AF25" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG25" t="inlineStr">
+        <is>
+          <t>6131</t>
         </is>
       </c>
     </row>
@@ -2610,9 +2720,15 @@
       <c r="AD26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE26" t="inlineStr">
-        <is>
-          <t>2965</t>
+      <c r="AE26" t="n">
+        <v>2965</v>
+      </c>
+      <c r="AF26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG26" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2713,9 +2829,15 @@
       <c r="AD27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE27" t="inlineStr">
-        <is>
-          <t>2532</t>
+      <c r="AE27" t="n">
+        <v>2532</v>
+      </c>
+      <c r="AF27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG27" t="inlineStr">
+        <is>
+          <t>2564</t>
         </is>
       </c>
     </row>
@@ -2771,6 +2893,8 @@
       <c r="AC28" t="inlineStr"/>
       <c r="AD28" s="4" t="inlineStr"/>
       <c r="AE28" t="inlineStr"/>
+      <c r="AF28" s="4" t="inlineStr"/>
+      <c r="AG28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2869,9 +2993,15 @@
       <c r="AD29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE29" t="inlineStr">
-        <is>
-          <t>3625</t>
+      <c r="AE29" t="n">
+        <v>3625</v>
+      </c>
+      <c r="AF29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG29" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2972,9 +3102,15 @@
       <c r="AD30" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AE30" t="inlineStr">
-        <is>
-          <t>5398</t>
+      <c r="AE30" t="n">
+        <v>5398</v>
+      </c>
+      <c r="AF30" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AG30" t="inlineStr">
+        <is>
+          <t>5403</t>
         </is>
       </c>
     </row>
@@ -3075,9 +3211,15 @@
       <c r="AD31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AE31" t="inlineStr">
-        <is>
-          <t>5421</t>
+      <c r="AE31" t="n">
+        <v>5421</v>
+      </c>
+      <c r="AF31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG31" t="inlineStr">
+        <is>
+          <t>5559</t>
         </is>
       </c>
     </row>
@@ -3178,9 +3320,15 @@
       <c r="AD32" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE32" t="inlineStr">
-        <is>
-          <t>4377</t>
+      <c r="AE32" t="n">
+        <v>4377</v>
+      </c>
+      <c r="AF32" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="AG32" t="inlineStr">
+        <is>
+          <t>4660</t>
         </is>
       </c>
     </row>
@@ -3248,6 +3396,8 @@
       <c r="AC33" t="inlineStr"/>
       <c r="AD33" s="4" t="inlineStr"/>
       <c r="AE33" t="inlineStr"/>
+      <c r="AF33" s="4" t="inlineStr"/>
+      <c r="AG33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3346,9 +3496,15 @@
       <c r="AD34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE34" t="inlineStr">
-        <is>
-          <t>2546</t>
+      <c r="AE34" t="n">
+        <v>2546</v>
+      </c>
+      <c r="AF34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG34" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3449,9 +3605,15 @@
       <c r="AD35" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE35" t="inlineStr">
-        <is>
-          <t>5205</t>
+      <c r="AE35" t="n">
+        <v>5205</v>
+      </c>
+      <c r="AF35" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG35" t="inlineStr">
+        <is>
+          <t>5280</t>
         </is>
       </c>
     </row>
@@ -3552,9 +3714,15 @@
       <c r="AD36" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE36" t="inlineStr">
-        <is>
-          <t>4480</t>
+      <c r="AE36" t="n">
+        <v>4480</v>
+      </c>
+      <c r="AF36" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AG36" t="inlineStr">
+        <is>
+          <t>4602</t>
         </is>
       </c>
     </row>
@@ -3655,9 +3823,15 @@
       <c r="AD37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AE37" t="inlineStr">
-        <is>
-          <t>5120</t>
+      <c r="AE37" t="n">
+        <v>5120</v>
+      </c>
+      <c r="AF37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG37" t="inlineStr">
+        <is>
+          <t>5212</t>
         </is>
       </c>
     </row>
@@ -3758,9 +3932,15 @@
       <c r="AD38" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AE38" t="inlineStr">
-        <is>
-          <t>5779</t>
+      <c r="AE38" t="n">
+        <v>5779</v>
+      </c>
+      <c r="AF38" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AG38" t="inlineStr">
+        <is>
+          <t>5944</t>
         </is>
       </c>
     </row>
@@ -3861,9 +4041,15 @@
       <c r="AD39" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AE39" t="inlineStr">
-        <is>
-          <t>4919</t>
+      <c r="AE39" t="n">
+        <v>4919</v>
+      </c>
+      <c r="AF39" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG39" t="inlineStr">
+        <is>
+          <t>5094</t>
         </is>
       </c>
     </row>
@@ -3964,7 +4150,13 @@
       <c r="AD40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE40" t="inlineStr">
+      <c r="AE40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4067,9 +4259,15 @@
       <c r="AD41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE41" t="inlineStr">
-        <is>
-          <t>4603</t>
+      <c r="AE41" t="n">
+        <v>4603</v>
+      </c>
+      <c r="AF41" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG41" t="inlineStr">
+        <is>
+          <t>4655</t>
         </is>
       </c>
     </row>
@@ -4170,9 +4368,15 @@
       <c r="AD42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE42" t="inlineStr">
-        <is>
-          <t>3291</t>
+      <c r="AE42" t="n">
+        <v>3291</v>
+      </c>
+      <c r="AF42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG42" t="inlineStr">
+        <is>
+          <t>3365</t>
         </is>
       </c>
     </row>
@@ -4232,6 +4436,8 @@
       <c r="AC43" t="inlineStr"/>
       <c r="AD43" s="4" t="inlineStr"/>
       <c r="AE43" t="inlineStr"/>
+      <c r="AF43" s="4" t="inlineStr"/>
+      <c r="AG43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -4317,6 +4523,8 @@
       <c r="AC44" t="inlineStr"/>
       <c r="AD44" s="4" t="inlineStr"/>
       <c r="AE44" t="inlineStr"/>
+      <c r="AF44" s="4" t="inlineStr"/>
+      <c r="AG44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -4415,9 +4623,15 @@
       <c r="AD45" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE45" t="inlineStr">
-        <is>
-          <t>4194</t>
+      <c r="AE45" t="n">
+        <v>4194</v>
+      </c>
+      <c r="AF45" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG45" t="inlineStr">
+        <is>
+          <t>4261</t>
         </is>
       </c>
     </row>
@@ -4518,9 +4732,15 @@
       <c r="AD46" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="AE46" t="inlineStr">
-        <is>
-          <t>4455</t>
+      <c r="AE46" t="n">
+        <v>4455</v>
+      </c>
+      <c r="AF46" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG46" t="inlineStr">
+        <is>
+          <t>4580</t>
         </is>
       </c>
     </row>
@@ -4621,9 +4841,15 @@
       <c r="AD47" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AE47" t="inlineStr">
-        <is>
-          <t>5883</t>
+      <c r="AE47" t="n">
+        <v>5883</v>
+      </c>
+      <c r="AF47" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AG47" t="inlineStr">
+        <is>
+          <t>6060</t>
         </is>
       </c>
     </row>
@@ -4724,9 +4950,15 @@
       <c r="AD48" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AE48" t="inlineStr">
-        <is>
-          <t>5636</t>
+      <c r="AE48" t="n">
+        <v>5636</v>
+      </c>
+      <c r="AF48" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="AG48" t="inlineStr">
+        <is>
+          <t>5878</t>
         </is>
       </c>
     </row>
@@ -4827,9 +5059,15 @@
       <c r="AD49" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AE49" t="inlineStr">
-        <is>
-          <t>5082</t>
+      <c r="AE49" t="n">
+        <v>5082</v>
+      </c>
+      <c r="AF49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG49" t="inlineStr">
+        <is>
+          <t>5124</t>
         </is>
       </c>
     </row>
@@ -4930,9 +5168,15 @@
       <c r="AD50" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AE50" t="inlineStr">
-        <is>
-          <t>5386</t>
+      <c r="AE50" t="n">
+        <v>5386</v>
+      </c>
+      <c r="AF50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AG50" t="inlineStr">
+        <is>
+          <t>5546</t>
         </is>
       </c>
     </row>
@@ -5033,9 +5277,15 @@
       <c r="AD51" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="AE51" t="inlineStr">
-        <is>
-          <t>4584</t>
+      <c r="AE51" t="n">
+        <v>4584</v>
+      </c>
+      <c r="AF51" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG51" t="inlineStr">
+        <is>
+          <t>4957</t>
         </is>
       </c>
     </row>
@@ -5136,9 +5386,15 @@
       <c r="AD52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AE52" t="inlineStr">
-        <is>
-          <t>5681</t>
+      <c r="AE52" t="n">
+        <v>5681</v>
+      </c>
+      <c r="AF52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG52" t="inlineStr">
+        <is>
+          <t>5856</t>
         </is>
       </c>
     </row>
@@ -5239,9 +5495,15 @@
       <c r="AD53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE53" t="inlineStr">
-        <is>
-          <t>4158</t>
+      <c r="AE53" t="n">
+        <v>4158</v>
+      </c>
+      <c r="AF53" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AG53" t="inlineStr">
+        <is>
+          <t>4333</t>
         </is>
       </c>
     </row>
@@ -5342,9 +5604,15 @@
       <c r="AD54" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE54" t="inlineStr">
-        <is>
-          <t>5101</t>
+      <c r="AE54" t="n">
+        <v>5101</v>
+      </c>
+      <c r="AF54" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="AG54" t="inlineStr">
+        <is>
+          <t>5224</t>
         </is>
       </c>
     </row>
@@ -5445,9 +5713,15 @@
       <c r="AD55" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE55" t="inlineStr">
-        <is>
-          <t>4230</t>
+      <c r="AE55" t="n">
+        <v>4230</v>
+      </c>
+      <c r="AF55" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG55" t="inlineStr">
+        <is>
+          <t>4608</t>
         </is>
       </c>
     </row>
@@ -5548,9 +5822,15 @@
       <c r="AD56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AE56" t="inlineStr">
-        <is>
-          <t>5755</t>
+      <c r="AE56" t="n">
+        <v>5755</v>
+      </c>
+      <c r="AF56" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="AG56" t="inlineStr">
+        <is>
+          <t>5863</t>
         </is>
       </c>
     </row>
@@ -5651,9 +5931,15 @@
       <c r="AD57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE57" t="inlineStr">
-        <is>
-          <t>4458</t>
+      <c r="AE57" t="n">
+        <v>4458</v>
+      </c>
+      <c r="AF57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG57" t="inlineStr">
+        <is>
+          <t>4566</t>
         </is>
       </c>
     </row>
@@ -5754,9 +6040,15 @@
       <c r="AD58" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AE58" t="inlineStr">
-        <is>
-          <t>4577</t>
+      <c r="AE58" t="n">
+        <v>4577</v>
+      </c>
+      <c r="AF58" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG58" t="inlineStr">
+        <is>
+          <t>4539</t>
         </is>
       </c>
     </row>
@@ -5857,9 +6149,15 @@
       <c r="AD59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE59" t="inlineStr">
-        <is>
-          <t>4450</t>
+      <c r="AE59" t="n">
+        <v>4450</v>
+      </c>
+      <c r="AF59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG59" t="inlineStr">
+        <is>
+          <t>4513</t>
         </is>
       </c>
     </row>
@@ -5960,9 +6258,15 @@
       <c r="AD60" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AE60" t="inlineStr">
-        <is>
-          <t>4520</t>
+      <c r="AE60" t="n">
+        <v>4520</v>
+      </c>
+      <c r="AF60" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AG60" t="inlineStr">
+        <is>
+          <t>4574</t>
         </is>
       </c>
     </row>
@@ -6018,6 +6322,8 @@
       <c r="AC61" t="inlineStr"/>
       <c r="AD61" s="4" t="inlineStr"/>
       <c r="AE61" t="inlineStr"/>
+      <c r="AF61" s="4" t="inlineStr"/>
+      <c r="AG61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -6116,9 +6422,15 @@
       <c r="AD62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AE62" t="inlineStr">
-        <is>
-          <t>4091</t>
+      <c r="AE62" t="n">
+        <v>4091</v>
+      </c>
+      <c r="AF62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG62" t="inlineStr">
+        <is>
+          <t>4190</t>
         </is>
       </c>
     </row>
@@ -6219,9 +6531,15 @@
       <c r="AD63" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="AE63" t="inlineStr">
-        <is>
-          <t>4184</t>
+      <c r="AE63" t="n">
+        <v>4184</v>
+      </c>
+      <c r="AF63" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AG63" t="inlineStr">
+        <is>
+          <t>4209</t>
         </is>
       </c>
     </row>
@@ -6322,9 +6640,15 @@
       <c r="AD64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE64" t="inlineStr">
-        <is>
-          <t>4583</t>
+      <c r="AE64" t="n">
+        <v>4583</v>
+      </c>
+      <c r="AF64" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="AG64" t="inlineStr">
+        <is>
+          <t>4616</t>
         </is>
       </c>
     </row>
@@ -6425,9 +6749,15 @@
       <c r="AD65" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AE65" t="inlineStr">
-        <is>
-          <t>4061</t>
+      <c r="AE65" t="n">
+        <v>4061</v>
+      </c>
+      <c r="AF65" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG65" t="inlineStr">
+        <is>
+          <t>4046</t>
         </is>
       </c>
     </row>
@@ -6528,7 +6858,13 @@
       <c r="AD66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE66" t="inlineStr">
+      <c r="AE66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6631,7 +6967,13 @@
       <c r="AD67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE67" t="inlineStr">
+      <c r="AE67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6734,9 +7076,15 @@
       <c r="AD68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE68" t="inlineStr">
-        <is>
-          <t>2520</t>
+      <c r="AE68" t="n">
+        <v>2520</v>
+      </c>
+      <c r="AF68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG68" t="inlineStr">
+        <is>
+          <t>2517</t>
         </is>
       </c>
     </row>
@@ -6837,9 +7185,15 @@
       <c r="AD69" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AE69" t="inlineStr">
-        <is>
-          <t>3497</t>
+      <c r="AE69" t="n">
+        <v>3497</v>
+      </c>
+      <c r="AF69" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AG69" t="inlineStr">
+        <is>
+          <t>3936</t>
         </is>
       </c>
     </row>
@@ -6940,9 +7294,15 @@
       <c r="AD70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE70" t="inlineStr">
-        <is>
-          <t>1499</t>
+      <c r="AE70" t="n">
+        <v>1499</v>
+      </c>
+      <c r="AF70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG70" t="inlineStr">
+        <is>
+          <t>1525</t>
         </is>
       </c>
     </row>
@@ -7043,7 +7403,13 @@
       <c r="AD71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE71" t="inlineStr">
+      <c r="AE71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7146,7 +7512,13 @@
       <c r="AD72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE72" t="inlineStr">
+      <c r="AE72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7249,9 +7621,15 @@
       <c r="AD73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE73" t="inlineStr">
-        <is>
-          <t>2662</t>
+      <c r="AE73" t="n">
+        <v>2662</v>
+      </c>
+      <c r="AF73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG73" t="inlineStr">
+        <is>
+          <t>2689</t>
         </is>
       </c>
     </row>
@@ -7352,7 +7730,13 @@
       <c r="AD74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE74" t="inlineStr">
+      <c r="AE74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7455,7 +7839,13 @@
       <c r="AD75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE75" t="inlineStr">
+      <c r="AE75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7558,9 +7948,15 @@
       <c r="AD76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE76" t="inlineStr">
-        <is>
-          <t>4657</t>
+      <c r="AE76" t="n">
+        <v>4657</v>
+      </c>
+      <c r="AF76" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG76" t="inlineStr">
+        <is>
+          <t>4743</t>
         </is>
       </c>
     </row>
@@ -7661,9 +8057,15 @@
       <c r="AD77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE77" t="inlineStr">
-        <is>
-          <t>3982</t>
+      <c r="AE77" t="n">
+        <v>3982</v>
+      </c>
+      <c r="AF77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG77" t="inlineStr">
+        <is>
+          <t>4002</t>
         </is>
       </c>
     </row>
@@ -7764,9 +8166,15 @@
       <c r="AD78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE78" t="inlineStr">
-        <is>
-          <t>3181</t>
+      <c r="AE78" t="n">
+        <v>3181</v>
+      </c>
+      <c r="AF78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG78" t="inlineStr">
+        <is>
+          <t>3209</t>
         </is>
       </c>
     </row>
@@ -7867,9 +8275,15 @@
       <c r="AD79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE79" t="inlineStr">
-        <is>
-          <t>1300</t>
+      <c r="AE79" t="n">
+        <v>1300</v>
+      </c>
+      <c r="AF79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG79" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -7970,7 +8384,13 @@
       <c r="AD80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE80" t="inlineStr">
+      <c r="AE80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8073,9 +8493,15 @@
       <c r="AD81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE81" t="inlineStr">
-        <is>
-          <t>2729</t>
+      <c r="AE81" t="n">
+        <v>2729</v>
+      </c>
+      <c r="AF81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG81" t="inlineStr">
+        <is>
+          <t>2722</t>
         </is>
       </c>
     </row>
@@ -8176,7 +8602,13 @@
       <c r="AD82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE82" t="inlineStr">
+      <c r="AE82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8279,7 +8711,13 @@
       <c r="AD83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE83" t="inlineStr">
+      <c r="AE83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8382,9 +8820,15 @@
       <c r="AD84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE84" t="inlineStr">
-        <is>
-          <t>1498</t>
+      <c r="AE84" t="n">
+        <v>1498</v>
+      </c>
+      <c r="AF84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG84" t="inlineStr">
+        <is>
+          <t>1494</t>
         </is>
       </c>
     </row>
@@ -8485,7 +8929,13 @@
       <c r="AD85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE85" t="inlineStr">
+      <c r="AE85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8588,7 +9038,13 @@
       <c r="AD86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE86" t="inlineStr">
+      <c r="AE86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8691,7 +9147,13 @@
       <c r="AD87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE87" t="inlineStr">
+      <c r="AE87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8794,7 +9256,13 @@
       <c r="AD88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE88" t="inlineStr">
+      <c r="AE88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8897,7 +9365,13 @@
       <c r="AD89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE89" t="inlineStr">
+      <c r="AE89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9000,7 +9474,13 @@
       <c r="AD90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE90" t="inlineStr">
+      <c r="AE90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9103,7 +9583,13 @@
       <c r="AD91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE91" t="inlineStr">
+      <c r="AE91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9206,7 +9692,13 @@
       <c r="AD92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE92" t="inlineStr">
+      <c r="AE92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9309,7 +9801,13 @@
       <c r="AD93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE93" t="inlineStr">
+      <c r="AE93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9412,7 +9910,13 @@
       <c r="AD94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE94" t="inlineStr">
+      <c r="AE94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9515,7 +10019,13 @@
       <c r="AD95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE95" t="inlineStr">
+      <c r="AE95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9618,9 +10128,15 @@
       <c r="AD96" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AE96" t="inlineStr">
-        <is>
-          <t>3521</t>
+      <c r="AE96" t="n">
+        <v>3521</v>
+      </c>
+      <c r="AF96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG96" t="inlineStr">
+        <is>
+          <t>3509</t>
         </is>
       </c>
     </row>
@@ -9721,7 +10237,13 @@
       <c r="AD97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE97" t="inlineStr">
+      <c r="AE97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9824,7 +10346,13 @@
       <c r="AD98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE98" t="inlineStr">
+      <c r="AE98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9927,7 +10455,13 @@
       <c r="AD99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE99" t="inlineStr">
+      <c r="AE99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10030,7 +10564,13 @@
       <c r="AD100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE100" t="inlineStr">
+      <c r="AE100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10133,7 +10673,13 @@
       <c r="AD101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE101" t="inlineStr">
+      <c r="AE101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10236,7 +10782,13 @@
       <c r="AD102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE102" t="inlineStr">
+      <c r="AE102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10339,7 +10891,13 @@
       <c r="AD103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE103" t="inlineStr">
+      <c r="AE103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10442,7 +11000,13 @@
       <c r="AD104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE104" t="inlineStr">
+      <c r="AE104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10545,7 +11109,13 @@
       <c r="AD105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE105" t="inlineStr">
+      <c r="AE105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10595,6 +11165,8 @@
       <c r="AC106" t="inlineStr"/>
       <c r="AD106" s="4" t="inlineStr"/>
       <c r="AE106" t="inlineStr"/>
+      <c r="AF106" s="4" t="inlineStr"/>
+      <c r="AG106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -10640,6 +11212,8 @@
       <c r="AC107" t="inlineStr"/>
       <c r="AD107" s="4" t="inlineStr"/>
       <c r="AE107" t="inlineStr"/>
+      <c r="AF107" s="4" t="inlineStr"/>
+      <c r="AG107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -10685,6 +11259,8 @@
       <c r="AC108" t="inlineStr"/>
       <c r="AD108" s="4" t="inlineStr"/>
       <c r="AE108" t="inlineStr"/>
+      <c r="AF108" s="4" t="inlineStr"/>
+      <c r="AG108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -10730,6 +11306,8 @@
       <c r="AC109" t="inlineStr"/>
       <c r="AD109" s="4" t="inlineStr"/>
       <c r="AE109" t="inlineStr"/>
+      <c r="AF109" s="4" t="inlineStr"/>
+      <c r="AG109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -10775,6 +11353,8 @@
       <c r="AC110" t="inlineStr"/>
       <c r="AD110" s="4" t="inlineStr"/>
       <c r="AE110" t="inlineStr"/>
+      <c r="AF110" s="4" t="inlineStr"/>
+      <c r="AG110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -10820,6 +11400,8 @@
       <c r="AC111" t="inlineStr"/>
       <c r="AD111" s="4" t="inlineStr"/>
       <c r="AE111" t="inlineStr"/>
+      <c r="AF111" s="4" t="inlineStr"/>
+      <c r="AG111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -10865,6 +11447,8 @@
       <c r="AC112" t="inlineStr"/>
       <c r="AD112" s="4" t="inlineStr"/>
       <c r="AE112" t="inlineStr"/>
+      <c r="AF112" s="4" t="inlineStr"/>
+      <c r="AG112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -10910,6 +11494,8 @@
       <c r="AC113" t="inlineStr"/>
       <c r="AD113" s="4" t="inlineStr"/>
       <c r="AE113" t="inlineStr"/>
+      <c r="AF113" s="4" t="inlineStr"/>
+      <c r="AG113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -10955,6 +11541,8 @@
       <c r="AC114" t="inlineStr"/>
       <c r="AD114" s="4" t="inlineStr"/>
       <c r="AE114" t="inlineStr"/>
+      <c r="AF114" s="4" t="inlineStr"/>
+      <c r="AG114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -11030,6 +11618,8 @@
       <c r="AC115" t="inlineStr"/>
       <c r="AD115" s="4" t="inlineStr"/>
       <c r="AE115" t="inlineStr"/>
+      <c r="AF115" s="4" t="inlineStr"/>
+      <c r="AG115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -11105,6 +11695,8 @@
       <c r="AC116" t="inlineStr"/>
       <c r="AD116" s="4" t="inlineStr"/>
       <c r="AE116" t="inlineStr"/>
+      <c r="AF116" s="4" t="inlineStr"/>
+      <c r="AG116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -11180,6 +11772,8 @@
       <c r="AC117" t="inlineStr"/>
       <c r="AD117" s="4" t="inlineStr"/>
       <c r="AE117" t="inlineStr"/>
+      <c r="AF117" s="4" t="inlineStr"/>
+      <c r="AG117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -11268,9 +11862,15 @@
       <c r="AD118" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AE118" t="inlineStr">
-        <is>
-          <t>6133</t>
+      <c r="AE118" t="n">
+        <v>6133</v>
+      </c>
+      <c r="AF118" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG118" t="inlineStr">
+        <is>
+          <t>6477</t>
         </is>
       </c>
     </row>
@@ -11349,9 +11949,15 @@
       <c r="AD119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE119" t="inlineStr">
-        <is>
-          <t>1635</t>
+      <c r="AE119" t="n">
+        <v>1635</v>
+      </c>
+      <c r="AF119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG119" t="inlineStr">
+        <is>
+          <t>1633</t>
         </is>
       </c>
     </row>
@@ -11410,9 +12016,15 @@
       <c r="AD120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE120" t="inlineStr">
-        <is>
-          <t>1913</t>
+      <c r="AE120" t="n">
+        <v>1913</v>
+      </c>
+      <c r="AF120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG120" t="inlineStr">
+        <is>
+          <t>1909</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-08 07:18:45
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG120"/>
+  <dimension ref="A1:AI120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,6 +556,16 @@
           <t>05-06_0</t>
         </is>
       </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>05-07_A</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>05-07_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -660,7 +670,13 @@
       <c r="AF2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG2" t="inlineStr">
+      <c r="AG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI2" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -769,7 +785,13 @@
       <c r="AF3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG3" t="inlineStr">
+      <c r="AG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -878,7 +900,13 @@
       <c r="AF4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG4" t="inlineStr">
+      <c r="AG4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -987,7 +1015,13 @@
       <c r="AF5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG5" t="inlineStr">
+      <c r="AG5" t="n">
+        <v>2592</v>
+      </c>
+      <c r="AH5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI5" t="inlineStr">
         <is>
           <t>2592</t>
         </is>
@@ -1096,7 +1130,13 @@
       <c r="AF6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG6" t="inlineStr">
+      <c r="AG6" t="n">
+        <v>2801</v>
+      </c>
+      <c r="AH6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI6" t="inlineStr">
         <is>
           <t>2801</t>
         </is>
@@ -1160,6 +1200,8 @@
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" s="4" t="inlineStr"/>
       <c r="AG7" t="inlineStr"/>
+      <c r="AH7" s="4" t="inlineStr"/>
+      <c r="AI7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1219,6 +1261,8 @@
       <c r="AE8" t="inlineStr"/>
       <c r="AF8" s="4" t="inlineStr"/>
       <c r="AG8" t="inlineStr"/>
+      <c r="AH8" s="4" t="inlineStr"/>
+      <c r="AI8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1278,6 +1322,8 @@
       <c r="AE9" t="inlineStr"/>
       <c r="AF9" s="4" t="inlineStr"/>
       <c r="AG9" t="inlineStr"/>
+      <c r="AH9" s="4" t="inlineStr"/>
+      <c r="AI9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1337,6 +1383,8 @@
       <c r="AE10" t="inlineStr"/>
       <c r="AF10" s="4" t="inlineStr"/>
       <c r="AG10" t="inlineStr"/>
+      <c r="AH10" s="4" t="inlineStr"/>
+      <c r="AI10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1396,6 +1444,8 @@
       <c r="AE11" t="inlineStr"/>
       <c r="AF11" s="4" t="inlineStr"/>
       <c r="AG11" t="inlineStr"/>
+      <c r="AH11" s="4" t="inlineStr"/>
+      <c r="AI11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1455,6 +1505,8 @@
       <c r="AE12" t="inlineStr"/>
       <c r="AF12" s="4" t="inlineStr"/>
       <c r="AG12" t="inlineStr"/>
+      <c r="AH12" s="4" t="inlineStr"/>
+      <c r="AI12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1514,6 +1566,8 @@
       <c r="AE13" t="inlineStr"/>
       <c r="AF13" s="4" t="inlineStr"/>
       <c r="AG13" t="inlineStr"/>
+      <c r="AH13" s="4" t="inlineStr"/>
+      <c r="AI13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1573,6 +1627,8 @@
       <c r="AE14" t="inlineStr"/>
       <c r="AF14" s="4" t="inlineStr"/>
       <c r="AG14" t="inlineStr"/>
+      <c r="AH14" s="4" t="inlineStr"/>
+      <c r="AI14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1632,6 +1688,8 @@
       <c r="AE15" t="inlineStr"/>
       <c r="AF15" s="4" t="inlineStr"/>
       <c r="AG15" t="inlineStr"/>
+      <c r="AH15" s="4" t="inlineStr"/>
+      <c r="AI15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1691,6 +1749,8 @@
       <c r="AE16" t="inlineStr"/>
       <c r="AF16" s="4" t="inlineStr"/>
       <c r="AG16" t="inlineStr"/>
+      <c r="AH16" s="4" t="inlineStr"/>
+      <c r="AI16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1750,6 +1810,8 @@
       <c r="AE17" t="inlineStr"/>
       <c r="AF17" s="4" t="inlineStr"/>
       <c r="AG17" t="inlineStr"/>
+      <c r="AH17" s="4" t="inlineStr"/>
+      <c r="AI17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1854,7 +1916,13 @@
       <c r="AF18" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="AG18" t="inlineStr">
+      <c r="AG18" t="n">
+        <v>4150</v>
+      </c>
+      <c r="AH18" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AI18" t="inlineStr">
         <is>
           <t>4150</t>
         </is>
@@ -1963,7 +2031,13 @@
       <c r="AF19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG19" t="inlineStr">
+      <c r="AG19" t="n">
+        <v>2853</v>
+      </c>
+      <c r="AH19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI19" t="inlineStr">
         <is>
           <t>2853</t>
         </is>
@@ -2072,7 +2146,13 @@
       <c r="AF20" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AG20" t="inlineStr">
+      <c r="AG20" t="n">
+        <v>4692</v>
+      </c>
+      <c r="AH20" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AI20" t="inlineStr">
         <is>
           <t>4692</t>
         </is>
@@ -2181,7 +2261,13 @@
       <c r="AF21" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="AG21" t="inlineStr">
+      <c r="AG21" t="n">
+        <v>5315</v>
+      </c>
+      <c r="AH21" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AI21" t="inlineStr">
         <is>
           <t>5315</t>
         </is>
@@ -2290,7 +2376,13 @@
       <c r="AF22" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="AG22" t="inlineStr">
+      <c r="AG22" t="n">
+        <v>5499</v>
+      </c>
+      <c r="AH22" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AI22" t="inlineStr">
         <is>
           <t>5499</t>
         </is>
@@ -2399,7 +2491,13 @@
       <c r="AF23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AG23" t="inlineStr">
+      <c r="AG23" t="n">
+        <v>6225</v>
+      </c>
+      <c r="AH23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AI23" t="inlineStr">
         <is>
           <t>6225</t>
         </is>
@@ -2508,7 +2606,13 @@
       <c r="AF24" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AG24" t="inlineStr">
+      <c r="AG24" t="n">
+        <v>5621</v>
+      </c>
+      <c r="AH24" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AI24" t="inlineStr">
         <is>
           <t>5621</t>
         </is>
@@ -2617,7 +2721,13 @@
       <c r="AF25" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AG25" t="inlineStr">
+      <c r="AG25" t="n">
+        <v>6131</v>
+      </c>
+      <c r="AH25" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI25" t="inlineStr">
         <is>
           <t>6131</t>
         </is>
@@ -2726,7 +2836,13 @@
       <c r="AF26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG26" t="inlineStr">
+      <c r="AG26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI26" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2835,7 +2951,13 @@
       <c r="AF27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG27" t="inlineStr">
+      <c r="AG27" t="n">
+        <v>2564</v>
+      </c>
+      <c r="AH27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI27" t="inlineStr">
         <is>
           <t>2564</t>
         </is>
@@ -2895,6 +3017,8 @@
       <c r="AE28" t="inlineStr"/>
       <c r="AF28" s="4" t="inlineStr"/>
       <c r="AG28" t="inlineStr"/>
+      <c r="AH28" s="4" t="inlineStr"/>
+      <c r="AI28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2999,7 +3123,13 @@
       <c r="AF29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG29" t="inlineStr">
+      <c r="AG29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI29" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3108,7 +3238,13 @@
       <c r="AF30" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="AG30" t="inlineStr">
+      <c r="AG30" t="n">
+        <v>5403</v>
+      </c>
+      <c r="AH30" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AI30" t="inlineStr">
         <is>
           <t>5403</t>
         </is>
@@ -3217,7 +3353,13 @@
       <c r="AF31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AG31" t="inlineStr">
+      <c r="AG31" t="n">
+        <v>5559</v>
+      </c>
+      <c r="AH31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI31" t="inlineStr">
         <is>
           <t>5559</t>
         </is>
@@ -3326,7 +3468,13 @@
       <c r="AF32" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="AG32" t="inlineStr">
+      <c r="AG32" t="n">
+        <v>4660</v>
+      </c>
+      <c r="AH32" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="AI32" t="inlineStr">
         <is>
           <t>4660</t>
         </is>
@@ -3398,6 +3546,8 @@
       <c r="AE33" t="inlineStr"/>
       <c r="AF33" s="4" t="inlineStr"/>
       <c r="AG33" t="inlineStr"/>
+      <c r="AH33" s="4" t="inlineStr"/>
+      <c r="AI33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3502,7 +3652,13 @@
       <c r="AF34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG34" t="inlineStr">
+      <c r="AG34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3611,7 +3767,13 @@
       <c r="AF35" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AG35" t="inlineStr">
+      <c r="AG35" t="n">
+        <v>5280</v>
+      </c>
+      <c r="AH35" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI35" t="inlineStr">
         <is>
           <t>5280</t>
         </is>
@@ -3720,7 +3882,13 @@
       <c r="AF36" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="AG36" t="inlineStr">
+      <c r="AG36" t="n">
+        <v>4602</v>
+      </c>
+      <c r="AH36" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AI36" t="inlineStr">
         <is>
           <t>4602</t>
         </is>
@@ -3829,7 +3997,13 @@
       <c r="AF37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AG37" t="inlineStr">
+      <c r="AG37" t="n">
+        <v>5212</v>
+      </c>
+      <c r="AH37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI37" t="inlineStr">
         <is>
           <t>5212</t>
         </is>
@@ -3938,7 +4112,13 @@
       <c r="AF38" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AG38" t="inlineStr">
+      <c r="AG38" t="n">
+        <v>5944</v>
+      </c>
+      <c r="AH38" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AI38" t="inlineStr">
         <is>
           <t>5944</t>
         </is>
@@ -4047,7 +4227,13 @@
       <c r="AF39" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="AG39" t="inlineStr">
+      <c r="AG39" t="n">
+        <v>5094</v>
+      </c>
+      <c r="AH39" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AI39" t="inlineStr">
         <is>
           <t>5094</t>
         </is>
@@ -4156,7 +4342,13 @@
       <c r="AF40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG40" t="inlineStr">
+      <c r="AG40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4265,7 +4457,13 @@
       <c r="AF41" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="AG41" t="inlineStr">
+      <c r="AG41" t="n">
+        <v>4655</v>
+      </c>
+      <c r="AH41" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI41" t="inlineStr">
         <is>
           <t>4655</t>
         </is>
@@ -4374,7 +4572,13 @@
       <c r="AF42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG42" t="inlineStr">
+      <c r="AG42" t="n">
+        <v>3365</v>
+      </c>
+      <c r="AH42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI42" t="inlineStr">
         <is>
           <t>3365</t>
         </is>
@@ -4438,6 +4642,8 @@
       <c r="AE43" t="inlineStr"/>
       <c r="AF43" s="4" t="inlineStr"/>
       <c r="AG43" t="inlineStr"/>
+      <c r="AH43" s="4" t="inlineStr"/>
+      <c r="AI43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -4525,6 +4731,8 @@
       <c r="AE44" t="inlineStr"/>
       <c r="AF44" s="4" t="inlineStr"/>
       <c r="AG44" t="inlineStr"/>
+      <c r="AH44" s="4" t="inlineStr"/>
+      <c r="AI44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -4629,7 +4837,13 @@
       <c r="AF45" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AG45" t="inlineStr">
+      <c r="AG45" t="n">
+        <v>4261</v>
+      </c>
+      <c r="AH45" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI45" t="inlineStr">
         <is>
           <t>4261</t>
         </is>
@@ -4738,7 +4952,13 @@
       <c r="AF46" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="AG46" t="inlineStr">
+      <c r="AG46" t="n">
+        <v>4580</v>
+      </c>
+      <c r="AH46" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AI46" t="inlineStr">
         <is>
           <t>4580</t>
         </is>
@@ -4847,7 +5067,13 @@
       <c r="AF47" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AG47" t="inlineStr">
+      <c r="AG47" t="n">
+        <v>6060</v>
+      </c>
+      <c r="AH47" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI47" t="inlineStr">
         <is>
           <t>6060</t>
         </is>
@@ -4956,7 +5182,13 @@
       <c r="AF48" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="AG48" t="inlineStr">
+      <c r="AG48" t="n">
+        <v>5878</v>
+      </c>
+      <c r="AH48" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="AI48" t="inlineStr">
         <is>
           <t>5878</t>
         </is>
@@ -5065,7 +5297,13 @@
       <c r="AF49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG49" t="inlineStr">
+      <c r="AG49" t="n">
+        <v>5124</v>
+      </c>
+      <c r="AH49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI49" t="inlineStr">
         <is>
           <t>5124</t>
         </is>
@@ -5174,7 +5412,13 @@
       <c r="AF50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AG50" t="inlineStr">
+      <c r="AG50" t="n">
+        <v>5546</v>
+      </c>
+      <c r="AH50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AI50" t="inlineStr">
         <is>
           <t>5546</t>
         </is>
@@ -5283,7 +5527,13 @@
       <c r="AF51" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AG51" t="inlineStr">
+      <c r="AG51" t="n">
+        <v>4957</v>
+      </c>
+      <c r="AH51" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI51" t="inlineStr">
         <is>
           <t>4957</t>
         </is>
@@ -5392,7 +5642,13 @@
       <c r="AF52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AG52" t="inlineStr">
+      <c r="AG52" t="n">
+        <v>5856</v>
+      </c>
+      <c r="AH52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI52" t="inlineStr">
         <is>
           <t>5856</t>
         </is>
@@ -5501,7 +5757,13 @@
       <c r="AF53" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="AG53" t="inlineStr">
+      <c r="AG53" t="n">
+        <v>4333</v>
+      </c>
+      <c r="AH53" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AI53" t="inlineStr">
         <is>
           <t>4333</t>
         </is>
@@ -5610,7 +5872,13 @@
       <c r="AF54" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="AG54" t="inlineStr">
+      <c r="AG54" t="n">
+        <v>5224</v>
+      </c>
+      <c r="AH54" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="AI54" t="inlineStr">
         <is>
           <t>5224</t>
         </is>
@@ -5719,7 +5987,13 @@
       <c r="AF55" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AG55" t="inlineStr">
+      <c r="AG55" t="n">
+        <v>4608</v>
+      </c>
+      <c r="AH55" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI55" t="inlineStr">
         <is>
           <t>4608</t>
         </is>
@@ -5828,7 +6102,13 @@
       <c r="AF56" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="AG56" t="inlineStr">
+      <c r="AG56" t="n">
+        <v>5863</v>
+      </c>
+      <c r="AH56" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="AI56" t="inlineStr">
         <is>
           <t>5863</t>
         </is>
@@ -5937,7 +6217,13 @@
       <c r="AF57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AG57" t="inlineStr">
+      <c r="AG57" t="n">
+        <v>4566</v>
+      </c>
+      <c r="AH57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI57" t="inlineStr">
         <is>
           <t>4566</t>
         </is>
@@ -6046,7 +6332,13 @@
       <c r="AF58" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="AG58" t="inlineStr">
+      <c r="AG58" t="n">
+        <v>4539</v>
+      </c>
+      <c r="AH58" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI58" t="inlineStr">
         <is>
           <t>4539</t>
         </is>
@@ -6155,7 +6447,13 @@
       <c r="AF59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AG59" t="inlineStr">
+      <c r="AG59" t="n">
+        <v>4513</v>
+      </c>
+      <c r="AH59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI59" t="inlineStr">
         <is>
           <t>4513</t>
         </is>
@@ -6264,7 +6562,13 @@
       <c r="AF60" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AG60" t="inlineStr">
+      <c r="AG60" t="n">
+        <v>4574</v>
+      </c>
+      <c r="AH60" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AI60" t="inlineStr">
         <is>
           <t>4574</t>
         </is>
@@ -6324,6 +6628,8 @@
       <c r="AE61" t="inlineStr"/>
       <c r="AF61" s="4" t="inlineStr"/>
       <c r="AG61" t="inlineStr"/>
+      <c r="AH61" s="4" t="inlineStr"/>
+      <c r="AI61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -6428,7 +6734,13 @@
       <c r="AF62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AG62" t="inlineStr">
+      <c r="AG62" t="n">
+        <v>4190</v>
+      </c>
+      <c r="AH62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI62" t="inlineStr">
         <is>
           <t>4190</t>
         </is>
@@ -6537,7 +6849,13 @@
       <c r="AF63" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="AG63" t="inlineStr">
+      <c r="AG63" t="n">
+        <v>4209</v>
+      </c>
+      <c r="AH63" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AI63" t="inlineStr">
         <is>
           <t>4209</t>
         </is>
@@ -6646,7 +6964,13 @@
       <c r="AF64" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="AG64" t="inlineStr">
+      <c r="AG64" t="n">
+        <v>4616</v>
+      </c>
+      <c r="AH64" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="AI64" t="inlineStr">
         <is>
           <t>4616</t>
         </is>
@@ -6755,7 +7079,13 @@
       <c r="AF65" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AG65" t="inlineStr">
+      <c r="AG65" t="n">
+        <v>4046</v>
+      </c>
+      <c r="AH65" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI65" t="inlineStr">
         <is>
           <t>4046</t>
         </is>
@@ -6864,7 +7194,13 @@
       <c r="AF66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG66" t="inlineStr">
+      <c r="AG66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6973,7 +7309,13 @@
       <c r="AF67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG67" t="inlineStr">
+      <c r="AG67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7082,7 +7424,13 @@
       <c r="AF68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG68" t="inlineStr">
+      <c r="AG68" t="n">
+        <v>2517</v>
+      </c>
+      <c r="AH68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI68" t="inlineStr">
         <is>
           <t>2517</t>
         </is>
@@ -7191,7 +7539,13 @@
       <c r="AF69" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AG69" t="inlineStr">
+      <c r="AG69" t="n">
+        <v>3936</v>
+      </c>
+      <c r="AH69" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AI69" t="inlineStr">
         <is>
           <t>3936</t>
         </is>
@@ -7300,7 +7654,13 @@
       <c r="AF70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG70" t="inlineStr">
+      <c r="AG70" t="n">
+        <v>1525</v>
+      </c>
+      <c r="AH70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI70" t="inlineStr">
         <is>
           <t>1525</t>
         </is>
@@ -7409,7 +7769,13 @@
       <c r="AF71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG71" t="inlineStr">
+      <c r="AG71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7518,7 +7884,13 @@
       <c r="AF72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG72" t="inlineStr">
+      <c r="AG72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7627,7 +7999,13 @@
       <c r="AF73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG73" t="inlineStr">
+      <c r="AG73" t="n">
+        <v>2689</v>
+      </c>
+      <c r="AH73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI73" t="inlineStr">
         <is>
           <t>2689</t>
         </is>
@@ -7736,7 +8114,13 @@
       <c r="AF74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG74" t="inlineStr">
+      <c r="AG74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7845,7 +8229,13 @@
       <c r="AF75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG75" t="inlineStr">
+      <c r="AG75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7954,7 +8344,13 @@
       <c r="AF76" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="AG76" t="inlineStr">
+      <c r="AG76" t="n">
+        <v>4743</v>
+      </c>
+      <c r="AH76" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI76" t="inlineStr">
         <is>
           <t>4743</t>
         </is>
@@ -8063,7 +8459,13 @@
       <c r="AF77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG77" t="inlineStr">
+      <c r="AG77" t="n">
+        <v>4002</v>
+      </c>
+      <c r="AH77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI77" t="inlineStr">
         <is>
           <t>4002</t>
         </is>
@@ -8172,7 +8574,13 @@
       <c r="AF78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG78" t="inlineStr">
+      <c r="AG78" t="n">
+        <v>3209</v>
+      </c>
+      <c r="AH78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI78" t="inlineStr">
         <is>
           <t>3209</t>
         </is>
@@ -8281,7 +8689,13 @@
       <c r="AF79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG79" t="inlineStr">
+      <c r="AG79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8390,7 +8804,13 @@
       <c r="AF80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG80" t="inlineStr">
+      <c r="AG80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8499,7 +8919,13 @@
       <c r="AF81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG81" t="inlineStr">
+      <c r="AG81" t="n">
+        <v>2722</v>
+      </c>
+      <c r="AH81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI81" t="inlineStr">
         <is>
           <t>2722</t>
         </is>
@@ -8608,7 +9034,13 @@
       <c r="AF82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG82" t="inlineStr">
+      <c r="AG82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8717,7 +9149,13 @@
       <c r="AF83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG83" t="inlineStr">
+      <c r="AG83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8826,7 +9264,13 @@
       <c r="AF84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG84" t="inlineStr">
+      <c r="AG84" t="n">
+        <v>1494</v>
+      </c>
+      <c r="AH84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI84" t="inlineStr">
         <is>
           <t>1494</t>
         </is>
@@ -8935,7 +9379,13 @@
       <c r="AF85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG85" t="inlineStr">
+      <c r="AG85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9044,7 +9494,13 @@
       <c r="AF86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG86" t="inlineStr">
+      <c r="AG86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9153,7 +9609,13 @@
       <c r="AF87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG87" t="inlineStr">
+      <c r="AG87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9262,7 +9724,13 @@
       <c r="AF88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG88" t="inlineStr">
+      <c r="AG88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9371,7 +9839,13 @@
       <c r="AF89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG89" t="inlineStr">
+      <c r="AG89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9480,7 +9954,13 @@
       <c r="AF90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG90" t="inlineStr">
+      <c r="AG90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9589,7 +10069,13 @@
       <c r="AF91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG91" t="inlineStr">
+      <c r="AG91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9698,7 +10184,13 @@
       <c r="AF92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG92" t="inlineStr">
+      <c r="AG92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9807,7 +10299,13 @@
       <c r="AF93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG93" t="inlineStr">
+      <c r="AG93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9916,7 +10414,13 @@
       <c r="AF94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG94" t="inlineStr">
+      <c r="AG94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10025,7 +10529,13 @@
       <c r="AF95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG95" t="inlineStr">
+      <c r="AG95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10134,7 +10644,13 @@
       <c r="AF96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG96" t="inlineStr">
+      <c r="AG96" t="n">
+        <v>3509</v>
+      </c>
+      <c r="AH96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI96" t="inlineStr">
         <is>
           <t>3509</t>
         </is>
@@ -10243,7 +10759,13 @@
       <c r="AF97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG97" t="inlineStr">
+      <c r="AG97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10352,7 +10874,13 @@
       <c r="AF98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG98" t="inlineStr">
+      <c r="AG98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10461,7 +10989,13 @@
       <c r="AF99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG99" t="inlineStr">
+      <c r="AG99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10570,7 +11104,13 @@
       <c r="AF100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG100" t="inlineStr">
+      <c r="AG100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10679,7 +11219,13 @@
       <c r="AF101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG101" t="inlineStr">
+      <c r="AG101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10788,7 +11334,13 @@
       <c r="AF102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG102" t="inlineStr">
+      <c r="AG102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10897,7 +11449,13 @@
       <c r="AF103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG103" t="inlineStr">
+      <c r="AG103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11006,7 +11564,13 @@
       <c r="AF104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG104" t="inlineStr">
+      <c r="AG104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11115,7 +11679,13 @@
       <c r="AF105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG105" t="inlineStr">
+      <c r="AG105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11167,6 +11737,8 @@
       <c r="AE106" t="inlineStr"/>
       <c r="AF106" s="4" t="inlineStr"/>
       <c r="AG106" t="inlineStr"/>
+      <c r="AH106" s="4" t="inlineStr"/>
+      <c r="AI106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -11214,6 +11786,8 @@
       <c r="AE107" t="inlineStr"/>
       <c r="AF107" s="4" t="inlineStr"/>
       <c r="AG107" t="inlineStr"/>
+      <c r="AH107" s="4" t="inlineStr"/>
+      <c r="AI107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -11261,6 +11835,8 @@
       <c r="AE108" t="inlineStr"/>
       <c r="AF108" s="4" t="inlineStr"/>
       <c r="AG108" t="inlineStr"/>
+      <c r="AH108" s="4" t="inlineStr"/>
+      <c r="AI108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -11308,6 +11884,8 @@
       <c r="AE109" t="inlineStr"/>
       <c r="AF109" s="4" t="inlineStr"/>
       <c r="AG109" t="inlineStr"/>
+      <c r="AH109" s="4" t="inlineStr"/>
+      <c r="AI109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -11355,6 +11933,8 @@
       <c r="AE110" t="inlineStr"/>
       <c r="AF110" s="4" t="inlineStr"/>
       <c r="AG110" t="inlineStr"/>
+      <c r="AH110" s="4" t="inlineStr"/>
+      <c r="AI110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -11402,6 +11982,8 @@
       <c r="AE111" t="inlineStr"/>
       <c r="AF111" s="4" t="inlineStr"/>
       <c r="AG111" t="inlineStr"/>
+      <c r="AH111" s="4" t="inlineStr"/>
+      <c r="AI111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -11449,6 +12031,8 @@
       <c r="AE112" t="inlineStr"/>
       <c r="AF112" s="4" t="inlineStr"/>
       <c r="AG112" t="inlineStr"/>
+      <c r="AH112" s="4" t="inlineStr"/>
+      <c r="AI112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -11496,6 +12080,8 @@
       <c r="AE113" t="inlineStr"/>
       <c r="AF113" s="4" t="inlineStr"/>
       <c r="AG113" t="inlineStr"/>
+      <c r="AH113" s="4" t="inlineStr"/>
+      <c r="AI113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -11543,6 +12129,8 @@
       <c r="AE114" t="inlineStr"/>
       <c r="AF114" s="4" t="inlineStr"/>
       <c r="AG114" t="inlineStr"/>
+      <c r="AH114" s="4" t="inlineStr"/>
+      <c r="AI114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -11620,6 +12208,8 @@
       <c r="AE115" t="inlineStr"/>
       <c r="AF115" s="4" t="inlineStr"/>
       <c r="AG115" t="inlineStr"/>
+      <c r="AH115" s="4" t="inlineStr"/>
+      <c r="AI115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -11697,6 +12287,8 @@
       <c r="AE116" t="inlineStr"/>
       <c r="AF116" s="4" t="inlineStr"/>
       <c r="AG116" t="inlineStr"/>
+      <c r="AH116" s="4" t="inlineStr"/>
+      <c r="AI116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -11774,6 +12366,8 @@
       <c r="AE117" t="inlineStr"/>
       <c r="AF117" s="4" t="inlineStr"/>
       <c r="AG117" t="inlineStr"/>
+      <c r="AH117" s="4" t="inlineStr"/>
+      <c r="AI117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -11868,7 +12462,13 @@
       <c r="AF118" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="AG118" t="inlineStr">
+      <c r="AG118" t="n">
+        <v>6477</v>
+      </c>
+      <c r="AH118" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AI118" t="inlineStr">
         <is>
           <t>6477</t>
         </is>
@@ -11955,7 +12555,13 @@
       <c r="AF119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG119" t="inlineStr">
+      <c r="AG119" t="n">
+        <v>1633</v>
+      </c>
+      <c r="AH119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI119" t="inlineStr">
         <is>
           <t>1633</t>
         </is>
@@ -12022,7 +12628,13 @@
       <c r="AF120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG120" t="inlineStr">
+      <c r="AG120" t="n">
+        <v>1909</v>
+      </c>
+      <c r="AH120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI120" t="inlineStr">
         <is>
           <t>1909</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-05-08 11:30:56
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -678,7 +678,7 @@
       </c>
       <c r="AI2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="AI5" t="inlineStr">
         <is>
-          <t>2592</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="AI6" t="inlineStr">
         <is>
-          <t>2801</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1919,12 +1919,12 @@
       <c r="AG18" t="n">
         <v>4150</v>
       </c>
-      <c r="AH18" s="3" t="n">
-        <v>9</v>
+      <c r="AH18" s="4" t="n">
+        <v>20</v>
       </c>
       <c r="AI18" t="inlineStr">
         <is>
-          <t>4150</t>
+          <t>2780</t>
         </is>
       </c>
     </row>
@@ -2039,7 +2039,7 @@
       </c>
       <c r="AI19" t="inlineStr">
         <is>
-          <t>2853</t>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -2150,11 +2150,11 @@
         <v>4692</v>
       </c>
       <c r="AH20" s="4" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="AI20" t="inlineStr">
         <is>
-          <t>4692</t>
+          <t>2783</t>
         </is>
       </c>
     </row>
@@ -2264,12 +2264,12 @@
       <c r="AG21" t="n">
         <v>5315</v>
       </c>
-      <c r="AH21" s="4" t="n">
-        <v>24</v>
+      <c r="AH21" s="5" t="n">
+        <v>40</v>
       </c>
       <c r="AI21" t="inlineStr">
         <is>
-          <t>5315</t>
+          <t>2975</t>
         </is>
       </c>
     </row>
@@ -2380,11 +2380,11 @@
         <v>5499</v>
       </c>
       <c r="AH22" s="4" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="AI22" t="inlineStr">
         <is>
-          <t>5499</t>
+          <t>2814</t>
         </is>
       </c>
     </row>
@@ -2499,7 +2499,7 @@
       </c>
       <c r="AI23" t="inlineStr">
         <is>
-          <t>6225</t>
+          <t>2870</t>
         </is>
       </c>
     </row>
@@ -2610,11 +2610,11 @@
         <v>5621</v>
       </c>
       <c r="AH24" s="5" t="n">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="AI24" t="inlineStr">
         <is>
-          <t>5621</t>
+          <t>2938</t>
         </is>
       </c>
     </row>
@@ -2725,11 +2725,11 @@
         <v>6131</v>
       </c>
       <c r="AH25" s="4" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="AI25" t="inlineStr">
         <is>
-          <t>6131</t>
+          <t>2952</t>
         </is>
       </c>
     </row>
@@ -2959,7 +2959,7 @@
       </c>
       <c r="AI27" t="inlineStr">
         <is>
-          <t>2564</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3126,12 +3126,12 @@
       <c r="AG29" t="n">
         <v>0</v>
       </c>
-      <c r="AH29" s="2" t="n">
-        <v>0</v>
+      <c r="AH29" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="AI29" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2516</t>
         </is>
       </c>
     </row>
@@ -3241,12 +3241,12 @@
       <c r="AG30" t="n">
         <v>5403</v>
       </c>
-      <c r="AH30" s="3" t="n">
-        <v>6</v>
+      <c r="AH30" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AI30" t="inlineStr">
         <is>
-          <t>5403</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -3356,12 +3356,12 @@
       <c r="AG31" t="n">
         <v>5559</v>
       </c>
-      <c r="AH31" s="4" t="n">
-        <v>30</v>
+      <c r="AH31" s="5" t="n">
+        <v>34</v>
       </c>
       <c r="AI31" t="inlineStr">
         <is>
-          <t>5559</t>
+          <t>2995</t>
         </is>
       </c>
     </row>
@@ -3471,12 +3471,12 @@
       <c r="AG32" t="n">
         <v>4660</v>
       </c>
-      <c r="AH32" s="3" t="n">
-        <v>12</v>
+      <c r="AH32" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AI32" t="inlineStr">
         <is>
-          <t>4660</t>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -3773,10 +3773,8 @@
       <c r="AH35" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AI35" t="inlineStr">
-        <is>
-          <t>5280</t>
-        </is>
+      <c r="AI35" t="n">
+        <v>5280</v>
       </c>
     </row>
     <row r="36">
@@ -3885,12 +3883,12 @@
       <c r="AG36" t="n">
         <v>4602</v>
       </c>
-      <c r="AH36" s="3" t="n">
-        <v>8</v>
+      <c r="AH36" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AI36" t="inlineStr">
         <is>
-          <t>4602</t>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -4005,7 +4003,7 @@
       </c>
       <c r="AI37" t="inlineStr">
         <is>
-          <t>5212</t>
+          <t>2950</t>
         </is>
       </c>
     </row>
@@ -4116,11 +4114,11 @@
         <v>5944</v>
       </c>
       <c r="AH38" s="4" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AI38" t="inlineStr">
         <is>
-          <t>5944</t>
+          <t>2985</t>
         </is>
       </c>
     </row>
@@ -4231,11 +4229,11 @@
         <v>5094</v>
       </c>
       <c r="AH39" s="4" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="AI39" t="inlineStr">
         <is>
-          <t>5094</t>
+          <t>2890</t>
         </is>
       </c>
     </row>
@@ -4460,12 +4458,12 @@
       <c r="AG41" t="n">
         <v>4655</v>
       </c>
-      <c r="AH41" s="3" t="n">
-        <v>4</v>
+      <c r="AH41" s="4" t="n">
+        <v>20</v>
       </c>
       <c r="AI41" t="inlineStr">
         <is>
-          <t>4655</t>
+          <t>2927</t>
         </is>
       </c>
     </row>
@@ -4580,7 +4578,7 @@
       </c>
       <c r="AI42" t="inlineStr">
         <is>
-          <t>3365</t>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -4841,11 +4839,11 @@
         <v>4261</v>
       </c>
       <c r="AH45" s="4" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AI45" t="inlineStr">
         <is>
-          <t>4261</t>
+          <t>2667</t>
         </is>
       </c>
     </row>
@@ -4960,7 +4958,7 @@
       </c>
       <c r="AI46" t="inlineStr">
         <is>
-          <t>4580</t>
+          <t>2740</t>
         </is>
       </c>
     </row>
@@ -5070,12 +5068,12 @@
       <c r="AG47" t="n">
         <v>6060</v>
       </c>
-      <c r="AH47" s="5" t="n">
-        <v>33</v>
+      <c r="AH47" s="4" t="n">
+        <v>30</v>
       </c>
       <c r="AI47" t="inlineStr">
         <is>
-          <t>6060</t>
+          <t>3005</t>
         </is>
       </c>
     </row>
@@ -5186,11 +5184,11 @@
         <v>5878</v>
       </c>
       <c r="AH48" s="4" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="AI48" t="inlineStr">
         <is>
-          <t>5878</t>
+          <t>3015</t>
         </is>
       </c>
     </row>
@@ -5300,12 +5298,12 @@
       <c r="AG49" t="n">
         <v>5124</v>
       </c>
-      <c r="AH49" s="2" t="n">
-        <v>0</v>
+      <c r="AH49" s="4" t="n">
+        <v>30</v>
       </c>
       <c r="AI49" t="inlineStr">
         <is>
-          <t>5124</t>
+          <t>3048</t>
         </is>
       </c>
     </row>
@@ -5420,7 +5418,7 @@
       </c>
       <c r="AI50" t="inlineStr">
         <is>
-          <t>5546</t>
+          <t>2970</t>
         </is>
       </c>
     </row>
@@ -5530,12 +5528,12 @@
       <c r="AG51" t="n">
         <v>4957</v>
       </c>
-      <c r="AH51" s="4" t="n">
-        <v>20</v>
+      <c r="AH51" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AI51" t="inlineStr">
         <is>
-          <t>4957</t>
+          <t>2573</t>
         </is>
       </c>
     </row>
@@ -5650,7 +5648,7 @@
       </c>
       <c r="AI52" t="inlineStr">
         <is>
-          <t>5856</t>
+          <t>3045</t>
         </is>
       </c>
     </row>
@@ -5761,11 +5759,11 @@
         <v>4333</v>
       </c>
       <c r="AH53" s="3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AI53" t="inlineStr">
         <is>
-          <t>4333</t>
+          <t>2689</t>
         </is>
       </c>
     </row>
@@ -5875,12 +5873,12 @@
       <c r="AG54" t="n">
         <v>5224</v>
       </c>
-      <c r="AH54" s="3" t="n">
-        <v>14</v>
+      <c r="AH54" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AI54" t="inlineStr">
         <is>
-          <t>5224</t>
+          <t>2518</t>
         </is>
       </c>
     </row>
@@ -5990,12 +5988,12 @@
       <c r="AG55" t="n">
         <v>4608</v>
       </c>
-      <c r="AH55" s="4" t="n">
-        <v>20</v>
+      <c r="AH55" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="AI55" t="inlineStr">
         <is>
-          <t>4608</t>
+          <t>2529</t>
         </is>
       </c>
     </row>
@@ -6106,11 +6104,11 @@
         <v>5863</v>
       </c>
       <c r="AH56" s="4" t="n">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="AI56" t="inlineStr">
         <is>
-          <t>5863</t>
+          <t>3091</t>
         </is>
       </c>
     </row>
@@ -6225,7 +6223,7 @@
       </c>
       <c r="AI57" t="inlineStr">
         <is>
-          <t>4566</t>
+          <t>2732</t>
         </is>
       </c>
     </row>
@@ -6335,12 +6333,12 @@
       <c r="AG58" t="n">
         <v>4539</v>
       </c>
-      <c r="AH58" s="3" t="n">
-        <v>2</v>
+      <c r="AH58" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AI58" t="inlineStr">
         <is>
-          <t>4539</t>
+          <t>2587</t>
         </is>
       </c>
     </row>
@@ -6455,7 +6453,7 @@
       </c>
       <c r="AI59" t="inlineStr">
         <is>
-          <t>4513</t>
+          <t>2765</t>
         </is>
       </c>
     </row>
@@ -6566,11 +6564,11 @@
         <v>4574</v>
       </c>
       <c r="AH60" s="4" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="AI60" t="inlineStr">
         <is>
-          <t>4574</t>
+          <t>2927</t>
         </is>
       </c>
     </row>
@@ -6742,7 +6740,7 @@
       </c>
       <c r="AI62" t="inlineStr">
         <is>
-          <t>4190</t>
+          <t>2752</t>
         </is>
       </c>
     </row>
@@ -6852,12 +6850,12 @@
       <c r="AG63" t="n">
         <v>4209</v>
       </c>
-      <c r="AH63" s="3" t="n">
-        <v>7</v>
+      <c r="AH63" s="4" t="n">
+        <v>20</v>
       </c>
       <c r="AI63" t="inlineStr">
         <is>
-          <t>4209</t>
+          <t>2787</t>
         </is>
       </c>
     </row>
@@ -6967,12 +6965,12 @@
       <c r="AG64" t="n">
         <v>4616</v>
       </c>
-      <c r="AH64" s="3" t="n">
-        <v>15</v>
+      <c r="AH64" s="4" t="n">
+        <v>20</v>
       </c>
       <c r="AI64" t="inlineStr">
         <is>
-          <t>4616</t>
+          <t>2866</t>
         </is>
       </c>
     </row>
@@ -7083,11 +7081,11 @@
         <v>4046</v>
       </c>
       <c r="AH65" s="4" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="AI65" t="inlineStr">
         <is>
-          <t>4046</t>
+          <t>2729</t>
         </is>
       </c>
     </row>
@@ -7432,7 +7430,7 @@
       </c>
       <c r="AI68" t="inlineStr">
         <is>
-          <t>2517</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -7542,12 +7540,12 @@
       <c r="AG69" t="n">
         <v>3936</v>
       </c>
-      <c r="AH69" s="4" t="n">
-        <v>21</v>
+      <c r="AH69" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AI69" t="inlineStr">
         <is>
-          <t>3936</t>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -7662,7 +7660,7 @@
       </c>
       <c r="AI70" t="inlineStr">
         <is>
-          <t>1525</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -8007,7 +8005,7 @@
       </c>
       <c r="AI73" t="inlineStr">
         <is>
-          <t>2689</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -8348,11 +8346,11 @@
         <v>4743</v>
       </c>
       <c r="AH76" s="3" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AI76" t="inlineStr">
         <is>
-          <t>4743</t>
+          <t>2594</t>
         </is>
       </c>
     </row>
@@ -8467,7 +8465,7 @@
       </c>
       <c r="AI77" t="inlineStr">
         <is>
-          <t>4002</t>
+          <t>2519</t>
         </is>
       </c>
     </row>
@@ -8582,7 +8580,7 @@
       </c>
       <c r="AI78" t="inlineStr">
         <is>
-          <t>3209</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -8927,7 +8925,7 @@
       </c>
       <c r="AI81" t="inlineStr">
         <is>
-          <t>2722</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -9157,7 +9155,7 @@
       </c>
       <c r="AI83" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2514</t>
         </is>
       </c>
     </row>
@@ -9272,7 +9270,7 @@
       </c>
       <c r="AI84" t="inlineStr">
         <is>
-          <t>1494</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -9962,7 +9960,7 @@
       </c>
       <c r="AI90" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
@@ -10652,7 +10650,7 @@
       </c>
       <c r="AI96" t="inlineStr">
         <is>
-          <t>3509</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -12466,11 +12464,11 @@
         <v>6477</v>
       </c>
       <c r="AH118" s="4" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="AI118" t="inlineStr">
         <is>
-          <t>6477</t>
+          <t>2858</t>
         </is>
       </c>
     </row>
@@ -12563,7 +12561,7 @@
       </c>
       <c r="AI119" t="inlineStr">
         <is>
-          <t>1633</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -12636,7 +12634,7 @@
       </c>
       <c r="AI120" t="inlineStr">
         <is>
-          <t>1909</t>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-09 11:30:56
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI120"/>
+  <dimension ref="A1:AK122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,6 +566,16 @@
           <t>05-07_0</t>
         </is>
       </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>05-08_A</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>05-08_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -676,7 +686,13 @@
       <c r="AH2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI2" t="inlineStr">
+      <c r="AI2" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AJ2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK2" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -791,7 +807,13 @@
       <c r="AH3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI3" t="inlineStr">
+      <c r="AI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -906,7 +928,13 @@
       <c r="AH4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI4" t="inlineStr">
+      <c r="AI4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1021,9 +1049,15 @@
       <c r="AH5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI5" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AI5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>2528</t>
         </is>
       </c>
     </row>
@@ -1136,7 +1170,13 @@
       <c r="AH6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI6" t="inlineStr">
+      <c r="AI6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1202,6 +1242,8 @@
       <c r="AG7" t="inlineStr"/>
       <c r="AH7" s="4" t="inlineStr"/>
       <c r="AI7" t="inlineStr"/>
+      <c r="AJ7" s="4" t="inlineStr"/>
+      <c r="AK7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1263,6 +1305,8 @@
       <c r="AG8" t="inlineStr"/>
       <c r="AH8" s="4" t="inlineStr"/>
       <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" s="4" t="inlineStr"/>
+      <c r="AK8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1324,6 +1368,8 @@
       <c r="AG9" t="inlineStr"/>
       <c r="AH9" s="4" t="inlineStr"/>
       <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" s="4" t="inlineStr"/>
+      <c r="AK9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1385,6 +1431,8 @@
       <c r="AG10" t="inlineStr"/>
       <c r="AH10" s="4" t="inlineStr"/>
       <c r="AI10" t="inlineStr"/>
+      <c r="AJ10" s="4" t="inlineStr"/>
+      <c r="AK10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1446,6 +1494,8 @@
       <c r="AG11" t="inlineStr"/>
       <c r="AH11" s="4" t="inlineStr"/>
       <c r="AI11" t="inlineStr"/>
+      <c r="AJ11" s="4" t="inlineStr"/>
+      <c r="AK11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1507,6 +1557,8 @@
       <c r="AG12" t="inlineStr"/>
       <c r="AH12" s="4" t="inlineStr"/>
       <c r="AI12" t="inlineStr"/>
+      <c r="AJ12" s="4" t="inlineStr"/>
+      <c r="AK12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1568,6 +1620,8 @@
       <c r="AG13" t="inlineStr"/>
       <c r="AH13" s="4" t="inlineStr"/>
       <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" s="4" t="inlineStr"/>
+      <c r="AK13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1629,6 +1683,8 @@
       <c r="AG14" t="inlineStr"/>
       <c r="AH14" s="4" t="inlineStr"/>
       <c r="AI14" t="inlineStr"/>
+      <c r="AJ14" s="4" t="inlineStr"/>
+      <c r="AK14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1690,6 +1746,8 @@
       <c r="AG15" t="inlineStr"/>
       <c r="AH15" s="4" t="inlineStr"/>
       <c r="AI15" t="inlineStr"/>
+      <c r="AJ15" s="4" t="inlineStr"/>
+      <c r="AK15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1751,6 +1809,8 @@
       <c r="AG16" t="inlineStr"/>
       <c r="AH16" s="4" t="inlineStr"/>
       <c r="AI16" t="inlineStr"/>
+      <c r="AJ16" s="4" t="inlineStr"/>
+      <c r="AK16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1812,6 +1872,8 @@
       <c r="AG17" t="inlineStr"/>
       <c r="AH17" s="4" t="inlineStr"/>
       <c r="AI17" t="inlineStr"/>
+      <c r="AJ17" s="4" t="inlineStr"/>
+      <c r="AK17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1922,9 +1984,15 @@
       <c r="AH18" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AI18" t="inlineStr">
-        <is>
-          <t>2780</t>
+      <c r="AI18" t="n">
+        <v>2780</v>
+      </c>
+      <c r="AJ18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK18" t="inlineStr">
+        <is>
+          <t>2766</t>
         </is>
       </c>
     </row>
@@ -2037,9 +2105,15 @@
       <c r="AH19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI19" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="AI19" t="n">
+        <v>2498</v>
+      </c>
+      <c r="AJ19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK19" t="inlineStr">
+        <is>
+          <t>2544</t>
         </is>
       </c>
     </row>
@@ -2152,9 +2226,15 @@
       <c r="AH20" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AI20" t="inlineStr">
-        <is>
-          <t>2783</t>
+      <c r="AI20" t="n">
+        <v>2783</v>
+      </c>
+      <c r="AJ20" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="AK20" t="inlineStr">
+        <is>
+          <t>2987</t>
         </is>
       </c>
     </row>
@@ -2267,9 +2347,15 @@
       <c r="AH21" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AI21" t="inlineStr">
-        <is>
-          <t>2975</t>
+      <c r="AI21" t="n">
+        <v>2975</v>
+      </c>
+      <c r="AJ21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK21" t="inlineStr">
+        <is>
+          <t>2995</t>
         </is>
       </c>
     </row>
@@ -2382,9 +2468,15 @@
       <c r="AH22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AI22" t="inlineStr">
-        <is>
-          <t>2814</t>
+      <c r="AI22" t="n">
+        <v>2814</v>
+      </c>
+      <c r="AJ22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK22" t="inlineStr">
+        <is>
+          <t>3140</t>
         </is>
       </c>
     </row>
@@ -2497,9 +2589,15 @@
       <c r="AH23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AI23" t="inlineStr">
-        <is>
-          <t>2870</t>
+      <c r="AI23" t="n">
+        <v>2870</v>
+      </c>
+      <c r="AJ23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AK23" t="inlineStr">
+        <is>
+          <t>3217</t>
         </is>
       </c>
     </row>
@@ -2612,9 +2710,15 @@
       <c r="AH24" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AI24" t="inlineStr">
-        <is>
-          <t>2938</t>
+      <c r="AI24" t="n">
+        <v>2938</v>
+      </c>
+      <c r="AJ24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AK24" t="inlineStr">
+        <is>
+          <t>3319</t>
         </is>
       </c>
     </row>
@@ -2727,9 +2831,15 @@
       <c r="AH25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AI25" t="inlineStr">
-        <is>
-          <t>2952</t>
+      <c r="AI25" t="n">
+        <v>2952</v>
+      </c>
+      <c r="AJ25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK25" t="inlineStr">
+        <is>
+          <t>3329</t>
         </is>
       </c>
     </row>
@@ -2842,7 +2952,13 @@
       <c r="AH26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI26" t="inlineStr">
+      <c r="AI26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK26" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2957,7 +3073,13 @@
       <c r="AH27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI27" t="inlineStr">
+      <c r="AI27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3019,6 +3141,8 @@
       <c r="AG28" t="inlineStr"/>
       <c r="AH28" s="4" t="inlineStr"/>
       <c r="AI28" t="inlineStr"/>
+      <c r="AJ28" s="4" t="inlineStr"/>
+      <c r="AK28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -3129,9 +3253,15 @@
       <c r="AH29" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="AI29" t="inlineStr">
-        <is>
-          <t>2516</t>
+      <c r="AI29" t="n">
+        <v>2516</v>
+      </c>
+      <c r="AJ29" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK29" t="inlineStr">
+        <is>
+          <t>2836</t>
         </is>
       </c>
     </row>
@@ -3244,7 +3374,13 @@
       <c r="AH30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI30" t="inlineStr">
+      <c r="AI30" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AJ30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK30" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3359,9 +3495,15 @@
       <c r="AH31" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AI31" t="inlineStr">
-        <is>
-          <t>2995</t>
+      <c r="AI31" t="n">
+        <v>2995</v>
+      </c>
+      <c r="AJ31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK31" t="inlineStr">
+        <is>
+          <t>3436</t>
         </is>
       </c>
     </row>
@@ -3474,7 +3616,13 @@
       <c r="AH32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI32" t="inlineStr">
+      <c r="AI32" t="n">
+        <v>2498</v>
+      </c>
+      <c r="AJ32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK32" t="inlineStr">
         <is>
           <t>2498</t>
         </is>
@@ -3548,6 +3696,8 @@
       <c r="AG33" t="inlineStr"/>
       <c r="AH33" s="4" t="inlineStr"/>
       <c r="AI33" t="inlineStr"/>
+      <c r="AJ33" s="4" t="inlineStr"/>
+      <c r="AK33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3658,7 +3808,13 @@
       <c r="AH34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI34" t="inlineStr">
+      <c r="AI34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3683,7 +3839,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>一馆</t>
+          <t>总馆</t>
         </is>
       </c>
       <c r="F35" s="4" t="n">
@@ -3775,6 +3931,14 @@
       </c>
       <c r="AI35" t="n">
         <v>5280</v>
+      </c>
+      <c r="AJ35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK35" t="inlineStr">
+        <is>
+          <t>2877</t>
+        </is>
       </c>
     </row>
     <row r="36">
@@ -3886,9 +4050,15 @@
       <c r="AH36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI36" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="AI36" t="n">
+        <v>2499</v>
+      </c>
+      <c r="AJ36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK36" t="inlineStr">
+        <is>
+          <t>2496</t>
         </is>
       </c>
     </row>
@@ -4001,9 +4171,15 @@
       <c r="AH37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AI37" t="inlineStr">
-        <is>
-          <t>2950</t>
+      <c r="AI37" t="n">
+        <v>2950</v>
+      </c>
+      <c r="AJ37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK37" t="inlineStr">
+        <is>
+          <t>3269</t>
         </is>
       </c>
     </row>
@@ -4116,9 +4292,15 @@
       <c r="AH38" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AI38" t="inlineStr">
-        <is>
-          <t>2985</t>
+      <c r="AI38" t="n">
+        <v>2985</v>
+      </c>
+      <c r="AJ38" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AK38" t="inlineStr">
+        <is>
+          <t>3470</t>
         </is>
       </c>
     </row>
@@ -4231,9 +4413,15 @@
       <c r="AH39" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AI39" t="inlineStr">
-        <is>
-          <t>2890</t>
+      <c r="AI39" t="n">
+        <v>2890</v>
+      </c>
+      <c r="AJ39" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AK39" t="inlineStr">
+        <is>
+          <t>3283</t>
         </is>
       </c>
     </row>
@@ -4346,7 +4534,13 @@
       <c r="AH40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI40" t="inlineStr">
+      <c r="AI40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4461,9 +4655,15 @@
       <c r="AH41" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AI41" t="inlineStr">
-        <is>
-          <t>2927</t>
+      <c r="AI41" t="n">
+        <v>2927</v>
+      </c>
+      <c r="AJ41" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AK41" t="inlineStr">
+        <is>
+          <t>3087</t>
         </is>
       </c>
     </row>
@@ -4576,9 +4776,15 @@
       <c r="AH42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI42" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="AI42" t="n">
+        <v>2498</v>
+      </c>
+      <c r="AJ42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK42" t="inlineStr">
+        <is>
+          <t>2582</t>
         </is>
       </c>
     </row>
@@ -4642,6 +4848,8 @@
       <c r="AG43" t="inlineStr"/>
       <c r="AH43" s="4" t="inlineStr"/>
       <c r="AI43" t="inlineStr"/>
+      <c r="AJ43" s="4" t="inlineStr"/>
+      <c r="AK43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -4731,6 +4939,8 @@
       <c r="AG44" t="inlineStr"/>
       <c r="AH44" s="4" t="inlineStr"/>
       <c r="AI44" t="inlineStr"/>
+      <c r="AJ44" s="4" t="inlineStr"/>
+      <c r="AK44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -4841,9 +5051,15 @@
       <c r="AH45" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AI45" t="inlineStr">
-        <is>
-          <t>2667</t>
+      <c r="AI45" t="n">
+        <v>2667</v>
+      </c>
+      <c r="AJ45" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AK45" t="inlineStr">
+        <is>
+          <t>2855</t>
         </is>
       </c>
     </row>
@@ -4956,9 +5172,15 @@
       <c r="AH46" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="AI46" t="inlineStr">
-        <is>
-          <t>2740</t>
+      <c r="AI46" t="n">
+        <v>2740</v>
+      </c>
+      <c r="AJ46" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="AK46" t="inlineStr">
+        <is>
+          <t>2941</t>
         </is>
       </c>
     </row>
@@ -5071,9 +5293,15 @@
       <c r="AH47" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AI47" t="inlineStr">
-        <is>
-          <t>3005</t>
+      <c r="AI47" t="n">
+        <v>3005</v>
+      </c>
+      <c r="AJ47" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AK47" t="inlineStr">
+        <is>
+          <t>3519</t>
         </is>
       </c>
     </row>
@@ -5186,9 +5414,15 @@
       <c r="AH48" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AI48" t="inlineStr">
-        <is>
-          <t>3015</t>
+      <c r="AI48" t="n">
+        <v>3015</v>
+      </c>
+      <c r="AJ48" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK48" t="inlineStr">
+        <is>
+          <t>3531</t>
         </is>
       </c>
     </row>
@@ -5301,9 +5535,15 @@
       <c r="AH49" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AI49" t="inlineStr">
-        <is>
-          <t>3048</t>
+      <c r="AI49" t="n">
+        <v>3048</v>
+      </c>
+      <c r="AJ49" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK49" t="inlineStr">
+        <is>
+          <t>3490</t>
         </is>
       </c>
     </row>
@@ -5416,9 +5656,15 @@
       <c r="AH50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AI50" t="inlineStr">
-        <is>
-          <t>2970</t>
+      <c r="AI50" t="n">
+        <v>2970</v>
+      </c>
+      <c r="AJ50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AK50" t="inlineStr">
+        <is>
+          <t>3400</t>
         </is>
       </c>
     </row>
@@ -5531,9 +5777,15 @@
       <c r="AH51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI51" t="inlineStr">
-        <is>
-          <t>2573</t>
+      <c r="AI51" t="n">
+        <v>2573</v>
+      </c>
+      <c r="AJ51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK51" t="inlineStr">
+        <is>
+          <t>2636</t>
         </is>
       </c>
     </row>
@@ -5646,9 +5898,15 @@
       <c r="AH52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AI52" t="inlineStr">
-        <is>
-          <t>3045</t>
+      <c r="AI52" t="n">
+        <v>3045</v>
+      </c>
+      <c r="AJ52" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AK52" t="inlineStr">
+        <is>
+          <t>3502</t>
         </is>
       </c>
     </row>
@@ -5761,9 +6019,15 @@
       <c r="AH53" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="AI53" t="inlineStr">
-        <is>
-          <t>2689</t>
+      <c r="AI53" t="n">
+        <v>2689</v>
+      </c>
+      <c r="AJ53" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AK53" t="inlineStr">
+        <is>
+          <t>2797</t>
         </is>
       </c>
     </row>
@@ -5876,9 +6140,15 @@
       <c r="AH54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI54" t="inlineStr">
-        <is>
-          <t>2518</t>
+      <c r="AI54" t="n">
+        <v>2518</v>
+      </c>
+      <c r="AJ54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK54" t="inlineStr">
+        <is>
+          <t>2517</t>
         </is>
       </c>
     </row>
@@ -5991,9 +6261,15 @@
       <c r="AH55" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="AI55" t="inlineStr">
-        <is>
-          <t>2529</t>
+      <c r="AI55" t="n">
+        <v>2529</v>
+      </c>
+      <c r="AJ55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK55" t="inlineStr">
+        <is>
+          <t>2601</t>
         </is>
       </c>
     </row>
@@ -6106,9 +6382,15 @@
       <c r="AH56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AI56" t="inlineStr">
-        <is>
-          <t>3091</t>
+      <c r="AI56" t="n">
+        <v>3091</v>
+      </c>
+      <c r="AJ56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK56" t="inlineStr">
+        <is>
+          <t>3614</t>
         </is>
       </c>
     </row>
@@ -6221,9 +6503,15 @@
       <c r="AH57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AI57" t="inlineStr">
-        <is>
-          <t>2732</t>
+      <c r="AI57" t="n">
+        <v>2732</v>
+      </c>
+      <c r="AJ57" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="AK57" t="inlineStr">
+        <is>
+          <t>2987</t>
         </is>
       </c>
     </row>
@@ -6336,9 +6624,15 @@
       <c r="AH58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI58" t="inlineStr">
-        <is>
-          <t>2587</t>
+      <c r="AI58" t="n">
+        <v>2587</v>
+      </c>
+      <c r="AJ58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK58" t="inlineStr">
+        <is>
+          <t>2619</t>
         </is>
       </c>
     </row>
@@ -6451,9 +6745,15 @@
       <c r="AH59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AI59" t="inlineStr">
-        <is>
-          <t>2765</t>
+      <c r="AI59" t="n">
+        <v>2765</v>
+      </c>
+      <c r="AJ59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK59" t="inlineStr">
+        <is>
+          <t>3014</t>
         </is>
       </c>
     </row>
@@ -6566,9 +6866,15 @@
       <c r="AH60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AI60" t="inlineStr">
-        <is>
-          <t>2927</t>
+      <c r="AI60" t="n">
+        <v>2927</v>
+      </c>
+      <c r="AJ60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AK60" t="inlineStr">
+        <is>
+          <t>3263</t>
         </is>
       </c>
     </row>
@@ -6628,6 +6934,8 @@
       <c r="AG61" t="inlineStr"/>
       <c r="AH61" s="4" t="inlineStr"/>
       <c r="AI61" t="inlineStr"/>
+      <c r="AJ61" s="4" t="inlineStr"/>
+      <c r="AK61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -6738,9 +7046,15 @@
       <c r="AH62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AI62" t="inlineStr">
-        <is>
-          <t>2752</t>
+      <c r="AI62" t="n">
+        <v>2752</v>
+      </c>
+      <c r="AJ62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK62" t="inlineStr">
+        <is>
+          <t>2877</t>
         </is>
       </c>
     </row>
@@ -6853,9 +7167,15 @@
       <c r="AH63" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AI63" t="inlineStr">
-        <is>
-          <t>2787</t>
+      <c r="AI63" t="n">
+        <v>2787</v>
+      </c>
+      <c r="AJ63" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK63" t="inlineStr">
+        <is>
+          <t>3002</t>
         </is>
       </c>
     </row>
@@ -6968,9 +7288,15 @@
       <c r="AH64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AI64" t="inlineStr">
-        <is>
-          <t>2866</t>
+      <c r="AI64" t="n">
+        <v>2866</v>
+      </c>
+      <c r="AJ64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK64" t="inlineStr">
+        <is>
+          <t>3168</t>
         </is>
       </c>
     </row>
@@ -7083,9 +7409,15 @@
       <c r="AH65" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AI65" t="inlineStr">
-        <is>
-          <t>2729</t>
+      <c r="AI65" t="n">
+        <v>2729</v>
+      </c>
+      <c r="AJ65" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AK65" t="inlineStr">
+        <is>
+          <t>2872</t>
         </is>
       </c>
     </row>
@@ -7198,7 +7530,13 @@
       <c r="AH66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI66" t="inlineStr">
+      <c r="AI66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7313,7 +7651,13 @@
       <c r="AH67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI67" t="inlineStr">
+      <c r="AI67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7428,7 +7772,13 @@
       <c r="AH68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI68" t="inlineStr">
+      <c r="AI68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7543,7 +7893,13 @@
       <c r="AH69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI69" t="inlineStr">
+      <c r="AI69" t="n">
+        <v>2499</v>
+      </c>
+      <c r="AJ69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK69" t="inlineStr">
         <is>
           <t>2499</t>
         </is>
@@ -7658,7 +8014,13 @@
       <c r="AH70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI70" t="inlineStr">
+      <c r="AI70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7773,7 +8135,13 @@
       <c r="AH71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI71" t="inlineStr">
+      <c r="AI71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7888,7 +8256,13 @@
       <c r="AH72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI72" t="inlineStr">
+      <c r="AI72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8003,9 +8377,15 @@
       <c r="AH73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI73" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AI73" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK73" t="inlineStr">
+        <is>
+          <t>2513</t>
         </is>
       </c>
     </row>
@@ -8118,7 +8498,13 @@
       <c r="AH74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI74" t="inlineStr">
+      <c r="AI74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8233,7 +8619,13 @@
       <c r="AH75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI75" t="inlineStr">
+      <c r="AI75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8348,9 +8740,15 @@
       <c r="AH76" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="AI76" t="inlineStr">
-        <is>
-          <t>2594</t>
+      <c r="AI76" t="n">
+        <v>2594</v>
+      </c>
+      <c r="AJ76" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AK76" t="inlineStr">
+        <is>
+          <t>2785</t>
         </is>
       </c>
     </row>
@@ -8463,9 +8861,15 @@
       <c r="AH77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI77" t="inlineStr">
-        <is>
-          <t>2519</t>
+      <c r="AI77" t="n">
+        <v>2519</v>
+      </c>
+      <c r="AJ77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK77" t="inlineStr">
+        <is>
+          <t>2514</t>
         </is>
       </c>
     </row>
@@ -8578,7 +8982,13 @@
       <c r="AH78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI78" t="inlineStr">
+      <c r="AI78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8693,9 +9103,15 @@
       <c r="AH79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI79" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AI79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK79" t="inlineStr">
+        <is>
+          <t>1300</t>
         </is>
       </c>
     </row>
@@ -8808,7 +9224,13 @@
       <c r="AH80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI80" t="inlineStr">
+      <c r="AI80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8923,7 +9345,13 @@
       <c r="AH81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI81" t="inlineStr">
+      <c r="AI81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9038,7 +9466,13 @@
       <c r="AH82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI82" t="inlineStr">
+      <c r="AI82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9153,9 +9587,15 @@
       <c r="AH83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI83" t="inlineStr">
-        <is>
-          <t>2514</t>
+      <c r="AI83" t="n">
+        <v>2514</v>
+      </c>
+      <c r="AJ83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK83" t="inlineStr">
+        <is>
+          <t>2511</t>
         </is>
       </c>
     </row>
@@ -9268,7 +9708,13 @@
       <c r="AH84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI84" t="inlineStr">
+      <c r="AI84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9383,7 +9829,13 @@
       <c r="AH85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI85" t="inlineStr">
+      <c r="AI85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9498,7 +9950,13 @@
       <c r="AH86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI86" t="inlineStr">
+      <c r="AI86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9613,7 +10071,13 @@
       <c r="AH87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI87" t="inlineStr">
+      <c r="AI87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9728,7 +10192,13 @@
       <c r="AH88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI88" t="inlineStr">
+      <c r="AI88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9843,7 +10313,13 @@
       <c r="AH89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI89" t="inlineStr">
+      <c r="AI89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9958,9 +10434,15 @@
       <c r="AH90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI90" t="inlineStr">
-        <is>
-          <t>1000</t>
+      <c r="AI90" t="n">
+        <v>1000</v>
+      </c>
+      <c r="AJ90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK90" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -10073,7 +10555,13 @@
       <c r="AH91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI91" t="inlineStr">
+      <c r="AI91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10188,7 +10676,13 @@
       <c r="AH92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI92" t="inlineStr">
+      <c r="AI92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10303,7 +10797,13 @@
       <c r="AH93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI93" t="inlineStr">
+      <c r="AI93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10418,7 +10918,13 @@
       <c r="AH94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI94" t="inlineStr">
+      <c r="AI94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10533,7 +11039,13 @@
       <c r="AH95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI95" t="inlineStr">
+      <c r="AI95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10648,9 +11160,15 @@
       <c r="AH96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI96" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AI96" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ96" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK96" t="inlineStr">
+        <is>
+          <t>2831</t>
         </is>
       </c>
     </row>
@@ -10763,7 +11281,13 @@
       <c r="AH97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI97" t="inlineStr">
+      <c r="AI97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10878,7 +11402,13 @@
       <c r="AH98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI98" t="inlineStr">
+      <c r="AI98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10993,7 +11523,13 @@
       <c r="AH99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI99" t="inlineStr">
+      <c r="AI99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11108,7 +11644,13 @@
       <c r="AH100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI100" t="inlineStr">
+      <c r="AI100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11223,7 +11765,13 @@
       <c r="AH101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI101" t="inlineStr">
+      <c r="AI101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11338,7 +11886,13 @@
       <c r="AH102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI102" t="inlineStr">
+      <c r="AI102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11453,7 +12007,13 @@
       <c r="AH103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI103" t="inlineStr">
+      <c r="AI103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11568,7 +12128,13 @@
       <c r="AH104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI104" t="inlineStr">
+      <c r="AI104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11683,7 +12249,13 @@
       <c r="AH105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI105" t="inlineStr">
+      <c r="AI105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11737,6 +12309,8 @@
       <c r="AG106" t="inlineStr"/>
       <c r="AH106" s="4" t="inlineStr"/>
       <c r="AI106" t="inlineStr"/>
+      <c r="AJ106" s="4" t="inlineStr"/>
+      <c r="AK106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -11786,6 +12360,8 @@
       <c r="AG107" t="inlineStr"/>
       <c r="AH107" s="4" t="inlineStr"/>
       <c r="AI107" t="inlineStr"/>
+      <c r="AJ107" s="4" t="inlineStr"/>
+      <c r="AK107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -11835,6 +12411,8 @@
       <c r="AG108" t="inlineStr"/>
       <c r="AH108" s="4" t="inlineStr"/>
       <c r="AI108" t="inlineStr"/>
+      <c r="AJ108" s="4" t="inlineStr"/>
+      <c r="AK108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -11884,6 +12462,8 @@
       <c r="AG109" t="inlineStr"/>
       <c r="AH109" s="4" t="inlineStr"/>
       <c r="AI109" t="inlineStr"/>
+      <c r="AJ109" s="4" t="inlineStr"/>
+      <c r="AK109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -11933,6 +12513,8 @@
       <c r="AG110" t="inlineStr"/>
       <c r="AH110" s="4" t="inlineStr"/>
       <c r="AI110" t="inlineStr"/>
+      <c r="AJ110" s="4" t="inlineStr"/>
+      <c r="AK110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -11982,6 +12564,8 @@
       <c r="AG111" t="inlineStr"/>
       <c r="AH111" s="4" t="inlineStr"/>
       <c r="AI111" t="inlineStr"/>
+      <c r="AJ111" s="4" t="inlineStr"/>
+      <c r="AK111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -12031,6 +12615,8 @@
       <c r="AG112" t="inlineStr"/>
       <c r="AH112" s="4" t="inlineStr"/>
       <c r="AI112" t="inlineStr"/>
+      <c r="AJ112" s="4" t="inlineStr"/>
+      <c r="AK112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -12080,6 +12666,8 @@
       <c r="AG113" t="inlineStr"/>
       <c r="AH113" s="4" t="inlineStr"/>
       <c r="AI113" t="inlineStr"/>
+      <c r="AJ113" s="4" t="inlineStr"/>
+      <c r="AK113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -12129,6 +12717,8 @@
       <c r="AG114" t="inlineStr"/>
       <c r="AH114" s="4" t="inlineStr"/>
       <c r="AI114" t="inlineStr"/>
+      <c r="AJ114" s="4" t="inlineStr"/>
+      <c r="AK114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -12208,6 +12798,8 @@
       <c r="AG115" t="inlineStr"/>
       <c r="AH115" s="4" t="inlineStr"/>
       <c r="AI115" t="inlineStr"/>
+      <c r="AJ115" s="4" t="inlineStr"/>
+      <c r="AK115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -12287,6 +12879,8 @@
       <c r="AG116" t="inlineStr"/>
       <c r="AH116" s="4" t="inlineStr"/>
       <c r="AI116" t="inlineStr"/>
+      <c r="AJ116" s="4" t="inlineStr"/>
+      <c r="AK116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -12366,6 +12960,8 @@
       <c r="AG117" t="inlineStr"/>
       <c r="AH117" s="4" t="inlineStr"/>
       <c r="AI117" t="inlineStr"/>
+      <c r="AJ117" s="4" t="inlineStr"/>
+      <c r="AK117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -12466,9 +13062,15 @@
       <c r="AH118" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AI118" t="inlineStr">
-        <is>
-          <t>2858</t>
+      <c r="AI118" t="n">
+        <v>2858</v>
+      </c>
+      <c r="AJ118" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AK118" t="inlineStr">
+        <is>
+          <t>3280</t>
         </is>
       </c>
     </row>
@@ -12559,9 +13161,15 @@
       <c r="AH119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI119" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AI119" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK119" t="inlineStr">
+        <is>
+          <t>1499</t>
         </is>
       </c>
     </row>
@@ -12632,9 +13240,129 @@
       <c r="AH120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI120" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AI120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ120" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK120" t="inlineStr">
+        <is>
+          <t>1778</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>138176</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Ze5kyphyr</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr"/>
+      <c r="D121" t="inlineStr"/>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F121" s="4" t="inlineStr"/>
+      <c r="G121" t="inlineStr"/>
+      <c r="H121" s="4" t="inlineStr"/>
+      <c r="I121" t="inlineStr"/>
+      <c r="J121" s="4" t="inlineStr"/>
+      <c r="K121" t="inlineStr"/>
+      <c r="L121" s="4" t="inlineStr"/>
+      <c r="M121" t="inlineStr"/>
+      <c r="N121" s="4" t="inlineStr"/>
+      <c r="O121" t="inlineStr"/>
+      <c r="P121" s="4" t="inlineStr"/>
+      <c r="Q121" t="inlineStr"/>
+      <c r="R121" s="4" t="inlineStr"/>
+      <c r="S121" t="inlineStr"/>
+      <c r="T121" s="4" t="inlineStr"/>
+      <c r="U121" t="inlineStr"/>
+      <c r="V121" s="4" t="inlineStr"/>
+      <c r="W121" t="inlineStr"/>
+      <c r="X121" s="4" t="inlineStr"/>
+      <c r="Y121" t="inlineStr"/>
+      <c r="Z121" s="4" t="inlineStr"/>
+      <c r="AA121" t="inlineStr"/>
+      <c r="AB121" s="4" t="inlineStr"/>
+      <c r="AC121" t="inlineStr"/>
+      <c r="AD121" s="4" t="inlineStr"/>
+      <c r="AE121" t="inlineStr"/>
+      <c r="AF121" s="4" t="inlineStr"/>
+      <c r="AG121" t="inlineStr"/>
+      <c r="AH121" s="4" t="inlineStr"/>
+      <c r="AI121" t="inlineStr"/>
+      <c r="AJ121" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AK121" t="inlineStr">
+        <is>
+          <t>3640</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>1976190</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>不要問問我是誰</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr"/>
+      <c r="D122" t="inlineStr"/>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F122" s="4" t="inlineStr"/>
+      <c r="G122" t="inlineStr"/>
+      <c r="H122" s="4" t="inlineStr"/>
+      <c r="I122" t="inlineStr"/>
+      <c r="J122" s="4" t="inlineStr"/>
+      <c r="K122" t="inlineStr"/>
+      <c r="L122" s="4" t="inlineStr"/>
+      <c r="M122" t="inlineStr"/>
+      <c r="N122" s="4" t="inlineStr"/>
+      <c r="O122" t="inlineStr"/>
+      <c r="P122" s="4" t="inlineStr"/>
+      <c r="Q122" t="inlineStr"/>
+      <c r="R122" s="4" t="inlineStr"/>
+      <c r="S122" t="inlineStr"/>
+      <c r="T122" s="4" t="inlineStr"/>
+      <c r="U122" t="inlineStr"/>
+      <c r="V122" s="4" t="inlineStr"/>
+      <c r="W122" t="inlineStr"/>
+      <c r="X122" s="4" t="inlineStr"/>
+      <c r="Y122" t="inlineStr"/>
+      <c r="Z122" s="4" t="inlineStr"/>
+      <c r="AA122" t="inlineStr"/>
+      <c r="AB122" s="4" t="inlineStr"/>
+      <c r="AC122" t="inlineStr"/>
+      <c r="AD122" s="4" t="inlineStr"/>
+      <c r="AE122" t="inlineStr"/>
+      <c r="AF122" s="4" t="inlineStr"/>
+      <c r="AG122" t="inlineStr"/>
+      <c r="AH122" s="4" t="inlineStr"/>
+      <c r="AI122" t="inlineStr"/>
+      <c r="AJ122" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK122" t="inlineStr">
+        <is>
+          <t>3085</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-09 12:23:34
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -13253,10 +13253,8 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>138176</t>
-        </is>
+      <c r="A121" t="n">
+        <v>138176</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
@@ -13310,10 +13308,8 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>1976190</t>
-        </is>
+      <c r="A122" t="n">
+        <v>1976190</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-05-10 09:24:33
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK122"/>
+  <dimension ref="A1:AM122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -576,6 +576,16 @@
           <t>05-08_0</t>
         </is>
       </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>05-09_A</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>05-09_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -692,7 +702,13 @@
       <c r="AJ2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK2" t="inlineStr">
+      <c r="AK2" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AL2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM2" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -813,7 +829,13 @@
       <c r="AJ3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK3" t="inlineStr">
+      <c r="AK3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -934,7 +956,13 @@
       <c r="AJ4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK4" t="inlineStr">
+      <c r="AK4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1055,7 +1083,13 @@
       <c r="AJ5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK5" t="inlineStr">
+      <c r="AK5" t="n">
+        <v>2528</v>
+      </c>
+      <c r="AL5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM5" t="inlineStr">
         <is>
           <t>2528</t>
         </is>
@@ -1176,7 +1210,13 @@
       <c r="AJ6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK6" t="inlineStr">
+      <c r="AK6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1244,6 +1284,8 @@
       <c r="AI7" t="inlineStr"/>
       <c r="AJ7" s="4" t="inlineStr"/>
       <c r="AK7" t="inlineStr"/>
+      <c r="AL7" s="4" t="inlineStr"/>
+      <c r="AM7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1307,6 +1349,8 @@
       <c r="AI8" t="inlineStr"/>
       <c r="AJ8" s="4" t="inlineStr"/>
       <c r="AK8" t="inlineStr"/>
+      <c r="AL8" s="4" t="inlineStr"/>
+      <c r="AM8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1370,6 +1414,8 @@
       <c r="AI9" t="inlineStr"/>
       <c r="AJ9" s="4" t="inlineStr"/>
       <c r="AK9" t="inlineStr"/>
+      <c r="AL9" s="4" t="inlineStr"/>
+      <c r="AM9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1433,6 +1479,8 @@
       <c r="AI10" t="inlineStr"/>
       <c r="AJ10" s="4" t="inlineStr"/>
       <c r="AK10" t="inlineStr"/>
+      <c r="AL10" s="4" t="inlineStr"/>
+      <c r="AM10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1496,6 +1544,8 @@
       <c r="AI11" t="inlineStr"/>
       <c r="AJ11" s="4" t="inlineStr"/>
       <c r="AK11" t="inlineStr"/>
+      <c r="AL11" s="4" t="inlineStr"/>
+      <c r="AM11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1559,6 +1609,8 @@
       <c r="AI12" t="inlineStr"/>
       <c r="AJ12" s="4" t="inlineStr"/>
       <c r="AK12" t="inlineStr"/>
+      <c r="AL12" s="4" t="inlineStr"/>
+      <c r="AM12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1622,6 +1674,8 @@
       <c r="AI13" t="inlineStr"/>
       <c r="AJ13" s="4" t="inlineStr"/>
       <c r="AK13" t="inlineStr"/>
+      <c r="AL13" s="4" t="inlineStr"/>
+      <c r="AM13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1685,6 +1739,8 @@
       <c r="AI14" t="inlineStr"/>
       <c r="AJ14" s="4" t="inlineStr"/>
       <c r="AK14" t="inlineStr"/>
+      <c r="AL14" s="4" t="inlineStr"/>
+      <c r="AM14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1748,6 +1804,8 @@
       <c r="AI15" t="inlineStr"/>
       <c r="AJ15" s="4" t="inlineStr"/>
       <c r="AK15" t="inlineStr"/>
+      <c r="AL15" s="4" t="inlineStr"/>
+      <c r="AM15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1811,6 +1869,8 @@
       <c r="AI16" t="inlineStr"/>
       <c r="AJ16" s="4" t="inlineStr"/>
       <c r="AK16" t="inlineStr"/>
+      <c r="AL16" s="4" t="inlineStr"/>
+      <c r="AM16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1874,6 +1934,8 @@
       <c r="AI17" t="inlineStr"/>
       <c r="AJ17" s="4" t="inlineStr"/>
       <c r="AK17" t="inlineStr"/>
+      <c r="AL17" s="4" t="inlineStr"/>
+      <c r="AM17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1990,7 +2052,13 @@
       <c r="AJ18" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK18" t="inlineStr">
+      <c r="AK18" t="n">
+        <v>2766</v>
+      </c>
+      <c r="AL18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM18" t="inlineStr">
         <is>
           <t>2766</t>
         </is>
@@ -2111,7 +2179,13 @@
       <c r="AJ19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK19" t="inlineStr">
+      <c r="AK19" t="n">
+        <v>2544</v>
+      </c>
+      <c r="AL19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM19" t="inlineStr">
         <is>
           <t>2544</t>
         </is>
@@ -2232,7 +2306,13 @@
       <c r="AJ20" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="AK20" t="inlineStr">
+      <c r="AK20" t="n">
+        <v>2987</v>
+      </c>
+      <c r="AL20" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="AM20" t="inlineStr">
         <is>
           <t>2987</t>
         </is>
@@ -2353,7 +2433,13 @@
       <c r="AJ21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK21" t="inlineStr">
+      <c r="AK21" t="n">
+        <v>2995</v>
+      </c>
+      <c r="AL21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM21" t="inlineStr">
         <is>
           <t>2995</t>
         </is>
@@ -2474,7 +2560,13 @@
       <c r="AJ22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AK22" t="inlineStr">
+      <c r="AK22" t="n">
+        <v>3140</v>
+      </c>
+      <c r="AL22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM22" t="inlineStr">
         <is>
           <t>3140</t>
         </is>
@@ -2595,7 +2687,13 @@
       <c r="AJ23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AK23" t="inlineStr">
+      <c r="AK23" t="n">
+        <v>3217</v>
+      </c>
+      <c r="AL23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AM23" t="inlineStr">
         <is>
           <t>3217</t>
         </is>
@@ -2716,7 +2814,13 @@
       <c r="AJ24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AK24" t="inlineStr">
+      <c r="AK24" t="n">
+        <v>3319</v>
+      </c>
+      <c r="AL24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM24" t="inlineStr">
         <is>
           <t>3319</t>
         </is>
@@ -2837,7 +2941,13 @@
       <c r="AJ25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AK25" t="inlineStr">
+      <c r="AK25" t="n">
+        <v>3329</v>
+      </c>
+      <c r="AL25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM25" t="inlineStr">
         <is>
           <t>3329</t>
         </is>
@@ -2958,7 +3068,13 @@
       <c r="AJ26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK26" t="inlineStr">
+      <c r="AK26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM26" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3079,7 +3195,13 @@
       <c r="AJ27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK27" t="inlineStr">
+      <c r="AK27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3143,6 +3265,8 @@
       <c r="AI28" t="inlineStr"/>
       <c r="AJ28" s="4" t="inlineStr"/>
       <c r="AK28" t="inlineStr"/>
+      <c r="AL28" s="4" t="inlineStr"/>
+      <c r="AM28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -3259,7 +3383,13 @@
       <c r="AJ29" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AK29" t="inlineStr">
+      <c r="AK29" t="n">
+        <v>2836</v>
+      </c>
+      <c r="AL29" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM29" t="inlineStr">
         <is>
           <t>2836</t>
         </is>
@@ -3380,7 +3510,13 @@
       <c r="AJ30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK30" t="inlineStr">
+      <c r="AK30" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AL30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM30" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3501,7 +3637,13 @@
       <c r="AJ31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AK31" t="inlineStr">
+      <c r="AK31" t="n">
+        <v>3436</v>
+      </c>
+      <c r="AL31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM31" t="inlineStr">
         <is>
           <t>3436</t>
         </is>
@@ -3622,7 +3764,13 @@
       <c r="AJ32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK32" t="inlineStr">
+      <c r="AK32" t="n">
+        <v>2498</v>
+      </c>
+      <c r="AL32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM32" t="inlineStr">
         <is>
           <t>2498</t>
         </is>
@@ -3698,6 +3846,8 @@
       <c r="AI33" t="inlineStr"/>
       <c r="AJ33" s="4" t="inlineStr"/>
       <c r="AK33" t="inlineStr"/>
+      <c r="AL33" s="4" t="inlineStr"/>
+      <c r="AM33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3814,7 +3964,13 @@
       <c r="AJ34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK34" t="inlineStr">
+      <c r="AK34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3935,7 +4091,13 @@
       <c r="AJ35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK35" t="inlineStr">
+      <c r="AK35" t="n">
+        <v>2877</v>
+      </c>
+      <c r="AL35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM35" t="inlineStr">
         <is>
           <t>2877</t>
         </is>
@@ -4056,7 +4218,13 @@
       <c r="AJ36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK36" t="inlineStr">
+      <c r="AK36" t="n">
+        <v>2496</v>
+      </c>
+      <c r="AL36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM36" t="inlineStr">
         <is>
           <t>2496</t>
         </is>
@@ -4177,7 +4345,13 @@
       <c r="AJ37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AK37" t="inlineStr">
+      <c r="AK37" t="n">
+        <v>3269</v>
+      </c>
+      <c r="AL37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM37" t="inlineStr">
         <is>
           <t>3269</t>
         </is>
@@ -4298,7 +4472,13 @@
       <c r="AJ38" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AK38" t="inlineStr">
+      <c r="AK38" t="n">
+        <v>3470</v>
+      </c>
+      <c r="AL38" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AM38" t="inlineStr">
         <is>
           <t>3470</t>
         </is>
@@ -4419,7 +4599,13 @@
       <c r="AJ39" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AK39" t="inlineStr">
+      <c r="AK39" t="n">
+        <v>3283</v>
+      </c>
+      <c r="AL39" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AM39" t="inlineStr">
         <is>
           <t>3283</t>
         </is>
@@ -4540,7 +4726,13 @@
       <c r="AJ40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK40" t="inlineStr">
+      <c r="AK40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4661,7 +4853,13 @@
       <c r="AJ41" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="AK41" t="inlineStr">
+      <c r="AK41" t="n">
+        <v>3087</v>
+      </c>
+      <c r="AL41" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AM41" t="inlineStr">
         <is>
           <t>3087</t>
         </is>
@@ -4782,7 +4980,13 @@
       <c r="AJ42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK42" t="inlineStr">
+      <c r="AK42" t="n">
+        <v>2582</v>
+      </c>
+      <c r="AL42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM42" t="inlineStr">
         <is>
           <t>2582</t>
         </is>
@@ -4850,6 +5054,8 @@
       <c r="AI43" t="inlineStr"/>
       <c r="AJ43" s="4" t="inlineStr"/>
       <c r="AK43" t="inlineStr"/>
+      <c r="AL43" s="4" t="inlineStr"/>
+      <c r="AM43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -4941,6 +5147,8 @@
       <c r="AI44" t="inlineStr"/>
       <c r="AJ44" s="4" t="inlineStr"/>
       <c r="AK44" t="inlineStr"/>
+      <c r="AL44" s="4" t="inlineStr"/>
+      <c r="AM44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -5057,7 +5265,13 @@
       <c r="AJ45" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AK45" t="inlineStr">
+      <c r="AK45" t="n">
+        <v>2855</v>
+      </c>
+      <c r="AL45" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AM45" t="inlineStr">
         <is>
           <t>2855</t>
         </is>
@@ -5178,7 +5392,13 @@
       <c r="AJ46" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="AK46" t="inlineStr">
+      <c r="AK46" t="n">
+        <v>2941</v>
+      </c>
+      <c r="AL46" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="AM46" t="inlineStr">
         <is>
           <t>2941</t>
         </is>
@@ -5299,7 +5519,13 @@
       <c r="AJ47" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AK47" t="inlineStr">
+      <c r="AK47" t="n">
+        <v>3519</v>
+      </c>
+      <c r="AL47" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AM47" t="inlineStr">
         <is>
           <t>3519</t>
         </is>
@@ -5420,7 +5646,13 @@
       <c r="AJ48" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AK48" t="inlineStr">
+      <c r="AK48" t="n">
+        <v>3531</v>
+      </c>
+      <c r="AL48" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM48" t="inlineStr">
         <is>
           <t>3531</t>
         </is>
@@ -5541,7 +5773,13 @@
       <c r="AJ49" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AK49" t="inlineStr">
+      <c r="AK49" t="n">
+        <v>3490</v>
+      </c>
+      <c r="AL49" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM49" t="inlineStr">
         <is>
           <t>3490</t>
         </is>
@@ -5662,7 +5900,13 @@
       <c r="AJ50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AK50" t="inlineStr">
+      <c r="AK50" t="n">
+        <v>3400</v>
+      </c>
+      <c r="AL50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AM50" t="inlineStr">
         <is>
           <t>3400</t>
         </is>
@@ -5783,7 +6027,13 @@
       <c r="AJ51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK51" t="inlineStr">
+      <c r="AK51" t="n">
+        <v>2636</v>
+      </c>
+      <c r="AL51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM51" t="inlineStr">
         <is>
           <t>2636</t>
         </is>
@@ -5904,7 +6154,13 @@
       <c r="AJ52" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AK52" t="inlineStr">
+      <c r="AK52" t="n">
+        <v>3502</v>
+      </c>
+      <c r="AL52" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AM52" t="inlineStr">
         <is>
           <t>3502</t>
         </is>
@@ -6025,7 +6281,13 @@
       <c r="AJ53" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="AK53" t="inlineStr">
+      <c r="AK53" t="n">
+        <v>2797</v>
+      </c>
+      <c r="AL53" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM53" t="inlineStr">
         <is>
           <t>2797</t>
         </is>
@@ -6146,7 +6408,13 @@
       <c r="AJ54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK54" t="inlineStr">
+      <c r="AK54" t="n">
+        <v>2517</v>
+      </c>
+      <c r="AL54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM54" t="inlineStr">
         <is>
           <t>2517</t>
         </is>
@@ -6267,7 +6535,13 @@
       <c r="AJ55" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK55" t="inlineStr">
+      <c r="AK55" t="n">
+        <v>2601</v>
+      </c>
+      <c r="AL55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM55" t="inlineStr">
         <is>
           <t>2601</t>
         </is>
@@ -6388,7 +6662,13 @@
       <c r="AJ56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AK56" t="inlineStr">
+      <c r="AK56" t="n">
+        <v>3614</v>
+      </c>
+      <c r="AL56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM56" t="inlineStr">
         <is>
           <t>3614</t>
         </is>
@@ -6509,7 +6789,13 @@
       <c r="AJ57" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="AK57" t="inlineStr">
+      <c r="AK57" t="n">
+        <v>2987</v>
+      </c>
+      <c r="AL57" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="AM57" t="inlineStr">
         <is>
           <t>2987</t>
         </is>
@@ -6630,7 +6916,13 @@
       <c r="AJ58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK58" t="inlineStr">
+      <c r="AK58" t="n">
+        <v>2619</v>
+      </c>
+      <c r="AL58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM58" t="inlineStr">
         <is>
           <t>2619</t>
         </is>
@@ -6751,7 +7043,13 @@
       <c r="AJ59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AK59" t="inlineStr">
+      <c r="AK59" t="n">
+        <v>3014</v>
+      </c>
+      <c r="AL59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM59" t="inlineStr">
         <is>
           <t>3014</t>
         </is>
@@ -6872,7 +7170,13 @@
       <c r="AJ60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AK60" t="inlineStr">
+      <c r="AK60" t="n">
+        <v>3263</v>
+      </c>
+      <c r="AL60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AM60" t="inlineStr">
         <is>
           <t>3263</t>
         </is>
@@ -6936,6 +7240,8 @@
       <c r="AI61" t="inlineStr"/>
       <c r="AJ61" s="4" t="inlineStr"/>
       <c r="AK61" t="inlineStr"/>
+      <c r="AL61" s="4" t="inlineStr"/>
+      <c r="AM61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -7052,7 +7358,13 @@
       <c r="AJ62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AK62" t="inlineStr">
+      <c r="AK62" t="n">
+        <v>2877</v>
+      </c>
+      <c r="AL62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM62" t="inlineStr">
         <is>
           <t>2877</t>
         </is>
@@ -7173,7 +7485,13 @@
       <c r="AJ63" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AK63" t="inlineStr">
+      <c r="AK63" t="n">
+        <v>3002</v>
+      </c>
+      <c r="AL63" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM63" t="inlineStr">
         <is>
           <t>3002</t>
         </is>
@@ -7294,7 +7612,13 @@
       <c r="AJ64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AK64" t="inlineStr">
+      <c r="AK64" t="n">
+        <v>3168</v>
+      </c>
+      <c r="AL64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM64" t="inlineStr">
         <is>
           <t>3168</t>
         </is>
@@ -7415,7 +7739,13 @@
       <c r="AJ65" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AK65" t="inlineStr">
+      <c r="AK65" t="n">
+        <v>2872</v>
+      </c>
+      <c r="AL65" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AM65" t="inlineStr">
         <is>
           <t>2872</t>
         </is>
@@ -7536,7 +7866,13 @@
       <c r="AJ66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK66" t="inlineStr">
+      <c r="AK66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7657,7 +7993,13 @@
       <c r="AJ67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK67" t="inlineStr">
+      <c r="AK67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7778,7 +8120,13 @@
       <c r="AJ68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK68" t="inlineStr">
+      <c r="AK68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7899,7 +8247,13 @@
       <c r="AJ69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK69" t="inlineStr">
+      <c r="AK69" t="n">
+        <v>2499</v>
+      </c>
+      <c r="AL69" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM69" t="inlineStr">
         <is>
           <t>2499</t>
         </is>
@@ -8020,7 +8374,13 @@
       <c r="AJ70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK70" t="inlineStr">
+      <c r="AK70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8141,7 +8501,13 @@
       <c r="AJ71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK71" t="inlineStr">
+      <c r="AK71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8262,7 +8628,13 @@
       <c r="AJ72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK72" t="inlineStr">
+      <c r="AK72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8383,7 +8755,13 @@
       <c r="AJ73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK73" t="inlineStr">
+      <c r="AK73" t="n">
+        <v>2513</v>
+      </c>
+      <c r="AL73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM73" t="inlineStr">
         <is>
           <t>2513</t>
         </is>
@@ -8504,7 +8882,13 @@
       <c r="AJ74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK74" t="inlineStr">
+      <c r="AK74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8625,7 +9009,13 @@
       <c r="AJ75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK75" t="inlineStr">
+      <c r="AK75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8746,7 +9136,13 @@
       <c r="AJ76" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="AK76" t="inlineStr">
+      <c r="AK76" t="n">
+        <v>2785</v>
+      </c>
+      <c r="AL76" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM76" t="inlineStr">
         <is>
           <t>2785</t>
         </is>
@@ -8867,7 +9263,13 @@
       <c r="AJ77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK77" t="inlineStr">
+      <c r="AK77" t="n">
+        <v>2514</v>
+      </c>
+      <c r="AL77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM77" t="inlineStr">
         <is>
           <t>2514</t>
         </is>
@@ -8988,7 +9390,13 @@
       <c r="AJ78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK78" t="inlineStr">
+      <c r="AK78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9109,7 +9517,13 @@
       <c r="AJ79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK79" t="inlineStr">
+      <c r="AK79" t="n">
+        <v>1300</v>
+      </c>
+      <c r="AL79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM79" t="inlineStr">
         <is>
           <t>1300</t>
         </is>
@@ -9230,7 +9644,13 @@
       <c r="AJ80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK80" t="inlineStr">
+      <c r="AK80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9351,7 +9771,13 @@
       <c r="AJ81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK81" t="inlineStr">
+      <c r="AK81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9472,7 +9898,13 @@
       <c r="AJ82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK82" t="inlineStr">
+      <c r="AK82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9593,7 +10025,13 @@
       <c r="AJ83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK83" t="inlineStr">
+      <c r="AK83" t="n">
+        <v>2511</v>
+      </c>
+      <c r="AL83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM83" t="inlineStr">
         <is>
           <t>2511</t>
         </is>
@@ -9714,7 +10152,13 @@
       <c r="AJ84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK84" t="inlineStr">
+      <c r="AK84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9835,7 +10279,13 @@
       <c r="AJ85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK85" t="inlineStr">
+      <c r="AK85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9956,7 +10406,13 @@
       <c r="AJ86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK86" t="inlineStr">
+      <c r="AK86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10077,7 +10533,13 @@
       <c r="AJ87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK87" t="inlineStr">
+      <c r="AK87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10198,7 +10660,13 @@
       <c r="AJ88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK88" t="inlineStr">
+      <c r="AK88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10319,7 +10787,13 @@
       <c r="AJ89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK89" t="inlineStr">
+      <c r="AK89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10440,7 +10914,13 @@
       <c r="AJ90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK90" t="inlineStr">
+      <c r="AK90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10561,7 +11041,13 @@
       <c r="AJ91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK91" t="inlineStr">
+      <c r="AK91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10682,7 +11168,13 @@
       <c r="AJ92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK92" t="inlineStr">
+      <c r="AK92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10803,7 +11295,13 @@
       <c r="AJ93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK93" t="inlineStr">
+      <c r="AK93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10924,7 +11422,13 @@
       <c r="AJ94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK94" t="inlineStr">
+      <c r="AK94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11045,7 +11549,13 @@
       <c r="AJ95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK95" t="inlineStr">
+      <c r="AK95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11166,7 +11676,13 @@
       <c r="AJ96" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AK96" t="inlineStr">
+      <c r="AK96" t="n">
+        <v>2831</v>
+      </c>
+      <c r="AL96" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM96" t="inlineStr">
         <is>
           <t>2831</t>
         </is>
@@ -11287,7 +11803,13 @@
       <c r="AJ97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK97" t="inlineStr">
+      <c r="AK97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11408,7 +11930,13 @@
       <c r="AJ98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK98" t="inlineStr">
+      <c r="AK98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11529,7 +12057,13 @@
       <c r="AJ99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK99" t="inlineStr">
+      <c r="AK99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11650,7 +12184,13 @@
       <c r="AJ100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK100" t="inlineStr">
+      <c r="AK100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11771,7 +12311,13 @@
       <c r="AJ101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK101" t="inlineStr">
+      <c r="AK101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11892,7 +12438,13 @@
       <c r="AJ102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK102" t="inlineStr">
+      <c r="AK102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12013,7 +12565,13 @@
       <c r="AJ103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK103" t="inlineStr">
+      <c r="AK103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12134,7 +12692,13 @@
       <c r="AJ104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK104" t="inlineStr">
+      <c r="AK104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12255,7 +12819,13 @@
       <c r="AJ105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK105" t="inlineStr">
+      <c r="AK105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12311,6 +12881,8 @@
       <c r="AI106" t="inlineStr"/>
       <c r="AJ106" s="4" t="inlineStr"/>
       <c r="AK106" t="inlineStr"/>
+      <c r="AL106" s="4" t="inlineStr"/>
+      <c r="AM106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -12362,6 +12934,8 @@
       <c r="AI107" t="inlineStr"/>
       <c r="AJ107" s="4" t="inlineStr"/>
       <c r="AK107" t="inlineStr"/>
+      <c r="AL107" s="4" t="inlineStr"/>
+      <c r="AM107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -12413,6 +12987,8 @@
       <c r="AI108" t="inlineStr"/>
       <c r="AJ108" s="4" t="inlineStr"/>
       <c r="AK108" t="inlineStr"/>
+      <c r="AL108" s="4" t="inlineStr"/>
+      <c r="AM108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -12464,6 +13040,8 @@
       <c r="AI109" t="inlineStr"/>
       <c r="AJ109" s="4" t="inlineStr"/>
       <c r="AK109" t="inlineStr"/>
+      <c r="AL109" s="4" t="inlineStr"/>
+      <c r="AM109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -12515,6 +13093,8 @@
       <c r="AI110" t="inlineStr"/>
       <c r="AJ110" s="4" t="inlineStr"/>
       <c r="AK110" t="inlineStr"/>
+      <c r="AL110" s="4" t="inlineStr"/>
+      <c r="AM110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -12566,6 +13146,8 @@
       <c r="AI111" t="inlineStr"/>
       <c r="AJ111" s="4" t="inlineStr"/>
       <c r="AK111" t="inlineStr"/>
+      <c r="AL111" s="4" t="inlineStr"/>
+      <c r="AM111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -12617,6 +13199,8 @@
       <c r="AI112" t="inlineStr"/>
       <c r="AJ112" s="4" t="inlineStr"/>
       <c r="AK112" t="inlineStr"/>
+      <c r="AL112" s="4" t="inlineStr"/>
+      <c r="AM112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -12668,6 +13252,8 @@
       <c r="AI113" t="inlineStr"/>
       <c r="AJ113" s="4" t="inlineStr"/>
       <c r="AK113" t="inlineStr"/>
+      <c r="AL113" s="4" t="inlineStr"/>
+      <c r="AM113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -12719,6 +13305,8 @@
       <c r="AI114" t="inlineStr"/>
       <c r="AJ114" s="4" t="inlineStr"/>
       <c r="AK114" t="inlineStr"/>
+      <c r="AL114" s="4" t="inlineStr"/>
+      <c r="AM114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -12800,6 +13388,8 @@
       <c r="AI115" t="inlineStr"/>
       <c r="AJ115" s="4" t="inlineStr"/>
       <c r="AK115" t="inlineStr"/>
+      <c r="AL115" s="4" t="inlineStr"/>
+      <c r="AM115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -12881,6 +13471,8 @@
       <c r="AI116" t="inlineStr"/>
       <c r="AJ116" s="4" t="inlineStr"/>
       <c r="AK116" t="inlineStr"/>
+      <c r="AL116" s="4" t="inlineStr"/>
+      <c r="AM116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -12962,6 +13554,8 @@
       <c r="AI117" t="inlineStr"/>
       <c r="AJ117" s="4" t="inlineStr"/>
       <c r="AK117" t="inlineStr"/>
+      <c r="AL117" s="4" t="inlineStr"/>
+      <c r="AM117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -13068,7 +13662,13 @@
       <c r="AJ118" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AK118" t="inlineStr">
+      <c r="AK118" t="n">
+        <v>3280</v>
+      </c>
+      <c r="AL118" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AM118" t="inlineStr">
         <is>
           <t>3280</t>
         </is>
@@ -13167,7 +13767,13 @@
       <c r="AJ119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK119" t="inlineStr">
+      <c r="AK119" t="n">
+        <v>1499</v>
+      </c>
+      <c r="AL119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM119" t="inlineStr">
         <is>
           <t>1499</t>
         </is>
@@ -13246,7 +13852,13 @@
       <c r="AJ120" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AK120" t="inlineStr">
+      <c r="AK120" t="n">
+        <v>1778</v>
+      </c>
+      <c r="AL120" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM120" t="inlineStr">
         <is>
           <t>1778</t>
         </is>
@@ -13301,7 +13913,13 @@
       <c r="AJ121" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AK121" t="inlineStr">
+      <c r="AK121" t="n">
+        <v>3640</v>
+      </c>
+      <c r="AL121" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AM121" t="inlineStr">
         <is>
           <t>3640</t>
         </is>
@@ -13356,7 +13974,13 @@
       <c r="AJ122" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AK122" t="inlineStr">
+      <c r="AK122" t="n">
+        <v>3085</v>
+      </c>
+      <c r="AL122" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM122" t="inlineStr">
         <is>
           <t>3085</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-05-10 11:30:55
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -710,7 +710,7 @@
       </c>
       <c r="AM2" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>2525</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="AM5" t="inlineStr">
         <is>
-          <t>2528</t>
+          <t>2535</t>
         </is>
       </c>
     </row>
@@ -1218,7 +1218,7 @@
       </c>
       <c r="AM6" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -2055,12 +2055,12 @@
       <c r="AK18" t="n">
         <v>2766</v>
       </c>
-      <c r="AL18" s="2" t="n">
-        <v>0</v>
+      <c r="AL18" s="4" t="n">
+        <v>20</v>
       </c>
       <c r="AM18" t="inlineStr">
         <is>
-          <t>2766</t>
+          <t>3083</t>
         </is>
       </c>
     </row>
@@ -2187,7 +2187,7 @@
       </c>
       <c r="AM19" t="inlineStr">
         <is>
-          <t>2544</t>
+          <t>2585</t>
         </is>
       </c>
     </row>
@@ -2310,11 +2310,11 @@
         <v>2987</v>
       </c>
       <c r="AL20" s="4" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="AM20" t="inlineStr">
         <is>
-          <t>2987</t>
+          <t>3279</t>
         </is>
       </c>
     </row>
@@ -2436,12 +2436,12 @@
       <c r="AK21" t="n">
         <v>2995</v>
       </c>
-      <c r="AL21" s="2" t="n">
-        <v>0</v>
+      <c r="AL21" s="5" t="n">
+        <v>38</v>
       </c>
       <c r="AM21" t="inlineStr">
         <is>
-          <t>2995</t>
+          <t>3407</t>
         </is>
       </c>
     </row>
@@ -2568,7 +2568,7 @@
       </c>
       <c r="AM22" t="inlineStr">
         <is>
-          <t>3140</t>
+          <t>3472</t>
         </is>
       </c>
     </row>
@@ -2695,7 +2695,7 @@
       </c>
       <c r="AM23" t="inlineStr">
         <is>
-          <t>3217</t>
+          <t>3617</t>
         </is>
       </c>
     </row>
@@ -2822,7 +2822,7 @@
       </c>
       <c r="AM24" t="inlineStr">
         <is>
-          <t>3319</t>
+          <t>3752</t>
         </is>
       </c>
     </row>
@@ -2945,11 +2945,11 @@
         <v>3329</v>
       </c>
       <c r="AL25" s="4" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AM25" t="inlineStr">
         <is>
-          <t>3329</t>
+          <t>3709</t>
         </is>
       </c>
     </row>
@@ -3076,7 +3076,7 @@
       </c>
       <c r="AM26" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -3203,7 +3203,7 @@
       </c>
       <c r="AM27" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -3386,12 +3386,12 @@
       <c r="AK29" t="n">
         <v>2836</v>
       </c>
-      <c r="AL29" s="4" t="n">
-        <v>20</v>
+      <c r="AL29" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="AM29" t="inlineStr">
         <is>
-          <t>2836</t>
+          <t>2866</t>
         </is>
       </c>
     </row>
@@ -3645,7 +3645,7 @@
       </c>
       <c r="AM31" t="inlineStr">
         <is>
-          <t>3436</t>
+          <t>3801</t>
         </is>
       </c>
     </row>
@@ -3767,12 +3767,12 @@
       <c r="AK32" t="n">
         <v>2498</v>
       </c>
-      <c r="AL32" s="2" t="n">
-        <v>0</v>
+      <c r="AL32" s="3" t="n">
+        <v>2</v>
       </c>
       <c r="AM32" t="inlineStr">
         <is>
-          <t>2498</t>
+          <t>2553</t>
         </is>
       </c>
     </row>
@@ -4099,7 +4099,7 @@
       </c>
       <c r="AM35" t="inlineStr">
         <is>
-          <t>2877</t>
+          <t>2944</t>
         </is>
       </c>
     </row>
@@ -4226,7 +4226,7 @@
       </c>
       <c r="AM36" t="inlineStr">
         <is>
-          <t>2496</t>
+          <t>2524</t>
         </is>
       </c>
     </row>
@@ -4353,7 +4353,7 @@
       </c>
       <c r="AM37" t="inlineStr">
         <is>
-          <t>3269</t>
+          <t>3638</t>
         </is>
       </c>
     </row>
@@ -4475,12 +4475,12 @@
       <c r="AK38" t="n">
         <v>3470</v>
       </c>
-      <c r="AL38" s="5" t="n">
-        <v>32</v>
+      <c r="AL38" s="4" t="n">
+        <v>30</v>
       </c>
       <c r="AM38" t="inlineStr">
         <is>
-          <t>3470</t>
+          <t>3891</t>
         </is>
       </c>
     </row>
@@ -4607,7 +4607,7 @@
       </c>
       <c r="AM39" t="inlineStr">
         <is>
-          <t>3283</t>
+          <t>3549</t>
         </is>
       </c>
     </row>
@@ -4857,11 +4857,11 @@
         <v>3087</v>
       </c>
       <c r="AL41" s="3" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="AM41" t="inlineStr">
         <is>
-          <t>3087</t>
+          <t>3250</t>
         </is>
       </c>
     </row>
@@ -4988,7 +4988,7 @@
       </c>
       <c r="AM42" t="inlineStr">
         <is>
-          <t>2582</t>
+          <t>2685</t>
         </is>
       </c>
     </row>
@@ -5269,11 +5269,11 @@
         <v>2855</v>
       </c>
       <c r="AL45" s="4" t="n">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="AM45" t="inlineStr">
         <is>
-          <t>2855</t>
+          <t>3072</t>
         </is>
       </c>
     </row>
@@ -5396,11 +5396,11 @@
         <v>2941</v>
       </c>
       <c r="AL46" s="3" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="AM46" t="inlineStr">
         <is>
-          <t>2941</t>
+          <t>3074</t>
         </is>
       </c>
     </row>
@@ -5523,11 +5523,11 @@
         <v>3519</v>
       </c>
       <c r="AL47" s="5" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="AM47" t="inlineStr">
         <is>
-          <t>3519</t>
+          <t>3987</t>
         </is>
       </c>
     </row>
@@ -5650,11 +5650,11 @@
         <v>3531</v>
       </c>
       <c r="AL48" s="4" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AM48" t="inlineStr">
         <is>
-          <t>3531</t>
+          <t>3985</t>
         </is>
       </c>
     </row>
@@ -5777,11 +5777,11 @@
         <v>3490</v>
       </c>
       <c r="AL49" s="4" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AM49" t="inlineStr">
         <is>
-          <t>3490</t>
+          <t>3771</t>
         </is>
       </c>
     </row>
@@ -5908,7 +5908,7 @@
       </c>
       <c r="AM50" t="inlineStr">
         <is>
-          <t>3400</t>
+          <t>3770</t>
         </is>
       </c>
     </row>
@@ -6035,7 +6035,7 @@
       </c>
       <c r="AM51" t="inlineStr">
         <is>
-          <t>2636</t>
+          <t>2686</t>
         </is>
       </c>
     </row>
@@ -6157,12 +6157,12 @@
       <c r="AK52" t="n">
         <v>3502</v>
       </c>
-      <c r="AL52" s="5" t="n">
-        <v>31</v>
+      <c r="AL52" s="4" t="n">
+        <v>30</v>
       </c>
       <c r="AM52" t="inlineStr">
         <is>
-          <t>3502</t>
+          <t>3779</t>
         </is>
       </c>
     </row>
@@ -6285,11 +6285,11 @@
         <v>2797</v>
       </c>
       <c r="AL53" s="3" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AM53" t="inlineStr">
         <is>
-          <t>2797</t>
+          <t>2981</t>
         </is>
       </c>
     </row>
@@ -6411,12 +6411,12 @@
       <c r="AK54" t="n">
         <v>2517</v>
       </c>
-      <c r="AL54" s="2" t="n">
-        <v>0</v>
+      <c r="AL54" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="AM54" t="inlineStr">
         <is>
-          <t>2517</t>
+          <t>2532</t>
         </is>
       </c>
     </row>
@@ -6538,12 +6538,12 @@
       <c r="AK55" t="n">
         <v>2601</v>
       </c>
-      <c r="AL55" s="2" t="n">
-        <v>0</v>
+      <c r="AL55" s="3" t="n">
+        <v>9</v>
       </c>
       <c r="AM55" t="inlineStr">
         <is>
-          <t>2601</t>
+          <t>2695</t>
         </is>
       </c>
     </row>
@@ -6670,7 +6670,7 @@
       </c>
       <c r="AM56" t="inlineStr">
         <is>
-          <t>3614</t>
+          <t>3996</t>
         </is>
       </c>
     </row>
@@ -6792,12 +6792,12 @@
       <c r="AK57" t="n">
         <v>2987</v>
       </c>
-      <c r="AL57" s="3" t="n">
-        <v>17</v>
+      <c r="AL57" s="4" t="n">
+        <v>20</v>
       </c>
       <c r="AM57" t="inlineStr">
         <is>
-          <t>2987</t>
+          <t>3253</t>
         </is>
       </c>
     </row>
@@ -6924,7 +6924,7 @@
       </c>
       <c r="AM58" t="inlineStr">
         <is>
-          <t>2619</t>
+          <t>2668</t>
         </is>
       </c>
     </row>
@@ -7051,7 +7051,7 @@
       </c>
       <c r="AM59" t="inlineStr">
         <is>
-          <t>3014</t>
+          <t>3183</t>
         </is>
       </c>
     </row>
@@ -7178,7 +7178,7 @@
       </c>
       <c r="AM60" t="inlineStr">
         <is>
-          <t>3263</t>
+          <t>3518</t>
         </is>
       </c>
     </row>
@@ -7366,7 +7366,7 @@
       </c>
       <c r="AM62" t="inlineStr">
         <is>
-          <t>2877</t>
+          <t>3059</t>
         </is>
       </c>
     </row>
@@ -7493,7 +7493,7 @@
       </c>
       <c r="AM63" t="inlineStr">
         <is>
-          <t>3002</t>
+          <t>3246</t>
         </is>
       </c>
     </row>
@@ -7620,7 +7620,7 @@
       </c>
       <c r="AM64" t="inlineStr">
         <is>
-          <t>3168</t>
+          <t>3465</t>
         </is>
       </c>
     </row>
@@ -7742,12 +7742,12 @@
       <c r="AK65" t="n">
         <v>2872</v>
       </c>
-      <c r="AL65" s="4" t="n">
-        <v>23</v>
+      <c r="AL65" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AM65" t="inlineStr">
         <is>
-          <t>2872</t>
+          <t>2832</t>
         </is>
       </c>
     </row>
@@ -8255,7 +8255,7 @@
       </c>
       <c r="AM69" t="inlineStr">
         <is>
-          <t>2499</t>
+          <t>2528</t>
         </is>
       </c>
     </row>
@@ -8763,7 +8763,7 @@
       </c>
       <c r="AM73" t="inlineStr">
         <is>
-          <t>2513</t>
+          <t>2526</t>
         </is>
       </c>
     </row>
@@ -8890,7 +8890,7 @@
       </c>
       <c r="AM74" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -9139,12 +9139,12 @@
       <c r="AK76" t="n">
         <v>2785</v>
       </c>
-      <c r="AL76" s="3" t="n">
-        <v>5</v>
+      <c r="AL76" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AM76" t="inlineStr">
         <is>
-          <t>2785</t>
+          <t>2837</t>
         </is>
       </c>
     </row>
@@ -9271,7 +9271,7 @@
       </c>
       <c r="AM77" t="inlineStr">
         <is>
-          <t>2514</t>
+          <t>2549</t>
         </is>
       </c>
     </row>
@@ -9525,7 +9525,7 @@
       </c>
       <c r="AM79" t="inlineStr">
         <is>
-          <t>1300</t>
+          <t>1330</t>
         </is>
       </c>
     </row>
@@ -10033,7 +10033,7 @@
       </c>
       <c r="AM83" t="inlineStr">
         <is>
-          <t>2511</t>
+          <t>2509</t>
         </is>
       </c>
     </row>
@@ -11684,7 +11684,7 @@
       </c>
       <c r="AM96" t="inlineStr">
         <is>
-          <t>2831</t>
+          <t>3058</t>
         </is>
       </c>
     </row>
@@ -13668,10 +13668,8 @@
       <c r="AL118" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AM118" t="inlineStr">
-        <is>
-          <t>3280</t>
-        </is>
+      <c r="AM118" t="n">
+        <v>3280</v>
       </c>
     </row>
     <row r="119">
@@ -13775,7 +13773,7 @@
       </c>
       <c r="AM119" t="inlineStr">
         <is>
-          <t>1499</t>
+          <t>1513</t>
         </is>
       </c>
     </row>
@@ -13855,12 +13853,12 @@
       <c r="AK120" t="n">
         <v>1778</v>
       </c>
-      <c r="AL120" s="4" t="n">
-        <v>20</v>
+      <c r="AL120" s="3" t="n">
+        <v>1</v>
       </c>
       <c r="AM120" t="inlineStr">
         <is>
-          <t>1778</t>
+          <t>1830</t>
         </is>
       </c>
     </row>
@@ -13917,11 +13915,11 @@
         <v>3640</v>
       </c>
       <c r="AL121" s="5" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="AM121" t="inlineStr">
         <is>
-          <t>3640</t>
+          <t>4075</t>
         </is>
       </c>
     </row>
@@ -13982,7 +13980,7 @@
       </c>
       <c r="AM122" t="inlineStr">
         <is>
-          <t>3085</t>
+          <t>3369</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-11 11:30:55
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM122"/>
+  <dimension ref="A1:AO123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -586,6 +586,16 @@
           <t>05-09_0</t>
         </is>
       </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>05-10_A</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>05-10_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -708,7 +718,13 @@
       <c r="AL2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM2" t="inlineStr">
+      <c r="AM2" t="n">
+        <v>2525</v>
+      </c>
+      <c r="AN2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO2" t="inlineStr">
         <is>
           <t>2525</t>
         </is>
@@ -835,7 +851,13 @@
       <c r="AL3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM3" t="inlineStr">
+      <c r="AM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -962,7 +984,13 @@
       <c r="AL4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM4" t="inlineStr">
+      <c r="AM4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1089,9 +1117,15 @@
       <c r="AL5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM5" t="inlineStr">
-        <is>
-          <t>2535</t>
+      <c r="AM5" t="n">
+        <v>2535</v>
+      </c>
+      <c r="AN5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO5" t="inlineStr">
+        <is>
+          <t>2527</t>
         </is>
       </c>
     </row>
@@ -1216,9 +1250,15 @@
       <c r="AL6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM6" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="AM6" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AN6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO6" t="inlineStr">
+        <is>
+          <t>2495</t>
         </is>
       </c>
     </row>
@@ -1286,6 +1326,8 @@
       <c r="AK7" t="inlineStr"/>
       <c r="AL7" s="4" t="inlineStr"/>
       <c r="AM7" t="inlineStr"/>
+      <c r="AN7" s="4" t="inlineStr"/>
+      <c r="AO7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1351,6 +1393,8 @@
       <c r="AK8" t="inlineStr"/>
       <c r="AL8" s="4" t="inlineStr"/>
       <c r="AM8" t="inlineStr"/>
+      <c r="AN8" s="4" t="inlineStr"/>
+      <c r="AO8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1416,6 +1460,8 @@
       <c r="AK9" t="inlineStr"/>
       <c r="AL9" s="4" t="inlineStr"/>
       <c r="AM9" t="inlineStr"/>
+      <c r="AN9" s="4" t="inlineStr"/>
+      <c r="AO9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1481,6 +1527,8 @@
       <c r="AK10" t="inlineStr"/>
       <c r="AL10" s="4" t="inlineStr"/>
       <c r="AM10" t="inlineStr"/>
+      <c r="AN10" s="4" t="inlineStr"/>
+      <c r="AO10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1546,6 +1594,8 @@
       <c r="AK11" t="inlineStr"/>
       <c r="AL11" s="4" t="inlineStr"/>
       <c r="AM11" t="inlineStr"/>
+      <c r="AN11" s="4" t="inlineStr"/>
+      <c r="AO11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1611,6 +1661,8 @@
       <c r="AK12" t="inlineStr"/>
       <c r="AL12" s="4" t="inlineStr"/>
       <c r="AM12" t="inlineStr"/>
+      <c r="AN12" s="4" t="inlineStr"/>
+      <c r="AO12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1676,6 +1728,8 @@
       <c r="AK13" t="inlineStr"/>
       <c r="AL13" s="4" t="inlineStr"/>
       <c r="AM13" t="inlineStr"/>
+      <c r="AN13" s="4" t="inlineStr"/>
+      <c r="AO13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1741,6 +1795,8 @@
       <c r="AK14" t="inlineStr"/>
       <c r="AL14" s="4" t="inlineStr"/>
       <c r="AM14" t="inlineStr"/>
+      <c r="AN14" s="4" t="inlineStr"/>
+      <c r="AO14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1806,6 +1862,8 @@
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" s="4" t="inlineStr"/>
       <c r="AM15" t="inlineStr"/>
+      <c r="AN15" s="4" t="inlineStr"/>
+      <c r="AO15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1871,6 +1929,8 @@
       <c r="AK16" t="inlineStr"/>
       <c r="AL16" s="4" t="inlineStr"/>
       <c r="AM16" t="inlineStr"/>
+      <c r="AN16" s="4" t="inlineStr"/>
+      <c r="AO16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1936,6 +1996,8 @@
       <c r="AK17" t="inlineStr"/>
       <c r="AL17" s="4" t="inlineStr"/>
       <c r="AM17" t="inlineStr"/>
+      <c r="AN17" s="4" t="inlineStr"/>
+      <c r="AO17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -2058,9 +2120,15 @@
       <c r="AL18" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AM18" t="inlineStr">
-        <is>
-          <t>3083</t>
+      <c r="AM18" t="n">
+        <v>3083</v>
+      </c>
+      <c r="AN18" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="AO18" t="inlineStr">
+        <is>
+          <t>3316</t>
         </is>
       </c>
     </row>
@@ -2185,9 +2253,15 @@
       <c r="AL19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM19" t="inlineStr">
-        <is>
-          <t>2585</t>
+      <c r="AM19" t="n">
+        <v>2585</v>
+      </c>
+      <c r="AN19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO19" t="inlineStr">
+        <is>
+          <t>2610</t>
         </is>
       </c>
     </row>
@@ -2312,9 +2386,15 @@
       <c r="AL20" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="AM20" t="inlineStr">
-        <is>
-          <t>3279</t>
+      <c r="AM20" t="n">
+        <v>3279</v>
+      </c>
+      <c r="AN20" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO20" t="inlineStr">
+        <is>
+          <t>3573</t>
         </is>
       </c>
     </row>
@@ -2439,9 +2519,15 @@
       <c r="AL21" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="AM21" t="inlineStr">
-        <is>
-          <t>3407</t>
+      <c r="AM21" t="n">
+        <v>3407</v>
+      </c>
+      <c r="AN21" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="AO21" t="inlineStr">
+        <is>
+          <t>3778</t>
         </is>
       </c>
     </row>
@@ -2566,9 +2652,15 @@
       <c r="AL22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AM22" t="inlineStr">
-        <is>
-          <t>3472</t>
+      <c r="AM22" t="n">
+        <v>3472</v>
+      </c>
+      <c r="AN22" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AO22" t="inlineStr">
+        <is>
+          <t>3775</t>
         </is>
       </c>
     </row>
@@ -2693,9 +2785,15 @@
       <c r="AL23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AM23" t="inlineStr">
-        <is>
-          <t>3617</t>
+      <c r="AM23" t="n">
+        <v>3617</v>
+      </c>
+      <c r="AN23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO23" t="inlineStr">
+        <is>
+          <t>3997</t>
         </is>
       </c>
     </row>
@@ -2820,9 +2918,15 @@
       <c r="AL24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AM24" t="inlineStr">
-        <is>
-          <t>3752</t>
+      <c r="AM24" t="n">
+        <v>3752</v>
+      </c>
+      <c r="AN24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AO24" t="inlineStr">
+        <is>
+          <t>3941</t>
         </is>
       </c>
     </row>
@@ -2947,9 +3051,15 @@
       <c r="AL25" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AM25" t="inlineStr">
-        <is>
-          <t>3709</t>
+      <c r="AM25" t="n">
+        <v>3709</v>
+      </c>
+      <c r="AN25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO25" t="inlineStr">
+        <is>
+          <t>4089</t>
         </is>
       </c>
     </row>
@@ -3074,7 +3184,13 @@
       <c r="AL26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM26" t="inlineStr">
+      <c r="AM26" t="n">
+        <v>2499</v>
+      </c>
+      <c r="AN26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO26" t="inlineStr">
         <is>
           <t>2499</t>
         </is>
@@ -3201,7 +3317,13 @@
       <c r="AL27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM27" t="inlineStr">
+      <c r="AM27" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AN27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO27" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3267,6 +3389,8 @@
       <c r="AK28" t="inlineStr"/>
       <c r="AL28" s="4" t="inlineStr"/>
       <c r="AM28" t="inlineStr"/>
+      <c r="AN28" s="4" t="inlineStr"/>
+      <c r="AO28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -3389,7 +3513,13 @@
       <c r="AL29" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="AM29" t="inlineStr">
+      <c r="AM29" t="n">
+        <v>2866</v>
+      </c>
+      <c r="AN29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO29" t="inlineStr">
         <is>
           <t>2866</t>
         </is>
@@ -3516,7 +3646,13 @@
       <c r="AL30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM30" t="inlineStr">
+      <c r="AM30" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AN30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO30" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3643,9 +3779,15 @@
       <c r="AL31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AM31" t="inlineStr">
-        <is>
-          <t>3801</t>
+      <c r="AM31" t="n">
+        <v>3801</v>
+      </c>
+      <c r="AN31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO31" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -3770,9 +3912,15 @@
       <c r="AL32" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="AM32" t="inlineStr">
-        <is>
-          <t>2553</t>
+      <c r="AM32" t="n">
+        <v>2553</v>
+      </c>
+      <c r="AN32" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO32" t="inlineStr">
+        <is>
+          <t>2899</t>
         </is>
       </c>
     </row>
@@ -3848,6 +3996,8 @@
       <c r="AK33" t="inlineStr"/>
       <c r="AL33" s="4" t="inlineStr"/>
       <c r="AM33" t="inlineStr"/>
+      <c r="AN33" s="4" t="inlineStr"/>
+      <c r="AO33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3970,7 +4120,13 @@
       <c r="AL34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM34" t="inlineStr">
+      <c r="AM34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4097,9 +4253,15 @@
       <c r="AL35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM35" t="inlineStr">
-        <is>
-          <t>2944</t>
+      <c r="AM35" t="n">
+        <v>2944</v>
+      </c>
+      <c r="AN35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO35" t="inlineStr">
+        <is>
+          <t>3006</t>
         </is>
       </c>
     </row>
@@ -4224,9 +4386,15 @@
       <c r="AL36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM36" t="inlineStr">
-        <is>
-          <t>2524</t>
+      <c r="AM36" t="n">
+        <v>2524</v>
+      </c>
+      <c r="AN36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO36" t="inlineStr">
+        <is>
+          <t>2521</t>
         </is>
       </c>
     </row>
@@ -4351,9 +4519,15 @@
       <c r="AL37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AM37" t="inlineStr">
-        <is>
-          <t>3638</t>
+      <c r="AM37" t="n">
+        <v>3638</v>
+      </c>
+      <c r="AN37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO37" t="inlineStr">
+        <is>
+          <t>3905</t>
         </is>
       </c>
     </row>
@@ -4478,9 +4652,15 @@
       <c r="AL38" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AM38" t="inlineStr">
-        <is>
-          <t>3891</t>
+      <c r="AM38" t="n">
+        <v>3891</v>
+      </c>
+      <c r="AN38" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AO38" t="inlineStr">
+        <is>
+          <t>4133</t>
         </is>
       </c>
     </row>
@@ -4605,9 +4785,15 @@
       <c r="AL39" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AM39" t="inlineStr">
-        <is>
-          <t>3549</t>
+      <c r="AM39" t="n">
+        <v>3549</v>
+      </c>
+      <c r="AN39" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AO39" t="inlineStr">
+        <is>
+          <t>3788</t>
         </is>
       </c>
     </row>
@@ -4732,7 +4918,13 @@
       <c r="AL40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM40" t="inlineStr">
+      <c r="AM40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4859,9 +5051,15 @@
       <c r="AL41" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="AM41" t="inlineStr">
-        <is>
-          <t>3250</t>
+      <c r="AM41" t="n">
+        <v>3250</v>
+      </c>
+      <c r="AN41" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO41" t="inlineStr">
+        <is>
+          <t>3700</t>
         </is>
       </c>
     </row>
@@ -4986,9 +5184,15 @@
       <c r="AL42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM42" t="inlineStr">
-        <is>
-          <t>2685</t>
+      <c r="AM42" t="n">
+        <v>2685</v>
+      </c>
+      <c r="AN42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO42" t="inlineStr">
+        <is>
+          <t>2728</t>
         </is>
       </c>
     </row>
@@ -5056,6 +5260,8 @@
       <c r="AK43" t="inlineStr"/>
       <c r="AL43" s="4" t="inlineStr"/>
       <c r="AM43" t="inlineStr"/>
+      <c r="AN43" s="4" t="inlineStr"/>
+      <c r="AO43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -5149,6 +5355,8 @@
       <c r="AK44" t="inlineStr"/>
       <c r="AL44" s="4" t="inlineStr"/>
       <c r="AM44" t="inlineStr"/>
+      <c r="AN44" s="4" t="inlineStr"/>
+      <c r="AO44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -5271,9 +5479,15 @@
       <c r="AL45" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AM45" t="inlineStr">
-        <is>
-          <t>3072</t>
+      <c r="AM45" t="n">
+        <v>3072</v>
+      </c>
+      <c r="AN45" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="AO45" t="inlineStr">
+        <is>
+          <t>3329</t>
         </is>
       </c>
     </row>
@@ -5398,9 +5612,15 @@
       <c r="AL46" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="AM46" t="inlineStr">
-        <is>
-          <t>3074</t>
+      <c r="AM46" t="n">
+        <v>3074</v>
+      </c>
+      <c r="AN46" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO46" t="inlineStr">
+        <is>
+          <t>3123</t>
         </is>
       </c>
     </row>
@@ -5525,9 +5745,15 @@
       <c r="AL47" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AM47" t="inlineStr">
-        <is>
-          <t>3987</t>
+      <c r="AM47" t="n">
+        <v>3987</v>
+      </c>
+      <c r="AN47" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AO47" t="inlineStr">
+        <is>
+          <t>4160</t>
         </is>
       </c>
     </row>
@@ -5652,9 +5878,15 @@
       <c r="AL48" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="AM48" t="inlineStr">
-        <is>
-          <t>3985</t>
+      <c r="AM48" t="n">
+        <v>3985</v>
+      </c>
+      <c r="AN48" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO48" t="inlineStr">
+        <is>
+          <t>4108</t>
         </is>
       </c>
     </row>
@@ -5779,9 +6011,15 @@
       <c r="AL49" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AM49" t="inlineStr">
-        <is>
-          <t>3771</t>
+      <c r="AM49" t="n">
+        <v>3771</v>
+      </c>
+      <c r="AN49" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AO49" t="inlineStr">
+        <is>
+          <t>3997</t>
         </is>
       </c>
     </row>
@@ -5906,9 +6144,15 @@
       <c r="AL50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AM50" t="inlineStr">
-        <is>
-          <t>3770</t>
+      <c r="AM50" t="n">
+        <v>3770</v>
+      </c>
+      <c r="AN50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO50" t="inlineStr">
+        <is>
+          <t>3990</t>
         </is>
       </c>
     </row>
@@ -6033,9 +6277,15 @@
       <c r="AL51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM51" t="inlineStr">
-        <is>
-          <t>2686</t>
+      <c r="AM51" t="n">
+        <v>2686</v>
+      </c>
+      <c r="AN51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO51" t="inlineStr">
+        <is>
+          <t>2749</t>
         </is>
       </c>
     </row>
@@ -6160,9 +6410,15 @@
       <c r="AL52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AM52" t="inlineStr">
-        <is>
-          <t>3779</t>
+      <c r="AM52" t="n">
+        <v>3779</v>
+      </c>
+      <c r="AN52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO52" t="inlineStr">
+        <is>
+          <t>3996</t>
         </is>
       </c>
     </row>
@@ -6287,9 +6543,15 @@
       <c r="AL53" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="AM53" t="inlineStr">
-        <is>
-          <t>2981</t>
+      <c r="AM53" t="n">
+        <v>2981</v>
+      </c>
+      <c r="AN53" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO53" t="inlineStr">
+        <is>
+          <t>3126</t>
         </is>
       </c>
     </row>
@@ -6414,9 +6676,15 @@
       <c r="AL54" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="AM54" t="inlineStr">
-        <is>
-          <t>2532</t>
+      <c r="AM54" t="n">
+        <v>2532</v>
+      </c>
+      <c r="AN54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO54" t="inlineStr">
+        <is>
+          <t>2530</t>
         </is>
       </c>
     </row>
@@ -6541,9 +6809,15 @@
       <c r="AL55" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="AM55" t="inlineStr">
-        <is>
-          <t>2695</t>
+      <c r="AM55" t="n">
+        <v>2695</v>
+      </c>
+      <c r="AN55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO55" t="inlineStr">
+        <is>
+          <t>2693</t>
         </is>
       </c>
     </row>
@@ -6668,9 +6942,15 @@
       <c r="AL56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AM56" t="inlineStr">
-        <is>
-          <t>3996</t>
+      <c r="AM56" t="n">
+        <v>3996</v>
+      </c>
+      <c r="AN56" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO56" t="inlineStr">
+        <is>
+          <t>3999</t>
         </is>
       </c>
     </row>
@@ -6795,9 +7075,15 @@
       <c r="AL57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AM57" t="inlineStr">
-        <is>
-          <t>3253</t>
+      <c r="AM57" t="n">
+        <v>3253</v>
+      </c>
+      <c r="AN57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO57" t="inlineStr">
+        <is>
+          <t>3552</t>
         </is>
       </c>
     </row>
@@ -6922,9 +7208,15 @@
       <c r="AL58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM58" t="inlineStr">
-        <is>
-          <t>2668</t>
+      <c r="AM58" t="n">
+        <v>2668</v>
+      </c>
+      <c r="AN58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO58" t="inlineStr">
+        <is>
+          <t>2744</t>
         </is>
       </c>
     </row>
@@ -7049,9 +7341,15 @@
       <c r="AL59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AM59" t="inlineStr">
-        <is>
-          <t>3183</t>
+      <c r="AM59" t="n">
+        <v>3183</v>
+      </c>
+      <c r="AN59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO59" t="inlineStr">
+        <is>
+          <t>3405</t>
         </is>
       </c>
     </row>
@@ -7176,9 +7474,15 @@
       <c r="AL60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AM60" t="inlineStr">
-        <is>
-          <t>3518</t>
+      <c r="AM60" t="n">
+        <v>3518</v>
+      </c>
+      <c r="AN60" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AO60" t="inlineStr">
+        <is>
+          <t>3805</t>
         </is>
       </c>
     </row>
@@ -7242,6 +7546,8 @@
       <c r="AK61" t="inlineStr"/>
       <c r="AL61" s="4" t="inlineStr"/>
       <c r="AM61" t="inlineStr"/>
+      <c r="AN61" s="4" t="inlineStr"/>
+      <c r="AO61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -7364,9 +7670,15 @@
       <c r="AL62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AM62" t="inlineStr">
-        <is>
-          <t>3059</t>
+      <c r="AM62" t="n">
+        <v>3059</v>
+      </c>
+      <c r="AN62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO62" t="inlineStr">
+        <is>
+          <t>3229</t>
         </is>
       </c>
     </row>
@@ -7491,9 +7803,15 @@
       <c r="AL63" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AM63" t="inlineStr">
-        <is>
-          <t>3246</t>
+      <c r="AM63" t="n">
+        <v>3246</v>
+      </c>
+      <c r="AN63" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO63" t="inlineStr">
+        <is>
+          <t>3226</t>
         </is>
       </c>
     </row>
@@ -7618,9 +7936,15 @@
       <c r="AL64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AM64" t="inlineStr">
-        <is>
-          <t>3465</t>
+      <c r="AM64" t="n">
+        <v>3465</v>
+      </c>
+      <c r="AN64" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AO64" t="inlineStr">
+        <is>
+          <t>3644</t>
         </is>
       </c>
     </row>
@@ -7745,9 +8069,15 @@
       <c r="AL65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM65" t="inlineStr">
-        <is>
-          <t>2832</t>
+      <c r="AM65" t="n">
+        <v>2832</v>
+      </c>
+      <c r="AN65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO65" t="inlineStr">
+        <is>
+          <t>2829</t>
         </is>
       </c>
     </row>
@@ -7872,7 +8202,13 @@
       <c r="AL66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM66" t="inlineStr">
+      <c r="AM66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7999,7 +8335,13 @@
       <c r="AL67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM67" t="inlineStr">
+      <c r="AM67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8126,7 +8468,13 @@
       <c r="AL68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM68" t="inlineStr">
+      <c r="AM68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8253,11 +8601,11 @@
       <c r="AL69" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM69" t="inlineStr">
-        <is>
-          <t>2528</t>
-        </is>
-      </c>
+      <c r="AM69" t="n">
+        <v>2528</v>
+      </c>
+      <c r="AN69" s="4" t="inlineStr"/>
+      <c r="AO69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -8380,7 +8728,13 @@
       <c r="AL70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM70" t="inlineStr">
+      <c r="AM70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8507,7 +8861,13 @@
       <c r="AL71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM71" t="inlineStr">
+      <c r="AM71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8634,7 +8994,13 @@
       <c r="AL72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM72" t="inlineStr">
+      <c r="AM72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8761,9 +9127,15 @@
       <c r="AL73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM73" t="inlineStr">
-        <is>
-          <t>2526</t>
+      <c r="AM73" t="n">
+        <v>2526</v>
+      </c>
+      <c r="AN73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO73" t="inlineStr">
+        <is>
+          <t>2554</t>
         </is>
       </c>
     </row>
@@ -8888,9 +9260,15 @@
       <c r="AL74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM74" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="AM74" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AN74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO74" t="inlineStr">
+        <is>
+          <t>2518</t>
         </is>
       </c>
     </row>
@@ -9015,7 +9393,13 @@
       <c r="AL75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM75" t="inlineStr">
+      <c r="AM75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9142,9 +9526,15 @@
       <c r="AL76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM76" t="inlineStr">
-        <is>
-          <t>2837</t>
+      <c r="AM76" t="n">
+        <v>2837</v>
+      </c>
+      <c r="AN76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO76" t="inlineStr">
+        <is>
+          <t>2915</t>
         </is>
       </c>
     </row>
@@ -9269,9 +9659,15 @@
       <c r="AL77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM77" t="inlineStr">
-        <is>
-          <t>2549</t>
+      <c r="AM77" t="n">
+        <v>2549</v>
+      </c>
+      <c r="AN77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO77" t="inlineStr">
+        <is>
+          <t>2542</t>
         </is>
       </c>
     </row>
@@ -9396,7 +9792,13 @@
       <c r="AL78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM78" t="inlineStr">
+      <c r="AM78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9523,9 +9925,15 @@
       <c r="AL79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM79" t="inlineStr">
-        <is>
-          <t>1330</t>
+      <c r="AM79" t="n">
+        <v>1330</v>
+      </c>
+      <c r="AN79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO79" t="inlineStr">
+        <is>
+          <t>1328</t>
         </is>
       </c>
     </row>
@@ -9650,7 +10058,13 @@
       <c r="AL80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM80" t="inlineStr">
+      <c r="AM80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9777,7 +10191,13 @@
       <c r="AL81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM81" t="inlineStr">
+      <c r="AM81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9904,7 +10324,13 @@
       <c r="AL82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM82" t="inlineStr">
+      <c r="AM82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10031,9 +10457,15 @@
       <c r="AL83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM83" t="inlineStr">
-        <is>
-          <t>2509</t>
+      <c r="AM83" t="n">
+        <v>2509</v>
+      </c>
+      <c r="AN83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO83" t="inlineStr">
+        <is>
+          <t>2532</t>
         </is>
       </c>
     </row>
@@ -10158,7 +10590,13 @@
       <c r="AL84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM84" t="inlineStr">
+      <c r="AM84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10285,7 +10723,13 @@
       <c r="AL85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM85" t="inlineStr">
+      <c r="AM85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10412,7 +10856,13 @@
       <c r="AL86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM86" t="inlineStr">
+      <c r="AM86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10539,7 +10989,13 @@
       <c r="AL87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM87" t="inlineStr">
+      <c r="AM87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10666,7 +11122,13 @@
       <c r="AL88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM88" t="inlineStr">
+      <c r="AM88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10793,7 +11255,13 @@
       <c r="AL89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM89" t="inlineStr">
+      <c r="AM89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10920,7 +11388,13 @@
       <c r="AL90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM90" t="inlineStr">
+      <c r="AM90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11047,7 +11521,13 @@
       <c r="AL91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM91" t="inlineStr">
+      <c r="AM91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11174,7 +11654,13 @@
       <c r="AL92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM92" t="inlineStr">
+      <c r="AM92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11301,7 +11787,13 @@
       <c r="AL93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM93" t="inlineStr">
+      <c r="AM93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11428,7 +11920,13 @@
       <c r="AL94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM94" t="inlineStr">
+      <c r="AM94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11555,7 +12053,13 @@
       <c r="AL95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM95" t="inlineStr">
+      <c r="AM95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11682,9 +12186,15 @@
       <c r="AL96" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AM96" t="inlineStr">
-        <is>
-          <t>3058</t>
+      <c r="AM96" t="n">
+        <v>3058</v>
+      </c>
+      <c r="AN96" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AO96" t="inlineStr">
+        <is>
+          <t>3301</t>
         </is>
       </c>
     </row>
@@ -11809,7 +12319,13 @@
       <c r="AL97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM97" t="inlineStr">
+      <c r="AM97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11936,7 +12452,13 @@
       <c r="AL98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM98" t="inlineStr">
+      <c r="AM98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12063,7 +12585,13 @@
       <c r="AL99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM99" t="inlineStr">
+      <c r="AM99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12190,7 +12718,13 @@
       <c r="AL100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM100" t="inlineStr">
+      <c r="AM100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12317,7 +12851,13 @@
       <c r="AL101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM101" t="inlineStr">
+      <c r="AM101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12444,7 +12984,13 @@
       <c r="AL102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM102" t="inlineStr">
+      <c r="AM102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12571,7 +13117,13 @@
       <c r="AL103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM103" t="inlineStr">
+      <c r="AM103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12698,7 +13250,13 @@
       <c r="AL104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM104" t="inlineStr">
+      <c r="AM104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12825,7 +13383,13 @@
       <c r="AL105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM105" t="inlineStr">
+      <c r="AM105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12883,6 +13447,8 @@
       <c r="AK106" t="inlineStr"/>
       <c r="AL106" s="4" t="inlineStr"/>
       <c r="AM106" t="inlineStr"/>
+      <c r="AN106" s="4" t="inlineStr"/>
+      <c r="AO106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -12936,6 +13502,8 @@
       <c r="AK107" t="inlineStr"/>
       <c r="AL107" s="4" t="inlineStr"/>
       <c r="AM107" t="inlineStr"/>
+      <c r="AN107" s="4" t="inlineStr"/>
+      <c r="AO107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -12989,6 +13557,8 @@
       <c r="AK108" t="inlineStr"/>
       <c r="AL108" s="4" t="inlineStr"/>
       <c r="AM108" t="inlineStr"/>
+      <c r="AN108" s="4" t="inlineStr"/>
+      <c r="AO108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -13042,6 +13612,8 @@
       <c r="AK109" t="inlineStr"/>
       <c r="AL109" s="4" t="inlineStr"/>
       <c r="AM109" t="inlineStr"/>
+      <c r="AN109" s="4" t="inlineStr"/>
+      <c r="AO109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -13095,6 +13667,8 @@
       <c r="AK110" t="inlineStr"/>
       <c r="AL110" s="4" t="inlineStr"/>
       <c r="AM110" t="inlineStr"/>
+      <c r="AN110" s="4" t="inlineStr"/>
+      <c r="AO110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -13148,6 +13722,8 @@
       <c r="AK111" t="inlineStr"/>
       <c r="AL111" s="4" t="inlineStr"/>
       <c r="AM111" t="inlineStr"/>
+      <c r="AN111" s="4" t="inlineStr"/>
+      <c r="AO111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -13201,6 +13777,8 @@
       <c r="AK112" t="inlineStr"/>
       <c r="AL112" s="4" t="inlineStr"/>
       <c r="AM112" t="inlineStr"/>
+      <c r="AN112" s="4" t="inlineStr"/>
+      <c r="AO112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -13254,6 +13832,8 @@
       <c r="AK113" t="inlineStr"/>
       <c r="AL113" s="4" t="inlineStr"/>
       <c r="AM113" t="inlineStr"/>
+      <c r="AN113" s="4" t="inlineStr"/>
+      <c r="AO113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -13307,6 +13887,8 @@
       <c r="AK114" t="inlineStr"/>
       <c r="AL114" s="4" t="inlineStr"/>
       <c r="AM114" t="inlineStr"/>
+      <c r="AN114" s="4" t="inlineStr"/>
+      <c r="AO114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -13390,6 +13972,8 @@
       <c r="AK115" t="inlineStr"/>
       <c r="AL115" s="4" t="inlineStr"/>
       <c r="AM115" t="inlineStr"/>
+      <c r="AN115" s="4" t="inlineStr"/>
+      <c r="AO115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -13473,6 +14057,8 @@
       <c r="AK116" t="inlineStr"/>
       <c r="AL116" s="4" t="inlineStr"/>
       <c r="AM116" t="inlineStr"/>
+      <c r="AN116" s="4" t="inlineStr"/>
+      <c r="AO116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -13556,6 +14142,8 @@
       <c r="AK117" t="inlineStr"/>
       <c r="AL117" s="4" t="inlineStr"/>
       <c r="AM117" t="inlineStr"/>
+      <c r="AN117" s="4" t="inlineStr"/>
+      <c r="AO117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -13671,6 +14259,8 @@
       <c r="AM118" t="n">
         <v>3280</v>
       </c>
+      <c r="AN118" s="4" t="inlineStr"/>
+      <c r="AO118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -13771,9 +14361,15 @@
       <c r="AL119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM119" t="inlineStr">
-        <is>
-          <t>1513</t>
+      <c r="AM119" t="n">
+        <v>1513</v>
+      </c>
+      <c r="AN119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO119" t="inlineStr">
+        <is>
+          <t>1512</t>
         </is>
       </c>
     </row>
@@ -13856,9 +14452,15 @@
       <c r="AL120" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="AM120" t="inlineStr">
-        <is>
-          <t>1830</t>
+      <c r="AM120" t="n">
+        <v>1830</v>
+      </c>
+      <c r="AN120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO120" t="inlineStr">
+        <is>
+          <t>1820</t>
         </is>
       </c>
     </row>
@@ -13917,9 +14519,15 @@
       <c r="AL121" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AM121" t="inlineStr">
-        <is>
-          <t>4075</t>
+      <c r="AM121" t="n">
+        <v>4075</v>
+      </c>
+      <c r="AN121" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AO121" t="inlineStr">
+        <is>
+          <t>4515</t>
         </is>
       </c>
     </row>
@@ -13978,9 +14586,76 @@
       <c r="AL122" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AM122" t="inlineStr">
-        <is>
-          <t>3369</t>
+      <c r="AM122" t="n">
+        <v>3369</v>
+      </c>
+      <c r="AN122" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO122" t="inlineStr">
+        <is>
+          <t>3669</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>38996518</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>"Hà Lê Gia Bảo"</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr"/>
+      <c r="D123" t="inlineStr"/>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F123" s="4" t="inlineStr"/>
+      <c r="G123" t="inlineStr"/>
+      <c r="H123" s="4" t="inlineStr"/>
+      <c r="I123" t="inlineStr"/>
+      <c r="J123" s="4" t="inlineStr"/>
+      <c r="K123" t="inlineStr"/>
+      <c r="L123" s="4" t="inlineStr"/>
+      <c r="M123" t="inlineStr"/>
+      <c r="N123" s="4" t="inlineStr"/>
+      <c r="O123" t="inlineStr"/>
+      <c r="P123" s="4" t="inlineStr"/>
+      <c r="Q123" t="inlineStr"/>
+      <c r="R123" s="4" t="inlineStr"/>
+      <c r="S123" t="inlineStr"/>
+      <c r="T123" s="4" t="inlineStr"/>
+      <c r="U123" t="inlineStr"/>
+      <c r="V123" s="4" t="inlineStr"/>
+      <c r="W123" t="inlineStr"/>
+      <c r="X123" s="4" t="inlineStr"/>
+      <c r="Y123" t="inlineStr"/>
+      <c r="Z123" s="4" t="inlineStr"/>
+      <c r="AA123" t="inlineStr"/>
+      <c r="AB123" s="4" t="inlineStr"/>
+      <c r="AC123" t="inlineStr"/>
+      <c r="AD123" s="4" t="inlineStr"/>
+      <c r="AE123" t="inlineStr"/>
+      <c r="AF123" s="4" t="inlineStr"/>
+      <c r="AG123" t="inlineStr"/>
+      <c r="AH123" s="4" t="inlineStr"/>
+      <c r="AI123" t="inlineStr"/>
+      <c r="AJ123" s="4" t="inlineStr"/>
+      <c r="AK123" t="inlineStr"/>
+      <c r="AL123" s="4" t="inlineStr"/>
+      <c r="AM123" t="inlineStr"/>
+      <c r="AN123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO123" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-11 12:47:27
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -14599,10 +14599,8 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>38996518</t>
-        </is>
+      <c r="A123" t="n">
+        <v>38996518</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-05-12 11:30:56
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO123"/>
+  <dimension ref="A1:AQ124"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -596,6 +596,16 @@
           <t>05-10_0</t>
         </is>
       </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>05-11_A</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>05-11_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -724,9 +734,15 @@
       <c r="AN2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO2" t="inlineStr">
-        <is>
-          <t>2525</t>
+      <c r="AO2" t="n">
+        <v>2525</v>
+      </c>
+      <c r="AP2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ2" t="inlineStr">
+        <is>
+          <t>2556</t>
         </is>
       </c>
     </row>
@@ -857,7 +873,13 @@
       <c r="AN3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO3" t="inlineStr">
+      <c r="AO3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -990,7 +1012,13 @@
       <c r="AN4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO4" t="inlineStr">
+      <c r="AO4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1123,9 +1151,15 @@
       <c r="AN5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO5" t="inlineStr">
-        <is>
-          <t>2527</t>
+      <c r="AO5" t="n">
+        <v>2527</v>
+      </c>
+      <c r="AP5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ5" t="inlineStr">
+        <is>
+          <t>2519</t>
         </is>
       </c>
     </row>
@@ -1256,9 +1290,15 @@
       <c r="AN6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO6" t="inlineStr">
-        <is>
-          <t>2495</t>
+      <c r="AO6" t="n">
+        <v>2495</v>
+      </c>
+      <c r="AP6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ6" t="inlineStr">
+        <is>
+          <t>2506</t>
         </is>
       </c>
     </row>
@@ -1328,6 +1368,8 @@
       <c r="AM7" t="inlineStr"/>
       <c r="AN7" s="4" t="inlineStr"/>
       <c r="AO7" t="inlineStr"/>
+      <c r="AP7" s="4" t="inlineStr"/>
+      <c r="AQ7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1395,6 +1437,8 @@
       <c r="AM8" t="inlineStr"/>
       <c r="AN8" s="4" t="inlineStr"/>
       <c r="AO8" t="inlineStr"/>
+      <c r="AP8" s="4" t="inlineStr"/>
+      <c r="AQ8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1462,6 +1506,8 @@
       <c r="AM9" t="inlineStr"/>
       <c r="AN9" s="4" t="inlineStr"/>
       <c r="AO9" t="inlineStr"/>
+      <c r="AP9" s="4" t="inlineStr"/>
+      <c r="AQ9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1529,6 +1575,8 @@
       <c r="AM10" t="inlineStr"/>
       <c r="AN10" s="4" t="inlineStr"/>
       <c r="AO10" t="inlineStr"/>
+      <c r="AP10" s="4" t="inlineStr"/>
+      <c r="AQ10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1596,6 +1644,8 @@
       <c r="AM11" t="inlineStr"/>
       <c r="AN11" s="4" t="inlineStr"/>
       <c r="AO11" t="inlineStr"/>
+      <c r="AP11" s="4" t="inlineStr"/>
+      <c r="AQ11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1663,6 +1713,8 @@
       <c r="AM12" t="inlineStr"/>
       <c r="AN12" s="4" t="inlineStr"/>
       <c r="AO12" t="inlineStr"/>
+      <c r="AP12" s="4" t="inlineStr"/>
+      <c r="AQ12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1730,6 +1782,8 @@
       <c r="AM13" t="inlineStr"/>
       <c r="AN13" s="4" t="inlineStr"/>
       <c r="AO13" t="inlineStr"/>
+      <c r="AP13" s="4" t="inlineStr"/>
+      <c r="AQ13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1797,6 +1851,8 @@
       <c r="AM14" t="inlineStr"/>
       <c r="AN14" s="4" t="inlineStr"/>
       <c r="AO14" t="inlineStr"/>
+      <c r="AP14" s="4" t="inlineStr"/>
+      <c r="AQ14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1864,6 +1920,8 @@
       <c r="AM15" t="inlineStr"/>
       <c r="AN15" s="4" t="inlineStr"/>
       <c r="AO15" t="inlineStr"/>
+      <c r="AP15" s="4" t="inlineStr"/>
+      <c r="AQ15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1931,6 +1989,8 @@
       <c r="AM16" t="inlineStr"/>
       <c r="AN16" s="4" t="inlineStr"/>
       <c r="AO16" t="inlineStr"/>
+      <c r="AP16" s="4" t="inlineStr"/>
+      <c r="AQ16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1998,6 +2058,8 @@
       <c r="AM17" t="inlineStr"/>
       <c r="AN17" s="4" t="inlineStr"/>
       <c r="AO17" t="inlineStr"/>
+      <c r="AP17" s="4" t="inlineStr"/>
+      <c r="AQ17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -2126,9 +2188,15 @@
       <c r="AN18" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="AO18" t="inlineStr">
-        <is>
-          <t>3316</t>
+      <c r="AO18" t="n">
+        <v>3316</v>
+      </c>
+      <c r="AP18" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ18" t="inlineStr">
+        <is>
+          <t>3594</t>
         </is>
       </c>
     </row>
@@ -2259,9 +2327,15 @@
       <c r="AN19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO19" t="inlineStr">
-        <is>
-          <t>2610</t>
+      <c r="AO19" t="n">
+        <v>2610</v>
+      </c>
+      <c r="AP19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ19" t="inlineStr">
+        <is>
+          <t>2641</t>
         </is>
       </c>
     </row>
@@ -2392,9 +2466,15 @@
       <c r="AN20" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AO20" t="inlineStr">
-        <is>
-          <t>3573</t>
+      <c r="AO20" t="n">
+        <v>3573</v>
+      </c>
+      <c r="AP20" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AQ20" t="inlineStr">
+        <is>
+          <t>3853</t>
         </is>
       </c>
     </row>
@@ -2525,9 +2605,15 @@
       <c r="AN21" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="AO21" t="inlineStr">
-        <is>
-          <t>3778</t>
+      <c r="AO21" t="n">
+        <v>3778</v>
+      </c>
+      <c r="AP21" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AQ21" t="inlineStr">
+        <is>
+          <t>4027</t>
         </is>
       </c>
     </row>
@@ -2658,9 +2744,15 @@
       <c r="AN22" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AO22" t="inlineStr">
-        <is>
-          <t>3775</t>
+      <c r="AO22" t="n">
+        <v>3775</v>
+      </c>
+      <c r="AP22" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AQ22" t="inlineStr">
+        <is>
+          <t>3996</t>
         </is>
       </c>
     </row>
@@ -2791,9 +2883,15 @@
       <c r="AN23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AO23" t="inlineStr">
-        <is>
-          <t>3997</t>
+      <c r="AO23" t="n">
+        <v>3997</v>
+      </c>
+      <c r="AP23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AQ23" t="inlineStr">
+        <is>
+          <t>4288</t>
         </is>
       </c>
     </row>
@@ -2924,9 +3022,15 @@
       <c r="AN24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AO24" t="inlineStr">
-        <is>
-          <t>3941</t>
+      <c r="AO24" t="n">
+        <v>3941</v>
+      </c>
+      <c r="AP24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AQ24" t="inlineStr">
+        <is>
+          <t>4002</t>
         </is>
       </c>
     </row>
@@ -3057,9 +3161,15 @@
       <c r="AN25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AO25" t="inlineStr">
-        <is>
-          <t>4089</t>
+      <c r="AO25" t="n">
+        <v>4089</v>
+      </c>
+      <c r="AP25" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AQ25" t="inlineStr">
+        <is>
+          <t>4193</t>
         </is>
       </c>
     </row>
@@ -3190,9 +3300,15 @@
       <c r="AN26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO26" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="AO26" t="n">
+        <v>2499</v>
+      </c>
+      <c r="AP26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ26" t="inlineStr">
+        <is>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -3323,7 +3439,13 @@
       <c r="AN27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO27" t="inlineStr">
+      <c r="AO27" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AP27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ27" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3391,6 +3513,8 @@
       <c r="AM28" t="inlineStr"/>
       <c r="AN28" s="4" t="inlineStr"/>
       <c r="AO28" t="inlineStr"/>
+      <c r="AP28" s="4" t="inlineStr"/>
+      <c r="AQ28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -3519,7 +3643,13 @@
       <c r="AN29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO29" t="inlineStr">
+      <c r="AO29" t="n">
+        <v>2866</v>
+      </c>
+      <c r="AP29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ29" t="inlineStr">
         <is>
           <t>2866</t>
         </is>
@@ -3652,7 +3782,13 @@
       <c r="AN30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO30" t="inlineStr">
+      <c r="AO30" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AP30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ30" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3785,9 +3921,15 @@
       <c r="AN31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AO31" t="inlineStr">
-        <is>
-          <t>3995</t>
+      <c r="AO31" t="n">
+        <v>3995</v>
+      </c>
+      <c r="AP31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ31" t="inlineStr">
+        <is>
+          <t>4201</t>
         </is>
       </c>
     </row>
@@ -3918,9 +4060,15 @@
       <c r="AN32" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AO32" t="inlineStr">
-        <is>
-          <t>2899</t>
+      <c r="AO32" t="n">
+        <v>2899</v>
+      </c>
+      <c r="AP32" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ32" t="inlineStr">
+        <is>
+          <t>3237</t>
         </is>
       </c>
     </row>
@@ -3998,6 +4146,8 @@
       <c r="AM33" t="inlineStr"/>
       <c r="AN33" s="4" t="inlineStr"/>
       <c r="AO33" t="inlineStr"/>
+      <c r="AP33" s="4" t="inlineStr"/>
+      <c r="AQ33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -4126,7 +4276,13 @@
       <c r="AN34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO34" t="inlineStr">
+      <c r="AO34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4259,9 +4415,15 @@
       <c r="AN35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO35" t="inlineStr">
-        <is>
-          <t>3006</t>
+      <c r="AO35" t="n">
+        <v>3006</v>
+      </c>
+      <c r="AP35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ35" t="inlineStr">
+        <is>
+          <t>3055</t>
         </is>
       </c>
     </row>
@@ -4392,9 +4554,15 @@
       <c r="AN36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO36" t="inlineStr">
-        <is>
-          <t>2521</t>
+      <c r="AO36" t="n">
+        <v>2521</v>
+      </c>
+      <c r="AP36" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ36" t="inlineStr">
+        <is>
+          <t>2870</t>
         </is>
       </c>
     </row>
@@ -4525,9 +4693,15 @@
       <c r="AN37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AO37" t="inlineStr">
-        <is>
-          <t>3905</t>
+      <c r="AO37" t="n">
+        <v>3905</v>
+      </c>
+      <c r="AP37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ37" t="inlineStr">
+        <is>
+          <t>4039</t>
         </is>
       </c>
     </row>
@@ -4658,9 +4832,15 @@
       <c r="AN38" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AO38" t="inlineStr">
-        <is>
-          <t>4133</t>
+      <c r="AO38" t="n">
+        <v>4133</v>
+      </c>
+      <c r="AP38" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="AQ38" t="inlineStr">
+        <is>
+          <t>4386</t>
         </is>
       </c>
     </row>
@@ -4791,9 +4971,15 @@
       <c r="AN39" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AO39" t="inlineStr">
-        <is>
-          <t>3788</t>
+      <c r="AO39" t="n">
+        <v>3788</v>
+      </c>
+      <c r="AP39" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AQ39" t="inlineStr">
+        <is>
+          <t>3994</t>
         </is>
       </c>
     </row>
@@ -4924,7 +5110,13 @@
       <c r="AN40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO40" t="inlineStr">
+      <c r="AO40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5057,9 +5249,15 @@
       <c r="AN41" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AO41" t="inlineStr">
-        <is>
-          <t>3700</t>
+      <c r="AO41" t="n">
+        <v>3700</v>
+      </c>
+      <c r="AP41" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AQ41" t="inlineStr">
+        <is>
+          <t>3993</t>
         </is>
       </c>
     </row>
@@ -5190,9 +5388,15 @@
       <c r="AN42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO42" t="inlineStr">
-        <is>
-          <t>2728</t>
+      <c r="AO42" t="n">
+        <v>2728</v>
+      </c>
+      <c r="AP42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ42" t="inlineStr">
+        <is>
+          <t>2860</t>
         </is>
       </c>
     </row>
@@ -5262,6 +5466,8 @@
       <c r="AM43" t="inlineStr"/>
       <c r="AN43" s="4" t="inlineStr"/>
       <c r="AO43" t="inlineStr"/>
+      <c r="AP43" s="4" t="inlineStr"/>
+      <c r="AQ43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -5357,6 +5563,8 @@
       <c r="AM44" t="inlineStr"/>
       <c r="AN44" s="4" t="inlineStr"/>
       <c r="AO44" t="inlineStr"/>
+      <c r="AP44" s="4" t="inlineStr"/>
+      <c r="AQ44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -5485,9 +5693,15 @@
       <c r="AN45" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="AO45" t="inlineStr">
-        <is>
-          <t>3329</t>
+      <c r="AO45" t="n">
+        <v>3329</v>
+      </c>
+      <c r="AP45" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AQ45" t="inlineStr">
+        <is>
+          <t>3550</t>
         </is>
       </c>
     </row>
@@ -5618,9 +5832,15 @@
       <c r="AN46" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="AO46" t="inlineStr">
-        <is>
-          <t>3123</t>
+      <c r="AO46" t="n">
+        <v>3123</v>
+      </c>
+      <c r="AP46" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AQ46" t="inlineStr">
+        <is>
+          <t>3313</t>
         </is>
       </c>
     </row>
@@ -5751,9 +5971,15 @@
       <c r="AN47" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AO47" t="inlineStr">
-        <is>
-          <t>4160</t>
+      <c r="AO47" t="n">
+        <v>4160</v>
+      </c>
+      <c r="AP47" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AQ47" t="inlineStr">
+        <is>
+          <t>4396</t>
         </is>
       </c>
     </row>
@@ -5884,9 +6110,15 @@
       <c r="AN48" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AO48" t="inlineStr">
-        <is>
-          <t>4108</t>
+      <c r="AO48" t="n">
+        <v>4108</v>
+      </c>
+      <c r="AP48" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ48" t="inlineStr">
+        <is>
+          <t>4297</t>
         </is>
       </c>
     </row>
@@ -6017,9 +6249,15 @@
       <c r="AN49" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AO49" t="inlineStr">
-        <is>
-          <t>3997</t>
+      <c r="AO49" t="n">
+        <v>3997</v>
+      </c>
+      <c r="AP49" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AQ49" t="inlineStr">
+        <is>
+          <t>4105</t>
         </is>
       </c>
     </row>
@@ -6150,9 +6388,15 @@
       <c r="AN50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AO50" t="inlineStr">
-        <is>
-          <t>3990</t>
+      <c r="AO50" t="n">
+        <v>3990</v>
+      </c>
+      <c r="AP50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AQ50" t="inlineStr">
+        <is>
+          <t>4133</t>
         </is>
       </c>
     </row>
@@ -6283,9 +6527,15 @@
       <c r="AN51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO51" t="inlineStr">
-        <is>
-          <t>2749</t>
+      <c r="AO51" t="n">
+        <v>2749</v>
+      </c>
+      <c r="AP51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ51" t="inlineStr">
+        <is>
+          <t>2801</t>
         </is>
       </c>
     </row>
@@ -6416,9 +6666,15 @@
       <c r="AN52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AO52" t="inlineStr">
-        <is>
-          <t>3996</t>
+      <c r="AO52" t="n">
+        <v>3996</v>
+      </c>
+      <c r="AP52" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AQ52" t="inlineStr">
+        <is>
+          <t>4045</t>
         </is>
       </c>
     </row>
@@ -6549,9 +6805,15 @@
       <c r="AN53" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="AO53" t="inlineStr">
-        <is>
-          <t>3126</t>
+      <c r="AO53" t="n">
+        <v>3126</v>
+      </c>
+      <c r="AP53" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="AQ53" t="inlineStr">
+        <is>
+          <t>3394</t>
         </is>
       </c>
     </row>
@@ -6682,9 +6944,15 @@
       <c r="AN54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO54" t="inlineStr">
-        <is>
-          <t>2530</t>
+      <c r="AO54" t="n">
+        <v>2530</v>
+      </c>
+      <c r="AP54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ54" t="inlineStr">
+        <is>
+          <t>2585</t>
         </is>
       </c>
     </row>
@@ -6815,9 +7083,15 @@
       <c r="AN55" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO55" t="inlineStr">
-        <is>
-          <t>2693</t>
+      <c r="AO55" t="n">
+        <v>2693</v>
+      </c>
+      <c r="AP55" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AQ55" t="inlineStr">
+        <is>
+          <t>2776</t>
         </is>
       </c>
     </row>
@@ -6948,9 +7222,15 @@
       <c r="AN56" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO56" t="inlineStr">
-        <is>
-          <t>3999</t>
+      <c r="AO56" t="n">
+        <v>3999</v>
+      </c>
+      <c r="AP56" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AQ56" t="inlineStr">
+        <is>
+          <t>4442</t>
         </is>
       </c>
     </row>
@@ -7081,9 +7361,15 @@
       <c r="AN57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AO57" t="inlineStr">
-        <is>
-          <t>3552</t>
+      <c r="AO57" t="n">
+        <v>3552</v>
+      </c>
+      <c r="AP57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ57" t="inlineStr">
+        <is>
+          <t>3746</t>
         </is>
       </c>
     </row>
@@ -7214,9 +7500,15 @@
       <c r="AN58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO58" t="inlineStr">
-        <is>
-          <t>2744</t>
+      <c r="AO58" t="n">
+        <v>2744</v>
+      </c>
+      <c r="AP58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AQ58" t="inlineStr">
+        <is>
+          <t>3024</t>
         </is>
       </c>
     </row>
@@ -7347,9 +7639,15 @@
       <c r="AN59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AO59" t="inlineStr">
-        <is>
-          <t>3405</t>
+      <c r="AO59" t="n">
+        <v>3405</v>
+      </c>
+      <c r="AP59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ59" t="inlineStr">
+        <is>
+          <t>3565</t>
         </is>
       </c>
     </row>
@@ -7480,9 +7778,15 @@
       <c r="AN60" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="AO60" t="inlineStr">
-        <is>
-          <t>3805</t>
+      <c r="AO60" t="n">
+        <v>3805</v>
+      </c>
+      <c r="AP60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AQ60" t="inlineStr">
+        <is>
+          <t>3985</t>
         </is>
       </c>
     </row>
@@ -7548,6 +7852,8 @@
       <c r="AM61" t="inlineStr"/>
       <c r="AN61" s="4" t="inlineStr"/>
       <c r="AO61" t="inlineStr"/>
+      <c r="AP61" s="4" t="inlineStr"/>
+      <c r="AQ61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -7676,9 +7982,15 @@
       <c r="AN62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AO62" t="inlineStr">
-        <is>
-          <t>3229</t>
+      <c r="AO62" t="n">
+        <v>3229</v>
+      </c>
+      <c r="AP62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ62" t="inlineStr">
+        <is>
+          <t>3428</t>
         </is>
       </c>
     </row>
@@ -7809,9 +8121,15 @@
       <c r="AN63" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO63" t="inlineStr">
-        <is>
-          <t>3226</t>
+      <c r="AO63" t="n">
+        <v>3226</v>
+      </c>
+      <c r="AP63" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AQ63" t="inlineStr">
+        <is>
+          <t>3527</t>
         </is>
       </c>
     </row>
@@ -7942,9 +8260,15 @@
       <c r="AN64" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="AO64" t="inlineStr">
-        <is>
-          <t>3644</t>
+      <c r="AO64" t="n">
+        <v>3644</v>
+      </c>
+      <c r="AP64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ64" t="inlineStr">
+        <is>
+          <t>3850</t>
         </is>
       </c>
     </row>
@@ -8075,9 +8399,15 @@
       <c r="AN65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO65" t="inlineStr">
-        <is>
-          <t>2829</t>
+      <c r="AO65" t="n">
+        <v>2829</v>
+      </c>
+      <c r="AP65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ65" t="inlineStr">
+        <is>
+          <t>2813</t>
         </is>
       </c>
     </row>
@@ -8208,7 +8538,13 @@
       <c r="AN66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO66" t="inlineStr">
+      <c r="AO66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8341,7 +8677,13 @@
       <c r="AN67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO67" t="inlineStr">
+      <c r="AO67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8474,7 +8816,13 @@
       <c r="AN68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO68" t="inlineStr">
+      <c r="AO68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8606,6 +8954,8 @@
       </c>
       <c r="AN69" s="4" t="inlineStr"/>
       <c r="AO69" t="inlineStr"/>
+      <c r="AP69" s="4" t="inlineStr"/>
+      <c r="AQ69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -8734,7 +9084,13 @@
       <c r="AN70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO70" t="inlineStr">
+      <c r="AO70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8867,7 +9223,13 @@
       <c r="AN71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO71" t="inlineStr">
+      <c r="AO71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9000,7 +9362,13 @@
       <c r="AN72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO72" t="inlineStr">
+      <c r="AO72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9133,9 +9501,15 @@
       <c r="AN73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO73" t="inlineStr">
-        <is>
-          <t>2554</t>
+      <c r="AO73" t="n">
+        <v>2554</v>
+      </c>
+      <c r="AP73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ73" t="inlineStr">
+        <is>
+          <t>2579</t>
         </is>
       </c>
     </row>
@@ -9266,9 +9640,15 @@
       <c r="AN74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO74" t="inlineStr">
-        <is>
-          <t>2518</t>
+      <c r="AO74" t="n">
+        <v>2518</v>
+      </c>
+      <c r="AP74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ74" t="inlineStr">
+        <is>
+          <t>2528</t>
         </is>
       </c>
     </row>
@@ -9399,7 +9779,13 @@
       <c r="AN75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO75" t="inlineStr">
+      <c r="AO75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9532,9 +9918,15 @@
       <c r="AN76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO76" t="inlineStr">
-        <is>
-          <t>2915</t>
+      <c r="AO76" t="n">
+        <v>2915</v>
+      </c>
+      <c r="AP76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ76" t="inlineStr">
+        <is>
+          <t>2946</t>
         </is>
       </c>
     </row>
@@ -9665,9 +10057,15 @@
       <c r="AN77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO77" t="inlineStr">
-        <is>
-          <t>2542</t>
+      <c r="AO77" t="n">
+        <v>2542</v>
+      </c>
+      <c r="AP77" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="AQ77" t="inlineStr">
+        <is>
+          <t>2830</t>
         </is>
       </c>
     </row>
@@ -9798,7 +10196,13 @@
       <c r="AN78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO78" t="inlineStr">
+      <c r="AO78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9931,9 +10335,15 @@
       <c r="AN79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO79" t="inlineStr">
-        <is>
-          <t>1328</t>
+      <c r="AO79" t="n">
+        <v>1328</v>
+      </c>
+      <c r="AP79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ79" t="inlineStr">
+        <is>
+          <t>1327</t>
         </is>
       </c>
     </row>
@@ -10064,7 +10474,13 @@
       <c r="AN80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO80" t="inlineStr">
+      <c r="AO80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10197,7 +10613,13 @@
       <c r="AN81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO81" t="inlineStr">
+      <c r="AO81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10330,7 +10752,13 @@
       <c r="AN82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO82" t="inlineStr">
+      <c r="AO82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10463,9 +10891,15 @@
       <c r="AN83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO83" t="inlineStr">
-        <is>
-          <t>2532</t>
+      <c r="AO83" t="n">
+        <v>2532</v>
+      </c>
+      <c r="AP83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ83" t="inlineStr">
+        <is>
+          <t>2585</t>
         </is>
       </c>
     </row>
@@ -10596,7 +11030,13 @@
       <c r="AN84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO84" t="inlineStr">
+      <c r="AO84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10729,7 +11169,13 @@
       <c r="AN85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO85" t="inlineStr">
+      <c r="AO85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10862,7 +11308,13 @@
       <c r="AN86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO86" t="inlineStr">
+      <c r="AO86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10995,7 +11447,13 @@
       <c r="AN87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO87" t="inlineStr">
+      <c r="AO87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11128,7 +11586,13 @@
       <c r="AN88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO88" t="inlineStr">
+      <c r="AO88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11261,7 +11725,13 @@
       <c r="AN89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO89" t="inlineStr">
+      <c r="AO89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11394,7 +11864,13 @@
       <c r="AN90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO90" t="inlineStr">
+      <c r="AO90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11527,7 +12003,13 @@
       <c r="AN91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO91" t="inlineStr">
+      <c r="AO91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11660,7 +12142,13 @@
       <c r="AN92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO92" t="inlineStr">
+      <c r="AO92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11793,7 +12281,13 @@
       <c r="AN93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO93" t="inlineStr">
+      <c r="AO93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11926,7 +12420,13 @@
       <c r="AN94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO94" t="inlineStr">
+      <c r="AO94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12059,7 +12559,13 @@
       <c r="AN95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO95" t="inlineStr">
+      <c r="AO95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12192,9 +12698,15 @@
       <c r="AN96" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AO96" t="inlineStr">
-        <is>
-          <t>3301</t>
+      <c r="AO96" t="n">
+        <v>3301</v>
+      </c>
+      <c r="AP96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ96" t="inlineStr">
+        <is>
+          <t>3263</t>
         </is>
       </c>
     </row>
@@ -12325,7 +12837,13 @@
       <c r="AN97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO97" t="inlineStr">
+      <c r="AO97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12458,7 +12976,13 @@
       <c r="AN98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO98" t="inlineStr">
+      <c r="AO98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12591,7 +13115,13 @@
       <c r="AN99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO99" t="inlineStr">
+      <c r="AO99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12724,7 +13254,13 @@
       <c r="AN100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO100" t="inlineStr">
+      <c r="AO100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12857,7 +13393,13 @@
       <c r="AN101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO101" t="inlineStr">
+      <c r="AO101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12990,7 +13532,13 @@
       <c r="AN102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO102" t="inlineStr">
+      <c r="AO102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13123,7 +13671,13 @@
       <c r="AN103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO103" t="inlineStr">
+      <c r="AO103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13256,7 +13810,13 @@
       <c r="AN104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO104" t="inlineStr">
+      <c r="AO104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13389,7 +13949,13 @@
       <c r="AN105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO105" t="inlineStr">
+      <c r="AO105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13449,6 +14015,8 @@
       <c r="AM106" t="inlineStr"/>
       <c r="AN106" s="4" t="inlineStr"/>
       <c r="AO106" t="inlineStr"/>
+      <c r="AP106" s="4" t="inlineStr"/>
+      <c r="AQ106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -13504,6 +14072,8 @@
       <c r="AM107" t="inlineStr"/>
       <c r="AN107" s="4" t="inlineStr"/>
       <c r="AO107" t="inlineStr"/>
+      <c r="AP107" s="4" t="inlineStr"/>
+      <c r="AQ107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -13559,6 +14129,8 @@
       <c r="AM108" t="inlineStr"/>
       <c r="AN108" s="4" t="inlineStr"/>
       <c r="AO108" t="inlineStr"/>
+      <c r="AP108" s="4" t="inlineStr"/>
+      <c r="AQ108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -13614,6 +14186,8 @@
       <c r="AM109" t="inlineStr"/>
       <c r="AN109" s="4" t="inlineStr"/>
       <c r="AO109" t="inlineStr"/>
+      <c r="AP109" s="4" t="inlineStr"/>
+      <c r="AQ109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -13669,6 +14243,8 @@
       <c r="AM110" t="inlineStr"/>
       <c r="AN110" s="4" t="inlineStr"/>
       <c r="AO110" t="inlineStr"/>
+      <c r="AP110" s="4" t="inlineStr"/>
+      <c r="AQ110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -13724,6 +14300,8 @@
       <c r="AM111" t="inlineStr"/>
       <c r="AN111" s="4" t="inlineStr"/>
       <c r="AO111" t="inlineStr"/>
+      <c r="AP111" s="4" t="inlineStr"/>
+      <c r="AQ111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -13779,6 +14357,8 @@
       <c r="AM112" t="inlineStr"/>
       <c r="AN112" s="4" t="inlineStr"/>
       <c r="AO112" t="inlineStr"/>
+      <c r="AP112" s="4" t="inlineStr"/>
+      <c r="AQ112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -13834,6 +14414,8 @@
       <c r="AM113" t="inlineStr"/>
       <c r="AN113" s="4" t="inlineStr"/>
       <c r="AO113" t="inlineStr"/>
+      <c r="AP113" s="4" t="inlineStr"/>
+      <c r="AQ113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -13889,6 +14471,8 @@
       <c r="AM114" t="inlineStr"/>
       <c r="AN114" s="4" t="inlineStr"/>
       <c r="AO114" t="inlineStr"/>
+      <c r="AP114" s="4" t="inlineStr"/>
+      <c r="AQ114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -13974,6 +14558,8 @@
       <c r="AM115" t="inlineStr"/>
       <c r="AN115" s="4" t="inlineStr"/>
       <c r="AO115" t="inlineStr"/>
+      <c r="AP115" s="4" t="inlineStr"/>
+      <c r="AQ115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -14059,6 +14645,8 @@
       <c r="AM116" t="inlineStr"/>
       <c r="AN116" s="4" t="inlineStr"/>
       <c r="AO116" t="inlineStr"/>
+      <c r="AP116" s="4" t="inlineStr"/>
+      <c r="AQ116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -14144,6 +14732,8 @@
       <c r="AM117" t="inlineStr"/>
       <c r="AN117" s="4" t="inlineStr"/>
       <c r="AO117" t="inlineStr"/>
+      <c r="AP117" s="4" t="inlineStr"/>
+      <c r="AQ117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -14261,6 +14851,8 @@
       </c>
       <c r="AN118" s="4" t="inlineStr"/>
       <c r="AO118" t="inlineStr"/>
+      <c r="AP118" s="4" t="inlineStr"/>
+      <c r="AQ118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -14367,9 +14959,15 @@
       <c r="AN119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO119" t="inlineStr">
-        <is>
-          <t>1512</t>
+      <c r="AO119" t="n">
+        <v>1512</v>
+      </c>
+      <c r="AP119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ119" t="inlineStr">
+        <is>
+          <t>1507</t>
         </is>
       </c>
     </row>
@@ -14458,9 +15056,15 @@
       <c r="AN120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO120" t="inlineStr">
-        <is>
-          <t>1820</t>
+      <c r="AO120" t="n">
+        <v>1820</v>
+      </c>
+      <c r="AP120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ120" t="inlineStr">
+        <is>
+          <t>1825</t>
         </is>
       </c>
     </row>
@@ -14525,9 +15129,15 @@
       <c r="AN121" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AO121" t="inlineStr">
-        <is>
-          <t>4515</t>
+      <c r="AO121" t="n">
+        <v>4515</v>
+      </c>
+      <c r="AP121" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ121" t="inlineStr">
+        <is>
+          <t>4941</t>
         </is>
       </c>
     </row>
@@ -14592,9 +15202,15 @@
       <c r="AN122" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AO122" t="inlineStr">
-        <is>
-          <t>3669</t>
+      <c r="AO122" t="n">
+        <v>3669</v>
+      </c>
+      <c r="AP122" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ122" t="inlineStr">
+        <is>
+          <t>3942</t>
         </is>
       </c>
     </row>
@@ -14651,9 +15267,78 @@
       <c r="AN123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO123" t="inlineStr">
+      <c r="AO123" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ123" t="inlineStr">
         <is>
           <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>59268644</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>"Time Keeper"</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr"/>
+      <c r="D124" t="inlineStr"/>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F124" s="4" t="inlineStr"/>
+      <c r="G124" t="inlineStr"/>
+      <c r="H124" s="4" t="inlineStr"/>
+      <c r="I124" t="inlineStr"/>
+      <c r="J124" s="4" t="inlineStr"/>
+      <c r="K124" t="inlineStr"/>
+      <c r="L124" s="4" t="inlineStr"/>
+      <c r="M124" t="inlineStr"/>
+      <c r="N124" s="4" t="inlineStr"/>
+      <c r="O124" t="inlineStr"/>
+      <c r="P124" s="4" t="inlineStr"/>
+      <c r="Q124" t="inlineStr"/>
+      <c r="R124" s="4" t="inlineStr"/>
+      <c r="S124" t="inlineStr"/>
+      <c r="T124" s="4" t="inlineStr"/>
+      <c r="U124" t="inlineStr"/>
+      <c r="V124" s="4" t="inlineStr"/>
+      <c r="W124" t="inlineStr"/>
+      <c r="X124" s="4" t="inlineStr"/>
+      <c r="Y124" t="inlineStr"/>
+      <c r="Z124" s="4" t="inlineStr"/>
+      <c r="AA124" t="inlineStr"/>
+      <c r="AB124" s="4" t="inlineStr"/>
+      <c r="AC124" t="inlineStr"/>
+      <c r="AD124" s="4" t="inlineStr"/>
+      <c r="AE124" t="inlineStr"/>
+      <c r="AF124" s="4" t="inlineStr"/>
+      <c r="AG124" t="inlineStr"/>
+      <c r="AH124" s="4" t="inlineStr"/>
+      <c r="AI124" t="inlineStr"/>
+      <c r="AJ124" s="4" t="inlineStr"/>
+      <c r="AK124" t="inlineStr"/>
+      <c r="AL124" s="4" t="inlineStr"/>
+      <c r="AM124" t="inlineStr"/>
+      <c r="AN124" s="4" t="inlineStr"/>
+      <c r="AO124" t="inlineStr"/>
+      <c r="AP124" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ124" t="inlineStr">
+        <is>
+          <t>1618</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-12 13:31:47
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -15280,10 +15280,8 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>59268644</t>
-        </is>
+      <c r="A124" t="n">
+        <v>59268644</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-05-13 13:14:17
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -3671,10 +3671,8 @@
       <c r="G114" t="inlineStr"/>
     </row>
     <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>21345373</t>
-        </is>
+      <c r="A115" t="n">
+        <v>21345373</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -3698,10 +3696,8 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="inlineStr">
-        <is>
-          <t>38996518</t>
-        </is>
+      <c r="A116" t="n">
+        <v>38996518</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
@@ -3725,10 +3721,8 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="inlineStr">
-        <is>
-          <t>138176</t>
-        </is>
+      <c r="A117" t="n">
+        <v>138176</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
@@ -3752,10 +3746,8 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="inlineStr">
-        <is>
-          <t>1976190</t>
-        </is>
+      <c r="A118" t="n">
+        <v>1976190</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -3779,10 +3771,8 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="inlineStr">
-        <is>
-          <t>8666978</t>
-        </is>
+      <c r="A119" t="n">
+        <v>8666978</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -3806,10 +3796,8 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="inlineStr">
-        <is>
-          <t>53947915</t>
-        </is>
+      <c r="A120" t="n">
+        <v>53947915</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
@@ -3833,10 +3821,8 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>59268644</t>
-        </is>
+      <c r="A121" t="n">
+        <v>59268644</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
@@ -3860,10 +3846,8 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>59304163</t>
-        </is>
+      <c r="A122" t="n">
+        <v>59304163</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-05-14 11:31:01
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G122"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,6 +426,16 @@
           <t>05-12_0</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>05-13_A</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>05-13_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -452,9 +462,15 @@
       <c r="F2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>2554</t>
+      <c r="G2" t="n">
+        <v>2554</v>
+      </c>
+      <c r="H2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2570</t>
         </is>
       </c>
     </row>
@@ -483,7 +499,13 @@
       <c r="F3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -514,7 +536,13 @@
       <c r="F4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -545,9 +573,15 @@
       <c r="F5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>2534</t>
+      <c r="G5" t="n">
+        <v>2534</v>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2561</t>
         </is>
       </c>
     </row>
@@ -576,9 +610,15 @@
       <c r="F6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>2503</t>
+      <c r="G6" t="n">
+        <v>2503</v>
+      </c>
+      <c r="H6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2544</t>
         </is>
       </c>
     </row>
@@ -602,6 +642,8 @@
       <c r="E7" t="inlineStr"/>
       <c r="F7" s="3" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
+      <c r="H7" s="3" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -623,6 +665,8 @@
       <c r="E8" t="inlineStr"/>
       <c r="F8" s="3" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
+      <c r="H8" s="3" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -644,6 +688,8 @@
       <c r="E9" t="inlineStr"/>
       <c r="F9" s="3" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
+      <c r="H9" s="3" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -665,6 +711,8 @@
       <c r="E10" t="inlineStr"/>
       <c r="F10" s="3" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
+      <c r="H10" s="3" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -686,6 +734,8 @@
       <c r="E11" t="inlineStr"/>
       <c r="F11" s="3" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
+      <c r="H11" s="3" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -707,6 +757,8 @@
       <c r="E12" t="inlineStr"/>
       <c r="F12" s="3" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
+      <c r="H12" s="3" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -728,6 +780,8 @@
       <c r="E13" t="inlineStr"/>
       <c r="F13" s="3" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
+      <c r="H13" s="3" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -749,6 +803,8 @@
       <c r="E14" t="inlineStr"/>
       <c r="F14" s="3" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
+      <c r="H14" s="3" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -770,6 +826,8 @@
       <c r="E15" t="inlineStr"/>
       <c r="F15" s="3" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
+      <c r="H15" s="3" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -791,6 +849,8 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" s="3" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
+      <c r="H16" s="3" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -812,6 +872,8 @@
       <c r="E17" t="inlineStr"/>
       <c r="F17" s="3" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
+      <c r="H17" s="3" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -838,9 +900,15 @@
       <c r="F18" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>3773</t>
+      <c r="G18" t="n">
+        <v>3773</v>
+      </c>
+      <c r="H18" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>3818</t>
         </is>
       </c>
     </row>
@@ -869,7 +937,13 @@
       <c r="F19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="G19" t="n">
+        <v>2669</v>
+      </c>
+      <c r="H19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="inlineStr">
         <is>
           <t>2669</t>
         </is>
@@ -900,9 +974,15 @@
       <c r="F20" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>3960</t>
+      <c r="G20" t="n">
+        <v>3960</v>
+      </c>
+      <c r="H20" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>4059</t>
         </is>
       </c>
     </row>
@@ -931,9 +1011,15 @@
       <c r="F21" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>4232</t>
+      <c r="G21" t="n">
+        <v>4232</v>
+      </c>
+      <c r="H21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>4182</t>
         </is>
       </c>
     </row>
@@ -962,9 +1048,15 @@
       <c r="F22" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>4234</t>
+      <c r="G22" t="n">
+        <v>4234</v>
+      </c>
+      <c r="H22" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>4458</t>
         </is>
       </c>
     </row>
@@ -993,9 +1085,15 @@
       <c r="F23" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>4591</t>
+      <c r="G23" t="n">
+        <v>4591</v>
+      </c>
+      <c r="H23" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>4913</t>
         </is>
       </c>
     </row>
@@ -1024,9 +1122,15 @@
       <c r="F24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>4184</t>
+      <c r="G24" t="n">
+        <v>4184</v>
+      </c>
+      <c r="H24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>4388</t>
         </is>
       </c>
     </row>
@@ -1055,9 +1159,15 @@
       <c r="F25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>4248</t>
+      <c r="G25" t="n">
+        <v>4248</v>
+      </c>
+      <c r="H25" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>4665</t>
         </is>
       </c>
     </row>
@@ -1086,9 +1196,15 @@
       <c r="F26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>2530</t>
+      <c r="G26" t="n">
+        <v>2530</v>
+      </c>
+      <c r="H26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>2578</t>
         </is>
       </c>
     </row>
@@ -1117,7 +1233,13 @@
       <c r="F27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="G27" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I27" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1143,6 +1265,8 @@
       <c r="E28" t="inlineStr"/>
       <c r="F28" s="3" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
+      <c r="H28" s="3" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1169,7 +1293,13 @@
       <c r="F29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="G29" t="n">
+        <v>2866</v>
+      </c>
+      <c r="H29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="inlineStr">
         <is>
           <t>2866</t>
         </is>
@@ -1200,7 +1330,13 @@
       <c r="F30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="G30" t="n">
+        <v>2500</v>
+      </c>
+      <c r="H30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1231,9 +1367,15 @@
       <c r="F31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>4306</t>
+      <c r="G31" t="n">
+        <v>4306</v>
+      </c>
+      <c r="H31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>4465</t>
         </is>
       </c>
     </row>
@@ -1262,9 +1404,15 @@
       <c r="F32" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>3597</t>
+      <c r="G32" t="n">
+        <v>3597</v>
+      </c>
+      <c r="H32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>3596</t>
         </is>
       </c>
     </row>
@@ -1288,6 +1436,8 @@
       <c r="E33" t="inlineStr"/>
       <c r="F33" s="3" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
+      <c r="H33" s="3" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1314,7 +1464,13 @@
       <c r="F34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1345,9 +1501,15 @@
       <c r="F35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>3050</t>
+      <c r="G35" t="n">
+        <v>3050</v>
+      </c>
+      <c r="H35" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>3424</t>
         </is>
       </c>
     </row>
@@ -1376,9 +1538,15 @@
       <c r="F36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>3252</t>
+      <c r="G36" t="n">
+        <v>3252</v>
+      </c>
+      <c r="H36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>3285</t>
         </is>
       </c>
     </row>
@@ -1407,9 +1575,15 @@
       <c r="F37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>4137</t>
+      <c r="G37" t="n">
+        <v>4137</v>
+      </c>
+      <c r="H37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>4346</t>
         </is>
       </c>
     </row>
@@ -1438,9 +1612,15 @@
       <c r="F38" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>4671</t>
+      <c r="G38" t="n">
+        <v>4671</v>
+      </c>
+      <c r="H38" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>4867</t>
         </is>
       </c>
     </row>
@@ -1469,9 +1649,15 @@
       <c r="F39" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>4122</t>
+      <c r="G39" t="n">
+        <v>4122</v>
+      </c>
+      <c r="H39" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>4295</t>
         </is>
       </c>
     </row>
@@ -1500,7 +1686,13 @@
       <c r="F40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+      <c r="H40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1531,9 +1723,15 @@
       <c r="F41" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>3995</t>
+      <c r="G41" t="n">
+        <v>3995</v>
+      </c>
+      <c r="H41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>4149</t>
         </is>
       </c>
     </row>
@@ -1562,9 +1760,15 @@
       <c r="F42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>2965</t>
+      <c r="G42" t="n">
+        <v>2965</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>3007</t>
         </is>
       </c>
     </row>
@@ -1588,6 +1792,8 @@
       <c r="E43" t="inlineStr"/>
       <c r="F43" s="3" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
+      <c r="H43" s="3" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1609,6 +1815,8 @@
       <c r="E44" t="inlineStr"/>
       <c r="F44" s="3" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
+      <c r="H44" s="3" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1635,9 +1843,15 @@
       <c r="F45" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>3773</t>
+      <c r="G45" t="n">
+        <v>3773</v>
+      </c>
+      <c r="H45" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>3940</t>
         </is>
       </c>
     </row>
@@ -1666,9 +1880,15 @@
       <c r="F46" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>3436</t>
+      <c r="G46" t="n">
+        <v>3436</v>
+      </c>
+      <c r="H46" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>3625</t>
         </is>
       </c>
     </row>
@@ -1697,9 +1917,15 @@
       <c r="F47" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>4665</t>
+      <c r="G47" t="n">
+        <v>4665</v>
+      </c>
+      <c r="H47" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>4818</t>
         </is>
       </c>
     </row>
@@ -1728,9 +1954,15 @@
       <c r="F48" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>4477</t>
+      <c r="G48" t="n">
+        <v>4477</v>
+      </c>
+      <c r="H48" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>4505</t>
         </is>
       </c>
     </row>
@@ -1759,9 +1991,15 @@
       <c r="F49" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>4259</t>
+      <c r="G49" t="n">
+        <v>4259</v>
+      </c>
+      <c r="H49" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>4419</t>
         </is>
       </c>
     </row>
@@ -1790,9 +2028,15 @@
       <c r="F50" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>4303</t>
+      <c r="G50" t="n">
+        <v>4303</v>
+      </c>
+      <c r="H50" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>4426</t>
         </is>
       </c>
     </row>
@@ -1821,9 +2065,15 @@
       <c r="F51" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>2902</t>
+      <c r="G51" t="n">
+        <v>2902</v>
+      </c>
+      <c r="H51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>2930</t>
         </is>
       </c>
     </row>
@@ -1852,9 +2102,15 @@
       <c r="F52" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>4337</t>
+      <c r="G52" t="n">
+        <v>4337</v>
+      </c>
+      <c r="H52" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>4474</t>
         </is>
       </c>
     </row>
@@ -1883,9 +2139,15 @@
       <c r="F53" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>3520</t>
+      <c r="G53" t="n">
+        <v>3520</v>
+      </c>
+      <c r="H53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>3593</t>
         </is>
       </c>
     </row>
@@ -1914,9 +2176,15 @@
       <c r="F54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>2636</t>
+      <c r="G54" t="n">
+        <v>2636</v>
+      </c>
+      <c r="H54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>2665</t>
         </is>
       </c>
     </row>
@@ -1945,9 +2213,15 @@
       <c r="F55" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>2916</t>
+      <c r="G55" t="n">
+        <v>2916</v>
+      </c>
+      <c r="H55" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>3364</t>
         </is>
       </c>
     </row>
@@ -1976,9 +2250,15 @@
       <c r="F56" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>4643</t>
+      <c r="G56" t="n">
+        <v>4643</v>
+      </c>
+      <c r="H56" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>4793</t>
         </is>
       </c>
     </row>
@@ -2007,9 +2287,15 @@
       <c r="F57" s="4" t="n">
         <v>19</v>
       </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>3976</t>
+      <c r="G57" t="n">
+        <v>3976</v>
+      </c>
+      <c r="H57" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>4040</t>
         </is>
       </c>
     </row>
@@ -2038,9 +2324,15 @@
       <c r="F58" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>3272</t>
+      <c r="G58" t="n">
+        <v>3272</v>
+      </c>
+      <c r="H58" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>3570</t>
         </is>
       </c>
     </row>
@@ -2069,9 +2361,15 @@
       <c r="F59" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>3806</t>
+      <c r="G59" t="n">
+        <v>3806</v>
+      </c>
+      <c r="H59" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>3992</t>
         </is>
       </c>
     </row>
@@ -2100,9 +2398,15 @@
       <c r="F60" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>3996</t>
+      <c r="G60" t="n">
+        <v>3996</v>
+      </c>
+      <c r="H60" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>4115</t>
         </is>
       </c>
     </row>
@@ -2126,6 +2430,8 @@
       <c r="E61" t="inlineStr"/>
       <c r="F61" s="3" t="inlineStr"/>
       <c r="G61" t="inlineStr"/>
+      <c r="H61" s="3" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -2152,9 +2458,15 @@
       <c r="F62" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>3617</t>
+      <c r="G62" t="n">
+        <v>3617</v>
+      </c>
+      <c r="H62" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>3823</t>
         </is>
       </c>
     </row>
@@ -2183,9 +2495,15 @@
       <c r="F63" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>3790</t>
+      <c r="G63" t="n">
+        <v>3790</v>
+      </c>
+      <c r="H63" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>3982</t>
         </is>
       </c>
     </row>
@@ -2214,9 +2532,15 @@
       <c r="F64" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>3992</t>
+      <c r="G64" t="n">
+        <v>3992</v>
+      </c>
+      <c r="H64" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>3999</t>
         </is>
       </c>
     </row>
@@ -2245,9 +2569,15 @@
       <c r="F65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>2809</t>
+      <c r="G65" t="n">
+        <v>2809</v>
+      </c>
+      <c r="H65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>2804</t>
         </is>
       </c>
     </row>
@@ -2276,7 +2606,13 @@
       <c r="F66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G66" t="inlineStr">
+      <c r="G66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2307,7 +2643,13 @@
       <c r="F67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G67" t="inlineStr">
+      <c r="G67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2338,7 +2680,13 @@
       <c r="F68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G68" t="inlineStr">
+      <c r="G68" t="n">
+        <v>0</v>
+      </c>
+      <c r="H68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2364,6 +2712,8 @@
       <c r="E69" t="inlineStr"/>
       <c r="F69" s="3" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
+      <c r="H69" s="3" t="inlineStr"/>
+      <c r="I69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -2390,7 +2740,13 @@
       <c r="F70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G70" t="inlineStr">
+      <c r="G70" t="n">
+        <v>0</v>
+      </c>
+      <c r="H70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2421,7 +2777,13 @@
       <c r="F71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G71" t="inlineStr">
+      <c r="G71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2452,7 +2814,13 @@
       <c r="F72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G72" t="inlineStr">
+      <c r="G72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2483,9 +2851,15 @@
       <c r="F73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>2594</t>
+      <c r="G73" t="n">
+        <v>2594</v>
+      </c>
+      <c r="H73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>2631</t>
         </is>
       </c>
     </row>
@@ -2514,9 +2888,15 @@
       <c r="F74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>2524</t>
+      <c r="G74" t="n">
+        <v>2524</v>
+      </c>
+      <c r="H74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>2553</t>
         </is>
       </c>
     </row>
@@ -2545,7 +2925,13 @@
       <c r="F75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G75" t="inlineStr">
+      <c r="G75" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2576,9 +2962,15 @@
       <c r="F76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>2946</t>
+      <c r="G76" t="n">
+        <v>2946</v>
+      </c>
+      <c r="H76" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>3241</t>
         </is>
       </c>
     </row>
@@ -2607,9 +2999,15 @@
       <c r="F77" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>2853</t>
+      <c r="G77" t="n">
+        <v>2853</v>
+      </c>
+      <c r="H77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>2850</t>
         </is>
       </c>
     </row>
@@ -2638,7 +3036,13 @@
       <c r="F78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G78" t="inlineStr">
+      <c r="G78" t="n">
+        <v>0</v>
+      </c>
+      <c r="H78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2669,9 +3073,15 @@
       <c r="F79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G79" t="inlineStr">
-        <is>
-          <t>1326</t>
+      <c r="G79" t="n">
+        <v>1326</v>
+      </c>
+      <c r="H79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>1323</t>
         </is>
       </c>
     </row>
@@ -2700,7 +3110,13 @@
       <c r="F80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G80" t="inlineStr">
+      <c r="G80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2731,7 +3147,13 @@
       <c r="F81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G81" t="inlineStr">
+      <c r="G81" t="n">
+        <v>0</v>
+      </c>
+      <c r="H81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2762,7 +3184,13 @@
       <c r="F82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G82" t="inlineStr">
+      <c r="G82" t="n">
+        <v>0</v>
+      </c>
+      <c r="H82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2793,9 +3221,15 @@
       <c r="F83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>2585</t>
+      <c r="G83" t="n">
+        <v>2585</v>
+      </c>
+      <c r="H83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>2584</t>
         </is>
       </c>
     </row>
@@ -2824,7 +3258,13 @@
       <c r="F84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G84" t="inlineStr">
+      <c r="G84" t="n">
+        <v>0</v>
+      </c>
+      <c r="H84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2855,7 +3295,13 @@
       <c r="F85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G85" t="inlineStr">
+      <c r="G85" t="n">
+        <v>0</v>
+      </c>
+      <c r="H85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2886,7 +3332,13 @@
       <c r="F86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G86" t="inlineStr">
+      <c r="G86" t="n">
+        <v>0</v>
+      </c>
+      <c r="H86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2917,7 +3369,13 @@
       <c r="F87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G87" t="inlineStr">
+      <c r="G87" t="n">
+        <v>0</v>
+      </c>
+      <c r="H87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2948,7 +3406,13 @@
       <c r="F88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G88" t="inlineStr">
+      <c r="G88" t="n">
+        <v>0</v>
+      </c>
+      <c r="H88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2979,7 +3443,13 @@
       <c r="F89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G89" t="inlineStr">
+      <c r="G89" t="n">
+        <v>0</v>
+      </c>
+      <c r="H89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3010,7 +3480,13 @@
       <c r="F90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G90" t="inlineStr">
+      <c r="G90" t="n">
+        <v>0</v>
+      </c>
+      <c r="H90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3041,7 +3517,13 @@
       <c r="F91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G91" t="inlineStr">
+      <c r="G91" t="n">
+        <v>0</v>
+      </c>
+      <c r="H91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3072,7 +3554,13 @@
       <c r="F92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G92" t="inlineStr">
+      <c r="G92" t="n">
+        <v>0</v>
+      </c>
+      <c r="H92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3103,7 +3591,13 @@
       <c r="F93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G93" t="inlineStr">
+      <c r="G93" t="n">
+        <v>0</v>
+      </c>
+      <c r="H93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3134,7 +3628,13 @@
       <c r="F94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G94" t="inlineStr">
+      <c r="G94" t="n">
+        <v>0</v>
+      </c>
+      <c r="H94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3165,7 +3665,13 @@
       <c r="F95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G95" t="inlineStr">
+      <c r="G95" t="n">
+        <v>0</v>
+      </c>
+      <c r="H95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3196,9 +3702,15 @@
       <c r="F96" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="G96" t="inlineStr">
-        <is>
-          <t>3721</t>
+      <c r="G96" t="n">
+        <v>3721</v>
+      </c>
+      <c r="H96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>3682</t>
         </is>
       </c>
     </row>
@@ -3227,7 +3739,13 @@
       <c r="F97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G97" t="inlineStr">
+      <c r="G97" t="n">
+        <v>0</v>
+      </c>
+      <c r="H97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3258,7 +3776,13 @@
       <c r="F98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G98" t="inlineStr">
+      <c r="G98" t="n">
+        <v>0</v>
+      </c>
+      <c r="H98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3289,7 +3813,13 @@
       <c r="F99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G99" t="inlineStr">
+      <c r="G99" t="n">
+        <v>0</v>
+      </c>
+      <c r="H99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3320,7 +3850,13 @@
       <c r="F100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G100" t="inlineStr">
+      <c r="G100" t="n">
+        <v>0</v>
+      </c>
+      <c r="H100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3351,7 +3887,13 @@
       <c r="F101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G101" t="inlineStr">
+      <c r="G101" t="n">
+        <v>0</v>
+      </c>
+      <c r="H101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3382,7 +3924,13 @@
       <c r="F102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G102" t="inlineStr">
+      <c r="G102" t="n">
+        <v>0</v>
+      </c>
+      <c r="H102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3413,7 +3961,13 @@
       <c r="F103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G103" t="inlineStr">
+      <c r="G103" t="n">
+        <v>0</v>
+      </c>
+      <c r="H103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3444,7 +3998,13 @@
       <c r="F104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G104" t="inlineStr">
+      <c r="G104" t="n">
+        <v>0</v>
+      </c>
+      <c r="H104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3475,7 +4035,13 @@
       <c r="F105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G105" t="inlineStr">
+      <c r="G105" t="n">
+        <v>0</v>
+      </c>
+      <c r="H105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3501,6 +4067,8 @@
       <c r="E106" t="inlineStr"/>
       <c r="F106" s="3" t="inlineStr"/>
       <c r="G106" t="inlineStr"/>
+      <c r="H106" s="3" t="inlineStr"/>
+      <c r="I106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -3522,6 +4090,8 @@
       <c r="E107" t="inlineStr"/>
       <c r="F107" s="3" t="inlineStr"/>
       <c r="G107" t="inlineStr"/>
+      <c r="H107" s="3" t="inlineStr"/>
+      <c r="I107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -3543,6 +4113,8 @@
       <c r="E108" t="inlineStr"/>
       <c r="F108" s="3" t="inlineStr"/>
       <c r="G108" t="inlineStr"/>
+      <c r="H108" s="3" t="inlineStr"/>
+      <c r="I108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -3564,6 +4136,8 @@
       <c r="E109" t="inlineStr"/>
       <c r="F109" s="3" t="inlineStr"/>
       <c r="G109" t="inlineStr"/>
+      <c r="H109" s="3" t="inlineStr"/>
+      <c r="I109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -3585,6 +4159,8 @@
       <c r="E110" t="inlineStr"/>
       <c r="F110" s="3" t="inlineStr"/>
       <c r="G110" t="inlineStr"/>
+      <c r="H110" s="3" t="inlineStr"/>
+      <c r="I110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -3606,6 +4182,8 @@
       <c r="E111" t="inlineStr"/>
       <c r="F111" s="3" t="inlineStr"/>
       <c r="G111" t="inlineStr"/>
+      <c r="H111" s="3" t="inlineStr"/>
+      <c r="I111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -3627,6 +4205,8 @@
       <c r="E112" t="inlineStr"/>
       <c r="F112" s="3" t="inlineStr"/>
       <c r="G112" t="inlineStr"/>
+      <c r="H112" s="3" t="inlineStr"/>
+      <c r="I112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -3648,6 +4228,8 @@
       <c r="E113" t="inlineStr"/>
       <c r="F113" s="3" t="inlineStr"/>
       <c r="G113" t="inlineStr"/>
+      <c r="H113" s="3" t="inlineStr"/>
+      <c r="I113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -3669,6 +4251,8 @@
       <c r="E114" t="inlineStr"/>
       <c r="F114" s="3" t="inlineStr"/>
       <c r="G114" t="inlineStr"/>
+      <c r="H114" s="3" t="inlineStr"/>
+      <c r="I114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -3689,9 +4273,15 @@
       <c r="F115" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="G115" t="inlineStr">
-        <is>
-          <t>4827</t>
+      <c r="G115" t="n">
+        <v>4827</v>
+      </c>
+      <c r="H115" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>5114</t>
         </is>
       </c>
     </row>
@@ -3714,9 +4304,15 @@
       <c r="F116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G116" t="inlineStr">
-        <is>
-          <t>999</t>
+      <c r="G116" t="n">
+        <v>999</v>
+      </c>
+      <c r="H116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3739,9 +4335,15 @@
       <c r="F117" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="G117" t="inlineStr">
-        <is>
-          <t>5111</t>
+      <c r="G117" t="n">
+        <v>5111</v>
+      </c>
+      <c r="H117" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>5412</t>
         </is>
       </c>
     </row>
@@ -3764,9 +4366,15 @@
       <c r="F118" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="G118" t="inlineStr">
-        <is>
-          <t>4211</t>
+      <c r="G118" t="n">
+        <v>4211</v>
+      </c>
+      <c r="H118" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>4355</t>
         </is>
       </c>
     </row>
@@ -3789,9 +4397,15 @@
       <c r="F119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G119" t="inlineStr">
-        <is>
-          <t>1506</t>
+      <c r="G119" t="n">
+        <v>1506</v>
+      </c>
+      <c r="H119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>1511</t>
         </is>
       </c>
     </row>
@@ -3814,9 +4428,15 @@
       <c r="F120" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="G120" t="inlineStr">
-        <is>
-          <t>1395</t>
+      <c r="G120" t="n">
+        <v>1395</v>
+      </c>
+      <c r="H120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>1727</t>
         </is>
       </c>
     </row>
@@ -3839,9 +4459,15 @@
       <c r="F121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G121" t="inlineStr">
-        <is>
-          <t>1617</t>
+      <c r="G121" t="n">
+        <v>1617</v>
+      </c>
+      <c r="H121" s="4" t="n">
+        <v>7</v>
+      </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>1729</t>
         </is>
       </c>
     </row>
@@ -3864,9 +4490,44 @@
       <c r="F122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="G122" t="inlineStr">
-        <is>
-          <t>1837</t>
+      <c r="G122" t="n">
+        <v>1837</v>
+      </c>
+      <c r="H122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>1876</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>29315425</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>"Terry Huang"</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr"/>
+      <c r="D123" t="inlineStr"/>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F123" s="3" t="inlineStr"/>
+      <c r="G123" t="inlineStr"/>
+      <c r="H123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>2612</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-15 11:30:49
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I123"/>
+  <dimension ref="A1:K125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,16 @@
           <t>05-13_0</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>05-14_A</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>05-14_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -468,7 +478,13 @@
       <c r="H2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" t="n">
+        <v>2570</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>2570</t>
         </is>
@@ -505,7 +521,13 @@
       <c r="H3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -542,7 +564,13 @@
       <c r="H4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -579,9 +607,15 @@
       <c r="H5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>2561</t>
+      <c r="I5" t="n">
+        <v>2561</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>2556</t>
         </is>
       </c>
     </row>
@@ -616,9 +650,15 @@
       <c r="H6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>2544</t>
+      <c r="I6" t="n">
+        <v>2544</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>2538</t>
         </is>
       </c>
     </row>
@@ -644,6 +684,8 @@
       <c r="G7" t="inlineStr"/>
       <c r="H7" s="3" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
+      <c r="J7" s="3" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -667,6 +709,8 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" s="3" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
+      <c r="J8" s="3" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -690,6 +734,8 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" s="3" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
+      <c r="J9" s="3" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -713,6 +759,8 @@
       <c r="G10" t="inlineStr"/>
       <c r="H10" s="3" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
+      <c r="J10" s="3" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -736,6 +784,8 @@
       <c r="G11" t="inlineStr"/>
       <c r="H11" s="3" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
+      <c r="J11" s="3" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -759,6 +809,8 @@
       <c r="G12" t="inlineStr"/>
       <c r="H12" s="3" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
+      <c r="J12" s="3" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -782,6 +834,8 @@
       <c r="G13" t="inlineStr"/>
       <c r="H13" s="3" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
+      <c r="J13" s="3" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -805,6 +859,8 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" s="3" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
+      <c r="J14" s="3" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -828,6 +884,8 @@
       <c r="G15" t="inlineStr"/>
       <c r="H15" s="3" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
+      <c r="J15" s="3" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -851,6 +909,8 @@
       <c r="G16" t="inlineStr"/>
       <c r="H16" s="3" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
+      <c r="J16" s="3" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -874,6 +934,8 @@
       <c r="G17" t="inlineStr"/>
       <c r="H17" s="3" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
+      <c r="J17" s="3" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -906,9 +968,15 @@
       <c r="H18" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>3818</t>
+      <c r="I18" t="n">
+        <v>3818</v>
+      </c>
+      <c r="J18" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>3990</t>
         </is>
       </c>
     </row>
@@ -943,7 +1011,13 @@
       <c r="H19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="I19" t="n">
+        <v>2669</v>
+      </c>
+      <c r="J19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="inlineStr">
         <is>
           <t>2669</t>
         </is>
@@ -980,9 +1054,15 @@
       <c r="H20" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>4059</t>
+      <c r="I20" t="n">
+        <v>4059</v>
+      </c>
+      <c r="J20" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>4100</t>
         </is>
       </c>
     </row>
@@ -1017,9 +1097,15 @@
       <c r="H21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>4182</t>
+      <c r="I21" t="n">
+        <v>4182</v>
+      </c>
+      <c r="J21" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>4441</t>
         </is>
       </c>
     </row>
@@ -1054,9 +1140,15 @@
       <c r="H22" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>4458</t>
+      <c r="I22" t="n">
+        <v>4458</v>
+      </c>
+      <c r="J22" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>4602</t>
         </is>
       </c>
     </row>
@@ -1091,9 +1183,15 @@
       <c r="H23" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>4913</t>
+      <c r="I23" t="n">
+        <v>4913</v>
+      </c>
+      <c r="J23" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>5129</t>
         </is>
       </c>
     </row>
@@ -1128,9 +1226,15 @@
       <c r="H24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I24" t="inlineStr">
-        <is>
-          <t>4388</t>
+      <c r="I24" t="n">
+        <v>4388</v>
+      </c>
+      <c r="J24" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>4566</t>
         </is>
       </c>
     </row>
@@ -1165,9 +1269,15 @@
       <c r="H25" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>4665</t>
+      <c r="I25" t="n">
+        <v>4665</v>
+      </c>
+      <c r="J25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>4706</t>
         </is>
       </c>
     </row>
@@ -1202,7 +1312,13 @@
       <c r="H26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="I26" t="n">
+        <v>2578</v>
+      </c>
+      <c r="J26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" t="inlineStr">
         <is>
           <t>2578</t>
         </is>
@@ -1239,7 +1355,13 @@
       <c r="H27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I27" t="inlineStr">
+      <c r="I27" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1267,6 +1389,8 @@
       <c r="G28" t="inlineStr"/>
       <c r="H28" s="3" t="inlineStr"/>
       <c r="I28" t="inlineStr"/>
+      <c r="J28" s="3" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1299,9 +1423,15 @@
       <c r="H29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>2866</t>
+      <c r="I29" t="n">
+        <v>2866</v>
+      </c>
+      <c r="J29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>2882</t>
         </is>
       </c>
     </row>
@@ -1336,7 +1466,13 @@
       <c r="H30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I30" t="inlineStr">
+      <c r="I30" t="n">
+        <v>2500</v>
+      </c>
+      <c r="J30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K30" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1373,9 +1509,15 @@
       <c r="H31" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>4465</t>
+      <c r="I31" t="n">
+        <v>4465</v>
+      </c>
+      <c r="J31" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>4626</t>
         </is>
       </c>
     </row>
@@ -1410,9 +1552,15 @@
       <c r="H32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>3596</t>
+      <c r="I32" t="n">
+        <v>3596</v>
+      </c>
+      <c r="J32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>3612</t>
         </is>
       </c>
     </row>
@@ -1438,6 +1586,8 @@
       <c r="G33" t="inlineStr"/>
       <c r="H33" s="3" t="inlineStr"/>
       <c r="I33" t="inlineStr"/>
+      <c r="J33" s="3" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1470,7 +1620,13 @@
       <c r="H34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I34" t="inlineStr">
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1507,9 +1663,15 @@
       <c r="H35" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>3424</t>
+      <c r="I35" t="n">
+        <v>3424</v>
+      </c>
+      <c r="J35" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>3985</t>
         </is>
       </c>
     </row>
@@ -1544,9 +1706,15 @@
       <c r="H36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>3285</t>
+      <c r="I36" t="n">
+        <v>3285</v>
+      </c>
+      <c r="J36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>3339</t>
         </is>
       </c>
     </row>
@@ -1581,9 +1749,15 @@
       <c r="H37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>4346</t>
+      <c r="I37" t="n">
+        <v>4346</v>
+      </c>
+      <c r="J37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>4485</t>
         </is>
       </c>
     </row>
@@ -1618,9 +1792,15 @@
       <c r="H38" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>4867</t>
+      <c r="I38" t="n">
+        <v>4867</v>
+      </c>
+      <c r="J38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>5001</t>
         </is>
       </c>
     </row>
@@ -1655,9 +1835,15 @@
       <c r="H39" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>4295</t>
+      <c r="I39" t="n">
+        <v>4295</v>
+      </c>
+      <c r="J39" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>4379</t>
         </is>
       </c>
     </row>
@@ -1692,7 +1878,13 @@
       <c r="H40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I40" t="inlineStr">
+      <c r="I40" t="n">
+        <v>0</v>
+      </c>
+      <c r="J40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1729,9 +1921,15 @@
       <c r="H41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I41" t="inlineStr">
-        <is>
-          <t>4149</t>
+      <c r="I41" t="n">
+        <v>4149</v>
+      </c>
+      <c r="J41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>4163</t>
         </is>
       </c>
     </row>
@@ -1766,9 +1964,15 @@
       <c r="H42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>3007</t>
+      <c r="I42" t="n">
+        <v>3007</v>
+      </c>
+      <c r="J42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>3076</t>
         </is>
       </c>
     </row>
@@ -1794,6 +1998,8 @@
       <c r="G43" t="inlineStr"/>
       <c r="H43" s="3" t="inlineStr"/>
       <c r="I43" t="inlineStr"/>
+      <c r="J43" s="3" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -1817,6 +2023,8 @@
       <c r="G44" t="inlineStr"/>
       <c r="H44" s="3" t="inlineStr"/>
       <c r="I44" t="inlineStr"/>
+      <c r="J44" s="3" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1849,9 +2057,15 @@
       <c r="H45" s="3" t="n">
         <v>27</v>
       </c>
-      <c r="I45" t="inlineStr">
-        <is>
-          <t>3940</t>
+      <c r="I45" t="n">
+        <v>3940</v>
+      </c>
+      <c r="J45" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>3982</t>
         </is>
       </c>
     </row>
@@ -1886,9 +2100,15 @@
       <c r="H46" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>3625</t>
+      <c r="I46" t="n">
+        <v>3625</v>
+      </c>
+      <c r="J46" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>3715</t>
         </is>
       </c>
     </row>
@@ -1923,9 +2143,15 @@
       <c r="H47" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>4818</t>
+      <c r="I47" t="n">
+        <v>4818</v>
+      </c>
+      <c r="J47" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>4990</t>
         </is>
       </c>
     </row>
@@ -1960,9 +2186,15 @@
       <c r="H48" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>4505</t>
+      <c r="I48" t="n">
+        <v>4505</v>
+      </c>
+      <c r="J48" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>4884</t>
         </is>
       </c>
     </row>
@@ -1997,9 +2229,15 @@
       <c r="H49" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="I49" t="inlineStr">
-        <is>
-          <t>4419</t>
+      <c r="I49" t="n">
+        <v>4419</v>
+      </c>
+      <c r="J49" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>4527</t>
         </is>
       </c>
     </row>
@@ -2034,9 +2272,15 @@
       <c r="H50" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>4426</t>
+      <c r="I50" t="n">
+        <v>4426</v>
+      </c>
+      <c r="J50" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>4611</t>
         </is>
       </c>
     </row>
@@ -2071,9 +2315,15 @@
       <c r="H51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>2930</t>
+      <c r="I51" t="n">
+        <v>2930</v>
+      </c>
+      <c r="J51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>3017</t>
         </is>
       </c>
     </row>
@@ -2108,9 +2358,15 @@
       <c r="H52" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>4474</t>
+      <c r="I52" t="n">
+        <v>4474</v>
+      </c>
+      <c r="J52" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>4786</t>
         </is>
       </c>
     </row>
@@ -2120,7 +2376,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Opalus</t>
+          <t>OPALUS</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2145,9 +2401,15 @@
       <c r="H53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>3593</t>
+      <c r="I53" t="n">
+        <v>3593</v>
+      </c>
+      <c r="J53" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>3673</t>
         </is>
       </c>
     </row>
@@ -2182,7 +2444,13 @@
       <c r="H54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I54" t="inlineStr">
+      <c r="I54" t="n">
+        <v>2665</v>
+      </c>
+      <c r="J54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K54" t="inlineStr">
         <is>
           <t>2665</t>
         </is>
@@ -2219,9 +2487,15 @@
       <c r="H55" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>3364</t>
+      <c r="I55" t="n">
+        <v>3364</v>
+      </c>
+      <c r="J55" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>3415</t>
         </is>
       </c>
     </row>
@@ -2256,9 +2530,15 @@
       <c r="H56" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>4793</t>
+      <c r="I56" t="n">
+        <v>4793</v>
+      </c>
+      <c r="J56" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>4951</t>
         </is>
       </c>
     </row>
@@ -2293,9 +2573,15 @@
       <c r="H57" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>4040</t>
+      <c r="I57" t="n">
+        <v>4040</v>
+      </c>
+      <c r="J57" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>4140</t>
         </is>
       </c>
     </row>
@@ -2330,9 +2616,15 @@
       <c r="H58" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>3570</t>
+      <c r="I58" t="n">
+        <v>3570</v>
+      </c>
+      <c r="J58" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>3811</t>
         </is>
       </c>
     </row>
@@ -2367,9 +2659,15 @@
       <c r="H59" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>3992</t>
+      <c r="I59" t="n">
+        <v>3992</v>
+      </c>
+      <c r="J59" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>3976</t>
         </is>
       </c>
     </row>
@@ -2404,9 +2702,15 @@
       <c r="H60" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>4115</t>
+      <c r="I60" t="n">
+        <v>4115</v>
+      </c>
+      <c r="J60" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>4180</t>
         </is>
       </c>
     </row>
@@ -2432,6 +2736,8 @@
       <c r="G61" t="inlineStr"/>
       <c r="H61" s="3" t="inlineStr"/>
       <c r="I61" t="inlineStr"/>
+      <c r="J61" s="3" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -2464,9 +2770,15 @@
       <c r="H62" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>3823</t>
+      <c r="I62" t="n">
+        <v>3823</v>
+      </c>
+      <c r="J62" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>3992</t>
         </is>
       </c>
     </row>
@@ -2501,9 +2813,15 @@
       <c r="H63" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>3982</t>
+      <c r="I63" t="n">
+        <v>3982</v>
+      </c>
+      <c r="J63" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -2538,9 +2856,15 @@
       <c r="H64" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>3999</t>
+      <c r="I64" t="n">
+        <v>3999</v>
+      </c>
+      <c r="J64" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>4012</t>
         </is>
       </c>
     </row>
@@ -2575,9 +2899,15 @@
       <c r="H65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>2804</t>
+      <c r="I65" t="n">
+        <v>2804</v>
+      </c>
+      <c r="J65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>2797</t>
         </is>
       </c>
     </row>
@@ -2612,7 +2942,13 @@
       <c r="H66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I66" t="inlineStr">
+      <c r="I66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2649,7 +2985,13 @@
       <c r="H67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I67" t="inlineStr">
+      <c r="I67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2686,7 +3028,13 @@
       <c r="H68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I68" t="inlineStr">
+      <c r="I68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2714,6 +3062,8 @@
       <c r="G69" t="inlineStr"/>
       <c r="H69" s="3" t="inlineStr"/>
       <c r="I69" t="inlineStr"/>
+      <c r="J69" s="3" t="inlineStr"/>
+      <c r="K69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -2746,7 +3096,13 @@
       <c r="H70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I70" t="inlineStr">
+      <c r="I70" t="n">
+        <v>0</v>
+      </c>
+      <c r="J70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2783,7 +3139,13 @@
       <c r="H71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I71" t="inlineStr">
+      <c r="I71" t="n">
+        <v>0</v>
+      </c>
+      <c r="J71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2820,7 +3182,13 @@
       <c r="H72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I72" t="inlineStr">
+      <c r="I72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2857,9 +3225,15 @@
       <c r="H73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>2631</t>
+      <c r="I73" t="n">
+        <v>2631</v>
+      </c>
+      <c r="J73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>2732</t>
         </is>
       </c>
     </row>
@@ -2894,9 +3268,15 @@
       <c r="H74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>2553</t>
+      <c r="I74" t="n">
+        <v>2553</v>
+      </c>
+      <c r="J74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>2548</t>
         </is>
       </c>
     </row>
@@ -2931,7 +3311,13 @@
       <c r="H75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I75" t="inlineStr">
+      <c r="I75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2968,9 +3354,15 @@
       <c r="H76" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t>3241</t>
+      <c r="I76" t="n">
+        <v>3241</v>
+      </c>
+      <c r="J76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>3267</t>
         </is>
       </c>
     </row>
@@ -3005,9 +3397,15 @@
       <c r="H77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>2850</t>
+      <c r="I77" t="n">
+        <v>2850</v>
+      </c>
+      <c r="J77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>2841</t>
         </is>
       </c>
     </row>
@@ -3042,7 +3440,13 @@
       <c r="H78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I78" t="inlineStr">
+      <c r="I78" t="n">
+        <v>0</v>
+      </c>
+      <c r="J78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3079,9 +3483,15 @@
       <c r="H79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>1323</t>
+      <c r="I79" t="n">
+        <v>1323</v>
+      </c>
+      <c r="J79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3116,7 +3526,13 @@
       <c r="H80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I80" t="inlineStr">
+      <c r="I80" t="n">
+        <v>0</v>
+      </c>
+      <c r="J80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3153,7 +3569,13 @@
       <c r="H81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I81" t="inlineStr">
+      <c r="I81" t="n">
+        <v>0</v>
+      </c>
+      <c r="J81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3190,7 +3612,13 @@
       <c r="H82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I82" t="inlineStr">
+      <c r="I82" t="n">
+        <v>0</v>
+      </c>
+      <c r="J82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3227,9 +3655,15 @@
       <c r="H83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>2584</t>
+      <c r="I83" t="n">
+        <v>2584</v>
+      </c>
+      <c r="J83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>2580</t>
         </is>
       </c>
     </row>
@@ -3264,7 +3698,13 @@
       <c r="H84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I84" t="inlineStr">
+      <c r="I84" t="n">
+        <v>0</v>
+      </c>
+      <c r="J84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3301,7 +3741,13 @@
       <c r="H85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I85" t="inlineStr">
+      <c r="I85" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3338,7 +3784,13 @@
       <c r="H86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I86" t="inlineStr">
+      <c r="I86" t="n">
+        <v>0</v>
+      </c>
+      <c r="J86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3375,7 +3827,13 @@
       <c r="H87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I87" t="inlineStr">
+      <c r="I87" t="n">
+        <v>0</v>
+      </c>
+      <c r="J87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3412,7 +3870,13 @@
       <c r="H88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I88" t="inlineStr">
+      <c r="I88" t="n">
+        <v>0</v>
+      </c>
+      <c r="J88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3449,7 +3913,13 @@
       <c r="H89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I89" t="inlineStr">
+      <c r="I89" t="n">
+        <v>0</v>
+      </c>
+      <c r="J89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3486,7 +3956,13 @@
       <c r="H90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I90" t="inlineStr">
+      <c r="I90" t="n">
+        <v>0</v>
+      </c>
+      <c r="J90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3523,7 +3999,13 @@
       <c r="H91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I91" t="inlineStr">
+      <c r="I91" t="n">
+        <v>0</v>
+      </c>
+      <c r="J91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3560,7 +4042,13 @@
       <c r="H92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I92" t="inlineStr">
+      <c r="I92" t="n">
+        <v>0</v>
+      </c>
+      <c r="J92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3597,7 +4085,13 @@
       <c r="H93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I93" t="inlineStr">
+      <c r="I93" t="n">
+        <v>0</v>
+      </c>
+      <c r="J93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3634,7 +4128,13 @@
       <c r="H94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I94" t="inlineStr">
+      <c r="I94" t="n">
+        <v>0</v>
+      </c>
+      <c r="J94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3671,7 +4171,13 @@
       <c r="H95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I95" t="inlineStr">
+      <c r="I95" t="n">
+        <v>0</v>
+      </c>
+      <c r="J95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3708,9 +4214,15 @@
       <c r="H96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>3682</t>
+      <c r="I96" t="n">
+        <v>3682</v>
+      </c>
+      <c r="J96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>3649</t>
         </is>
       </c>
     </row>
@@ -3745,7 +4257,13 @@
       <c r="H97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I97" t="inlineStr">
+      <c r="I97" t="n">
+        <v>0</v>
+      </c>
+      <c r="J97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3782,7 +4300,13 @@
       <c r="H98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I98" t="inlineStr">
+      <c r="I98" t="n">
+        <v>0</v>
+      </c>
+      <c r="J98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3819,7 +4343,13 @@
       <c r="H99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I99" t="inlineStr">
+      <c r="I99" t="n">
+        <v>0</v>
+      </c>
+      <c r="J99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3856,7 +4386,13 @@
       <c r="H100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I100" t="inlineStr">
+      <c r="I100" t="n">
+        <v>0</v>
+      </c>
+      <c r="J100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3893,7 +4429,13 @@
       <c r="H101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I101" t="inlineStr">
+      <c r="I101" t="n">
+        <v>0</v>
+      </c>
+      <c r="J101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3930,7 +4472,13 @@
       <c r="H102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I102" t="inlineStr">
+      <c r="I102" t="n">
+        <v>0</v>
+      </c>
+      <c r="J102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3967,7 +4515,13 @@
       <c r="H103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I103" t="inlineStr">
+      <c r="I103" t="n">
+        <v>0</v>
+      </c>
+      <c r="J103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4004,7 +4558,13 @@
       <c r="H104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I104" t="inlineStr">
+      <c r="I104" t="n">
+        <v>0</v>
+      </c>
+      <c r="J104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4041,7 +4601,13 @@
       <c r="H105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I105" t="inlineStr">
+      <c r="I105" t="n">
+        <v>0</v>
+      </c>
+      <c r="J105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4069,6 +4635,8 @@
       <c r="G106" t="inlineStr"/>
       <c r="H106" s="3" t="inlineStr"/>
       <c r="I106" t="inlineStr"/>
+      <c r="J106" s="3" t="inlineStr"/>
+      <c r="K106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -4092,6 +4660,8 @@
       <c r="G107" t="inlineStr"/>
       <c r="H107" s="3" t="inlineStr"/>
       <c r="I107" t="inlineStr"/>
+      <c r="J107" s="3" t="inlineStr"/>
+      <c r="K107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -4115,6 +4685,8 @@
       <c r="G108" t="inlineStr"/>
       <c r="H108" s="3" t="inlineStr"/>
       <c r="I108" t="inlineStr"/>
+      <c r="J108" s="3" t="inlineStr"/>
+      <c r="K108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -4138,6 +4710,8 @@
       <c r="G109" t="inlineStr"/>
       <c r="H109" s="3" t="inlineStr"/>
       <c r="I109" t="inlineStr"/>
+      <c r="J109" s="3" t="inlineStr"/>
+      <c r="K109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -4161,6 +4735,8 @@
       <c r="G110" t="inlineStr"/>
       <c r="H110" s="3" t="inlineStr"/>
       <c r="I110" t="inlineStr"/>
+      <c r="J110" s="3" t="inlineStr"/>
+      <c r="K110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -4184,6 +4760,8 @@
       <c r="G111" t="inlineStr"/>
       <c r="H111" s="3" t="inlineStr"/>
       <c r="I111" t="inlineStr"/>
+      <c r="J111" s="3" t="inlineStr"/>
+      <c r="K111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -4207,6 +4785,8 @@
       <c r="G112" t="inlineStr"/>
       <c r="H112" s="3" t="inlineStr"/>
       <c r="I112" t="inlineStr"/>
+      <c r="J112" s="3" t="inlineStr"/>
+      <c r="K112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -4230,6 +4810,8 @@
       <c r="G113" t="inlineStr"/>
       <c r="H113" s="3" t="inlineStr"/>
       <c r="I113" t="inlineStr"/>
+      <c r="J113" s="3" t="inlineStr"/>
+      <c r="K113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -4253,6 +4835,8 @@
       <c r="G114" t="inlineStr"/>
       <c r="H114" s="3" t="inlineStr"/>
       <c r="I114" t="inlineStr"/>
+      <c r="J114" s="3" t="inlineStr"/>
+      <c r="K114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -4279,9 +4863,15 @@
       <c r="H115" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>5114</t>
+      <c r="I115" t="n">
+        <v>5114</v>
+      </c>
+      <c r="J115" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>5535</t>
         </is>
       </c>
     </row>
@@ -4310,9 +4900,15 @@
       <c r="H116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="I116" t="n">
+        <v>0</v>
+      </c>
+      <c r="J116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>998</t>
         </is>
       </c>
     </row>
@@ -4341,9 +4937,15 @@
       <c r="H117" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="I117" t="inlineStr">
-        <is>
-          <t>5412</t>
+      <c r="I117" t="n">
+        <v>5412</v>
+      </c>
+      <c r="J117" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>5414</t>
         </is>
       </c>
     </row>
@@ -4372,9 +4974,15 @@
       <c r="H118" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I118" t="inlineStr">
-        <is>
-          <t>4355</t>
+      <c r="I118" t="n">
+        <v>4355</v>
+      </c>
+      <c r="J118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>4366</t>
         </is>
       </c>
     </row>
@@ -4403,9 +5011,15 @@
       <c r="H119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I119" t="inlineStr">
-        <is>
-          <t>1511</t>
+      <c r="I119" t="n">
+        <v>1511</v>
+      </c>
+      <c r="J119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>1541</t>
         </is>
       </c>
     </row>
@@ -4434,9 +5048,15 @@
       <c r="H120" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="I120" t="inlineStr">
-        <is>
-          <t>1727</t>
+      <c r="I120" t="n">
+        <v>1727</v>
+      </c>
+      <c r="J120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>2031</t>
         </is>
       </c>
     </row>
@@ -4465,9 +5085,15 @@
       <c r="H121" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="I121" t="inlineStr">
-        <is>
-          <t>1729</t>
+      <c r="I121" t="n">
+        <v>1729</v>
+      </c>
+      <c r="J121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>1727</t>
         </is>
       </c>
     </row>
@@ -4496,17 +5122,21 @@
       <c r="H122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I122" t="inlineStr">
-        <is>
-          <t>1876</t>
+      <c r="I122" t="n">
+        <v>1876</v>
+      </c>
+      <c r="J122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>1938</t>
         </is>
       </c>
     </row>
     <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>29315425</t>
-        </is>
+      <c r="A123" t="n">
+        <v>29315425</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
@@ -4525,9 +5155,77 @@
       <c r="H123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I123" t="inlineStr">
-        <is>
-          <t>2612</t>
+      <c r="I123" t="n">
+        <v>2612</v>
+      </c>
+      <c r="J123" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>2713</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>50975641</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>"dit nhau"</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr"/>
+      <c r="D124" t="inlineStr"/>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F124" s="3" t="inlineStr"/>
+      <c r="G124" t="inlineStr"/>
+      <c r="H124" s="3" t="inlineStr"/>
+      <c r="I124" t="inlineStr"/>
+      <c r="J124" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>3992</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>57467416</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>IntentFormula46</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr"/>
+      <c r="D125" t="inlineStr"/>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F125" s="3" t="inlineStr"/>
+      <c r="G125" t="inlineStr"/>
+      <c r="H125" s="3" t="inlineStr"/>
+      <c r="I125" t="inlineStr"/>
+      <c r="J125" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>1534</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-16 11:30:55
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K125"/>
+  <dimension ref="A1:M125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,6 +446,16 @@
           <t>05-14_0</t>
         </is>
       </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>05-15_A</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>05-15_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -484,9 +494,15 @@
       <c r="J2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>2570</t>
+      <c r="K2" t="n">
+        <v>2570</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>2586</t>
         </is>
       </c>
     </row>
@@ -527,7 +543,13 @@
       <c r="J3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K3" t="inlineStr">
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -570,7 +592,13 @@
       <c r="J4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -613,9 +641,15 @@
       <c r="J5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>2556</t>
+      <c r="K5" t="n">
+        <v>2556</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>2552</t>
         </is>
       </c>
     </row>
@@ -656,9 +690,15 @@
       <c r="J6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>2538</t>
+      <c r="K6" t="n">
+        <v>2538</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>2570</t>
         </is>
       </c>
     </row>
@@ -686,6 +726,8 @@
       <c r="I7" t="inlineStr"/>
       <c r="J7" s="3" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
+      <c r="L7" s="3" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -711,6 +753,8 @@
       <c r="I8" t="inlineStr"/>
       <c r="J8" s="3" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
+      <c r="L8" s="3" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -736,6 +780,8 @@
       <c r="I9" t="inlineStr"/>
       <c r="J9" s="3" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
+      <c r="L9" s="3" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -761,6 +807,8 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" s="3" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
+      <c r="L10" s="3" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -786,6 +834,8 @@
       <c r="I11" t="inlineStr"/>
       <c r="J11" s="3" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
+      <c r="L11" s="3" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -811,6 +861,8 @@
       <c r="I12" t="inlineStr"/>
       <c r="J12" s="3" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
+      <c r="L12" s="3" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -836,6 +888,8 @@
       <c r="I13" t="inlineStr"/>
       <c r="J13" s="3" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
+      <c r="L13" s="3" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -861,6 +915,8 @@
       <c r="I14" t="inlineStr"/>
       <c r="J14" s="3" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
+      <c r="L14" s="3" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -886,6 +942,8 @@
       <c r="I15" t="inlineStr"/>
       <c r="J15" s="3" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
+      <c r="L15" s="3" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -911,6 +969,8 @@
       <c r="I16" t="inlineStr"/>
       <c r="J16" s="3" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
+      <c r="L16" s="3" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -936,6 +996,8 @@
       <c r="I17" t="inlineStr"/>
       <c r="J17" s="3" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
+      <c r="L17" s="3" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -974,9 +1036,15 @@
       <c r="J18" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>3990</t>
+      <c r="K18" t="n">
+        <v>3990</v>
+      </c>
+      <c r="L18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>3983</t>
         </is>
       </c>
     </row>
@@ -1017,9 +1085,15 @@
       <c r="J19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>2669</t>
+      <c r="K19" t="n">
+        <v>2669</v>
+      </c>
+      <c r="L19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>2701</t>
         </is>
       </c>
     </row>
@@ -1060,9 +1134,15 @@
       <c r="J20" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>4100</t>
+      <c r="K20" t="n">
+        <v>4100</v>
+      </c>
+      <c r="L20" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>4217</t>
         </is>
       </c>
     </row>
@@ -1103,9 +1183,15 @@
       <c r="J21" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>4441</t>
+      <c r="K21" t="n">
+        <v>4441</v>
+      </c>
+      <c r="L21" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>4591</t>
         </is>
       </c>
     </row>
@@ -1146,9 +1232,15 @@
       <c r="J22" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K22" t="inlineStr">
-        <is>
-          <t>4602</t>
+      <c r="K22" t="n">
+        <v>4602</v>
+      </c>
+      <c r="L22" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>4759</t>
         </is>
       </c>
     </row>
@@ -1189,9 +1281,15 @@
       <c r="J23" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K23" t="inlineStr">
-        <is>
-          <t>5129</t>
+      <c r="K23" t="n">
+        <v>5129</v>
+      </c>
+      <c r="L23" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>5387</t>
         </is>
       </c>
     </row>
@@ -1232,9 +1330,15 @@
       <c r="J24" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="K24" t="inlineStr">
-        <is>
-          <t>4566</t>
+      <c r="K24" t="n">
+        <v>4566</v>
+      </c>
+      <c r="L24" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>4737</t>
         </is>
       </c>
     </row>
@@ -1275,9 +1379,15 @@
       <c r="J25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K25" t="inlineStr">
-        <is>
-          <t>4706</t>
+      <c r="K25" t="n">
+        <v>4706</v>
+      </c>
+      <c r="L25" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>5075</t>
         </is>
       </c>
     </row>
@@ -1318,7 +1428,13 @@
       <c r="J26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K26" t="inlineStr">
+      <c r="K26" t="n">
+        <v>2578</v>
+      </c>
+      <c r="L26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M26" t="inlineStr">
         <is>
           <t>2578</t>
         </is>
@@ -1361,9 +1477,15 @@
       <c r="J27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="K27" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>2516</t>
         </is>
       </c>
     </row>
@@ -1391,6 +1513,8 @@
       <c r="I28" t="inlineStr"/>
       <c r="J28" s="3" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
+      <c r="L28" s="3" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1429,9 +1553,15 @@
       <c r="J29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K29" t="inlineStr">
-        <is>
-          <t>2882</t>
+      <c r="K29" t="n">
+        <v>2882</v>
+      </c>
+      <c r="L29" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>3420</t>
         </is>
       </c>
     </row>
@@ -1472,7 +1602,13 @@
       <c r="J30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K30" t="inlineStr">
+      <c r="K30" t="n">
+        <v>2500</v>
+      </c>
+      <c r="L30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M30" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1515,9 +1651,15 @@
       <c r="J31" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="K31" t="inlineStr">
-        <is>
-          <t>4626</t>
+      <c r="K31" t="n">
+        <v>4626</v>
+      </c>
+      <c r="L31" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>4793</t>
         </is>
       </c>
     </row>
@@ -1558,9 +1700,15 @@
       <c r="J32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K32" t="inlineStr">
-        <is>
-          <t>3612</t>
+      <c r="K32" t="n">
+        <v>3612</v>
+      </c>
+      <c r="L32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>3640</t>
         </is>
       </c>
     </row>
@@ -1588,6 +1736,8 @@
       <c r="I33" t="inlineStr"/>
       <c r="J33" s="3" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
+      <c r="L33" s="3" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1626,7 +1776,13 @@
       <c r="J34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K34" t="inlineStr">
+      <c r="K34" t="n">
+        <v>0</v>
+      </c>
+      <c r="L34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1669,9 +1825,15 @@
       <c r="J35" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K35" t="inlineStr">
-        <is>
-          <t>3985</t>
+      <c r="K35" t="n">
+        <v>3985</v>
+      </c>
+      <c r="L35" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>4316</t>
         </is>
       </c>
     </row>
@@ -1712,9 +1874,15 @@
       <c r="J36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K36" t="inlineStr">
-        <is>
-          <t>3339</t>
+      <c r="K36" t="n">
+        <v>3339</v>
+      </c>
+      <c r="L36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>3716</t>
         </is>
       </c>
     </row>
@@ -1755,9 +1923,15 @@
       <c r="J37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K37" t="inlineStr">
-        <is>
-          <t>4485</t>
+      <c r="K37" t="n">
+        <v>4485</v>
+      </c>
+      <c r="L37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>4581</t>
         </is>
       </c>
     </row>
@@ -1798,9 +1972,15 @@
       <c r="J38" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K38" t="inlineStr">
-        <is>
-          <t>5001</t>
+      <c r="K38" t="n">
+        <v>5001</v>
+      </c>
+      <c r="L38" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>5210</t>
         </is>
       </c>
     </row>
@@ -1841,9 +2021,15 @@
       <c r="J39" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K39" t="inlineStr">
-        <is>
-          <t>4379</t>
+      <c r="K39" t="n">
+        <v>4379</v>
+      </c>
+      <c r="L39" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>4457</t>
         </is>
       </c>
     </row>
@@ -1884,7 +2070,13 @@
       <c r="J40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K40" t="inlineStr">
+      <c r="K40" t="n">
+        <v>0</v>
+      </c>
+      <c r="L40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1927,9 +2119,15 @@
       <c r="J41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K41" t="inlineStr">
-        <is>
-          <t>4163</t>
+      <c r="K41" t="n">
+        <v>4163</v>
+      </c>
+      <c r="L41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>4275</t>
         </is>
       </c>
     </row>
@@ -1970,9 +2168,15 @@
       <c r="J42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>3076</t>
+      <c r="K42" t="n">
+        <v>3076</v>
+      </c>
+      <c r="L42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>3232</t>
         </is>
       </c>
     </row>
@@ -2000,6 +2204,8 @@
       <c r="I43" t="inlineStr"/>
       <c r="J43" s="3" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
+      <c r="L43" s="3" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2025,6 +2231,8 @@
       <c r="I44" t="inlineStr"/>
       <c r="J44" s="3" t="inlineStr"/>
       <c r="K44" t="inlineStr"/>
+      <c r="L44" s="3" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -2063,9 +2271,15 @@
       <c r="J45" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="K45" t="inlineStr">
-        <is>
-          <t>3982</t>
+      <c r="K45" t="n">
+        <v>3982</v>
+      </c>
+      <c r="L45" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>3986</t>
         </is>
       </c>
     </row>
@@ -2106,9 +2320,15 @@
       <c r="J46" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="K46" t="inlineStr">
-        <is>
-          <t>3715</t>
+      <c r="K46" t="n">
+        <v>3715</v>
+      </c>
+      <c r="L46" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>3789</t>
         </is>
       </c>
     </row>
@@ -2149,9 +2369,15 @@
       <c r="J47" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="K47" t="inlineStr">
-        <is>
-          <t>4990</t>
+      <c r="K47" t="n">
+        <v>4990</v>
+      </c>
+      <c r="L47" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>5209</t>
         </is>
       </c>
     </row>
@@ -2192,9 +2418,15 @@
       <c r="J48" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>4884</t>
+      <c r="K48" t="n">
+        <v>4884</v>
+      </c>
+      <c r="L48" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>5064</t>
         </is>
       </c>
     </row>
@@ -2235,9 +2467,15 @@
       <c r="J49" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>4527</t>
+      <c r="K49" t="n">
+        <v>4527</v>
+      </c>
+      <c r="L49" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>4658</t>
         </is>
       </c>
     </row>
@@ -2278,9 +2516,15 @@
       <c r="J50" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>4611</t>
+      <c r="K50" t="n">
+        <v>4611</v>
+      </c>
+      <c r="L50" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>4779</t>
         </is>
       </c>
     </row>
@@ -2321,9 +2565,15 @@
       <c r="J51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>3017</t>
+      <c r="K51" t="n">
+        <v>3017</v>
+      </c>
+      <c r="L51" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>3341</t>
         </is>
       </c>
     </row>
@@ -2364,9 +2614,15 @@
       <c r="J52" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>4786</t>
+      <c r="K52" t="n">
+        <v>4786</v>
+      </c>
+      <c r="L52" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>4919</t>
         </is>
       </c>
     </row>
@@ -2407,9 +2663,15 @@
       <c r="J53" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>3673</t>
+      <c r="K53" t="n">
+        <v>3673</v>
+      </c>
+      <c r="L53" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>3799</t>
         </is>
       </c>
     </row>
@@ -2450,9 +2712,15 @@
       <c r="J54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>2665</t>
+      <c r="K54" t="n">
+        <v>2665</v>
+      </c>
+      <c r="L54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>2696</t>
         </is>
       </c>
     </row>
@@ -2493,9 +2761,15 @@
       <c r="J55" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>3415</t>
+      <c r="K55" t="n">
+        <v>3415</v>
+      </c>
+      <c r="L55" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>3614</t>
         </is>
       </c>
     </row>
@@ -2536,9 +2810,15 @@
       <c r="J56" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>4951</t>
+      <c r="K56" t="n">
+        <v>4951</v>
+      </c>
+      <c r="L56" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>5132</t>
         </is>
       </c>
     </row>
@@ -2579,9 +2859,15 @@
       <c r="J57" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>4140</t>
+      <c r="K57" t="n">
+        <v>4140</v>
+      </c>
+      <c r="L57" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>4201</t>
         </is>
       </c>
     </row>
@@ -2622,9 +2908,15 @@
       <c r="J58" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>3811</t>
+      <c r="K58" t="n">
+        <v>3811</v>
+      </c>
+      <c r="L58" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>4022</t>
         </is>
       </c>
     </row>
@@ -2665,9 +2957,15 @@
       <c r="J59" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>3976</t>
+      <c r="K59" t="n">
+        <v>3976</v>
+      </c>
+      <c r="L59" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>4057</t>
         </is>
       </c>
     </row>
@@ -2708,9 +3006,15 @@
       <c r="J60" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>4180</t>
+      <c r="K60" t="n">
+        <v>4180</v>
+      </c>
+      <c r="L60" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>4298</t>
         </is>
       </c>
     </row>
@@ -2738,6 +3042,8 @@
       <c r="I61" t="inlineStr"/>
       <c r="J61" s="3" t="inlineStr"/>
       <c r="K61" t="inlineStr"/>
+      <c r="L61" s="3" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -2776,9 +3082,15 @@
       <c r="J62" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>3992</t>
+      <c r="K62" t="n">
+        <v>3992</v>
+      </c>
+      <c r="L62" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>4013</t>
         </is>
       </c>
     </row>
@@ -2819,9 +3131,15 @@
       <c r="J63" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>3995</t>
+      <c r="K63" t="n">
+        <v>3995</v>
+      </c>
+      <c r="L63" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>4025</t>
         </is>
       </c>
     </row>
@@ -2862,9 +3180,15 @@
       <c r="J64" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>4012</t>
+      <c r="K64" t="n">
+        <v>4012</v>
+      </c>
+      <c r="L64" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>4120</t>
         </is>
       </c>
     </row>
@@ -2905,9 +3229,15 @@
       <c r="J65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>2797</t>
+      <c r="K65" t="n">
+        <v>2797</v>
+      </c>
+      <c r="L65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>2792</t>
         </is>
       </c>
     </row>
@@ -2948,7 +3278,13 @@
       <c r="J66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K66" t="inlineStr">
+      <c r="K66" t="n">
+        <v>0</v>
+      </c>
+      <c r="L66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2991,7 +3327,13 @@
       <c r="J67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K67" t="inlineStr">
+      <c r="K67" t="n">
+        <v>0</v>
+      </c>
+      <c r="L67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3034,7 +3376,13 @@
       <c r="J68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K68" t="inlineStr">
+      <c r="K68" t="n">
+        <v>0</v>
+      </c>
+      <c r="L68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3064,6 +3412,8 @@
       <c r="I69" t="inlineStr"/>
       <c r="J69" s="3" t="inlineStr"/>
       <c r="K69" t="inlineStr"/>
+      <c r="L69" s="3" t="inlineStr"/>
+      <c r="M69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -3102,7 +3452,13 @@
       <c r="J70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K70" t="inlineStr">
+      <c r="K70" t="n">
+        <v>0</v>
+      </c>
+      <c r="L70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3145,7 +3501,13 @@
       <c r="J71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K71" t="inlineStr">
+      <c r="K71" t="n">
+        <v>0</v>
+      </c>
+      <c r="L71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3188,7 +3550,13 @@
       <c r="J72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K72" t="inlineStr">
+      <c r="K72" t="n">
+        <v>0</v>
+      </c>
+      <c r="L72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3231,9 +3599,15 @@
       <c r="J73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K73" t="inlineStr">
-        <is>
-          <t>2732</t>
+      <c r="K73" t="n">
+        <v>2732</v>
+      </c>
+      <c r="L73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>2802</t>
         </is>
       </c>
     </row>
@@ -3274,9 +3648,15 @@
       <c r="J74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K74" t="inlineStr">
-        <is>
-          <t>2548</t>
+      <c r="K74" t="n">
+        <v>2548</v>
+      </c>
+      <c r="L74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>2541</t>
         </is>
       </c>
     </row>
@@ -3317,7 +3697,13 @@
       <c r="J75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K75" t="inlineStr">
+      <c r="K75" t="n">
+        <v>0</v>
+      </c>
+      <c r="L75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3360,9 +3746,15 @@
       <c r="J76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K76" t="inlineStr">
-        <is>
-          <t>3267</t>
+      <c r="K76" t="n">
+        <v>3267</v>
+      </c>
+      <c r="L76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>3326</t>
         </is>
       </c>
     </row>
@@ -3403,9 +3795,15 @@
       <c r="J77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K77" t="inlineStr">
-        <is>
-          <t>2841</t>
+      <c r="K77" t="n">
+        <v>2841</v>
+      </c>
+      <c r="L77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>2896</t>
         </is>
       </c>
     </row>
@@ -3446,7 +3844,13 @@
       <c r="J78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K78" t="inlineStr">
+      <c r="K78" t="n">
+        <v>0</v>
+      </c>
+      <c r="L78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3489,9 +3893,15 @@
       <c r="J79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K79" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K79" t="n">
+        <v>0</v>
+      </c>
+      <c r="L79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>1322</t>
         </is>
       </c>
     </row>
@@ -3532,7 +3942,13 @@
       <c r="J80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K80" t="inlineStr">
+      <c r="K80" t="n">
+        <v>0</v>
+      </c>
+      <c r="L80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3575,7 +3991,13 @@
       <c r="J81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K81" t="inlineStr">
+      <c r="K81" t="n">
+        <v>0</v>
+      </c>
+      <c r="L81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3618,7 +4040,13 @@
       <c r="J82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K82" t="inlineStr">
+      <c r="K82" t="n">
+        <v>0</v>
+      </c>
+      <c r="L82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3661,9 +4089,15 @@
       <c r="J83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>2580</t>
+      <c r="K83" t="n">
+        <v>2580</v>
+      </c>
+      <c r="L83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>2579</t>
         </is>
       </c>
     </row>
@@ -3704,7 +4138,13 @@
       <c r="J84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K84" t="inlineStr">
+      <c r="K84" t="n">
+        <v>0</v>
+      </c>
+      <c r="L84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3747,7 +4187,13 @@
       <c r="J85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K85" t="inlineStr">
+      <c r="K85" t="n">
+        <v>0</v>
+      </c>
+      <c r="L85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3790,7 +4236,13 @@
       <c r="J86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K86" t="inlineStr">
+      <c r="K86" t="n">
+        <v>0</v>
+      </c>
+      <c r="L86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3833,7 +4285,13 @@
       <c r="J87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K87" t="inlineStr">
+      <c r="K87" t="n">
+        <v>0</v>
+      </c>
+      <c r="L87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3876,7 +4334,13 @@
       <c r="J88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K88" t="inlineStr">
+      <c r="K88" t="n">
+        <v>0</v>
+      </c>
+      <c r="L88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3919,7 +4383,13 @@
       <c r="J89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K89" t="inlineStr">
+      <c r="K89" t="n">
+        <v>0</v>
+      </c>
+      <c r="L89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3962,7 +4432,13 @@
       <c r="J90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K90" t="inlineStr">
+      <c r="K90" t="n">
+        <v>0</v>
+      </c>
+      <c r="L90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4005,9 +4481,15 @@
       <c r="J91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="K91" t="n">
+        <v>0</v>
+      </c>
+      <c r="L91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>999</t>
         </is>
       </c>
     </row>
@@ -4048,7 +4530,13 @@
       <c r="J92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K92" t="inlineStr">
+      <c r="K92" t="n">
+        <v>0</v>
+      </c>
+      <c r="L92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4091,7 +4579,13 @@
       <c r="J93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K93" t="inlineStr">
+      <c r="K93" t="n">
+        <v>0</v>
+      </c>
+      <c r="L93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4134,7 +4628,13 @@
       <c r="J94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K94" t="inlineStr">
+      <c r="K94" t="n">
+        <v>0</v>
+      </c>
+      <c r="L94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4177,7 +4677,13 @@
       <c r="J95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K95" t="inlineStr">
+      <c r="K95" t="n">
+        <v>0</v>
+      </c>
+      <c r="L95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4220,9 +4726,15 @@
       <c r="J96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K96" t="inlineStr">
-        <is>
-          <t>3649</t>
+      <c r="K96" t="n">
+        <v>3649</v>
+      </c>
+      <c r="L96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>3632</t>
         </is>
       </c>
     </row>
@@ -4263,7 +4775,13 @@
       <c r="J97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K97" t="inlineStr">
+      <c r="K97" t="n">
+        <v>0</v>
+      </c>
+      <c r="L97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4306,7 +4824,13 @@
       <c r="J98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K98" t="inlineStr">
+      <c r="K98" t="n">
+        <v>0</v>
+      </c>
+      <c r="L98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4349,7 +4873,13 @@
       <c r="J99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K99" t="inlineStr">
+      <c r="K99" t="n">
+        <v>0</v>
+      </c>
+      <c r="L99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4392,7 +4922,13 @@
       <c r="J100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K100" t="inlineStr">
+      <c r="K100" t="n">
+        <v>0</v>
+      </c>
+      <c r="L100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4435,7 +4971,13 @@
       <c r="J101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K101" t="inlineStr">
+      <c r="K101" t="n">
+        <v>0</v>
+      </c>
+      <c r="L101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4478,7 +5020,13 @@
       <c r="J102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K102" t="inlineStr">
+      <c r="K102" t="n">
+        <v>0</v>
+      </c>
+      <c r="L102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4521,7 +5069,13 @@
       <c r="J103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K103" t="inlineStr">
+      <c r="K103" t="n">
+        <v>0</v>
+      </c>
+      <c r="L103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4564,7 +5118,13 @@
       <c r="J104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K104" t="inlineStr">
+      <c r="K104" t="n">
+        <v>0</v>
+      </c>
+      <c r="L104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4607,7 +5167,13 @@
       <c r="J105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K105" t="inlineStr">
+      <c r="K105" t="n">
+        <v>0</v>
+      </c>
+      <c r="L105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4637,6 +5203,8 @@
       <c r="I106" t="inlineStr"/>
       <c r="J106" s="3" t="inlineStr"/>
       <c r="K106" t="inlineStr"/>
+      <c r="L106" s="3" t="inlineStr"/>
+      <c r="M106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -4662,6 +5230,8 @@
       <c r="I107" t="inlineStr"/>
       <c r="J107" s="3" t="inlineStr"/>
       <c r="K107" t="inlineStr"/>
+      <c r="L107" s="3" t="inlineStr"/>
+      <c r="M107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -4687,6 +5257,8 @@
       <c r="I108" t="inlineStr"/>
       <c r="J108" s="3" t="inlineStr"/>
       <c r="K108" t="inlineStr"/>
+      <c r="L108" s="3" t="inlineStr"/>
+      <c r="M108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -4712,6 +5284,8 @@
       <c r="I109" t="inlineStr"/>
       <c r="J109" s="3" t="inlineStr"/>
       <c r="K109" t="inlineStr"/>
+      <c r="L109" s="3" t="inlineStr"/>
+      <c r="M109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -4737,6 +5311,8 @@
       <c r="I110" t="inlineStr"/>
       <c r="J110" s="3" t="inlineStr"/>
       <c r="K110" t="inlineStr"/>
+      <c r="L110" s="3" t="inlineStr"/>
+      <c r="M110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -4762,6 +5338,8 @@
       <c r="I111" t="inlineStr"/>
       <c r="J111" s="3" t="inlineStr"/>
       <c r="K111" t="inlineStr"/>
+      <c r="L111" s="3" t="inlineStr"/>
+      <c r="M111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -4787,6 +5365,8 @@
       <c r="I112" t="inlineStr"/>
       <c r="J112" s="3" t="inlineStr"/>
       <c r="K112" t="inlineStr"/>
+      <c r="L112" s="3" t="inlineStr"/>
+      <c r="M112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -4812,6 +5392,8 @@
       <c r="I113" t="inlineStr"/>
       <c r="J113" s="3" t="inlineStr"/>
       <c r="K113" t="inlineStr"/>
+      <c r="L113" s="3" t="inlineStr"/>
+      <c r="M113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -4837,6 +5419,8 @@
       <c r="I114" t="inlineStr"/>
       <c r="J114" s="3" t="inlineStr"/>
       <c r="K114" t="inlineStr"/>
+      <c r="L114" s="3" t="inlineStr"/>
+      <c r="M114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -4869,9 +5453,15 @@
       <c r="J115" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="K115" t="inlineStr">
-        <is>
-          <t>5535</t>
+      <c r="K115" t="n">
+        <v>5535</v>
+      </c>
+      <c r="L115" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="M115" t="inlineStr">
+        <is>
+          <t>5699</t>
         </is>
       </c>
     </row>
@@ -4906,9 +5496,15 @@
       <c r="J116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K116" t="inlineStr">
-        <is>
-          <t>998</t>
+      <c r="K116" t="n">
+        <v>998</v>
+      </c>
+      <c r="L116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M116" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4943,11 +5539,11 @@
       <c r="J117" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="K117" t="inlineStr">
-        <is>
-          <t>5414</t>
-        </is>
-      </c>
+      <c r="K117" t="n">
+        <v>5414</v>
+      </c>
+      <c r="L117" s="3" t="inlineStr"/>
+      <c r="M117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -4980,9 +5576,15 @@
       <c r="J118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K118" t="inlineStr">
-        <is>
-          <t>4366</t>
+      <c r="K118" t="n">
+        <v>4366</v>
+      </c>
+      <c r="L118" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="M118" t="inlineStr">
+        <is>
+          <t>4482</t>
         </is>
       </c>
     </row>
@@ -5017,9 +5619,15 @@
       <c r="J119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K119" t="inlineStr">
-        <is>
-          <t>1541</t>
+      <c r="K119" t="n">
+        <v>1541</v>
+      </c>
+      <c r="L119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M119" t="inlineStr">
+        <is>
+          <t>1557</t>
         </is>
       </c>
     </row>
@@ -5054,9 +5662,15 @@
       <c r="J120" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="K120" t="inlineStr">
-        <is>
-          <t>2031</t>
+      <c r="K120" t="n">
+        <v>2031</v>
+      </c>
+      <c r="L120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M120" t="inlineStr">
+        <is>
+          <t>2327</t>
         </is>
       </c>
     </row>
@@ -5091,9 +5705,15 @@
       <c r="J121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K121" t="inlineStr">
-        <is>
-          <t>1727</t>
+      <c r="K121" t="n">
+        <v>1727</v>
+      </c>
+      <c r="L121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M121" t="inlineStr">
+        <is>
+          <t>1720</t>
         </is>
       </c>
     </row>
@@ -5128,9 +5748,15 @@
       <c r="J122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="K122" t="inlineStr">
-        <is>
-          <t>1938</t>
+      <c r="K122" t="n">
+        <v>1938</v>
+      </c>
+      <c r="L122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>1988</t>
         </is>
       </c>
     </row>
@@ -5161,17 +5787,21 @@
       <c r="J123" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="K123" t="inlineStr">
+      <c r="K123" t="n">
+        <v>2713</v>
+      </c>
+      <c r="L123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M123" t="inlineStr">
         <is>
           <t>2713</t>
         </is>
       </c>
     </row>
     <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>50975641</t>
-        </is>
+      <c r="A124" t="n">
+        <v>50975641</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
@@ -5192,17 +5822,21 @@
       <c r="J124" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="K124" t="inlineStr">
-        <is>
-          <t>3992</t>
+      <c r="K124" t="n">
+        <v>3992</v>
+      </c>
+      <c r="L124" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="M124" t="inlineStr">
+        <is>
+          <t>4117</t>
         </is>
       </c>
     </row>
     <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>57467416</t>
-        </is>
+      <c r="A125" t="n">
+        <v>57467416</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
@@ -5223,9 +5857,15 @@
       <c r="J125" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="K125" t="inlineStr">
-        <is>
-          <t>1534</t>
+      <c r="K125" t="n">
+        <v>1534</v>
+      </c>
+      <c r="L125" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="M125" t="inlineStr">
+        <is>
+          <t>1805</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-17 11:30:58
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M125"/>
+  <dimension ref="A1:O125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,16 @@
           <t>05-15_0</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>05-16_A</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>05-16_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -500,7 +510,13 @@
       <c r="L2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="M2" t="n">
+        <v>2586</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="inlineStr">
         <is>
           <t>2586</t>
         </is>
@@ -549,7 +565,13 @@
       <c r="L3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -598,7 +620,13 @@
       <c r="L4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -647,9 +675,15 @@
       <c r="L5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>2552</t>
+      <c r="M5" t="n">
+        <v>2552</v>
+      </c>
+      <c r="N5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>2563</t>
         </is>
       </c>
     </row>
@@ -696,9 +730,15 @@
       <c r="L6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>2570</t>
+      <c r="M6" t="n">
+        <v>2570</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>2567</t>
         </is>
       </c>
     </row>
@@ -728,6 +768,8 @@
       <c r="K7" t="inlineStr"/>
       <c r="L7" s="3" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
+      <c r="N7" s="3" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -755,6 +797,8 @@
       <c r="K8" t="inlineStr"/>
       <c r="L8" s="3" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
+      <c r="N8" s="3" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -782,6 +826,8 @@
       <c r="K9" t="inlineStr"/>
       <c r="L9" s="3" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
+      <c r="N9" s="3" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -809,6 +855,8 @@
       <c r="K10" t="inlineStr"/>
       <c r="L10" s="3" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
+      <c r="N10" s="3" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -836,6 +884,8 @@
       <c r="K11" t="inlineStr"/>
       <c r="L11" s="3" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
+      <c r="N11" s="3" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -863,6 +913,8 @@
       <c r="K12" t="inlineStr"/>
       <c r="L12" s="3" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
+      <c r="N12" s="3" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -890,6 +942,8 @@
       <c r="K13" t="inlineStr"/>
       <c r="L13" s="3" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
+      <c r="N13" s="3" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -917,6 +971,8 @@
       <c r="K14" t="inlineStr"/>
       <c r="L14" s="3" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
+      <c r="N14" s="3" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -944,6 +1000,8 @@
       <c r="K15" t="inlineStr"/>
       <c r="L15" s="3" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
+      <c r="N15" s="3" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -971,6 +1029,8 @@
       <c r="K16" t="inlineStr"/>
       <c r="L16" s="3" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
+      <c r="N16" s="3" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -998,6 +1058,8 @@
       <c r="K17" t="inlineStr"/>
       <c r="L17" s="3" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
+      <c r="N17" s="3" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1042,9 +1104,15 @@
       <c r="L18" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>3983</t>
+      <c r="M18" t="n">
+        <v>3983</v>
+      </c>
+      <c r="N18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>3966</t>
         </is>
       </c>
     </row>
@@ -1091,7 +1159,13 @@
       <c r="L19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M19" t="inlineStr">
+      <c r="M19" t="n">
+        <v>2701</v>
+      </c>
+      <c r="N19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="inlineStr">
         <is>
           <t>2701</t>
         </is>
@@ -1140,9 +1214,15 @@
       <c r="L20" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>4217</t>
+      <c r="M20" t="n">
+        <v>4217</v>
+      </c>
+      <c r="N20" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>4313</t>
         </is>
       </c>
     </row>
@@ -1189,9 +1269,15 @@
       <c r="L21" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>4591</t>
+      <c r="M21" t="n">
+        <v>4591</v>
+      </c>
+      <c r="N21" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>4841</t>
         </is>
       </c>
     </row>
@@ -1238,9 +1324,15 @@
       <c r="L22" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M22" t="inlineStr">
-        <is>
-          <t>4759</t>
+      <c r="M22" t="n">
+        <v>4759</v>
+      </c>
+      <c r="N22" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>4945</t>
         </is>
       </c>
     </row>
@@ -1287,9 +1379,15 @@
       <c r="L23" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M23" t="inlineStr">
-        <is>
-          <t>5387</t>
+      <c r="M23" t="n">
+        <v>5387</v>
+      </c>
+      <c r="N23" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>5541</t>
         </is>
       </c>
     </row>
@@ -1336,9 +1434,15 @@
       <c r="L24" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="M24" t="inlineStr">
-        <is>
-          <t>4737</t>
+      <c r="M24" t="n">
+        <v>4737</v>
+      </c>
+      <c r="N24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>4949</t>
         </is>
       </c>
     </row>
@@ -1385,9 +1489,15 @@
       <c r="L25" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M25" t="inlineStr">
-        <is>
-          <t>5075</t>
+      <c r="M25" t="n">
+        <v>5075</v>
+      </c>
+      <c r="N25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>5138</t>
         </is>
       </c>
     </row>
@@ -1434,7 +1544,13 @@
       <c r="L26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M26" t="inlineStr">
+      <c r="M26" t="n">
+        <v>2578</v>
+      </c>
+      <c r="N26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O26" t="inlineStr">
         <is>
           <t>2578</t>
         </is>
@@ -1483,7 +1599,13 @@
       <c r="L27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M27" t="inlineStr">
+      <c r="M27" t="n">
+        <v>2516</v>
+      </c>
+      <c r="N27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O27" t="inlineStr">
         <is>
           <t>2516</t>
         </is>
@@ -1515,6 +1637,8 @@
       <c r="K28" t="inlineStr"/>
       <c r="L28" s="3" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
+      <c r="N28" s="3" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1559,7 +1683,13 @@
       <c r="L29" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="M29" t="inlineStr">
+      <c r="M29" t="n">
+        <v>3420</v>
+      </c>
+      <c r="N29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O29" t="inlineStr">
         <is>
           <t>3420</t>
         </is>
@@ -1608,7 +1738,13 @@
       <c r="L30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M30" t="inlineStr">
+      <c r="M30" t="n">
+        <v>2500</v>
+      </c>
+      <c r="N30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O30" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1657,9 +1793,15 @@
       <c r="L31" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="M31" t="inlineStr">
-        <is>
-          <t>4793</t>
+      <c r="M31" t="n">
+        <v>4793</v>
+      </c>
+      <c r="N31" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>4902</t>
         </is>
       </c>
     </row>
@@ -1706,9 +1848,15 @@
       <c r="L32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M32" t="inlineStr">
-        <is>
-          <t>3640</t>
+      <c r="M32" t="n">
+        <v>3640</v>
+      </c>
+      <c r="N32" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>3947</t>
         </is>
       </c>
     </row>
@@ -1738,6 +1886,8 @@
       <c r="K33" t="inlineStr"/>
       <c r="L33" s="3" t="inlineStr"/>
       <c r="M33" t="inlineStr"/>
+      <c r="N33" s="3" t="inlineStr"/>
+      <c r="O33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1782,7 +1932,13 @@
       <c r="L34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M34" t="inlineStr">
+      <c r="M34" t="n">
+        <v>0</v>
+      </c>
+      <c r="N34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1831,7 +1987,13 @@
       <c r="L35" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M35" t="inlineStr">
+      <c r="M35" t="n">
+        <v>4316</v>
+      </c>
+      <c r="N35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O35" t="inlineStr">
         <is>
           <t>4316</t>
         </is>
@@ -1880,9 +2042,15 @@
       <c r="L36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M36" t="inlineStr">
-        <is>
-          <t>3716</t>
+      <c r="M36" t="n">
+        <v>3716</v>
+      </c>
+      <c r="N36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>3711</t>
         </is>
       </c>
     </row>
@@ -1929,9 +2097,15 @@
       <c r="L37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M37" t="inlineStr">
-        <is>
-          <t>4581</t>
+      <c r="M37" t="n">
+        <v>4581</v>
+      </c>
+      <c r="N37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>4648</t>
         </is>
       </c>
     </row>
@@ -1978,9 +2152,15 @@
       <c r="L38" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="M38" t="inlineStr">
-        <is>
-          <t>5210</t>
+      <c r="M38" t="n">
+        <v>5210</v>
+      </c>
+      <c r="N38" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>5442</t>
         </is>
       </c>
     </row>
@@ -2027,9 +2207,15 @@
       <c r="L39" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>4457</t>
+      <c r="M39" t="n">
+        <v>4457</v>
+      </c>
+      <c r="N39" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>4566</t>
         </is>
       </c>
     </row>
@@ -2076,7 +2262,13 @@
       <c r="L40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M40" t="inlineStr">
+      <c r="M40" t="n">
+        <v>0</v>
+      </c>
+      <c r="N40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2125,9 +2317,15 @@
       <c r="L41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M41" t="inlineStr">
-        <is>
-          <t>4275</t>
+      <c r="M41" t="n">
+        <v>4275</v>
+      </c>
+      <c r="N41" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>4321</t>
         </is>
       </c>
     </row>
@@ -2174,9 +2372,15 @@
       <c r="L42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>3232</t>
+      <c r="M42" t="n">
+        <v>3232</v>
+      </c>
+      <c r="N42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>3242</t>
         </is>
       </c>
     </row>
@@ -2206,6 +2410,8 @@
       <c r="K43" t="inlineStr"/>
       <c r="L43" s="3" t="inlineStr"/>
       <c r="M43" t="inlineStr"/>
+      <c r="N43" s="3" t="inlineStr"/>
+      <c r="O43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2233,6 +2439,8 @@
       <c r="K44" t="inlineStr"/>
       <c r="L44" s="3" t="inlineStr"/>
       <c r="M44" t="inlineStr"/>
+      <c r="N44" s="3" t="inlineStr"/>
+      <c r="O44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -2277,9 +2485,15 @@
       <c r="L45" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="M45" t="inlineStr">
-        <is>
-          <t>3986</t>
+      <c r="M45" t="n">
+        <v>3986</v>
+      </c>
+      <c r="N45" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>4018</t>
         </is>
       </c>
     </row>
@@ -2326,9 +2540,15 @@
       <c r="L46" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="M46" t="inlineStr">
-        <is>
-          <t>3789</t>
+      <c r="M46" t="n">
+        <v>3789</v>
+      </c>
+      <c r="N46" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>4010</t>
         </is>
       </c>
     </row>
@@ -2375,9 +2595,15 @@
       <c r="L47" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M47" t="inlineStr">
-        <is>
-          <t>5209</t>
+      <c r="M47" t="n">
+        <v>5209</v>
+      </c>
+      <c r="N47" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>5435</t>
         </is>
       </c>
     </row>
@@ -2424,9 +2650,15 @@
       <c r="L48" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M48" t="inlineStr">
-        <is>
-          <t>5064</t>
+      <c r="M48" t="n">
+        <v>5064</v>
+      </c>
+      <c r="N48" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>5032</t>
         </is>
       </c>
     </row>
@@ -2473,9 +2705,15 @@
       <c r="L49" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="M49" t="inlineStr">
-        <is>
-          <t>4658</t>
+      <c r="M49" t="n">
+        <v>4658</v>
+      </c>
+      <c r="N49" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>4672</t>
         </is>
       </c>
     </row>
@@ -2522,9 +2760,15 @@
       <c r="L50" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="M50" t="inlineStr">
-        <is>
-          <t>4779</t>
+      <c r="M50" t="n">
+        <v>4779</v>
+      </c>
+      <c r="N50" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>4951</t>
         </is>
       </c>
     </row>
@@ -2571,9 +2815,15 @@
       <c r="L51" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="M51" t="inlineStr">
-        <is>
-          <t>3341</t>
+      <c r="M51" t="n">
+        <v>3341</v>
+      </c>
+      <c r="N51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>3378</t>
         </is>
       </c>
     </row>
@@ -2620,9 +2870,15 @@
       <c r="L52" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M52" t="inlineStr">
-        <is>
-          <t>4919</t>
+      <c r="M52" t="n">
+        <v>4919</v>
+      </c>
+      <c r="N52" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>5139</t>
         </is>
       </c>
     </row>
@@ -2669,9 +2925,15 @@
       <c r="L53" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="M53" t="inlineStr">
-        <is>
-          <t>3799</t>
+      <c r="M53" t="n">
+        <v>3799</v>
+      </c>
+      <c r="N53" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>3949</t>
         </is>
       </c>
     </row>
@@ -2718,9 +2980,15 @@
       <c r="L54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M54" t="inlineStr">
-        <is>
-          <t>2696</t>
+      <c r="M54" t="n">
+        <v>2696</v>
+      </c>
+      <c r="N54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>2802</t>
         </is>
       </c>
     </row>
@@ -2767,9 +3035,15 @@
       <c r="L55" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="M55" t="inlineStr">
-        <is>
-          <t>3614</t>
+      <c r="M55" t="n">
+        <v>3614</v>
+      </c>
+      <c r="N55" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>4022</t>
         </is>
       </c>
     </row>
@@ -2816,9 +3090,15 @@
       <c r="L56" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="M56" t="inlineStr">
-        <is>
-          <t>5132</t>
+      <c r="M56" t="n">
+        <v>5132</v>
+      </c>
+      <c r="N56" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>5332</t>
         </is>
       </c>
     </row>
@@ -2865,9 +3145,15 @@
       <c r="L57" s="4" t="n">
         <v>17</v>
       </c>
-      <c r="M57" t="inlineStr">
-        <is>
-          <t>4201</t>
+      <c r="M57" t="n">
+        <v>4201</v>
+      </c>
+      <c r="N57" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>4266</t>
         </is>
       </c>
     </row>
@@ -2914,9 +3200,15 @@
       <c r="L58" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="M58" t="inlineStr">
-        <is>
-          <t>4022</t>
+      <c r="M58" t="n">
+        <v>4022</v>
+      </c>
+      <c r="N58" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>4175</t>
         </is>
       </c>
     </row>
@@ -2963,9 +3255,15 @@
       <c r="L59" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M59" t="inlineStr">
-        <is>
-          <t>4057</t>
+      <c r="M59" t="n">
+        <v>4057</v>
+      </c>
+      <c r="N59" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>4080</t>
         </is>
       </c>
     </row>
@@ -3012,9 +3310,15 @@
       <c r="L60" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="M60" t="inlineStr">
-        <is>
-          <t>4298</t>
+      <c r="M60" t="n">
+        <v>4298</v>
+      </c>
+      <c r="N60" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>4299</t>
         </is>
       </c>
     </row>
@@ -3044,6 +3348,8 @@
       <c r="K61" t="inlineStr"/>
       <c r="L61" s="3" t="inlineStr"/>
       <c r="M61" t="inlineStr"/>
+      <c r="N61" s="3" t="inlineStr"/>
+      <c r="O61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -3088,9 +3394,15 @@
       <c r="L62" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="M62" t="inlineStr">
-        <is>
-          <t>4013</t>
+      <c r="M62" t="n">
+        <v>4013</v>
+      </c>
+      <c r="N62" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -3137,9 +3449,15 @@
       <c r="L63" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M63" t="inlineStr">
-        <is>
-          <t>4025</t>
+      <c r="M63" t="n">
+        <v>4025</v>
+      </c>
+      <c r="N63" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>4081</t>
         </is>
       </c>
     </row>
@@ -3186,9 +3504,15 @@
       <c r="L64" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M64" t="inlineStr">
-        <is>
-          <t>4120</t>
+      <c r="M64" t="n">
+        <v>4120</v>
+      </c>
+      <c r="N64" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>4252</t>
         </is>
       </c>
     </row>
@@ -3235,9 +3559,15 @@
       <c r="L65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M65" t="inlineStr">
-        <is>
-          <t>2792</t>
+      <c r="M65" t="n">
+        <v>2792</v>
+      </c>
+      <c r="N65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>2787</t>
         </is>
       </c>
     </row>
@@ -3284,7 +3614,13 @@
       <c r="L66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M66" t="inlineStr">
+      <c r="M66" t="n">
+        <v>0</v>
+      </c>
+      <c r="N66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3333,7 +3669,13 @@
       <c r="L67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M67" t="inlineStr">
+      <c r="M67" t="n">
+        <v>0</v>
+      </c>
+      <c r="N67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3382,7 +3724,13 @@
       <c r="L68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M68" t="inlineStr">
+      <c r="M68" t="n">
+        <v>0</v>
+      </c>
+      <c r="N68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3414,6 +3762,8 @@
       <c r="K69" t="inlineStr"/>
       <c r="L69" s="3" t="inlineStr"/>
       <c r="M69" t="inlineStr"/>
+      <c r="N69" s="3" t="inlineStr"/>
+      <c r="O69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -3458,7 +3808,13 @@
       <c r="L70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M70" t="inlineStr">
+      <c r="M70" t="n">
+        <v>0</v>
+      </c>
+      <c r="N70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3507,7 +3863,13 @@
       <c r="L71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M71" t="inlineStr">
+      <c r="M71" t="n">
+        <v>0</v>
+      </c>
+      <c r="N71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3556,7 +3918,13 @@
       <c r="L72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M72" t="inlineStr">
+      <c r="M72" t="n">
+        <v>0</v>
+      </c>
+      <c r="N72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3605,9 +3973,15 @@
       <c r="L73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M73" t="inlineStr">
-        <is>
-          <t>2802</t>
+      <c r="M73" t="n">
+        <v>2802</v>
+      </c>
+      <c r="N73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>2794</t>
         </is>
       </c>
     </row>
@@ -3654,9 +4028,15 @@
       <c r="L74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M74" t="inlineStr">
-        <is>
-          <t>2541</t>
+      <c r="M74" t="n">
+        <v>2541</v>
+      </c>
+      <c r="N74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>2568</t>
         </is>
       </c>
     </row>
@@ -3703,7 +4083,13 @@
       <c r="L75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M75" t="inlineStr">
+      <c r="M75" t="n">
+        <v>0</v>
+      </c>
+      <c r="N75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3752,9 +4138,15 @@
       <c r="L76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M76" t="inlineStr">
-        <is>
-          <t>3326</t>
+      <c r="M76" t="n">
+        <v>3326</v>
+      </c>
+      <c r="N76" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>3394</t>
         </is>
       </c>
     </row>
@@ -3801,9 +4193,15 @@
       <c r="L77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M77" t="inlineStr">
-        <is>
-          <t>2896</t>
+      <c r="M77" t="n">
+        <v>2896</v>
+      </c>
+      <c r="N77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>2924</t>
         </is>
       </c>
     </row>
@@ -3850,7 +4248,13 @@
       <c r="L78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M78" t="inlineStr">
+      <c r="M78" t="n">
+        <v>0</v>
+      </c>
+      <c r="N78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3899,9 +4303,15 @@
       <c r="L79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M79" t="inlineStr">
-        <is>
-          <t>1322</t>
+      <c r="M79" t="n">
+        <v>1322</v>
+      </c>
+      <c r="N79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>1321</t>
         </is>
       </c>
     </row>
@@ -3948,7 +4358,13 @@
       <c r="L80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M80" t="inlineStr">
+      <c r="M80" t="n">
+        <v>0</v>
+      </c>
+      <c r="N80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3997,7 +4413,13 @@
       <c r="L81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M81" t="inlineStr">
+      <c r="M81" t="n">
+        <v>0</v>
+      </c>
+      <c r="N81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4046,7 +4468,13 @@
       <c r="L82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M82" t="inlineStr">
+      <c r="M82" t="n">
+        <v>0</v>
+      </c>
+      <c r="N82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4095,9 +4523,15 @@
       <c r="L83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M83" t="inlineStr">
-        <is>
-          <t>2579</t>
+      <c r="M83" t="n">
+        <v>2579</v>
+      </c>
+      <c r="N83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>2575</t>
         </is>
       </c>
     </row>
@@ -4144,9 +4578,15 @@
       <c r="L84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M84" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M84" t="n">
+        <v>0</v>
+      </c>
+      <c r="N84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>1398</t>
         </is>
       </c>
     </row>
@@ -4193,7 +4633,13 @@
       <c r="L85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M85" t="inlineStr">
+      <c r="M85" t="n">
+        <v>0</v>
+      </c>
+      <c r="N85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4242,7 +4688,13 @@
       <c r="L86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M86" t="inlineStr">
+      <c r="M86" t="n">
+        <v>0</v>
+      </c>
+      <c r="N86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4291,7 +4743,13 @@
       <c r="L87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M87" t="inlineStr">
+      <c r="M87" t="n">
+        <v>0</v>
+      </c>
+      <c r="N87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4340,7 +4798,13 @@
       <c r="L88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M88" t="inlineStr">
+      <c r="M88" t="n">
+        <v>0</v>
+      </c>
+      <c r="N88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4389,7 +4853,13 @@
       <c r="L89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M89" t="inlineStr">
+      <c r="M89" t="n">
+        <v>0</v>
+      </c>
+      <c r="N89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4438,9 +4908,15 @@
       <c r="L90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M90" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="M90" t="n">
+        <v>0</v>
+      </c>
+      <c r="N90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>999</t>
         </is>
       </c>
     </row>
@@ -4487,9 +4963,15 @@
       <c r="L91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M91" t="inlineStr">
-        <is>
-          <t>999</t>
+      <c r="M91" t="n">
+        <v>999</v>
+      </c>
+      <c r="N91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4536,7 +5018,13 @@
       <c r="L92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M92" t="inlineStr">
+      <c r="M92" t="n">
+        <v>0</v>
+      </c>
+      <c r="N92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4585,7 +5073,13 @@
       <c r="L93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M93" t="inlineStr">
+      <c r="M93" t="n">
+        <v>0</v>
+      </c>
+      <c r="N93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4634,7 +5128,13 @@
       <c r="L94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M94" t="inlineStr">
+      <c r="M94" t="n">
+        <v>0</v>
+      </c>
+      <c r="N94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4683,7 +5183,13 @@
       <c r="L95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M95" t="inlineStr">
+      <c r="M95" t="n">
+        <v>0</v>
+      </c>
+      <c r="N95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4732,9 +5238,15 @@
       <c r="L96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M96" t="inlineStr">
-        <is>
-          <t>3632</t>
+      <c r="M96" t="n">
+        <v>3632</v>
+      </c>
+      <c r="N96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O96" t="inlineStr">
+        <is>
+          <t>3615</t>
         </is>
       </c>
     </row>
@@ -4781,7 +5293,13 @@
       <c r="L97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M97" t="inlineStr">
+      <c r="M97" t="n">
+        <v>0</v>
+      </c>
+      <c r="N97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4830,7 +5348,13 @@
       <c r="L98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M98" t="inlineStr">
+      <c r="M98" t="n">
+        <v>0</v>
+      </c>
+      <c r="N98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4879,7 +5403,13 @@
       <c r="L99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M99" t="inlineStr">
+      <c r="M99" t="n">
+        <v>0</v>
+      </c>
+      <c r="N99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4928,7 +5458,13 @@
       <c r="L100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M100" t="inlineStr">
+      <c r="M100" t="n">
+        <v>0</v>
+      </c>
+      <c r="N100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4977,7 +5513,13 @@
       <c r="L101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M101" t="inlineStr">
+      <c r="M101" t="n">
+        <v>0</v>
+      </c>
+      <c r="N101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5026,7 +5568,13 @@
       <c r="L102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M102" t="inlineStr">
+      <c r="M102" t="n">
+        <v>0</v>
+      </c>
+      <c r="N102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5075,7 +5623,13 @@
       <c r="L103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M103" t="inlineStr">
+      <c r="M103" t="n">
+        <v>0</v>
+      </c>
+      <c r="N103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5124,7 +5678,13 @@
       <c r="L104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M104" t="inlineStr">
+      <c r="M104" t="n">
+        <v>0</v>
+      </c>
+      <c r="N104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5173,7 +5733,13 @@
       <c r="L105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M105" t="inlineStr">
+      <c r="M105" t="n">
+        <v>0</v>
+      </c>
+      <c r="N105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5205,6 +5771,8 @@
       <c r="K106" t="inlineStr"/>
       <c r="L106" s="3" t="inlineStr"/>
       <c r="M106" t="inlineStr"/>
+      <c r="N106" s="3" t="inlineStr"/>
+      <c r="O106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -5232,6 +5800,8 @@
       <c r="K107" t="inlineStr"/>
       <c r="L107" s="3" t="inlineStr"/>
       <c r="M107" t="inlineStr"/>
+      <c r="N107" s="3" t="inlineStr"/>
+      <c r="O107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -5259,6 +5829,8 @@
       <c r="K108" t="inlineStr"/>
       <c r="L108" s="3" t="inlineStr"/>
       <c r="M108" t="inlineStr"/>
+      <c r="N108" s="3" t="inlineStr"/>
+      <c r="O108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -5286,6 +5858,8 @@
       <c r="K109" t="inlineStr"/>
       <c r="L109" s="3" t="inlineStr"/>
       <c r="M109" t="inlineStr"/>
+      <c r="N109" s="3" t="inlineStr"/>
+      <c r="O109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -5313,6 +5887,8 @@
       <c r="K110" t="inlineStr"/>
       <c r="L110" s="3" t="inlineStr"/>
       <c r="M110" t="inlineStr"/>
+      <c r="N110" s="3" t="inlineStr"/>
+      <c r="O110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -5340,6 +5916,8 @@
       <c r="K111" t="inlineStr"/>
       <c r="L111" s="3" t="inlineStr"/>
       <c r="M111" t="inlineStr"/>
+      <c r="N111" s="3" t="inlineStr"/>
+      <c r="O111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -5367,6 +5945,8 @@
       <c r="K112" t="inlineStr"/>
       <c r="L112" s="3" t="inlineStr"/>
       <c r="M112" t="inlineStr"/>
+      <c r="N112" s="3" t="inlineStr"/>
+      <c r="O112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -5394,6 +5974,8 @@
       <c r="K113" t="inlineStr"/>
       <c r="L113" s="3" t="inlineStr"/>
       <c r="M113" t="inlineStr"/>
+      <c r="N113" s="3" t="inlineStr"/>
+      <c r="O113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -5421,6 +6003,8 @@
       <c r="K114" t="inlineStr"/>
       <c r="L114" s="3" t="inlineStr"/>
       <c r="M114" t="inlineStr"/>
+      <c r="N114" s="3" t="inlineStr"/>
+      <c r="O114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -5459,11 +6043,11 @@
       <c r="L115" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="M115" t="inlineStr">
-        <is>
-          <t>5699</t>
-        </is>
-      </c>
+      <c r="M115" t="n">
+        <v>5699</v>
+      </c>
+      <c r="N115" s="3" t="inlineStr"/>
+      <c r="O115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -5502,7 +6086,13 @@
       <c r="L116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M116" t="inlineStr">
+      <c r="M116" t="n">
+        <v>0</v>
+      </c>
+      <c r="N116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5544,6 +6134,8 @@
       </c>
       <c r="L117" s="3" t="inlineStr"/>
       <c r="M117" t="inlineStr"/>
+      <c r="N117" s="3" t="inlineStr"/>
+      <c r="O117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -5582,9 +6174,15 @@
       <c r="L118" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="M118" t="inlineStr">
-        <is>
-          <t>4482</t>
+      <c r="M118" t="n">
+        <v>4482</v>
+      </c>
+      <c r="N118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>4474</t>
         </is>
       </c>
     </row>
@@ -5625,9 +6223,15 @@
       <c r="L119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M119" t="inlineStr">
-        <is>
-          <t>1557</t>
+      <c r="M119" t="n">
+        <v>1557</v>
+      </c>
+      <c r="N119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O119" t="inlineStr">
+        <is>
+          <t>1569</t>
         </is>
       </c>
     </row>
@@ -5668,9 +6272,15 @@
       <c r="L120" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M120" t="inlineStr">
-        <is>
-          <t>2327</t>
+      <c r="M120" t="n">
+        <v>2327</v>
+      </c>
+      <c r="N120" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="O120" t="inlineStr">
+        <is>
+          <t>2350</t>
         </is>
       </c>
     </row>
@@ -5711,9 +6321,15 @@
       <c r="L121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M121" t="inlineStr">
-        <is>
-          <t>1720</t>
+      <c r="M121" t="n">
+        <v>1720</v>
+      </c>
+      <c r="N121" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="O121" t="inlineStr">
+        <is>
+          <t>1786</t>
         </is>
       </c>
     </row>
@@ -5754,9 +6370,15 @@
       <c r="L122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M122" t="inlineStr">
-        <is>
-          <t>1988</t>
+      <c r="M122" t="n">
+        <v>1988</v>
+      </c>
+      <c r="N122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>1984</t>
         </is>
       </c>
     </row>
@@ -5793,7 +6415,13 @@
       <c r="L123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="M123" t="inlineStr">
+      <c r="M123" t="n">
+        <v>2713</v>
+      </c>
+      <c r="N123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O123" t="inlineStr">
         <is>
           <t>2713</t>
         </is>
@@ -5828,9 +6456,15 @@
       <c r="L124" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="M124" t="inlineStr">
-        <is>
-          <t>4117</t>
+      <c r="M124" t="n">
+        <v>4117</v>
+      </c>
+      <c r="N124" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="O124" t="inlineStr">
+        <is>
+          <t>4175</t>
         </is>
       </c>
     </row>
@@ -5863,9 +6497,15 @@
       <c r="L125" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="M125" t="inlineStr">
-        <is>
-          <t>1805</t>
+      <c r="M125" t="n">
+        <v>1805</v>
+      </c>
+      <c r="N125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O125" t="inlineStr">
+        <is>
+          <t>1819</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-18 11:30:56
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O125"/>
+  <dimension ref="A1:Q126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,6 +466,16 @@
           <t>05-16_0</t>
         </is>
       </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>05-17_A</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>05-17_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -516,7 +526,13 @@
       <c r="N2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="O2" t="n">
+        <v>2586</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="inlineStr">
         <is>
           <t>2586</t>
         </is>
@@ -571,7 +587,13 @@
       <c r="N3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O3" t="inlineStr">
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -626,7 +648,13 @@
       <c r="N4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -681,9 +709,15 @@
       <c r="N5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>2563</t>
+      <c r="O5" t="n">
+        <v>2563</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>2592</t>
         </is>
       </c>
     </row>
@@ -736,9 +770,15 @@
       <c r="N6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>2567</t>
+      <c r="O6" t="n">
+        <v>2567</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>2564</t>
         </is>
       </c>
     </row>
@@ -770,6 +810,8 @@
       <c r="M7" t="inlineStr"/>
       <c r="N7" s="3" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
+      <c r="P7" s="3" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -799,6 +841,8 @@
       <c r="M8" t="inlineStr"/>
       <c r="N8" s="3" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
+      <c r="P8" s="3" t="inlineStr"/>
+      <c r="Q8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -828,6 +872,8 @@
       <c r="M9" t="inlineStr"/>
       <c r="N9" s="3" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
+      <c r="P9" s="3" t="inlineStr"/>
+      <c r="Q9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -857,6 +903,8 @@
       <c r="M10" t="inlineStr"/>
       <c r="N10" s="3" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
+      <c r="P10" s="3" t="inlineStr"/>
+      <c r="Q10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -886,6 +934,8 @@
       <c r="M11" t="inlineStr"/>
       <c r="N11" s="3" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
+      <c r="P11" s="3" t="inlineStr"/>
+      <c r="Q11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -915,6 +965,8 @@
       <c r="M12" t="inlineStr"/>
       <c r="N12" s="3" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
+      <c r="P12" s="3" t="inlineStr"/>
+      <c r="Q12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -944,6 +996,8 @@
       <c r="M13" t="inlineStr"/>
       <c r="N13" s="3" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
+      <c r="P13" s="3" t="inlineStr"/>
+      <c r="Q13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -973,6 +1027,8 @@
       <c r="M14" t="inlineStr"/>
       <c r="N14" s="3" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
+      <c r="P14" s="3" t="inlineStr"/>
+      <c r="Q14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1002,6 +1058,8 @@
       <c r="M15" t="inlineStr"/>
       <c r="N15" s="3" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
+      <c r="P15" s="3" t="inlineStr"/>
+      <c r="Q15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1031,6 +1089,8 @@
       <c r="M16" t="inlineStr"/>
       <c r="N16" s="3" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
+      <c r="P16" s="3" t="inlineStr"/>
+      <c r="Q16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1060,6 +1120,8 @@
       <c r="M17" t="inlineStr"/>
       <c r="N17" s="3" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
+      <c r="P17" s="3" t="inlineStr"/>
+      <c r="Q17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1110,9 +1172,15 @@
       <c r="N18" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>3966</t>
+      <c r="O18" t="n">
+        <v>3966</v>
+      </c>
+      <c r="P18" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>3980</t>
         </is>
       </c>
     </row>
@@ -1165,9 +1233,15 @@
       <c r="N19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>2701</t>
+      <c r="O19" t="n">
+        <v>2701</v>
+      </c>
+      <c r="P19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>2717</t>
         </is>
       </c>
     </row>
@@ -1220,9 +1294,15 @@
       <c r="N20" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>4313</t>
+      <c r="O20" t="n">
+        <v>4313</v>
+      </c>
+      <c r="P20" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>4413</t>
         </is>
       </c>
     </row>
@@ -1275,9 +1355,15 @@
       <c r="N21" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>4841</t>
+      <c r="O21" t="n">
+        <v>4841</v>
+      </c>
+      <c r="P21" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>4971</t>
         </is>
       </c>
     </row>
@@ -1330,9 +1416,15 @@
       <c r="N22" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>4945</t>
+      <c r="O22" t="n">
+        <v>4945</v>
+      </c>
+      <c r="P22" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>5166</t>
         </is>
       </c>
     </row>
@@ -1385,9 +1477,15 @@
       <c r="N23" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>5541</t>
+      <c r="O23" t="n">
+        <v>5541</v>
+      </c>
+      <c r="P23" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>5679</t>
         </is>
       </c>
     </row>
@@ -1440,9 +1538,15 @@
       <c r="N24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>4949</t>
+      <c r="O24" t="n">
+        <v>4949</v>
+      </c>
+      <c r="P24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>4986</t>
         </is>
       </c>
     </row>
@@ -1495,9 +1599,15 @@
       <c r="N25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>5138</t>
+      <c r="O25" t="n">
+        <v>5138</v>
+      </c>
+      <c r="P25" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>5493</t>
         </is>
       </c>
     </row>
@@ -1550,7 +1660,13 @@
       <c r="N26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O26" t="inlineStr">
+      <c r="O26" t="n">
+        <v>2578</v>
+      </c>
+      <c r="P26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="inlineStr">
         <is>
           <t>2578</t>
         </is>
@@ -1605,7 +1721,13 @@
       <c r="N27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O27" t="inlineStr">
+      <c r="O27" t="n">
+        <v>2516</v>
+      </c>
+      <c r="P27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="inlineStr">
         <is>
           <t>2516</t>
         </is>
@@ -1639,6 +1761,8 @@
       <c r="M28" t="inlineStr"/>
       <c r="N28" s="3" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
+      <c r="P28" s="3" t="inlineStr"/>
+      <c r="Q28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1689,7 +1813,13 @@
       <c r="N29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O29" t="inlineStr">
+      <c r="O29" t="n">
+        <v>3420</v>
+      </c>
+      <c r="P29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q29" t="inlineStr">
         <is>
           <t>3420</t>
         </is>
@@ -1744,7 +1874,13 @@
       <c r="N30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O30" t="inlineStr">
+      <c r="O30" t="n">
+        <v>2500</v>
+      </c>
+      <c r="P30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q30" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1799,9 +1935,15 @@
       <c r="N31" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="O31" t="inlineStr">
-        <is>
-          <t>4902</t>
+      <c r="O31" t="n">
+        <v>4902</v>
+      </c>
+      <c r="P31" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>5104</t>
         </is>
       </c>
     </row>
@@ -1854,9 +1996,15 @@
       <c r="N32" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O32" t="inlineStr">
-        <is>
-          <t>3947</t>
+      <c r="O32" t="n">
+        <v>3947</v>
+      </c>
+      <c r="P32" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>4311</t>
         </is>
       </c>
     </row>
@@ -1888,6 +2036,8 @@
       <c r="M33" t="inlineStr"/>
       <c r="N33" s="3" t="inlineStr"/>
       <c r="O33" t="inlineStr"/>
+      <c r="P33" s="3" t="inlineStr"/>
+      <c r="Q33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -1938,7 +2088,13 @@
       <c r="N34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O34" t="inlineStr">
+      <c r="O34" t="n">
+        <v>0</v>
+      </c>
+      <c r="P34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1993,7 +2149,13 @@
       <c r="N35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O35" t="inlineStr">
+      <c r="O35" t="n">
+        <v>4316</v>
+      </c>
+      <c r="P35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q35" t="inlineStr">
         <is>
           <t>4316</t>
         </is>
@@ -2048,9 +2210,15 @@
       <c r="N36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>3711</t>
+      <c r="O36" t="n">
+        <v>3711</v>
+      </c>
+      <c r="P36" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>4052</t>
         </is>
       </c>
     </row>
@@ -2103,9 +2271,15 @@
       <c r="N37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>4648</t>
+      <c r="O37" t="n">
+        <v>4648</v>
+      </c>
+      <c r="P37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>4837</t>
         </is>
       </c>
     </row>
@@ -2158,9 +2332,15 @@
       <c r="N38" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>5442</t>
+      <c r="O38" t="n">
+        <v>5442</v>
+      </c>
+      <c r="P38" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>5585</t>
         </is>
       </c>
     </row>
@@ -2213,9 +2393,15 @@
       <c r="N39" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>4566</t>
+      <c r="O39" t="n">
+        <v>4566</v>
+      </c>
+      <c r="P39" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>4713</t>
         </is>
       </c>
     </row>
@@ -2268,7 +2454,13 @@
       <c r="N40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O40" t="inlineStr">
+      <c r="O40" t="n">
+        <v>0</v>
+      </c>
+      <c r="P40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2323,9 +2515,15 @@
       <c r="N41" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>4321</t>
+      <c r="O41" t="n">
+        <v>4321</v>
+      </c>
+      <c r="P41" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>4472</t>
         </is>
       </c>
     </row>
@@ -2378,9 +2576,15 @@
       <c r="N42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>3242</t>
+      <c r="O42" t="n">
+        <v>3242</v>
+      </c>
+      <c r="P42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>3277</t>
         </is>
       </c>
     </row>
@@ -2412,6 +2616,8 @@
       <c r="M43" t="inlineStr"/>
       <c r="N43" s="3" t="inlineStr"/>
       <c r="O43" t="inlineStr"/>
+      <c r="P43" s="3" t="inlineStr"/>
+      <c r="Q43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2441,6 +2647,8 @@
       <c r="M44" t="inlineStr"/>
       <c r="N44" s="3" t="inlineStr"/>
       <c r="O44" t="inlineStr"/>
+      <c r="P44" s="3" t="inlineStr"/>
+      <c r="Q44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -2491,9 +2699,15 @@
       <c r="N45" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>4018</t>
+      <c r="O45" t="n">
+        <v>4018</v>
+      </c>
+      <c r="P45" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>4086</t>
         </is>
       </c>
     </row>
@@ -2546,9 +2760,15 @@
       <c r="N46" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>4010</t>
+      <c r="O46" t="n">
+        <v>4010</v>
+      </c>
+      <c r="P46" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>4150</t>
         </is>
       </c>
     </row>
@@ -2601,9 +2821,15 @@
       <c r="N47" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>5435</t>
+      <c r="O47" t="n">
+        <v>5435</v>
+      </c>
+      <c r="P47" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>5566</t>
         </is>
       </c>
     </row>
@@ -2656,9 +2882,15 @@
       <c r="N48" s="4" t="n">
         <v>13</v>
       </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>5032</t>
+      <c r="O48" t="n">
+        <v>5032</v>
+      </c>
+      <c r="P48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>4971</t>
         </is>
       </c>
     </row>
@@ -2711,9 +2943,15 @@
       <c r="N49" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>4672</t>
+      <c r="O49" t="n">
+        <v>4672</v>
+      </c>
+      <c r="P49" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>4874</t>
         </is>
       </c>
     </row>
@@ -2766,9 +3004,15 @@
       <c r="N50" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>4951</t>
+      <c r="O50" t="n">
+        <v>4951</v>
+      </c>
+      <c r="P50" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>5066</t>
         </is>
       </c>
     </row>
@@ -2821,9 +3065,15 @@
       <c r="N51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>3378</t>
+      <c r="O51" t="n">
+        <v>3378</v>
+      </c>
+      <c r="P51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>3446</t>
         </is>
       </c>
     </row>
@@ -2876,9 +3126,15 @@
       <c r="N52" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>5139</t>
+      <c r="O52" t="n">
+        <v>5139</v>
+      </c>
+      <c r="P52" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>5263</t>
         </is>
       </c>
     </row>
@@ -2931,9 +3187,15 @@
       <c r="N53" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>3949</t>
+      <c r="O53" t="n">
+        <v>3949</v>
+      </c>
+      <c r="P53" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>4127</t>
         </is>
       </c>
     </row>
@@ -2986,9 +3248,15 @@
       <c r="N54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>2802</t>
+      <c r="O54" t="n">
+        <v>2802</v>
+      </c>
+      <c r="P54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>2860</t>
         </is>
       </c>
     </row>
@@ -3041,9 +3309,15 @@
       <c r="N55" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>4022</t>
+      <c r="O55" t="n">
+        <v>4022</v>
+      </c>
+      <c r="P55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>4024</t>
         </is>
       </c>
     </row>
@@ -3096,9 +3370,15 @@
       <c r="N56" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>5332</t>
+      <c r="O56" t="n">
+        <v>5332</v>
+      </c>
+      <c r="P56" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>5365</t>
         </is>
       </c>
     </row>
@@ -3151,9 +3431,15 @@
       <c r="N57" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>4266</t>
+      <c r="O57" t="n">
+        <v>4266</v>
+      </c>
+      <c r="P57" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>4348</t>
         </is>
       </c>
     </row>
@@ -3206,9 +3492,15 @@
       <c r="N58" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>4175</t>
+      <c r="O58" t="n">
+        <v>4175</v>
+      </c>
+      <c r="P58" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>4228</t>
         </is>
       </c>
     </row>
@@ -3261,9 +3553,15 @@
       <c r="N59" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>4080</t>
+      <c r="O59" t="n">
+        <v>4080</v>
+      </c>
+      <c r="P59" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>4173</t>
         </is>
       </c>
     </row>
@@ -3316,9 +3614,15 @@
       <c r="N60" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="O60" t="inlineStr">
-        <is>
-          <t>4299</t>
+      <c r="O60" t="n">
+        <v>4299</v>
+      </c>
+      <c r="P60" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>4462</t>
         </is>
       </c>
     </row>
@@ -3350,6 +3654,8 @@
       <c r="M61" t="inlineStr"/>
       <c r="N61" s="3" t="inlineStr"/>
       <c r="O61" t="inlineStr"/>
+      <c r="P61" s="3" t="inlineStr"/>
+      <c r="Q61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -3400,9 +3706,15 @@
       <c r="N62" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>3995</t>
+      <c r="O62" t="n">
+        <v>3995</v>
+      </c>
+      <c r="P62" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>4046</t>
         </is>
       </c>
     </row>
@@ -3455,9 +3767,15 @@
       <c r="N63" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>4081</t>
+      <c r="O63" t="n">
+        <v>4081</v>
+      </c>
+      <c r="P63" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>4161</t>
         </is>
       </c>
     </row>
@@ -3510,9 +3828,15 @@
       <c r="N64" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>4252</t>
+      <c r="O64" t="n">
+        <v>4252</v>
+      </c>
+      <c r="P64" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>4265</t>
         </is>
       </c>
     </row>
@@ -3565,9 +3889,15 @@
       <c r="N65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O65" t="inlineStr">
-        <is>
-          <t>2787</t>
+      <c r="O65" t="n">
+        <v>2787</v>
+      </c>
+      <c r="P65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>2780</t>
         </is>
       </c>
     </row>
@@ -3620,7 +3950,13 @@
       <c r="N66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O66" t="inlineStr">
+      <c r="O66" t="n">
+        <v>0</v>
+      </c>
+      <c r="P66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3675,7 +4011,13 @@
       <c r="N67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O67" t="inlineStr">
+      <c r="O67" t="n">
+        <v>0</v>
+      </c>
+      <c r="P67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3730,7 +4072,13 @@
       <c r="N68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O68" t="inlineStr">
+      <c r="O68" t="n">
+        <v>0</v>
+      </c>
+      <c r="P68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3764,6 +4112,8 @@
       <c r="M69" t="inlineStr"/>
       <c r="N69" s="3" t="inlineStr"/>
       <c r="O69" t="inlineStr"/>
+      <c r="P69" s="3" t="inlineStr"/>
+      <c r="Q69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -3814,7 +4164,13 @@
       <c r="N70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O70" t="inlineStr">
+      <c r="O70" t="n">
+        <v>0</v>
+      </c>
+      <c r="P70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3869,7 +4225,13 @@
       <c r="N71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O71" t="inlineStr">
+      <c r="O71" t="n">
+        <v>0</v>
+      </c>
+      <c r="P71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3924,7 +4286,13 @@
       <c r="N72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O72" t="inlineStr">
+      <c r="O72" t="n">
+        <v>0</v>
+      </c>
+      <c r="P72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3979,9 +4347,15 @@
       <c r="N73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O73" t="inlineStr">
-        <is>
-          <t>2794</t>
+      <c r="O73" t="n">
+        <v>2794</v>
+      </c>
+      <c r="P73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>2809</t>
         </is>
       </c>
     </row>
@@ -4034,9 +4408,15 @@
       <c r="N74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O74" t="inlineStr">
-        <is>
-          <t>2568</t>
+      <c r="O74" t="n">
+        <v>2568</v>
+      </c>
+      <c r="P74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>2565</t>
         </is>
       </c>
     </row>
@@ -4089,7 +4469,13 @@
       <c r="N75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O75" t="inlineStr">
+      <c r="O75" t="n">
+        <v>0</v>
+      </c>
+      <c r="P75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4144,9 +4530,15 @@
       <c r="N76" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="O76" t="inlineStr">
-        <is>
-          <t>3394</t>
+      <c r="O76" t="n">
+        <v>3394</v>
+      </c>
+      <c r="P76" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>3609</t>
         </is>
       </c>
     </row>
@@ -4199,9 +4591,15 @@
       <c r="N77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>2924</t>
+      <c r="O77" t="n">
+        <v>2924</v>
+      </c>
+      <c r="P77" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>3231</t>
         </is>
       </c>
     </row>
@@ -4254,7 +4652,13 @@
       <c r="N78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O78" t="inlineStr">
+      <c r="O78" t="n">
+        <v>0</v>
+      </c>
+      <c r="P78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4309,9 +4713,15 @@
       <c r="N79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>1321</t>
+      <c r="O79" t="n">
+        <v>1321</v>
+      </c>
+      <c r="P79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>1317</t>
         </is>
       </c>
     </row>
@@ -4364,7 +4774,13 @@
       <c r="N80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O80" t="inlineStr">
+      <c r="O80" t="n">
+        <v>0</v>
+      </c>
+      <c r="P80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4419,7 +4835,13 @@
       <c r="N81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O81" t="inlineStr">
+      <c r="O81" t="n">
+        <v>0</v>
+      </c>
+      <c r="P81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4474,7 +4896,13 @@
       <c r="N82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O82" t="inlineStr">
+      <c r="O82" t="n">
+        <v>0</v>
+      </c>
+      <c r="P82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4529,9 +4957,15 @@
       <c r="N83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>2575</t>
+      <c r="O83" t="n">
+        <v>2575</v>
+      </c>
+      <c r="P83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>2604</t>
         </is>
       </c>
     </row>
@@ -4584,9 +5018,15 @@
       <c r="N84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>1398</t>
+      <c r="O84" t="n">
+        <v>1398</v>
+      </c>
+      <c r="P84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>1424</t>
         </is>
       </c>
     </row>
@@ -4639,7 +5079,13 @@
       <c r="N85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O85" t="inlineStr">
+      <c r="O85" t="n">
+        <v>0</v>
+      </c>
+      <c r="P85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4694,7 +5140,13 @@
       <c r="N86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O86" t="inlineStr">
+      <c r="O86" t="n">
+        <v>0</v>
+      </c>
+      <c r="P86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4749,7 +5201,13 @@
       <c r="N87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O87" t="inlineStr">
+      <c r="O87" t="n">
+        <v>0</v>
+      </c>
+      <c r="P87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4804,7 +5262,13 @@
       <c r="N88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O88" t="inlineStr">
+      <c r="O88" t="n">
+        <v>0</v>
+      </c>
+      <c r="P88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4859,7 +5323,13 @@
       <c r="N89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O89" t="inlineStr">
+      <c r="O89" t="n">
+        <v>0</v>
+      </c>
+      <c r="P89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4914,9 +5384,15 @@
       <c r="N90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>999</t>
+      <c r="O90" t="n">
+        <v>999</v>
+      </c>
+      <c r="P90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4969,7 +5445,13 @@
       <c r="N91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O91" t="inlineStr">
+      <c r="O91" t="n">
+        <v>0</v>
+      </c>
+      <c r="P91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5024,7 +5506,13 @@
       <c r="N92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O92" t="inlineStr">
+      <c r="O92" t="n">
+        <v>0</v>
+      </c>
+      <c r="P92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5079,7 +5567,13 @@
       <c r="N93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O93" t="inlineStr">
+      <c r="O93" t="n">
+        <v>0</v>
+      </c>
+      <c r="P93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5134,7 +5628,13 @@
       <c r="N94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O94" t="inlineStr">
+      <c r="O94" t="n">
+        <v>0</v>
+      </c>
+      <c r="P94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5189,7 +5689,13 @@
       <c r="N95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O95" t="inlineStr">
+      <c r="O95" t="n">
+        <v>0</v>
+      </c>
+      <c r="P95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5244,9 +5750,15 @@
       <c r="N96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>3615</t>
+      <c r="O96" t="n">
+        <v>3615</v>
+      </c>
+      <c r="P96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q96" t="inlineStr">
+        <is>
+          <t>3603</t>
         </is>
       </c>
     </row>
@@ -5299,7 +5811,13 @@
       <c r="N97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O97" t="inlineStr">
+      <c r="O97" t="n">
+        <v>0</v>
+      </c>
+      <c r="P97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5354,7 +5872,13 @@
       <c r="N98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O98" t="inlineStr">
+      <c r="O98" t="n">
+        <v>0</v>
+      </c>
+      <c r="P98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5409,7 +5933,13 @@
       <c r="N99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O99" t="inlineStr">
+      <c r="O99" t="n">
+        <v>0</v>
+      </c>
+      <c r="P99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5464,7 +5994,13 @@
       <c r="N100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O100" t="inlineStr">
+      <c r="O100" t="n">
+        <v>0</v>
+      </c>
+      <c r="P100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5519,7 +6055,13 @@
       <c r="N101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O101" t="inlineStr">
+      <c r="O101" t="n">
+        <v>0</v>
+      </c>
+      <c r="P101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5574,7 +6116,13 @@
       <c r="N102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O102" t="inlineStr">
+      <c r="O102" t="n">
+        <v>0</v>
+      </c>
+      <c r="P102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5629,7 +6177,13 @@
       <c r="N103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O103" t="inlineStr">
+      <c r="O103" t="n">
+        <v>0</v>
+      </c>
+      <c r="P103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5684,7 +6238,13 @@
       <c r="N104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O104" t="inlineStr">
+      <c r="O104" t="n">
+        <v>0</v>
+      </c>
+      <c r="P104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5739,7 +6299,13 @@
       <c r="N105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O105" t="inlineStr">
+      <c r="O105" t="n">
+        <v>0</v>
+      </c>
+      <c r="P105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5773,6 +6339,8 @@
       <c r="M106" t="inlineStr"/>
       <c r="N106" s="3" t="inlineStr"/>
       <c r="O106" t="inlineStr"/>
+      <c r="P106" s="3" t="inlineStr"/>
+      <c r="Q106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -5802,6 +6370,8 @@
       <c r="M107" t="inlineStr"/>
       <c r="N107" s="3" t="inlineStr"/>
       <c r="O107" t="inlineStr"/>
+      <c r="P107" s="3" t="inlineStr"/>
+      <c r="Q107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -5831,6 +6401,8 @@
       <c r="M108" t="inlineStr"/>
       <c r="N108" s="3" t="inlineStr"/>
       <c r="O108" t="inlineStr"/>
+      <c r="P108" s="3" t="inlineStr"/>
+      <c r="Q108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -5860,6 +6432,8 @@
       <c r="M109" t="inlineStr"/>
       <c r="N109" s="3" t="inlineStr"/>
       <c r="O109" t="inlineStr"/>
+      <c r="P109" s="3" t="inlineStr"/>
+      <c r="Q109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -5889,6 +6463,8 @@
       <c r="M110" t="inlineStr"/>
       <c r="N110" s="3" t="inlineStr"/>
       <c r="O110" t="inlineStr"/>
+      <c r="P110" s="3" t="inlineStr"/>
+      <c r="Q110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -5918,6 +6494,8 @@
       <c r="M111" t="inlineStr"/>
       <c r="N111" s="3" t="inlineStr"/>
       <c r="O111" t="inlineStr"/>
+      <c r="P111" s="3" t="inlineStr"/>
+      <c r="Q111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -5947,6 +6525,8 @@
       <c r="M112" t="inlineStr"/>
       <c r="N112" s="3" t="inlineStr"/>
       <c r="O112" t="inlineStr"/>
+      <c r="P112" s="3" t="inlineStr"/>
+      <c r="Q112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -5976,6 +6556,8 @@
       <c r="M113" t="inlineStr"/>
       <c r="N113" s="3" t="inlineStr"/>
       <c r="O113" t="inlineStr"/>
+      <c r="P113" s="3" t="inlineStr"/>
+      <c r="Q113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -6005,6 +6587,8 @@
       <c r="M114" t="inlineStr"/>
       <c r="N114" s="3" t="inlineStr"/>
       <c r="O114" t="inlineStr"/>
+      <c r="P114" s="3" t="inlineStr"/>
+      <c r="Q114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -6048,6 +6632,8 @@
       </c>
       <c r="N115" s="3" t="inlineStr"/>
       <c r="O115" t="inlineStr"/>
+      <c r="P115" s="3" t="inlineStr"/>
+      <c r="Q115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -6092,7 +6678,13 @@
       <c r="N116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O116" t="inlineStr">
+      <c r="O116" t="n">
+        <v>0</v>
+      </c>
+      <c r="P116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6136,6 +6728,8 @@
       <c r="M117" t="inlineStr"/>
       <c r="N117" s="3" t="inlineStr"/>
       <c r="O117" t="inlineStr"/>
+      <c r="P117" s="3" t="inlineStr"/>
+      <c r="Q117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -6180,7 +6774,13 @@
       <c r="N118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O118" t="inlineStr">
+      <c r="O118" t="n">
+        <v>4474</v>
+      </c>
+      <c r="P118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q118" t="inlineStr">
         <is>
           <t>4474</t>
         </is>
@@ -6229,7 +6829,13 @@
       <c r="N119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O119" t="inlineStr">
+      <c r="O119" t="n">
+        <v>1569</v>
+      </c>
+      <c r="P119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q119" t="inlineStr">
         <is>
           <t>1569</t>
         </is>
@@ -6278,9 +6884,15 @@
       <c r="N120" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="O120" t="inlineStr">
-        <is>
-          <t>2350</t>
+      <c r="O120" t="n">
+        <v>2350</v>
+      </c>
+      <c r="P120" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q120" t="inlineStr">
+        <is>
+          <t>2457</t>
         </is>
       </c>
     </row>
@@ -6327,9 +6939,15 @@
       <c r="N121" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="O121" t="inlineStr">
-        <is>
-          <t>1786</t>
+      <c r="O121" t="n">
+        <v>1786</v>
+      </c>
+      <c r="P121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>1783</t>
         </is>
       </c>
     </row>
@@ -6376,9 +6994,15 @@
       <c r="N122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O122" t="inlineStr">
-        <is>
-          <t>1984</t>
+      <c r="O122" t="n">
+        <v>1984</v>
+      </c>
+      <c r="P122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>1993</t>
         </is>
       </c>
     </row>
@@ -6421,9 +7045,15 @@
       <c r="N123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O123" t="inlineStr">
-        <is>
-          <t>2713</t>
+      <c r="O123" t="n">
+        <v>2713</v>
+      </c>
+      <c r="P123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q123" t="inlineStr">
+        <is>
+          <t>2741</t>
         </is>
       </c>
     </row>
@@ -6462,9 +7092,15 @@
       <c r="N124" s="3" t="n">
         <v>28</v>
       </c>
-      <c r="O124" t="inlineStr">
-        <is>
-          <t>4175</t>
+      <c r="O124" t="n">
+        <v>4175</v>
+      </c>
+      <c r="P124" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="Q124" t="inlineStr">
+        <is>
+          <t>4217</t>
         </is>
       </c>
     </row>
@@ -6474,7 +7110,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>IntentFormula46</t>
+          <t>Nik11</t>
         </is>
       </c>
       <c r="C125" t="inlineStr"/>
@@ -6503,9 +7139,52 @@
       <c r="N125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="O125" t="inlineStr">
-        <is>
-          <t>1819</t>
+      <c r="O125" t="n">
+        <v>1819</v>
+      </c>
+      <c r="P125" s="4" t="n">
+        <v>8</v>
+      </c>
+      <c r="Q125" t="inlineStr">
+        <is>
+          <t>1868</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>40152068</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>TigerHunter</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr"/>
+      <c r="D126" t="inlineStr"/>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F126" s="3" t="inlineStr"/>
+      <c r="G126" t="inlineStr"/>
+      <c r="H126" s="3" t="inlineStr"/>
+      <c r="I126" t="inlineStr"/>
+      <c r="J126" s="3" t="inlineStr"/>
+      <c r="K126" t="inlineStr"/>
+      <c r="L126" s="3" t="inlineStr"/>
+      <c r="M126" t="inlineStr"/>
+      <c r="N126" s="3" t="inlineStr"/>
+      <c r="O126" t="inlineStr"/>
+      <c r="P126" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="Q126" t="inlineStr">
+        <is>
+          <t>1344</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-18 15:51:41
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -7152,10 +7152,8 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>40152068</t>
-        </is>
+      <c r="A126" t="n">
+        <v>40152068</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-05-19 11:30:54
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q126"/>
+  <dimension ref="A1:S127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,6 +476,16 @@
           <t>05-17_0</t>
         </is>
       </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>05-18_A</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>05-18_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -532,7 +542,13 @@
       <c r="P2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q2" t="inlineStr">
+      <c r="Q2" t="n">
+        <v>2586</v>
+      </c>
+      <c r="R2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="inlineStr">
         <is>
           <t>2586</t>
         </is>
@@ -593,7 +609,13 @@
       <c r="P3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q3" t="inlineStr">
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -654,7 +676,13 @@
       <c r="P4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q4" t="inlineStr">
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -715,9 +743,15 @@
       <c r="P5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>2592</t>
+      <c r="Q5" t="n">
+        <v>2592</v>
+      </c>
+      <c r="R5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>2587</t>
         </is>
       </c>
     </row>
@@ -776,9 +810,15 @@
       <c r="P6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>2564</t>
+      <c r="Q6" t="n">
+        <v>2564</v>
+      </c>
+      <c r="R6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>2585</t>
         </is>
       </c>
     </row>
@@ -812,6 +852,8 @@
       <c r="O7" t="inlineStr"/>
       <c r="P7" s="3" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
+      <c r="R7" s="3" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -843,6 +885,8 @@
       <c r="O8" t="inlineStr"/>
       <c r="P8" s="3" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
+      <c r="R8" s="3" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -874,6 +918,8 @@
       <c r="O9" t="inlineStr"/>
       <c r="P9" s="3" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
+      <c r="R9" s="3" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -905,6 +951,8 @@
       <c r="O10" t="inlineStr"/>
       <c r="P10" s="3" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
+      <c r="R10" s="3" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -936,6 +984,8 @@
       <c r="O11" t="inlineStr"/>
       <c r="P11" s="3" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
+      <c r="R11" s="3" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -967,6 +1017,8 @@
       <c r="O12" t="inlineStr"/>
       <c r="P12" s="3" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
+      <c r="R12" s="3" t="inlineStr"/>
+      <c r="S12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -998,6 +1050,8 @@
       <c r="O13" t="inlineStr"/>
       <c r="P13" s="3" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
+      <c r="R13" s="3" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1029,6 +1083,8 @@
       <c r="O14" t="inlineStr"/>
       <c r="P14" s="3" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
+      <c r="R14" s="3" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1060,6 +1116,8 @@
       <c r="O15" t="inlineStr"/>
       <c r="P15" s="3" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
+      <c r="R15" s="3" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1091,6 +1149,8 @@
       <c r="O16" t="inlineStr"/>
       <c r="P16" s="3" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
+      <c r="R16" s="3" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1122,6 +1182,8 @@
       <c r="O17" t="inlineStr"/>
       <c r="P17" s="3" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
+      <c r="R17" s="3" t="inlineStr"/>
+      <c r="S17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1178,9 +1240,15 @@
       <c r="P18" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>3980</t>
+      <c r="Q18" t="n">
+        <v>3980</v>
+      </c>
+      <c r="R18" s="4" t="n">
+        <v>17</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>4141</t>
         </is>
       </c>
     </row>
@@ -1239,9 +1307,15 @@
       <c r="P19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>2717</t>
+      <c r="Q19" t="n">
+        <v>2717</v>
+      </c>
+      <c r="R19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>2780</t>
         </is>
       </c>
     </row>
@@ -1300,9 +1374,15 @@
       <c r="P20" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>4413</t>
+      <c r="Q20" t="n">
+        <v>4413</v>
+      </c>
+      <c r="R20" s="4" t="n">
+        <v>16</v>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>4459</t>
         </is>
       </c>
     </row>
@@ -1361,9 +1441,15 @@
       <c r="P21" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>4971</t>
+      <c r="Q21" t="n">
+        <v>4971</v>
+      </c>
+      <c r="R21" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>5089</t>
         </is>
       </c>
     </row>
@@ -1422,9 +1508,15 @@
       <c r="P22" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>5166</t>
+      <c r="Q22" t="n">
+        <v>5166</v>
+      </c>
+      <c r="R22" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>5289</t>
         </is>
       </c>
     </row>
@@ -1483,9 +1575,15 @@
       <c r="P23" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>5679</t>
+      <c r="Q23" t="n">
+        <v>5679</v>
+      </c>
+      <c r="R23" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>5982</t>
         </is>
       </c>
     </row>
@@ -1544,9 +1642,15 @@
       <c r="P24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>4986</t>
+      <c r="Q24" t="n">
+        <v>4986</v>
+      </c>
+      <c r="R24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>5103</t>
         </is>
       </c>
     </row>
@@ -1605,9 +1709,15 @@
       <c r="P25" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>5493</t>
+      <c r="Q25" t="n">
+        <v>5493</v>
+      </c>
+      <c r="R25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>5591</t>
         </is>
       </c>
     </row>
@@ -1666,7 +1776,13 @@
       <c r="P26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q26" t="inlineStr">
+      <c r="Q26" t="n">
+        <v>2578</v>
+      </c>
+      <c r="R26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" t="inlineStr">
         <is>
           <t>2578</t>
         </is>
@@ -1727,7 +1843,13 @@
       <c r="P27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q27" t="inlineStr">
+      <c r="Q27" t="n">
+        <v>2516</v>
+      </c>
+      <c r="R27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" t="inlineStr">
         <is>
           <t>2516</t>
         </is>
@@ -1763,6 +1885,8 @@
       <c r="O28" t="inlineStr"/>
       <c r="P28" s="3" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
+      <c r="R28" s="3" t="inlineStr"/>
+      <c r="S28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1819,9 +1943,15 @@
       <c r="P29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>3420</t>
+      <c r="Q29" t="n">
+        <v>3420</v>
+      </c>
+      <c r="R29" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>4152</t>
         </is>
       </c>
     </row>
@@ -1880,7 +2010,13 @@
       <c r="P30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q30" t="inlineStr">
+      <c r="Q30" t="n">
+        <v>2500</v>
+      </c>
+      <c r="R30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S30" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1941,9 +2077,15 @@
       <c r="P31" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>5104</t>
+      <c r="Q31" t="n">
+        <v>5104</v>
+      </c>
+      <c r="R31" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>5217</t>
         </is>
       </c>
     </row>
@@ -2002,9 +2144,15 @@
       <c r="P32" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>4311</t>
+      <c r="Q32" t="n">
+        <v>4311</v>
+      </c>
+      <c r="R32" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>4597</t>
         </is>
       </c>
     </row>
@@ -2038,6 +2186,8 @@
       <c r="O33" t="inlineStr"/>
       <c r="P33" s="3" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
+      <c r="R33" s="3" t="inlineStr"/>
+      <c r="S33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2094,7 +2244,13 @@
       <c r="P34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q34" t="inlineStr">
+      <c r="Q34" t="n">
+        <v>0</v>
+      </c>
+      <c r="R34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2155,7 +2311,13 @@
       <c r="P35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q35" t="inlineStr">
+      <c r="Q35" t="n">
+        <v>4316</v>
+      </c>
+      <c r="R35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S35" t="inlineStr">
         <is>
           <t>4316</t>
         </is>
@@ -2216,9 +2378,15 @@
       <c r="P36" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>4052</t>
+      <c r="Q36" t="n">
+        <v>4052</v>
+      </c>
+      <c r="R36" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>4447</t>
         </is>
       </c>
     </row>
@@ -2277,9 +2445,15 @@
       <c r="P37" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>4837</t>
+      <c r="Q37" t="n">
+        <v>4837</v>
+      </c>
+      <c r="R37" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>4945</t>
         </is>
       </c>
     </row>
@@ -2338,9 +2512,15 @@
       <c r="P38" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>5585</t>
+      <c r="Q38" t="n">
+        <v>5585</v>
+      </c>
+      <c r="R38" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>5750</t>
         </is>
       </c>
     </row>
@@ -2399,9 +2579,15 @@
       <c r="P39" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>4713</t>
+      <c r="Q39" t="n">
+        <v>4713</v>
+      </c>
+      <c r="R39" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>4796</t>
         </is>
       </c>
     </row>
@@ -2460,7 +2646,13 @@
       <c r="P40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q40" t="inlineStr">
+      <c r="Q40" t="n">
+        <v>0</v>
+      </c>
+      <c r="R40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2521,9 +2713,15 @@
       <c r="P41" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="Q41" t="inlineStr">
-        <is>
-          <t>4472</t>
+      <c r="Q41" t="n">
+        <v>4472</v>
+      </c>
+      <c r="R41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>4469</t>
         </is>
       </c>
     </row>
@@ -2582,9 +2780,15 @@
       <c r="P42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>3277</t>
+      <c r="Q42" t="n">
+        <v>3277</v>
+      </c>
+      <c r="R42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>3336</t>
         </is>
       </c>
     </row>
@@ -2618,6 +2822,8 @@
       <c r="O43" t="inlineStr"/>
       <c r="P43" s="3" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
+      <c r="R43" s="3" t="inlineStr"/>
+      <c r="S43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2649,6 +2855,8 @@
       <c r="O44" t="inlineStr"/>
       <c r="P44" s="3" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
+      <c r="R44" s="3" t="inlineStr"/>
+      <c r="S44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -2705,9 +2913,15 @@
       <c r="P45" s="3" t="n">
         <v>26</v>
       </c>
-      <c r="Q45" t="inlineStr">
-        <is>
-          <t>4086</t>
+      <c r="Q45" t="n">
+        <v>4086</v>
+      </c>
+      <c r="R45" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>4119</t>
         </is>
       </c>
     </row>
@@ -2766,9 +2980,15 @@
       <c r="P46" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="Q46" t="inlineStr">
-        <is>
-          <t>4150</t>
+      <c r="Q46" t="n">
+        <v>4150</v>
+      </c>
+      <c r="R46" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>4379</t>
         </is>
       </c>
     </row>
@@ -2827,9 +3047,15 @@
       <c r="P47" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Q47" t="inlineStr">
-        <is>
-          <t>5566</t>
+      <c r="Q47" t="n">
+        <v>5566</v>
+      </c>
+      <c r="R47" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>5820</t>
         </is>
       </c>
     </row>
@@ -2888,9 +3114,15 @@
       <c r="P48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q48" t="inlineStr">
-        <is>
-          <t>4971</t>
+      <c r="Q48" t="n">
+        <v>4971</v>
+      </c>
+      <c r="R48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>5002</t>
         </is>
       </c>
     </row>
@@ -2949,9 +3181,15 @@
       <c r="P49" s="3" t="n">
         <v>29</v>
       </c>
-      <c r="Q49" t="inlineStr">
-        <is>
-          <t>4874</t>
+      <c r="Q49" t="n">
+        <v>4874</v>
+      </c>
+      <c r="R49" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>4999</t>
         </is>
       </c>
     </row>
@@ -3010,9 +3248,15 @@
       <c r="P50" s="3" t="n">
         <v>24</v>
       </c>
-      <c r="Q50" t="inlineStr">
-        <is>
-          <t>5066</t>
+      <c r="Q50" t="n">
+        <v>5066</v>
+      </c>
+      <c r="R50" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>5198</t>
         </is>
       </c>
     </row>
@@ -3071,9 +3315,15 @@
       <c r="P51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q51" t="inlineStr">
-        <is>
-          <t>3446</t>
+      <c r="Q51" t="n">
+        <v>3446</v>
+      </c>
+      <c r="R51" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>3538</t>
         </is>
       </c>
     </row>
@@ -3132,9 +3382,15 @@
       <c r="P52" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="Q52" t="inlineStr">
-        <is>
-          <t>5263</t>
+      <c r="Q52" t="n">
+        <v>5263</v>
+      </c>
+      <c r="R52" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>5398</t>
         </is>
       </c>
     </row>
@@ -3193,9 +3449,15 @@
       <c r="P53" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="Q53" t="inlineStr">
-        <is>
-          <t>4127</t>
+      <c r="Q53" t="n">
+        <v>4127</v>
+      </c>
+      <c r="R53" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>4242</t>
         </is>
       </c>
     </row>
@@ -3254,9 +3516,15 @@
       <c r="P54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q54" t="inlineStr">
-        <is>
-          <t>2860</t>
+      <c r="Q54" t="n">
+        <v>2860</v>
+      </c>
+      <c r="R54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>2889</t>
         </is>
       </c>
     </row>
@@ -3315,9 +3583,15 @@
       <c r="P55" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q55" t="inlineStr">
-        <is>
-          <t>4024</t>
+      <c r="Q55" t="n">
+        <v>4024</v>
+      </c>
+      <c r="R55" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>4337</t>
         </is>
       </c>
     </row>
@@ -3376,9 +3650,15 @@
       <c r="P56" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Q56" t="inlineStr">
-        <is>
-          <t>5365</t>
+      <c r="Q56" t="n">
+        <v>5365</v>
+      </c>
+      <c r="R56" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>5598</t>
         </is>
       </c>
     </row>
@@ -3437,9 +3717,15 @@
       <c r="P57" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="Q57" t="inlineStr">
-        <is>
-          <t>4348</t>
+      <c r="Q57" t="n">
+        <v>4348</v>
+      </c>
+      <c r="R57" s="4" t="n">
+        <v>12</v>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>4350</t>
         </is>
       </c>
     </row>
@@ -3498,9 +3784,15 @@
       <c r="P58" s="3" t="n">
         <v>23</v>
       </c>
-      <c r="Q58" t="inlineStr">
-        <is>
-          <t>4228</t>
+      <c r="Q58" t="n">
+        <v>4228</v>
+      </c>
+      <c r="R58" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>4323</t>
         </is>
       </c>
     </row>
@@ -3559,9 +3851,15 @@
       <c r="P59" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q59" t="inlineStr">
-        <is>
-          <t>4173</t>
+      <c r="Q59" t="n">
+        <v>4173</v>
+      </c>
+      <c r="R59" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>4241</t>
         </is>
       </c>
     </row>
@@ -3620,9 +3918,15 @@
       <c r="P60" s="3" t="n">
         <v>25</v>
       </c>
-      <c r="Q60" t="inlineStr">
-        <is>
-          <t>4462</t>
+      <c r="Q60" t="n">
+        <v>4462</v>
+      </c>
+      <c r="R60" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>4558</t>
         </is>
       </c>
     </row>
@@ -3656,6 +3960,8 @@
       <c r="O61" t="inlineStr"/>
       <c r="P61" s="3" t="inlineStr"/>
       <c r="Q61" t="inlineStr"/>
+      <c r="R61" s="3" t="inlineStr"/>
+      <c r="S61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -3712,9 +4018,15 @@
       <c r="P62" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q62" t="inlineStr">
-        <is>
-          <t>4046</t>
+      <c r="Q62" t="n">
+        <v>4046</v>
+      </c>
+      <c r="R62" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>4130</t>
         </is>
       </c>
     </row>
@@ -3773,9 +4085,15 @@
       <c r="P63" s="3" t="n">
         <v>22</v>
       </c>
-      <c r="Q63" t="inlineStr">
-        <is>
-          <t>4161</t>
+      <c r="Q63" t="n">
+        <v>4161</v>
+      </c>
+      <c r="R63" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>4135</t>
         </is>
       </c>
     </row>
@@ -3834,9 +4152,15 @@
       <c r="P64" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q64" t="inlineStr">
-        <is>
-          <t>4265</t>
+      <c r="Q64" t="n">
+        <v>4265</v>
+      </c>
+      <c r="R64" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="S64" t="inlineStr">
+        <is>
+          <t>4373</t>
         </is>
       </c>
     </row>
@@ -3895,9 +4219,15 @@
       <c r="P65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q65" t="inlineStr">
-        <is>
-          <t>2780</t>
+      <c r="Q65" t="n">
+        <v>2780</v>
+      </c>
+      <c r="R65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S65" t="inlineStr">
+        <is>
+          <t>2776</t>
         </is>
       </c>
     </row>
@@ -3956,7 +4286,13 @@
       <c r="P66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q66" t="inlineStr">
+      <c r="Q66" t="n">
+        <v>0</v>
+      </c>
+      <c r="R66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4017,7 +4353,13 @@
       <c r="P67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q67" t="inlineStr">
+      <c r="Q67" t="n">
+        <v>0</v>
+      </c>
+      <c r="R67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4078,7 +4420,13 @@
       <c r="P68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q68" t="inlineStr">
+      <c r="Q68" t="n">
+        <v>0</v>
+      </c>
+      <c r="R68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4114,6 +4462,8 @@
       <c r="O69" t="inlineStr"/>
       <c r="P69" s="3" t="inlineStr"/>
       <c r="Q69" t="inlineStr"/>
+      <c r="R69" s="3" t="inlineStr"/>
+      <c r="S69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -4170,7 +4520,13 @@
       <c r="P70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q70" t="inlineStr">
+      <c r="Q70" t="n">
+        <v>0</v>
+      </c>
+      <c r="R70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4231,7 +4587,13 @@
       <c r="P71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q71" t="inlineStr">
+      <c r="Q71" t="n">
+        <v>0</v>
+      </c>
+      <c r="R71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4292,7 +4654,13 @@
       <c r="P72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q72" t="inlineStr">
+      <c r="Q72" t="n">
+        <v>0</v>
+      </c>
+      <c r="R72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4353,9 +4721,15 @@
       <c r="P73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q73" t="inlineStr">
-        <is>
-          <t>2809</t>
+      <c r="Q73" t="n">
+        <v>2809</v>
+      </c>
+      <c r="R73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>2837</t>
         </is>
       </c>
     </row>
@@ -4414,9 +4788,15 @@
       <c r="P74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q74" t="inlineStr">
-        <is>
-          <t>2565</t>
+      <c r="Q74" t="n">
+        <v>2565</v>
+      </c>
+      <c r="R74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t>2589</t>
         </is>
       </c>
     </row>
@@ -4475,7 +4855,13 @@
       <c r="P75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q75" t="inlineStr">
+      <c r="Q75" t="n">
+        <v>0</v>
+      </c>
+      <c r="R75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4536,9 +4922,15 @@
       <c r="P76" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="Q76" t="inlineStr">
-        <is>
-          <t>3609</t>
+      <c r="Q76" t="n">
+        <v>3609</v>
+      </c>
+      <c r="R76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>3723</t>
         </is>
       </c>
     </row>
@@ -4597,9 +4989,15 @@
       <c r="P77" s="3" t="n">
         <v>20</v>
       </c>
-      <c r="Q77" t="inlineStr">
-        <is>
-          <t>3231</t>
+      <c r="Q77" t="n">
+        <v>3231</v>
+      </c>
+      <c r="R77" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="S77" t="inlineStr">
+        <is>
+          <t>3393</t>
         </is>
       </c>
     </row>
@@ -4658,7 +5056,13 @@
       <c r="P78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q78" t="inlineStr">
+      <c r="Q78" t="n">
+        <v>0</v>
+      </c>
+      <c r="R78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4719,9 +5123,15 @@
       <c r="P79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q79" t="inlineStr">
-        <is>
-          <t>1317</t>
+      <c r="Q79" t="n">
+        <v>1317</v>
+      </c>
+      <c r="R79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S79" t="inlineStr">
+        <is>
+          <t>1343</t>
         </is>
       </c>
     </row>
@@ -4780,7 +5190,13 @@
       <c r="P80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q80" t="inlineStr">
+      <c r="Q80" t="n">
+        <v>0</v>
+      </c>
+      <c r="R80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4841,7 +5257,13 @@
       <c r="P81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q81" t="inlineStr">
+      <c r="Q81" t="n">
+        <v>0</v>
+      </c>
+      <c r="R81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4902,7 +5324,13 @@
       <c r="P82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q82" t="inlineStr">
+      <c r="Q82" t="n">
+        <v>0</v>
+      </c>
+      <c r="R82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4963,9 +5391,15 @@
       <c r="P83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q83" t="inlineStr">
-        <is>
-          <t>2604</t>
+      <c r="Q83" t="n">
+        <v>2604</v>
+      </c>
+      <c r="R83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S83" t="inlineStr">
+        <is>
+          <t>2665</t>
         </is>
       </c>
     </row>
@@ -5024,9 +5458,15 @@
       <c r="P84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q84" t="inlineStr">
-        <is>
-          <t>1424</t>
+      <c r="Q84" t="n">
+        <v>1424</v>
+      </c>
+      <c r="R84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S84" t="inlineStr">
+        <is>
+          <t>1434</t>
         </is>
       </c>
     </row>
@@ -5085,7 +5525,13 @@
       <c r="P85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q85" t="inlineStr">
+      <c r="Q85" t="n">
+        <v>0</v>
+      </c>
+      <c r="R85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5146,7 +5592,13 @@
       <c r="P86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q86" t="inlineStr">
+      <c r="Q86" t="n">
+        <v>0</v>
+      </c>
+      <c r="R86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5207,7 +5659,13 @@
       <c r="P87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q87" t="inlineStr">
+      <c r="Q87" t="n">
+        <v>0</v>
+      </c>
+      <c r="R87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5268,7 +5726,13 @@
       <c r="P88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q88" t="inlineStr">
+      <c r="Q88" t="n">
+        <v>0</v>
+      </c>
+      <c r="R88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5329,7 +5793,13 @@
       <c r="P89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q89" t="inlineStr">
+      <c r="Q89" t="n">
+        <v>0</v>
+      </c>
+      <c r="R89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5390,7 +5860,13 @@
       <c r="P90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q90" t="inlineStr">
+      <c r="Q90" t="n">
+        <v>0</v>
+      </c>
+      <c r="R90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5451,9 +5927,15 @@
       <c r="P91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q91" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="Q91" t="n">
+        <v>0</v>
+      </c>
+      <c r="R91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S91" t="inlineStr">
+        <is>
+          <t>996</t>
         </is>
       </c>
     </row>
@@ -5512,7 +5994,13 @@
       <c r="P92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q92" t="inlineStr">
+      <c r="Q92" t="n">
+        <v>0</v>
+      </c>
+      <c r="R92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5573,7 +6061,13 @@
       <c r="P93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q93" t="inlineStr">
+      <c r="Q93" t="n">
+        <v>0</v>
+      </c>
+      <c r="R93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5634,7 +6128,13 @@
       <c r="P94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q94" t="inlineStr">
+      <c r="Q94" t="n">
+        <v>0</v>
+      </c>
+      <c r="R94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5695,7 +6195,13 @@
       <c r="P95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q95" t="inlineStr">
+      <c r="Q95" t="n">
+        <v>0</v>
+      </c>
+      <c r="R95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5756,9 +6262,15 @@
       <c r="P96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q96" t="inlineStr">
-        <is>
-          <t>3603</t>
+      <c r="Q96" t="n">
+        <v>3603</v>
+      </c>
+      <c r="R96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S96" t="inlineStr">
+        <is>
+          <t>3588</t>
         </is>
       </c>
     </row>
@@ -5817,7 +6329,13 @@
       <c r="P97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q97" t="inlineStr">
+      <c r="Q97" t="n">
+        <v>0</v>
+      </c>
+      <c r="R97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5878,7 +6396,13 @@
       <c r="P98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q98" t="inlineStr">
+      <c r="Q98" t="n">
+        <v>0</v>
+      </c>
+      <c r="R98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5939,7 +6463,13 @@
       <c r="P99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q99" t="inlineStr">
+      <c r="Q99" t="n">
+        <v>0</v>
+      </c>
+      <c r="R99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6000,7 +6530,13 @@
       <c r="P100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q100" t="inlineStr">
+      <c r="Q100" t="n">
+        <v>0</v>
+      </c>
+      <c r="R100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6061,7 +6597,13 @@
       <c r="P101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q101" t="inlineStr">
+      <c r="Q101" t="n">
+        <v>0</v>
+      </c>
+      <c r="R101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6122,7 +6664,13 @@
       <c r="P102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q102" t="inlineStr">
+      <c r="Q102" t="n">
+        <v>0</v>
+      </c>
+      <c r="R102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6183,7 +6731,13 @@
       <c r="P103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q103" t="inlineStr">
+      <c r="Q103" t="n">
+        <v>0</v>
+      </c>
+      <c r="R103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6244,7 +6798,13 @@
       <c r="P104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q104" t="inlineStr">
+      <c r="Q104" t="n">
+        <v>0</v>
+      </c>
+      <c r="R104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6305,7 +6865,13 @@
       <c r="P105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q105" t="inlineStr">
+      <c r="Q105" t="n">
+        <v>0</v>
+      </c>
+      <c r="R105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6341,6 +6907,8 @@
       <c r="O106" t="inlineStr"/>
       <c r="P106" s="3" t="inlineStr"/>
       <c r="Q106" t="inlineStr"/>
+      <c r="R106" s="3" t="inlineStr"/>
+      <c r="S106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -6372,6 +6940,8 @@
       <c r="O107" t="inlineStr"/>
       <c r="P107" s="3" t="inlineStr"/>
       <c r="Q107" t="inlineStr"/>
+      <c r="R107" s="3" t="inlineStr"/>
+      <c r="S107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -6403,6 +6973,8 @@
       <c r="O108" t="inlineStr"/>
       <c r="P108" s="3" t="inlineStr"/>
       <c r="Q108" t="inlineStr"/>
+      <c r="R108" s="3" t="inlineStr"/>
+      <c r="S108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -6434,6 +7006,8 @@
       <c r="O109" t="inlineStr"/>
       <c r="P109" s="3" t="inlineStr"/>
       <c r="Q109" t="inlineStr"/>
+      <c r="R109" s="3" t="inlineStr"/>
+      <c r="S109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -6465,6 +7039,8 @@
       <c r="O110" t="inlineStr"/>
       <c r="P110" s="3" t="inlineStr"/>
       <c r="Q110" t="inlineStr"/>
+      <c r="R110" s="3" t="inlineStr"/>
+      <c r="S110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -6496,6 +7072,8 @@
       <c r="O111" t="inlineStr"/>
       <c r="P111" s="3" t="inlineStr"/>
       <c r="Q111" t="inlineStr"/>
+      <c r="R111" s="3" t="inlineStr"/>
+      <c r="S111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -6527,6 +7105,8 @@
       <c r="O112" t="inlineStr"/>
       <c r="P112" s="3" t="inlineStr"/>
       <c r="Q112" t="inlineStr"/>
+      <c r="R112" s="3" t="inlineStr"/>
+      <c r="S112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -6558,6 +7138,8 @@
       <c r="O113" t="inlineStr"/>
       <c r="P113" s="3" t="inlineStr"/>
       <c r="Q113" t="inlineStr"/>
+      <c r="R113" s="3" t="inlineStr"/>
+      <c r="S113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -6589,6 +7171,8 @@
       <c r="O114" t="inlineStr"/>
       <c r="P114" s="3" t="inlineStr"/>
       <c r="Q114" t="inlineStr"/>
+      <c r="R114" s="3" t="inlineStr"/>
+      <c r="S114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -6634,6 +7218,8 @@
       <c r="O115" t="inlineStr"/>
       <c r="P115" s="3" t="inlineStr"/>
       <c r="Q115" t="inlineStr"/>
+      <c r="R115" s="3" t="inlineStr"/>
+      <c r="S115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -6684,7 +7270,13 @@
       <c r="P116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q116" t="inlineStr">
+      <c r="Q116" t="n">
+        <v>0</v>
+      </c>
+      <c r="R116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6730,6 +7322,8 @@
       <c r="O117" t="inlineStr"/>
       <c r="P117" s="3" t="inlineStr"/>
       <c r="Q117" t="inlineStr"/>
+      <c r="R117" s="3" t="inlineStr"/>
+      <c r="S117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -6780,9 +7374,15 @@
       <c r="P118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q118" t="inlineStr">
-        <is>
-          <t>4474</t>
+      <c r="Q118" t="n">
+        <v>4474</v>
+      </c>
+      <c r="R118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S118" t="inlineStr">
+        <is>
+          <t>4468</t>
         </is>
       </c>
     </row>
@@ -6835,9 +7435,15 @@
       <c r="P119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q119" t="inlineStr">
-        <is>
-          <t>1569</t>
+      <c r="Q119" t="n">
+        <v>1569</v>
+      </c>
+      <c r="R119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S119" t="inlineStr">
+        <is>
+          <t>1578</t>
         </is>
       </c>
     </row>
@@ -6890,9 +7496,15 @@
       <c r="P120" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="Q120" t="inlineStr">
-        <is>
-          <t>2457</t>
+      <c r="Q120" t="n">
+        <v>2457</v>
+      </c>
+      <c r="R120" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="S120" t="inlineStr">
+        <is>
+          <t>2680</t>
         </is>
       </c>
     </row>
@@ -6945,9 +7557,15 @@
       <c r="P121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q121" t="inlineStr">
-        <is>
-          <t>1783</t>
+      <c r="Q121" t="n">
+        <v>1783</v>
+      </c>
+      <c r="R121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S121" t="inlineStr">
+        <is>
+          <t>1781</t>
         </is>
       </c>
     </row>
@@ -7000,9 +7618,15 @@
       <c r="P122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q122" t="inlineStr">
-        <is>
-          <t>1993</t>
+      <c r="Q122" t="n">
+        <v>1993</v>
+      </c>
+      <c r="R122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S122" t="inlineStr">
+        <is>
+          <t>1989</t>
         </is>
       </c>
     </row>
@@ -7051,9 +7675,15 @@
       <c r="P123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Q123" t="inlineStr">
-        <is>
-          <t>2741</t>
+      <c r="Q123" t="n">
+        <v>2741</v>
+      </c>
+      <c r="R123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S123" t="inlineStr">
+        <is>
+          <t>2756</t>
         </is>
       </c>
     </row>
@@ -7098,9 +7728,15 @@
       <c r="P124" s="3" t="n">
         <v>30</v>
       </c>
-      <c r="Q124" t="inlineStr">
-        <is>
-          <t>4217</t>
+      <c r="Q124" t="n">
+        <v>4217</v>
+      </c>
+      <c r="R124" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="S124" t="inlineStr">
+        <is>
+          <t>4362</t>
         </is>
       </c>
     </row>
@@ -7145,9 +7781,15 @@
       <c r="P125" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="Q125" t="inlineStr">
-        <is>
-          <t>1868</t>
+      <c r="Q125" t="n">
+        <v>1868</v>
+      </c>
+      <c r="R125" s="4" t="n">
+        <v>14</v>
+      </c>
+      <c r="S125" t="inlineStr">
+        <is>
+          <t>1978</t>
         </is>
       </c>
     </row>
@@ -7157,7 +7799,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>TigerHunter</t>
+          <t>BL4Z3DEMON</t>
         </is>
       </c>
       <c r="C126" t="inlineStr"/>
@@ -7180,9 +7822,54 @@
       <c r="P126" s="3" t="n">
         <v>21</v>
       </c>
-      <c r="Q126" t="inlineStr">
-        <is>
-          <t>1344</t>
+      <c r="Q126" t="n">
+        <v>1344</v>
+      </c>
+      <c r="R126" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="S126" t="inlineStr">
+        <is>
+          <t>1452</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>59358630</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Player-59358630</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr"/>
+      <c r="D127" t="inlineStr"/>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F127" s="3" t="inlineStr"/>
+      <c r="G127" t="inlineStr"/>
+      <c r="H127" s="3" t="inlineStr"/>
+      <c r="I127" t="inlineStr"/>
+      <c r="J127" s="3" t="inlineStr"/>
+      <c r="K127" t="inlineStr"/>
+      <c r="L127" s="3" t="inlineStr"/>
+      <c r="M127" t="inlineStr"/>
+      <c r="N127" s="3" t="inlineStr"/>
+      <c r="O127" t="inlineStr"/>
+      <c r="P127" s="3" t="inlineStr"/>
+      <c r="Q127" t="inlineStr"/>
+      <c r="R127" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="S127" t="inlineStr">
+        <is>
+          <t>1387</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-19 16:51:08
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -7835,10 +7835,8 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>59358630</t>
-        </is>
+      <c r="A127" t="n">
+        <v>59358630</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-05-21 11:30:59
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -82,8 +82,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S127"/>
+  <dimension ref="A1:U130"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,6 +486,16 @@
           <t>05-18_0</t>
         </is>
       </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>05-20_A</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>05-20_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -548,9 +558,15 @@
       <c r="R2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>2586</t>
+      <c r="S2" t="n">
+        <v>2586</v>
+      </c>
+      <c r="T2" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>2918</t>
         </is>
       </c>
     </row>
@@ -615,7 +631,13 @@
       <c r="R3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S3" t="inlineStr">
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -682,7 +704,13 @@
       <c r="R4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S4" t="inlineStr">
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -749,9 +777,15 @@
       <c r="R5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>2587</t>
+      <c r="S5" t="n">
+        <v>2587</v>
+      </c>
+      <c r="T5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>2638</t>
         </is>
       </c>
     </row>
@@ -816,9 +850,15 @@
       <c r="R6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>2585</t>
+      <c r="S6" t="n">
+        <v>2585</v>
+      </c>
+      <c r="T6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>2628</t>
         </is>
       </c>
     </row>
@@ -840,20 +880,22 @@
         <v>2911</v>
       </c>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" s="3" t="inlineStr"/>
+      <c r="F7" s="4" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
-      <c r="H7" s="3" t="inlineStr"/>
+      <c r="H7" s="4" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
-      <c r="J7" s="3" t="inlineStr"/>
+      <c r="J7" s="4" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
-      <c r="L7" s="3" t="inlineStr"/>
+      <c r="L7" s="4" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
-      <c r="N7" s="3" t="inlineStr"/>
+      <c r="N7" s="4" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
-      <c r="P7" s="3" t="inlineStr"/>
+      <c r="P7" s="4" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
-      <c r="R7" s="3" t="inlineStr"/>
+      <c r="R7" s="4" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
+      <c r="T7" s="4" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -873,20 +915,22 @@
         <v>2595</v>
       </c>
       <c r="E8" t="inlineStr"/>
-      <c r="F8" s="3" t="inlineStr"/>
+      <c r="F8" s="4" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
-      <c r="H8" s="3" t="inlineStr"/>
+      <c r="H8" s="4" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
-      <c r="J8" s="3" t="inlineStr"/>
+      <c r="J8" s="4" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
-      <c r="L8" s="3" t="inlineStr"/>
+      <c r="L8" s="4" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
-      <c r="N8" s="3" t="inlineStr"/>
+      <c r="N8" s="4" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
-      <c r="P8" s="3" t="inlineStr"/>
+      <c r="P8" s="4" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
-      <c r="R8" s="3" t="inlineStr"/>
+      <c r="R8" s="4" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
+      <c r="T8" s="4" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -906,20 +950,22 @@
         <v>1587</v>
       </c>
       <c r="E9" t="inlineStr"/>
-      <c r="F9" s="3" t="inlineStr"/>
+      <c r="F9" s="4" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
-      <c r="H9" s="3" t="inlineStr"/>
+      <c r="H9" s="4" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
-      <c r="J9" s="3" t="inlineStr"/>
+      <c r="J9" s="4" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" s="3" t="inlineStr"/>
+      <c r="L9" s="4" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
-      <c r="N9" s="3" t="inlineStr"/>
+      <c r="N9" s="4" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
-      <c r="P9" s="3" t="inlineStr"/>
+      <c r="P9" s="4" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
-      <c r="R9" s="3" t="inlineStr"/>
+      <c r="R9" s="4" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
+      <c r="T9" s="4" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -939,20 +985,22 @@
         <v>3047</v>
       </c>
       <c r="E10" t="inlineStr"/>
-      <c r="F10" s="3" t="inlineStr"/>
+      <c r="F10" s="4" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
-      <c r="H10" s="3" t="inlineStr"/>
+      <c r="H10" s="4" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
-      <c r="J10" s="3" t="inlineStr"/>
+      <c r="J10" s="4" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
-      <c r="L10" s="3" t="inlineStr"/>
+      <c r="L10" s="4" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
-      <c r="N10" s="3" t="inlineStr"/>
+      <c r="N10" s="4" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
-      <c r="P10" s="3" t="inlineStr"/>
+      <c r="P10" s="4" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
-      <c r="R10" s="3" t="inlineStr"/>
+      <c r="R10" s="4" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
+      <c r="T10" s="4" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -972,20 +1020,22 @@
         <v>0</v>
       </c>
       <c r="E11" t="inlineStr"/>
-      <c r="F11" s="3" t="inlineStr"/>
+      <c r="F11" s="4" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
-      <c r="H11" s="3" t="inlineStr"/>
+      <c r="H11" s="4" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
-      <c r="J11" s="3" t="inlineStr"/>
+      <c r="J11" s="4" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
-      <c r="L11" s="3" t="inlineStr"/>
+      <c r="L11" s="4" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
-      <c r="N11" s="3" t="inlineStr"/>
+      <c r="N11" s="4" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
-      <c r="P11" s="3" t="inlineStr"/>
+      <c r="P11" s="4" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
-      <c r="R11" s="3" t="inlineStr"/>
+      <c r="R11" s="4" t="inlineStr"/>
       <c r="S11" t="inlineStr"/>
+      <c r="T11" s="4" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1005,20 +1055,22 @@
         <v>0</v>
       </c>
       <c r="E12" t="inlineStr"/>
-      <c r="F12" s="3" t="inlineStr"/>
+      <c r="F12" s="4" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
-      <c r="H12" s="3" t="inlineStr"/>
+      <c r="H12" s="4" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
-      <c r="J12" s="3" t="inlineStr"/>
+      <c r="J12" s="4" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
-      <c r="L12" s="3" t="inlineStr"/>
+      <c r="L12" s="4" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
-      <c r="N12" s="3" t="inlineStr"/>
+      <c r="N12" s="4" t="inlineStr"/>
       <c r="O12" t="inlineStr"/>
-      <c r="P12" s="3" t="inlineStr"/>
+      <c r="P12" s="4" t="inlineStr"/>
       <c r="Q12" t="inlineStr"/>
-      <c r="R12" s="3" t="inlineStr"/>
+      <c r="R12" s="4" t="inlineStr"/>
       <c r="S12" t="inlineStr"/>
+      <c r="T12" s="4" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1038,20 +1090,22 @@
         <v>0</v>
       </c>
       <c r="E13" t="inlineStr"/>
-      <c r="F13" s="3" t="inlineStr"/>
+      <c r="F13" s="4" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
-      <c r="H13" s="3" t="inlineStr"/>
+      <c r="H13" s="4" t="inlineStr"/>
       <c r="I13" t="inlineStr"/>
-      <c r="J13" s="3" t="inlineStr"/>
+      <c r="J13" s="4" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
-      <c r="L13" s="3" t="inlineStr"/>
+      <c r="L13" s="4" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
-      <c r="N13" s="3" t="inlineStr"/>
+      <c r="N13" s="4" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
-      <c r="P13" s="3" t="inlineStr"/>
+      <c r="P13" s="4" t="inlineStr"/>
       <c r="Q13" t="inlineStr"/>
-      <c r="R13" s="3" t="inlineStr"/>
+      <c r="R13" s="4" t="inlineStr"/>
       <c r="S13" t="inlineStr"/>
+      <c r="T13" s="4" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1071,20 +1125,22 @@
         <v>1496</v>
       </c>
       <c r="E14" t="inlineStr"/>
-      <c r="F14" s="3" t="inlineStr"/>
+      <c r="F14" s="4" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
-      <c r="H14" s="3" t="inlineStr"/>
+      <c r="H14" s="4" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" s="3" t="inlineStr"/>
+      <c r="J14" s="4" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
-      <c r="L14" s="3" t="inlineStr"/>
+      <c r="L14" s="4" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
-      <c r="N14" s="3" t="inlineStr"/>
+      <c r="N14" s="4" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
-      <c r="P14" s="3" t="inlineStr"/>
+      <c r="P14" s="4" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
-      <c r="R14" s="3" t="inlineStr"/>
+      <c r="R14" s="4" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
+      <c r="T14" s="4" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1104,20 +1160,22 @@
         <v>1454</v>
       </c>
       <c r="E15" t="inlineStr"/>
-      <c r="F15" s="3" t="inlineStr"/>
+      <c r="F15" s="4" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
-      <c r="H15" s="3" t="inlineStr"/>
+      <c r="H15" s="4" t="inlineStr"/>
       <c r="I15" t="inlineStr"/>
-      <c r="J15" s="3" t="inlineStr"/>
+      <c r="J15" s="4" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
-      <c r="L15" s="3" t="inlineStr"/>
+      <c r="L15" s="4" t="inlineStr"/>
       <c r="M15" t="inlineStr"/>
-      <c r="N15" s="3" t="inlineStr"/>
+      <c r="N15" s="4" t="inlineStr"/>
       <c r="O15" t="inlineStr"/>
-      <c r="P15" s="3" t="inlineStr"/>
+      <c r="P15" s="4" t="inlineStr"/>
       <c r="Q15" t="inlineStr"/>
-      <c r="R15" s="3" t="inlineStr"/>
+      <c r="R15" s="4" t="inlineStr"/>
       <c r="S15" t="inlineStr"/>
+      <c r="T15" s="4" t="inlineStr"/>
+      <c r="U15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1137,20 +1195,22 @@
         <v>1742</v>
       </c>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" s="3" t="inlineStr"/>
+      <c r="F16" s="4" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
-      <c r="H16" s="3" t="inlineStr"/>
+      <c r="H16" s="4" t="inlineStr"/>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" s="3" t="inlineStr"/>
+      <c r="J16" s="4" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
-      <c r="L16" s="3" t="inlineStr"/>
+      <c r="L16" s="4" t="inlineStr"/>
       <c r="M16" t="inlineStr"/>
-      <c r="N16" s="3" t="inlineStr"/>
+      <c r="N16" s="4" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
-      <c r="P16" s="3" t="inlineStr"/>
+      <c r="P16" s="4" t="inlineStr"/>
       <c r="Q16" t="inlineStr"/>
-      <c r="R16" s="3" t="inlineStr"/>
+      <c r="R16" s="4" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
+      <c r="T16" s="4" t="inlineStr"/>
+      <c r="U16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1170,20 +1230,22 @@
         <v>1624</v>
       </c>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" s="3" t="inlineStr"/>
+      <c r="F17" s="4" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
-      <c r="H17" s="3" t="inlineStr"/>
+      <c r="H17" s="4" t="inlineStr"/>
       <c r="I17" t="inlineStr"/>
-      <c r="J17" s="3" t="inlineStr"/>
+      <c r="J17" s="4" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
-      <c r="L17" s="3" t="inlineStr"/>
+      <c r="L17" s="4" t="inlineStr"/>
       <c r="M17" t="inlineStr"/>
-      <c r="N17" s="3" t="inlineStr"/>
+      <c r="N17" s="4" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
-      <c r="P17" s="3" t="inlineStr"/>
+      <c r="P17" s="4" t="inlineStr"/>
       <c r="Q17" t="inlineStr"/>
-      <c r="R17" s="3" t="inlineStr"/>
+      <c r="R17" s="4" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
+      <c r="T17" s="4" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1207,19 +1269,19 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F18" s="4" t="n">
+      <c r="F18" s="3" t="n">
         <v>17</v>
       </c>
       <c r="G18" t="n">
         <v>3773</v>
       </c>
-      <c r="H18" s="4" t="n">
+      <c r="H18" s="3" t="n">
         <v>8</v>
       </c>
       <c r="I18" t="n">
         <v>3818</v>
       </c>
-      <c r="J18" s="3" t="n">
+      <c r="J18" s="4" t="n">
         <v>20</v>
       </c>
       <c r="K18" t="n">
@@ -1237,18 +1299,24 @@
       <c r="O18" t="n">
         <v>3966</v>
       </c>
-      <c r="P18" s="4" t="n">
+      <c r="P18" s="3" t="n">
         <v>2</v>
       </c>
       <c r="Q18" t="n">
         <v>3980</v>
       </c>
-      <c r="R18" s="4" t="n">
+      <c r="R18" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>4141</t>
+      <c r="S18" t="n">
+        <v>4141</v>
+      </c>
+      <c r="T18" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>4240</t>
         </is>
       </c>
     </row>
@@ -1313,9 +1381,15 @@
       <c r="R19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>2780</t>
+      <c r="S19" t="n">
+        <v>2780</v>
+      </c>
+      <c r="T19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>2875</t>
         </is>
       </c>
     </row>
@@ -1341,48 +1415,54 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F20" s="4" t="n">
+      <c r="F20" s="3" t="n">
         <v>19</v>
       </c>
       <c r="G20" t="n">
         <v>3960</v>
       </c>
-      <c r="H20" s="3" t="n">
+      <c r="H20" s="4" t="n">
         <v>30</v>
       </c>
       <c r="I20" t="n">
         <v>4059</v>
       </c>
-      <c r="J20" s="3" t="n">
+      <c r="J20" s="4" t="n">
         <v>25</v>
       </c>
       <c r="K20" t="n">
         <v>4100</v>
       </c>
-      <c r="L20" s="3" t="n">
+      <c r="L20" s="4" t="n">
         <v>26</v>
       </c>
       <c r="M20" t="n">
         <v>4217</v>
       </c>
-      <c r="N20" s="3" t="n">
+      <c r="N20" s="4" t="n">
         <v>20</v>
       </c>
       <c r="O20" t="n">
         <v>4313</v>
       </c>
-      <c r="P20" s="3" t="n">
+      <c r="P20" s="4" t="n">
         <v>25</v>
       </c>
       <c r="Q20" t="n">
         <v>4413</v>
       </c>
-      <c r="R20" s="4" t="n">
+      <c r="R20" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="S20" t="inlineStr">
-        <is>
-          <t>4459</t>
+      <c r="S20" t="n">
+        <v>4459</v>
+      </c>
+      <c r="T20" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>4648</t>
         </is>
       </c>
     </row>
@@ -1420,13 +1500,13 @@
       <c r="I21" t="n">
         <v>4182</v>
       </c>
-      <c r="J21" s="3" t="n">
+      <c r="J21" s="4" t="n">
         <v>30</v>
       </c>
       <c r="K21" t="n">
         <v>4441</v>
       </c>
-      <c r="L21" s="3" t="n">
+      <c r="L21" s="4" t="n">
         <v>30</v>
       </c>
       <c r="M21" t="n">
@@ -1447,9 +1527,15 @@
       <c r="R21" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="S21" t="inlineStr">
-        <is>
-          <t>5089</t>
+      <c r="S21" t="n">
+        <v>5089</v>
+      </c>
+      <c r="T21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>5198</t>
         </is>
       </c>
     </row>
@@ -1475,48 +1561,54 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F22" s="3" t="n">
+      <c r="F22" s="4" t="n">
         <v>21</v>
       </c>
       <c r="G22" t="n">
         <v>4234</v>
       </c>
-      <c r="H22" s="3" t="n">
+      <c r="H22" s="4" t="n">
         <v>21</v>
       </c>
       <c r="I22" t="n">
         <v>4458</v>
       </c>
-      <c r="J22" s="3" t="n">
+      <c r="J22" s="4" t="n">
         <v>20</v>
       </c>
       <c r="K22" t="n">
         <v>4602</v>
       </c>
-      <c r="L22" s="3" t="n">
+      <c r="L22" s="4" t="n">
         <v>20</v>
       </c>
       <c r="M22" t="n">
         <v>4759</v>
       </c>
-      <c r="N22" s="3" t="n">
+      <c r="N22" s="4" t="n">
         <v>23</v>
       </c>
       <c r="O22" t="n">
         <v>4945</v>
       </c>
-      <c r="P22" s="3" t="n">
+      <c r="P22" s="4" t="n">
         <v>20</v>
       </c>
       <c r="Q22" t="n">
         <v>5166</v>
       </c>
-      <c r="R22" s="3" t="n">
+      <c r="R22" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>5289</t>
+      <c r="S22" t="n">
+        <v>5289</v>
+      </c>
+      <c r="T22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>5508</t>
         </is>
       </c>
     </row>
@@ -1542,48 +1634,54 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F23" s="3" t="n">
+      <c r="F23" s="4" t="n">
         <v>23</v>
       </c>
       <c r="G23" t="n">
         <v>4591</v>
       </c>
-      <c r="H23" s="3" t="n">
+      <c r="H23" s="4" t="n">
         <v>23</v>
       </c>
       <c r="I23" t="n">
         <v>4913</v>
       </c>
-      <c r="J23" s="3" t="n">
+      <c r="J23" s="4" t="n">
         <v>23</v>
       </c>
       <c r="K23" t="n">
         <v>5129</v>
       </c>
-      <c r="L23" s="3" t="n">
+      <c r="L23" s="4" t="n">
         <v>23</v>
       </c>
       <c r="M23" t="n">
         <v>5387</v>
       </c>
-      <c r="N23" s="3" t="n">
+      <c r="N23" s="4" t="n">
         <v>23</v>
       </c>
       <c r="O23" t="n">
         <v>5541</v>
       </c>
-      <c r="P23" s="3" t="n">
+      <c r="P23" s="4" t="n">
         <v>23</v>
       </c>
       <c r="Q23" t="n">
         <v>5679</v>
       </c>
-      <c r="R23" s="3" t="n">
+      <c r="R23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>5982</t>
+      <c r="S23" t="n">
+        <v>5982</v>
+      </c>
+      <c r="T23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>6206</t>
         </is>
       </c>
     </row>
@@ -1648,9 +1746,15 @@
       <c r="R24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="S24" t="inlineStr">
-        <is>
-          <t>5103</t>
+      <c r="S24" t="n">
+        <v>5103</v>
+      </c>
+      <c r="T24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>5643</t>
         </is>
       </c>
     </row>
@@ -1682,7 +1786,7 @@
       <c r="G25" t="n">
         <v>4248</v>
       </c>
-      <c r="H25" s="3" t="n">
+      <c r="H25" s="4" t="n">
         <v>30</v>
       </c>
       <c r="I25" t="n">
@@ -1694,7 +1798,7 @@
       <c r="K25" t="n">
         <v>4706</v>
       </c>
-      <c r="L25" s="3" t="n">
+      <c r="L25" s="4" t="n">
         <v>30</v>
       </c>
       <c r="M25" t="n">
@@ -1706,7 +1810,7 @@
       <c r="O25" t="n">
         <v>5138</v>
       </c>
-      <c r="P25" s="3" t="n">
+      <c r="P25" s="4" t="n">
         <v>30</v>
       </c>
       <c r="Q25" t="n">
@@ -1715,9 +1819,15 @@
       <c r="R25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>5591</t>
+      <c r="S25" t="n">
+        <v>5591</v>
+      </c>
+      <c r="T25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>5827</t>
         </is>
       </c>
     </row>
@@ -1782,9 +1892,15 @@
       <c r="R26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>2578</t>
+      <c r="S26" t="n">
+        <v>2578</v>
+      </c>
+      <c r="T26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>2594</t>
         </is>
       </c>
     </row>
@@ -1849,9 +1965,15 @@
       <c r="R27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>2516</t>
+      <c r="S27" t="n">
+        <v>2516</v>
+      </c>
+      <c r="T27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1873,20 +1995,22 @@
         <v>0</v>
       </c>
       <c r="E28" t="inlineStr"/>
-      <c r="F28" s="3" t="inlineStr"/>
+      <c r="F28" s="4" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
-      <c r="H28" s="3" t="inlineStr"/>
+      <c r="H28" s="4" t="inlineStr"/>
       <c r="I28" t="inlineStr"/>
-      <c r="J28" s="3" t="inlineStr"/>
+      <c r="J28" s="4" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
-      <c r="L28" s="3" t="inlineStr"/>
+      <c r="L28" s="4" t="inlineStr"/>
       <c r="M28" t="inlineStr"/>
-      <c r="N28" s="3" t="inlineStr"/>
+      <c r="N28" s="4" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
-      <c r="P28" s="3" t="inlineStr"/>
+      <c r="P28" s="4" t="inlineStr"/>
       <c r="Q28" t="inlineStr"/>
-      <c r="R28" s="3" t="inlineStr"/>
+      <c r="R28" s="4" t="inlineStr"/>
       <c r="S28" t="inlineStr"/>
+      <c r="T28" s="4" t="inlineStr"/>
+      <c r="U28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1928,7 +2052,7 @@
       <c r="K29" t="n">
         <v>2882</v>
       </c>
-      <c r="L29" s="3" t="n">
+      <c r="L29" s="4" t="n">
         <v>21</v>
       </c>
       <c r="M29" t="n">
@@ -1946,12 +2070,18 @@
       <c r="Q29" t="n">
         <v>3420</v>
       </c>
-      <c r="R29" s="3" t="n">
+      <c r="R29" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="S29" t="inlineStr">
-        <is>
-          <t>4152</t>
+      <c r="S29" t="n">
+        <v>4152</v>
+      </c>
+      <c r="T29" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>5026</t>
         </is>
       </c>
     </row>
@@ -2016,9 +2146,15 @@
       <c r="R30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="S30" t="n">
+        <v>2500</v>
+      </c>
+      <c r="T30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2044,13 +2180,13 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F31" s="3" t="n">
+      <c r="F31" s="4" t="n">
         <v>30</v>
       </c>
       <c r="G31" t="n">
         <v>4306</v>
       </c>
-      <c r="H31" s="3" t="n">
+      <c r="H31" s="4" t="n">
         <v>30</v>
       </c>
       <c r="I31" t="n">
@@ -2080,12 +2216,18 @@
       <c r="Q31" t="n">
         <v>5104</v>
       </c>
-      <c r="R31" s="3" t="n">
+      <c r="R31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="S31" t="inlineStr">
-        <is>
-          <t>5217</t>
+      <c r="S31" t="n">
+        <v>5217</v>
+      </c>
+      <c r="T31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>5496</t>
         </is>
       </c>
     </row>
@@ -2111,7 +2253,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F32" s="3" t="n">
+      <c r="F32" s="4" t="n">
         <v>20</v>
       </c>
       <c r="G32" t="n">
@@ -2135,24 +2277,30 @@
       <c r="M32" t="n">
         <v>3640</v>
       </c>
-      <c r="N32" s="3" t="n">
+      <c r="N32" s="4" t="n">
         <v>20</v>
       </c>
       <c r="O32" t="n">
         <v>3947</v>
       </c>
-      <c r="P32" s="3" t="n">
+      <c r="P32" s="4" t="n">
         <v>20</v>
       </c>
       <c r="Q32" t="n">
         <v>4311</v>
       </c>
-      <c r="R32" s="3" t="n">
+      <c r="R32" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="S32" t="inlineStr">
-        <is>
-          <t>4597</t>
+      <c r="S32" t="n">
+        <v>4597</v>
+      </c>
+      <c r="T32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>4618</t>
         </is>
       </c>
     </row>
@@ -2174,20 +2322,22 @@
         <v>4556</v>
       </c>
       <c r="E33" t="inlineStr"/>
-      <c r="F33" s="3" t="inlineStr"/>
+      <c r="F33" s="4" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
-      <c r="H33" s="3" t="inlineStr"/>
+      <c r="H33" s="4" t="inlineStr"/>
       <c r="I33" t="inlineStr"/>
-      <c r="J33" s="3" t="inlineStr"/>
+      <c r="J33" s="4" t="inlineStr"/>
       <c r="K33" t="inlineStr"/>
-      <c r="L33" s="3" t="inlineStr"/>
+      <c r="L33" s="4" t="inlineStr"/>
       <c r="M33" t="inlineStr"/>
-      <c r="N33" s="3" t="inlineStr"/>
+      <c r="N33" s="4" t="inlineStr"/>
       <c r="O33" t="inlineStr"/>
-      <c r="P33" s="3" t="inlineStr"/>
+      <c r="P33" s="4" t="inlineStr"/>
       <c r="Q33" t="inlineStr"/>
-      <c r="R33" s="3" t="inlineStr"/>
+      <c r="R33" s="4" t="inlineStr"/>
       <c r="S33" t="inlineStr"/>
+      <c r="T33" s="4" t="inlineStr"/>
+      <c r="U33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2250,7 +2400,13 @@
       <c r="R34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S34" t="inlineStr">
+      <c r="S34" t="n">
+        <v>0</v>
+      </c>
+      <c r="T34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2284,19 +2440,19 @@
       <c r="G35" t="n">
         <v>3050</v>
       </c>
-      <c r="H35" s="3" t="n">
+      <c r="H35" s="4" t="n">
         <v>20</v>
       </c>
       <c r="I35" t="n">
         <v>3424</v>
       </c>
-      <c r="J35" s="3" t="n">
+      <c r="J35" s="4" t="n">
         <v>20</v>
       </c>
       <c r="K35" t="n">
         <v>3985</v>
       </c>
-      <c r="L35" s="3" t="n">
+      <c r="L35" s="4" t="n">
         <v>20</v>
       </c>
       <c r="M35" t="n">
@@ -2317,9 +2473,15 @@
       <c r="R35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S35" t="inlineStr">
-        <is>
-          <t>4316</t>
+      <c r="S35" t="n">
+        <v>4316</v>
+      </c>
+      <c r="T35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2345,7 +2507,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F36" s="3" t="n">
+      <c r="F36" s="4" t="n">
         <v>20</v>
       </c>
       <c r="G36" t="n">
@@ -2363,7 +2525,7 @@
       <c r="K36" t="n">
         <v>3339</v>
       </c>
-      <c r="L36" s="3" t="n">
+      <c r="L36" s="4" t="n">
         <v>20</v>
       </c>
       <c r="M36" t="n">
@@ -2375,18 +2537,24 @@
       <c r="O36" t="n">
         <v>3711</v>
       </c>
-      <c r="P36" s="3" t="n">
+      <c r="P36" s="4" t="n">
         <v>20</v>
       </c>
       <c r="Q36" t="n">
         <v>4052</v>
       </c>
-      <c r="R36" s="4" t="n">
+      <c r="R36" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="S36" t="inlineStr">
-        <is>
-          <t>4447</t>
+      <c r="S36" t="n">
+        <v>4447</v>
+      </c>
+      <c r="T36" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>4585</t>
         </is>
       </c>
     </row>
@@ -2412,48 +2580,54 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F37" s="3" t="n">
+      <c r="F37" s="4" t="n">
         <v>30</v>
       </c>
       <c r="G37" t="n">
         <v>4137</v>
       </c>
-      <c r="H37" s="3" t="n">
+      <c r="H37" s="4" t="n">
         <v>30</v>
       </c>
       <c r="I37" t="n">
         <v>4346</v>
       </c>
-      <c r="J37" s="3" t="n">
+      <c r="J37" s="4" t="n">
         <v>30</v>
       </c>
       <c r="K37" t="n">
         <v>4485</v>
       </c>
-      <c r="L37" s="3" t="n">
+      <c r="L37" s="4" t="n">
         <v>30</v>
       </c>
       <c r="M37" t="n">
         <v>4581</v>
       </c>
-      <c r="N37" s="3" t="n">
+      <c r="N37" s="4" t="n">
         <v>30</v>
       </c>
       <c r="O37" t="n">
         <v>4648</v>
       </c>
-      <c r="P37" s="3" t="n">
+      <c r="P37" s="4" t="n">
         <v>30</v>
       </c>
       <c r="Q37" t="n">
         <v>4837</v>
       </c>
-      <c r="R37" s="3" t="n">
+      <c r="R37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="S37" t="inlineStr">
-        <is>
-          <t>4945</t>
+      <c r="S37" t="n">
+        <v>4945</v>
+      </c>
+      <c r="T37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>5224</t>
         </is>
       </c>
     </row>
@@ -2491,7 +2665,7 @@
       <c r="I38" t="n">
         <v>4867</v>
       </c>
-      <c r="J38" s="3" t="n">
+      <c r="J38" s="4" t="n">
         <v>30</v>
       </c>
       <c r="K38" t="n">
@@ -2515,12 +2689,18 @@
       <c r="Q38" t="n">
         <v>5585</v>
       </c>
-      <c r="R38" s="3" t="n">
+      <c r="R38" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="S38" t="inlineStr">
-        <is>
-          <t>5750</t>
+      <c r="S38" t="n">
+        <v>5750</v>
+      </c>
+      <c r="T38" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>6080</t>
         </is>
       </c>
     </row>
@@ -2546,48 +2726,54 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F39" s="3" t="n">
+      <c r="F39" s="4" t="n">
         <v>29</v>
       </c>
       <c r="G39" t="n">
         <v>4122</v>
       </c>
-      <c r="H39" s="3" t="n">
+      <c r="H39" s="4" t="n">
         <v>29</v>
       </c>
       <c r="I39" t="n">
         <v>4295</v>
       </c>
-      <c r="J39" s="3" t="n">
+      <c r="J39" s="4" t="n">
         <v>20</v>
       </c>
       <c r="K39" t="n">
         <v>4379</v>
       </c>
-      <c r="L39" s="3" t="n">
+      <c r="L39" s="4" t="n">
         <v>29</v>
       </c>
       <c r="M39" t="n">
         <v>4457</v>
       </c>
-      <c r="N39" s="3" t="n">
+      <c r="N39" s="4" t="n">
         <v>29</v>
       </c>
       <c r="O39" t="n">
         <v>4566</v>
       </c>
-      <c r="P39" s="3" t="n">
+      <c r="P39" s="4" t="n">
         <v>26</v>
       </c>
       <c r="Q39" t="n">
         <v>4713</v>
       </c>
-      <c r="R39" s="3" t="n">
+      <c r="R39" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="S39" t="inlineStr">
-        <is>
-          <t>4796</t>
+      <c r="S39" t="n">
+        <v>4796</v>
+      </c>
+      <c r="T39" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>5024</t>
         </is>
       </c>
     </row>
@@ -2652,7 +2838,13 @@
       <c r="R40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S40" t="inlineStr">
+      <c r="S40" t="n">
+        <v>0</v>
+      </c>
+      <c r="T40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2680,7 +2872,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F41" s="4" t="n">
+      <c r="F41" s="3" t="n">
         <v>7</v>
       </c>
       <c r="G41" t="n">
@@ -2704,13 +2896,13 @@
       <c r="M41" t="n">
         <v>4275</v>
       </c>
-      <c r="N41" s="4" t="n">
+      <c r="N41" s="3" t="n">
         <v>1</v>
       </c>
       <c r="O41" t="n">
         <v>4321</v>
       </c>
-      <c r="P41" s="4" t="n">
+      <c r="P41" s="3" t="n">
         <v>6</v>
       </c>
       <c r="Q41" t="n">
@@ -2719,9 +2911,15 @@
       <c r="R41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S41" t="inlineStr">
-        <is>
-          <t>4469</t>
+      <c r="S41" t="n">
+        <v>4469</v>
+      </c>
+      <c r="T41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>4606</t>
         </is>
       </c>
     </row>
@@ -2786,9 +2984,15 @@
       <c r="R42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S42" t="inlineStr">
-        <is>
-          <t>3336</t>
+      <c r="S42" t="n">
+        <v>3336</v>
+      </c>
+      <c r="T42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>3429</t>
         </is>
       </c>
     </row>
@@ -2810,20 +3014,22 @@
         <v>5787</v>
       </c>
       <c r="E43" t="inlineStr"/>
-      <c r="F43" s="3" t="inlineStr"/>
+      <c r="F43" s="4" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
-      <c r="H43" s="3" t="inlineStr"/>
+      <c r="H43" s="4" t="inlineStr"/>
       <c r="I43" t="inlineStr"/>
-      <c r="J43" s="3" t="inlineStr"/>
+      <c r="J43" s="4" t="inlineStr"/>
       <c r="K43" t="inlineStr"/>
-      <c r="L43" s="3" t="inlineStr"/>
+      <c r="L43" s="4" t="inlineStr"/>
       <c r="M43" t="inlineStr"/>
-      <c r="N43" s="3" t="inlineStr"/>
+      <c r="N43" s="4" t="inlineStr"/>
       <c r="O43" t="inlineStr"/>
-      <c r="P43" s="3" t="inlineStr"/>
+      <c r="P43" s="4" t="inlineStr"/>
       <c r="Q43" t="inlineStr"/>
-      <c r="R43" s="3" t="inlineStr"/>
+      <c r="R43" s="4" t="inlineStr"/>
       <c r="S43" t="inlineStr"/>
+      <c r="T43" s="4" t="inlineStr"/>
+      <c r="U43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -2843,20 +3049,22 @@
         <v>6019</v>
       </c>
       <c r="E44" t="inlineStr"/>
-      <c r="F44" s="3" t="inlineStr"/>
+      <c r="F44" s="4" t="inlineStr"/>
       <c r="G44" t="inlineStr"/>
-      <c r="H44" s="3" t="inlineStr"/>
+      <c r="H44" s="4" t="inlineStr"/>
       <c r="I44" t="inlineStr"/>
-      <c r="J44" s="3" t="inlineStr"/>
+      <c r="J44" s="4" t="inlineStr"/>
       <c r="K44" t="inlineStr"/>
-      <c r="L44" s="3" t="inlineStr"/>
+      <c r="L44" s="4" t="inlineStr"/>
       <c r="M44" t="inlineStr"/>
-      <c r="N44" s="3" t="inlineStr"/>
+      <c r="N44" s="4" t="inlineStr"/>
       <c r="O44" t="inlineStr"/>
-      <c r="P44" s="3" t="inlineStr"/>
+      <c r="P44" s="4" t="inlineStr"/>
       <c r="Q44" t="inlineStr"/>
-      <c r="R44" s="3" t="inlineStr"/>
+      <c r="R44" s="4" t="inlineStr"/>
       <c r="S44" t="inlineStr"/>
+      <c r="T44" s="4" t="inlineStr"/>
+      <c r="U44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -2880,50 +3088,50 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F45" s="3" t="n">
+      <c r="F45" s="4" t="n">
         <v>26</v>
       </c>
       <c r="G45" t="n">
         <v>3773</v>
       </c>
-      <c r="H45" s="3" t="n">
+      <c r="H45" s="4" t="n">
         <v>27</v>
       </c>
       <c r="I45" t="n">
         <v>3940</v>
       </c>
-      <c r="J45" s="3" t="n">
+      <c r="J45" s="4" t="n">
         <v>26</v>
       </c>
       <c r="K45" t="n">
         <v>3982</v>
       </c>
-      <c r="L45" s="3" t="n">
+      <c r="L45" s="4" t="n">
         <v>28</v>
       </c>
       <c r="M45" t="n">
         <v>3986</v>
       </c>
-      <c r="N45" s="3" t="n">
+      <c r="N45" s="4" t="n">
         <v>25</v>
       </c>
       <c r="O45" t="n">
         <v>4018</v>
       </c>
-      <c r="P45" s="3" t="n">
+      <c r="P45" s="4" t="n">
         <v>26</v>
       </c>
       <c r="Q45" t="n">
         <v>4086</v>
       </c>
-      <c r="R45" s="3" t="n">
+      <c r="R45" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="S45" t="inlineStr">
-        <is>
-          <t>4119</t>
-        </is>
-      </c>
+      <c r="S45" t="n">
+        <v>4119</v>
+      </c>
+      <c r="T45" s="4" t="inlineStr"/>
+      <c r="U45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -2947,48 +3155,54 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F46" s="4" t="n">
+      <c r="F46" s="3" t="n">
         <v>10</v>
       </c>
       <c r="G46" t="n">
         <v>3436</v>
       </c>
-      <c r="H46" s="4" t="n">
+      <c r="H46" s="3" t="n">
         <v>10</v>
       </c>
       <c r="I46" t="n">
         <v>3625</v>
       </c>
-      <c r="J46" s="4" t="n">
+      <c r="J46" s="3" t="n">
         <v>6</v>
       </c>
       <c r="K46" t="n">
         <v>3715</v>
       </c>
-      <c r="L46" s="4" t="n">
+      <c r="L46" s="3" t="n">
         <v>9</v>
       </c>
       <c r="M46" t="n">
         <v>3789</v>
       </c>
-      <c r="N46" s="4" t="n">
+      <c r="N46" s="3" t="n">
         <v>10</v>
       </c>
       <c r="O46" t="n">
         <v>4010</v>
       </c>
-      <c r="P46" s="4" t="n">
+      <c r="P46" s="3" t="n">
         <v>5</v>
       </c>
       <c r="Q46" t="n">
         <v>4150</v>
       </c>
-      <c r="R46" s="4" t="n">
+      <c r="R46" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="S46" t="inlineStr">
-        <is>
-          <t>4379</t>
+      <c r="S46" t="n">
+        <v>4379</v>
+      </c>
+      <c r="T46" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>4769</t>
         </is>
       </c>
     </row>
@@ -3038,7 +3252,7 @@
       <c r="M47" t="n">
         <v>5209</v>
       </c>
-      <c r="N47" s="3" t="n">
+      <c r="N47" s="4" t="n">
         <v>30</v>
       </c>
       <c r="O47" t="n">
@@ -3053,9 +3267,15 @@
       <c r="R47" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="S47" t="inlineStr">
-        <is>
-          <t>5820</t>
+      <c r="S47" t="n">
+        <v>5820</v>
+      </c>
+      <c r="T47" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>6040</t>
         </is>
       </c>
     </row>
@@ -3081,31 +3301,31 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F48" s="3" t="n">
+      <c r="F48" s="4" t="n">
         <v>30</v>
       </c>
       <c r="G48" t="n">
         <v>4477</v>
       </c>
-      <c r="H48" s="4" t="n">
+      <c r="H48" s="3" t="n">
         <v>10</v>
       </c>
       <c r="I48" t="n">
         <v>4505</v>
       </c>
-      <c r="J48" s="3" t="n">
+      <c r="J48" s="4" t="n">
         <v>28</v>
       </c>
       <c r="K48" t="n">
         <v>4884</v>
       </c>
-      <c r="L48" s="3" t="n">
+      <c r="L48" s="4" t="n">
         <v>30</v>
       </c>
       <c r="M48" t="n">
         <v>5064</v>
       </c>
-      <c r="N48" s="4" t="n">
+      <c r="N48" s="3" t="n">
         <v>13</v>
       </c>
       <c r="O48" t="n">
@@ -3120,9 +3340,15 @@
       <c r="R48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S48" t="inlineStr">
-        <is>
-          <t>5002</t>
+      <c r="S48" t="n">
+        <v>5002</v>
+      </c>
+      <c r="T48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>5138</t>
         </is>
       </c>
     </row>
@@ -3148,48 +3374,54 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F49" s="3" t="n">
+      <c r="F49" s="4" t="n">
         <v>29</v>
       </c>
       <c r="G49" t="n">
         <v>4259</v>
       </c>
-      <c r="H49" s="3" t="n">
+      <c r="H49" s="4" t="n">
         <v>29</v>
       </c>
       <c r="I49" t="n">
         <v>4419</v>
       </c>
-      <c r="J49" s="3" t="n">
+      <c r="J49" s="4" t="n">
         <v>29</v>
       </c>
       <c r="K49" t="n">
         <v>4527</v>
       </c>
-      <c r="L49" s="3" t="n">
+      <c r="L49" s="4" t="n">
         <v>29</v>
       </c>
       <c r="M49" t="n">
         <v>4658</v>
       </c>
-      <c r="N49" s="3" t="n">
+      <c r="N49" s="4" t="n">
         <v>29</v>
       </c>
       <c r="O49" t="n">
         <v>4672</v>
       </c>
-      <c r="P49" s="3" t="n">
+      <c r="P49" s="4" t="n">
         <v>29</v>
       </c>
       <c r="Q49" t="n">
         <v>4874</v>
       </c>
-      <c r="R49" s="3" t="n">
+      <c r="R49" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="S49" t="inlineStr">
-        <is>
-          <t>4999</t>
+      <c r="S49" t="n">
+        <v>4999</v>
+      </c>
+      <c r="T49" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>5242</t>
         </is>
       </c>
     </row>
@@ -3215,48 +3447,54 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F50" s="3" t="n">
+      <c r="F50" s="4" t="n">
         <v>23</v>
       </c>
       <c r="G50" t="n">
         <v>4303</v>
       </c>
-      <c r="H50" s="3" t="n">
+      <c r="H50" s="4" t="n">
         <v>23</v>
       </c>
       <c r="I50" t="n">
         <v>4426</v>
       </c>
-      <c r="J50" s="3" t="n">
+      <c r="J50" s="4" t="n">
         <v>23</v>
       </c>
       <c r="K50" t="n">
         <v>4611</v>
       </c>
-      <c r="L50" s="3" t="n">
+      <c r="L50" s="4" t="n">
         <v>25</v>
       </c>
       <c r="M50" t="n">
         <v>4779</v>
       </c>
-      <c r="N50" s="3" t="n">
+      <c r="N50" s="4" t="n">
         <v>24</v>
       </c>
       <c r="O50" t="n">
         <v>4951</v>
       </c>
-      <c r="P50" s="3" t="n">
+      <c r="P50" s="4" t="n">
         <v>24</v>
       </c>
       <c r="Q50" t="n">
         <v>5066</v>
       </c>
-      <c r="R50" s="3" t="n">
+      <c r="R50" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="S50" t="inlineStr">
-        <is>
-          <t>5198</t>
+      <c r="S50" t="n">
+        <v>5198</v>
+      </c>
+      <c r="T50" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>5616</t>
         </is>
       </c>
     </row>
@@ -3282,7 +3520,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F51" s="4" t="n">
+      <c r="F51" s="3" t="n">
         <v>2</v>
       </c>
       <c r="G51" t="n">
@@ -3300,7 +3538,7 @@
       <c r="K51" t="n">
         <v>3017</v>
       </c>
-      <c r="L51" s="4" t="n">
+      <c r="L51" s="3" t="n">
         <v>9</v>
       </c>
       <c r="M51" t="n">
@@ -3321,11 +3559,11 @@
       <c r="R51" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S51" t="inlineStr">
-        <is>
-          <t>3538</t>
-        </is>
-      </c>
+      <c r="S51" t="n">
+        <v>3538</v>
+      </c>
+      <c r="T51" s="4" t="inlineStr"/>
+      <c r="U51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -3349,31 +3587,31 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F52" s="3" t="n">
+      <c r="F52" s="4" t="n">
         <v>30</v>
       </c>
       <c r="G52" t="n">
         <v>4337</v>
       </c>
-      <c r="H52" s="3" t="n">
+      <c r="H52" s="4" t="n">
         <v>30</v>
       </c>
       <c r="I52" t="n">
         <v>4474</v>
       </c>
-      <c r="J52" s="3" t="n">
+      <c r="J52" s="4" t="n">
         <v>30</v>
       </c>
       <c r="K52" t="n">
         <v>4786</v>
       </c>
-      <c r="L52" s="3" t="n">
+      <c r="L52" s="4" t="n">
         <v>30</v>
       </c>
       <c r="M52" t="n">
         <v>4919</v>
       </c>
-      <c r="N52" s="3" t="n">
+      <c r="N52" s="4" t="n">
         <v>30</v>
       </c>
       <c r="O52" t="n">
@@ -3385,12 +3623,18 @@
       <c r="Q52" t="n">
         <v>5263</v>
       </c>
-      <c r="R52" s="3" t="n">
+      <c r="R52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="S52" t="inlineStr">
-        <is>
-          <t>5398</t>
+      <c r="S52" t="n">
+        <v>5398</v>
+      </c>
+      <c r="T52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>5743</t>
         </is>
       </c>
     </row>
@@ -3416,7 +3660,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F53" s="4" t="n">
+      <c r="F53" s="3" t="n">
         <v>5</v>
       </c>
       <c r="G53" t="n">
@@ -3428,36 +3672,42 @@
       <c r="I53" t="n">
         <v>3593</v>
       </c>
-      <c r="J53" s="4" t="n">
+      <c r="J53" s="3" t="n">
         <v>5</v>
       </c>
       <c r="K53" t="n">
         <v>3673</v>
       </c>
-      <c r="L53" s="4" t="n">
+      <c r="L53" s="3" t="n">
         <v>8</v>
       </c>
       <c r="M53" t="n">
         <v>3799</v>
       </c>
-      <c r="N53" s="4" t="n">
+      <c r="N53" s="3" t="n">
         <v>8</v>
       </c>
       <c r="O53" t="n">
         <v>3949</v>
       </c>
-      <c r="P53" s="4" t="n">
+      <c r="P53" s="3" t="n">
         <v>8</v>
       </c>
       <c r="Q53" t="n">
         <v>4127</v>
       </c>
-      <c r="R53" s="4" t="n">
+      <c r="R53" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="S53" t="inlineStr">
-        <is>
-          <t>4242</t>
+      <c r="S53" t="n">
+        <v>4242</v>
+      </c>
+      <c r="T53" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>4519</t>
         </is>
       </c>
     </row>
@@ -3522,11 +3772,11 @@
       <c r="R54" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S54" t="inlineStr">
-        <is>
-          <t>2889</t>
-        </is>
-      </c>
+      <c r="S54" t="n">
+        <v>2889</v>
+      </c>
+      <c r="T54" s="4" t="inlineStr"/>
+      <c r="U54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -3550,31 +3800,31 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F55" s="4" t="n">
+      <c r="F55" s="3" t="n">
         <v>10</v>
       </c>
       <c r="G55" t="n">
         <v>2916</v>
       </c>
-      <c r="H55" s="3" t="n">
+      <c r="H55" s="4" t="n">
         <v>20</v>
       </c>
       <c r="I55" t="n">
         <v>3364</v>
       </c>
-      <c r="J55" s="4" t="n">
+      <c r="J55" s="3" t="n">
         <v>3</v>
       </c>
       <c r="K55" t="n">
         <v>3415</v>
       </c>
-      <c r="L55" s="4" t="n">
+      <c r="L55" s="3" t="n">
         <v>10</v>
       </c>
       <c r="M55" t="n">
         <v>3614</v>
       </c>
-      <c r="N55" s="3" t="n">
+      <c r="N55" s="4" t="n">
         <v>20</v>
       </c>
       <c r="O55" t="n">
@@ -3586,12 +3836,18 @@
       <c r="Q55" t="n">
         <v>4024</v>
       </c>
-      <c r="R55" s="3" t="n">
+      <c r="R55" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="S55" t="inlineStr">
-        <is>
-          <t>4337</t>
+      <c r="S55" t="n">
+        <v>4337</v>
+      </c>
+      <c r="T55" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>4822</t>
         </is>
       </c>
     </row>
@@ -3629,7 +3885,7 @@
       <c r="I56" t="n">
         <v>4793</v>
       </c>
-      <c r="J56" s="3" t="n">
+      <c r="J56" s="4" t="n">
         <v>30</v>
       </c>
       <c r="K56" t="n">
@@ -3656,9 +3912,15 @@
       <c r="R56" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="S56" t="inlineStr">
-        <is>
-          <t>5598</t>
+      <c r="S56" t="n">
+        <v>5598</v>
+      </c>
+      <c r="T56" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="U56" t="inlineStr">
+        <is>
+          <t>5995</t>
         </is>
       </c>
     </row>
@@ -3684,48 +3946,54 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F57" s="4" t="n">
+      <c r="F57" s="3" t="n">
         <v>19</v>
       </c>
       <c r="G57" t="n">
         <v>3976</v>
       </c>
-      <c r="H57" s="4" t="n">
+      <c r="H57" s="3" t="n">
         <v>18</v>
       </c>
       <c r="I57" t="n">
         <v>4040</v>
       </c>
-      <c r="J57" s="3" t="n">
+      <c r="J57" s="4" t="n">
         <v>20</v>
       </c>
       <c r="K57" t="n">
         <v>4140</v>
       </c>
-      <c r="L57" s="4" t="n">
+      <c r="L57" s="3" t="n">
         <v>17</v>
       </c>
       <c r="M57" t="n">
         <v>4201</v>
       </c>
-      <c r="N57" s="4" t="n">
+      <c r="N57" s="3" t="n">
         <v>12</v>
       </c>
       <c r="O57" t="n">
         <v>4266</v>
       </c>
-      <c r="P57" s="4" t="n">
+      <c r="P57" s="3" t="n">
         <v>18</v>
       </c>
       <c r="Q57" t="n">
         <v>4348</v>
       </c>
-      <c r="R57" s="4" t="n">
+      <c r="R57" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="S57" t="inlineStr">
-        <is>
-          <t>4350</t>
+      <c r="S57" t="n">
+        <v>4350</v>
+      </c>
+      <c r="T57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="U57" t="inlineStr">
+        <is>
+          <t>4513</t>
         </is>
       </c>
     </row>
@@ -3751,48 +4019,54 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F58" s="3" t="n">
+      <c r="F58" s="4" t="n">
         <v>23</v>
       </c>
       <c r="G58" t="n">
         <v>3272</v>
       </c>
-      <c r="H58" s="3" t="n">
+      <c r="H58" s="4" t="n">
         <v>23</v>
       </c>
       <c r="I58" t="n">
         <v>3570</v>
       </c>
-      <c r="J58" s="3" t="n">
+      <c r="J58" s="4" t="n">
         <v>23</v>
       </c>
       <c r="K58" t="n">
         <v>3811</v>
       </c>
-      <c r="L58" s="3" t="n">
+      <c r="L58" s="4" t="n">
         <v>23</v>
       </c>
       <c r="M58" t="n">
         <v>4022</v>
       </c>
-      <c r="N58" s="3" t="n">
+      <c r="N58" s="4" t="n">
         <v>23</v>
       </c>
       <c r="O58" t="n">
         <v>4175</v>
       </c>
-      <c r="P58" s="3" t="n">
+      <c r="P58" s="4" t="n">
         <v>23</v>
       </c>
       <c r="Q58" t="n">
         <v>4228</v>
       </c>
-      <c r="R58" s="3" t="n">
+      <c r="R58" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="S58" t="inlineStr">
-        <is>
-          <t>4323</t>
+      <c r="S58" t="n">
+        <v>4323</v>
+      </c>
+      <c r="T58" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="U58" t="inlineStr">
+        <is>
+          <t>4498</t>
         </is>
       </c>
     </row>
@@ -3818,13 +4092,13 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F59" s="3" t="n">
+      <c r="F59" s="4" t="n">
         <v>20</v>
       </c>
       <c r="G59" t="n">
         <v>3806</v>
       </c>
-      <c r="H59" s="3" t="n">
+      <c r="H59" s="4" t="n">
         <v>20</v>
       </c>
       <c r="I59" t="n">
@@ -3836,30 +4110,36 @@
       <c r="K59" t="n">
         <v>3976</v>
       </c>
-      <c r="L59" s="3" t="n">
+      <c r="L59" s="4" t="n">
         <v>20</v>
       </c>
       <c r="M59" t="n">
         <v>4057</v>
       </c>
-      <c r="N59" s="4" t="n">
+      <c r="N59" s="3" t="n">
         <v>3</v>
       </c>
       <c r="O59" t="n">
         <v>4080</v>
       </c>
-      <c r="P59" s="3" t="n">
+      <c r="P59" s="4" t="n">
         <v>20</v>
       </c>
       <c r="Q59" t="n">
         <v>4173</v>
       </c>
-      <c r="R59" s="3" t="n">
+      <c r="R59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="S59" t="inlineStr">
-        <is>
-          <t>4241</t>
+      <c r="S59" t="n">
+        <v>4241</v>
+      </c>
+      <c r="T59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="U59" t="inlineStr">
+        <is>
+          <t>4484</t>
         </is>
       </c>
     </row>
@@ -3885,48 +4165,54 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F60" s="3" t="n">
+      <c r="F60" s="4" t="n">
         <v>25</v>
       </c>
       <c r="G60" t="n">
         <v>3996</v>
       </c>
-      <c r="H60" s="3" t="n">
+      <c r="H60" s="4" t="n">
         <v>25</v>
       </c>
       <c r="I60" t="n">
         <v>4115</v>
       </c>
-      <c r="J60" s="3" t="n">
+      <c r="J60" s="4" t="n">
         <v>25</v>
       </c>
       <c r="K60" t="n">
         <v>4180</v>
       </c>
-      <c r="L60" s="3" t="n">
+      <c r="L60" s="4" t="n">
         <v>25</v>
       </c>
       <c r="M60" t="n">
         <v>4298</v>
       </c>
-      <c r="N60" s="3" t="n">
+      <c r="N60" s="4" t="n">
         <v>25</v>
       </c>
       <c r="O60" t="n">
         <v>4299</v>
       </c>
-      <c r="P60" s="3" t="n">
+      <c r="P60" s="4" t="n">
         <v>25</v>
       </c>
       <c r="Q60" t="n">
         <v>4462</v>
       </c>
-      <c r="R60" s="3" t="n">
+      <c r="R60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="S60" t="inlineStr">
-        <is>
-          <t>4558</t>
+      <c r="S60" t="n">
+        <v>4558</v>
+      </c>
+      <c r="T60" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="U60" t="inlineStr">
+        <is>
+          <t>4692</t>
         </is>
       </c>
     </row>
@@ -3948,20 +4234,22 @@
         <v>4095</v>
       </c>
       <c r="E61" t="inlineStr"/>
-      <c r="F61" s="3" t="inlineStr"/>
+      <c r="F61" s="4" t="inlineStr"/>
       <c r="G61" t="inlineStr"/>
-      <c r="H61" s="3" t="inlineStr"/>
+      <c r="H61" s="4" t="inlineStr"/>
       <c r="I61" t="inlineStr"/>
-      <c r="J61" s="3" t="inlineStr"/>
+      <c r="J61" s="4" t="inlineStr"/>
       <c r="K61" t="inlineStr"/>
-      <c r="L61" s="3" t="inlineStr"/>
+      <c r="L61" s="4" t="inlineStr"/>
       <c r="M61" t="inlineStr"/>
-      <c r="N61" s="3" t="inlineStr"/>
+      <c r="N61" s="4" t="inlineStr"/>
       <c r="O61" t="inlineStr"/>
-      <c r="P61" s="3" t="inlineStr"/>
+      <c r="P61" s="4" t="inlineStr"/>
       <c r="Q61" t="inlineStr"/>
-      <c r="R61" s="3" t="inlineStr"/>
+      <c r="R61" s="4" t="inlineStr"/>
       <c r="S61" t="inlineStr"/>
+      <c r="T61" s="4" t="inlineStr"/>
+      <c r="U61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -3985,48 +4273,54 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F62" s="3" t="n">
+      <c r="F62" s="4" t="n">
         <v>30</v>
       </c>
       <c r="G62" t="n">
         <v>3617</v>
       </c>
-      <c r="H62" s="3" t="n">
+      <c r="H62" s="4" t="n">
         <v>30</v>
       </c>
       <c r="I62" t="n">
         <v>3823</v>
       </c>
-      <c r="J62" s="3" t="n">
+      <c r="J62" s="4" t="n">
         <v>30</v>
       </c>
       <c r="K62" t="n">
         <v>3992</v>
       </c>
-      <c r="L62" s="3" t="n">
+      <c r="L62" s="4" t="n">
         <v>30</v>
       </c>
       <c r="M62" t="n">
         <v>4013</v>
       </c>
-      <c r="N62" s="3" t="n">
+      <c r="N62" s="4" t="n">
         <v>30</v>
       </c>
       <c r="O62" t="n">
         <v>3995</v>
       </c>
-      <c r="P62" s="3" t="n">
+      <c r="P62" s="4" t="n">
         <v>30</v>
       </c>
       <c r="Q62" t="n">
         <v>4046</v>
       </c>
-      <c r="R62" s="3" t="n">
+      <c r="R62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="S62" t="inlineStr">
-        <is>
-          <t>4130</t>
+      <c r="S62" t="n">
+        <v>4130</v>
+      </c>
+      <c r="T62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="U62" t="inlineStr">
+        <is>
+          <t>4260</t>
         </is>
       </c>
     </row>
@@ -4052,48 +4346,54 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F63" s="3" t="n">
+      <c r="F63" s="4" t="n">
         <v>20</v>
       </c>
       <c r="G63" t="n">
         <v>3790</v>
       </c>
-      <c r="H63" s="3" t="n">
+      <c r="H63" s="4" t="n">
         <v>20</v>
       </c>
       <c r="I63" t="n">
         <v>3982</v>
       </c>
-      <c r="J63" s="3" t="n">
+      <c r="J63" s="4" t="n">
         <v>22</v>
       </c>
       <c r="K63" t="n">
         <v>3995</v>
       </c>
-      <c r="L63" s="3" t="n">
+      <c r="L63" s="4" t="n">
         <v>20</v>
       </c>
       <c r="M63" t="n">
         <v>4025</v>
       </c>
-      <c r="N63" s="3" t="n">
+      <c r="N63" s="4" t="n">
         <v>20</v>
       </c>
       <c r="O63" t="n">
         <v>4081</v>
       </c>
-      <c r="P63" s="3" t="n">
+      <c r="P63" s="4" t="n">
         <v>22</v>
       </c>
       <c r="Q63" t="n">
         <v>4161</v>
       </c>
-      <c r="R63" s="3" t="n">
+      <c r="R63" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="S63" t="inlineStr">
-        <is>
-          <t>4135</t>
+      <c r="S63" t="n">
+        <v>4135</v>
+      </c>
+      <c r="T63" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="U63" t="inlineStr">
+        <is>
+          <t>4264</t>
         </is>
       </c>
     </row>
@@ -4119,48 +4419,54 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F64" s="4" t="n">
+      <c r="F64" s="3" t="n">
         <v>18</v>
       </c>
       <c r="G64" t="n">
         <v>3992</v>
       </c>
-      <c r="H64" s="3" t="n">
+      <c r="H64" s="4" t="n">
         <v>20</v>
       </c>
       <c r="I64" t="n">
         <v>3999</v>
       </c>
-      <c r="J64" s="4" t="n">
+      <c r="J64" s="3" t="n">
         <v>4</v>
       </c>
       <c r="K64" t="n">
         <v>4012</v>
       </c>
-      <c r="L64" s="3" t="n">
+      <c r="L64" s="4" t="n">
         <v>20</v>
       </c>
       <c r="M64" t="n">
         <v>4120</v>
       </c>
-      <c r="N64" s="3" t="n">
+      <c r="N64" s="4" t="n">
         <v>20</v>
       </c>
       <c r="O64" t="n">
         <v>4252</v>
       </c>
-      <c r="P64" s="3" t="n">
+      <c r="P64" s="4" t="n">
         <v>20</v>
       </c>
       <c r="Q64" t="n">
         <v>4265</v>
       </c>
-      <c r="R64" s="4" t="n">
+      <c r="R64" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="S64" t="inlineStr">
-        <is>
-          <t>4373</t>
+      <c r="S64" t="n">
+        <v>4373</v>
+      </c>
+      <c r="T64" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="U64" t="inlineStr">
+        <is>
+          <t>4548</t>
         </is>
       </c>
     </row>
@@ -4225,9 +4531,15 @@
       <c r="R65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S65" t="inlineStr">
-        <is>
-          <t>2776</t>
+      <c r="S65" t="n">
+        <v>2776</v>
+      </c>
+      <c r="T65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U65" t="inlineStr">
+        <is>
+          <t>2770</t>
         </is>
       </c>
     </row>
@@ -4292,7 +4604,13 @@
       <c r="R66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S66" t="inlineStr">
+      <c r="S66" t="n">
+        <v>0</v>
+      </c>
+      <c r="T66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4359,7 +4677,13 @@
       <c r="R67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S67" t="inlineStr">
+      <c r="S67" t="n">
+        <v>0</v>
+      </c>
+      <c r="T67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4426,7 +4750,13 @@
       <c r="R68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S68" t="inlineStr">
+      <c r="S68" t="n">
+        <v>0</v>
+      </c>
+      <c r="T68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4450,20 +4780,22 @@
         <v>4437</v>
       </c>
       <c r="E69" t="inlineStr"/>
-      <c r="F69" s="3" t="inlineStr"/>
+      <c r="F69" s="4" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
-      <c r="H69" s="3" t="inlineStr"/>
+      <c r="H69" s="4" t="inlineStr"/>
       <c r="I69" t="inlineStr"/>
-      <c r="J69" s="3" t="inlineStr"/>
+      <c r="J69" s="4" t="inlineStr"/>
       <c r="K69" t="inlineStr"/>
-      <c r="L69" s="3" t="inlineStr"/>
+      <c r="L69" s="4" t="inlineStr"/>
       <c r="M69" t="inlineStr"/>
-      <c r="N69" s="3" t="inlineStr"/>
+      <c r="N69" s="4" t="inlineStr"/>
       <c r="O69" t="inlineStr"/>
-      <c r="P69" s="3" t="inlineStr"/>
+      <c r="P69" s="4" t="inlineStr"/>
       <c r="Q69" t="inlineStr"/>
-      <c r="R69" s="3" t="inlineStr"/>
+      <c r="R69" s="4" t="inlineStr"/>
       <c r="S69" t="inlineStr"/>
+      <c r="T69" s="4" t="inlineStr"/>
+      <c r="U69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -4526,7 +4858,13 @@
       <c r="R70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S70" t="inlineStr">
+      <c r="S70" t="n">
+        <v>0</v>
+      </c>
+      <c r="T70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4593,7 +4931,13 @@
       <c r="R71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S71" t="inlineStr">
+      <c r="S71" t="n">
+        <v>0</v>
+      </c>
+      <c r="T71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4660,7 +5004,13 @@
       <c r="R72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S72" t="inlineStr">
+      <c r="S72" t="n">
+        <v>0</v>
+      </c>
+      <c r="T72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4727,9 +5077,15 @@
       <c r="R73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S73" t="inlineStr">
-        <is>
-          <t>2837</t>
+      <c r="S73" t="n">
+        <v>2837</v>
+      </c>
+      <c r="T73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U73" t="inlineStr">
+        <is>
+          <t>2887</t>
         </is>
       </c>
     </row>
@@ -4794,9 +5150,15 @@
       <c r="R74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S74" t="inlineStr">
-        <is>
-          <t>2589</t>
+      <c r="S74" t="n">
+        <v>2589</v>
+      </c>
+      <c r="T74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U74" t="inlineStr">
+        <is>
+          <t>2624</t>
         </is>
       </c>
     </row>
@@ -4861,7 +5223,13 @@
       <c r="R75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S75" t="inlineStr">
+      <c r="S75" t="n">
+        <v>0</v>
+      </c>
+      <c r="T75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4895,7 +5263,7 @@
       <c r="G76" t="n">
         <v>2946</v>
       </c>
-      <c r="H76" s="4" t="n">
+      <c r="H76" s="3" t="n">
         <v>10</v>
       </c>
       <c r="I76" t="n">
@@ -4913,13 +5281,13 @@
       <c r="M76" t="n">
         <v>3326</v>
       </c>
-      <c r="N76" s="4" t="n">
+      <c r="N76" s="3" t="n">
         <v>3</v>
       </c>
       <c r="O76" t="n">
         <v>3394</v>
       </c>
-      <c r="P76" s="4" t="n">
+      <c r="P76" s="3" t="n">
         <v>12</v>
       </c>
       <c r="Q76" t="n">
@@ -4928,9 +5296,15 @@
       <c r="R76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S76" t="inlineStr">
-        <is>
-          <t>3723</t>
+      <c r="S76" t="n">
+        <v>3723</v>
+      </c>
+      <c r="T76" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="U76" t="inlineStr">
+        <is>
+          <t>4247</t>
         </is>
       </c>
     </row>
@@ -4956,7 +5330,7 @@
           <t>二馆</t>
         </is>
       </c>
-      <c r="F77" s="4" t="n">
+      <c r="F77" s="3" t="n">
         <v>2</v>
       </c>
       <c r="G77" t="n">
@@ -4986,18 +5360,24 @@
       <c r="O77" t="n">
         <v>2924</v>
       </c>
-      <c r="P77" s="3" t="n">
+      <c r="P77" s="4" t="n">
         <v>20</v>
       </c>
       <c r="Q77" t="n">
         <v>3231</v>
       </c>
-      <c r="R77" s="4" t="n">
+      <c r="R77" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="S77" t="inlineStr">
-        <is>
-          <t>3393</t>
+      <c r="S77" t="n">
+        <v>3393</v>
+      </c>
+      <c r="T77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U77" t="inlineStr">
+        <is>
+          <t>3426</t>
         </is>
       </c>
     </row>
@@ -5062,7 +5442,13 @@
       <c r="R78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S78" t="inlineStr">
+      <c r="S78" t="n">
+        <v>0</v>
+      </c>
+      <c r="T78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5129,9 +5515,15 @@
       <c r="R79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S79" t="inlineStr">
-        <is>
-          <t>1343</t>
+      <c r="S79" t="n">
+        <v>1343</v>
+      </c>
+      <c r="T79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U79" t="inlineStr">
+        <is>
+          <t>1341</t>
         </is>
       </c>
     </row>
@@ -5196,7 +5588,13 @@
       <c r="R80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S80" t="inlineStr">
+      <c r="S80" t="n">
+        <v>0</v>
+      </c>
+      <c r="T80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5263,7 +5661,13 @@
       <c r="R81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S81" t="inlineStr">
+      <c r="S81" t="n">
+        <v>0</v>
+      </c>
+      <c r="T81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5330,7 +5734,13 @@
       <c r="R82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S82" t="inlineStr">
+      <c r="S82" t="n">
+        <v>0</v>
+      </c>
+      <c r="T82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5397,9 +5807,15 @@
       <c r="R83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S83" t="inlineStr">
-        <is>
-          <t>2665</t>
+      <c r="S83" t="n">
+        <v>2665</v>
+      </c>
+      <c r="T83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U83" t="inlineStr">
+        <is>
+          <t>2735</t>
         </is>
       </c>
     </row>
@@ -5464,9 +5880,15 @@
       <c r="R84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S84" t="inlineStr">
-        <is>
-          <t>1434</t>
+      <c r="S84" t="n">
+        <v>1434</v>
+      </c>
+      <c r="T84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U84" t="inlineStr">
+        <is>
+          <t>1428</t>
         </is>
       </c>
     </row>
@@ -5531,7 +5953,13 @@
       <c r="R85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S85" t="inlineStr">
+      <c r="S85" t="n">
+        <v>0</v>
+      </c>
+      <c r="T85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5598,7 +6026,13 @@
       <c r="R86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S86" t="inlineStr">
+      <c r="S86" t="n">
+        <v>0</v>
+      </c>
+      <c r="T86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5665,7 +6099,13 @@
       <c r="R87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S87" t="inlineStr">
+      <c r="S87" t="n">
+        <v>0</v>
+      </c>
+      <c r="T87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5732,7 +6172,13 @@
       <c r="R88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S88" t="inlineStr">
+      <c r="S88" t="n">
+        <v>0</v>
+      </c>
+      <c r="T88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5799,7 +6245,13 @@
       <c r="R89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S89" t="inlineStr">
+      <c r="S89" t="n">
+        <v>0</v>
+      </c>
+      <c r="T89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5866,7 +6318,13 @@
       <c r="R90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S90" t="inlineStr">
+      <c r="S90" t="n">
+        <v>0</v>
+      </c>
+      <c r="T90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5933,9 +6391,15 @@
       <c r="R91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S91" t="inlineStr">
-        <is>
-          <t>996</t>
+      <c r="S91" t="n">
+        <v>996</v>
+      </c>
+      <c r="T91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U91" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -6000,7 +6464,13 @@
       <c r="R92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S92" t="inlineStr">
+      <c r="S92" t="n">
+        <v>0</v>
+      </c>
+      <c r="T92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6067,7 +6537,13 @@
       <c r="R93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S93" t="inlineStr">
+      <c r="S93" t="n">
+        <v>0</v>
+      </c>
+      <c r="T93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6134,7 +6610,13 @@
       <c r="R94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S94" t="inlineStr">
+      <c r="S94" t="n">
+        <v>0</v>
+      </c>
+      <c r="T94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6201,7 +6683,13 @@
       <c r="R95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S95" t="inlineStr">
+      <c r="S95" t="n">
+        <v>0</v>
+      </c>
+      <c r="T95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6229,7 +6717,7 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F96" s="3" t="n">
+      <c r="F96" s="4" t="n">
         <v>30</v>
       </c>
       <c r="G96" t="n">
@@ -6268,9 +6756,15 @@
       <c r="R96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S96" t="inlineStr">
-        <is>
-          <t>3588</t>
+      <c r="S96" t="n">
+        <v>3588</v>
+      </c>
+      <c r="T96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U96" t="inlineStr">
+        <is>
+          <t>3566</t>
         </is>
       </c>
     </row>
@@ -6335,7 +6829,13 @@
       <c r="R97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S97" t="inlineStr">
+      <c r="S97" t="n">
+        <v>0</v>
+      </c>
+      <c r="T97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6402,7 +6902,13 @@
       <c r="R98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S98" t="inlineStr">
+      <c r="S98" t="n">
+        <v>0</v>
+      </c>
+      <c r="T98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6469,7 +6975,13 @@
       <c r="R99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S99" t="inlineStr">
+      <c r="S99" t="n">
+        <v>0</v>
+      </c>
+      <c r="T99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6536,7 +7048,13 @@
       <c r="R100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S100" t="inlineStr">
+      <c r="S100" t="n">
+        <v>0</v>
+      </c>
+      <c r="T100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6603,7 +7121,13 @@
       <c r="R101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S101" t="inlineStr">
+      <c r="S101" t="n">
+        <v>0</v>
+      </c>
+      <c r="T101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6670,7 +7194,13 @@
       <c r="R102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S102" t="inlineStr">
+      <c r="S102" t="n">
+        <v>0</v>
+      </c>
+      <c r="T102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6737,7 +7267,13 @@
       <c r="R103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S103" t="inlineStr">
+      <c r="S103" t="n">
+        <v>0</v>
+      </c>
+      <c r="T103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6804,7 +7340,13 @@
       <c r="R104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S104" t="inlineStr">
+      <c r="S104" t="n">
+        <v>0</v>
+      </c>
+      <c r="T104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6871,7 +7413,13 @@
       <c r="R105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S105" t="inlineStr">
+      <c r="S105" t="n">
+        <v>0</v>
+      </c>
+      <c r="T105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6895,20 +7443,22 @@
         <v>0</v>
       </c>
       <c r="E106" t="inlineStr"/>
-      <c r="F106" s="3" t="inlineStr"/>
+      <c r="F106" s="4" t="inlineStr"/>
       <c r="G106" t="inlineStr"/>
-      <c r="H106" s="3" t="inlineStr"/>
+      <c r="H106" s="4" t="inlineStr"/>
       <c r="I106" t="inlineStr"/>
-      <c r="J106" s="3" t="inlineStr"/>
+      <c r="J106" s="4" t="inlineStr"/>
       <c r="K106" t="inlineStr"/>
-      <c r="L106" s="3" t="inlineStr"/>
+      <c r="L106" s="4" t="inlineStr"/>
       <c r="M106" t="inlineStr"/>
-      <c r="N106" s="3" t="inlineStr"/>
+      <c r="N106" s="4" t="inlineStr"/>
       <c r="O106" t="inlineStr"/>
-      <c r="P106" s="3" t="inlineStr"/>
+      <c r="P106" s="4" t="inlineStr"/>
       <c r="Q106" t="inlineStr"/>
-      <c r="R106" s="3" t="inlineStr"/>
+      <c r="R106" s="4" t="inlineStr"/>
       <c r="S106" t="inlineStr"/>
+      <c r="T106" s="4" t="inlineStr"/>
+      <c r="U106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -6928,20 +7478,22 @@
         <v>0</v>
       </c>
       <c r="E107" t="inlineStr"/>
-      <c r="F107" s="3" t="inlineStr"/>
+      <c r="F107" s="4" t="inlineStr"/>
       <c r="G107" t="inlineStr"/>
-      <c r="H107" s="3" t="inlineStr"/>
+      <c r="H107" s="4" t="inlineStr"/>
       <c r="I107" t="inlineStr"/>
-      <c r="J107" s="3" t="inlineStr"/>
+      <c r="J107" s="4" t="inlineStr"/>
       <c r="K107" t="inlineStr"/>
-      <c r="L107" s="3" t="inlineStr"/>
+      <c r="L107" s="4" t="inlineStr"/>
       <c r="M107" t="inlineStr"/>
-      <c r="N107" s="3" t="inlineStr"/>
+      <c r="N107" s="4" t="inlineStr"/>
       <c r="O107" t="inlineStr"/>
-      <c r="P107" s="3" t="inlineStr"/>
+      <c r="P107" s="4" t="inlineStr"/>
       <c r="Q107" t="inlineStr"/>
-      <c r="R107" s="3" t="inlineStr"/>
+      <c r="R107" s="4" t="inlineStr"/>
       <c r="S107" t="inlineStr"/>
+      <c r="T107" s="4" t="inlineStr"/>
+      <c r="U107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -6961,20 +7513,22 @@
         <v>0</v>
       </c>
       <c r="E108" t="inlineStr"/>
-      <c r="F108" s="3" t="inlineStr"/>
+      <c r="F108" s="4" t="inlineStr"/>
       <c r="G108" t="inlineStr"/>
-      <c r="H108" s="3" t="inlineStr"/>
+      <c r="H108" s="4" t="inlineStr"/>
       <c r="I108" t="inlineStr"/>
-      <c r="J108" s="3" t="inlineStr"/>
+      <c r="J108" s="4" t="inlineStr"/>
       <c r="K108" t="inlineStr"/>
-      <c r="L108" s="3" t="inlineStr"/>
+      <c r="L108" s="4" t="inlineStr"/>
       <c r="M108" t="inlineStr"/>
-      <c r="N108" s="3" t="inlineStr"/>
+      <c r="N108" s="4" t="inlineStr"/>
       <c r="O108" t="inlineStr"/>
-      <c r="P108" s="3" t="inlineStr"/>
+      <c r="P108" s="4" t="inlineStr"/>
       <c r="Q108" t="inlineStr"/>
-      <c r="R108" s="3" t="inlineStr"/>
+      <c r="R108" s="4" t="inlineStr"/>
       <c r="S108" t="inlineStr"/>
+      <c r="T108" s="4" t="inlineStr"/>
+      <c r="U108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -6994,20 +7548,22 @@
         <v>0</v>
       </c>
       <c r="E109" t="inlineStr"/>
-      <c r="F109" s="3" t="inlineStr"/>
+      <c r="F109" s="4" t="inlineStr"/>
       <c r="G109" t="inlineStr"/>
-      <c r="H109" s="3" t="inlineStr"/>
+      <c r="H109" s="4" t="inlineStr"/>
       <c r="I109" t="inlineStr"/>
-      <c r="J109" s="3" t="inlineStr"/>
+      <c r="J109" s="4" t="inlineStr"/>
       <c r="K109" t="inlineStr"/>
-      <c r="L109" s="3" t="inlineStr"/>
+      <c r="L109" s="4" t="inlineStr"/>
       <c r="M109" t="inlineStr"/>
-      <c r="N109" s="3" t="inlineStr"/>
+      <c r="N109" s="4" t="inlineStr"/>
       <c r="O109" t="inlineStr"/>
-      <c r="P109" s="3" t="inlineStr"/>
+      <c r="P109" s="4" t="inlineStr"/>
       <c r="Q109" t="inlineStr"/>
-      <c r="R109" s="3" t="inlineStr"/>
+      <c r="R109" s="4" t="inlineStr"/>
       <c r="S109" t="inlineStr"/>
+      <c r="T109" s="4" t="inlineStr"/>
+      <c r="U109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -7027,20 +7583,22 @@
         <v>0</v>
       </c>
       <c r="E110" t="inlineStr"/>
-      <c r="F110" s="3" t="inlineStr"/>
+      <c r="F110" s="4" t="inlineStr"/>
       <c r="G110" t="inlineStr"/>
-      <c r="H110" s="3" t="inlineStr"/>
+      <c r="H110" s="4" t="inlineStr"/>
       <c r="I110" t="inlineStr"/>
-      <c r="J110" s="3" t="inlineStr"/>
+      <c r="J110" s="4" t="inlineStr"/>
       <c r="K110" t="inlineStr"/>
-      <c r="L110" s="3" t="inlineStr"/>
+      <c r="L110" s="4" t="inlineStr"/>
       <c r="M110" t="inlineStr"/>
-      <c r="N110" s="3" t="inlineStr"/>
+      <c r="N110" s="4" t="inlineStr"/>
       <c r="O110" t="inlineStr"/>
-      <c r="P110" s="3" t="inlineStr"/>
+      <c r="P110" s="4" t="inlineStr"/>
       <c r="Q110" t="inlineStr"/>
-      <c r="R110" s="3" t="inlineStr"/>
+      <c r="R110" s="4" t="inlineStr"/>
       <c r="S110" t="inlineStr"/>
+      <c r="T110" s="4" t="inlineStr"/>
+      <c r="U110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -7060,20 +7618,22 @@
         <v>0</v>
       </c>
       <c r="E111" t="inlineStr"/>
-      <c r="F111" s="3" t="inlineStr"/>
+      <c r="F111" s="4" t="inlineStr"/>
       <c r="G111" t="inlineStr"/>
-      <c r="H111" s="3" t="inlineStr"/>
+      <c r="H111" s="4" t="inlineStr"/>
       <c r="I111" t="inlineStr"/>
-      <c r="J111" s="3" t="inlineStr"/>
+      <c r="J111" s="4" t="inlineStr"/>
       <c r="K111" t="inlineStr"/>
-      <c r="L111" s="3" t="inlineStr"/>
+      <c r="L111" s="4" t="inlineStr"/>
       <c r="M111" t="inlineStr"/>
-      <c r="N111" s="3" t="inlineStr"/>
+      <c r="N111" s="4" t="inlineStr"/>
       <c r="O111" t="inlineStr"/>
-      <c r="P111" s="3" t="inlineStr"/>
+      <c r="P111" s="4" t="inlineStr"/>
       <c r="Q111" t="inlineStr"/>
-      <c r="R111" s="3" t="inlineStr"/>
+      <c r="R111" s="4" t="inlineStr"/>
       <c r="S111" t="inlineStr"/>
+      <c r="T111" s="4" t="inlineStr"/>
+      <c r="U111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -7093,20 +7653,22 @@
         <v>0</v>
       </c>
       <c r="E112" t="inlineStr"/>
-      <c r="F112" s="3" t="inlineStr"/>
+      <c r="F112" s="4" t="inlineStr"/>
       <c r="G112" t="inlineStr"/>
-      <c r="H112" s="3" t="inlineStr"/>
+      <c r="H112" s="4" t="inlineStr"/>
       <c r="I112" t="inlineStr"/>
-      <c r="J112" s="3" t="inlineStr"/>
+      <c r="J112" s="4" t="inlineStr"/>
       <c r="K112" t="inlineStr"/>
-      <c r="L112" s="3" t="inlineStr"/>
+      <c r="L112" s="4" t="inlineStr"/>
       <c r="M112" t="inlineStr"/>
-      <c r="N112" s="3" t="inlineStr"/>
+      <c r="N112" s="4" t="inlineStr"/>
       <c r="O112" t="inlineStr"/>
-      <c r="P112" s="3" t="inlineStr"/>
+      <c r="P112" s="4" t="inlineStr"/>
       <c r="Q112" t="inlineStr"/>
-      <c r="R112" s="3" t="inlineStr"/>
+      <c r="R112" s="4" t="inlineStr"/>
       <c r="S112" t="inlineStr"/>
+      <c r="T112" s="4" t="inlineStr"/>
+      <c r="U112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -7126,20 +7688,22 @@
         <v>0</v>
       </c>
       <c r="E113" t="inlineStr"/>
-      <c r="F113" s="3" t="inlineStr"/>
+      <c r="F113" s="4" t="inlineStr"/>
       <c r="G113" t="inlineStr"/>
-      <c r="H113" s="3" t="inlineStr"/>
+      <c r="H113" s="4" t="inlineStr"/>
       <c r="I113" t="inlineStr"/>
-      <c r="J113" s="3" t="inlineStr"/>
+      <c r="J113" s="4" t="inlineStr"/>
       <c r="K113" t="inlineStr"/>
-      <c r="L113" s="3" t="inlineStr"/>
+      <c r="L113" s="4" t="inlineStr"/>
       <c r="M113" t="inlineStr"/>
-      <c r="N113" s="3" t="inlineStr"/>
+      <c r="N113" s="4" t="inlineStr"/>
       <c r="O113" t="inlineStr"/>
-      <c r="P113" s="3" t="inlineStr"/>
+      <c r="P113" s="4" t="inlineStr"/>
       <c r="Q113" t="inlineStr"/>
-      <c r="R113" s="3" t="inlineStr"/>
+      <c r="R113" s="4" t="inlineStr"/>
       <c r="S113" t="inlineStr"/>
+      <c r="T113" s="4" t="inlineStr"/>
+      <c r="U113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -7159,20 +7723,22 @@
         <v>0</v>
       </c>
       <c r="E114" t="inlineStr"/>
-      <c r="F114" s="3" t="inlineStr"/>
+      <c r="F114" s="4" t="inlineStr"/>
       <c r="G114" t="inlineStr"/>
-      <c r="H114" s="3" t="inlineStr"/>
+      <c r="H114" s="4" t="inlineStr"/>
       <c r="I114" t="inlineStr"/>
-      <c r="J114" s="3" t="inlineStr"/>
+      <c r="J114" s="4" t="inlineStr"/>
       <c r="K114" t="inlineStr"/>
-      <c r="L114" s="3" t="inlineStr"/>
+      <c r="L114" s="4" t="inlineStr"/>
       <c r="M114" t="inlineStr"/>
-      <c r="N114" s="3" t="inlineStr"/>
+      <c r="N114" s="4" t="inlineStr"/>
       <c r="O114" t="inlineStr"/>
-      <c r="P114" s="3" t="inlineStr"/>
+      <c r="P114" s="4" t="inlineStr"/>
       <c r="Q114" t="inlineStr"/>
-      <c r="R114" s="3" t="inlineStr"/>
+      <c r="R114" s="4" t="inlineStr"/>
       <c r="S114" t="inlineStr"/>
+      <c r="T114" s="4" t="inlineStr"/>
+      <c r="U114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -7214,12 +7780,14 @@
       <c r="M115" t="n">
         <v>5699</v>
       </c>
-      <c r="N115" s="3" t="inlineStr"/>
+      <c r="N115" s="4" t="inlineStr"/>
       <c r="O115" t="inlineStr"/>
-      <c r="P115" s="3" t="inlineStr"/>
+      <c r="P115" s="4" t="inlineStr"/>
       <c r="Q115" t="inlineStr"/>
-      <c r="R115" s="3" t="inlineStr"/>
+      <c r="R115" s="4" t="inlineStr"/>
       <c r="S115" t="inlineStr"/>
+      <c r="T115" s="4" t="inlineStr"/>
+      <c r="U115" t="inlineStr"/>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -7276,7 +7844,13 @@
       <c r="R116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S116" t="inlineStr">
+      <c r="S116" t="n">
+        <v>0</v>
+      </c>
+      <c r="T116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7316,14 +7890,16 @@
       <c r="K117" t="n">
         <v>5414</v>
       </c>
-      <c r="L117" s="3" t="inlineStr"/>
+      <c r="L117" s="4" t="inlineStr"/>
       <c r="M117" t="inlineStr"/>
-      <c r="N117" s="3" t="inlineStr"/>
+      <c r="N117" s="4" t="inlineStr"/>
       <c r="O117" t="inlineStr"/>
-      <c r="P117" s="3" t="inlineStr"/>
+      <c r="P117" s="4" t="inlineStr"/>
       <c r="Q117" t="inlineStr"/>
-      <c r="R117" s="3" t="inlineStr"/>
+      <c r="R117" s="4" t="inlineStr"/>
       <c r="S117" t="inlineStr"/>
+      <c r="T117" s="4" t="inlineStr"/>
+      <c r="U117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -7341,13 +7917,13 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F118" s="3" t="n">
+      <c r="F118" s="4" t="n">
         <v>20</v>
       </c>
       <c r="G118" t="n">
         <v>4211</v>
       </c>
-      <c r="H118" s="3" t="n">
+      <c r="H118" s="4" t="n">
         <v>20</v>
       </c>
       <c r="I118" t="n">
@@ -7359,7 +7935,7 @@
       <c r="K118" t="n">
         <v>4366</v>
       </c>
-      <c r="L118" s="4" t="n">
+      <c r="L118" s="3" t="n">
         <v>8</v>
       </c>
       <c r="M118" t="n">
@@ -7380,9 +7956,15 @@
       <c r="R118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S118" t="inlineStr">
-        <is>
-          <t>4468</t>
+      <c r="S118" t="n">
+        <v>4468</v>
+      </c>
+      <c r="T118" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="U118" t="inlineStr">
+        <is>
+          <t>5043</t>
         </is>
       </c>
     </row>
@@ -7441,9 +8023,15 @@
       <c r="R119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S119" t="inlineStr">
-        <is>
-          <t>1578</t>
+      <c r="S119" t="n">
+        <v>1578</v>
+      </c>
+      <c r="T119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U119" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -7463,48 +8051,54 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F120" s="3" t="n">
+      <c r="F120" s="4" t="n">
         <v>21</v>
       </c>
       <c r="G120" t="n">
         <v>1395</v>
       </c>
-      <c r="H120" s="3" t="n">
+      <c r="H120" s="4" t="n">
         <v>20</v>
       </c>
       <c r="I120" t="n">
         <v>1727</v>
       </c>
-      <c r="J120" s="3" t="n">
+      <c r="J120" s="4" t="n">
         <v>20</v>
       </c>
       <c r="K120" t="n">
         <v>2031</v>
       </c>
-      <c r="L120" s="3" t="n">
+      <c r="L120" s="4" t="n">
         <v>20</v>
       </c>
       <c r="M120" t="n">
         <v>2327</v>
       </c>
-      <c r="N120" s="4" t="n">
+      <c r="N120" s="3" t="n">
         <v>3</v>
       </c>
       <c r="O120" t="n">
         <v>2350</v>
       </c>
-      <c r="P120" s="4" t="n">
+      <c r="P120" s="3" t="n">
         <v>8</v>
       </c>
       <c r="Q120" t="n">
         <v>2457</v>
       </c>
-      <c r="R120" s="3" t="n">
+      <c r="R120" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="S120" t="inlineStr">
-        <is>
-          <t>2680</t>
+      <c r="S120" t="n">
+        <v>2680</v>
+      </c>
+      <c r="T120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U120" t="inlineStr">
+        <is>
+          <t>2882</t>
         </is>
       </c>
     </row>
@@ -7530,7 +8124,7 @@
       <c r="G121" t="n">
         <v>1617</v>
       </c>
-      <c r="H121" s="4" t="n">
+      <c r="H121" s="3" t="n">
         <v>7</v>
       </c>
       <c r="I121" t="n">
@@ -7548,7 +8142,7 @@
       <c r="M121" t="n">
         <v>1720</v>
       </c>
-      <c r="N121" s="4" t="n">
+      <c r="N121" s="3" t="n">
         <v>8</v>
       </c>
       <c r="O121" t="n">
@@ -7563,9 +8157,15 @@
       <c r="R121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S121" t="inlineStr">
-        <is>
-          <t>1781</t>
+      <c r="S121" t="n">
+        <v>1781</v>
+      </c>
+      <c r="T121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U121" t="inlineStr">
+        <is>
+          <t>1780</t>
         </is>
       </c>
     </row>
@@ -7624,9 +8224,15 @@
       <c r="R122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S122" t="inlineStr">
-        <is>
-          <t>1989</t>
+      <c r="S122" t="n">
+        <v>1989</v>
+      </c>
+      <c r="T122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U122" t="inlineStr">
+        <is>
+          <t>1983</t>
         </is>
       </c>
     </row>
@@ -7646,7 +8252,7 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F123" s="3" t="inlineStr"/>
+      <c r="F123" s="4" t="inlineStr"/>
       <c r="G123" t="inlineStr"/>
       <c r="H123" s="2" t="n">
         <v>0</v>
@@ -7654,7 +8260,7 @@
       <c r="I123" t="n">
         <v>2612</v>
       </c>
-      <c r="J123" s="4" t="n">
+      <c r="J123" s="3" t="n">
         <v>8</v>
       </c>
       <c r="K123" t="n">
@@ -7681,9 +8287,15 @@
       <c r="R123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="S123" t="inlineStr">
-        <is>
-          <t>2756</t>
+      <c r="S123" t="n">
+        <v>2756</v>
+      </c>
+      <c r="T123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U123" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -7703,40 +8315,46 @@
           <t>一馆</t>
         </is>
       </c>
-      <c r="F124" s="3" t="inlineStr"/>
+      <c r="F124" s="4" t="inlineStr"/>
       <c r="G124" t="inlineStr"/>
-      <c r="H124" s="3" t="inlineStr"/>
+      <c r="H124" s="4" t="inlineStr"/>
       <c r="I124" t="inlineStr"/>
-      <c r="J124" s="3" t="n">
+      <c r="J124" s="4" t="n">
         <v>28</v>
       </c>
       <c r="K124" t="n">
         <v>3992</v>
       </c>
-      <c r="L124" s="3" t="n">
+      <c r="L124" s="4" t="n">
         <v>28</v>
       </c>
       <c r="M124" t="n">
         <v>4117</v>
       </c>
-      <c r="N124" s="3" t="n">
+      <c r="N124" s="4" t="n">
         <v>28</v>
       </c>
       <c r="O124" t="n">
         <v>4175</v>
       </c>
-      <c r="P124" s="3" t="n">
+      <c r="P124" s="4" t="n">
         <v>30</v>
       </c>
       <c r="Q124" t="n">
         <v>4217</v>
       </c>
-      <c r="R124" s="3" t="n">
+      <c r="R124" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="S124" t="inlineStr">
-        <is>
-          <t>4362</t>
+      <c r="S124" t="n">
+        <v>4362</v>
+      </c>
+      <c r="T124" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="U124" t="inlineStr">
+        <is>
+          <t>4461</t>
         </is>
       </c>
     </row>
@@ -7756,17 +8374,17 @@
           <t>三馆</t>
         </is>
       </c>
-      <c r="F125" s="3" t="inlineStr"/>
+      <c r="F125" s="4" t="inlineStr"/>
       <c r="G125" t="inlineStr"/>
-      <c r="H125" s="3" t="inlineStr"/>
+      <c r="H125" s="4" t="inlineStr"/>
       <c r="I125" t="inlineStr"/>
-      <c r="J125" s="3" t="n">
+      <c r="J125" s="4" t="n">
         <v>21</v>
       </c>
       <c r="K125" t="n">
         <v>1534</v>
       </c>
-      <c r="L125" s="3" t="n">
+      <c r="L125" s="4" t="n">
         <v>20</v>
       </c>
       <c r="M125" t="n">
@@ -7778,18 +8396,24 @@
       <c r="O125" t="n">
         <v>1819</v>
       </c>
-      <c r="P125" s="4" t="n">
+      <c r="P125" s="3" t="n">
         <v>8</v>
       </c>
       <c r="Q125" t="n">
         <v>1868</v>
       </c>
-      <c r="R125" s="4" t="n">
+      <c r="R125" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="S125" t="inlineStr">
-        <is>
-          <t>1978</t>
+      <c r="S125" t="n">
+        <v>1978</v>
+      </c>
+      <c r="T125" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="U125" t="inlineStr">
+        <is>
+          <t>2044</t>
         </is>
       </c>
     </row>
@@ -7809,28 +8433,34 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F126" s="3" t="inlineStr"/>
+      <c r="F126" s="4" t="inlineStr"/>
       <c r="G126" t="inlineStr"/>
-      <c r="H126" s="3" t="inlineStr"/>
+      <c r="H126" s="4" t="inlineStr"/>
       <c r="I126" t="inlineStr"/>
-      <c r="J126" s="3" t="inlineStr"/>
+      <c r="J126" s="4" t="inlineStr"/>
       <c r="K126" t="inlineStr"/>
-      <c r="L126" s="3" t="inlineStr"/>
+      <c r="L126" s="4" t="inlineStr"/>
       <c r="M126" t="inlineStr"/>
-      <c r="N126" s="3" t="inlineStr"/>
+      <c r="N126" s="4" t="inlineStr"/>
       <c r="O126" t="inlineStr"/>
-      <c r="P126" s="3" t="n">
+      <c r="P126" s="4" t="n">
         <v>21</v>
       </c>
       <c r="Q126" t="n">
         <v>1344</v>
       </c>
-      <c r="R126" s="4" t="n">
+      <c r="R126" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="S126" t="inlineStr">
-        <is>
-          <t>1452</t>
+      <c r="S126" t="n">
+        <v>1452</v>
+      </c>
+      <c r="T126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U126" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -7850,24 +8480,153 @@
           <t>总馆</t>
         </is>
       </c>
-      <c r="F127" s="3" t="inlineStr"/>
+      <c r="F127" s="4" t="inlineStr"/>
       <c r="G127" t="inlineStr"/>
-      <c r="H127" s="3" t="inlineStr"/>
+      <c r="H127" s="4" t="inlineStr"/>
       <c r="I127" t="inlineStr"/>
-      <c r="J127" s="3" t="inlineStr"/>
+      <c r="J127" s="4" t="inlineStr"/>
       <c r="K127" t="inlineStr"/>
-      <c r="L127" s="3" t="inlineStr"/>
+      <c r="L127" s="4" t="inlineStr"/>
       <c r="M127" t="inlineStr"/>
-      <c r="N127" s="3" t="inlineStr"/>
+      <c r="N127" s="4" t="inlineStr"/>
       <c r="O127" t="inlineStr"/>
-      <c r="P127" s="3" t="inlineStr"/>
+      <c r="P127" s="4" t="inlineStr"/>
       <c r="Q127" t="inlineStr"/>
-      <c r="R127" s="3" t="n">
+      <c r="R127" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="S127" t="inlineStr">
-        <is>
-          <t>1387</t>
+      <c r="S127" t="n">
+        <v>1387</v>
+      </c>
+      <c r="T127" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="U127" t="inlineStr">
+        <is>
+          <t>1566</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>52547954</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Tài</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr"/>
+      <c r="D128" t="inlineStr"/>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F128" s="4" t="inlineStr"/>
+      <c r="G128" t="inlineStr"/>
+      <c r="H128" s="4" t="inlineStr"/>
+      <c r="I128" t="inlineStr"/>
+      <c r="J128" s="4" t="inlineStr"/>
+      <c r="K128" t="inlineStr"/>
+      <c r="L128" s="4" t="inlineStr"/>
+      <c r="M128" t="inlineStr"/>
+      <c r="N128" s="4" t="inlineStr"/>
+      <c r="O128" t="inlineStr"/>
+      <c r="P128" s="4" t="inlineStr"/>
+      <c r="Q128" t="inlineStr"/>
+      <c r="R128" s="4" t="inlineStr"/>
+      <c r="S128" t="inlineStr"/>
+      <c r="T128" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="U128" t="inlineStr">
+        <is>
+          <t>1522</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>52626466</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>刊得夫因缺斯汀</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr"/>
+      <c r="D129" t="inlineStr"/>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F129" s="4" t="inlineStr"/>
+      <c r="G129" t="inlineStr"/>
+      <c r="H129" s="4" t="inlineStr"/>
+      <c r="I129" t="inlineStr"/>
+      <c r="J129" s="4" t="inlineStr"/>
+      <c r="K129" t="inlineStr"/>
+      <c r="L129" s="4" t="inlineStr"/>
+      <c r="M129" t="inlineStr"/>
+      <c r="N129" s="4" t="inlineStr"/>
+      <c r="O129" t="inlineStr"/>
+      <c r="P129" s="4" t="inlineStr"/>
+      <c r="Q129" t="inlineStr"/>
+      <c r="R129" s="4" t="inlineStr"/>
+      <c r="S129" t="inlineStr"/>
+      <c r="T129" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="U129" t="inlineStr">
+        <is>
+          <t>2739</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>58975056</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>tejas</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr"/>
+      <c r="D130" t="inlineStr"/>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F130" s="4" t="inlineStr"/>
+      <c r="G130" t="inlineStr"/>
+      <c r="H130" s="4" t="inlineStr"/>
+      <c r="I130" t="inlineStr"/>
+      <c r="J130" s="4" t="inlineStr"/>
+      <c r="K130" t="inlineStr"/>
+      <c r="L130" s="4" t="inlineStr"/>
+      <c r="M130" t="inlineStr"/>
+      <c r="N130" s="4" t="inlineStr"/>
+      <c r="O130" t="inlineStr"/>
+      <c r="P130" s="4" t="inlineStr"/>
+      <c r="Q130" t="inlineStr"/>
+      <c r="R130" s="4" t="inlineStr"/>
+      <c r="S130" t="inlineStr"/>
+      <c r="T130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U130" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-22 11:30:55
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U130"/>
+  <dimension ref="A1:W131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,6 +496,16 @@
           <t>05-20_0</t>
         </is>
       </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>05-21_A</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>05-21_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -564,9 +574,15 @@
       <c r="T2" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>2918</t>
+      <c r="U2" t="n">
+        <v>2918</v>
+      </c>
+      <c r="V2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -637,7 +653,13 @@
       <c r="T3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U3" t="inlineStr">
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -710,7 +732,13 @@
       <c r="T4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U4" t="inlineStr">
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -783,9 +811,15 @@
       <c r="T5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>2638</t>
+      <c r="U5" t="n">
+        <v>2638</v>
+      </c>
+      <c r="V5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>2544</t>
         </is>
       </c>
     </row>
@@ -856,9 +890,15 @@
       <c r="T6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>2628</t>
+      <c r="U6" t="n">
+        <v>2628</v>
+      </c>
+      <c r="V6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -896,6 +936,8 @@
       <c r="S7" t="inlineStr"/>
       <c r="T7" s="4" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
+      <c r="V7" s="4" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -931,6 +973,8 @@
       <c r="S8" t="inlineStr"/>
       <c r="T8" s="4" t="inlineStr"/>
       <c r="U8" t="inlineStr"/>
+      <c r="V8" s="4" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -966,6 +1010,8 @@
       <c r="S9" t="inlineStr"/>
       <c r="T9" s="4" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
+      <c r="V9" s="4" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1001,6 +1047,8 @@
       <c r="S10" t="inlineStr"/>
       <c r="T10" s="4" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
+      <c r="V10" s="4" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1036,6 +1084,8 @@
       <c r="S11" t="inlineStr"/>
       <c r="T11" s="4" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
+      <c r="V11" s="4" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1071,6 +1121,8 @@
       <c r="S12" t="inlineStr"/>
       <c r="T12" s="4" t="inlineStr"/>
       <c r="U12" t="inlineStr"/>
+      <c r="V12" s="4" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1106,6 +1158,8 @@
       <c r="S13" t="inlineStr"/>
       <c r="T13" s="4" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
+      <c r="V13" s="4" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1141,6 +1195,8 @@
       <c r="S14" t="inlineStr"/>
       <c r="T14" s="4" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
+      <c r="V14" s="4" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1176,6 +1232,8 @@
       <c r="S15" t="inlineStr"/>
       <c r="T15" s="4" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
+      <c r="V15" s="4" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1211,6 +1269,8 @@
       <c r="S16" t="inlineStr"/>
       <c r="T16" s="4" t="inlineStr"/>
       <c r="U16" t="inlineStr"/>
+      <c r="V16" s="4" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1246,6 +1306,8 @@
       <c r="S17" t="inlineStr"/>
       <c r="T17" s="4" t="inlineStr"/>
       <c r="U17" t="inlineStr"/>
+      <c r="V17" s="4" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1314,9 +1376,15 @@
       <c r="T18" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="U18" t="inlineStr">
-        <is>
-          <t>4240</t>
+      <c r="U18" t="n">
+        <v>4240</v>
+      </c>
+      <c r="V18" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>2503</t>
         </is>
       </c>
     </row>
@@ -1387,9 +1455,15 @@
       <c r="T19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U19" t="inlineStr">
-        <is>
-          <t>2875</t>
+      <c r="U19" t="n">
+        <v>2875</v>
+      </c>
+      <c r="V19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -1460,9 +1534,15 @@
       <c r="T20" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="U20" t="inlineStr">
-        <is>
-          <t>4648</t>
+      <c r="U20" t="n">
+        <v>4648</v>
+      </c>
+      <c r="V20" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>2692</t>
         </is>
       </c>
     </row>
@@ -1533,9 +1613,15 @@
       <c r="T21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U21" t="inlineStr">
-        <is>
-          <t>5198</t>
+      <c r="U21" t="n">
+        <v>5198</v>
+      </c>
+      <c r="V21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>2554</t>
         </is>
       </c>
     </row>
@@ -1606,9 +1692,15 @@
       <c r="T22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="U22" t="inlineStr">
-        <is>
-          <t>5508</t>
+      <c r="U22" t="n">
+        <v>5508</v>
+      </c>
+      <c r="V22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>2813</t>
         </is>
       </c>
     </row>
@@ -1679,9 +1771,15 @@
       <c r="T23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="U23" t="inlineStr">
-        <is>
-          <t>6206</t>
+      <c r="U23" t="n">
+        <v>6206</v>
+      </c>
+      <c r="V23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>2943</t>
         </is>
       </c>
     </row>
@@ -1752,9 +1850,15 @@
       <c r="T24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="U24" t="inlineStr">
-        <is>
-          <t>5643</t>
+      <c r="U24" t="n">
+        <v>5643</v>
+      </c>
+      <c r="V24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>3014</t>
         </is>
       </c>
     </row>
@@ -1825,9 +1929,15 @@
       <c r="T25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U25" t="inlineStr">
-        <is>
-          <t>5827</t>
+      <c r="U25" t="n">
+        <v>5827</v>
+      </c>
+      <c r="V25" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -1898,9 +2008,15 @@
       <c r="T26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U26" t="inlineStr">
-        <is>
-          <t>2594</t>
+      <c r="U26" t="n">
+        <v>2594</v>
+      </c>
+      <c r="V26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1971,7 +2087,13 @@
       <c r="T27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U27" t="inlineStr">
+      <c r="U27" t="n">
+        <v>0</v>
+      </c>
+      <c r="V27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2011,6 +2133,8 @@
       <c r="S28" t="inlineStr"/>
       <c r="T28" s="4" t="inlineStr"/>
       <c r="U28" t="inlineStr"/>
+      <c r="V28" s="4" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2079,9 +2203,15 @@
       <c r="T29" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="U29" t="inlineStr">
-        <is>
-          <t>5026</t>
+      <c r="U29" t="n">
+        <v>5026</v>
+      </c>
+      <c r="V29" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>2799</t>
         </is>
       </c>
     </row>
@@ -2152,9 +2282,15 @@
       <c r="T30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U30" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="U30" t="n">
+        <v>0</v>
+      </c>
+      <c r="V30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -2225,9 +2361,15 @@
       <c r="T31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="U31" t="inlineStr">
-        <is>
-          <t>5496</t>
+      <c r="U31" t="n">
+        <v>5496</v>
+      </c>
+      <c r="V31" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>2960</t>
         </is>
       </c>
     </row>
@@ -2298,9 +2440,15 @@
       <c r="T32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U32" t="inlineStr">
-        <is>
-          <t>4618</t>
+      <c r="U32" t="n">
+        <v>4618</v>
+      </c>
+      <c r="V32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>2516</t>
         </is>
       </c>
     </row>
@@ -2338,6 +2486,8 @@
       <c r="S33" t="inlineStr"/>
       <c r="T33" s="4" t="inlineStr"/>
       <c r="U33" t="inlineStr"/>
+      <c r="V33" s="4" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2406,7 +2556,13 @@
       <c r="T34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U34" t="inlineStr">
+      <c r="U34" t="n">
+        <v>0</v>
+      </c>
+      <c r="V34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2479,7 +2635,13 @@
       <c r="T35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U35" t="inlineStr">
+      <c r="U35" t="n">
+        <v>0</v>
+      </c>
+      <c r="V35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W35" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2552,9 +2714,15 @@
       <c r="T36" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="U36" t="inlineStr">
-        <is>
-          <t>4585</t>
+      <c r="U36" t="n">
+        <v>4585</v>
+      </c>
+      <c r="V36" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>2793</t>
         </is>
       </c>
     </row>
@@ -2625,9 +2793,15 @@
       <c r="T37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="U37" t="inlineStr">
-        <is>
-          <t>5224</t>
+      <c r="U37" t="n">
+        <v>5224</v>
+      </c>
+      <c r="V37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>2940</t>
         </is>
       </c>
     </row>
@@ -2698,9 +2872,15 @@
       <c r="T38" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="U38" t="inlineStr">
-        <is>
-          <t>6080</t>
+      <c r="U38" t="n">
+        <v>6080</v>
+      </c>
+      <c r="V38" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>3003</t>
         </is>
       </c>
     </row>
@@ -2771,9 +2951,15 @@
       <c r="T39" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="U39" t="inlineStr">
-        <is>
-          <t>5024</t>
+      <c r="U39" t="n">
+        <v>5024</v>
+      </c>
+      <c r="V39" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>2866</t>
         </is>
       </c>
     </row>
@@ -2844,7 +3030,13 @@
       <c r="T40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U40" t="inlineStr">
+      <c r="U40" t="n">
+        <v>0</v>
+      </c>
+      <c r="V40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2917,9 +3109,15 @@
       <c r="T41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U41" t="inlineStr">
-        <is>
-          <t>4606</t>
+      <c r="U41" t="n">
+        <v>4606</v>
+      </c>
+      <c r="V41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W41" t="inlineStr">
+        <is>
+          <t>2498</t>
         </is>
       </c>
     </row>
@@ -2990,9 +3188,15 @@
       <c r="T42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U42" t="inlineStr">
-        <is>
-          <t>3429</t>
+      <c r="U42" t="n">
+        <v>3429</v>
+      </c>
+      <c r="V42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3030,6 +3234,8 @@
       <c r="S43" t="inlineStr"/>
       <c r="T43" s="4" t="inlineStr"/>
       <c r="U43" t="inlineStr"/>
+      <c r="V43" s="4" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3065,6 +3271,8 @@
       <c r="S44" t="inlineStr"/>
       <c r="T44" s="4" t="inlineStr"/>
       <c r="U44" t="inlineStr"/>
+      <c r="V44" s="4" t="inlineStr"/>
+      <c r="W44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3132,6 +3340,8 @@
       </c>
       <c r="T45" s="4" t="inlineStr"/>
       <c r="U45" t="inlineStr"/>
+      <c r="V45" s="4" t="inlineStr"/>
+      <c r="W45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -3200,9 +3410,15 @@
       <c r="T46" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="U46" t="inlineStr">
-        <is>
-          <t>4769</t>
+      <c r="U46" t="n">
+        <v>4769</v>
+      </c>
+      <c r="V46" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="W46" t="inlineStr">
+        <is>
+          <t>2664</t>
         </is>
       </c>
     </row>
@@ -3273,9 +3489,15 @@
       <c r="T47" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="U47" t="inlineStr">
-        <is>
-          <t>6040</t>
+      <c r="U47" t="n">
+        <v>6040</v>
+      </c>
+      <c r="V47" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="W47" t="inlineStr">
+        <is>
+          <t>2970</t>
         </is>
       </c>
     </row>
@@ -3346,9 +3568,15 @@
       <c r="T48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U48" t="inlineStr">
-        <is>
-          <t>5138</t>
+      <c r="U48" t="n">
+        <v>5138</v>
+      </c>
+      <c r="V48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W48" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3419,9 +3647,15 @@
       <c r="T49" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="U49" t="inlineStr">
-        <is>
-          <t>5242</t>
+      <c r="U49" t="n">
+        <v>5242</v>
+      </c>
+      <c r="V49" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="W49" t="inlineStr">
+        <is>
+          <t>2982</t>
         </is>
       </c>
     </row>
@@ -3492,9 +3726,15 @@
       <c r="T50" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="U50" t="inlineStr">
-        <is>
-          <t>5616</t>
+      <c r="U50" t="n">
+        <v>5616</v>
+      </c>
+      <c r="V50" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="W50" t="inlineStr">
+        <is>
+          <t>2973</t>
         </is>
       </c>
     </row>
@@ -3564,6 +3804,8 @@
       </c>
       <c r="T51" s="4" t="inlineStr"/>
       <c r="U51" t="inlineStr"/>
+      <c r="V51" s="4" t="inlineStr"/>
+      <c r="W51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -3632,9 +3874,15 @@
       <c r="T52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="U52" t="inlineStr">
-        <is>
-          <t>5743</t>
+      <c r="U52" t="n">
+        <v>5743</v>
+      </c>
+      <c r="V52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="W52" t="inlineStr">
+        <is>
+          <t>3028</t>
         </is>
       </c>
     </row>
@@ -3705,9 +3953,15 @@
       <c r="T53" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="U53" t="inlineStr">
-        <is>
-          <t>4519</t>
+      <c r="U53" t="n">
+        <v>4519</v>
+      </c>
+      <c r="V53" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="W53" t="inlineStr">
+        <is>
+          <t>2689</t>
         </is>
       </c>
     </row>
@@ -3777,6 +4031,8 @@
       </c>
       <c r="T54" s="4" t="inlineStr"/>
       <c r="U54" t="inlineStr"/>
+      <c r="V54" s="4" t="inlineStr"/>
+      <c r="W54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -3845,9 +4101,15 @@
       <c r="T55" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="U55" t="inlineStr">
-        <is>
-          <t>4822</t>
+      <c r="U55" t="n">
+        <v>4822</v>
+      </c>
+      <c r="V55" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="W55" t="inlineStr">
+        <is>
+          <t>2555</t>
         </is>
       </c>
     </row>
@@ -3918,9 +4180,15 @@
       <c r="T56" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="U56" t="inlineStr">
-        <is>
-          <t>5995</t>
+      <c r="U56" t="n">
+        <v>5995</v>
+      </c>
+      <c r="V56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="W56" t="inlineStr">
+        <is>
+          <t>3091</t>
         </is>
       </c>
     </row>
@@ -3991,9 +4259,15 @@
       <c r="T57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="U57" t="inlineStr">
-        <is>
-          <t>4513</t>
+      <c r="U57" t="n">
+        <v>4513</v>
+      </c>
+      <c r="V57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="W57" t="inlineStr">
+        <is>
+          <t>2766</t>
         </is>
       </c>
     </row>
@@ -4064,9 +4338,15 @@
       <c r="T58" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="U58" t="inlineStr">
-        <is>
-          <t>4498</t>
+      <c r="U58" t="n">
+        <v>4498</v>
+      </c>
+      <c r="V58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="W58" t="inlineStr">
+        <is>
+          <t>2890</t>
         </is>
       </c>
     </row>
@@ -4137,9 +4417,15 @@
       <c r="T59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="U59" t="inlineStr">
-        <is>
-          <t>4484</t>
+      <c r="U59" t="n">
+        <v>4484</v>
+      </c>
+      <c r="V59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="W59" t="inlineStr">
+        <is>
+          <t>2769</t>
         </is>
       </c>
     </row>
@@ -4210,9 +4496,15 @@
       <c r="T60" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="U60" t="inlineStr">
-        <is>
-          <t>4692</t>
+      <c r="U60" t="n">
+        <v>4692</v>
+      </c>
+      <c r="V60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="W60" t="inlineStr">
+        <is>
+          <t>3003</t>
         </is>
       </c>
     </row>
@@ -4250,6 +4542,8 @@
       <c r="S61" t="inlineStr"/>
       <c r="T61" s="4" t="inlineStr"/>
       <c r="U61" t="inlineStr"/>
+      <c r="V61" s="4" t="inlineStr"/>
+      <c r="W61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -4318,9 +4612,15 @@
       <c r="T62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="U62" t="inlineStr">
-        <is>
-          <t>4260</t>
+      <c r="U62" t="n">
+        <v>4260</v>
+      </c>
+      <c r="V62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="W62" t="inlineStr">
+        <is>
+          <t>2807</t>
         </is>
       </c>
     </row>
@@ -4391,9 +4691,15 @@
       <c r="T63" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="U63" t="inlineStr">
-        <is>
-          <t>4264</t>
+      <c r="U63" t="n">
+        <v>4264</v>
+      </c>
+      <c r="V63" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="W63" t="inlineStr">
+        <is>
+          <t>2835</t>
         </is>
       </c>
     </row>
@@ -4464,9 +4770,15 @@
       <c r="T64" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="U64" t="inlineStr">
-        <is>
-          <t>4548</t>
+      <c r="U64" t="n">
+        <v>4548</v>
+      </c>
+      <c r="V64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="W64" t="inlineStr">
+        <is>
+          <t>2856</t>
         </is>
       </c>
     </row>
@@ -4537,9 +4849,15 @@
       <c r="T65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U65" t="inlineStr">
-        <is>
-          <t>2770</t>
+      <c r="U65" t="n">
+        <v>2770</v>
+      </c>
+      <c r="V65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W65" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4610,7 +4928,13 @@
       <c r="T66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U66" t="inlineStr">
+      <c r="U66" t="n">
+        <v>0</v>
+      </c>
+      <c r="V66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4683,7 +5007,13 @@
       <c r="T67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U67" t="inlineStr">
+      <c r="U67" t="n">
+        <v>0</v>
+      </c>
+      <c r="V67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4756,7 +5086,13 @@
       <c r="T68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U68" t="inlineStr">
+      <c r="U68" t="n">
+        <v>0</v>
+      </c>
+      <c r="V68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4796,6 +5132,8 @@
       <c r="S69" t="inlineStr"/>
       <c r="T69" s="4" t="inlineStr"/>
       <c r="U69" t="inlineStr"/>
+      <c r="V69" s="4" t="inlineStr"/>
+      <c r="W69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -4864,7 +5202,13 @@
       <c r="T70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U70" t="inlineStr">
+      <c r="U70" t="n">
+        <v>0</v>
+      </c>
+      <c r="V70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4937,7 +5281,13 @@
       <c r="T71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U71" t="inlineStr">
+      <c r="U71" t="n">
+        <v>0</v>
+      </c>
+      <c r="V71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5010,7 +5360,13 @@
       <c r="T72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U72" t="inlineStr">
+      <c r="U72" t="n">
+        <v>0</v>
+      </c>
+      <c r="V72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5083,9 +5439,15 @@
       <c r="T73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U73" t="inlineStr">
-        <is>
-          <t>2887</t>
+      <c r="U73" t="n">
+        <v>2887</v>
+      </c>
+      <c r="V73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W73" t="inlineStr">
+        <is>
+          <t>2493</t>
         </is>
       </c>
     </row>
@@ -5156,9 +5518,15 @@
       <c r="T74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U74" t="inlineStr">
-        <is>
-          <t>2624</t>
+      <c r="U74" t="n">
+        <v>2624</v>
+      </c>
+      <c r="V74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W74" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5229,7 +5597,13 @@
       <c r="T75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U75" t="inlineStr">
+      <c r="U75" t="n">
+        <v>0</v>
+      </c>
+      <c r="V75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5302,9 +5676,15 @@
       <c r="T76" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="U76" t="inlineStr">
-        <is>
-          <t>4247</t>
+      <c r="U76" t="n">
+        <v>4247</v>
+      </c>
+      <c r="V76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W76" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -5375,9 +5755,15 @@
       <c r="T77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U77" t="inlineStr">
-        <is>
-          <t>3426</t>
+      <c r="U77" t="n">
+        <v>3426</v>
+      </c>
+      <c r="V77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W77" t="inlineStr">
+        <is>
+          <t>2517</t>
         </is>
       </c>
     </row>
@@ -5448,7 +5834,13 @@
       <c r="T78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U78" t="inlineStr">
+      <c r="U78" t="n">
+        <v>0</v>
+      </c>
+      <c r="V78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5521,9 +5913,15 @@
       <c r="T79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U79" t="inlineStr">
-        <is>
-          <t>1341</t>
+      <c r="U79" t="n">
+        <v>1341</v>
+      </c>
+      <c r="V79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W79" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5594,7 +5992,13 @@
       <c r="T80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U80" t="inlineStr">
+      <c r="U80" t="n">
+        <v>0</v>
+      </c>
+      <c r="V80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5667,7 +6071,13 @@
       <c r="T81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U81" t="inlineStr">
+      <c r="U81" t="n">
+        <v>0</v>
+      </c>
+      <c r="V81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5740,7 +6150,13 @@
       <c r="T82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U82" t="inlineStr">
+      <c r="U82" t="n">
+        <v>0</v>
+      </c>
+      <c r="V82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5813,9 +6229,15 @@
       <c r="T83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U83" t="inlineStr">
-        <is>
-          <t>2735</t>
+      <c r="U83" t="n">
+        <v>2735</v>
+      </c>
+      <c r="V83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W83" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5886,9 +6308,15 @@
       <c r="T84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U84" t="inlineStr">
-        <is>
-          <t>1428</t>
+      <c r="U84" t="n">
+        <v>1428</v>
+      </c>
+      <c r="V84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W84" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -5959,7 +6387,13 @@
       <c r="T85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U85" t="inlineStr">
+      <c r="U85" t="n">
+        <v>0</v>
+      </c>
+      <c r="V85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6032,7 +6466,13 @@
       <c r="T86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U86" t="inlineStr">
+      <c r="U86" t="n">
+        <v>0</v>
+      </c>
+      <c r="V86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6105,7 +6545,13 @@
       <c r="T87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U87" t="inlineStr">
+      <c r="U87" t="n">
+        <v>0</v>
+      </c>
+      <c r="V87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6178,7 +6624,13 @@
       <c r="T88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U88" t="inlineStr">
+      <c r="U88" t="n">
+        <v>0</v>
+      </c>
+      <c r="V88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6251,7 +6703,13 @@
       <c r="T89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U89" t="inlineStr">
+      <c r="U89" t="n">
+        <v>0</v>
+      </c>
+      <c r="V89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6324,7 +6782,13 @@
       <c r="T90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U90" t="inlineStr">
+      <c r="U90" t="n">
+        <v>0</v>
+      </c>
+      <c r="V90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6397,7 +6861,13 @@
       <c r="T91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U91" t="inlineStr">
+      <c r="U91" t="n">
+        <v>0</v>
+      </c>
+      <c r="V91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6470,7 +6940,13 @@
       <c r="T92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U92" t="inlineStr">
+      <c r="U92" t="n">
+        <v>0</v>
+      </c>
+      <c r="V92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6543,7 +7019,13 @@
       <c r="T93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U93" t="inlineStr">
+      <c r="U93" t="n">
+        <v>0</v>
+      </c>
+      <c r="V93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6616,7 +7098,13 @@
       <c r="T94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U94" t="inlineStr">
+      <c r="U94" t="n">
+        <v>0</v>
+      </c>
+      <c r="V94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6689,7 +7177,13 @@
       <c r="T95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U95" t="inlineStr">
+      <c r="U95" t="n">
+        <v>0</v>
+      </c>
+      <c r="V95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6762,9 +7256,15 @@
       <c r="T96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U96" t="inlineStr">
-        <is>
-          <t>3566</t>
+      <c r="U96" t="n">
+        <v>3566</v>
+      </c>
+      <c r="V96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W96" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -6835,7 +7335,13 @@
       <c r="T97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U97" t="inlineStr">
+      <c r="U97" t="n">
+        <v>0</v>
+      </c>
+      <c r="V97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6908,7 +7414,13 @@
       <c r="T98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U98" t="inlineStr">
+      <c r="U98" t="n">
+        <v>0</v>
+      </c>
+      <c r="V98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6981,7 +7493,13 @@
       <c r="T99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U99" t="inlineStr">
+      <c r="U99" t="n">
+        <v>0</v>
+      </c>
+      <c r="V99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7054,7 +7572,13 @@
       <c r="T100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U100" t="inlineStr">
+      <c r="U100" t="n">
+        <v>0</v>
+      </c>
+      <c r="V100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7127,7 +7651,13 @@
       <c r="T101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U101" t="inlineStr">
+      <c r="U101" t="n">
+        <v>0</v>
+      </c>
+      <c r="V101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7200,7 +7730,13 @@
       <c r="T102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U102" t="inlineStr">
+      <c r="U102" t="n">
+        <v>0</v>
+      </c>
+      <c r="V102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7273,7 +7809,13 @@
       <c r="T103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U103" t="inlineStr">
+      <c r="U103" t="n">
+        <v>0</v>
+      </c>
+      <c r="V103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7346,7 +7888,13 @@
       <c r="T104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U104" t="inlineStr">
+      <c r="U104" t="n">
+        <v>0</v>
+      </c>
+      <c r="V104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7419,7 +7967,13 @@
       <c r="T105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U105" t="inlineStr">
+      <c r="U105" t="n">
+        <v>0</v>
+      </c>
+      <c r="V105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7459,6 +8013,8 @@
       <c r="S106" t="inlineStr"/>
       <c r="T106" s="4" t="inlineStr"/>
       <c r="U106" t="inlineStr"/>
+      <c r="V106" s="4" t="inlineStr"/>
+      <c r="W106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -7494,6 +8050,8 @@
       <c r="S107" t="inlineStr"/>
       <c r="T107" s="4" t="inlineStr"/>
       <c r="U107" t="inlineStr"/>
+      <c r="V107" s="4" t="inlineStr"/>
+      <c r="W107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -7529,6 +8087,8 @@
       <c r="S108" t="inlineStr"/>
       <c r="T108" s="4" t="inlineStr"/>
       <c r="U108" t="inlineStr"/>
+      <c r="V108" s="4" t="inlineStr"/>
+      <c r="W108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -7564,6 +8124,8 @@
       <c r="S109" t="inlineStr"/>
       <c r="T109" s="4" t="inlineStr"/>
       <c r="U109" t="inlineStr"/>
+      <c r="V109" s="4" t="inlineStr"/>
+      <c r="W109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -7599,6 +8161,8 @@
       <c r="S110" t="inlineStr"/>
       <c r="T110" s="4" t="inlineStr"/>
       <c r="U110" t="inlineStr"/>
+      <c r="V110" s="4" t="inlineStr"/>
+      <c r="W110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -7634,6 +8198,8 @@
       <c r="S111" t="inlineStr"/>
       <c r="T111" s="4" t="inlineStr"/>
       <c r="U111" t="inlineStr"/>
+      <c r="V111" s="4" t="inlineStr"/>
+      <c r="W111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -7669,6 +8235,8 @@
       <c r="S112" t="inlineStr"/>
       <c r="T112" s="4" t="inlineStr"/>
       <c r="U112" t="inlineStr"/>
+      <c r="V112" s="4" t="inlineStr"/>
+      <c r="W112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -7704,6 +8272,8 @@
       <c r="S113" t="inlineStr"/>
       <c r="T113" s="4" t="inlineStr"/>
       <c r="U113" t="inlineStr"/>
+      <c r="V113" s="4" t="inlineStr"/>
+      <c r="W113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -7739,6 +8309,8 @@
       <c r="S114" t="inlineStr"/>
       <c r="T114" s="4" t="inlineStr"/>
       <c r="U114" t="inlineStr"/>
+      <c r="V114" s="4" t="inlineStr"/>
+      <c r="W114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -7788,6 +8360,14 @@
       <c r="S115" t="inlineStr"/>
       <c r="T115" s="4" t="inlineStr"/>
       <c r="U115" t="inlineStr"/>
+      <c r="V115" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="W115" t="inlineStr">
+        <is>
+          <t>2939</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -7850,7 +8430,13 @@
       <c r="T116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U116" t="inlineStr">
+      <c r="U116" t="n">
+        <v>0</v>
+      </c>
+      <c r="V116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7862,7 +8448,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Ze5kyphyr</t>
+          <t>"Zephyr-5ky zgx"</t>
         </is>
       </c>
       <c r="C117" t="inlineStr"/>
@@ -7900,6 +8486,14 @@
       <c r="S117" t="inlineStr"/>
       <c r="T117" s="4" t="inlineStr"/>
       <c r="U117" t="inlineStr"/>
+      <c r="V117" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="W117" t="inlineStr">
+        <is>
+          <t>3157</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -7962,9 +8556,15 @@
       <c r="T118" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="U118" t="inlineStr">
-        <is>
-          <t>5043</t>
+      <c r="U118" t="n">
+        <v>5043</v>
+      </c>
+      <c r="V118" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="W118" t="inlineStr">
+        <is>
+          <t>2823</t>
         </is>
       </c>
     </row>
@@ -8029,7 +8629,13 @@
       <c r="T119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U119" t="inlineStr">
+      <c r="U119" t="n">
+        <v>0</v>
+      </c>
+      <c r="V119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W119" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8096,9 +8702,15 @@
       <c r="T120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U120" t="inlineStr">
-        <is>
-          <t>2882</t>
+      <c r="U120" t="n">
+        <v>2882</v>
+      </c>
+      <c r="V120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W120" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -8163,9 +8775,15 @@
       <c r="T121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U121" t="inlineStr">
-        <is>
-          <t>1780</t>
+      <c r="U121" t="n">
+        <v>1780</v>
+      </c>
+      <c r="V121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W121" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -8230,9 +8848,15 @@
       <c r="T122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U122" t="inlineStr">
-        <is>
-          <t>1983</t>
+      <c r="U122" t="n">
+        <v>1983</v>
+      </c>
+      <c r="V122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W122" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -8293,9 +8917,15 @@
       <c r="T123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U123" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="U123" t="n">
+        <v>0</v>
+      </c>
+      <c r="V123" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="W123" t="inlineStr">
+        <is>
+          <t>2664</t>
         </is>
       </c>
     </row>
@@ -8352,9 +8982,15 @@
       <c r="T124" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="U124" t="inlineStr">
-        <is>
-          <t>4461</t>
+      <c r="U124" t="n">
+        <v>4461</v>
+      </c>
+      <c r="V124" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="W124" t="inlineStr">
+        <is>
+          <t>2766</t>
         </is>
       </c>
     </row>
@@ -8411,9 +9047,15 @@
       <c r="T125" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="U125" t="inlineStr">
-        <is>
-          <t>2044</t>
+      <c r="U125" t="n">
+        <v>2044</v>
+      </c>
+      <c r="V125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W125" t="inlineStr">
+        <is>
+          <t>2000</t>
         </is>
       </c>
     </row>
@@ -8458,9 +9100,15 @@
       <c r="T126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U126" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="U126" t="n">
+        <v>0</v>
+      </c>
+      <c r="V126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W126" t="inlineStr">
+        <is>
+          <t>1500</t>
         </is>
       </c>
     </row>
@@ -8501,17 +9149,21 @@
       <c r="T127" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="U127" t="inlineStr">
-        <is>
-          <t>1566</t>
+      <c r="U127" t="n">
+        <v>1566</v>
+      </c>
+      <c r="V127" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="W127" t="inlineStr">
+        <is>
+          <t>1490</t>
         </is>
       </c>
     </row>
     <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>52547954</t>
-        </is>
+      <c r="A128" t="n">
+        <v>52547954</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
@@ -8542,17 +9194,21 @@
       <c r="T128" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="U128" t="inlineStr">
-        <is>
-          <t>1522</t>
+      <c r="U128" t="n">
+        <v>1522</v>
+      </c>
+      <c r="V128" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="W128" t="inlineStr">
+        <is>
+          <t>2214</t>
         </is>
       </c>
     </row>
     <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>52626466</t>
-        </is>
+      <c r="A129" t="n">
+        <v>52626466</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
@@ -8583,17 +9239,21 @@
       <c r="T129" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="U129" t="inlineStr">
-        <is>
-          <t>2739</t>
+      <c r="U129" t="n">
+        <v>2739</v>
+      </c>
+      <c r="V129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W129" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
     <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>58975056</t>
-        </is>
+      <c r="A130" t="n">
+        <v>58975056</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
@@ -8624,9 +9284,58 @@
       <c r="T130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="U130" t="inlineStr">
+      <c r="U130" t="n">
+        <v>0</v>
+      </c>
+      <c r="V130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W130" t="inlineStr">
         <is>
           <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>47928278</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>垃圾游戏草</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr"/>
+      <c r="D131" t="inlineStr"/>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F131" s="4" t="inlineStr"/>
+      <c r="G131" t="inlineStr"/>
+      <c r="H131" s="4" t="inlineStr"/>
+      <c r="I131" t="inlineStr"/>
+      <c r="J131" s="4" t="inlineStr"/>
+      <c r="K131" t="inlineStr"/>
+      <c r="L131" s="4" t="inlineStr"/>
+      <c r="M131" t="inlineStr"/>
+      <c r="N131" s="4" t="inlineStr"/>
+      <c r="O131" t="inlineStr"/>
+      <c r="P131" s="4" t="inlineStr"/>
+      <c r="Q131" t="inlineStr"/>
+      <c r="R131" s="4" t="inlineStr"/>
+      <c r="S131" t="inlineStr"/>
+      <c r="T131" s="4" t="inlineStr"/>
+      <c r="U131" t="inlineStr"/>
+      <c r="V131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W131" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-24 11:30:53
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W131"/>
+  <dimension ref="A1:Y131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,6 +506,16 @@
           <t>05-21_0</t>
         </is>
       </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>05-23_A</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>05-23_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -580,7 +590,13 @@
       <c r="V2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W2" t="inlineStr">
+      <c r="W2" t="n">
+        <v>2500</v>
+      </c>
+      <c r="X2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -659,7 +675,13 @@
       <c r="V3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W3" t="inlineStr">
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -738,7 +760,13 @@
       <c r="V4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W4" t="inlineStr">
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -817,9 +845,15 @@
       <c r="V5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>2544</t>
+      <c r="W5" t="n">
+        <v>2544</v>
+      </c>
+      <c r="X5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>2587</t>
         </is>
       </c>
     </row>
@@ -896,7 +930,13 @@
       <c r="V6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W6" t="inlineStr">
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -938,6 +978,8 @@
       <c r="U7" t="inlineStr"/>
       <c r="V7" s="4" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
+      <c r="X7" s="4" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -975,6 +1017,8 @@
       <c r="U8" t="inlineStr"/>
       <c r="V8" s="4" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
+      <c r="X8" s="4" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1012,6 +1056,8 @@
       <c r="U9" t="inlineStr"/>
       <c r="V9" s="4" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
+      <c r="X9" s="4" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1049,6 +1095,8 @@
       <c r="U10" t="inlineStr"/>
       <c r="V10" s="4" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
+      <c r="X10" s="4" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1086,6 +1134,8 @@
       <c r="U11" t="inlineStr"/>
       <c r="V11" s="4" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
+      <c r="X11" s="4" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1123,6 +1173,8 @@
       <c r="U12" t="inlineStr"/>
       <c r="V12" s="4" t="inlineStr"/>
       <c r="W12" t="inlineStr"/>
+      <c r="X12" s="4" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1160,6 +1212,8 @@
       <c r="U13" t="inlineStr"/>
       <c r="V13" s="4" t="inlineStr"/>
       <c r="W13" t="inlineStr"/>
+      <c r="X13" s="4" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1197,6 +1251,8 @@
       <c r="U14" t="inlineStr"/>
       <c r="V14" s="4" t="inlineStr"/>
       <c r="W14" t="inlineStr"/>
+      <c r="X14" s="4" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1234,6 +1290,8 @@
       <c r="U15" t="inlineStr"/>
       <c r="V15" s="4" t="inlineStr"/>
       <c r="W15" t="inlineStr"/>
+      <c r="X15" s="4" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1271,6 +1329,8 @@
       <c r="U16" t="inlineStr"/>
       <c r="V16" s="4" t="inlineStr"/>
       <c r="W16" t="inlineStr"/>
+      <c r="X16" s="4" t="inlineStr"/>
+      <c r="Y16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1308,6 +1368,8 @@
       <c r="U17" t="inlineStr"/>
       <c r="V17" s="4" t="inlineStr"/>
       <c r="W17" t="inlineStr"/>
+      <c r="X17" s="4" t="inlineStr"/>
+      <c r="Y17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1382,9 +1444,15 @@
       <c r="V18" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="W18" t="inlineStr">
-        <is>
-          <t>2503</t>
+      <c r="W18" t="n">
+        <v>2503</v>
+      </c>
+      <c r="X18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>2755</t>
         </is>
       </c>
     </row>
@@ -1461,9 +1529,15 @@
       <c r="V19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W19" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="W19" t="n">
+        <v>2498</v>
+      </c>
+      <c r="X19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>2568</t>
         </is>
       </c>
     </row>
@@ -1540,9 +1614,15 @@
       <c r="V20" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="W20" t="inlineStr">
-        <is>
-          <t>2692</t>
+      <c r="W20" t="n">
+        <v>2692</v>
+      </c>
+      <c r="X20" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>3241</t>
         </is>
       </c>
     </row>
@@ -1619,9 +1699,15 @@
       <c r="V21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W21" t="inlineStr">
-        <is>
-          <t>2554</t>
+      <c r="W21" t="n">
+        <v>2554</v>
+      </c>
+      <c r="X21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>2692</t>
         </is>
       </c>
     </row>
@@ -1698,9 +1784,15 @@
       <c r="V22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="W22" t="inlineStr">
-        <is>
-          <t>2813</t>
+      <c r="W22" t="n">
+        <v>2813</v>
+      </c>
+      <c r="X22" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>3447</t>
         </is>
       </c>
     </row>
@@ -1777,9 +1869,15 @@
       <c r="V23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="W23" t="inlineStr">
-        <is>
-          <t>2943</t>
+      <c r="W23" t="n">
+        <v>2943</v>
+      </c>
+      <c r="X23" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>3539</t>
         </is>
       </c>
     </row>
@@ -1856,9 +1954,15 @@
       <c r="V24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="W24" t="inlineStr">
-        <is>
-          <t>3014</t>
+      <c r="W24" t="n">
+        <v>3014</v>
+      </c>
+      <c r="X24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="Y24" t="inlineStr">
+        <is>
+          <t>3702</t>
         </is>
       </c>
     </row>
@@ -1935,9 +2039,15 @@
       <c r="V25" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W25" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="W25" t="n">
+        <v>2500</v>
+      </c>
+      <c r="X25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y25" t="inlineStr">
+        <is>
+          <t>3465</t>
         </is>
       </c>
     </row>
@@ -2014,7 +2124,13 @@
       <c r="V26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W26" t="inlineStr">
+      <c r="W26" t="n">
+        <v>0</v>
+      </c>
+      <c r="X26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y26" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2093,7 +2209,13 @@
       <c r="V27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W27" t="inlineStr">
+      <c r="W27" t="n">
+        <v>0</v>
+      </c>
+      <c r="X27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2135,6 +2257,8 @@
       <c r="U28" t="inlineStr"/>
       <c r="V28" s="4" t="inlineStr"/>
       <c r="W28" t="inlineStr"/>
+      <c r="X28" s="4" t="inlineStr"/>
+      <c r="Y28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2209,9 +2333,15 @@
       <c r="V29" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="W29" t="inlineStr">
-        <is>
-          <t>2799</t>
+      <c r="W29" t="n">
+        <v>2799</v>
+      </c>
+      <c r="X29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>3095</t>
         </is>
       </c>
     </row>
@@ -2288,9 +2418,15 @@
       <c r="V30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W30" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="W30" t="n">
+        <v>2499</v>
+      </c>
+      <c r="X30" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>2890</t>
         </is>
       </c>
     </row>
@@ -2367,9 +2503,15 @@
       <c r="V31" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="W31" t="inlineStr">
-        <is>
-          <t>2960</t>
+      <c r="W31" t="n">
+        <v>2960</v>
+      </c>
+      <c r="X31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>3700</t>
         </is>
       </c>
     </row>
@@ -2446,9 +2588,15 @@
       <c r="V32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W32" t="inlineStr">
-        <is>
-          <t>2516</t>
+      <c r="W32" t="n">
+        <v>2516</v>
+      </c>
+      <c r="X32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t>2514</t>
         </is>
       </c>
     </row>
@@ -2488,6 +2636,8 @@
       <c r="U33" t="inlineStr"/>
       <c r="V33" s="4" t="inlineStr"/>
       <c r="W33" t="inlineStr"/>
+      <c r="X33" s="4" t="inlineStr"/>
+      <c r="Y33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2562,7 +2712,13 @@
       <c r="V34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W34" t="inlineStr">
+      <c r="W34" t="n">
+        <v>0</v>
+      </c>
+      <c r="X34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2641,7 +2797,13 @@
       <c r="V35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W35" t="inlineStr">
+      <c r="W35" t="n">
+        <v>0</v>
+      </c>
+      <c r="X35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y35" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2720,9 +2882,15 @@
       <c r="V36" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="W36" t="inlineStr">
-        <is>
-          <t>2793</t>
+      <c r="W36" t="n">
+        <v>2793</v>
+      </c>
+      <c r="X36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y36" t="inlineStr">
+        <is>
+          <t>2817</t>
         </is>
       </c>
     </row>
@@ -2799,9 +2967,15 @@
       <c r="V37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="W37" t="inlineStr">
-        <is>
-          <t>2940</t>
+      <c r="W37" t="n">
+        <v>2940</v>
+      </c>
+      <c r="X37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y37" t="inlineStr">
+        <is>
+          <t>3615</t>
         </is>
       </c>
     </row>
@@ -2878,9 +3052,15 @@
       <c r="V38" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="W38" t="inlineStr">
-        <is>
-          <t>3003</t>
+      <c r="W38" t="n">
+        <v>3003</v>
+      </c>
+      <c r="X38" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="Y38" t="inlineStr">
+        <is>
+          <t>3893</t>
         </is>
       </c>
     </row>
@@ -2957,9 +3137,15 @@
       <c r="V39" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="W39" t="inlineStr">
-        <is>
-          <t>2866</t>
+      <c r="W39" t="n">
+        <v>2866</v>
+      </c>
+      <c r="X39" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="Y39" t="inlineStr">
+        <is>
+          <t>3637</t>
         </is>
       </c>
     </row>
@@ -3036,7 +3222,13 @@
       <c r="V40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W40" t="inlineStr">
+      <c r="W40" t="n">
+        <v>0</v>
+      </c>
+      <c r="X40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3115,9 +3307,15 @@
       <c r="V41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W41" t="inlineStr">
-        <is>
-          <t>2498</t>
+      <c r="W41" t="n">
+        <v>2498</v>
+      </c>
+      <c r="X41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y41" t="inlineStr">
+        <is>
+          <t>3045</t>
         </is>
       </c>
     </row>
@@ -3194,7 +3392,13 @@
       <c r="V42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W42" t="inlineStr">
+      <c r="W42" t="n">
+        <v>0</v>
+      </c>
+      <c r="X42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y42" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3236,6 +3440,8 @@
       <c r="U43" t="inlineStr"/>
       <c r="V43" s="4" t="inlineStr"/>
       <c r="W43" t="inlineStr"/>
+      <c r="X43" s="4" t="inlineStr"/>
+      <c r="Y43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3273,6 +3479,8 @@
       <c r="U44" t="inlineStr"/>
       <c r="V44" s="4" t="inlineStr"/>
       <c r="W44" t="inlineStr"/>
+      <c r="X44" s="4" t="inlineStr"/>
+      <c r="Y44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3342,6 +3550,8 @@
       <c r="U45" t="inlineStr"/>
       <c r="V45" s="4" t="inlineStr"/>
       <c r="W45" t="inlineStr"/>
+      <c r="X45" s="4" t="inlineStr"/>
+      <c r="Y45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -3416,9 +3626,15 @@
       <c r="V46" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="W46" t="inlineStr">
-        <is>
-          <t>2664</t>
+      <c r="W46" t="n">
+        <v>2664</v>
+      </c>
+      <c r="X46" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y46" t="inlineStr">
+        <is>
+          <t>2860</t>
         </is>
       </c>
     </row>
@@ -3495,9 +3711,15 @@
       <c r="V47" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="W47" t="inlineStr">
-        <is>
-          <t>2970</t>
+      <c r="W47" t="n">
+        <v>2970</v>
+      </c>
+      <c r="X47" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y47" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -3574,7 +3796,13 @@
       <c r="V48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W48" t="inlineStr">
+      <c r="W48" t="n">
+        <v>0</v>
+      </c>
+      <c r="X48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3653,9 +3881,15 @@
       <c r="V49" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="W49" t="inlineStr">
-        <is>
-          <t>2982</t>
+      <c r="W49" t="n">
+        <v>2982</v>
+      </c>
+      <c r="X49" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="Y49" t="inlineStr">
+        <is>
+          <t>3769</t>
         </is>
       </c>
     </row>
@@ -3732,9 +3966,15 @@
       <c r="V50" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="W50" t="inlineStr">
-        <is>
-          <t>2973</t>
+      <c r="W50" t="n">
+        <v>2973</v>
+      </c>
+      <c r="X50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y50" t="inlineStr">
+        <is>
+          <t>3826</t>
         </is>
       </c>
     </row>
@@ -3806,6 +4046,8 @@
       <c r="U51" t="inlineStr"/>
       <c r="V51" s="4" t="inlineStr"/>
       <c r="W51" t="inlineStr"/>
+      <c r="X51" s="4" t="inlineStr"/>
+      <c r="Y51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -3880,9 +4122,15 @@
       <c r="V52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="W52" t="inlineStr">
-        <is>
-          <t>3028</t>
+      <c r="W52" t="n">
+        <v>3028</v>
+      </c>
+      <c r="X52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y52" t="inlineStr">
+        <is>
+          <t>3764</t>
         </is>
       </c>
     </row>
@@ -3959,9 +4207,15 @@
       <c r="V53" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="W53" t="inlineStr">
-        <is>
-          <t>2689</t>
+      <c r="W53" t="n">
+        <v>2689</v>
+      </c>
+      <c r="X53" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y53" t="inlineStr">
+        <is>
+          <t>2928</t>
         </is>
       </c>
     </row>
@@ -4033,6 +4287,8 @@
       <c r="U54" t="inlineStr"/>
       <c r="V54" s="4" t="inlineStr"/>
       <c r="W54" t="inlineStr"/>
+      <c r="X54" s="4" t="inlineStr"/>
+      <c r="Y54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -4107,9 +4363,15 @@
       <c r="V55" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="W55" t="inlineStr">
-        <is>
-          <t>2555</t>
+      <c r="W55" t="n">
+        <v>2555</v>
+      </c>
+      <c r="X55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y55" t="inlineStr">
+        <is>
+          <t>2562</t>
         </is>
       </c>
     </row>
@@ -4186,9 +4448,15 @@
       <c r="V56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="W56" t="inlineStr">
-        <is>
-          <t>3091</t>
+      <c r="W56" t="n">
+        <v>3091</v>
+      </c>
+      <c r="X56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y56" t="inlineStr">
+        <is>
+          <t>3921</t>
         </is>
       </c>
     </row>
@@ -4265,9 +4533,15 @@
       <c r="V57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="W57" t="inlineStr">
-        <is>
-          <t>2766</t>
+      <c r="W57" t="n">
+        <v>2766</v>
+      </c>
+      <c r="X57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y57" t="inlineStr">
+        <is>
+          <t>3288</t>
         </is>
       </c>
     </row>
@@ -4344,9 +4618,15 @@
       <c r="V58" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="W58" t="inlineStr">
-        <is>
-          <t>2890</t>
+      <c r="W58" t="n">
+        <v>2890</v>
+      </c>
+      <c r="X58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="Y58" t="inlineStr">
+        <is>
+          <t>3237</t>
         </is>
       </c>
     </row>
@@ -4423,9 +4703,15 @@
       <c r="V59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="W59" t="inlineStr">
-        <is>
-          <t>2769</t>
+      <c r="W59" t="n">
+        <v>2769</v>
+      </c>
+      <c r="X59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y59" t="inlineStr">
+        <is>
+          <t>3236</t>
         </is>
       </c>
     </row>
@@ -4502,9 +4788,15 @@
       <c r="V60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="W60" t="inlineStr">
-        <is>
-          <t>3003</t>
+      <c r="W60" t="n">
+        <v>3003</v>
+      </c>
+      <c r="X60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="Y60" t="inlineStr">
+        <is>
+          <t>3563</t>
         </is>
       </c>
     </row>
@@ -4544,6 +4836,8 @@
       <c r="U61" t="inlineStr"/>
       <c r="V61" s="4" t="inlineStr"/>
       <c r="W61" t="inlineStr"/>
+      <c r="X61" s="4" t="inlineStr"/>
+      <c r="Y61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -4618,9 +4912,15 @@
       <c r="V62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="W62" t="inlineStr">
-        <is>
-          <t>2807</t>
+      <c r="W62" t="n">
+        <v>2807</v>
+      </c>
+      <c r="X62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y62" t="inlineStr">
+        <is>
+          <t>3182</t>
         </is>
       </c>
     </row>
@@ -4697,9 +4997,15 @@
       <c r="V63" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="W63" t="inlineStr">
-        <is>
-          <t>2835</t>
+      <c r="W63" t="n">
+        <v>2835</v>
+      </c>
+      <c r="X63" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y63" t="inlineStr">
+        <is>
+          <t>3228</t>
         </is>
       </c>
     </row>
@@ -4776,9 +5082,15 @@
       <c r="V64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="W64" t="inlineStr">
-        <is>
-          <t>2856</t>
+      <c r="W64" t="n">
+        <v>2856</v>
+      </c>
+      <c r="X64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y64" t="inlineStr">
+        <is>
+          <t>3312</t>
         </is>
       </c>
     </row>
@@ -4855,7 +5167,13 @@
       <c r="V65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W65" t="inlineStr">
+      <c r="W65" t="n">
+        <v>0</v>
+      </c>
+      <c r="X65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y65" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4934,7 +5252,13 @@
       <c r="V66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W66" t="inlineStr">
+      <c r="W66" t="n">
+        <v>0</v>
+      </c>
+      <c r="X66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5013,7 +5337,13 @@
       <c r="V67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W67" t="inlineStr">
+      <c r="W67" t="n">
+        <v>0</v>
+      </c>
+      <c r="X67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5092,7 +5422,13 @@
       <c r="V68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W68" t="inlineStr">
+      <c r="W68" t="n">
+        <v>0</v>
+      </c>
+      <c r="X68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5134,6 +5470,8 @@
       <c r="U69" t="inlineStr"/>
       <c r="V69" s="4" t="inlineStr"/>
       <c r="W69" t="inlineStr"/>
+      <c r="X69" s="4" t="inlineStr"/>
+      <c r="Y69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -5208,7 +5546,13 @@
       <c r="V70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W70" t="inlineStr">
+      <c r="W70" t="n">
+        <v>0</v>
+      </c>
+      <c r="X70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5287,7 +5631,13 @@
       <c r="V71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W71" t="inlineStr">
+      <c r="W71" t="n">
+        <v>0</v>
+      </c>
+      <c r="X71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5366,7 +5716,13 @@
       <c r="V72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W72" t="inlineStr">
+      <c r="W72" t="n">
+        <v>0</v>
+      </c>
+      <c r="X72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5445,9 +5801,15 @@
       <c r="V73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W73" t="inlineStr">
-        <is>
-          <t>2493</t>
+      <c r="W73" t="n">
+        <v>2493</v>
+      </c>
+      <c r="X73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y73" t="inlineStr">
+        <is>
+          <t>2515</t>
         </is>
       </c>
     </row>
@@ -5524,7 +5886,13 @@
       <c r="V74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W74" t="inlineStr">
+      <c r="W74" t="n">
+        <v>0</v>
+      </c>
+      <c r="X74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5603,7 +5971,13 @@
       <c r="V75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W75" t="inlineStr">
+      <c r="W75" t="n">
+        <v>0</v>
+      </c>
+      <c r="X75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5682,9 +6056,15 @@
       <c r="V76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W76" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="W76" t="n">
+        <v>2500</v>
+      </c>
+      <c r="X76" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y76" t="inlineStr">
+        <is>
+          <t>2726</t>
         </is>
       </c>
     </row>
@@ -5761,9 +6141,15 @@
       <c r="V77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W77" t="inlineStr">
-        <is>
-          <t>2517</t>
+      <c r="W77" t="n">
+        <v>2517</v>
+      </c>
+      <c r="X77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y77" t="inlineStr">
+        <is>
+          <t>2561</t>
         </is>
       </c>
     </row>
@@ -5840,7 +6226,13 @@
       <c r="V78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W78" t="inlineStr">
+      <c r="W78" t="n">
+        <v>0</v>
+      </c>
+      <c r="X78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5919,7 +6311,13 @@
       <c r="V79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W79" t="inlineStr">
+      <c r="W79" t="n">
+        <v>0</v>
+      </c>
+      <c r="X79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5998,7 +6396,13 @@
       <c r="V80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W80" t="inlineStr">
+      <c r="W80" t="n">
+        <v>0</v>
+      </c>
+      <c r="X80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6077,7 +6481,13 @@
       <c r="V81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W81" t="inlineStr">
+      <c r="W81" t="n">
+        <v>0</v>
+      </c>
+      <c r="X81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6156,7 +6566,13 @@
       <c r="V82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W82" t="inlineStr">
+      <c r="W82" t="n">
+        <v>0</v>
+      </c>
+      <c r="X82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6235,7 +6651,13 @@
       <c r="V83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W83" t="inlineStr">
+      <c r="W83" t="n">
+        <v>0</v>
+      </c>
+      <c r="X83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6314,7 +6736,13 @@
       <c r="V84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W84" t="inlineStr">
+      <c r="W84" t="n">
+        <v>0</v>
+      </c>
+      <c r="X84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6393,7 +6821,13 @@
       <c r="V85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W85" t="inlineStr">
+      <c r="W85" t="n">
+        <v>0</v>
+      </c>
+      <c r="X85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6472,7 +6906,13 @@
       <c r="V86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W86" t="inlineStr">
+      <c r="W86" t="n">
+        <v>0</v>
+      </c>
+      <c r="X86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6551,7 +6991,13 @@
       <c r="V87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W87" t="inlineStr">
+      <c r="W87" t="n">
+        <v>0</v>
+      </c>
+      <c r="X87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6630,7 +7076,13 @@
       <c r="V88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W88" t="inlineStr">
+      <c r="W88" t="n">
+        <v>0</v>
+      </c>
+      <c r="X88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6709,7 +7161,13 @@
       <c r="V89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W89" t="inlineStr">
+      <c r="W89" t="n">
+        <v>0</v>
+      </c>
+      <c r="X89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6788,7 +7246,13 @@
       <c r="V90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W90" t="inlineStr">
+      <c r="W90" t="n">
+        <v>0</v>
+      </c>
+      <c r="X90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6867,7 +7331,13 @@
       <c r="V91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W91" t="inlineStr">
+      <c r="W91" t="n">
+        <v>0</v>
+      </c>
+      <c r="X91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6946,7 +7416,13 @@
       <c r="V92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W92" t="inlineStr">
+      <c r="W92" t="n">
+        <v>0</v>
+      </c>
+      <c r="X92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7025,7 +7501,13 @@
       <c r="V93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W93" t="inlineStr">
+      <c r="W93" t="n">
+        <v>0</v>
+      </c>
+      <c r="X93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7104,7 +7586,13 @@
       <c r="V94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W94" t="inlineStr">
+      <c r="W94" t="n">
+        <v>0</v>
+      </c>
+      <c r="X94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7183,7 +7671,13 @@
       <c r="V95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W95" t="inlineStr">
+      <c r="W95" t="n">
+        <v>0</v>
+      </c>
+      <c r="X95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7262,7 +7756,13 @@
       <c r="V96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W96" t="inlineStr">
+      <c r="W96" t="n">
+        <v>0</v>
+      </c>
+      <c r="X96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y96" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7341,7 +7841,13 @@
       <c r="V97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W97" t="inlineStr">
+      <c r="W97" t="n">
+        <v>0</v>
+      </c>
+      <c r="X97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7420,7 +7926,13 @@
       <c r="V98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W98" t="inlineStr">
+      <c r="W98" t="n">
+        <v>0</v>
+      </c>
+      <c r="X98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7499,7 +8011,13 @@
       <c r="V99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W99" t="inlineStr">
+      <c r="W99" t="n">
+        <v>0</v>
+      </c>
+      <c r="X99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7578,7 +8096,13 @@
       <c r="V100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W100" t="inlineStr">
+      <c r="W100" t="n">
+        <v>0</v>
+      </c>
+      <c r="X100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7657,7 +8181,13 @@
       <c r="V101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W101" t="inlineStr">
+      <c r="W101" t="n">
+        <v>0</v>
+      </c>
+      <c r="X101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7736,7 +8266,13 @@
       <c r="V102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W102" t="inlineStr">
+      <c r="W102" t="n">
+        <v>0</v>
+      </c>
+      <c r="X102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7815,7 +8351,13 @@
       <c r="V103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W103" t="inlineStr">
+      <c r="W103" t="n">
+        <v>0</v>
+      </c>
+      <c r="X103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7894,7 +8436,13 @@
       <c r="V104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W104" t="inlineStr">
+      <c r="W104" t="n">
+        <v>0</v>
+      </c>
+      <c r="X104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7973,7 +8521,13 @@
       <c r="V105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W105" t="inlineStr">
+      <c r="W105" t="n">
+        <v>0</v>
+      </c>
+      <c r="X105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8015,6 +8569,8 @@
       <c r="U106" t="inlineStr"/>
       <c r="V106" s="4" t="inlineStr"/>
       <c r="W106" t="inlineStr"/>
+      <c r="X106" s="4" t="inlineStr"/>
+      <c r="Y106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -8052,6 +8608,8 @@
       <c r="U107" t="inlineStr"/>
       <c r="V107" s="4" t="inlineStr"/>
       <c r="W107" t="inlineStr"/>
+      <c r="X107" s="4" t="inlineStr"/>
+      <c r="Y107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -8089,6 +8647,8 @@
       <c r="U108" t="inlineStr"/>
       <c r="V108" s="4" t="inlineStr"/>
       <c r="W108" t="inlineStr"/>
+      <c r="X108" s="4" t="inlineStr"/>
+      <c r="Y108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -8126,6 +8686,8 @@
       <c r="U109" t="inlineStr"/>
       <c r="V109" s="4" t="inlineStr"/>
       <c r="W109" t="inlineStr"/>
+      <c r="X109" s="4" t="inlineStr"/>
+      <c r="Y109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -8163,6 +8725,8 @@
       <c r="U110" t="inlineStr"/>
       <c r="V110" s="4" t="inlineStr"/>
       <c r="W110" t="inlineStr"/>
+      <c r="X110" s="4" t="inlineStr"/>
+      <c r="Y110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -8200,6 +8764,8 @@
       <c r="U111" t="inlineStr"/>
       <c r="V111" s="4" t="inlineStr"/>
       <c r="W111" t="inlineStr"/>
+      <c r="X111" s="4" t="inlineStr"/>
+      <c r="Y111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -8237,6 +8803,8 @@
       <c r="U112" t="inlineStr"/>
       <c r="V112" s="4" t="inlineStr"/>
       <c r="W112" t="inlineStr"/>
+      <c r="X112" s="4" t="inlineStr"/>
+      <c r="Y112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -8274,6 +8842,8 @@
       <c r="U113" t="inlineStr"/>
       <c r="V113" s="4" t="inlineStr"/>
       <c r="W113" t="inlineStr"/>
+      <c r="X113" s="4" t="inlineStr"/>
+      <c r="Y113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -8311,6 +8881,8 @@
       <c r="U114" t="inlineStr"/>
       <c r="V114" s="4" t="inlineStr"/>
       <c r="W114" t="inlineStr"/>
+      <c r="X114" s="4" t="inlineStr"/>
+      <c r="Y114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -8363,9 +8935,15 @@
       <c r="V115" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="W115" t="inlineStr">
-        <is>
-          <t>2939</t>
+      <c r="W115" t="n">
+        <v>2939</v>
+      </c>
+      <c r="X115" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="Y115" t="inlineStr">
+        <is>
+          <t>3781</t>
         </is>
       </c>
     </row>
@@ -8436,7 +9014,13 @@
       <c r="V116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W116" t="inlineStr">
+      <c r="W116" t="n">
+        <v>0</v>
+      </c>
+      <c r="X116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8489,9 +9073,15 @@
       <c r="V117" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="W117" t="inlineStr">
-        <is>
-          <t>3157</t>
+      <c r="W117" t="n">
+        <v>3157</v>
+      </c>
+      <c r="X117" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="Y117" t="inlineStr">
+        <is>
+          <t>4128</t>
         </is>
       </c>
     </row>
@@ -8562,9 +9152,15 @@
       <c r="V118" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="W118" t="inlineStr">
-        <is>
-          <t>2823</t>
+      <c r="W118" t="n">
+        <v>2823</v>
+      </c>
+      <c r="X118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y118" t="inlineStr">
+        <is>
+          <t>2969</t>
         </is>
       </c>
     </row>
@@ -8635,9 +9231,15 @@
       <c r="V119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W119" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="W119" t="n">
+        <v>0</v>
+      </c>
+      <c r="X119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y119" t="inlineStr">
+        <is>
+          <t>1500</t>
         </is>
       </c>
     </row>
@@ -8708,7 +9310,13 @@
       <c r="V120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W120" t="inlineStr">
+      <c r="W120" t="n">
+        <v>0</v>
+      </c>
+      <c r="X120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y120" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8781,7 +9389,13 @@
       <c r="V121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W121" t="inlineStr">
+      <c r="W121" t="n">
+        <v>0</v>
+      </c>
+      <c r="X121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8854,7 +9468,13 @@
       <c r="V122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W122" t="inlineStr">
+      <c r="W122" t="n">
+        <v>0</v>
+      </c>
+      <c r="X122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8923,7 +9543,13 @@
       <c r="V123" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="W123" t="inlineStr">
+      <c r="W123" t="n">
+        <v>2664</v>
+      </c>
+      <c r="X123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y123" t="inlineStr">
         <is>
           <t>2664</t>
         </is>
@@ -8988,11 +9614,11 @@
       <c r="V124" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="W124" t="inlineStr">
-        <is>
-          <t>2766</t>
-        </is>
-      </c>
+      <c r="W124" t="n">
+        <v>2766</v>
+      </c>
+      <c r="X124" s="4" t="inlineStr"/>
+      <c r="Y124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -9053,9 +9679,15 @@
       <c r="V125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W125" t="inlineStr">
-        <is>
-          <t>2000</t>
+      <c r="W125" t="n">
+        <v>2000</v>
+      </c>
+      <c r="X125" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="Y125" t="inlineStr">
+        <is>
+          <t>2178</t>
         </is>
       </c>
     </row>
@@ -9106,9 +9738,15 @@
       <c r="V126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W126" t="inlineStr">
-        <is>
-          <t>1500</t>
+      <c r="W126" t="n">
+        <v>1500</v>
+      </c>
+      <c r="X126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y126" t="inlineStr">
+        <is>
+          <t>1527</t>
         </is>
       </c>
     </row>
@@ -9155,9 +9793,15 @@
       <c r="V127" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="W127" t="inlineStr">
-        <is>
-          <t>1490</t>
+      <c r="W127" t="n">
+        <v>1490</v>
+      </c>
+      <c r="X127" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y127" t="inlineStr">
+        <is>
+          <t>1527</t>
         </is>
       </c>
     </row>
@@ -9200,9 +9844,15 @@
       <c r="V128" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="W128" t="inlineStr">
-        <is>
-          <t>2214</t>
+      <c r="W128" t="n">
+        <v>2214</v>
+      </c>
+      <c r="X128" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="Y128" t="inlineStr">
+        <is>
+          <t>3002</t>
         </is>
       </c>
     </row>
@@ -9245,9 +9895,15 @@
       <c r="V129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W129" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="W129" t="n">
+        <v>2500</v>
+      </c>
+      <c r="X129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y129" t="inlineStr">
+        <is>
+          <t>2775</t>
         </is>
       </c>
     </row>
@@ -9290,17 +9946,21 @@
       <c r="V130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W130" t="inlineStr">
+      <c r="W130" t="n">
+        <v>0</v>
+      </c>
+      <c r="X130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y130" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
     <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t>47928278</t>
-        </is>
+      <c r="A131" t="n">
+        <v>47928278</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
@@ -9333,7 +9993,13 @@
       <c r="V131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="W131" t="inlineStr">
+      <c r="W131" t="n">
+        <v>2500</v>
+      </c>
+      <c r="X131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y131" t="inlineStr">
         <is>
           <t>2500</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-05-25 11:30:55
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y131"/>
+  <dimension ref="A1:AA131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -516,6 +516,16 @@
           <t>05-23_0</t>
         </is>
       </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>05-24_A</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>05-24_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -596,9 +606,15 @@
       <c r="X2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="Y2" t="n">
+        <v>2500</v>
+      </c>
+      <c r="Z2" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>2984</t>
         </is>
       </c>
     </row>
@@ -681,7 +697,13 @@
       <c r="X3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y3" t="inlineStr">
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -766,7 +788,13 @@
       <c r="X4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y4" t="inlineStr">
+      <c r="Y4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -851,9 +879,15 @@
       <c r="X5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>2587</t>
+      <c r="Y5" t="n">
+        <v>2587</v>
+      </c>
+      <c r="Z5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>2624</t>
         </is>
       </c>
     </row>
@@ -936,7 +970,13 @@
       <c r="X6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y6" t="inlineStr">
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -980,6 +1020,8 @@
       <c r="W7" t="inlineStr"/>
       <c r="X7" s="4" t="inlineStr"/>
       <c r="Y7" t="inlineStr"/>
+      <c r="Z7" s="4" t="inlineStr"/>
+      <c r="AA7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1019,6 +1061,8 @@
       <c r="W8" t="inlineStr"/>
       <c r="X8" s="4" t="inlineStr"/>
       <c r="Y8" t="inlineStr"/>
+      <c r="Z8" s="4" t="inlineStr"/>
+      <c r="AA8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1058,6 +1102,8 @@
       <c r="W9" t="inlineStr"/>
       <c r="X9" s="4" t="inlineStr"/>
       <c r="Y9" t="inlineStr"/>
+      <c r="Z9" s="4" t="inlineStr"/>
+      <c r="AA9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1097,6 +1143,8 @@
       <c r="W10" t="inlineStr"/>
       <c r="X10" s="4" t="inlineStr"/>
       <c r="Y10" t="inlineStr"/>
+      <c r="Z10" s="4" t="inlineStr"/>
+      <c r="AA10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1136,6 +1184,8 @@
       <c r="W11" t="inlineStr"/>
       <c r="X11" s="4" t="inlineStr"/>
       <c r="Y11" t="inlineStr"/>
+      <c r="Z11" s="4" t="inlineStr"/>
+      <c r="AA11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1175,6 +1225,8 @@
       <c r="W12" t="inlineStr"/>
       <c r="X12" s="4" t="inlineStr"/>
       <c r="Y12" t="inlineStr"/>
+      <c r="Z12" s="4" t="inlineStr"/>
+      <c r="AA12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1214,6 +1266,8 @@
       <c r="W13" t="inlineStr"/>
       <c r="X13" s="4" t="inlineStr"/>
       <c r="Y13" t="inlineStr"/>
+      <c r="Z13" s="4" t="inlineStr"/>
+      <c r="AA13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1253,6 +1307,8 @@
       <c r="W14" t="inlineStr"/>
       <c r="X14" s="4" t="inlineStr"/>
       <c r="Y14" t="inlineStr"/>
+      <c r="Z14" s="4" t="inlineStr"/>
+      <c r="AA14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1292,6 +1348,8 @@
       <c r="W15" t="inlineStr"/>
       <c r="X15" s="4" t="inlineStr"/>
       <c r="Y15" t="inlineStr"/>
+      <c r="Z15" s="4" t="inlineStr"/>
+      <c r="AA15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1331,6 +1389,8 @@
       <c r="W16" t="inlineStr"/>
       <c r="X16" s="4" t="inlineStr"/>
       <c r="Y16" t="inlineStr"/>
+      <c r="Z16" s="4" t="inlineStr"/>
+      <c r="AA16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1370,6 +1430,8 @@
       <c r="W17" t="inlineStr"/>
       <c r="X17" s="4" t="inlineStr"/>
       <c r="Y17" t="inlineStr"/>
+      <c r="Z17" s="4" t="inlineStr"/>
+      <c r="AA17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1450,9 +1512,15 @@
       <c r="X18" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y18" t="inlineStr">
-        <is>
-          <t>2755</t>
+      <c r="Y18" t="n">
+        <v>2755</v>
+      </c>
+      <c r="Z18" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA18" t="inlineStr">
+        <is>
+          <t>3056</t>
         </is>
       </c>
     </row>
@@ -1535,7 +1603,13 @@
       <c r="X19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y19" t="inlineStr">
+      <c r="Y19" t="n">
+        <v>2568</v>
+      </c>
+      <c r="Z19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA19" t="inlineStr">
         <is>
           <t>2568</t>
         </is>
@@ -1620,9 +1694,15 @@
       <c r="X20" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="Y20" t="inlineStr">
-        <is>
-          <t>3241</t>
+      <c r="Y20" t="n">
+        <v>3241</v>
+      </c>
+      <c r="Z20" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA20" t="inlineStr">
+        <is>
+          <t>3480</t>
         </is>
       </c>
     </row>
@@ -1705,9 +1785,15 @@
       <c r="X21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y21" t="inlineStr">
-        <is>
-          <t>2692</t>
+      <c r="Y21" t="n">
+        <v>2692</v>
+      </c>
+      <c r="Z21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA21" t="inlineStr">
+        <is>
+          <t>2690</t>
         </is>
       </c>
     </row>
@@ -1790,9 +1876,15 @@
       <c r="X22" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="Y22" t="inlineStr">
-        <is>
-          <t>3447</t>
+      <c r="Y22" t="n">
+        <v>3447</v>
+      </c>
+      <c r="Z22" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA22" t="inlineStr">
+        <is>
+          <t>3745</t>
         </is>
       </c>
     </row>
@@ -1875,9 +1967,15 @@
       <c r="X23" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="Y23" t="inlineStr">
-        <is>
-          <t>3539</t>
+      <c r="Y23" t="n">
+        <v>3539</v>
+      </c>
+      <c r="Z23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA23" t="inlineStr">
+        <is>
+          <t>3969</t>
         </is>
       </c>
     </row>
@@ -1960,9 +2058,15 @@
       <c r="X24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="Y24" t="inlineStr">
-        <is>
-          <t>3702</t>
+      <c r="Y24" t="n">
+        <v>3702</v>
+      </c>
+      <c r="Z24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AA24" t="inlineStr">
+        <is>
+          <t>3991</t>
         </is>
       </c>
     </row>
@@ -2045,9 +2149,15 @@
       <c r="X25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Y25" t="inlineStr">
-        <is>
-          <t>3465</t>
+      <c r="Y25" t="n">
+        <v>3465</v>
+      </c>
+      <c r="Z25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA25" t="inlineStr">
+        <is>
+          <t>3953</t>
         </is>
       </c>
     </row>
@@ -2130,7 +2240,13 @@
       <c r="X26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y26" t="inlineStr">
+      <c r="Y26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA26" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2215,7 +2331,13 @@
       <c r="X27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y27" t="inlineStr">
+      <c r="Y27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2259,6 +2381,8 @@
       <c r="W28" t="inlineStr"/>
       <c r="X28" s="4" t="inlineStr"/>
       <c r="Y28" t="inlineStr"/>
+      <c r="Z28" s="4" t="inlineStr"/>
+      <c r="AA28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2339,7 +2463,13 @@
       <c r="X29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y29" t="inlineStr">
+      <c r="Y29" t="n">
+        <v>3095</v>
+      </c>
+      <c r="Z29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA29" t="inlineStr">
         <is>
           <t>3095</t>
         </is>
@@ -2424,9 +2554,15 @@
       <c r="X30" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="Y30" t="inlineStr">
-        <is>
-          <t>2890</t>
+      <c r="Y30" t="n">
+        <v>2890</v>
+      </c>
+      <c r="Z30" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA30" t="inlineStr">
+        <is>
+          <t>3241</t>
         </is>
       </c>
     </row>
@@ -2509,9 +2645,15 @@
       <c r="X31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Y31" t="inlineStr">
-        <is>
-          <t>3700</t>
+      <c r="Y31" t="n">
+        <v>3700</v>
+      </c>
+      <c r="Z31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA31" t="inlineStr">
+        <is>
+          <t>3997</t>
         </is>
       </c>
     </row>
@@ -2594,9 +2736,15 @@
       <c r="X32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y32" t="inlineStr">
-        <is>
-          <t>2514</t>
+      <c r="Y32" t="n">
+        <v>2514</v>
+      </c>
+      <c r="Z32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA32" t="inlineStr">
+        <is>
+          <t>2530</t>
         </is>
       </c>
     </row>
@@ -2638,6 +2786,8 @@
       <c r="W33" t="inlineStr"/>
       <c r="X33" s="4" t="inlineStr"/>
       <c r="Y33" t="inlineStr"/>
+      <c r="Z33" s="4" t="inlineStr"/>
+      <c r="AA33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2718,7 +2868,13 @@
       <c r="X34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y34" t="inlineStr">
+      <c r="Y34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2803,7 +2959,13 @@
       <c r="X35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y35" t="inlineStr">
+      <c r="Y35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA35" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2888,9 +3050,15 @@
       <c r="X36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y36" t="inlineStr">
-        <is>
-          <t>2817</t>
+      <c r="Y36" t="n">
+        <v>2817</v>
+      </c>
+      <c r="Z36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA36" t="inlineStr">
+        <is>
+          <t>2813</t>
         </is>
       </c>
     </row>
@@ -2973,9 +3141,15 @@
       <c r="X37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Y37" t="inlineStr">
-        <is>
-          <t>3615</t>
+      <c r="Y37" t="n">
+        <v>3615</v>
+      </c>
+      <c r="Z37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA37" t="inlineStr">
+        <is>
+          <t>3901</t>
         </is>
       </c>
     </row>
@@ -3058,9 +3232,15 @@
       <c r="X38" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="Y38" t="inlineStr">
-        <is>
-          <t>3893</t>
+      <c r="Y38" t="n">
+        <v>3893</v>
+      </c>
+      <c r="Z38" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA38" t="inlineStr">
+        <is>
+          <t>4202</t>
         </is>
       </c>
     </row>
@@ -3143,9 +3323,15 @@
       <c r="X39" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="Y39" t="inlineStr">
-        <is>
-          <t>3637</t>
+      <c r="Y39" t="n">
+        <v>3637</v>
+      </c>
+      <c r="Z39" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA39" t="inlineStr">
+        <is>
+          <t>3809</t>
         </is>
       </c>
     </row>
@@ -3228,7 +3414,13 @@
       <c r="X40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y40" t="inlineStr">
+      <c r="Y40" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3313,9 +3505,15 @@
       <c r="X41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y41" t="inlineStr">
-        <is>
-          <t>3045</t>
+      <c r="Y41" t="n">
+        <v>3045</v>
+      </c>
+      <c r="Z41" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA41" t="inlineStr">
+        <is>
+          <t>3243</t>
         </is>
       </c>
     </row>
@@ -3398,7 +3596,13 @@
       <c r="X42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y42" t="inlineStr">
+      <c r="Y42" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA42" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3442,6 +3646,8 @@
       <c r="W43" t="inlineStr"/>
       <c r="X43" s="4" t="inlineStr"/>
       <c r="Y43" t="inlineStr"/>
+      <c r="Z43" s="4" t="inlineStr"/>
+      <c r="AA43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3481,6 +3687,8 @@
       <c r="W44" t="inlineStr"/>
       <c r="X44" s="4" t="inlineStr"/>
       <c r="Y44" t="inlineStr"/>
+      <c r="Z44" s="4" t="inlineStr"/>
+      <c r="AA44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3552,6 +3760,8 @@
       <c r="W45" t="inlineStr"/>
       <c r="X45" s="4" t="inlineStr"/>
       <c r="Y45" t="inlineStr"/>
+      <c r="Z45" s="4" t="inlineStr"/>
+      <c r="AA45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -3632,9 +3842,15 @@
       <c r="X46" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="Y46" t="inlineStr">
-        <is>
-          <t>2860</t>
+      <c r="Y46" t="n">
+        <v>2860</v>
+      </c>
+      <c r="Z46" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA46" t="inlineStr">
+        <is>
+          <t>3009</t>
         </is>
       </c>
     </row>
@@ -3717,9 +3933,15 @@
       <c r="X47" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Y47" t="inlineStr">
-        <is>
-          <t>3995</t>
+      <c r="Y47" t="n">
+        <v>3995</v>
+      </c>
+      <c r="Z47" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA47" t="inlineStr">
+        <is>
+          <t>4202</t>
         </is>
       </c>
     </row>
@@ -3802,7 +4024,13 @@
       <c r="X48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y48" t="inlineStr">
+      <c r="Y48" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3887,9 +4115,15 @@
       <c r="X49" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="Y49" t="inlineStr">
-        <is>
-          <t>3769</t>
+      <c r="Y49" t="n">
+        <v>3769</v>
+      </c>
+      <c r="Z49" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AA49" t="inlineStr">
+        <is>
+          <t>3987</t>
         </is>
       </c>
     </row>
@@ -3972,9 +4206,15 @@
       <c r="X50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="Y50" t="inlineStr">
-        <is>
-          <t>3826</t>
+      <c r="Y50" t="n">
+        <v>3826</v>
+      </c>
+      <c r="Z50" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA50" t="inlineStr">
+        <is>
+          <t>3986</t>
         </is>
       </c>
     </row>
@@ -4048,6 +4288,8 @@
       <c r="W51" t="inlineStr"/>
       <c r="X51" s="4" t="inlineStr"/>
       <c r="Y51" t="inlineStr"/>
+      <c r="Z51" s="4" t="inlineStr"/>
+      <c r="AA51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -4128,9 +4370,15 @@
       <c r="X52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Y52" t="inlineStr">
-        <is>
-          <t>3764</t>
+      <c r="Y52" t="n">
+        <v>3764</v>
+      </c>
+      <c r="Z52" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AA52" t="inlineStr">
+        <is>
+          <t>3996</t>
         </is>
       </c>
     </row>
@@ -4213,9 +4461,15 @@
       <c r="X53" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="Y53" t="inlineStr">
-        <is>
-          <t>2928</t>
+      <c r="Y53" t="n">
+        <v>2928</v>
+      </c>
+      <c r="Z53" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA53" t="inlineStr">
+        <is>
+          <t>3201</t>
         </is>
       </c>
     </row>
@@ -4289,6 +4543,8 @@
       <c r="W54" t="inlineStr"/>
       <c r="X54" s="4" t="inlineStr"/>
       <c r="Y54" t="inlineStr"/>
+      <c r="Z54" s="4" t="inlineStr"/>
+      <c r="AA54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -4369,9 +4625,15 @@
       <c r="X55" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y55" t="inlineStr">
-        <is>
-          <t>2562</t>
+      <c r="Y55" t="n">
+        <v>2562</v>
+      </c>
+      <c r="Z55" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA55" t="inlineStr">
+        <is>
+          <t>3099</t>
         </is>
       </c>
     </row>
@@ -4454,9 +4716,15 @@
       <c r="X56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Y56" t="inlineStr">
-        <is>
-          <t>3921</t>
+      <c r="Y56" t="n">
+        <v>3921</v>
+      </c>
+      <c r="Z56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA56" t="inlineStr">
+        <is>
+          <t>4141</t>
         </is>
       </c>
     </row>
@@ -4539,9 +4807,15 @@
       <c r="X57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Y57" t="inlineStr">
-        <is>
-          <t>3288</t>
+      <c r="Y57" t="n">
+        <v>3288</v>
+      </c>
+      <c r="Z57" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA57" t="inlineStr">
+        <is>
+          <t>3424</t>
         </is>
       </c>
     </row>
@@ -4624,9 +4898,15 @@
       <c r="X58" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="Y58" t="inlineStr">
-        <is>
-          <t>3237</t>
+      <c r="Y58" t="n">
+        <v>3237</v>
+      </c>
+      <c r="Z58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA58" t="inlineStr">
+        <is>
+          <t>3373</t>
         </is>
       </c>
     </row>
@@ -4709,9 +4989,15 @@
       <c r="X59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Y59" t="inlineStr">
-        <is>
-          <t>3236</t>
+      <c r="Y59" t="n">
+        <v>3236</v>
+      </c>
+      <c r="Z59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA59" t="inlineStr">
+        <is>
+          <t>3472</t>
         </is>
       </c>
     </row>
@@ -4794,9 +5080,15 @@
       <c r="X60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="Y60" t="inlineStr">
-        <is>
-          <t>3563</t>
+      <c r="Y60" t="n">
+        <v>3563</v>
+      </c>
+      <c r="Z60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA60" t="inlineStr">
+        <is>
+          <t>3798</t>
         </is>
       </c>
     </row>
@@ -4838,6 +5130,8 @@
       <c r="W61" t="inlineStr"/>
       <c r="X61" s="4" t="inlineStr"/>
       <c r="Y61" t="inlineStr"/>
+      <c r="Z61" s="4" t="inlineStr"/>
+      <c r="AA61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -4918,9 +5212,15 @@
       <c r="X62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Y62" t="inlineStr">
-        <is>
-          <t>3182</t>
+      <c r="Y62" t="n">
+        <v>3182</v>
+      </c>
+      <c r="Z62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA62" t="inlineStr">
+        <is>
+          <t>3318</t>
         </is>
       </c>
     </row>
@@ -5003,9 +5303,15 @@
       <c r="X63" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Y63" t="inlineStr">
-        <is>
-          <t>3228</t>
+      <c r="Y63" t="n">
+        <v>3228</v>
+      </c>
+      <c r="Z63" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA63" t="inlineStr">
+        <is>
+          <t>3451</t>
         </is>
       </c>
     </row>
@@ -5088,9 +5394,15 @@
       <c r="X64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="Y64" t="inlineStr">
-        <is>
-          <t>3312</t>
+      <c r="Y64" t="n">
+        <v>3312</v>
+      </c>
+      <c r="Z64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA64" t="inlineStr">
+        <is>
+          <t>3606</t>
         </is>
       </c>
     </row>
@@ -5173,7 +5485,13 @@
       <c r="X65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y65" t="inlineStr">
+      <c r="Y65" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA65" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5258,7 +5576,13 @@
       <c r="X66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y66" t="inlineStr">
+      <c r="Y66" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5343,7 +5667,13 @@
       <c r="X67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y67" t="inlineStr">
+      <c r="Y67" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5428,7 +5758,13 @@
       <c r="X68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y68" t="inlineStr">
+      <c r="Y68" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5472,6 +5808,8 @@
       <c r="W69" t="inlineStr"/>
       <c r="X69" s="4" t="inlineStr"/>
       <c r="Y69" t="inlineStr"/>
+      <c r="Z69" s="4" t="inlineStr"/>
+      <c r="AA69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -5552,7 +5890,13 @@
       <c r="X70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y70" t="inlineStr">
+      <c r="Y70" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5637,7 +5981,13 @@
       <c r="X71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y71" t="inlineStr">
+      <c r="Y71" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5722,7 +6072,13 @@
       <c r="X72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y72" t="inlineStr">
+      <c r="Y72" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5807,9 +6163,15 @@
       <c r="X73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y73" t="inlineStr">
-        <is>
-          <t>2515</t>
+      <c r="Y73" t="n">
+        <v>2515</v>
+      </c>
+      <c r="Z73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA73" t="inlineStr">
+        <is>
+          <t>2582</t>
         </is>
       </c>
     </row>
@@ -5892,7 +6254,13 @@
       <c r="X74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y74" t="inlineStr">
+      <c r="Y74" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5977,7 +6345,13 @@
       <c r="X75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y75" t="inlineStr">
+      <c r="Y75" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6062,9 +6436,15 @@
       <c r="X76" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="Y76" t="inlineStr">
-        <is>
-          <t>2726</t>
+      <c r="Y76" t="n">
+        <v>2726</v>
+      </c>
+      <c r="Z76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA76" t="inlineStr">
+        <is>
+          <t>2802</t>
         </is>
       </c>
     </row>
@@ -6147,9 +6527,15 @@
       <c r="X77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y77" t="inlineStr">
-        <is>
-          <t>2561</t>
+      <c r="Y77" t="n">
+        <v>2561</v>
+      </c>
+      <c r="Z77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA77" t="inlineStr">
+        <is>
+          <t>2555</t>
         </is>
       </c>
     </row>
@@ -6232,7 +6618,13 @@
       <c r="X78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y78" t="inlineStr">
+      <c r="Y78" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6317,7 +6709,13 @@
       <c r="X79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y79" t="inlineStr">
+      <c r="Y79" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6402,7 +6800,13 @@
       <c r="X80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y80" t="inlineStr">
+      <c r="Y80" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6487,7 +6891,13 @@
       <c r="X81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y81" t="inlineStr">
+      <c r="Y81" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6572,7 +6982,13 @@
       <c r="X82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y82" t="inlineStr">
+      <c r="Y82" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6657,7 +7073,13 @@
       <c r="X83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y83" t="inlineStr">
+      <c r="Y83" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6742,7 +7164,13 @@
       <c r="X84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y84" t="inlineStr">
+      <c r="Y84" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6827,7 +7255,13 @@
       <c r="X85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y85" t="inlineStr">
+      <c r="Y85" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6912,7 +7346,13 @@
       <c r="X86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y86" t="inlineStr">
+      <c r="Y86" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6997,7 +7437,13 @@
       <c r="X87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y87" t="inlineStr">
+      <c r="Y87" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7082,7 +7528,13 @@
       <c r="X88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y88" t="inlineStr">
+      <c r="Y88" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7167,7 +7619,13 @@
       <c r="X89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y89" t="inlineStr">
+      <c r="Y89" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7252,7 +7710,13 @@
       <c r="X90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y90" t="inlineStr">
+      <c r="Y90" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7337,7 +7801,13 @@
       <c r="X91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y91" t="inlineStr">
+      <c r="Y91" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7422,7 +7892,13 @@
       <c r="X92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y92" t="inlineStr">
+      <c r="Y92" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7507,7 +7983,13 @@
       <c r="X93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y93" t="inlineStr">
+      <c r="Y93" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7592,7 +8074,13 @@
       <c r="X94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y94" t="inlineStr">
+      <c r="Y94" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7677,7 +8165,13 @@
       <c r="X95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y95" t="inlineStr">
+      <c r="Y95" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7762,7 +8256,13 @@
       <c r="X96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y96" t="inlineStr">
+      <c r="Y96" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA96" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7847,7 +8347,13 @@
       <c r="X97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y97" t="inlineStr">
+      <c r="Y97" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7932,7 +8438,13 @@
       <c r="X98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y98" t="inlineStr">
+      <c r="Y98" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8017,7 +8529,13 @@
       <c r="X99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y99" t="inlineStr">
+      <c r="Y99" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8102,7 +8620,13 @@
       <c r="X100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y100" t="inlineStr">
+      <c r="Y100" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8187,7 +8711,13 @@
       <c r="X101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y101" t="inlineStr">
+      <c r="Y101" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8272,7 +8802,13 @@
       <c r="X102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y102" t="inlineStr">
+      <c r="Y102" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8357,7 +8893,13 @@
       <c r="X103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y103" t="inlineStr">
+      <c r="Y103" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8442,7 +8984,13 @@
       <c r="X104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y104" t="inlineStr">
+      <c r="Y104" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8527,7 +9075,13 @@
       <c r="X105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y105" t="inlineStr">
+      <c r="Y105" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8571,6 +9125,8 @@
       <c r="W106" t="inlineStr"/>
       <c r="X106" s="4" t="inlineStr"/>
       <c r="Y106" t="inlineStr"/>
+      <c r="Z106" s="4" t="inlineStr"/>
+      <c r="AA106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -8610,6 +9166,8 @@
       <c r="W107" t="inlineStr"/>
       <c r="X107" s="4" t="inlineStr"/>
       <c r="Y107" t="inlineStr"/>
+      <c r="Z107" s="4" t="inlineStr"/>
+      <c r="AA107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -8649,6 +9207,8 @@
       <c r="W108" t="inlineStr"/>
       <c r="X108" s="4" t="inlineStr"/>
       <c r="Y108" t="inlineStr"/>
+      <c r="Z108" s="4" t="inlineStr"/>
+      <c r="AA108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -8688,6 +9248,8 @@
       <c r="W109" t="inlineStr"/>
       <c r="X109" s="4" t="inlineStr"/>
       <c r="Y109" t="inlineStr"/>
+      <c r="Z109" s="4" t="inlineStr"/>
+      <c r="AA109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -8727,6 +9289,8 @@
       <c r="W110" t="inlineStr"/>
       <c r="X110" s="4" t="inlineStr"/>
       <c r="Y110" t="inlineStr"/>
+      <c r="Z110" s="4" t="inlineStr"/>
+      <c r="AA110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -8766,6 +9330,8 @@
       <c r="W111" t="inlineStr"/>
       <c r="X111" s="4" t="inlineStr"/>
       <c r="Y111" t="inlineStr"/>
+      <c r="Z111" s="4" t="inlineStr"/>
+      <c r="AA111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -8805,6 +9371,8 @@
       <c r="W112" t="inlineStr"/>
       <c r="X112" s="4" t="inlineStr"/>
       <c r="Y112" t="inlineStr"/>
+      <c r="Z112" s="4" t="inlineStr"/>
+      <c r="AA112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -8844,6 +9412,8 @@
       <c r="W113" t="inlineStr"/>
       <c r="X113" s="4" t="inlineStr"/>
       <c r="Y113" t="inlineStr"/>
+      <c r="Z113" s="4" t="inlineStr"/>
+      <c r="AA113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -8883,6 +9453,8 @@
       <c r="W114" t="inlineStr"/>
       <c r="X114" s="4" t="inlineStr"/>
       <c r="Y114" t="inlineStr"/>
+      <c r="Z114" s="4" t="inlineStr"/>
+      <c r="AA114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -8941,9 +9513,15 @@
       <c r="X115" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="Y115" t="inlineStr">
-        <is>
-          <t>3781</t>
+      <c r="Y115" t="n">
+        <v>3781</v>
+      </c>
+      <c r="Z115" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA115" t="inlineStr">
+        <is>
+          <t>4201</t>
         </is>
       </c>
     </row>
@@ -9020,7 +9598,13 @@
       <c r="X116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y116" t="inlineStr">
+      <c r="Y116" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9079,9 +9663,15 @@
       <c r="X117" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="Y117" t="inlineStr">
-        <is>
-          <t>4128</t>
+      <c r="Y117" t="n">
+        <v>4128</v>
+      </c>
+      <c r="Z117" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AA117" t="inlineStr">
+        <is>
+          <t>4541</t>
         </is>
       </c>
     </row>
@@ -9158,9 +9748,15 @@
       <c r="X118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y118" t="inlineStr">
-        <is>
-          <t>2969</t>
+      <c r="Y118" t="n">
+        <v>2969</v>
+      </c>
+      <c r="Z118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA118" t="inlineStr">
+        <is>
+          <t>2968</t>
         </is>
       </c>
     </row>
@@ -9237,9 +9833,15 @@
       <c r="X119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y119" t="inlineStr">
-        <is>
-          <t>1500</t>
+      <c r="Y119" t="n">
+        <v>1500</v>
+      </c>
+      <c r="Z119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA119" t="inlineStr">
+        <is>
+          <t>1521</t>
         </is>
       </c>
     </row>
@@ -9316,7 +9918,13 @@
       <c r="X120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y120" t="inlineStr">
+      <c r="Y120" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA120" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9395,7 +10003,13 @@
       <c r="X121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y121" t="inlineStr">
+      <c r="Y121" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9474,7 +10088,13 @@
       <c r="X122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y122" t="inlineStr">
+      <c r="Y122" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9549,7 +10169,13 @@
       <c r="X123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y123" t="inlineStr">
+      <c r="Y123" t="n">
+        <v>2664</v>
+      </c>
+      <c r="Z123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA123" t="inlineStr">
         <is>
           <t>2664</t>
         </is>
@@ -9619,6 +10245,8 @@
       </c>
       <c r="X124" s="4" t="inlineStr"/>
       <c r="Y124" t="inlineStr"/>
+      <c r="Z124" s="4" t="inlineStr"/>
+      <c r="AA124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -9685,9 +10313,15 @@
       <c r="X125" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="Y125" t="inlineStr">
-        <is>
-          <t>2178</t>
+      <c r="Y125" t="n">
+        <v>2178</v>
+      </c>
+      <c r="Z125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA125" t="inlineStr">
+        <is>
+          <t>2186</t>
         </is>
       </c>
     </row>
@@ -9744,9 +10378,15 @@
       <c r="X126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y126" t="inlineStr">
-        <is>
-          <t>1527</t>
+      <c r="Y126" t="n">
+        <v>1527</v>
+      </c>
+      <c r="Z126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA126" t="inlineStr">
+        <is>
+          <t>1526</t>
         </is>
       </c>
     </row>
@@ -9799,9 +10439,15 @@
       <c r="X127" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y127" t="inlineStr">
-        <is>
-          <t>1527</t>
+      <c r="Y127" t="n">
+        <v>1527</v>
+      </c>
+      <c r="Z127" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA127" t="inlineStr">
+        <is>
+          <t>1539</t>
         </is>
       </c>
     </row>
@@ -9850,9 +10496,15 @@
       <c r="X128" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="Y128" t="inlineStr">
-        <is>
-          <t>3002</t>
+      <c r="Y128" t="n">
+        <v>3002</v>
+      </c>
+      <c r="Z128" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AA128" t="inlineStr">
+        <is>
+          <t>3265</t>
         </is>
       </c>
     </row>
@@ -9901,9 +10553,15 @@
       <c r="X129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y129" t="inlineStr">
-        <is>
-          <t>2775</t>
+      <c r="Y129" t="n">
+        <v>2775</v>
+      </c>
+      <c r="Z129" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA129" t="inlineStr">
+        <is>
+          <t>2882</t>
         </is>
       </c>
     </row>
@@ -9952,9 +10610,15 @@
       <c r="X130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y130" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="Y130" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA130" t="inlineStr">
+        <is>
+          <t>1300</t>
         </is>
       </c>
     </row>
@@ -9999,7 +10663,13 @@
       <c r="X131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="Y131" t="inlineStr">
+      <c r="Y131" t="n">
+        <v>2500</v>
+      </c>
+      <c r="Z131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA131" t="inlineStr">
         <is>
           <t>2500</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-05-26 11:30:58
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA131"/>
+  <dimension ref="A1:AC133"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -526,6 +526,16 @@
           <t>05-24_0</t>
         </is>
       </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>05-25_A</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>05-25_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -612,9 +622,15 @@
       <c r="Z2" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>2984</t>
+      <c r="AA2" t="n">
+        <v>2984</v>
+      </c>
+      <c r="AB2" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>3115</t>
         </is>
       </c>
     </row>
@@ -703,7 +719,13 @@
       <c r="Z3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA3" t="inlineStr">
+      <c r="AA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -794,7 +816,13 @@
       <c r="Z4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA4" t="inlineStr">
+      <c r="AA4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -885,9 +913,15 @@
       <c r="Z5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>2624</t>
+      <c r="AA5" t="n">
+        <v>2624</v>
+      </c>
+      <c r="AB5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>2664</t>
         </is>
       </c>
     </row>
@@ -976,7 +1010,13 @@
       <c r="Z6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA6" t="inlineStr">
+      <c r="AA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1022,6 +1062,8 @@
       <c r="Y7" t="inlineStr"/>
       <c r="Z7" s="4" t="inlineStr"/>
       <c r="AA7" t="inlineStr"/>
+      <c r="AB7" s="4" t="inlineStr"/>
+      <c r="AC7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1063,6 +1105,8 @@
       <c r="Y8" t="inlineStr"/>
       <c r="Z8" s="4" t="inlineStr"/>
       <c r="AA8" t="inlineStr"/>
+      <c r="AB8" s="4" t="inlineStr"/>
+      <c r="AC8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1104,6 +1148,8 @@
       <c r="Y9" t="inlineStr"/>
       <c r="Z9" s="4" t="inlineStr"/>
       <c r="AA9" t="inlineStr"/>
+      <c r="AB9" s="4" t="inlineStr"/>
+      <c r="AC9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1145,6 +1191,8 @@
       <c r="Y10" t="inlineStr"/>
       <c r="Z10" s="4" t="inlineStr"/>
       <c r="AA10" t="inlineStr"/>
+      <c r="AB10" s="4" t="inlineStr"/>
+      <c r="AC10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1186,6 +1234,8 @@
       <c r="Y11" t="inlineStr"/>
       <c r="Z11" s="4" t="inlineStr"/>
       <c r="AA11" t="inlineStr"/>
+      <c r="AB11" s="4" t="inlineStr"/>
+      <c r="AC11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1227,6 +1277,8 @@
       <c r="Y12" t="inlineStr"/>
       <c r="Z12" s="4" t="inlineStr"/>
       <c r="AA12" t="inlineStr"/>
+      <c r="AB12" s="4" t="inlineStr"/>
+      <c r="AC12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1268,6 +1320,8 @@
       <c r="Y13" t="inlineStr"/>
       <c r="Z13" s="4" t="inlineStr"/>
       <c r="AA13" t="inlineStr"/>
+      <c r="AB13" s="4" t="inlineStr"/>
+      <c r="AC13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1309,6 +1363,8 @@
       <c r="Y14" t="inlineStr"/>
       <c r="Z14" s="4" t="inlineStr"/>
       <c r="AA14" t="inlineStr"/>
+      <c r="AB14" s="4" t="inlineStr"/>
+      <c r="AC14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1350,6 +1406,8 @@
       <c r="Y15" t="inlineStr"/>
       <c r="Z15" s="4" t="inlineStr"/>
       <c r="AA15" t="inlineStr"/>
+      <c r="AB15" s="4" t="inlineStr"/>
+      <c r="AC15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1391,6 +1449,8 @@
       <c r="Y16" t="inlineStr"/>
       <c r="Z16" s="4" t="inlineStr"/>
       <c r="AA16" t="inlineStr"/>
+      <c r="AB16" s="4" t="inlineStr"/>
+      <c r="AC16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1432,6 +1492,8 @@
       <c r="Y17" t="inlineStr"/>
       <c r="Z17" s="4" t="inlineStr"/>
       <c r="AA17" t="inlineStr"/>
+      <c r="AB17" s="4" t="inlineStr"/>
+      <c r="AC17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1518,9 +1580,15 @@
       <c r="Z18" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AA18" t="inlineStr">
-        <is>
-          <t>3056</t>
+      <c r="AA18" t="n">
+        <v>3056</v>
+      </c>
+      <c r="AB18" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>3197</t>
         </is>
       </c>
     </row>
@@ -1609,9 +1677,15 @@
       <c r="Z19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA19" t="inlineStr">
-        <is>
-          <t>2568</t>
+      <c r="AA19" t="n">
+        <v>2568</v>
+      </c>
+      <c r="AB19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>2643</t>
         </is>
       </c>
     </row>
@@ -1700,9 +1774,15 @@
       <c r="Z20" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AA20" t="inlineStr">
-        <is>
-          <t>3480</t>
+      <c r="AA20" t="n">
+        <v>3480</v>
+      </c>
+      <c r="AB20" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>3746</t>
         </is>
       </c>
     </row>
@@ -1791,9 +1871,15 @@
       <c r="Z21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA21" t="inlineStr">
-        <is>
-          <t>2690</t>
+      <c r="AA21" t="n">
+        <v>2690</v>
+      </c>
+      <c r="AB21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC21" t="inlineStr">
+        <is>
+          <t>2719</t>
         </is>
       </c>
     </row>
@@ -1882,9 +1968,15 @@
       <c r="Z22" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="AA22" t="inlineStr">
-        <is>
-          <t>3745</t>
+      <c r="AA22" t="n">
+        <v>3745</v>
+      </c>
+      <c r="AB22" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC22" t="inlineStr">
+        <is>
+          <t>4012</t>
         </is>
       </c>
     </row>
@@ -1973,9 +2065,15 @@
       <c r="Z23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AA23" t="inlineStr">
-        <is>
-          <t>3969</t>
+      <c r="AA23" t="n">
+        <v>3969</v>
+      </c>
+      <c r="AB23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC23" t="inlineStr">
+        <is>
+          <t>4326</t>
         </is>
       </c>
     </row>
@@ -2064,9 +2162,15 @@
       <c r="Z24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AA24" t="inlineStr">
-        <is>
-          <t>3991</t>
+      <c r="AA24" t="n">
+        <v>3991</v>
+      </c>
+      <c r="AB24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AC24" t="inlineStr">
+        <is>
+          <t>4125</t>
         </is>
       </c>
     </row>
@@ -2155,9 +2259,15 @@
       <c r="Z25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AA25" t="inlineStr">
-        <is>
-          <t>3953</t>
+      <c r="AA25" t="n">
+        <v>3953</v>
+      </c>
+      <c r="AB25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC25" t="inlineStr">
+        <is>
+          <t>4310</t>
         </is>
       </c>
     </row>
@@ -2246,7 +2356,13 @@
       <c r="Z26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA26" t="inlineStr">
+      <c r="AA26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC26" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2337,7 +2453,13 @@
       <c r="Z27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA27" t="inlineStr">
+      <c r="AA27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2383,6 +2505,8 @@
       <c r="Y28" t="inlineStr"/>
       <c r="Z28" s="4" t="inlineStr"/>
       <c r="AA28" t="inlineStr"/>
+      <c r="AB28" s="4" t="inlineStr"/>
+      <c r="AC28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2469,7 +2593,13 @@
       <c r="Z29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA29" t="inlineStr">
+      <c r="AA29" t="n">
+        <v>3095</v>
+      </c>
+      <c r="AB29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC29" t="inlineStr">
         <is>
           <t>3095</t>
         </is>
@@ -2560,9 +2690,15 @@
       <c r="Z30" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AA30" t="inlineStr">
-        <is>
-          <t>3241</t>
+      <c r="AA30" t="n">
+        <v>3241</v>
+      </c>
+      <c r="AB30" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AC30" t="inlineStr">
+        <is>
+          <t>3598</t>
         </is>
       </c>
     </row>
@@ -2651,9 +2787,15 @@
       <c r="Z31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AA31" t="inlineStr">
-        <is>
-          <t>3997</t>
+      <c r="AA31" t="n">
+        <v>3997</v>
+      </c>
+      <c r="AB31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC31" t="inlineStr">
+        <is>
+          <t>4180</t>
         </is>
       </c>
     </row>
@@ -2742,9 +2884,15 @@
       <c r="Z32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA32" t="inlineStr">
-        <is>
-          <t>2530</t>
+      <c r="AA32" t="n">
+        <v>2530</v>
+      </c>
+      <c r="AB32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC32" t="inlineStr">
+        <is>
+          <t>2529</t>
         </is>
       </c>
     </row>
@@ -2788,6 +2936,8 @@
       <c r="Y33" t="inlineStr"/>
       <c r="Z33" s="4" t="inlineStr"/>
       <c r="AA33" t="inlineStr"/>
+      <c r="AB33" s="4" t="inlineStr"/>
+      <c r="AC33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2874,7 +3024,13 @@
       <c r="Z34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA34" t="inlineStr">
+      <c r="AA34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2965,7 +3121,13 @@
       <c r="Z35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA35" t="inlineStr">
+      <c r="AA35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC35" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3056,9 +3218,15 @@
       <c r="Z36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA36" t="inlineStr">
-        <is>
-          <t>2813</t>
+      <c r="AA36" t="n">
+        <v>2813</v>
+      </c>
+      <c r="AB36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC36" t="inlineStr">
+        <is>
+          <t>2828</t>
         </is>
       </c>
     </row>
@@ -3147,9 +3315,15 @@
       <c r="Z37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AA37" t="inlineStr">
-        <is>
-          <t>3901</t>
+      <c r="AA37" t="n">
+        <v>3901</v>
+      </c>
+      <c r="AB37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC37" t="inlineStr">
+        <is>
+          <t>3991</t>
         </is>
       </c>
     </row>
@@ -3238,9 +3412,15 @@
       <c r="Z38" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AA38" t="inlineStr">
-        <is>
-          <t>4202</t>
+      <c r="AA38" t="n">
+        <v>4202</v>
+      </c>
+      <c r="AB38" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AC38" t="inlineStr">
+        <is>
+          <t>4432</t>
         </is>
       </c>
     </row>
@@ -3329,9 +3509,15 @@
       <c r="Z39" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="AA39" t="inlineStr">
-        <is>
-          <t>3809</t>
+      <c r="AA39" t="n">
+        <v>3809</v>
+      </c>
+      <c r="AB39" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="AC39" t="inlineStr">
+        <is>
+          <t>3990</t>
         </is>
       </c>
     </row>
@@ -3420,7 +3606,13 @@
       <c r="Z40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA40" t="inlineStr">
+      <c r="AA40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3511,9 +3703,15 @@
       <c r="Z41" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="AA41" t="inlineStr">
-        <is>
-          <t>3243</t>
+      <c r="AA41" t="n">
+        <v>3243</v>
+      </c>
+      <c r="AB41" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC41" t="inlineStr">
+        <is>
+          <t>3534</t>
         </is>
       </c>
     </row>
@@ -3602,9 +3800,15 @@
       <c r="Z42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA42" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AA42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC42" t="inlineStr">
+        <is>
+          <t>2526</t>
         </is>
       </c>
     </row>
@@ -3648,6 +3852,8 @@
       <c r="Y43" t="inlineStr"/>
       <c r="Z43" s="4" t="inlineStr"/>
       <c r="AA43" t="inlineStr"/>
+      <c r="AB43" s="4" t="inlineStr"/>
+      <c r="AC43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3689,6 +3895,8 @@
       <c r="Y44" t="inlineStr"/>
       <c r="Z44" s="4" t="inlineStr"/>
       <c r="AA44" t="inlineStr"/>
+      <c r="AB44" s="4" t="inlineStr"/>
+      <c r="AC44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3762,6 +3970,8 @@
       <c r="Y45" t="inlineStr"/>
       <c r="Z45" s="4" t="inlineStr"/>
       <c r="AA45" t="inlineStr"/>
+      <c r="AB45" s="4" t="inlineStr"/>
+      <c r="AC45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -3848,9 +4058,15 @@
       <c r="Z46" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="AA46" t="inlineStr">
-        <is>
-          <t>3009</t>
+      <c r="AA46" t="n">
+        <v>3009</v>
+      </c>
+      <c r="AB46" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AC46" t="inlineStr">
+        <is>
+          <t>3183</t>
         </is>
       </c>
     </row>
@@ -3939,9 +4155,15 @@
       <c r="Z47" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AA47" t="inlineStr">
-        <is>
-          <t>4202</t>
+      <c r="AA47" t="n">
+        <v>4202</v>
+      </c>
+      <c r="AB47" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AC47" t="inlineStr">
+        <is>
+          <t>4399</t>
         </is>
       </c>
     </row>
@@ -4030,7 +4252,13 @@
       <c r="Z48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA48" t="inlineStr">
+      <c r="AA48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4121,9 +4349,15 @@
       <c r="Z49" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AA49" t="inlineStr">
-        <is>
-          <t>3987</t>
+      <c r="AA49" t="n">
+        <v>3987</v>
+      </c>
+      <c r="AB49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC49" t="inlineStr">
+        <is>
+          <t>4020</t>
         </is>
       </c>
     </row>
@@ -4212,9 +4446,15 @@
       <c r="Z50" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="AA50" t="inlineStr">
-        <is>
-          <t>3986</t>
+      <c r="AA50" t="n">
+        <v>3986</v>
+      </c>
+      <c r="AB50" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC50" t="inlineStr">
+        <is>
+          <t>4157</t>
         </is>
       </c>
     </row>
@@ -4290,6 +4530,8 @@
       <c r="Y51" t="inlineStr"/>
       <c r="Z51" s="4" t="inlineStr"/>
       <c r="AA51" t="inlineStr"/>
+      <c r="AB51" s="4" t="inlineStr"/>
+      <c r="AC51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -4376,9 +4618,15 @@
       <c r="Z52" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AA52" t="inlineStr">
-        <is>
-          <t>3996</t>
+      <c r="AA52" t="n">
+        <v>3996</v>
+      </c>
+      <c r="AB52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC52" t="inlineStr">
+        <is>
+          <t>4174</t>
         </is>
       </c>
     </row>
@@ -4467,9 +4715,15 @@
       <c r="Z53" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="AA53" t="inlineStr">
-        <is>
-          <t>3201</t>
+      <c r="AA53" t="n">
+        <v>3201</v>
+      </c>
+      <c r="AB53" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC53" t="inlineStr">
+        <is>
+          <t>3377</t>
         </is>
       </c>
     </row>
@@ -4545,6 +4799,8 @@
       <c r="Y54" t="inlineStr"/>
       <c r="Z54" s="4" t="inlineStr"/>
       <c r="AA54" t="inlineStr"/>
+      <c r="AB54" s="4" t="inlineStr"/>
+      <c r="AC54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -4631,9 +4887,15 @@
       <c r="Z55" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AA55" t="inlineStr">
-        <is>
-          <t>3099</t>
+      <c r="AA55" t="n">
+        <v>3099</v>
+      </c>
+      <c r="AB55" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC55" t="inlineStr">
+        <is>
+          <t>3547</t>
         </is>
       </c>
     </row>
@@ -4722,9 +4984,15 @@
       <c r="Z56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AA56" t="inlineStr">
-        <is>
-          <t>4141</t>
+      <c r="AA56" t="n">
+        <v>4141</v>
+      </c>
+      <c r="AB56" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="AC56" t="inlineStr">
+        <is>
+          <t>4228</t>
         </is>
       </c>
     </row>
@@ -4813,9 +5081,15 @@
       <c r="Z57" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="AA57" t="inlineStr">
-        <is>
-          <t>3424</t>
+      <c r="AA57" t="n">
+        <v>3424</v>
+      </c>
+      <c r="AB57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC57" t="inlineStr">
+        <is>
+          <t>3689</t>
         </is>
       </c>
     </row>
@@ -4904,9 +5178,15 @@
       <c r="Z58" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AA58" t="inlineStr">
-        <is>
-          <t>3373</t>
+      <c r="AA58" t="n">
+        <v>3373</v>
+      </c>
+      <c r="AB58" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC58" t="inlineStr">
+        <is>
+          <t>3381</t>
         </is>
       </c>
     </row>
@@ -4995,9 +5275,15 @@
       <c r="Z59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AA59" t="inlineStr">
-        <is>
-          <t>3472</t>
+      <c r="AA59" t="n">
+        <v>3472</v>
+      </c>
+      <c r="AB59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC59" t="inlineStr">
+        <is>
+          <t>3690</t>
         </is>
       </c>
     </row>
@@ -5086,9 +5372,15 @@
       <c r="Z60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AA60" t="inlineStr">
-        <is>
-          <t>3798</t>
+      <c r="AA60" t="n">
+        <v>3798</v>
+      </c>
+      <c r="AB60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC60" t="inlineStr">
+        <is>
+          <t>3984</t>
         </is>
       </c>
     </row>
@@ -5132,6 +5424,8 @@
       <c r="Y61" t="inlineStr"/>
       <c r="Z61" s="4" t="inlineStr"/>
       <c r="AA61" t="inlineStr"/>
+      <c r="AB61" s="4" t="inlineStr"/>
+      <c r="AC61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -5218,9 +5512,15 @@
       <c r="Z62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AA62" t="inlineStr">
-        <is>
-          <t>3318</t>
+      <c r="AA62" t="n">
+        <v>3318</v>
+      </c>
+      <c r="AB62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC62" t="inlineStr">
+        <is>
+          <t>3489</t>
         </is>
       </c>
     </row>
@@ -5309,9 +5609,15 @@
       <c r="Z63" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AA63" t="inlineStr">
-        <is>
-          <t>3451</t>
+      <c r="AA63" t="n">
+        <v>3451</v>
+      </c>
+      <c r="AB63" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC63" t="inlineStr">
+        <is>
+          <t>3678</t>
         </is>
       </c>
     </row>
@@ -5400,9 +5706,15 @@
       <c r="Z64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AA64" t="inlineStr">
-        <is>
-          <t>3606</t>
+      <c r="AA64" t="n">
+        <v>3606</v>
+      </c>
+      <c r="AB64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC64" t="inlineStr">
+        <is>
+          <t>3970</t>
         </is>
       </c>
     </row>
@@ -5491,7 +5803,13 @@
       <c r="Z65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA65" t="inlineStr">
+      <c r="AA65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB65" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC65" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5582,7 +5900,13 @@
       <c r="Z66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA66" t="inlineStr">
+      <c r="AA66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5673,7 +5997,13 @@
       <c r="Z67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA67" t="inlineStr">
+      <c r="AA67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5764,7 +6094,13 @@
       <c r="Z68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA68" t="inlineStr">
+      <c r="AA68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5810,6 +6146,8 @@
       <c r="Y69" t="inlineStr"/>
       <c r="Z69" s="4" t="inlineStr"/>
       <c r="AA69" t="inlineStr"/>
+      <c r="AB69" s="4" t="inlineStr"/>
+      <c r="AC69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -5896,7 +6234,13 @@
       <c r="Z70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA70" t="inlineStr">
+      <c r="AA70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5987,7 +6331,13 @@
       <c r="Z71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA71" t="inlineStr">
+      <c r="AA71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6078,7 +6428,13 @@
       <c r="Z72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA72" t="inlineStr">
+      <c r="AA72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6169,9 +6525,15 @@
       <c r="Z73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA73" t="inlineStr">
-        <is>
-          <t>2582</t>
+      <c r="AA73" t="n">
+        <v>2582</v>
+      </c>
+      <c r="AB73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC73" t="inlineStr">
+        <is>
+          <t>2646</t>
         </is>
       </c>
     </row>
@@ -6260,7 +6622,13 @@
       <c r="Z74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA74" t="inlineStr">
+      <c r="AA74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6351,7 +6719,13 @@
       <c r="Z75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA75" t="inlineStr">
+      <c r="AA75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6442,9 +6816,15 @@
       <c r="Z76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA76" t="inlineStr">
-        <is>
-          <t>2802</t>
+      <c r="AA76" t="n">
+        <v>2802</v>
+      </c>
+      <c r="AB76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC76" t="inlineStr">
+        <is>
+          <t>2798</t>
         </is>
       </c>
     </row>
@@ -6533,9 +6913,15 @@
       <c r="Z77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA77" t="inlineStr">
-        <is>
-          <t>2555</t>
+      <c r="AA77" t="n">
+        <v>2555</v>
+      </c>
+      <c r="AB77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC77" t="inlineStr">
+        <is>
+          <t>2549</t>
         </is>
       </c>
     </row>
@@ -6624,7 +7010,13 @@
       <c r="Z78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA78" t="inlineStr">
+      <c r="AA78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6715,7 +7107,13 @@
       <c r="Z79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA79" t="inlineStr">
+      <c r="AA79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6806,7 +7204,13 @@
       <c r="Z80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA80" t="inlineStr">
+      <c r="AA80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6897,7 +7301,13 @@
       <c r="Z81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA81" t="inlineStr">
+      <c r="AA81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6988,7 +7398,13 @@
       <c r="Z82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA82" t="inlineStr">
+      <c r="AA82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7079,7 +7495,13 @@
       <c r="Z83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA83" t="inlineStr">
+      <c r="AA83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7170,7 +7592,13 @@
       <c r="Z84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA84" t="inlineStr">
+      <c r="AA84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7261,7 +7689,13 @@
       <c r="Z85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA85" t="inlineStr">
+      <c r="AA85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7352,7 +7786,13 @@
       <c r="Z86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA86" t="inlineStr">
+      <c r="AA86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7443,7 +7883,13 @@
       <c r="Z87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA87" t="inlineStr">
+      <c r="AA87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7534,7 +7980,13 @@
       <c r="Z88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA88" t="inlineStr">
+      <c r="AA88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7625,7 +8077,13 @@
       <c r="Z89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA89" t="inlineStr">
+      <c r="AA89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7716,7 +8174,13 @@
       <c r="Z90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA90" t="inlineStr">
+      <c r="AA90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7807,7 +8271,13 @@
       <c r="Z91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA91" t="inlineStr">
+      <c r="AA91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7898,7 +8368,13 @@
       <c r="Z92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA92" t="inlineStr">
+      <c r="AA92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7989,7 +8465,13 @@
       <c r="Z93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA93" t="inlineStr">
+      <c r="AA93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8080,7 +8562,13 @@
       <c r="Z94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA94" t="inlineStr">
+      <c r="AA94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8171,7 +8659,13 @@
       <c r="Z95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA95" t="inlineStr">
+      <c r="AA95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8262,7 +8756,13 @@
       <c r="Z96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA96" t="inlineStr">
+      <c r="AA96" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC96" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8353,7 +8853,13 @@
       <c r="Z97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA97" t="inlineStr">
+      <c r="AA97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8444,7 +8950,13 @@
       <c r="Z98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA98" t="inlineStr">
+      <c r="AA98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8535,7 +9047,13 @@
       <c r="Z99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA99" t="inlineStr">
+      <c r="AA99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8626,7 +9144,13 @@
       <c r="Z100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA100" t="inlineStr">
+      <c r="AA100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8717,7 +9241,13 @@
       <c r="Z101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA101" t="inlineStr">
+      <c r="AA101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8808,7 +9338,13 @@
       <c r="Z102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA102" t="inlineStr">
+      <c r="AA102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8899,7 +9435,13 @@
       <c r="Z103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA103" t="inlineStr">
+      <c r="AA103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8990,7 +9532,13 @@
       <c r="Z104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA104" t="inlineStr">
+      <c r="AA104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9081,7 +9629,13 @@
       <c r="Z105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA105" t="inlineStr">
+      <c r="AA105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9127,6 +9681,8 @@
       <c r="Y106" t="inlineStr"/>
       <c r="Z106" s="4" t="inlineStr"/>
       <c r="AA106" t="inlineStr"/>
+      <c r="AB106" s="4" t="inlineStr"/>
+      <c r="AC106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -9168,6 +9724,8 @@
       <c r="Y107" t="inlineStr"/>
       <c r="Z107" s="4" t="inlineStr"/>
       <c r="AA107" t="inlineStr"/>
+      <c r="AB107" s="4" t="inlineStr"/>
+      <c r="AC107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -9209,6 +9767,8 @@
       <c r="Y108" t="inlineStr"/>
       <c r="Z108" s="4" t="inlineStr"/>
       <c r="AA108" t="inlineStr"/>
+      <c r="AB108" s="4" t="inlineStr"/>
+      <c r="AC108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -9250,6 +9810,8 @@
       <c r="Y109" t="inlineStr"/>
       <c r="Z109" s="4" t="inlineStr"/>
       <c r="AA109" t="inlineStr"/>
+      <c r="AB109" s="4" t="inlineStr"/>
+      <c r="AC109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -9291,6 +9853,8 @@
       <c r="Y110" t="inlineStr"/>
       <c r="Z110" s="4" t="inlineStr"/>
       <c r="AA110" t="inlineStr"/>
+      <c r="AB110" s="4" t="inlineStr"/>
+      <c r="AC110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -9332,6 +9896,8 @@
       <c r="Y111" t="inlineStr"/>
       <c r="Z111" s="4" t="inlineStr"/>
       <c r="AA111" t="inlineStr"/>
+      <c r="AB111" s="4" t="inlineStr"/>
+      <c r="AC111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -9373,6 +9939,8 @@
       <c r="Y112" t="inlineStr"/>
       <c r="Z112" s="4" t="inlineStr"/>
       <c r="AA112" t="inlineStr"/>
+      <c r="AB112" s="4" t="inlineStr"/>
+      <c r="AC112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -9414,6 +9982,8 @@
       <c r="Y113" t="inlineStr"/>
       <c r="Z113" s="4" t="inlineStr"/>
       <c r="AA113" t="inlineStr"/>
+      <c r="AB113" s="4" t="inlineStr"/>
+      <c r="AC113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -9455,6 +10025,8 @@
       <c r="Y114" t="inlineStr"/>
       <c r="Z114" s="4" t="inlineStr"/>
       <c r="AA114" t="inlineStr"/>
+      <c r="AB114" s="4" t="inlineStr"/>
+      <c r="AC114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -9519,9 +10091,15 @@
       <c r="Z115" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AA115" t="inlineStr">
-        <is>
-          <t>4201</t>
+      <c r="AA115" t="n">
+        <v>4201</v>
+      </c>
+      <c r="AB115" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC115" t="inlineStr">
+        <is>
+          <t>4465</t>
         </is>
       </c>
     </row>
@@ -9604,7 +10182,13 @@
       <c r="Z116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA116" t="inlineStr">
+      <c r="AA116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9669,9 +10253,15 @@
       <c r="Z117" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AA117" t="inlineStr">
-        <is>
-          <t>4541</t>
+      <c r="AA117" t="n">
+        <v>4541</v>
+      </c>
+      <c r="AB117" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AC117" t="inlineStr">
+        <is>
+          <t>4813</t>
         </is>
       </c>
     </row>
@@ -9754,7 +10344,13 @@
       <c r="Z118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA118" t="inlineStr">
+      <c r="AA118" t="n">
+        <v>2968</v>
+      </c>
+      <c r="AB118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC118" t="inlineStr">
         <is>
           <t>2968</t>
         </is>
@@ -9839,9 +10435,15 @@
       <c r="Z119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA119" t="inlineStr">
-        <is>
-          <t>1521</t>
+      <c r="AA119" t="n">
+        <v>1521</v>
+      </c>
+      <c r="AB119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC119" t="inlineStr">
+        <is>
+          <t>1539</t>
         </is>
       </c>
     </row>
@@ -9924,7 +10526,13 @@
       <c r="Z120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA120" t="inlineStr">
+      <c r="AA120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC120" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10009,7 +10617,13 @@
       <c r="Z121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA121" t="inlineStr">
+      <c r="AA121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10094,7 +10708,13 @@
       <c r="Z122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA122" t="inlineStr">
+      <c r="AA122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10175,9 +10795,15 @@
       <c r="Z123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA123" t="inlineStr">
-        <is>
-          <t>2664</t>
+      <c r="AA123" t="n">
+        <v>2664</v>
+      </c>
+      <c r="AB123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC123" t="inlineStr">
+        <is>
+          <t>2680</t>
         </is>
       </c>
     </row>
@@ -10247,6 +10873,8 @@
       <c r="Y124" t="inlineStr"/>
       <c r="Z124" s="4" t="inlineStr"/>
       <c r="AA124" t="inlineStr"/>
+      <c r="AB124" s="4" t="inlineStr"/>
+      <c r="AC124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -10319,9 +10947,15 @@
       <c r="Z125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA125" t="inlineStr">
-        <is>
-          <t>2186</t>
+      <c r="AA125" t="n">
+        <v>2186</v>
+      </c>
+      <c r="AB125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC125" t="inlineStr">
+        <is>
+          <t>2179</t>
         </is>
       </c>
     </row>
@@ -10384,7 +11018,13 @@
       <c r="Z126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA126" t="inlineStr">
+      <c r="AA126" t="n">
+        <v>1526</v>
+      </c>
+      <c r="AB126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC126" t="inlineStr">
         <is>
           <t>1526</t>
         </is>
@@ -10445,11 +11085,11 @@
       <c r="Z127" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="AA127" t="inlineStr">
-        <is>
-          <t>1539</t>
-        </is>
-      </c>
+      <c r="AA127" t="n">
+        <v>1539</v>
+      </c>
+      <c r="AB127" s="4" t="inlineStr"/>
+      <c r="AC127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -10502,9 +11142,15 @@
       <c r="Z128" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AA128" t="inlineStr">
-        <is>
-          <t>3265</t>
+      <c r="AA128" t="n">
+        <v>3265</v>
+      </c>
+      <c r="AB128" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AC128" t="inlineStr">
+        <is>
+          <t>3379</t>
         </is>
       </c>
     </row>
@@ -10559,9 +11205,15 @@
       <c r="Z129" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="AA129" t="inlineStr">
-        <is>
-          <t>2882</t>
+      <c r="AA129" t="n">
+        <v>2882</v>
+      </c>
+      <c r="AB129" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="AC129" t="inlineStr">
+        <is>
+          <t>3123</t>
         </is>
       </c>
     </row>
@@ -10616,9 +11268,15 @@
       <c r="Z130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA130" t="inlineStr">
-        <is>
-          <t>1300</t>
+      <c r="AA130" t="n">
+        <v>1300</v>
+      </c>
+      <c r="AB130" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC130" t="inlineStr">
+        <is>
+          <t>1299</t>
         </is>
       </c>
     </row>
@@ -10669,9 +11327,113 @@
       <c r="Z131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AA131" t="inlineStr">
+      <c r="AA131" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AB131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC131" t="inlineStr">
         <is>
           <t>2500</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>54576721</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Maxhappy</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr"/>
+      <c r="D132" t="inlineStr"/>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F132" s="4" t="inlineStr"/>
+      <c r="G132" t="inlineStr"/>
+      <c r="H132" s="4" t="inlineStr"/>
+      <c r="I132" t="inlineStr"/>
+      <c r="J132" s="4" t="inlineStr"/>
+      <c r="K132" t="inlineStr"/>
+      <c r="L132" s="4" t="inlineStr"/>
+      <c r="M132" t="inlineStr"/>
+      <c r="N132" s="4" t="inlineStr"/>
+      <c r="O132" t="inlineStr"/>
+      <c r="P132" s="4" t="inlineStr"/>
+      <c r="Q132" t="inlineStr"/>
+      <c r="R132" s="4" t="inlineStr"/>
+      <c r="S132" t="inlineStr"/>
+      <c r="T132" s="4" t="inlineStr"/>
+      <c r="U132" t="inlineStr"/>
+      <c r="V132" s="4" t="inlineStr"/>
+      <c r="W132" t="inlineStr"/>
+      <c r="X132" s="4" t="inlineStr"/>
+      <c r="Y132" t="inlineStr"/>
+      <c r="Z132" s="4" t="inlineStr"/>
+      <c r="AA132" t="inlineStr"/>
+      <c r="AB132" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC132" t="inlineStr">
+        <is>
+          <t>2971</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>55653457</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>"free Lin"</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr"/>
+      <c r="D133" t="inlineStr"/>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F133" s="4" t="inlineStr"/>
+      <c r="G133" t="inlineStr"/>
+      <c r="H133" s="4" t="inlineStr"/>
+      <c r="I133" t="inlineStr"/>
+      <c r="J133" s="4" t="inlineStr"/>
+      <c r="K133" t="inlineStr"/>
+      <c r="L133" s="4" t="inlineStr"/>
+      <c r="M133" t="inlineStr"/>
+      <c r="N133" s="4" t="inlineStr"/>
+      <c r="O133" t="inlineStr"/>
+      <c r="P133" s="4" t="inlineStr"/>
+      <c r="Q133" t="inlineStr"/>
+      <c r="R133" s="4" t="inlineStr"/>
+      <c r="S133" t="inlineStr"/>
+      <c r="T133" s="4" t="inlineStr"/>
+      <c r="U133" t="inlineStr"/>
+      <c r="V133" s="4" t="inlineStr"/>
+      <c r="W133" t="inlineStr"/>
+      <c r="X133" s="4" t="inlineStr"/>
+      <c r="Y133" t="inlineStr"/>
+      <c r="Z133" s="4" t="inlineStr"/>
+      <c r="AA133" t="inlineStr"/>
+      <c r="AB133" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC133" t="inlineStr">
+        <is>
+          <t>2563</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-26 16:11:11
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -11340,10 +11340,8 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>54576721</t>
-        </is>
+      <c r="A132" t="n">
+        <v>54576721</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
@@ -11389,10 +11387,8 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>55653457</t>
-        </is>
+      <c r="A133" t="n">
+        <v>55653457</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-05-28 11:31:08
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC133"/>
+  <dimension ref="A1:AE139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,6 +536,16 @@
           <t>05-25_0</t>
         </is>
       </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>05-27_A</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>05-27_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -628,9 +638,15 @@
       <c r="AB2" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>3115</t>
+      <c r="AC2" t="n">
+        <v>3115</v>
+      </c>
+      <c r="AD2" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>3450</t>
         </is>
       </c>
     </row>
@@ -725,7 +741,13 @@
       <c r="AB3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC3" t="inlineStr">
+      <c r="AC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -822,9 +844,15 @@
       <c r="AB4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AC4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -919,9 +947,15 @@
       <c r="AB5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>2664</t>
+      <c r="AC5" t="n">
+        <v>2664</v>
+      </c>
+      <c r="AD5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>2720</t>
         </is>
       </c>
     </row>
@@ -1016,7 +1050,13 @@
       <c r="AB6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC6" t="inlineStr">
+      <c r="AC6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1064,6 +1104,8 @@
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" s="4" t="inlineStr"/>
       <c r="AC7" t="inlineStr"/>
+      <c r="AD7" s="4" t="inlineStr"/>
+      <c r="AE7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1107,6 +1149,8 @@
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" s="4" t="inlineStr"/>
       <c r="AC8" t="inlineStr"/>
+      <c r="AD8" s="4" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1150,6 +1194,8 @@
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" s="4" t="inlineStr"/>
       <c r="AC9" t="inlineStr"/>
+      <c r="AD9" s="4" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1193,6 +1239,8 @@
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" s="4" t="inlineStr"/>
       <c r="AC10" t="inlineStr"/>
+      <c r="AD10" s="4" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1236,6 +1284,8 @@
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" s="4" t="inlineStr"/>
       <c r="AC11" t="inlineStr"/>
+      <c r="AD11" s="4" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1279,6 +1329,8 @@
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" s="4" t="inlineStr"/>
       <c r="AC12" t="inlineStr"/>
+      <c r="AD12" s="4" t="inlineStr"/>
+      <c r="AE12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1322,6 +1374,8 @@
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" s="4" t="inlineStr"/>
       <c r="AC13" t="inlineStr"/>
+      <c r="AD13" s="4" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1365,6 +1419,8 @@
       <c r="AA14" t="inlineStr"/>
       <c r="AB14" s="4" t="inlineStr"/>
       <c r="AC14" t="inlineStr"/>
+      <c r="AD14" s="4" t="inlineStr"/>
+      <c r="AE14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1408,6 +1464,8 @@
       <c r="AA15" t="inlineStr"/>
       <c r="AB15" s="4" t="inlineStr"/>
       <c r="AC15" t="inlineStr"/>
+      <c r="AD15" s="4" t="inlineStr"/>
+      <c r="AE15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1451,6 +1509,8 @@
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" s="4" t="inlineStr"/>
       <c r="AC16" t="inlineStr"/>
+      <c r="AD16" s="4" t="inlineStr"/>
+      <c r="AE16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1494,6 +1554,8 @@
       <c r="AA17" t="inlineStr"/>
       <c r="AB17" s="4" t="inlineStr"/>
       <c r="AC17" t="inlineStr"/>
+      <c r="AD17" s="4" t="inlineStr"/>
+      <c r="AE17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1586,9 +1648,15 @@
       <c r="AB18" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="AC18" t="inlineStr">
-        <is>
-          <t>3197</t>
+      <c r="AC18" t="n">
+        <v>3197</v>
+      </c>
+      <c r="AD18" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>3824</t>
         </is>
       </c>
     </row>
@@ -1683,9 +1751,15 @@
       <c r="AB19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC19" t="inlineStr">
-        <is>
-          <t>2643</t>
+      <c r="AC19" t="n">
+        <v>2643</v>
+      </c>
+      <c r="AD19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>2673</t>
         </is>
       </c>
     </row>
@@ -1780,9 +1854,15 @@
       <c r="AB20" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AC20" t="inlineStr">
-        <is>
-          <t>3746</t>
+      <c r="AC20" t="n">
+        <v>3746</v>
+      </c>
+      <c r="AD20" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE20" t="inlineStr">
+        <is>
+          <t>4049</t>
         </is>
       </c>
     </row>
@@ -1877,9 +1957,15 @@
       <c r="AB21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC21" t="inlineStr">
-        <is>
-          <t>2719</t>
+      <c r="AC21" t="n">
+        <v>2719</v>
+      </c>
+      <c r="AD21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE21" t="inlineStr">
+        <is>
+          <t>2815</t>
         </is>
       </c>
     </row>
@@ -1974,9 +2060,15 @@
       <c r="AB22" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AC22" t="inlineStr">
-        <is>
-          <t>4012</t>
+      <c r="AC22" t="n">
+        <v>4012</v>
+      </c>
+      <c r="AD22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE22" t="inlineStr">
+        <is>
+          <t>4501</t>
         </is>
       </c>
     </row>
@@ -2071,9 +2163,15 @@
       <c r="AB23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AC23" t="inlineStr">
-        <is>
-          <t>4326</t>
+      <c r="AC23" t="n">
+        <v>4326</v>
+      </c>
+      <c r="AD23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE23" t="inlineStr">
+        <is>
+          <t>4830</t>
         </is>
       </c>
     </row>
@@ -2168,9 +2266,15 @@
       <c r="AB24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AC24" t="inlineStr">
-        <is>
-          <t>4125</t>
+      <c r="AC24" t="n">
+        <v>4125</v>
+      </c>
+      <c r="AD24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AE24" t="inlineStr">
+        <is>
+          <t>4361</t>
         </is>
       </c>
     </row>
@@ -2265,9 +2369,15 @@
       <c r="AB25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AC25" t="inlineStr">
-        <is>
-          <t>4310</t>
+      <c r="AC25" t="n">
+        <v>4310</v>
+      </c>
+      <c r="AD25" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="AE25" t="inlineStr">
+        <is>
+          <t>4537</t>
         </is>
       </c>
     </row>
@@ -2362,11 +2472,11 @@
       <c r="AB26" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC26" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="AC26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD26" s="4" t="inlineStr"/>
+      <c r="AE26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2459,7 +2569,13 @@
       <c r="AB27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC27" t="inlineStr">
+      <c r="AC27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2507,6 +2623,8 @@
       <c r="AA28" t="inlineStr"/>
       <c r="AB28" s="4" t="inlineStr"/>
       <c r="AC28" t="inlineStr"/>
+      <c r="AD28" s="4" t="inlineStr"/>
+      <c r="AE28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2599,9 +2717,15 @@
       <c r="AB29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC29" t="inlineStr">
-        <is>
-          <t>3095</t>
+      <c r="AC29" t="n">
+        <v>3095</v>
+      </c>
+      <c r="AD29" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE29" t="inlineStr">
+        <is>
+          <t>3429</t>
         </is>
       </c>
     </row>
@@ -2696,7 +2820,13 @@
       <c r="AB30" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AC30" t="inlineStr">
+      <c r="AC30" t="n">
+        <v>3598</v>
+      </c>
+      <c r="AD30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE30" t="inlineStr">
         <is>
           <t>3598</t>
         </is>
@@ -2793,9 +2923,15 @@
       <c r="AB31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AC31" t="inlineStr">
-        <is>
-          <t>4180</t>
+      <c r="AC31" t="n">
+        <v>4180</v>
+      </c>
+      <c r="AD31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE31" t="inlineStr">
+        <is>
+          <t>4450</t>
         </is>
       </c>
     </row>
@@ -2890,9 +3026,15 @@
       <c r="AB32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC32" t="inlineStr">
-        <is>
-          <t>2529</t>
+      <c r="AC32" t="n">
+        <v>2529</v>
+      </c>
+      <c r="AD32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE32" t="inlineStr">
+        <is>
+          <t>2526</t>
         </is>
       </c>
     </row>
@@ -2938,6 +3080,8 @@
       <c r="AA33" t="inlineStr"/>
       <c r="AB33" s="4" t="inlineStr"/>
       <c r="AC33" t="inlineStr"/>
+      <c r="AD33" s="4" t="inlineStr"/>
+      <c r="AE33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3030,9 +3174,15 @@
       <c r="AB34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC34" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AC34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE34" t="inlineStr">
+        <is>
+          <t>2524</t>
         </is>
       </c>
     </row>
@@ -3127,7 +3277,13 @@
       <c r="AB35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC35" t="inlineStr">
+      <c r="AC35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE35" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3224,9 +3380,15 @@
       <c r="AB36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC36" t="inlineStr">
-        <is>
-          <t>2828</t>
+      <c r="AC36" t="n">
+        <v>2828</v>
+      </c>
+      <c r="AD36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE36" t="inlineStr">
+        <is>
+          <t>2867</t>
         </is>
       </c>
     </row>
@@ -3321,9 +3483,15 @@
       <c r="AB37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AC37" t="inlineStr">
-        <is>
-          <t>3991</t>
+      <c r="AC37" t="n">
+        <v>3991</v>
+      </c>
+      <c r="AD37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE37" t="inlineStr">
+        <is>
+          <t>4312</t>
         </is>
       </c>
     </row>
@@ -3418,9 +3586,15 @@
       <c r="AB38" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AC38" t="inlineStr">
-        <is>
-          <t>4432</t>
+      <c r="AC38" t="n">
+        <v>4432</v>
+      </c>
+      <c r="AD38" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE38" t="inlineStr">
+        <is>
+          <t>4905</t>
         </is>
       </c>
     </row>
@@ -3515,9 +3689,15 @@
       <c r="AB39" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="AC39" t="inlineStr">
-        <is>
-          <t>3990</t>
+      <c r="AC39" t="n">
+        <v>3990</v>
+      </c>
+      <c r="AD39" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AE39" t="inlineStr">
+        <is>
+          <t>4280</t>
         </is>
       </c>
     </row>
@@ -3612,7 +3792,13 @@
       <c r="AB40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC40" t="inlineStr">
+      <c r="AC40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3709,9 +3895,15 @@
       <c r="AB41" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="AC41" t="inlineStr">
-        <is>
-          <t>3534</t>
+      <c r="AC41" t="n">
+        <v>3534</v>
+      </c>
+      <c r="AD41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE41" t="inlineStr">
+        <is>
+          <t>4114</t>
         </is>
       </c>
     </row>
@@ -3806,9 +3998,15 @@
       <c r="AB42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC42" t="inlineStr">
-        <is>
-          <t>2526</t>
+      <c r="AC42" t="n">
+        <v>2526</v>
+      </c>
+      <c r="AD42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE42" t="inlineStr">
+        <is>
+          <t>2656</t>
         </is>
       </c>
     </row>
@@ -3854,6 +4052,8 @@
       <c r="AA43" t="inlineStr"/>
       <c r="AB43" s="4" t="inlineStr"/>
       <c r="AC43" t="inlineStr"/>
+      <c r="AD43" s="4" t="inlineStr"/>
+      <c r="AE43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3897,6 +4097,8 @@
       <c r="AA44" t="inlineStr"/>
       <c r="AB44" s="4" t="inlineStr"/>
       <c r="AC44" t="inlineStr"/>
+      <c r="AD44" s="4" t="inlineStr"/>
+      <c r="AE44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3972,6 +4174,8 @@
       <c r="AA45" t="inlineStr"/>
       <c r="AB45" s="4" t="inlineStr"/>
       <c r="AC45" t="inlineStr"/>
+      <c r="AD45" s="4" t="inlineStr"/>
+      <c r="AE45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -4064,9 +4268,15 @@
       <c r="AB46" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="AC46" t="inlineStr">
-        <is>
-          <t>3183</t>
+      <c r="AC46" t="n">
+        <v>3183</v>
+      </c>
+      <c r="AD46" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE46" t="inlineStr">
+        <is>
+          <t>3474</t>
         </is>
       </c>
     </row>
@@ -4161,9 +4371,15 @@
       <c r="AB47" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AC47" t="inlineStr">
-        <is>
-          <t>4399</t>
+      <c r="AC47" t="n">
+        <v>4399</v>
+      </c>
+      <c r="AD47" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE47" t="inlineStr">
+        <is>
+          <t>4844</t>
         </is>
       </c>
     </row>
@@ -4258,7 +4474,13 @@
       <c r="AB48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC48" t="inlineStr">
+      <c r="AC48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4355,9 +4577,15 @@
       <c r="AB49" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC49" t="inlineStr">
-        <is>
-          <t>4020</t>
+      <c r="AC49" t="n">
+        <v>4020</v>
+      </c>
+      <c r="AD49" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AE49" t="inlineStr">
+        <is>
+          <t>4357</t>
         </is>
       </c>
     </row>
@@ -4452,9 +4680,15 @@
       <c r="AB50" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="AC50" t="inlineStr">
-        <is>
-          <t>4157</t>
+      <c r="AC50" t="n">
+        <v>4157</v>
+      </c>
+      <c r="AD50" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AE50" t="inlineStr">
+        <is>
+          <t>4532</t>
         </is>
       </c>
     </row>
@@ -4532,6 +4766,8 @@
       <c r="AA51" t="inlineStr"/>
       <c r="AB51" s="4" t="inlineStr"/>
       <c r="AC51" t="inlineStr"/>
+      <c r="AD51" s="4" t="inlineStr"/>
+      <c r="AE51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -4624,9 +4860,15 @@
       <c r="AB52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AC52" t="inlineStr">
-        <is>
-          <t>4174</t>
+      <c r="AC52" t="n">
+        <v>4174</v>
+      </c>
+      <c r="AD52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE52" t="inlineStr">
+        <is>
+          <t>4569</t>
         </is>
       </c>
     </row>
@@ -4721,9 +4963,15 @@
       <c r="AB53" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="AC53" t="inlineStr">
-        <is>
-          <t>3377</t>
+      <c r="AC53" t="n">
+        <v>3377</v>
+      </c>
+      <c r="AD53" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE53" t="inlineStr">
+        <is>
+          <t>3666</t>
         </is>
       </c>
     </row>
@@ -4801,6 +5049,8 @@
       <c r="AA54" t="inlineStr"/>
       <c r="AB54" s="4" t="inlineStr"/>
       <c r="AC54" t="inlineStr"/>
+      <c r="AD54" s="4" t="inlineStr"/>
+      <c r="AE54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -4893,9 +5143,15 @@
       <c r="AB55" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AC55" t="inlineStr">
-        <is>
-          <t>3547</t>
+      <c r="AC55" t="n">
+        <v>3547</v>
+      </c>
+      <c r="AD55" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE55" t="inlineStr">
+        <is>
+          <t>4026</t>
         </is>
       </c>
     </row>
@@ -4990,9 +5246,15 @@
       <c r="AB56" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="AC56" t="inlineStr">
-        <is>
-          <t>4228</t>
+      <c r="AC56" t="n">
+        <v>4228</v>
+      </c>
+      <c r="AD56" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="AE56" t="inlineStr">
+        <is>
+          <t>4746</t>
         </is>
       </c>
     </row>
@@ -5087,9 +5349,15 @@
       <c r="AB57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AC57" t="inlineStr">
-        <is>
-          <t>3689</t>
+      <c r="AC57" t="n">
+        <v>3689</v>
+      </c>
+      <c r="AD57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE57" t="inlineStr">
+        <is>
+          <t>4098</t>
         </is>
       </c>
     </row>
@@ -5184,9 +5452,15 @@
       <c r="AB58" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="AC58" t="inlineStr">
-        <is>
-          <t>3381</t>
+      <c r="AC58" t="n">
+        <v>3381</v>
+      </c>
+      <c r="AD58" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE58" t="inlineStr">
+        <is>
+          <t>3694</t>
         </is>
       </c>
     </row>
@@ -5281,9 +5555,15 @@
       <c r="AB59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AC59" t="inlineStr">
-        <is>
-          <t>3690</t>
+      <c r="AC59" t="n">
+        <v>3690</v>
+      </c>
+      <c r="AD59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE59" t="inlineStr">
+        <is>
+          <t>3996</t>
         </is>
       </c>
     </row>
@@ -5378,9 +5658,15 @@
       <c r="AB60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AC60" t="inlineStr">
-        <is>
-          <t>3984</t>
+      <c r="AC60" t="n">
+        <v>3984</v>
+      </c>
+      <c r="AD60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AE60" t="inlineStr">
+        <is>
+          <t>4072</t>
         </is>
       </c>
     </row>
@@ -5426,6 +5712,8 @@
       <c r="AA61" t="inlineStr"/>
       <c r="AB61" s="4" t="inlineStr"/>
       <c r="AC61" t="inlineStr"/>
+      <c r="AD61" s="4" t="inlineStr"/>
+      <c r="AE61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -5518,9 +5806,15 @@
       <c r="AB62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AC62" t="inlineStr">
-        <is>
-          <t>3489</t>
+      <c r="AC62" t="n">
+        <v>3489</v>
+      </c>
+      <c r="AD62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE62" t="inlineStr">
+        <is>
+          <t>3812</t>
         </is>
       </c>
     </row>
@@ -5615,9 +5909,15 @@
       <c r="AB63" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AC63" t="inlineStr">
-        <is>
-          <t>3678</t>
+      <c r="AC63" t="n">
+        <v>3678</v>
+      </c>
+      <c r="AD63" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE63" t="inlineStr">
+        <is>
+          <t>3990</t>
         </is>
       </c>
     </row>
@@ -5712,9 +6012,15 @@
       <c r="AB64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AC64" t="inlineStr">
-        <is>
-          <t>3970</t>
+      <c r="AC64" t="n">
+        <v>3970</v>
+      </c>
+      <c r="AD64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE64" t="inlineStr">
+        <is>
+          <t>4093</t>
         </is>
       </c>
     </row>
@@ -5809,11 +6115,11 @@
       <c r="AB65" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC65" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
+      <c r="AC65" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD65" s="4" t="inlineStr"/>
+      <c r="AE65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -5906,7 +6212,13 @@
       <c r="AB66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC66" t="inlineStr">
+      <c r="AC66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6003,7 +6315,13 @@
       <c r="AB67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC67" t="inlineStr">
+      <c r="AC67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6100,7 +6418,13 @@
       <c r="AB68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC68" t="inlineStr">
+      <c r="AC68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6148,6 +6472,8 @@
       <c r="AA69" t="inlineStr"/>
       <c r="AB69" s="4" t="inlineStr"/>
       <c r="AC69" t="inlineStr"/>
+      <c r="AD69" s="4" t="inlineStr"/>
+      <c r="AE69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -6240,7 +6566,13 @@
       <c r="AB70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC70" t="inlineStr">
+      <c r="AC70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6337,7 +6669,13 @@
       <c r="AB71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC71" t="inlineStr">
+      <c r="AC71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6434,7 +6772,13 @@
       <c r="AB72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC72" t="inlineStr">
+      <c r="AC72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6531,9 +6875,15 @@
       <c r="AB73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC73" t="inlineStr">
-        <is>
-          <t>2646</t>
+      <c r="AC73" t="n">
+        <v>2646</v>
+      </c>
+      <c r="AD73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE73" t="inlineStr">
+        <is>
+          <t>2753</t>
         </is>
       </c>
     </row>
@@ -6628,7 +6978,13 @@
       <c r="AB74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC74" t="inlineStr">
+      <c r="AC74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6725,7 +7081,13 @@
       <c r="AB75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC75" t="inlineStr">
+      <c r="AC75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6822,9 +7184,15 @@
       <c r="AB76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC76" t="inlineStr">
-        <is>
-          <t>2798</t>
+      <c r="AC76" t="n">
+        <v>2798</v>
+      </c>
+      <c r="AD76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE76" t="inlineStr">
+        <is>
+          <t>2840</t>
         </is>
       </c>
     </row>
@@ -6919,9 +7287,15 @@
       <c r="AB77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC77" t="inlineStr">
-        <is>
-          <t>2549</t>
+      <c r="AC77" t="n">
+        <v>2549</v>
+      </c>
+      <c r="AD77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE77" t="inlineStr">
+        <is>
+          <t>2582</t>
         </is>
       </c>
     </row>
@@ -7016,7 +7390,13 @@
       <c r="AB78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC78" t="inlineStr">
+      <c r="AC78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7113,7 +7493,13 @@
       <c r="AB79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC79" t="inlineStr">
+      <c r="AC79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7210,7 +7596,13 @@
       <c r="AB80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC80" t="inlineStr">
+      <c r="AC80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7307,7 +7699,13 @@
       <c r="AB81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC81" t="inlineStr">
+      <c r="AC81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7404,7 +7802,13 @@
       <c r="AB82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC82" t="inlineStr">
+      <c r="AC82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7501,7 +7905,13 @@
       <c r="AB83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC83" t="inlineStr">
+      <c r="AC83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7598,7 +8008,13 @@
       <c r="AB84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC84" t="inlineStr">
+      <c r="AC84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7695,7 +8111,13 @@
       <c r="AB85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC85" t="inlineStr">
+      <c r="AC85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7792,7 +8214,13 @@
       <c r="AB86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC86" t="inlineStr">
+      <c r="AC86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7889,7 +8317,13 @@
       <c r="AB87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC87" t="inlineStr">
+      <c r="AC87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7986,7 +8420,13 @@
       <c r="AB88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC88" t="inlineStr">
+      <c r="AC88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8083,7 +8523,13 @@
       <c r="AB89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC89" t="inlineStr">
+      <c r="AC89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8180,7 +8626,13 @@
       <c r="AB90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC90" t="inlineStr">
+      <c r="AC90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8277,7 +8729,13 @@
       <c r="AB91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC91" t="inlineStr">
+      <c r="AC91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8374,7 +8832,13 @@
       <c r="AB92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC92" t="inlineStr">
+      <c r="AC92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8471,7 +8935,13 @@
       <c r="AB93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC93" t="inlineStr">
+      <c r="AC93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8568,7 +9038,13 @@
       <c r="AB94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC94" t="inlineStr">
+      <c r="AC94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8665,7 +9141,13 @@
       <c r="AB95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC95" t="inlineStr">
+      <c r="AC95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8762,7 +9244,13 @@
       <c r="AB96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC96" t="inlineStr">
+      <c r="AC96" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE96" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8859,7 +9347,13 @@
       <c r="AB97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC97" t="inlineStr">
+      <c r="AC97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8956,7 +9450,13 @@
       <c r="AB98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC98" t="inlineStr">
+      <c r="AC98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9053,7 +9553,13 @@
       <c r="AB99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC99" t="inlineStr">
+      <c r="AC99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9150,7 +9656,13 @@
       <c r="AB100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC100" t="inlineStr">
+      <c r="AC100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9247,7 +9759,13 @@
       <c r="AB101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC101" t="inlineStr">
+      <c r="AC101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9344,7 +9862,13 @@
       <c r="AB102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC102" t="inlineStr">
+      <c r="AC102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9441,7 +9965,13 @@
       <c r="AB103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC103" t="inlineStr">
+      <c r="AC103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9538,7 +10068,13 @@
       <c r="AB104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC104" t="inlineStr">
+      <c r="AC104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9635,7 +10171,13 @@
       <c r="AB105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC105" t="inlineStr">
+      <c r="AC105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9683,6 +10225,8 @@
       <c r="AA106" t="inlineStr"/>
       <c r="AB106" s="4" t="inlineStr"/>
       <c r="AC106" t="inlineStr"/>
+      <c r="AD106" s="4" t="inlineStr"/>
+      <c r="AE106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -9726,6 +10270,8 @@
       <c r="AA107" t="inlineStr"/>
       <c r="AB107" s="4" t="inlineStr"/>
       <c r="AC107" t="inlineStr"/>
+      <c r="AD107" s="4" t="inlineStr"/>
+      <c r="AE107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -9769,6 +10315,8 @@
       <c r="AA108" t="inlineStr"/>
       <c r="AB108" s="4" t="inlineStr"/>
       <c r="AC108" t="inlineStr"/>
+      <c r="AD108" s="4" t="inlineStr"/>
+      <c r="AE108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -9812,6 +10360,8 @@
       <c r="AA109" t="inlineStr"/>
       <c r="AB109" s="4" t="inlineStr"/>
       <c r="AC109" t="inlineStr"/>
+      <c r="AD109" s="4" t="inlineStr"/>
+      <c r="AE109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -9855,6 +10405,8 @@
       <c r="AA110" t="inlineStr"/>
       <c r="AB110" s="4" t="inlineStr"/>
       <c r="AC110" t="inlineStr"/>
+      <c r="AD110" s="4" t="inlineStr"/>
+      <c r="AE110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -9898,6 +10450,8 @@
       <c r="AA111" t="inlineStr"/>
       <c r="AB111" s="4" t="inlineStr"/>
       <c r="AC111" t="inlineStr"/>
+      <c r="AD111" s="4" t="inlineStr"/>
+      <c r="AE111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -9941,6 +10495,8 @@
       <c r="AA112" t="inlineStr"/>
       <c r="AB112" s="4" t="inlineStr"/>
       <c r="AC112" t="inlineStr"/>
+      <c r="AD112" s="4" t="inlineStr"/>
+      <c r="AE112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -9984,6 +10540,8 @@
       <c r="AA113" t="inlineStr"/>
       <c r="AB113" s="4" t="inlineStr"/>
       <c r="AC113" t="inlineStr"/>
+      <c r="AD113" s="4" t="inlineStr"/>
+      <c r="AE113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -10027,6 +10585,8 @@
       <c r="AA114" t="inlineStr"/>
       <c r="AB114" s="4" t="inlineStr"/>
       <c r="AC114" t="inlineStr"/>
+      <c r="AD114" s="4" t="inlineStr"/>
+      <c r="AE114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -10097,9 +10657,15 @@
       <c r="AB115" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AC115" t="inlineStr">
-        <is>
-          <t>4465</t>
+      <c r="AC115" t="n">
+        <v>4465</v>
+      </c>
+      <c r="AD115" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AE115" t="inlineStr">
+        <is>
+          <t>4875</t>
         </is>
       </c>
     </row>
@@ -10188,7 +10754,13 @@
       <c r="AB116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC116" t="inlineStr">
+      <c r="AC116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10259,9 +10831,15 @@
       <c r="AB117" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AC117" t="inlineStr">
-        <is>
-          <t>4813</t>
+      <c r="AC117" t="n">
+        <v>4813</v>
+      </c>
+      <c r="AD117" s="5" t="n">
+        <v>40</v>
+      </c>
+      <c r="AE117" t="inlineStr">
+        <is>
+          <t>5555</t>
         </is>
       </c>
     </row>
@@ -10350,9 +10928,15 @@
       <c r="AB118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC118" t="inlineStr">
-        <is>
-          <t>2968</t>
+      <c r="AC118" t="n">
+        <v>2968</v>
+      </c>
+      <c r="AD118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE118" t="inlineStr">
+        <is>
+          <t>2986</t>
         </is>
       </c>
     </row>
@@ -10441,9 +11025,15 @@
       <c r="AB119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC119" t="inlineStr">
-        <is>
-          <t>1539</t>
+      <c r="AC119" t="n">
+        <v>1539</v>
+      </c>
+      <c r="AD119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE119" t="inlineStr">
+        <is>
+          <t>1568</t>
         </is>
       </c>
     </row>
@@ -10532,7 +11122,13 @@
       <c r="AB120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC120" t="inlineStr">
+      <c r="AC120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE120" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10623,7 +11219,13 @@
       <c r="AB121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC121" t="inlineStr">
+      <c r="AC121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10714,7 +11316,13 @@
       <c r="AB122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC122" t="inlineStr">
+      <c r="AC122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10801,7 +11409,13 @@
       <c r="AB123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC123" t="inlineStr">
+      <c r="AC123" t="n">
+        <v>2680</v>
+      </c>
+      <c r="AD123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE123" t="inlineStr">
         <is>
           <t>2680</t>
         </is>
@@ -10875,6 +11489,8 @@
       <c r="AA124" t="inlineStr"/>
       <c r="AB124" s="4" t="inlineStr"/>
       <c r="AC124" t="inlineStr"/>
+      <c r="AD124" s="4" t="inlineStr"/>
+      <c r="AE124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -10953,9 +11569,15 @@
       <c r="AB125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC125" t="inlineStr">
-        <is>
-          <t>2179</t>
+      <c r="AC125" t="n">
+        <v>2179</v>
+      </c>
+      <c r="AD125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE125" t="inlineStr">
+        <is>
+          <t>2208</t>
         </is>
       </c>
     </row>
@@ -11024,7 +11646,13 @@
       <c r="AB126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC126" t="inlineStr">
+      <c r="AC126" t="n">
+        <v>1526</v>
+      </c>
+      <c r="AD126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE126" t="inlineStr">
         <is>
           <t>1526</t>
         </is>
@@ -11090,6 +11718,8 @@
       </c>
       <c r="AB127" s="4" t="inlineStr"/>
       <c r="AC127" t="inlineStr"/>
+      <c r="AD127" s="4" t="inlineStr"/>
+      <c r="AE127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -11148,9 +11778,15 @@
       <c r="AB128" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AC128" t="inlineStr">
-        <is>
-          <t>3379</t>
+      <c r="AC128" t="n">
+        <v>3379</v>
+      </c>
+      <c r="AD128" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AE128" t="inlineStr">
+        <is>
+          <t>3813</t>
         </is>
       </c>
     </row>
@@ -11211,9 +11847,15 @@
       <c r="AB129" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="AC129" t="inlineStr">
-        <is>
-          <t>3123</t>
+      <c r="AC129" t="n">
+        <v>3123</v>
+      </c>
+      <c r="AD129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE129" t="inlineStr">
+        <is>
+          <t>3125</t>
         </is>
       </c>
     </row>
@@ -11274,9 +11916,15 @@
       <c r="AB130" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC130" t="inlineStr">
-        <is>
-          <t>1299</t>
+      <c r="AC130" t="n">
+        <v>1299</v>
+      </c>
+      <c r="AD130" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="AE130" t="inlineStr">
+        <is>
+          <t>1478</t>
         </is>
       </c>
     </row>
@@ -11333,7 +11981,13 @@
       <c r="AB131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AC131" t="inlineStr">
+      <c r="AC131" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AD131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE131" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -11380,9 +12034,15 @@
       <c r="AB132" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AC132" t="inlineStr">
-        <is>
-          <t>2971</t>
+      <c r="AC132" t="n">
+        <v>2971</v>
+      </c>
+      <c r="AD132" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE132" t="inlineStr">
+        <is>
+          <t>3751</t>
         </is>
       </c>
     </row>
@@ -11427,9 +12087,321 @@
       <c r="AB133" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="AC133" t="inlineStr">
-        <is>
-          <t>2563</t>
+      <c r="AC133" t="n">
+        <v>2563</v>
+      </c>
+      <c r="AD133" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE133" t="inlineStr">
+        <is>
+          <t>3142</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>8741713</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">㊥大咖玩家ky </t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr"/>
+      <c r="D134" t="inlineStr"/>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F134" s="4" t="inlineStr"/>
+      <c r="G134" t="inlineStr"/>
+      <c r="H134" s="4" t="inlineStr"/>
+      <c r="I134" t="inlineStr"/>
+      <c r="J134" s="4" t="inlineStr"/>
+      <c r="K134" t="inlineStr"/>
+      <c r="L134" s="4" t="inlineStr"/>
+      <c r="M134" t="inlineStr"/>
+      <c r="N134" s="4" t="inlineStr"/>
+      <c r="O134" t="inlineStr"/>
+      <c r="P134" s="4" t="inlineStr"/>
+      <c r="Q134" t="inlineStr"/>
+      <c r="R134" s="4" t="inlineStr"/>
+      <c r="S134" t="inlineStr"/>
+      <c r="T134" s="4" t="inlineStr"/>
+      <c r="U134" t="inlineStr"/>
+      <c r="V134" s="4" t="inlineStr"/>
+      <c r="W134" t="inlineStr"/>
+      <c r="X134" s="4" t="inlineStr"/>
+      <c r="Y134" t="inlineStr"/>
+      <c r="Z134" s="4" t="inlineStr"/>
+      <c r="AA134" t="inlineStr"/>
+      <c r="AB134" s="4" t="inlineStr"/>
+      <c r="AC134" t="inlineStr"/>
+      <c r="AD134" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AE134" t="inlineStr">
+        <is>
+          <t>5434</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>57454274</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Player-57454274</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr"/>
+      <c r="D135" t="inlineStr"/>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F135" s="4" t="inlineStr"/>
+      <c r="G135" t="inlineStr"/>
+      <c r="H135" s="4" t="inlineStr"/>
+      <c r="I135" t="inlineStr"/>
+      <c r="J135" s="4" t="inlineStr"/>
+      <c r="K135" t="inlineStr"/>
+      <c r="L135" s="4" t="inlineStr"/>
+      <c r="M135" t="inlineStr"/>
+      <c r="N135" s="4" t="inlineStr"/>
+      <c r="O135" t="inlineStr"/>
+      <c r="P135" s="4" t="inlineStr"/>
+      <c r="Q135" t="inlineStr"/>
+      <c r="R135" s="4" t="inlineStr"/>
+      <c r="S135" t="inlineStr"/>
+      <c r="T135" s="4" t="inlineStr"/>
+      <c r="U135" t="inlineStr"/>
+      <c r="V135" s="4" t="inlineStr"/>
+      <c r="W135" t="inlineStr"/>
+      <c r="X135" s="4" t="inlineStr"/>
+      <c r="Y135" t="inlineStr"/>
+      <c r="Z135" s="4" t="inlineStr"/>
+      <c r="AA135" t="inlineStr"/>
+      <c r="AB135" s="4" t="inlineStr"/>
+      <c r="AC135" t="inlineStr"/>
+      <c r="AD135" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE135" t="inlineStr">
+        <is>
+          <t>1635</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>3946814</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>"小瑩 潘"</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr"/>
+      <c r="D136" t="inlineStr"/>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F136" s="4" t="inlineStr"/>
+      <c r="G136" t="inlineStr"/>
+      <c r="H136" s="4" t="inlineStr"/>
+      <c r="I136" t="inlineStr"/>
+      <c r="J136" s="4" t="inlineStr"/>
+      <c r="K136" t="inlineStr"/>
+      <c r="L136" s="4" t="inlineStr"/>
+      <c r="M136" t="inlineStr"/>
+      <c r="N136" s="4" t="inlineStr"/>
+      <c r="O136" t="inlineStr"/>
+      <c r="P136" s="4" t="inlineStr"/>
+      <c r="Q136" t="inlineStr"/>
+      <c r="R136" s="4" t="inlineStr"/>
+      <c r="S136" t="inlineStr"/>
+      <c r="T136" s="4" t="inlineStr"/>
+      <c r="U136" t="inlineStr"/>
+      <c r="V136" s="4" t="inlineStr"/>
+      <c r="W136" t="inlineStr"/>
+      <c r="X136" s="4" t="inlineStr"/>
+      <c r="Y136" t="inlineStr"/>
+      <c r="Z136" s="4" t="inlineStr"/>
+      <c r="AA136" t="inlineStr"/>
+      <c r="AB136" s="4" t="inlineStr"/>
+      <c r="AC136" t="inlineStr"/>
+      <c r="AD136" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AE136" t="inlineStr">
+        <is>
+          <t>5335</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>6940556</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>"Cry ab it林黛玉ᶻᵍˣ"</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr"/>
+      <c r="D137" t="inlineStr"/>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F137" s="4" t="inlineStr"/>
+      <c r="G137" t="inlineStr"/>
+      <c r="H137" s="4" t="inlineStr"/>
+      <c r="I137" t="inlineStr"/>
+      <c r="J137" s="4" t="inlineStr"/>
+      <c r="K137" t="inlineStr"/>
+      <c r="L137" s="4" t="inlineStr"/>
+      <c r="M137" t="inlineStr"/>
+      <c r="N137" s="4" t="inlineStr"/>
+      <c r="O137" t="inlineStr"/>
+      <c r="P137" s="4" t="inlineStr"/>
+      <c r="Q137" t="inlineStr"/>
+      <c r="R137" s="4" t="inlineStr"/>
+      <c r="S137" t="inlineStr"/>
+      <c r="T137" s="4" t="inlineStr"/>
+      <c r="U137" t="inlineStr"/>
+      <c r="V137" s="4" t="inlineStr"/>
+      <c r="W137" t="inlineStr"/>
+      <c r="X137" s="4" t="inlineStr"/>
+      <c r="Y137" t="inlineStr"/>
+      <c r="Z137" s="4" t="inlineStr"/>
+      <c r="AA137" t="inlineStr"/>
+      <c r="AB137" s="4" t="inlineStr"/>
+      <c r="AC137" t="inlineStr"/>
+      <c r="AD137" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE137" t="inlineStr">
+        <is>
+          <t>5525</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>25376635</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>"sanchez ᶻᵍˣ"</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr"/>
+      <c r="D138" t="inlineStr"/>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F138" s="4" t="inlineStr"/>
+      <c r="G138" t="inlineStr"/>
+      <c r="H138" s="4" t="inlineStr"/>
+      <c r="I138" t="inlineStr"/>
+      <c r="J138" s="4" t="inlineStr"/>
+      <c r="K138" t="inlineStr"/>
+      <c r="L138" s="4" t="inlineStr"/>
+      <c r="M138" t="inlineStr"/>
+      <c r="N138" s="4" t="inlineStr"/>
+      <c r="O138" t="inlineStr"/>
+      <c r="P138" s="4" t="inlineStr"/>
+      <c r="Q138" t="inlineStr"/>
+      <c r="R138" s="4" t="inlineStr"/>
+      <c r="S138" t="inlineStr"/>
+      <c r="T138" s="4" t="inlineStr"/>
+      <c r="U138" t="inlineStr"/>
+      <c r="V138" s="4" t="inlineStr"/>
+      <c r="W138" t="inlineStr"/>
+      <c r="X138" s="4" t="inlineStr"/>
+      <c r="Y138" t="inlineStr"/>
+      <c r="Z138" s="4" t="inlineStr"/>
+      <c r="AA138" t="inlineStr"/>
+      <c r="AB138" s="4" t="inlineStr"/>
+      <c r="AC138" t="inlineStr"/>
+      <c r="AD138" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AE138" t="inlineStr">
+        <is>
+          <t>4965</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>29211638</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>"㊥ PhononDisperse"</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr"/>
+      <c r="D139" t="inlineStr"/>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F139" s="4" t="inlineStr"/>
+      <c r="G139" t="inlineStr"/>
+      <c r="H139" s="4" t="inlineStr"/>
+      <c r="I139" t="inlineStr"/>
+      <c r="J139" s="4" t="inlineStr"/>
+      <c r="K139" t="inlineStr"/>
+      <c r="L139" s="4" t="inlineStr"/>
+      <c r="M139" t="inlineStr"/>
+      <c r="N139" s="4" t="inlineStr"/>
+      <c r="O139" t="inlineStr"/>
+      <c r="P139" s="4" t="inlineStr"/>
+      <c r="Q139" t="inlineStr"/>
+      <c r="R139" s="4" t="inlineStr"/>
+      <c r="S139" t="inlineStr"/>
+      <c r="T139" s="4" t="inlineStr"/>
+      <c r="U139" t="inlineStr"/>
+      <c r="V139" s="4" t="inlineStr"/>
+      <c r="W139" t="inlineStr"/>
+      <c r="X139" s="4" t="inlineStr"/>
+      <c r="Y139" t="inlineStr"/>
+      <c r="Z139" s="4" t="inlineStr"/>
+      <c r="AA139" t="inlineStr"/>
+      <c r="AB139" s="4" t="inlineStr"/>
+      <c r="AC139" t="inlineStr"/>
+      <c r="AD139" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AE139" t="inlineStr">
+        <is>
+          <t>5431</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-29 21:41:18
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE139"/>
+  <dimension ref="A1:AG139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,6 +546,16 @@
           <t>05-27_0</t>
         </is>
       </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>05-28_A</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>05-28_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -644,9 +654,15 @@
       <c r="AD2" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>3450</t>
+      <c r="AE2" t="n">
+        <v>3450</v>
+      </c>
+      <c r="AF2" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>3908</t>
         </is>
       </c>
     </row>
@@ -747,7 +763,13 @@
       <c r="AD3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE3" t="inlineStr">
+      <c r="AE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -850,7 +872,13 @@
       <c r="AD4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE4" t="inlineStr">
+      <c r="AE4" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AF4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG4" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -953,9 +981,15 @@
       <c r="AD5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t>2720</t>
+      <c r="AE5" t="n">
+        <v>2720</v>
+      </c>
+      <c r="AF5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>2733</t>
         </is>
       </c>
     </row>
@@ -1056,7 +1090,13 @@
       <c r="AD6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE6" t="inlineStr">
+      <c r="AE6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1106,6 +1146,8 @@
       <c r="AC7" t="inlineStr"/>
       <c r="AD7" s="4" t="inlineStr"/>
       <c r="AE7" t="inlineStr"/>
+      <c r="AF7" s="4" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1151,6 +1193,8 @@
       <c r="AC8" t="inlineStr"/>
       <c r="AD8" s="4" t="inlineStr"/>
       <c r="AE8" t="inlineStr"/>
+      <c r="AF8" s="4" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1196,6 +1240,8 @@
       <c r="AC9" t="inlineStr"/>
       <c r="AD9" s="4" t="inlineStr"/>
       <c r="AE9" t="inlineStr"/>
+      <c r="AF9" s="4" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1241,6 +1287,8 @@
       <c r="AC10" t="inlineStr"/>
       <c r="AD10" s="4" t="inlineStr"/>
       <c r="AE10" t="inlineStr"/>
+      <c r="AF10" s="4" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1286,6 +1334,8 @@
       <c r="AC11" t="inlineStr"/>
       <c r="AD11" s="4" t="inlineStr"/>
       <c r="AE11" t="inlineStr"/>
+      <c r="AF11" s="4" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1331,6 +1381,8 @@
       <c r="AC12" t="inlineStr"/>
       <c r="AD12" s="4" t="inlineStr"/>
       <c r="AE12" t="inlineStr"/>
+      <c r="AF12" s="4" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1376,6 +1428,8 @@
       <c r="AC13" t="inlineStr"/>
       <c r="AD13" s="4" t="inlineStr"/>
       <c r="AE13" t="inlineStr"/>
+      <c r="AF13" s="4" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1421,6 +1475,8 @@
       <c r="AC14" t="inlineStr"/>
       <c r="AD14" s="4" t="inlineStr"/>
       <c r="AE14" t="inlineStr"/>
+      <c r="AF14" s="4" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1466,6 +1522,8 @@
       <c r="AC15" t="inlineStr"/>
       <c r="AD15" s="4" t="inlineStr"/>
       <c r="AE15" t="inlineStr"/>
+      <c r="AF15" s="4" t="inlineStr"/>
+      <c r="AG15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1511,6 +1569,8 @@
       <c r="AC16" t="inlineStr"/>
       <c r="AD16" s="4" t="inlineStr"/>
       <c r="AE16" t="inlineStr"/>
+      <c r="AF16" s="4" t="inlineStr"/>
+      <c r="AG16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1556,6 +1616,8 @@
       <c r="AC17" t="inlineStr"/>
       <c r="AD17" s="4" t="inlineStr"/>
       <c r="AE17" t="inlineStr"/>
+      <c r="AF17" s="4" t="inlineStr"/>
+      <c r="AG17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1654,9 +1716,15 @@
       <c r="AD18" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE18" t="inlineStr">
-        <is>
-          <t>3824</t>
+      <c r="AE18" t="n">
+        <v>3824</v>
+      </c>
+      <c r="AF18" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG18" t="inlineStr">
+        <is>
+          <t>3977</t>
         </is>
       </c>
     </row>
@@ -1757,9 +1825,15 @@
       <c r="AD19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE19" t="inlineStr">
-        <is>
-          <t>2673</t>
+      <c r="AE19" t="n">
+        <v>2673</v>
+      </c>
+      <c r="AF19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG19" t="inlineStr">
+        <is>
+          <t>2703</t>
         </is>
       </c>
     </row>
@@ -1860,9 +1934,15 @@
       <c r="AD20" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AE20" t="inlineStr">
-        <is>
-          <t>4049</t>
+      <c r="AE20" t="n">
+        <v>4049</v>
+      </c>
+      <c r="AF20" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG20" t="inlineStr">
+        <is>
+          <t>4234</t>
         </is>
       </c>
     </row>
@@ -1963,9 +2043,15 @@
       <c r="AD21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE21" t="inlineStr">
-        <is>
-          <t>2815</t>
+      <c r="AE21" t="n">
+        <v>2815</v>
+      </c>
+      <c r="AF21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG21" t="inlineStr">
+        <is>
+          <t>2879</t>
         </is>
       </c>
     </row>
@@ -2066,9 +2152,15 @@
       <c r="AD22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE22" t="inlineStr">
-        <is>
-          <t>4501</t>
+      <c r="AE22" t="n">
+        <v>4501</v>
+      </c>
+      <c r="AF22" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AG22" t="inlineStr">
+        <is>
+          <t>4657</t>
         </is>
       </c>
     </row>
@@ -2169,9 +2261,15 @@
       <c r="AD23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AE23" t="inlineStr">
-        <is>
-          <t>4830</t>
+      <c r="AE23" t="n">
+        <v>4830</v>
+      </c>
+      <c r="AF23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AG23" t="inlineStr">
+        <is>
+          <t>5083</t>
         </is>
       </c>
     </row>
@@ -2272,9 +2370,15 @@
       <c r="AD24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AE24" t="inlineStr">
-        <is>
-          <t>4361</t>
+      <c r="AE24" t="n">
+        <v>4361</v>
+      </c>
+      <c r="AF24" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AG24" t="inlineStr">
+        <is>
+          <t>4538</t>
         </is>
       </c>
     </row>
@@ -2375,9 +2479,15 @@
       <c r="AD25" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="AE25" t="inlineStr">
-        <is>
-          <t>4537</t>
+      <c r="AE25" t="n">
+        <v>4537</v>
+      </c>
+      <c r="AF25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG25" t="inlineStr">
+        <is>
+          <t>4977</t>
         </is>
       </c>
     </row>
@@ -2477,6 +2587,8 @@
       </c>
       <c r="AD26" s="4" t="inlineStr"/>
       <c r="AE26" t="inlineStr"/>
+      <c r="AF26" s="4" t="inlineStr"/>
+      <c r="AG26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2575,7 +2687,13 @@
       <c r="AD27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE27" t="inlineStr">
+      <c r="AE27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2625,6 +2743,8 @@
       <c r="AC28" t="inlineStr"/>
       <c r="AD28" s="4" t="inlineStr"/>
       <c r="AE28" t="inlineStr"/>
+      <c r="AF28" s="4" t="inlineStr"/>
+      <c r="AG28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2723,7 +2843,13 @@
       <c r="AD29" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE29" t="inlineStr">
+      <c r="AE29" t="n">
+        <v>3429</v>
+      </c>
+      <c r="AF29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG29" t="inlineStr">
         <is>
           <t>3429</t>
         </is>
@@ -2826,7 +2952,13 @@
       <c r="AD30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE30" t="inlineStr">
+      <c r="AE30" t="n">
+        <v>3598</v>
+      </c>
+      <c r="AF30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG30" t="inlineStr">
         <is>
           <t>3598</t>
         </is>
@@ -2929,9 +3061,15 @@
       <c r="AD31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AE31" t="inlineStr">
-        <is>
-          <t>4450</t>
+      <c r="AE31" t="n">
+        <v>4450</v>
+      </c>
+      <c r="AF31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG31" t="inlineStr">
+        <is>
+          <t>4661</t>
         </is>
       </c>
     </row>
@@ -3032,7 +3170,13 @@
       <c r="AD32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE32" t="inlineStr">
+      <c r="AE32" t="n">
+        <v>2526</v>
+      </c>
+      <c r="AF32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG32" t="inlineStr">
         <is>
           <t>2526</t>
         </is>
@@ -3082,6 +3226,8 @@
       <c r="AC33" t="inlineStr"/>
       <c r="AD33" s="4" t="inlineStr"/>
       <c r="AE33" t="inlineStr"/>
+      <c r="AF33" s="4" t="inlineStr"/>
+      <c r="AG33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3180,9 +3326,15 @@
       <c r="AD34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE34" t="inlineStr">
-        <is>
-          <t>2524</t>
+      <c r="AE34" t="n">
+        <v>2524</v>
+      </c>
+      <c r="AF34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG34" t="inlineStr">
+        <is>
+          <t>2548</t>
         </is>
       </c>
     </row>
@@ -3283,7 +3435,13 @@
       <c r="AD35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE35" t="inlineStr">
+      <c r="AE35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG35" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3386,9 +3544,15 @@
       <c r="AD36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE36" t="inlineStr">
-        <is>
-          <t>2867</t>
+      <c r="AE36" t="n">
+        <v>2867</v>
+      </c>
+      <c r="AF36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG36" t="inlineStr">
+        <is>
+          <t>2892</t>
         </is>
       </c>
     </row>
@@ -3489,9 +3653,15 @@
       <c r="AD37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AE37" t="inlineStr">
-        <is>
-          <t>4312</t>
+      <c r="AE37" t="n">
+        <v>4312</v>
+      </c>
+      <c r="AF37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG37" t="inlineStr">
+        <is>
+          <t>4452</t>
         </is>
       </c>
     </row>
@@ -3592,9 +3762,15 @@
       <c r="AD38" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AE38" t="inlineStr">
-        <is>
-          <t>4905</t>
+      <c r="AE38" t="n">
+        <v>4905</v>
+      </c>
+      <c r="AF38" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AG38" t="inlineStr">
+        <is>
+          <t>5086</t>
         </is>
       </c>
     </row>
@@ -3695,9 +3871,15 @@
       <c r="AD39" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AE39" t="inlineStr">
-        <is>
-          <t>4280</t>
+      <c r="AE39" t="n">
+        <v>4280</v>
+      </c>
+      <c r="AF39" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="AG39" t="inlineStr">
+        <is>
+          <t>4413</t>
         </is>
       </c>
     </row>
@@ -3798,7 +3980,13 @@
       <c r="AD40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE40" t="inlineStr">
+      <c r="AE40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3901,9 +4089,15 @@
       <c r="AD41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE41" t="inlineStr">
-        <is>
-          <t>4114</t>
+      <c r="AE41" t="n">
+        <v>4114</v>
+      </c>
+      <c r="AF41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG41" t="inlineStr">
+        <is>
+          <t>4186</t>
         </is>
       </c>
     </row>
@@ -4004,9 +4198,15 @@
       <c r="AD42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE42" t="inlineStr">
-        <is>
-          <t>2656</t>
+      <c r="AE42" t="n">
+        <v>2656</v>
+      </c>
+      <c r="AF42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG42" t="inlineStr">
+        <is>
+          <t>2664</t>
         </is>
       </c>
     </row>
@@ -4054,6 +4254,8 @@
       <c r="AC43" t="inlineStr"/>
       <c r="AD43" s="4" t="inlineStr"/>
       <c r="AE43" t="inlineStr"/>
+      <c r="AF43" s="4" t="inlineStr"/>
+      <c r="AG43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -4099,6 +4301,8 @@
       <c r="AC44" t="inlineStr"/>
       <c r="AD44" s="4" t="inlineStr"/>
       <c r="AE44" t="inlineStr"/>
+      <c r="AF44" s="4" t="inlineStr"/>
+      <c r="AG44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -4176,6 +4380,8 @@
       <c r="AC45" t="inlineStr"/>
       <c r="AD45" s="4" t="inlineStr"/>
       <c r="AE45" t="inlineStr"/>
+      <c r="AF45" s="4" t="inlineStr"/>
+      <c r="AG45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -4274,9 +4480,15 @@
       <c r="AD46" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="AE46" t="inlineStr">
-        <is>
-          <t>3474</t>
+      <c r="AE46" t="n">
+        <v>3474</v>
+      </c>
+      <c r="AF46" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="AG46" t="inlineStr">
+        <is>
+          <t>3681</t>
         </is>
       </c>
     </row>
@@ -4377,9 +4589,15 @@
       <c r="AD47" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AE47" t="inlineStr">
-        <is>
-          <t>4844</t>
+      <c r="AE47" t="n">
+        <v>4844</v>
+      </c>
+      <c r="AF47" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AG47" t="inlineStr">
+        <is>
+          <t>5041</t>
         </is>
       </c>
     </row>
@@ -4480,7 +4698,13 @@
       <c r="AD48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE48" t="inlineStr">
+      <c r="AE48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4583,9 +4807,15 @@
       <c r="AD49" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AE49" t="inlineStr">
-        <is>
-          <t>4357</t>
+      <c r="AE49" t="n">
+        <v>4357</v>
+      </c>
+      <c r="AF49" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AG49" t="inlineStr">
+        <is>
+          <t>4510</t>
         </is>
       </c>
     </row>
@@ -4686,9 +4916,15 @@
       <c r="AD50" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="AE50" t="inlineStr">
-        <is>
-          <t>4532</t>
+      <c r="AE50" t="n">
+        <v>4532</v>
+      </c>
+      <c r="AF50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AG50" t="inlineStr">
+        <is>
+          <t>4679</t>
         </is>
       </c>
     </row>
@@ -4768,6 +5004,8 @@
       <c r="AC51" t="inlineStr"/>
       <c r="AD51" s="4" t="inlineStr"/>
       <c r="AE51" t="inlineStr"/>
+      <c r="AF51" s="4" t="inlineStr"/>
+      <c r="AG51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -4866,9 +5104,15 @@
       <c r="AD52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AE52" t="inlineStr">
-        <is>
-          <t>4569</t>
+      <c r="AE52" t="n">
+        <v>4569</v>
+      </c>
+      <c r="AF52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG52" t="inlineStr">
+        <is>
+          <t>4780</t>
         </is>
       </c>
     </row>
@@ -4969,9 +5213,15 @@
       <c r="AD53" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="AE53" t="inlineStr">
-        <is>
-          <t>3666</t>
+      <c r="AE53" t="n">
+        <v>3666</v>
+      </c>
+      <c r="AF53" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG53" t="inlineStr">
+        <is>
+          <t>3880</t>
         </is>
       </c>
     </row>
@@ -5051,6 +5301,8 @@
       <c r="AC54" t="inlineStr"/>
       <c r="AD54" s="4" t="inlineStr"/>
       <c r="AE54" t="inlineStr"/>
+      <c r="AF54" s="4" t="inlineStr"/>
+      <c r="AG54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -5149,9 +5401,15 @@
       <c r="AD55" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE55" t="inlineStr">
-        <is>
-          <t>4026</t>
+      <c r="AE55" t="n">
+        <v>4026</v>
+      </c>
+      <c r="AF55" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG55" t="inlineStr">
+        <is>
+          <t>4178</t>
         </is>
       </c>
     </row>
@@ -5252,9 +5510,15 @@
       <c r="AD56" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="AE56" t="inlineStr">
-        <is>
-          <t>4746</t>
+      <c r="AE56" t="n">
+        <v>4746</v>
+      </c>
+      <c r="AF56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG56" t="inlineStr">
+        <is>
+          <t>4941</t>
         </is>
       </c>
     </row>
@@ -5355,9 +5619,15 @@
       <c r="AD57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE57" t="inlineStr">
-        <is>
-          <t>4098</t>
+      <c r="AE57" t="n">
+        <v>4098</v>
+      </c>
+      <c r="AF57" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="AG57" t="inlineStr">
+        <is>
+          <t>4171</t>
         </is>
       </c>
     </row>
@@ -5458,9 +5728,15 @@
       <c r="AD58" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE58" t="inlineStr">
-        <is>
-          <t>3694</t>
+      <c r="AE58" t="n">
+        <v>3694</v>
+      </c>
+      <c r="AF58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AG58" t="inlineStr">
+        <is>
+          <t>3988</t>
         </is>
       </c>
     </row>
@@ -5561,9 +5837,15 @@
       <c r="AD59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE59" t="inlineStr">
-        <is>
-          <t>3996</t>
+      <c r="AE59" t="n">
+        <v>3996</v>
+      </c>
+      <c r="AF59" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AG59" t="inlineStr">
+        <is>
+          <t>4012</t>
         </is>
       </c>
     </row>
@@ -5664,9 +5946,15 @@
       <c r="AD60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AE60" t="inlineStr">
-        <is>
-          <t>4072</t>
+      <c r="AE60" t="n">
+        <v>4072</v>
+      </c>
+      <c r="AF60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AG60" t="inlineStr">
+        <is>
+          <t>4186</t>
         </is>
       </c>
     </row>
@@ -5714,6 +6002,8 @@
       <c r="AC61" t="inlineStr"/>
       <c r="AD61" s="4" t="inlineStr"/>
       <c r="AE61" t="inlineStr"/>
+      <c r="AF61" s="4" t="inlineStr"/>
+      <c r="AG61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -5812,9 +6102,15 @@
       <c r="AD62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AE62" t="inlineStr">
-        <is>
-          <t>3812</t>
+      <c r="AE62" t="n">
+        <v>3812</v>
+      </c>
+      <c r="AF62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG62" t="inlineStr">
+        <is>
+          <t>3974</t>
         </is>
       </c>
     </row>
@@ -5915,9 +6211,15 @@
       <c r="AD63" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE63" t="inlineStr">
-        <is>
-          <t>3990</t>
+      <c r="AE63" t="n">
+        <v>3990</v>
+      </c>
+      <c r="AF63" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG63" t="inlineStr">
+        <is>
+          <t>4021</t>
         </is>
       </c>
     </row>
@@ -6018,9 +6320,15 @@
       <c r="AD64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE64" t="inlineStr">
-        <is>
-          <t>4093</t>
+      <c r="AE64" t="n">
+        <v>4093</v>
+      </c>
+      <c r="AF64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG64" t="inlineStr">
+        <is>
+          <t>4199</t>
         </is>
       </c>
     </row>
@@ -6120,6 +6428,8 @@
       </c>
       <c r="AD65" s="4" t="inlineStr"/>
       <c r="AE65" t="inlineStr"/>
+      <c r="AF65" s="4" t="inlineStr"/>
+      <c r="AG65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -6218,7 +6528,13 @@
       <c r="AD66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE66" t="inlineStr">
+      <c r="AE66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6321,7 +6637,13 @@
       <c r="AD67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE67" t="inlineStr">
+      <c r="AE67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6424,7 +6746,13 @@
       <c r="AD68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE68" t="inlineStr">
+      <c r="AE68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6474,6 +6802,8 @@
       <c r="AC69" t="inlineStr"/>
       <c r="AD69" s="4" t="inlineStr"/>
       <c r="AE69" t="inlineStr"/>
+      <c r="AF69" s="4" t="inlineStr"/>
+      <c r="AG69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -6572,7 +6902,13 @@
       <c r="AD70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE70" t="inlineStr">
+      <c r="AE70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6675,7 +7011,13 @@
       <c r="AD71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE71" t="inlineStr">
+      <c r="AE71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6778,7 +7120,13 @@
       <c r="AD72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE72" t="inlineStr">
+      <c r="AE72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6881,9 +7229,15 @@
       <c r="AD73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE73" t="inlineStr">
-        <is>
-          <t>2753</t>
+      <c r="AE73" t="n">
+        <v>2753</v>
+      </c>
+      <c r="AF73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG73" t="inlineStr">
+        <is>
+          <t>2805</t>
         </is>
       </c>
     </row>
@@ -6984,7 +7338,13 @@
       <c r="AD74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE74" t="inlineStr">
+      <c r="AE74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7087,7 +7447,13 @@
       <c r="AD75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE75" t="inlineStr">
+      <c r="AE75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7190,9 +7556,15 @@
       <c r="AD76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE76" t="inlineStr">
-        <is>
-          <t>2840</t>
+      <c r="AE76" t="n">
+        <v>2840</v>
+      </c>
+      <c r="AF76" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG76" t="inlineStr">
+        <is>
+          <t>2894</t>
         </is>
       </c>
     </row>
@@ -7293,9 +7665,15 @@
       <c r="AD77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE77" t="inlineStr">
-        <is>
-          <t>2582</t>
+      <c r="AE77" t="n">
+        <v>2582</v>
+      </c>
+      <c r="AF77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG77" t="inlineStr">
+        <is>
+          <t>2608</t>
         </is>
       </c>
     </row>
@@ -7396,7 +7774,13 @@
       <c r="AD78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE78" t="inlineStr">
+      <c r="AE78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7499,7 +7883,13 @@
       <c r="AD79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE79" t="inlineStr">
+      <c r="AE79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7602,7 +7992,13 @@
       <c r="AD80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE80" t="inlineStr">
+      <c r="AE80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7705,7 +8101,13 @@
       <c r="AD81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE81" t="inlineStr">
+      <c r="AE81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7808,7 +8210,13 @@
       <c r="AD82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE82" t="inlineStr">
+      <c r="AE82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7911,7 +8319,13 @@
       <c r="AD83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE83" t="inlineStr">
+      <c r="AE83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8014,7 +8428,13 @@
       <c r="AD84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE84" t="inlineStr">
+      <c r="AE84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8117,7 +8537,13 @@
       <c r="AD85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE85" t="inlineStr">
+      <c r="AE85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8220,7 +8646,13 @@
       <c r="AD86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE86" t="inlineStr">
+      <c r="AE86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8323,7 +8755,13 @@
       <c r="AD87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE87" t="inlineStr">
+      <c r="AE87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8426,7 +8864,13 @@
       <c r="AD88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE88" t="inlineStr">
+      <c r="AE88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8529,7 +8973,13 @@
       <c r="AD89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE89" t="inlineStr">
+      <c r="AE89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8632,7 +9082,13 @@
       <c r="AD90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE90" t="inlineStr">
+      <c r="AE90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8735,7 +9191,13 @@
       <c r="AD91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE91" t="inlineStr">
+      <c r="AE91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8838,7 +9300,13 @@
       <c r="AD92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE92" t="inlineStr">
+      <c r="AE92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8941,7 +9409,13 @@
       <c r="AD93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE93" t="inlineStr">
+      <c r="AE93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9044,7 +9518,13 @@
       <c r="AD94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE94" t="inlineStr">
+      <c r="AE94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9147,7 +9627,13 @@
       <c r="AD95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE95" t="inlineStr">
+      <c r="AE95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9250,7 +9736,13 @@
       <c r="AD96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE96" t="inlineStr">
+      <c r="AE96" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG96" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9353,7 +9845,13 @@
       <c r="AD97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE97" t="inlineStr">
+      <c r="AE97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9456,7 +9954,13 @@
       <c r="AD98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE98" t="inlineStr">
+      <c r="AE98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9559,7 +10063,13 @@
       <c r="AD99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE99" t="inlineStr">
+      <c r="AE99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9662,7 +10172,13 @@
       <c r="AD100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE100" t="inlineStr">
+      <c r="AE100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9765,7 +10281,13 @@
       <c r="AD101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE101" t="inlineStr">
+      <c r="AE101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9868,7 +10390,13 @@
       <c r="AD102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE102" t="inlineStr">
+      <c r="AE102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9971,7 +10499,13 @@
       <c r="AD103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE103" t="inlineStr">
+      <c r="AE103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10074,7 +10608,13 @@
       <c r="AD104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE104" t="inlineStr">
+      <c r="AE104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10177,7 +10717,13 @@
       <c r="AD105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE105" t="inlineStr">
+      <c r="AE105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10227,6 +10773,8 @@
       <c r="AC106" t="inlineStr"/>
       <c r="AD106" s="4" t="inlineStr"/>
       <c r="AE106" t="inlineStr"/>
+      <c r="AF106" s="4" t="inlineStr"/>
+      <c r="AG106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -10272,6 +10820,8 @@
       <c r="AC107" t="inlineStr"/>
       <c r="AD107" s="4" t="inlineStr"/>
       <c r="AE107" t="inlineStr"/>
+      <c r="AF107" s="4" t="inlineStr"/>
+      <c r="AG107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -10317,6 +10867,8 @@
       <c r="AC108" t="inlineStr"/>
       <c r="AD108" s="4" t="inlineStr"/>
       <c r="AE108" t="inlineStr"/>
+      <c r="AF108" s="4" t="inlineStr"/>
+      <c r="AG108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -10362,6 +10914,8 @@
       <c r="AC109" t="inlineStr"/>
       <c r="AD109" s="4" t="inlineStr"/>
       <c r="AE109" t="inlineStr"/>
+      <c r="AF109" s="4" t="inlineStr"/>
+      <c r="AG109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -10407,6 +10961,8 @@
       <c r="AC110" t="inlineStr"/>
       <c r="AD110" s="4" t="inlineStr"/>
       <c r="AE110" t="inlineStr"/>
+      <c r="AF110" s="4" t="inlineStr"/>
+      <c r="AG110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -10452,6 +11008,8 @@
       <c r="AC111" t="inlineStr"/>
       <c r="AD111" s="4" t="inlineStr"/>
       <c r="AE111" t="inlineStr"/>
+      <c r="AF111" s="4" t="inlineStr"/>
+      <c r="AG111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -10497,6 +11055,8 @@
       <c r="AC112" t="inlineStr"/>
       <c r="AD112" s="4" t="inlineStr"/>
       <c r="AE112" t="inlineStr"/>
+      <c r="AF112" s="4" t="inlineStr"/>
+      <c r="AG112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -10542,6 +11102,8 @@
       <c r="AC113" t="inlineStr"/>
       <c r="AD113" s="4" t="inlineStr"/>
       <c r="AE113" t="inlineStr"/>
+      <c r="AF113" s="4" t="inlineStr"/>
+      <c r="AG113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -10587,6 +11149,8 @@
       <c r="AC114" t="inlineStr"/>
       <c r="AD114" s="4" t="inlineStr"/>
       <c r="AE114" t="inlineStr"/>
+      <c r="AF114" s="4" t="inlineStr"/>
+      <c r="AG114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -10663,9 +11227,15 @@
       <c r="AD115" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AE115" t="inlineStr">
-        <is>
-          <t>4875</t>
+      <c r="AE115" t="n">
+        <v>4875</v>
+      </c>
+      <c r="AF115" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG115" t="inlineStr">
+        <is>
+          <t>5083</t>
         </is>
       </c>
     </row>
@@ -10760,7 +11330,13 @@
       <c r="AD116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE116" t="inlineStr">
+      <c r="AE116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10837,9 +11413,15 @@
       <c r="AD117" s="5" t="n">
         <v>40</v>
       </c>
-      <c r="AE117" t="inlineStr">
-        <is>
-          <t>5555</t>
+      <c r="AE117" t="n">
+        <v>5555</v>
+      </c>
+      <c r="AF117" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AG117" t="inlineStr">
+        <is>
+          <t>5994</t>
         </is>
       </c>
     </row>
@@ -10934,9 +11516,15 @@
       <c r="AD118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE118" t="inlineStr">
-        <is>
-          <t>2986</t>
+      <c r="AE118" t="n">
+        <v>2986</v>
+      </c>
+      <c r="AF118" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="AG118" t="inlineStr">
+        <is>
+          <t>3304</t>
         </is>
       </c>
     </row>
@@ -11031,9 +11619,15 @@
       <c r="AD119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE119" t="inlineStr">
-        <is>
-          <t>1568</t>
+      <c r="AE119" t="n">
+        <v>1568</v>
+      </c>
+      <c r="AF119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG119" t="inlineStr">
+        <is>
+          <t>1580</t>
         </is>
       </c>
     </row>
@@ -11128,7 +11722,13 @@
       <c r="AD120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE120" t="inlineStr">
+      <c r="AE120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG120" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11225,7 +11825,13 @@
       <c r="AD121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE121" t="inlineStr">
+      <c r="AE121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11322,7 +11928,13 @@
       <c r="AD122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE122" t="inlineStr">
+      <c r="AE122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11415,7 +12027,13 @@
       <c r="AD123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE123" t="inlineStr">
+      <c r="AE123" t="n">
+        <v>2680</v>
+      </c>
+      <c r="AF123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG123" t="inlineStr">
         <is>
           <t>2680</t>
         </is>
@@ -11491,6 +12109,8 @@
       <c r="AC124" t="inlineStr"/>
       <c r="AD124" s="4" t="inlineStr"/>
       <c r="AE124" t="inlineStr"/>
+      <c r="AF124" s="4" t="inlineStr"/>
+      <c r="AG124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -11575,9 +12195,15 @@
       <c r="AD125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE125" t="inlineStr">
-        <is>
-          <t>2208</t>
+      <c r="AE125" t="n">
+        <v>2208</v>
+      </c>
+      <c r="AF125" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AG125" t="inlineStr">
+        <is>
+          <t>2288</t>
         </is>
       </c>
     </row>
@@ -11652,7 +12278,13 @@
       <c r="AD126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE126" t="inlineStr">
+      <c r="AE126" t="n">
+        <v>1526</v>
+      </c>
+      <c r="AF126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG126" t="inlineStr">
         <is>
           <t>1526</t>
         </is>
@@ -11720,6 +12352,8 @@
       <c r="AC127" t="inlineStr"/>
       <c r="AD127" s="4" t="inlineStr"/>
       <c r="AE127" t="inlineStr"/>
+      <c r="AF127" s="4" t="inlineStr"/>
+      <c r="AG127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -11784,9 +12418,15 @@
       <c r="AD128" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AE128" t="inlineStr">
-        <is>
-          <t>3813</t>
+      <c r="AE128" t="n">
+        <v>3813</v>
+      </c>
+      <c r="AF128" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG128" t="inlineStr">
+        <is>
+          <t>3768</t>
         </is>
       </c>
     </row>
@@ -11853,9 +12493,15 @@
       <c r="AD129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE129" t="inlineStr">
-        <is>
-          <t>3125</t>
+      <c r="AE129" t="n">
+        <v>3125</v>
+      </c>
+      <c r="AF129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG129" t="inlineStr">
+        <is>
+          <t>3127</t>
         </is>
       </c>
     </row>
@@ -11922,9 +12568,15 @@
       <c r="AD130" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="AE130" t="inlineStr">
-        <is>
-          <t>1478</t>
+      <c r="AE130" t="n">
+        <v>1478</v>
+      </c>
+      <c r="AF130" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG130" t="inlineStr">
+        <is>
+          <t>1512</t>
         </is>
       </c>
     </row>
@@ -11987,7 +12639,13 @@
       <c r="AD131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE131" t="inlineStr">
+      <c r="AE131" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AF131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG131" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -12040,9 +12698,15 @@
       <c r="AD132" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AE132" t="inlineStr">
-        <is>
-          <t>3751</t>
+      <c r="AE132" t="n">
+        <v>3751</v>
+      </c>
+      <c r="AF132" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AG132" t="inlineStr">
+        <is>
+          <t>4113</t>
         </is>
       </c>
     </row>
@@ -12093,17 +12757,21 @@
       <c r="AD133" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AE133" t="inlineStr">
-        <is>
-          <t>3142</t>
+      <c r="AE133" t="n">
+        <v>3142</v>
+      </c>
+      <c r="AF133" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG133" t="inlineStr">
+        <is>
+          <t>3291</t>
         </is>
       </c>
     </row>
     <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>8741713</t>
-        </is>
+      <c r="A134" t="n">
+        <v>8741713</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
@@ -12144,17 +12812,15 @@
       <c r="AD134" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AE134" t="inlineStr">
-        <is>
-          <t>5434</t>
-        </is>
-      </c>
+      <c r="AE134" t="n">
+        <v>5434</v>
+      </c>
+      <c r="AF134" s="4" t="inlineStr"/>
+      <c r="AG134" t="inlineStr"/>
     </row>
     <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>57454274</t>
-        </is>
+      <c r="A135" t="n">
+        <v>57454274</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
@@ -12195,17 +12861,21 @@
       <c r="AD135" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AE135" t="inlineStr">
-        <is>
-          <t>1635</t>
+      <c r="AE135" t="n">
+        <v>1635</v>
+      </c>
+      <c r="AF135" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="AG135" t="inlineStr">
+        <is>
+          <t>1832</t>
         </is>
       </c>
     </row>
     <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>3946814</t>
-        </is>
+      <c r="A136" t="n">
+        <v>3946814</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
@@ -12246,17 +12916,21 @@
       <c r="AD136" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AE136" t="inlineStr">
-        <is>
-          <t>5335</t>
+      <c r="AE136" t="n">
+        <v>5335</v>
+      </c>
+      <c r="AF136" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG136" t="inlineStr">
+        <is>
+          <t>5695</t>
         </is>
       </c>
     </row>
     <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>6940556</t>
-        </is>
+      <c r="A137" t="n">
+        <v>6940556</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
@@ -12297,17 +12971,21 @@
       <c r="AD137" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AE137" t="inlineStr">
-        <is>
-          <t>5525</t>
+      <c r="AE137" t="n">
+        <v>5525</v>
+      </c>
+      <c r="AF137" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG137" t="inlineStr">
+        <is>
+          <t>5682</t>
         </is>
       </c>
     </row>
     <row r="138">
-      <c r="A138" t="inlineStr">
-        <is>
-          <t>25376635</t>
-        </is>
+      <c r="A138" t="n">
+        <v>25376635</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
@@ -12348,17 +13026,21 @@
       <c r="AD138" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AE138" t="inlineStr">
-        <is>
-          <t>4965</t>
+      <c r="AE138" t="n">
+        <v>4965</v>
+      </c>
+      <c r="AF138" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG138" t="inlineStr">
+        <is>
+          <t>5307</t>
         </is>
       </c>
     </row>
     <row r="139">
-      <c r="A139" t="inlineStr">
-        <is>
-          <t>29211638</t>
-        </is>
+      <c r="A139" t="n">
+        <v>29211638</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
@@ -12399,9 +13081,15 @@
       <c r="AD139" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AE139" t="inlineStr">
-        <is>
-          <t>5431</t>
+      <c r="AE139" t="n">
+        <v>5431</v>
+      </c>
+      <c r="AF139" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AG139" t="inlineStr">
+        <is>
+          <t>5682</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-05-30 14:42:52
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG139"/>
+  <dimension ref="A1:AI139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -556,6 +556,16 @@
           <t>05-28_0</t>
         </is>
       </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>05-29_A</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>05-29_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -660,9 +670,15 @@
       <c r="AF2" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>3908</t>
+      <c r="AG2" t="n">
+        <v>3908</v>
+      </c>
+      <c r="AH2" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>4301</t>
         </is>
       </c>
     </row>
@@ -769,7 +785,13 @@
       <c r="AF3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG3" t="inlineStr">
+      <c r="AG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -878,7 +900,13 @@
       <c r="AF4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG4" t="inlineStr">
+      <c r="AG4" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AH4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI4" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -987,9 +1015,15 @@
       <c r="AF5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>2733</t>
+      <c r="AG5" t="n">
+        <v>2733</v>
+      </c>
+      <c r="AH5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>2731</t>
         </is>
       </c>
     </row>
@@ -1096,7 +1130,13 @@
       <c r="AF6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG6" t="inlineStr">
+      <c r="AG6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1148,6 +1188,8 @@
       <c r="AE7" t="inlineStr"/>
       <c r="AF7" s="4" t="inlineStr"/>
       <c r="AG7" t="inlineStr"/>
+      <c r="AH7" s="4" t="inlineStr"/>
+      <c r="AI7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1195,6 +1237,8 @@
       <c r="AE8" t="inlineStr"/>
       <c r="AF8" s="4" t="inlineStr"/>
       <c r="AG8" t="inlineStr"/>
+      <c r="AH8" s="4" t="inlineStr"/>
+      <c r="AI8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1242,6 +1286,8 @@
       <c r="AE9" t="inlineStr"/>
       <c r="AF9" s="4" t="inlineStr"/>
       <c r="AG9" t="inlineStr"/>
+      <c r="AH9" s="4" t="inlineStr"/>
+      <c r="AI9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1289,6 +1335,8 @@
       <c r="AE10" t="inlineStr"/>
       <c r="AF10" s="4" t="inlineStr"/>
       <c r="AG10" t="inlineStr"/>
+      <c r="AH10" s="4" t="inlineStr"/>
+      <c r="AI10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1336,6 +1384,8 @@
       <c r="AE11" t="inlineStr"/>
       <c r="AF11" s="4" t="inlineStr"/>
       <c r="AG11" t="inlineStr"/>
+      <c r="AH11" s="4" t="inlineStr"/>
+      <c r="AI11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1383,6 +1433,8 @@
       <c r="AE12" t="inlineStr"/>
       <c r="AF12" s="4" t="inlineStr"/>
       <c r="AG12" t="inlineStr"/>
+      <c r="AH12" s="4" t="inlineStr"/>
+      <c r="AI12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1430,6 +1482,8 @@
       <c r="AE13" t="inlineStr"/>
       <c r="AF13" s="4" t="inlineStr"/>
       <c r="AG13" t="inlineStr"/>
+      <c r="AH13" s="4" t="inlineStr"/>
+      <c r="AI13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1477,6 +1531,8 @@
       <c r="AE14" t="inlineStr"/>
       <c r="AF14" s="4" t="inlineStr"/>
       <c r="AG14" t="inlineStr"/>
+      <c r="AH14" s="4" t="inlineStr"/>
+      <c r="AI14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1524,6 +1580,8 @@
       <c r="AE15" t="inlineStr"/>
       <c r="AF15" s="4" t="inlineStr"/>
       <c r="AG15" t="inlineStr"/>
+      <c r="AH15" s="4" t="inlineStr"/>
+      <c r="AI15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1571,6 +1629,8 @@
       <c r="AE16" t="inlineStr"/>
       <c r="AF16" s="4" t="inlineStr"/>
       <c r="AG16" t="inlineStr"/>
+      <c r="AH16" s="4" t="inlineStr"/>
+      <c r="AI16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1618,6 +1678,8 @@
       <c r="AE17" t="inlineStr"/>
       <c r="AF17" s="4" t="inlineStr"/>
       <c r="AG17" t="inlineStr"/>
+      <c r="AH17" s="4" t="inlineStr"/>
+      <c r="AI17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1722,9 +1784,15 @@
       <c r="AF18" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AG18" t="inlineStr">
-        <is>
-          <t>3977</t>
+      <c r="AG18" t="n">
+        <v>3977</v>
+      </c>
+      <c r="AH18" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AI18" t="inlineStr">
+        <is>
+          <t>3994</t>
         </is>
       </c>
     </row>
@@ -1831,9 +1899,15 @@
       <c r="AF19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG19" t="inlineStr">
-        <is>
-          <t>2703</t>
+      <c r="AG19" t="n">
+        <v>2703</v>
+      </c>
+      <c r="AH19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI19" t="inlineStr">
+        <is>
+          <t>2780</t>
         </is>
       </c>
     </row>
@@ -1940,9 +2014,15 @@
       <c r="AF20" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AG20" t="inlineStr">
-        <is>
-          <t>4234</t>
+      <c r="AG20" t="n">
+        <v>4234</v>
+      </c>
+      <c r="AH20" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AI20" t="inlineStr">
+        <is>
+          <t>4366</t>
         </is>
       </c>
     </row>
@@ -2049,9 +2129,15 @@
       <c r="AF21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG21" t="inlineStr">
-        <is>
-          <t>2879</t>
+      <c r="AG21" t="n">
+        <v>2879</v>
+      </c>
+      <c r="AH21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI21" t="inlineStr">
+        <is>
+          <t>2908</t>
         </is>
       </c>
     </row>
@@ -2158,9 +2244,15 @@
       <c r="AF22" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AG22" t="inlineStr">
-        <is>
-          <t>4657</t>
+      <c r="AG22" t="n">
+        <v>4657</v>
+      </c>
+      <c r="AH22" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AI22" t="inlineStr">
+        <is>
+          <t>4864</t>
         </is>
       </c>
     </row>
@@ -2267,9 +2359,15 @@
       <c r="AF23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AG23" t="inlineStr">
-        <is>
-          <t>5083</t>
+      <c r="AG23" t="n">
+        <v>5083</v>
+      </c>
+      <c r="AH23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AI23" t="inlineStr">
+        <is>
+          <t>5340</t>
         </is>
       </c>
     </row>
@@ -2376,9 +2474,15 @@
       <c r="AF24" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AG24" t="inlineStr">
-        <is>
-          <t>4538</t>
+      <c r="AG24" t="n">
+        <v>4538</v>
+      </c>
+      <c r="AH24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI24" t="inlineStr">
+        <is>
+          <t>4767</t>
         </is>
       </c>
     </row>
@@ -2485,9 +2589,15 @@
       <c r="AF25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AG25" t="inlineStr">
-        <is>
-          <t>4977</t>
+      <c r="AG25" t="n">
+        <v>4977</v>
+      </c>
+      <c r="AH25" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI25" t="inlineStr">
+        <is>
+          <t>5177</t>
         </is>
       </c>
     </row>
@@ -2589,6 +2699,8 @@
       <c r="AE26" t="inlineStr"/>
       <c r="AF26" s="4" t="inlineStr"/>
       <c r="AG26" t="inlineStr"/>
+      <c r="AH26" s="4" t="inlineStr"/>
+      <c r="AI26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2693,7 +2805,13 @@
       <c r="AF27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG27" t="inlineStr">
+      <c r="AG27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2745,6 +2863,8 @@
       <c r="AE28" t="inlineStr"/>
       <c r="AF28" s="4" t="inlineStr"/>
       <c r="AG28" t="inlineStr"/>
+      <c r="AH28" s="4" t="inlineStr"/>
+      <c r="AI28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2849,7 +2969,13 @@
       <c r="AF29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG29" t="inlineStr">
+      <c r="AG29" t="n">
+        <v>3429</v>
+      </c>
+      <c r="AH29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI29" t="inlineStr">
         <is>
           <t>3429</t>
         </is>
@@ -2958,7 +3084,13 @@
       <c r="AF30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG30" t="inlineStr">
+      <c r="AG30" t="n">
+        <v>3598</v>
+      </c>
+      <c r="AH30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI30" t="inlineStr">
         <is>
           <t>3598</t>
         </is>
@@ -3067,9 +3199,15 @@
       <c r="AF31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AG31" t="inlineStr">
-        <is>
-          <t>4661</t>
+      <c r="AG31" t="n">
+        <v>4661</v>
+      </c>
+      <c r="AH31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI31" t="inlineStr">
+        <is>
+          <t>4891</t>
         </is>
       </c>
     </row>
@@ -3176,9 +3314,15 @@
       <c r="AF32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG32" t="inlineStr">
-        <is>
-          <t>2526</t>
+      <c r="AG32" t="n">
+        <v>2526</v>
+      </c>
+      <c r="AH32" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI32" t="inlineStr">
+        <is>
+          <t>2887</t>
         </is>
       </c>
     </row>
@@ -3228,6 +3372,8 @@
       <c r="AE33" t="inlineStr"/>
       <c r="AF33" s="4" t="inlineStr"/>
       <c r="AG33" t="inlineStr"/>
+      <c r="AH33" s="4" t="inlineStr"/>
+      <c r="AI33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3332,9 +3478,15 @@
       <c r="AF34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG34" t="inlineStr">
-        <is>
-          <t>2548</t>
+      <c r="AG34" t="n">
+        <v>2548</v>
+      </c>
+      <c r="AH34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI34" t="inlineStr">
+        <is>
+          <t>2571</t>
         </is>
       </c>
     </row>
@@ -3441,7 +3593,13 @@
       <c r="AF35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG35" t="inlineStr">
+      <c r="AG35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI35" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3550,9 +3708,15 @@
       <c r="AF36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG36" t="inlineStr">
-        <is>
-          <t>2892</t>
+      <c r="AG36" t="n">
+        <v>2892</v>
+      </c>
+      <c r="AH36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI36" t="inlineStr">
+        <is>
+          <t>2921</t>
         </is>
       </c>
     </row>
@@ -3659,9 +3823,15 @@
       <c r="AF37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AG37" t="inlineStr">
-        <is>
-          <t>4452</t>
+      <c r="AG37" t="n">
+        <v>4452</v>
+      </c>
+      <c r="AH37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI37" t="inlineStr">
+        <is>
+          <t>4610</t>
         </is>
       </c>
     </row>
@@ -3768,9 +3938,15 @@
       <c r="AF38" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AG38" t="inlineStr">
-        <is>
-          <t>5086</t>
+      <c r="AG38" t="n">
+        <v>5086</v>
+      </c>
+      <c r="AH38" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AI38" t="inlineStr">
+        <is>
+          <t>5269</t>
         </is>
       </c>
     </row>
@@ -3877,9 +4053,15 @@
       <c r="AF39" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="AG39" t="inlineStr">
-        <is>
-          <t>4413</t>
+      <c r="AG39" t="n">
+        <v>4413</v>
+      </c>
+      <c r="AH39" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="AI39" t="inlineStr">
+        <is>
+          <t>4496</t>
         </is>
       </c>
     </row>
@@ -3986,7 +4168,13 @@
       <c r="AF40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG40" t="inlineStr">
+      <c r="AG40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4095,9 +4283,15 @@
       <c r="AF41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG41" t="inlineStr">
-        <is>
-          <t>4186</t>
+      <c r="AG41" t="n">
+        <v>4186</v>
+      </c>
+      <c r="AH41" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AI41" t="inlineStr">
+        <is>
+          <t>4319</t>
         </is>
       </c>
     </row>
@@ -4204,9 +4398,15 @@
       <c r="AF42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG42" t="inlineStr">
-        <is>
-          <t>2664</t>
+      <c r="AG42" t="n">
+        <v>2664</v>
+      </c>
+      <c r="AH42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI42" t="inlineStr">
+        <is>
+          <t>2762</t>
         </is>
       </c>
     </row>
@@ -4256,6 +4456,8 @@
       <c r="AE43" t="inlineStr"/>
       <c r="AF43" s="4" t="inlineStr"/>
       <c r="AG43" t="inlineStr"/>
+      <c r="AH43" s="4" t="inlineStr"/>
+      <c r="AI43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -4303,6 +4505,8 @@
       <c r="AE44" t="inlineStr"/>
       <c r="AF44" s="4" t="inlineStr"/>
       <c r="AG44" t="inlineStr"/>
+      <c r="AH44" s="4" t="inlineStr"/>
+      <c r="AI44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -4382,6 +4586,8 @@
       <c r="AE45" t="inlineStr"/>
       <c r="AF45" s="4" t="inlineStr"/>
       <c r="AG45" t="inlineStr"/>
+      <c r="AH45" s="4" t="inlineStr"/>
+      <c r="AI45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -4486,9 +4692,15 @@
       <c r="AF46" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="AG46" t="inlineStr">
-        <is>
-          <t>3681</t>
+      <c r="AG46" t="n">
+        <v>3681</v>
+      </c>
+      <c r="AH46" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="AI46" t="inlineStr">
+        <is>
+          <t>3851</t>
         </is>
       </c>
     </row>
@@ -4595,9 +4807,15 @@
       <c r="AF47" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AG47" t="inlineStr">
-        <is>
-          <t>5041</t>
+      <c r="AG47" t="n">
+        <v>5041</v>
+      </c>
+      <c r="AH47" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AI47" t="inlineStr">
+        <is>
+          <t>5146</t>
         </is>
       </c>
     </row>
@@ -4704,7 +4922,13 @@
       <c r="AF48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG48" t="inlineStr">
+      <c r="AG48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4813,9 +5037,15 @@
       <c r="AF49" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AG49" t="inlineStr">
-        <is>
-          <t>4510</t>
+      <c r="AG49" t="n">
+        <v>4510</v>
+      </c>
+      <c r="AH49" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AI49" t="inlineStr">
+        <is>
+          <t>4690</t>
         </is>
       </c>
     </row>
@@ -4922,9 +5152,15 @@
       <c r="AF50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AG50" t="inlineStr">
-        <is>
-          <t>4679</t>
+      <c r="AG50" t="n">
+        <v>4679</v>
+      </c>
+      <c r="AH50" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AI50" t="inlineStr">
+        <is>
+          <t>4857</t>
         </is>
       </c>
     </row>
@@ -5006,6 +5242,8 @@
       <c r="AE51" t="inlineStr"/>
       <c r="AF51" s="4" t="inlineStr"/>
       <c r="AG51" t="inlineStr"/>
+      <c r="AH51" s="4" t="inlineStr"/>
+      <c r="AI51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -5110,9 +5348,15 @@
       <c r="AF52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AG52" t="inlineStr">
-        <is>
-          <t>4780</t>
+      <c r="AG52" t="n">
+        <v>4780</v>
+      </c>
+      <c r="AH52" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AI52" t="inlineStr">
+        <is>
+          <t>4879</t>
         </is>
       </c>
     </row>
@@ -5219,9 +5463,15 @@
       <c r="AF53" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="AG53" t="inlineStr">
-        <is>
-          <t>3880</t>
+      <c r="AG53" t="n">
+        <v>3880</v>
+      </c>
+      <c r="AH53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI53" t="inlineStr">
+        <is>
+          <t>3936</t>
         </is>
       </c>
     </row>
@@ -5303,6 +5553,8 @@
       <c r="AE54" t="inlineStr"/>
       <c r="AF54" s="4" t="inlineStr"/>
       <c r="AG54" t="inlineStr"/>
+      <c r="AH54" s="4" t="inlineStr"/>
+      <c r="AI54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -5407,9 +5659,15 @@
       <c r="AF55" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AG55" t="inlineStr">
-        <is>
-          <t>4178</t>
+      <c r="AG55" t="n">
+        <v>4178</v>
+      </c>
+      <c r="AH55" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI55" t="inlineStr">
+        <is>
+          <t>4430</t>
         </is>
       </c>
     </row>
@@ -5516,9 +5774,15 @@
       <c r="AF56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AG56" t="inlineStr">
-        <is>
-          <t>4941</t>
+      <c r="AG56" t="n">
+        <v>4941</v>
+      </c>
+      <c r="AH56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI56" t="inlineStr">
+        <is>
+          <t>5087</t>
         </is>
       </c>
     </row>
@@ -5625,9 +5889,15 @@
       <c r="AF57" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="AG57" t="inlineStr">
-        <is>
-          <t>4171</t>
+      <c r="AG57" t="n">
+        <v>4171</v>
+      </c>
+      <c r="AH57" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="AI57" t="inlineStr">
+        <is>
+          <t>4167</t>
         </is>
       </c>
     </row>
@@ -5734,9 +6004,15 @@
       <c r="AF58" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AG58" t="inlineStr">
-        <is>
-          <t>3988</t>
+      <c r="AG58" t="n">
+        <v>3988</v>
+      </c>
+      <c r="AH58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AI58" t="inlineStr">
+        <is>
+          <t>4191</t>
         </is>
       </c>
     </row>
@@ -5843,9 +6119,15 @@
       <c r="AF59" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="AG59" t="inlineStr">
-        <is>
-          <t>4012</t>
+      <c r="AG59" t="n">
+        <v>4012</v>
+      </c>
+      <c r="AH59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI59" t="inlineStr">
+        <is>
+          <t>4083</t>
         </is>
       </c>
     </row>
@@ -5952,9 +6234,15 @@
       <c r="AF60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AG60" t="inlineStr">
-        <is>
-          <t>4186</t>
+      <c r="AG60" t="n">
+        <v>4186</v>
+      </c>
+      <c r="AH60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AI60" t="inlineStr">
+        <is>
+          <t>4324</t>
         </is>
       </c>
     </row>
@@ -6004,6 +6292,8 @@
       <c r="AE61" t="inlineStr"/>
       <c r="AF61" s="4" t="inlineStr"/>
       <c r="AG61" t="inlineStr"/>
+      <c r="AH61" s="4" t="inlineStr"/>
+      <c r="AI61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -6108,9 +6398,15 @@
       <c r="AF62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AG62" t="inlineStr">
-        <is>
-          <t>3974</t>
+      <c r="AG62" t="n">
+        <v>3974</v>
+      </c>
+      <c r="AH62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI62" t="inlineStr">
+        <is>
+          <t>4074</t>
         </is>
       </c>
     </row>
@@ -6217,9 +6513,15 @@
       <c r="AF63" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AG63" t="inlineStr">
-        <is>
-          <t>4021</t>
+      <c r="AG63" t="n">
+        <v>4021</v>
+      </c>
+      <c r="AH63" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI63" t="inlineStr">
+        <is>
+          <t>3992</t>
         </is>
       </c>
     </row>
@@ -6326,9 +6628,15 @@
       <c r="AF64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AG64" t="inlineStr">
-        <is>
-          <t>4199</t>
+      <c r="AG64" t="n">
+        <v>4199</v>
+      </c>
+      <c r="AH64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI64" t="inlineStr">
+        <is>
+          <t>4281</t>
         </is>
       </c>
     </row>
@@ -6430,6 +6738,8 @@
       <c r="AE65" t="inlineStr"/>
       <c r="AF65" s="4" t="inlineStr"/>
       <c r="AG65" t="inlineStr"/>
+      <c r="AH65" s="4" t="inlineStr"/>
+      <c r="AI65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -6534,7 +6844,13 @@
       <c r="AF66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG66" t="inlineStr">
+      <c r="AG66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6643,7 +6959,13 @@
       <c r="AF67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG67" t="inlineStr">
+      <c r="AG67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6752,7 +7074,13 @@
       <c r="AF68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG68" t="inlineStr">
+      <c r="AG68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6804,6 +7132,8 @@
       <c r="AE69" t="inlineStr"/>
       <c r="AF69" s="4" t="inlineStr"/>
       <c r="AG69" t="inlineStr"/>
+      <c r="AH69" s="4" t="inlineStr"/>
+      <c r="AI69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -6908,7 +7238,13 @@
       <c r="AF70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG70" t="inlineStr">
+      <c r="AG70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7017,7 +7353,13 @@
       <c r="AF71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG71" t="inlineStr">
+      <c r="AG71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7126,7 +7468,13 @@
       <c r="AF72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG72" t="inlineStr">
+      <c r="AG72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7235,9 +7583,15 @@
       <c r="AF73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG73" t="inlineStr">
-        <is>
-          <t>2805</t>
+      <c r="AG73" t="n">
+        <v>2805</v>
+      </c>
+      <c r="AH73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI73" t="inlineStr">
+        <is>
+          <t>2815</t>
         </is>
       </c>
     </row>
@@ -7344,7 +7698,13 @@
       <c r="AF74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG74" t="inlineStr">
+      <c r="AG74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7453,7 +7813,13 @@
       <c r="AF75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG75" t="inlineStr">
+      <c r="AG75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7562,9 +7928,15 @@
       <c r="AF76" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="AG76" t="inlineStr">
-        <is>
-          <t>2894</t>
+      <c r="AG76" t="n">
+        <v>2894</v>
+      </c>
+      <c r="AH76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI76" t="inlineStr">
+        <is>
+          <t>2922</t>
         </is>
       </c>
     </row>
@@ -7671,9 +8043,15 @@
       <c r="AF77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG77" t="inlineStr">
-        <is>
-          <t>2608</t>
+      <c r="AG77" t="n">
+        <v>2608</v>
+      </c>
+      <c r="AH77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI77" t="inlineStr">
+        <is>
+          <t>2631</t>
         </is>
       </c>
     </row>
@@ -7780,7 +8158,13 @@
       <c r="AF78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG78" t="inlineStr">
+      <c r="AG78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7889,7 +8273,13 @@
       <c r="AF79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG79" t="inlineStr">
+      <c r="AG79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7998,7 +8388,13 @@
       <c r="AF80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG80" t="inlineStr">
+      <c r="AG80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8107,7 +8503,13 @@
       <c r="AF81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG81" t="inlineStr">
+      <c r="AG81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8216,7 +8618,13 @@
       <c r="AF82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG82" t="inlineStr">
+      <c r="AG82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8325,7 +8733,13 @@
       <c r="AF83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG83" t="inlineStr">
+      <c r="AG83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8434,7 +8848,13 @@
       <c r="AF84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG84" t="inlineStr">
+      <c r="AG84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8543,7 +8963,13 @@
       <c r="AF85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG85" t="inlineStr">
+      <c r="AG85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8652,9 +9078,15 @@
       <c r="AF86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG86" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AG86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH86" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AI86" t="inlineStr">
+        <is>
+          <t>1085</t>
         </is>
       </c>
     </row>
@@ -8761,7 +9193,13 @@
       <c r="AF87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG87" t="inlineStr">
+      <c r="AG87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8870,7 +9308,13 @@
       <c r="AF88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG88" t="inlineStr">
+      <c r="AG88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8979,7 +9423,13 @@
       <c r="AF89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG89" t="inlineStr">
+      <c r="AG89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9088,7 +9538,13 @@
       <c r="AF90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG90" t="inlineStr">
+      <c r="AG90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9197,7 +9653,13 @@
       <c r="AF91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG91" t="inlineStr">
+      <c r="AG91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9306,7 +9768,13 @@
       <c r="AF92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG92" t="inlineStr">
+      <c r="AG92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9415,7 +9883,13 @@
       <c r="AF93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG93" t="inlineStr">
+      <c r="AG93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9524,7 +9998,13 @@
       <c r="AF94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG94" t="inlineStr">
+      <c r="AG94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9633,7 +10113,13 @@
       <c r="AF95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG95" t="inlineStr">
+      <c r="AG95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9742,7 +10228,13 @@
       <c r="AF96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG96" t="inlineStr">
+      <c r="AG96" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI96" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9851,7 +10343,13 @@
       <c r="AF97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG97" t="inlineStr">
+      <c r="AG97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9960,7 +10458,13 @@
       <c r="AF98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG98" t="inlineStr">
+      <c r="AG98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10069,7 +10573,13 @@
       <c r="AF99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG99" t="inlineStr">
+      <c r="AG99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10178,7 +10688,13 @@
       <c r="AF100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG100" t="inlineStr">
+      <c r="AG100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10287,7 +10803,13 @@
       <c r="AF101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG101" t="inlineStr">
+      <c r="AG101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10396,7 +10918,13 @@
       <c r="AF102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG102" t="inlineStr">
+      <c r="AG102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10505,7 +11033,13 @@
       <c r="AF103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG103" t="inlineStr">
+      <c r="AG103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10614,7 +11148,13 @@
       <c r="AF104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG104" t="inlineStr">
+      <c r="AG104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10723,7 +11263,13 @@
       <c r="AF105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG105" t="inlineStr">
+      <c r="AG105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10775,6 +11321,8 @@
       <c r="AE106" t="inlineStr"/>
       <c r="AF106" s="4" t="inlineStr"/>
       <c r="AG106" t="inlineStr"/>
+      <c r="AH106" s="4" t="inlineStr"/>
+      <c r="AI106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -10822,6 +11370,8 @@
       <c r="AE107" t="inlineStr"/>
       <c r="AF107" s="4" t="inlineStr"/>
       <c r="AG107" t="inlineStr"/>
+      <c r="AH107" s="4" t="inlineStr"/>
+      <c r="AI107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -10869,6 +11419,8 @@
       <c r="AE108" t="inlineStr"/>
       <c r="AF108" s="4" t="inlineStr"/>
       <c r="AG108" t="inlineStr"/>
+      <c r="AH108" s="4" t="inlineStr"/>
+      <c r="AI108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -10916,6 +11468,8 @@
       <c r="AE109" t="inlineStr"/>
       <c r="AF109" s="4" t="inlineStr"/>
       <c r="AG109" t="inlineStr"/>
+      <c r="AH109" s="4" t="inlineStr"/>
+      <c r="AI109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -10963,6 +11517,8 @@
       <c r="AE110" t="inlineStr"/>
       <c r="AF110" s="4" t="inlineStr"/>
       <c r="AG110" t="inlineStr"/>
+      <c r="AH110" s="4" t="inlineStr"/>
+      <c r="AI110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -11010,6 +11566,8 @@
       <c r="AE111" t="inlineStr"/>
       <c r="AF111" s="4" t="inlineStr"/>
       <c r="AG111" t="inlineStr"/>
+      <c r="AH111" s="4" t="inlineStr"/>
+      <c r="AI111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -11057,6 +11615,8 @@
       <c r="AE112" t="inlineStr"/>
       <c r="AF112" s="4" t="inlineStr"/>
       <c r="AG112" t="inlineStr"/>
+      <c r="AH112" s="4" t="inlineStr"/>
+      <c r="AI112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -11104,6 +11664,8 @@
       <c r="AE113" t="inlineStr"/>
       <c r="AF113" s="4" t="inlineStr"/>
       <c r="AG113" t="inlineStr"/>
+      <c r="AH113" s="4" t="inlineStr"/>
+      <c r="AI113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -11151,6 +11713,8 @@
       <c r="AE114" t="inlineStr"/>
       <c r="AF114" s="4" t="inlineStr"/>
       <c r="AG114" t="inlineStr"/>
+      <c r="AH114" s="4" t="inlineStr"/>
+      <c r="AI114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -11233,9 +11797,15 @@
       <c r="AF115" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AG115" t="inlineStr">
-        <is>
-          <t>5083</t>
+      <c r="AG115" t="n">
+        <v>5083</v>
+      </c>
+      <c r="AH115" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AI115" t="inlineStr">
+        <is>
+          <t>5368</t>
         </is>
       </c>
     </row>
@@ -11336,7 +11906,13 @@
       <c r="AF116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG116" t="inlineStr">
+      <c r="AG116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11419,11 +11995,11 @@
       <c r="AF117" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AG117" t="inlineStr">
-        <is>
-          <t>5994</t>
-        </is>
-      </c>
+      <c r="AG117" t="n">
+        <v>5994</v>
+      </c>
+      <c r="AH117" s="4" t="inlineStr"/>
+      <c r="AI117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -11522,7 +12098,13 @@
       <c r="AF118" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="AG118" t="inlineStr">
+      <c r="AG118" t="n">
+        <v>3304</v>
+      </c>
+      <c r="AH118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI118" t="inlineStr">
         <is>
           <t>3304</t>
         </is>
@@ -11625,9 +12207,15 @@
       <c r="AF119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG119" t="inlineStr">
-        <is>
-          <t>1580</t>
+      <c r="AG119" t="n">
+        <v>1580</v>
+      </c>
+      <c r="AH119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI119" t="inlineStr">
+        <is>
+          <t>1578</t>
         </is>
       </c>
     </row>
@@ -11728,7 +12316,13 @@
       <c r="AF120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG120" t="inlineStr">
+      <c r="AG120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI120" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11831,7 +12425,13 @@
       <c r="AF121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG121" t="inlineStr">
+      <c r="AG121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11934,7 +12534,13 @@
       <c r="AF122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG122" t="inlineStr">
+      <c r="AG122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12033,7 +12639,13 @@
       <c r="AF123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG123" t="inlineStr">
+      <c r="AG123" t="n">
+        <v>2680</v>
+      </c>
+      <c r="AH123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI123" t="inlineStr">
         <is>
           <t>2680</t>
         </is>
@@ -12111,6 +12723,8 @@
       <c r="AE124" t="inlineStr"/>
       <c r="AF124" s="4" t="inlineStr"/>
       <c r="AG124" t="inlineStr"/>
+      <c r="AH124" s="4" t="inlineStr"/>
+      <c r="AI124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -12201,9 +12815,15 @@
       <c r="AF125" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="AG125" t="inlineStr">
-        <is>
-          <t>2288</t>
+      <c r="AG125" t="n">
+        <v>2288</v>
+      </c>
+      <c r="AH125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI125" t="inlineStr">
+        <is>
+          <t>2280</t>
         </is>
       </c>
     </row>
@@ -12284,7 +12904,13 @@
       <c r="AF126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG126" t="inlineStr">
+      <c r="AG126" t="n">
+        <v>1526</v>
+      </c>
+      <c r="AH126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI126" t="inlineStr">
         <is>
           <t>1526</t>
         </is>
@@ -12354,6 +12980,8 @@
       <c r="AE127" t="inlineStr"/>
       <c r="AF127" s="4" t="inlineStr"/>
       <c r="AG127" t="inlineStr"/>
+      <c r="AH127" s="4" t="inlineStr"/>
+      <c r="AI127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -12424,9 +13052,15 @@
       <c r="AF128" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="AG128" t="inlineStr">
-        <is>
-          <t>3768</t>
+      <c r="AG128" t="n">
+        <v>3768</v>
+      </c>
+      <c r="AH128" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AI128" t="inlineStr">
+        <is>
+          <t>3972</t>
         </is>
       </c>
     </row>
@@ -12499,9 +13133,15 @@
       <c r="AF129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG129" t="inlineStr">
-        <is>
-          <t>3127</t>
+      <c r="AG129" t="n">
+        <v>3127</v>
+      </c>
+      <c r="AH129" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI129" t="inlineStr">
+        <is>
+          <t>3411</t>
         </is>
       </c>
     </row>
@@ -12574,9 +13214,15 @@
       <c r="AF130" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="AG130" t="inlineStr">
-        <is>
-          <t>1512</t>
+      <c r="AG130" t="n">
+        <v>1512</v>
+      </c>
+      <c r="AH130" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI130" t="inlineStr">
+        <is>
+          <t>1520</t>
         </is>
       </c>
     </row>
@@ -12645,7 +13291,13 @@
       <c r="AF131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AG131" t="inlineStr">
+      <c r="AG131" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AH131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI131" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -12704,9 +13356,15 @@
       <c r="AF132" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AG132" t="inlineStr">
-        <is>
-          <t>4113</t>
+      <c r="AG132" t="n">
+        <v>4113</v>
+      </c>
+      <c r="AH132" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="AI132" t="inlineStr">
+        <is>
+          <t>4206</t>
         </is>
       </c>
     </row>
@@ -12763,9 +13421,15 @@
       <c r="AF133" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="AG133" t="inlineStr">
-        <is>
-          <t>3291</t>
+      <c r="AG133" t="n">
+        <v>3291</v>
+      </c>
+      <c r="AH133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI133" t="inlineStr">
+        <is>
+          <t>3272</t>
         </is>
       </c>
     </row>
@@ -12817,6 +13481,8 @@
       </c>
       <c r="AF134" s="4" t="inlineStr"/>
       <c r="AG134" t="inlineStr"/>
+      <c r="AH134" s="4" t="inlineStr"/>
+      <c r="AI134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -12867,11 +13533,11 @@
       <c r="AF135" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="AG135" t="inlineStr">
-        <is>
-          <t>1832</t>
-        </is>
-      </c>
+      <c r="AG135" t="n">
+        <v>1832</v>
+      </c>
+      <c r="AH135" s="4" t="inlineStr"/>
+      <c r="AI135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -12922,11 +13588,11 @@
       <c r="AF136" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AG136" t="inlineStr">
-        <is>
-          <t>5695</t>
-        </is>
-      </c>
+      <c r="AG136" t="n">
+        <v>5695</v>
+      </c>
+      <c r="AH136" s="4" t="inlineStr"/>
+      <c r="AI136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -12977,11 +13643,11 @@
       <c r="AF137" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AG137" t="inlineStr">
-        <is>
-          <t>5682</t>
-        </is>
-      </c>
+      <c r="AG137" t="n">
+        <v>5682</v>
+      </c>
+      <c r="AH137" s="4" t="inlineStr"/>
+      <c r="AI137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -13032,11 +13698,11 @@
       <c r="AF138" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AG138" t="inlineStr">
-        <is>
-          <t>5307</t>
-        </is>
-      </c>
+      <c r="AG138" t="n">
+        <v>5307</v>
+      </c>
+      <c r="AH138" s="4" t="inlineStr"/>
+      <c r="AI138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -13087,11 +13753,11 @@
       <c r="AF139" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AG139" t="inlineStr">
-        <is>
-          <t>5682</t>
-        </is>
-      </c>
+      <c r="AG139" t="n">
+        <v>5682</v>
+      </c>
+      <c r="AH139" s="4" t="inlineStr"/>
+      <c r="AI139" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Code updated 23-06-02 04:03:31
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AI139"/>
+  <dimension ref="A1:AK140"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -566,6 +566,16 @@
           <t>05-29_0</t>
         </is>
       </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>06-01_A</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>06-01_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -676,9 +686,15 @@
       <c r="AH2" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>4301</t>
+      <c r="AI2" t="n">
+        <v>4301</v>
+      </c>
+      <c r="AJ2" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>4708</t>
         </is>
       </c>
     </row>
@@ -791,7 +807,13 @@
       <c r="AH3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI3" t="inlineStr">
+      <c r="AI3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -906,7 +928,13 @@
       <c r="AH4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI4" t="inlineStr">
+      <c r="AI4" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AJ4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK4" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1021,9 +1049,15 @@
       <c r="AH5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI5" t="inlineStr">
-        <is>
-          <t>2731</t>
+      <c r="AI5" t="n">
+        <v>2731</v>
+      </c>
+      <c r="AJ5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>2814</t>
         </is>
       </c>
     </row>
@@ -1136,7 +1170,13 @@
       <c r="AH6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI6" t="inlineStr">
+      <c r="AI6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1190,6 +1230,8 @@
       <c r="AG7" t="inlineStr"/>
       <c r="AH7" s="4" t="inlineStr"/>
       <c r="AI7" t="inlineStr"/>
+      <c r="AJ7" s="4" t="inlineStr"/>
+      <c r="AK7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1239,6 +1281,8 @@
       <c r="AG8" t="inlineStr"/>
       <c r="AH8" s="4" t="inlineStr"/>
       <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" s="4" t="inlineStr"/>
+      <c r="AK8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1288,6 +1332,8 @@
       <c r="AG9" t="inlineStr"/>
       <c r="AH9" s="4" t="inlineStr"/>
       <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" s="4" t="inlineStr"/>
+      <c r="AK9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1337,6 +1383,8 @@
       <c r="AG10" t="inlineStr"/>
       <c r="AH10" s="4" t="inlineStr"/>
       <c r="AI10" t="inlineStr"/>
+      <c r="AJ10" s="4" t="inlineStr"/>
+      <c r="AK10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1386,6 +1434,8 @@
       <c r="AG11" t="inlineStr"/>
       <c r="AH11" s="4" t="inlineStr"/>
       <c r="AI11" t="inlineStr"/>
+      <c r="AJ11" s="4" t="inlineStr"/>
+      <c r="AK11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1435,6 +1485,8 @@
       <c r="AG12" t="inlineStr"/>
       <c r="AH12" s="4" t="inlineStr"/>
       <c r="AI12" t="inlineStr"/>
+      <c r="AJ12" s="4" t="inlineStr"/>
+      <c r="AK12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1484,6 +1536,8 @@
       <c r="AG13" t="inlineStr"/>
       <c r="AH13" s="4" t="inlineStr"/>
       <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" s="4" t="inlineStr"/>
+      <c r="AK13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1533,6 +1587,8 @@
       <c r="AG14" t="inlineStr"/>
       <c r="AH14" s="4" t="inlineStr"/>
       <c r="AI14" t="inlineStr"/>
+      <c r="AJ14" s="4" t="inlineStr"/>
+      <c r="AK14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1582,6 +1638,8 @@
       <c r="AG15" t="inlineStr"/>
       <c r="AH15" s="4" t="inlineStr"/>
       <c r="AI15" t="inlineStr"/>
+      <c r="AJ15" s="4" t="inlineStr"/>
+      <c r="AK15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1631,6 +1689,8 @@
       <c r="AG16" t="inlineStr"/>
       <c r="AH16" s="4" t="inlineStr"/>
       <c r="AI16" t="inlineStr"/>
+      <c r="AJ16" s="4" t="inlineStr"/>
+      <c r="AK16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1680,6 +1740,8 @@
       <c r="AG17" t="inlineStr"/>
       <c r="AH17" s="4" t="inlineStr"/>
       <c r="AI17" t="inlineStr"/>
+      <c r="AJ17" s="4" t="inlineStr"/>
+      <c r="AK17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1790,9 +1852,15 @@
       <c r="AH18" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="AI18" t="inlineStr">
-        <is>
-          <t>3994</t>
+      <c r="AI18" t="n">
+        <v>3994</v>
+      </c>
+      <c r="AJ18" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AK18" t="inlineStr">
+        <is>
+          <t>4017</t>
         </is>
       </c>
     </row>
@@ -1905,9 +1973,15 @@
       <c r="AH19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI19" t="inlineStr">
-        <is>
-          <t>2780</t>
+      <c r="AI19" t="n">
+        <v>2780</v>
+      </c>
+      <c r="AJ19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK19" t="inlineStr">
+        <is>
+          <t>2811</t>
         </is>
       </c>
     </row>
@@ -2020,9 +2094,15 @@
       <c r="AH20" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AI20" t="inlineStr">
-        <is>
-          <t>4366</t>
+      <c r="AI20" t="n">
+        <v>4366</v>
+      </c>
+      <c r="AJ20" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK20" t="inlineStr">
+        <is>
+          <t>4476</t>
         </is>
       </c>
     </row>
@@ -2135,9 +2215,15 @@
       <c r="AH21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI21" t="inlineStr">
-        <is>
-          <t>2908</t>
+      <c r="AI21" t="n">
+        <v>2908</v>
+      </c>
+      <c r="AJ21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK21" t="inlineStr">
+        <is>
+          <t>3007</t>
         </is>
       </c>
     </row>
@@ -2250,9 +2336,15 @@
       <c r="AH22" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AI22" t="inlineStr">
-        <is>
-          <t>4864</t>
+      <c r="AI22" t="n">
+        <v>4864</v>
+      </c>
+      <c r="AJ22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK22" t="inlineStr">
+        <is>
+          <t>5166</t>
         </is>
       </c>
     </row>
@@ -2365,9 +2457,15 @@
       <c r="AH23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AI23" t="inlineStr">
-        <is>
-          <t>5340</t>
+      <c r="AI23" t="n">
+        <v>5340</v>
+      </c>
+      <c r="AJ23" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AK23" t="inlineStr">
+        <is>
+          <t>5773</t>
         </is>
       </c>
     </row>
@@ -2480,9 +2578,15 @@
       <c r="AH24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AI24" t="inlineStr">
-        <is>
-          <t>4767</t>
+      <c r="AI24" t="n">
+        <v>4767</v>
+      </c>
+      <c r="AJ24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AK24" t="inlineStr">
+        <is>
+          <t>5060</t>
         </is>
       </c>
     </row>
@@ -2595,11 +2699,11 @@
       <c r="AH25" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AI25" t="inlineStr">
-        <is>
-          <t>5177</t>
-        </is>
-      </c>
+      <c r="AI25" t="n">
+        <v>5177</v>
+      </c>
+      <c r="AJ25" s="4" t="inlineStr"/>
+      <c r="AK25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2701,6 +2805,8 @@
       <c r="AG26" t="inlineStr"/>
       <c r="AH26" s="4" t="inlineStr"/>
       <c r="AI26" t="inlineStr"/>
+      <c r="AJ26" s="4" t="inlineStr"/>
+      <c r="AK26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2811,9 +2917,15 @@
       <c r="AH27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI27" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AI27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK27" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -2865,6 +2977,8 @@
       <c r="AG28" t="inlineStr"/>
       <c r="AH28" s="4" t="inlineStr"/>
       <c r="AI28" t="inlineStr"/>
+      <c r="AJ28" s="4" t="inlineStr"/>
+      <c r="AK28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2975,7 +3089,13 @@
       <c r="AH29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI29" t="inlineStr">
+      <c r="AI29" t="n">
+        <v>3429</v>
+      </c>
+      <c r="AJ29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK29" t="inlineStr">
         <is>
           <t>3429</t>
         </is>
@@ -3090,9 +3210,15 @@
       <c r="AH30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI30" t="inlineStr">
-        <is>
-          <t>3598</t>
+      <c r="AI30" t="n">
+        <v>3598</v>
+      </c>
+      <c r="AJ30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK30" t="inlineStr">
+        <is>
+          <t>3597</t>
         </is>
       </c>
     </row>
@@ -3205,9 +3331,15 @@
       <c r="AH31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AI31" t="inlineStr">
-        <is>
-          <t>4891</t>
+      <c r="AI31" t="n">
+        <v>4891</v>
+      </c>
+      <c r="AJ31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK31" t="inlineStr">
+        <is>
+          <t>5129</t>
         </is>
       </c>
     </row>
@@ -3320,9 +3452,15 @@
       <c r="AH32" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AI32" t="inlineStr">
-        <is>
-          <t>2887</t>
+      <c r="AI32" t="n">
+        <v>2887</v>
+      </c>
+      <c r="AJ32" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK32" t="inlineStr">
+        <is>
+          <t>3262</t>
         </is>
       </c>
     </row>
@@ -3374,6 +3512,8 @@
       <c r="AG33" t="inlineStr"/>
       <c r="AH33" s="4" t="inlineStr"/>
       <c r="AI33" t="inlineStr"/>
+      <c r="AJ33" s="4" t="inlineStr"/>
+      <c r="AK33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3484,9 +3624,15 @@
       <c r="AH34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI34" t="inlineStr">
-        <is>
-          <t>2571</t>
+      <c r="AI34" t="n">
+        <v>2571</v>
+      </c>
+      <c r="AJ34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK34" t="inlineStr">
+        <is>
+          <t>2593</t>
         </is>
       </c>
     </row>
@@ -3599,7 +3745,13 @@
       <c r="AH35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI35" t="inlineStr">
+      <c r="AI35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK35" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3714,9 +3866,15 @@
       <c r="AH36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI36" t="inlineStr">
-        <is>
-          <t>2921</t>
+      <c r="AI36" t="n">
+        <v>2921</v>
+      </c>
+      <c r="AJ36" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK36" t="inlineStr">
+        <is>
+          <t>3663</t>
         </is>
       </c>
     </row>
@@ -3829,9 +3987,15 @@
       <c r="AH37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AI37" t="inlineStr">
-        <is>
-          <t>4610</t>
+      <c r="AI37" t="n">
+        <v>4610</v>
+      </c>
+      <c r="AJ37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK37" t="inlineStr">
+        <is>
+          <t>4889</t>
         </is>
       </c>
     </row>
@@ -3944,9 +4108,15 @@
       <c r="AH38" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AI38" t="inlineStr">
-        <is>
-          <t>5269</t>
+      <c r="AI38" t="n">
+        <v>5269</v>
+      </c>
+      <c r="AJ38" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AK38" t="inlineStr">
+        <is>
+          <t>5617</t>
         </is>
       </c>
     </row>
@@ -4059,9 +4229,15 @@
       <c r="AH39" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="AI39" t="inlineStr">
-        <is>
-          <t>4496</t>
+      <c r="AI39" t="n">
+        <v>4496</v>
+      </c>
+      <c r="AJ39" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="AK39" t="inlineStr">
+        <is>
+          <t>4725</t>
         </is>
       </c>
     </row>
@@ -4174,7 +4350,13 @@
       <c r="AH40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI40" t="inlineStr">
+      <c r="AI40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4289,9 +4471,15 @@
       <c r="AH41" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="AI41" t="inlineStr">
-        <is>
-          <t>4319</t>
+      <c r="AI41" t="n">
+        <v>4319</v>
+      </c>
+      <c r="AJ41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK41" t="inlineStr">
+        <is>
+          <t>4519</t>
         </is>
       </c>
     </row>
@@ -4404,9 +4592,15 @@
       <c r="AH42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI42" t="inlineStr">
-        <is>
-          <t>2762</t>
+      <c r="AI42" t="n">
+        <v>2762</v>
+      </c>
+      <c r="AJ42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK42" t="inlineStr">
+        <is>
+          <t>2988</t>
         </is>
       </c>
     </row>
@@ -4458,6 +4652,8 @@
       <c r="AG43" t="inlineStr"/>
       <c r="AH43" s="4" t="inlineStr"/>
       <c r="AI43" t="inlineStr"/>
+      <c r="AJ43" s="4" t="inlineStr"/>
+      <c r="AK43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -4507,6 +4703,8 @@
       <c r="AG44" t="inlineStr"/>
       <c r="AH44" s="4" t="inlineStr"/>
       <c r="AI44" t="inlineStr"/>
+      <c r="AJ44" s="4" t="inlineStr"/>
+      <c r="AK44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -4588,6 +4786,8 @@
       <c r="AG45" t="inlineStr"/>
       <c r="AH45" s="4" t="inlineStr"/>
       <c r="AI45" t="inlineStr"/>
+      <c r="AJ45" s="4" t="inlineStr"/>
+      <c r="AK45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -4698,9 +4898,15 @@
       <c r="AH46" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="AI46" t="inlineStr">
-        <is>
-          <t>3851</t>
+      <c r="AI46" t="n">
+        <v>3851</v>
+      </c>
+      <c r="AJ46" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="AK46" t="inlineStr">
+        <is>
+          <t>4246</t>
         </is>
       </c>
     </row>
@@ -4813,9 +5019,15 @@
       <c r="AH47" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AI47" t="inlineStr">
-        <is>
-          <t>5146</t>
+      <c r="AI47" t="n">
+        <v>5146</v>
+      </c>
+      <c r="AJ47" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AK47" t="inlineStr">
+        <is>
+          <t>5653</t>
         </is>
       </c>
     </row>
@@ -4928,7 +5140,13 @@
       <c r="AH48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI48" t="inlineStr">
+      <c r="AI48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5043,9 +5261,15 @@
       <c r="AH49" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AI49" t="inlineStr">
-        <is>
-          <t>4690</t>
+      <c r="AI49" t="n">
+        <v>4690</v>
+      </c>
+      <c r="AJ49" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK49" t="inlineStr">
+        <is>
+          <t>4896</t>
         </is>
       </c>
     </row>
@@ -5158,9 +5382,15 @@
       <c r="AH50" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="AI50" t="inlineStr">
-        <is>
-          <t>4857</t>
+      <c r="AI50" t="n">
+        <v>4857</v>
+      </c>
+      <c r="AJ50" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AK50" t="inlineStr">
+        <is>
+          <t>5240</t>
         </is>
       </c>
     </row>
@@ -5244,6 +5474,8 @@
       <c r="AG51" t="inlineStr"/>
       <c r="AH51" s="4" t="inlineStr"/>
       <c r="AI51" t="inlineStr"/>
+      <c r="AJ51" s="4" t="inlineStr"/>
+      <c r="AK51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -5354,9 +5586,15 @@
       <c r="AH52" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AI52" t="inlineStr">
-        <is>
-          <t>4879</t>
+      <c r="AI52" t="n">
+        <v>4879</v>
+      </c>
+      <c r="AJ52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK52" t="inlineStr">
+        <is>
+          <t>5263</t>
         </is>
       </c>
     </row>
@@ -5469,9 +5707,15 @@
       <c r="AH53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI53" t="inlineStr">
-        <is>
-          <t>3936</t>
+      <c r="AI53" t="n">
+        <v>3936</v>
+      </c>
+      <c r="AJ53" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AK53" t="inlineStr">
+        <is>
+          <t>4273</t>
         </is>
       </c>
     </row>
@@ -5555,6 +5799,8 @@
       <c r="AG54" t="inlineStr"/>
       <c r="AH54" s="4" t="inlineStr"/>
       <c r="AI54" t="inlineStr"/>
+      <c r="AJ54" s="4" t="inlineStr"/>
+      <c r="AK54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -5665,9 +5911,15 @@
       <c r="AH55" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AI55" t="inlineStr">
-        <is>
-          <t>4430</t>
+      <c r="AI55" t="n">
+        <v>4430</v>
+      </c>
+      <c r="AJ55" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK55" t="inlineStr">
+        <is>
+          <t>4553</t>
         </is>
       </c>
     </row>
@@ -5780,9 +6032,15 @@
       <c r="AH56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AI56" t="inlineStr">
-        <is>
-          <t>5087</t>
+      <c r="AI56" t="n">
+        <v>5087</v>
+      </c>
+      <c r="AJ56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK56" t="inlineStr">
+        <is>
+          <t>5422</t>
         </is>
       </c>
     </row>
@@ -5895,9 +6153,15 @@
       <c r="AH57" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="AI57" t="inlineStr">
-        <is>
-          <t>4167</t>
+      <c r="AI57" t="n">
+        <v>4167</v>
+      </c>
+      <c r="AJ57" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AK57" t="inlineStr">
+        <is>
+          <t>4218</t>
         </is>
       </c>
     </row>
@@ -6010,9 +6274,15 @@
       <c r="AH58" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AI58" t="inlineStr">
-        <is>
-          <t>4191</t>
+      <c r="AI58" t="n">
+        <v>4191</v>
+      </c>
+      <c r="AJ58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AK58" t="inlineStr">
+        <is>
+          <t>4418</t>
         </is>
       </c>
     </row>
@@ -6125,9 +6395,15 @@
       <c r="AH59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AI59" t="inlineStr">
-        <is>
-          <t>4083</t>
+      <c r="AI59" t="n">
+        <v>4083</v>
+      </c>
+      <c r="AJ59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK59" t="inlineStr">
+        <is>
+          <t>4161</t>
         </is>
       </c>
     </row>
@@ -6240,9 +6516,15 @@
       <c r="AH60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AI60" t="inlineStr">
-        <is>
-          <t>4324</t>
+      <c r="AI60" t="n">
+        <v>4324</v>
+      </c>
+      <c r="AJ60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AK60" t="inlineStr">
+        <is>
+          <t>4475</t>
         </is>
       </c>
     </row>
@@ -6294,6 +6576,8 @@
       <c r="AG61" t="inlineStr"/>
       <c r="AH61" s="4" t="inlineStr"/>
       <c r="AI61" t="inlineStr"/>
+      <c r="AJ61" s="4" t="inlineStr"/>
+      <c r="AK61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -6404,9 +6688,15 @@
       <c r="AH62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AI62" t="inlineStr">
-        <is>
-          <t>4074</t>
+      <c r="AI62" t="n">
+        <v>4074</v>
+      </c>
+      <c r="AJ62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AK62" t="inlineStr">
+        <is>
+          <t>4129</t>
         </is>
       </c>
     </row>
@@ -6519,9 +6809,15 @@
       <c r="AH63" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AI63" t="inlineStr">
-        <is>
-          <t>3992</t>
+      <c r="AI63" t="n">
+        <v>3992</v>
+      </c>
+      <c r="AJ63" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AK63" t="inlineStr">
+        <is>
+          <t>4083</t>
         </is>
       </c>
     </row>
@@ -6634,9 +6930,15 @@
       <c r="AH64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AI64" t="inlineStr">
-        <is>
-          <t>4281</t>
+      <c r="AI64" t="n">
+        <v>4281</v>
+      </c>
+      <c r="AJ64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK64" t="inlineStr">
+        <is>
+          <t>4402</t>
         </is>
       </c>
     </row>
@@ -6740,6 +7042,8 @@
       <c r="AG65" t="inlineStr"/>
       <c r="AH65" s="4" t="inlineStr"/>
       <c r="AI65" t="inlineStr"/>
+      <c r="AJ65" s="4" t="inlineStr"/>
+      <c r="AK65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -6850,7 +7154,13 @@
       <c r="AH66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI66" t="inlineStr">
+      <c r="AI66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6965,7 +7275,13 @@
       <c r="AH67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI67" t="inlineStr">
+      <c r="AI67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7080,7 +7396,13 @@
       <c r="AH68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI68" t="inlineStr">
+      <c r="AI68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7134,6 +7456,8 @@
       <c r="AG69" t="inlineStr"/>
       <c r="AH69" s="4" t="inlineStr"/>
       <c r="AI69" t="inlineStr"/>
+      <c r="AJ69" s="4" t="inlineStr"/>
+      <c r="AK69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -7244,7 +7568,13 @@
       <c r="AH70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI70" t="inlineStr">
+      <c r="AI70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7359,7 +7689,13 @@
       <c r="AH71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI71" t="inlineStr">
+      <c r="AI71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7474,7 +7810,13 @@
       <c r="AH72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI72" t="inlineStr">
+      <c r="AI72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7589,9 +7931,15 @@
       <c r="AH73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI73" t="inlineStr">
-        <is>
-          <t>2815</t>
+      <c r="AI73" t="n">
+        <v>2815</v>
+      </c>
+      <c r="AJ73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK73" t="inlineStr">
+        <is>
+          <t>2862</t>
         </is>
       </c>
     </row>
@@ -7704,7 +8052,13 @@
       <c r="AH74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI74" t="inlineStr">
+      <c r="AI74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7819,7 +8173,13 @@
       <c r="AH75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI75" t="inlineStr">
+      <c r="AI75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7934,9 +8294,15 @@
       <c r="AH76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI76" t="inlineStr">
-        <is>
-          <t>2922</t>
+      <c r="AI76" t="n">
+        <v>2922</v>
+      </c>
+      <c r="AJ76" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AK76" t="inlineStr">
+        <is>
+          <t>3583</t>
         </is>
       </c>
     </row>
@@ -8049,9 +8415,15 @@
       <c r="AH77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI77" t="inlineStr">
-        <is>
-          <t>2631</t>
+      <c r="AI77" t="n">
+        <v>2631</v>
+      </c>
+      <c r="AJ77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK77" t="inlineStr">
+        <is>
+          <t>2673</t>
         </is>
       </c>
     </row>
@@ -8164,7 +8536,13 @@
       <c r="AH78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI78" t="inlineStr">
+      <c r="AI78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8279,7 +8657,13 @@
       <c r="AH79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI79" t="inlineStr">
+      <c r="AI79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8394,7 +8778,13 @@
       <c r="AH80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI80" t="inlineStr">
+      <c r="AI80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8509,7 +8899,13 @@
       <c r="AH81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI81" t="inlineStr">
+      <c r="AI81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8624,7 +9020,13 @@
       <c r="AH82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI82" t="inlineStr">
+      <c r="AI82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8739,7 +9141,13 @@
       <c r="AH83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI83" t="inlineStr">
+      <c r="AI83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8854,7 +9262,13 @@
       <c r="AH84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI84" t="inlineStr">
+      <c r="AI84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8969,7 +9383,13 @@
       <c r="AH85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI85" t="inlineStr">
+      <c r="AI85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9084,9 +9504,15 @@
       <c r="AH86" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="AI86" t="inlineStr">
-        <is>
-          <t>1085</t>
+      <c r="AI86" t="n">
+        <v>1085</v>
+      </c>
+      <c r="AJ86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK86" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -9199,7 +9625,13 @@
       <c r="AH87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI87" t="inlineStr">
+      <c r="AI87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9314,7 +9746,13 @@
       <c r="AH88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI88" t="inlineStr">
+      <c r="AI88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9429,7 +9867,13 @@
       <c r="AH89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI89" t="inlineStr">
+      <c r="AI89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9544,7 +9988,13 @@
       <c r="AH90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI90" t="inlineStr">
+      <c r="AI90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9659,7 +10109,13 @@
       <c r="AH91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI91" t="inlineStr">
+      <c r="AI91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9774,7 +10230,13 @@
       <c r="AH92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI92" t="inlineStr">
+      <c r="AI92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9889,7 +10351,13 @@
       <c r="AH93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI93" t="inlineStr">
+      <c r="AI93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10004,7 +10472,13 @@
       <c r="AH94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI94" t="inlineStr">
+      <c r="AI94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10119,7 +10593,13 @@
       <c r="AH95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI95" t="inlineStr">
+      <c r="AI95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10234,9 +10714,15 @@
       <c r="AH96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI96" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AI96" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK96" t="inlineStr">
+        <is>
+          <t>2493</t>
         </is>
       </c>
     </row>
@@ -10349,7 +10835,13 @@
       <c r="AH97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI97" t="inlineStr">
+      <c r="AI97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10464,7 +10956,13 @@
       <c r="AH98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI98" t="inlineStr">
+      <c r="AI98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10579,7 +11077,13 @@
       <c r="AH99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI99" t="inlineStr">
+      <c r="AI99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10694,7 +11198,13 @@
       <c r="AH100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI100" t="inlineStr">
+      <c r="AI100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10809,7 +11319,13 @@
       <c r="AH101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI101" t="inlineStr">
+      <c r="AI101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10924,7 +11440,13 @@
       <c r="AH102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI102" t="inlineStr">
+      <c r="AI102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11039,7 +11561,13 @@
       <c r="AH103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI103" t="inlineStr">
+      <c r="AI103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11154,7 +11682,13 @@
       <c r="AH104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI104" t="inlineStr">
+      <c r="AI104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11269,7 +11803,13 @@
       <c r="AH105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI105" t="inlineStr">
+      <c r="AI105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11323,6 +11863,8 @@
       <c r="AG106" t="inlineStr"/>
       <c r="AH106" s="4" t="inlineStr"/>
       <c r="AI106" t="inlineStr"/>
+      <c r="AJ106" s="4" t="inlineStr"/>
+      <c r="AK106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -11372,6 +11914,8 @@
       <c r="AG107" t="inlineStr"/>
       <c r="AH107" s="4" t="inlineStr"/>
       <c r="AI107" t="inlineStr"/>
+      <c r="AJ107" s="4" t="inlineStr"/>
+      <c r="AK107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -11421,6 +11965,8 @@
       <c r="AG108" t="inlineStr"/>
       <c r="AH108" s="4" t="inlineStr"/>
       <c r="AI108" t="inlineStr"/>
+      <c r="AJ108" s="4" t="inlineStr"/>
+      <c r="AK108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -11470,6 +12016,8 @@
       <c r="AG109" t="inlineStr"/>
       <c r="AH109" s="4" t="inlineStr"/>
       <c r="AI109" t="inlineStr"/>
+      <c r="AJ109" s="4" t="inlineStr"/>
+      <c r="AK109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -11519,6 +12067,8 @@
       <c r="AG110" t="inlineStr"/>
       <c r="AH110" s="4" t="inlineStr"/>
       <c r="AI110" t="inlineStr"/>
+      <c r="AJ110" s="4" t="inlineStr"/>
+      <c r="AK110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -11568,6 +12118,8 @@
       <c r="AG111" t="inlineStr"/>
       <c r="AH111" s="4" t="inlineStr"/>
       <c r="AI111" t="inlineStr"/>
+      <c r="AJ111" s="4" t="inlineStr"/>
+      <c r="AK111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -11617,6 +12169,8 @@
       <c r="AG112" t="inlineStr"/>
       <c r="AH112" s="4" t="inlineStr"/>
       <c r="AI112" t="inlineStr"/>
+      <c r="AJ112" s="4" t="inlineStr"/>
+      <c r="AK112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -11666,6 +12220,8 @@
       <c r="AG113" t="inlineStr"/>
       <c r="AH113" s="4" t="inlineStr"/>
       <c r="AI113" t="inlineStr"/>
+      <c r="AJ113" s="4" t="inlineStr"/>
+      <c r="AK113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -11715,6 +12271,8 @@
       <c r="AG114" t="inlineStr"/>
       <c r="AH114" s="4" t="inlineStr"/>
       <c r="AI114" t="inlineStr"/>
+      <c r="AJ114" s="4" t="inlineStr"/>
+      <c r="AK114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -11803,9 +12361,15 @@
       <c r="AH115" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AI115" t="inlineStr">
-        <is>
-          <t>5368</t>
+      <c r="AI115" t="n">
+        <v>5368</v>
+      </c>
+      <c r="AJ115" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AK115" t="inlineStr">
+        <is>
+          <t>5742</t>
         </is>
       </c>
     </row>
@@ -11912,7 +12476,13 @@
       <c r="AH116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI116" t="inlineStr">
+      <c r="AI116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12000,6 +12570,8 @@
       </c>
       <c r="AH117" s="4" t="inlineStr"/>
       <c r="AI117" t="inlineStr"/>
+      <c r="AJ117" s="4" t="inlineStr"/>
+      <c r="AK117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -12104,9 +12676,15 @@
       <c r="AH118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI118" t="inlineStr">
-        <is>
-          <t>3304</t>
+      <c r="AI118" t="n">
+        <v>3304</v>
+      </c>
+      <c r="AJ118" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK118" t="inlineStr">
+        <is>
+          <t>3319</t>
         </is>
       </c>
     </row>
@@ -12213,9 +12791,15 @@
       <c r="AH119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI119" t="inlineStr">
-        <is>
-          <t>1578</t>
+      <c r="AI119" t="n">
+        <v>1578</v>
+      </c>
+      <c r="AJ119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK119" t="inlineStr">
+        <is>
+          <t>1574</t>
         </is>
       </c>
     </row>
@@ -12322,7 +12906,13 @@
       <c r="AH120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI120" t="inlineStr">
+      <c r="AI120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK120" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12431,7 +13021,13 @@
       <c r="AH121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI121" t="inlineStr">
+      <c r="AI121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12540,7 +13136,13 @@
       <c r="AH122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI122" t="inlineStr">
+      <c r="AI122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12645,7 +13247,13 @@
       <c r="AH123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI123" t="inlineStr">
+      <c r="AI123" t="n">
+        <v>2680</v>
+      </c>
+      <c r="AJ123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK123" t="inlineStr">
         <is>
           <t>2680</t>
         </is>
@@ -12725,6 +13333,8 @@
       <c r="AG124" t="inlineStr"/>
       <c r="AH124" s="4" t="inlineStr"/>
       <c r="AI124" t="inlineStr"/>
+      <c r="AJ124" s="4" t="inlineStr"/>
+      <c r="AK124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -12821,9 +13431,15 @@
       <c r="AH125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI125" t="inlineStr">
-        <is>
-          <t>2280</t>
+      <c r="AI125" t="n">
+        <v>2280</v>
+      </c>
+      <c r="AJ125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK125" t="inlineStr">
+        <is>
+          <t>2286</t>
         </is>
       </c>
     </row>
@@ -12910,9 +13526,15 @@
       <c r="AH126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI126" t="inlineStr">
-        <is>
-          <t>1526</t>
+      <c r="AI126" t="n">
+        <v>1526</v>
+      </c>
+      <c r="AJ126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK126" t="inlineStr">
+        <is>
+          <t>1553</t>
         </is>
       </c>
     </row>
@@ -12982,6 +13604,8 @@
       <c r="AG127" t="inlineStr"/>
       <c r="AH127" s="4" t="inlineStr"/>
       <c r="AI127" t="inlineStr"/>
+      <c r="AJ127" s="4" t="inlineStr"/>
+      <c r="AK127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -13058,11 +13682,11 @@
       <c r="AH128" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AI128" t="inlineStr">
-        <is>
-          <t>3972</t>
-        </is>
-      </c>
+      <c r="AI128" t="n">
+        <v>3972</v>
+      </c>
+      <c r="AJ128" s="4" t="inlineStr"/>
+      <c r="AK128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -13139,9 +13763,15 @@
       <c r="AH129" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AI129" t="inlineStr">
-        <is>
-          <t>3411</t>
+      <c r="AI129" t="n">
+        <v>3411</v>
+      </c>
+      <c r="AJ129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK129" t="inlineStr">
+        <is>
+          <t>3414</t>
         </is>
       </c>
     </row>
@@ -13220,11 +13850,11 @@
       <c r="AH130" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="AI130" t="inlineStr">
-        <is>
-          <t>1520</t>
-        </is>
-      </c>
+      <c r="AI130" t="n">
+        <v>1520</v>
+      </c>
+      <c r="AJ130" s="4" t="inlineStr"/>
+      <c r="AK130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -13297,7 +13927,13 @@
       <c r="AH131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI131" t="inlineStr">
+      <c r="AI131" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AJ131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK131" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -13362,9 +13998,15 @@
       <c r="AH132" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="AI132" t="inlineStr">
-        <is>
-          <t>4206</t>
+      <c r="AI132" t="n">
+        <v>4206</v>
+      </c>
+      <c r="AJ132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK132" t="inlineStr">
+        <is>
+          <t>4249</t>
         </is>
       </c>
     </row>
@@ -13427,9 +14069,15 @@
       <c r="AH133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AI133" t="inlineStr">
-        <is>
-          <t>3272</t>
+      <c r="AI133" t="n">
+        <v>3272</v>
+      </c>
+      <c r="AJ133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AK133" t="inlineStr">
+        <is>
+          <t>3241</t>
         </is>
       </c>
     </row>
@@ -13483,6 +14131,8 @@
       <c r="AG134" t="inlineStr"/>
       <c r="AH134" s="4" t="inlineStr"/>
       <c r="AI134" t="inlineStr"/>
+      <c r="AJ134" s="4" t="inlineStr"/>
+      <c r="AK134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -13538,6 +14188,8 @@
       </c>
       <c r="AH135" s="4" t="inlineStr"/>
       <c r="AI135" t="inlineStr"/>
+      <c r="AJ135" s="4" t="inlineStr"/>
+      <c r="AK135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -13593,6 +14245,8 @@
       </c>
       <c r="AH136" s="4" t="inlineStr"/>
       <c r="AI136" t="inlineStr"/>
+      <c r="AJ136" s="4" t="inlineStr"/>
+      <c r="AK136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -13648,6 +14302,8 @@
       </c>
       <c r="AH137" s="4" t="inlineStr"/>
       <c r="AI137" t="inlineStr"/>
+      <c r="AJ137" s="4" t="inlineStr"/>
+      <c r="AK137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -13703,6 +14359,8 @@
       </c>
       <c r="AH138" s="4" t="inlineStr"/>
       <c r="AI138" t="inlineStr"/>
+      <c r="AJ138" s="4" t="inlineStr"/>
+      <c r="AK138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -13758,6 +14416,65 @@
       </c>
       <c r="AH139" s="4" t="inlineStr"/>
       <c r="AI139" t="inlineStr"/>
+      <c r="AJ139" s="4" t="inlineStr"/>
+      <c r="AK139" t="inlineStr"/>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>6108533</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Harsh_Shukla</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr"/>
+      <c r="D140" t="inlineStr"/>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F140" s="4" t="inlineStr"/>
+      <c r="G140" t="inlineStr"/>
+      <c r="H140" s="4" t="inlineStr"/>
+      <c r="I140" t="inlineStr"/>
+      <c r="J140" s="4" t="inlineStr"/>
+      <c r="K140" t="inlineStr"/>
+      <c r="L140" s="4" t="inlineStr"/>
+      <c r="M140" t="inlineStr"/>
+      <c r="N140" s="4" t="inlineStr"/>
+      <c r="O140" t="inlineStr"/>
+      <c r="P140" s="4" t="inlineStr"/>
+      <c r="Q140" t="inlineStr"/>
+      <c r="R140" s="4" t="inlineStr"/>
+      <c r="S140" t="inlineStr"/>
+      <c r="T140" s="4" t="inlineStr"/>
+      <c r="U140" t="inlineStr"/>
+      <c r="V140" s="4" t="inlineStr"/>
+      <c r="W140" t="inlineStr"/>
+      <c r="X140" s="4" t="inlineStr"/>
+      <c r="Y140" t="inlineStr"/>
+      <c r="Z140" s="4" t="inlineStr"/>
+      <c r="AA140" t="inlineStr"/>
+      <c r="AB140" s="4" t="inlineStr"/>
+      <c r="AC140" t="inlineStr"/>
+      <c r="AD140" s="4" t="inlineStr"/>
+      <c r="AE140" t="inlineStr"/>
+      <c r="AF140" s="4" t="inlineStr"/>
+      <c r="AG140" t="inlineStr"/>
+      <c r="AH140" s="4" t="inlineStr"/>
+      <c r="AI140" t="inlineStr"/>
+      <c r="AJ140" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK140" t="inlineStr">
+        <is>
+          <t>2075</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Code updated 23-06-02 11:31:00
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK140"/>
+  <dimension ref="A1:AK141"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -694,7 +694,7 @@
       </c>
       <c r="AK2" t="inlineStr">
         <is>
-          <t>4708</t>
+          <t>5007</t>
         </is>
       </c>
     </row>
@@ -1057,7 +1057,7 @@
       </c>
       <c r="AK5" t="inlineStr">
         <is>
-          <t>2814</t>
+          <t>2809</t>
         </is>
       </c>
     </row>
@@ -1856,11 +1856,11 @@
         <v>3994</v>
       </c>
       <c r="AJ18" s="3" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="AK18" t="inlineStr">
         <is>
-          <t>4017</t>
+          <t>4076</t>
         </is>
       </c>
     </row>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="AK19" t="inlineStr">
         <is>
-          <t>2811</t>
+          <t>2859</t>
         </is>
       </c>
     </row>
@@ -2098,11 +2098,11 @@
         <v>4366</v>
       </c>
       <c r="AJ20" s="4" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="AK20" t="inlineStr">
         <is>
-          <t>4476</t>
+          <t>4532</t>
         </is>
       </c>
     </row>
@@ -2223,7 +2223,7 @@
       </c>
       <c r="AK21" t="inlineStr">
         <is>
-          <t>3007</t>
+          <t>3006</t>
         </is>
       </c>
     </row>
@@ -2344,7 +2344,7 @@
       </c>
       <c r="AK22" t="inlineStr">
         <is>
-          <t>5166</t>
+          <t>5288</t>
         </is>
       </c>
     </row>
@@ -2461,11 +2461,11 @@
         <v>5340</v>
       </c>
       <c r="AJ23" s="4" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AK23" t="inlineStr">
         <is>
-          <t>5773</t>
+          <t>6027</t>
         </is>
       </c>
     </row>
@@ -2586,7 +2586,7 @@
       </c>
       <c r="AK24" t="inlineStr">
         <is>
-          <t>5060</t>
+          <t>5194</t>
         </is>
       </c>
     </row>
@@ -3339,7 +3339,7 @@
       </c>
       <c r="AK31" t="inlineStr">
         <is>
-          <t>5129</t>
+          <t>5255</t>
         </is>
       </c>
     </row>
@@ -3460,7 +3460,7 @@
       </c>
       <c r="AK32" t="inlineStr">
         <is>
-          <t>3262</t>
+          <t>3687</t>
         </is>
       </c>
     </row>
@@ -3632,7 +3632,7 @@
       </c>
       <c r="AK34" t="inlineStr">
         <is>
-          <t>2593</t>
+          <t>2625</t>
         </is>
       </c>
     </row>
@@ -3753,7 +3753,7 @@
       </c>
       <c r="AK35" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -3874,7 +3874,7 @@
       </c>
       <c r="AK36" t="inlineStr">
         <is>
-          <t>3663</t>
+          <t>4059</t>
         </is>
       </c>
     </row>
@@ -3995,7 +3995,7 @@
       </c>
       <c r="AK37" t="inlineStr">
         <is>
-          <t>4889</t>
+          <t>5008</t>
         </is>
       </c>
     </row>
@@ -4111,12 +4111,12 @@
       <c r="AI38" t="n">
         <v>5269</v>
       </c>
-      <c r="AJ38" s="5" t="n">
-        <v>32</v>
+      <c r="AJ38" s="4" t="n">
+        <v>30</v>
       </c>
       <c r="AK38" t="inlineStr">
         <is>
-          <t>5617</t>
+          <t>5802</t>
         </is>
       </c>
     </row>
@@ -4237,7 +4237,7 @@
       </c>
       <c r="AK39" t="inlineStr">
         <is>
-          <t>4725</t>
+          <t>4859</t>
         </is>
       </c>
     </row>
@@ -4479,7 +4479,7 @@
       </c>
       <c r="AK41" t="inlineStr">
         <is>
-          <t>4519</t>
+          <t>4506</t>
         </is>
       </c>
     </row>
@@ -4600,7 +4600,7 @@
       </c>
       <c r="AK42" t="inlineStr">
         <is>
-          <t>2988</t>
+          <t>3047</t>
         </is>
       </c>
     </row>
@@ -4906,7 +4906,7 @@
       </c>
       <c r="AK46" t="inlineStr">
         <is>
-          <t>4246</t>
+          <t>4394</t>
         </is>
       </c>
     </row>
@@ -5027,7 +5027,7 @@
       </c>
       <c r="AK47" t="inlineStr">
         <is>
-          <t>5653</t>
+          <t>5881</t>
         </is>
       </c>
     </row>
@@ -5264,12 +5264,12 @@
       <c r="AI49" t="n">
         <v>4690</v>
       </c>
-      <c r="AJ49" s="2" t="n">
-        <v>0</v>
+      <c r="AJ49" s="4" t="n">
+        <v>29</v>
       </c>
       <c r="AK49" t="inlineStr">
         <is>
-          <t>4896</t>
+          <t>5066</t>
         </is>
       </c>
     </row>
@@ -5390,7 +5390,7 @@
       </c>
       <c r="AK50" t="inlineStr">
         <is>
-          <t>5240</t>
+          <t>5374</t>
         </is>
       </c>
     </row>
@@ -5594,7 +5594,7 @@
       </c>
       <c r="AK52" t="inlineStr">
         <is>
-          <t>5263</t>
+          <t>5361</t>
         </is>
       </c>
     </row>
@@ -5711,11 +5711,11 @@
         <v>3936</v>
       </c>
       <c r="AJ53" s="3" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AK53" t="inlineStr">
         <is>
-          <t>4273</t>
+          <t>4366</t>
         </is>
       </c>
     </row>
@@ -5919,7 +5919,7 @@
       </c>
       <c r="AK55" t="inlineStr">
         <is>
-          <t>4553</t>
+          <t>4639</t>
         </is>
       </c>
     </row>
@@ -6040,7 +6040,7 @@
       </c>
       <c r="AK56" t="inlineStr">
         <is>
-          <t>5422</t>
+          <t>5617</t>
         </is>
       </c>
     </row>
@@ -6157,11 +6157,11 @@
         <v>4167</v>
       </c>
       <c r="AJ57" s="3" t="n">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="AK57" t="inlineStr">
         <is>
-          <t>4218</t>
+          <t>4365</t>
         </is>
       </c>
     </row>
@@ -6282,7 +6282,7 @@
       </c>
       <c r="AK58" t="inlineStr">
         <is>
-          <t>4418</t>
+          <t>4514</t>
         </is>
       </c>
     </row>
@@ -6403,7 +6403,7 @@
       </c>
       <c r="AK59" t="inlineStr">
         <is>
-          <t>4161</t>
+          <t>4229</t>
         </is>
       </c>
     </row>
@@ -6524,7 +6524,7 @@
       </c>
       <c r="AK60" t="inlineStr">
         <is>
-          <t>4475</t>
+          <t>4596</t>
         </is>
       </c>
     </row>
@@ -6696,7 +6696,7 @@
       </c>
       <c r="AK62" t="inlineStr">
         <is>
-          <t>4129</t>
+          <t>4183</t>
         </is>
       </c>
     </row>
@@ -6813,11 +6813,11 @@
         <v>3992</v>
       </c>
       <c r="AJ63" s="3" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AK63" t="inlineStr">
         <is>
-          <t>4083</t>
+          <t>4046</t>
         </is>
       </c>
     </row>
@@ -6938,7 +6938,7 @@
       </c>
       <c r="AK64" t="inlineStr">
         <is>
-          <t>4402</t>
+          <t>4590</t>
         </is>
       </c>
     </row>
@@ -7939,7 +7939,7 @@
       </c>
       <c r="AK73" t="inlineStr">
         <is>
-          <t>2862</t>
+          <t>2934</t>
         </is>
       </c>
     </row>
@@ -8297,12 +8297,12 @@
       <c r="AI76" t="n">
         <v>2922</v>
       </c>
-      <c r="AJ76" s="4" t="n">
-        <v>21</v>
+      <c r="AJ76" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AK76" t="inlineStr">
         <is>
-          <t>3583</t>
+          <t>3587</t>
         </is>
       </c>
     </row>
@@ -8423,7 +8423,7 @@
       </c>
       <c r="AK77" t="inlineStr">
         <is>
-          <t>2673</t>
+          <t>2778</t>
         </is>
       </c>
     </row>
@@ -10722,7 +10722,7 @@
       </c>
       <c r="AK96" t="inlineStr">
         <is>
-          <t>2493</t>
+          <t>2489</t>
         </is>
       </c>
     </row>
@@ -12365,11 +12365,11 @@
         <v>5368</v>
       </c>
       <c r="AJ115" s="4" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="AK115" t="inlineStr">
         <is>
-          <t>5742</t>
+          <t>5887</t>
         </is>
       </c>
     </row>
@@ -12679,12 +12679,12 @@
       <c r="AI118" t="n">
         <v>3304</v>
       </c>
-      <c r="AJ118" s="3" t="n">
-        <v>2</v>
+      <c r="AJ118" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AK118" t="inlineStr">
         <is>
-          <t>3319</t>
+          <t>3318</t>
         </is>
       </c>
     </row>
@@ -13439,7 +13439,7 @@
       </c>
       <c r="AK125" t="inlineStr">
         <is>
-          <t>2286</t>
+          <t>2284</t>
         </is>
       </c>
     </row>
@@ -13766,12 +13766,12 @@
       <c r="AI129" t="n">
         <v>3411</v>
       </c>
-      <c r="AJ129" s="2" t="n">
-        <v>0</v>
+      <c r="AJ129" s="3" t="n">
+        <v>11</v>
       </c>
       <c r="AK129" t="inlineStr">
         <is>
-          <t>3414</t>
+          <t>3568</t>
         </is>
       </c>
     </row>
@@ -14001,12 +14001,12 @@
       <c r="AI132" t="n">
         <v>4206</v>
       </c>
-      <c r="AJ132" s="2" t="n">
-        <v>0</v>
+      <c r="AJ132" s="3" t="n">
+        <v>3</v>
       </c>
       <c r="AK132" t="inlineStr">
         <is>
-          <t>4249</t>
+          <t>4253</t>
         </is>
       </c>
     </row>
@@ -14077,7 +14077,7 @@
       </c>
       <c r="AK133" t="inlineStr">
         <is>
-          <t>3241</t>
+          <t>3248</t>
         </is>
       </c>
     </row>
@@ -14420,10 +14420,8 @@
       <c r="AK139" t="inlineStr"/>
     </row>
     <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>6108533</t>
-        </is>
+      <c r="A140" t="n">
+        <v>6108533</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
@@ -14467,12 +14465,69 @@
       <c r="AG140" t="inlineStr"/>
       <c r="AH140" s="4" t="inlineStr"/>
       <c r="AI140" t="inlineStr"/>
-      <c r="AJ140" s="3" t="n">
-        <v>3</v>
+      <c r="AJ140" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AK140" t="inlineStr">
         <is>
-          <t>2075</t>
+          <t>2069</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>59437166</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>AbsurdRestoration29</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr"/>
+      <c r="D141" t="inlineStr"/>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F141" s="4" t="inlineStr"/>
+      <c r="G141" t="inlineStr"/>
+      <c r="H141" s="4" t="inlineStr"/>
+      <c r="I141" t="inlineStr"/>
+      <c r="J141" s="4" t="inlineStr"/>
+      <c r="K141" t="inlineStr"/>
+      <c r="L141" s="4" t="inlineStr"/>
+      <c r="M141" t="inlineStr"/>
+      <c r="N141" s="4" t="inlineStr"/>
+      <c r="O141" t="inlineStr"/>
+      <c r="P141" s="4" t="inlineStr"/>
+      <c r="Q141" t="inlineStr"/>
+      <c r="R141" s="4" t="inlineStr"/>
+      <c r="S141" t="inlineStr"/>
+      <c r="T141" s="4" t="inlineStr"/>
+      <c r="U141" t="inlineStr"/>
+      <c r="V141" s="4" t="inlineStr"/>
+      <c r="W141" t="inlineStr"/>
+      <c r="X141" s="4" t="inlineStr"/>
+      <c r="Y141" t="inlineStr"/>
+      <c r="Z141" s="4" t="inlineStr"/>
+      <c r="AA141" t="inlineStr"/>
+      <c r="AB141" s="4" t="inlineStr"/>
+      <c r="AC141" t="inlineStr"/>
+      <c r="AD141" s="4" t="inlineStr"/>
+      <c r="AE141" t="inlineStr"/>
+      <c r="AF141" s="4" t="inlineStr"/>
+      <c r="AG141" t="inlineStr"/>
+      <c r="AH141" s="4" t="inlineStr"/>
+      <c r="AI141" t="inlineStr"/>
+      <c r="AJ141" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="AK141" t="inlineStr">
+        <is>
+          <t>1750</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-06-03 23:24:58
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK141"/>
+  <dimension ref="A1:AM143"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -576,6 +576,16 @@
           <t>06-01_0</t>
         </is>
       </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>06-02_A</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>06-02_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -692,9 +702,15 @@
       <c r="AJ2" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="AK2" t="inlineStr">
-        <is>
-          <t>5007</t>
+      <c r="AK2" t="n">
+        <v>5007</v>
+      </c>
+      <c r="AL2" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM2" t="inlineStr">
+        <is>
+          <t>5055</t>
         </is>
       </c>
     </row>
@@ -813,7 +829,13 @@
       <c r="AJ3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK3" t="inlineStr">
+      <c r="AK3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -934,7 +956,13 @@
       <c r="AJ4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK4" t="inlineStr">
+      <c r="AK4" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AL4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM4" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -1055,9 +1083,15 @@
       <c r="AJ5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK5" t="inlineStr">
-        <is>
-          <t>2809</t>
+      <c r="AK5" t="n">
+        <v>2809</v>
+      </c>
+      <c r="AL5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM5" t="inlineStr">
+        <is>
+          <t>2834</t>
         </is>
       </c>
     </row>
@@ -1176,7 +1210,13 @@
       <c r="AJ6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK6" t="inlineStr">
+      <c r="AK6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1232,6 +1272,8 @@
       <c r="AI7" t="inlineStr"/>
       <c r="AJ7" s="4" t="inlineStr"/>
       <c r="AK7" t="inlineStr"/>
+      <c r="AL7" s="4" t="inlineStr"/>
+      <c r="AM7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1283,6 +1325,8 @@
       <c r="AI8" t="inlineStr"/>
       <c r="AJ8" s="4" t="inlineStr"/>
       <c r="AK8" t="inlineStr"/>
+      <c r="AL8" s="4" t="inlineStr"/>
+      <c r="AM8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1334,6 +1378,8 @@
       <c r="AI9" t="inlineStr"/>
       <c r="AJ9" s="4" t="inlineStr"/>
       <c r="AK9" t="inlineStr"/>
+      <c r="AL9" s="4" t="inlineStr"/>
+      <c r="AM9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1385,6 +1431,8 @@
       <c r="AI10" t="inlineStr"/>
       <c r="AJ10" s="4" t="inlineStr"/>
       <c r="AK10" t="inlineStr"/>
+      <c r="AL10" s="4" t="inlineStr"/>
+      <c r="AM10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1436,6 +1484,8 @@
       <c r="AI11" t="inlineStr"/>
       <c r="AJ11" s="4" t="inlineStr"/>
       <c r="AK11" t="inlineStr"/>
+      <c r="AL11" s="4" t="inlineStr"/>
+      <c r="AM11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1487,6 +1537,8 @@
       <c r="AI12" t="inlineStr"/>
       <c r="AJ12" s="4" t="inlineStr"/>
       <c r="AK12" t="inlineStr"/>
+      <c r="AL12" s="4" t="inlineStr"/>
+      <c r="AM12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1538,6 +1590,8 @@
       <c r="AI13" t="inlineStr"/>
       <c r="AJ13" s="4" t="inlineStr"/>
       <c r="AK13" t="inlineStr"/>
+      <c r="AL13" s="4" t="inlineStr"/>
+      <c r="AM13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1589,6 +1643,8 @@
       <c r="AI14" t="inlineStr"/>
       <c r="AJ14" s="4" t="inlineStr"/>
       <c r="AK14" t="inlineStr"/>
+      <c r="AL14" s="4" t="inlineStr"/>
+      <c r="AM14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1640,6 +1696,8 @@
       <c r="AI15" t="inlineStr"/>
       <c r="AJ15" s="4" t="inlineStr"/>
       <c r="AK15" t="inlineStr"/>
+      <c r="AL15" s="4" t="inlineStr"/>
+      <c r="AM15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1691,6 +1749,8 @@
       <c r="AI16" t="inlineStr"/>
       <c r="AJ16" s="4" t="inlineStr"/>
       <c r="AK16" t="inlineStr"/>
+      <c r="AL16" s="4" t="inlineStr"/>
+      <c r="AM16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1742,6 +1802,8 @@
       <c r="AI17" t="inlineStr"/>
       <c r="AJ17" s="4" t="inlineStr"/>
       <c r="AK17" t="inlineStr"/>
+      <c r="AL17" s="4" t="inlineStr"/>
+      <c r="AM17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1858,9 +1920,15 @@
       <c r="AJ18" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="AK18" t="inlineStr">
-        <is>
-          <t>4076</t>
+      <c r="AK18" t="n">
+        <v>4076</v>
+      </c>
+      <c r="AL18" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AM18" t="inlineStr">
+        <is>
+          <t>4112</t>
         </is>
       </c>
     </row>
@@ -1979,9 +2047,15 @@
       <c r="AJ19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK19" t="inlineStr">
-        <is>
-          <t>2859</t>
+      <c r="AK19" t="n">
+        <v>2859</v>
+      </c>
+      <c r="AL19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM19" t="inlineStr">
+        <is>
+          <t>2857</t>
         </is>
       </c>
     </row>
@@ -2100,9 +2174,15 @@
       <c r="AJ20" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="AK20" t="inlineStr">
-        <is>
-          <t>4532</t>
+      <c r="AK20" t="n">
+        <v>4532</v>
+      </c>
+      <c r="AL20" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM20" t="inlineStr">
+        <is>
+          <t>4601</t>
         </is>
       </c>
     </row>
@@ -2221,9 +2301,15 @@
       <c r="AJ21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK21" t="inlineStr">
-        <is>
-          <t>3006</t>
+      <c r="AK21" t="n">
+        <v>3006</v>
+      </c>
+      <c r="AL21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM21" t="inlineStr">
+        <is>
+          <t>3002</t>
         </is>
       </c>
     </row>
@@ -2342,9 +2428,15 @@
       <c r="AJ22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AK22" t="inlineStr">
-        <is>
-          <t>5288</t>
+      <c r="AK22" t="n">
+        <v>5288</v>
+      </c>
+      <c r="AL22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM22" t="inlineStr">
+        <is>
+          <t>5405</t>
         </is>
       </c>
     </row>
@@ -2463,9 +2555,15 @@
       <c r="AJ23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AK23" t="inlineStr">
-        <is>
-          <t>6027</t>
+      <c r="AK23" t="n">
+        <v>6027</v>
+      </c>
+      <c r="AL23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AM23" t="inlineStr">
+        <is>
+          <t>6176</t>
         </is>
       </c>
     </row>
@@ -2584,9 +2682,15 @@
       <c r="AJ24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AK24" t="inlineStr">
-        <is>
-          <t>5194</t>
+      <c r="AK24" t="n">
+        <v>5194</v>
+      </c>
+      <c r="AL24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AM24" t="inlineStr">
+        <is>
+          <t>5423</t>
         </is>
       </c>
     </row>
@@ -2704,6 +2808,8 @@
       </c>
       <c r="AJ25" s="4" t="inlineStr"/>
       <c r="AK25" t="inlineStr"/>
+      <c r="AL25" s="4" t="inlineStr"/>
+      <c r="AM25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2807,6 +2913,8 @@
       <c r="AI26" t="inlineStr"/>
       <c r="AJ26" s="4" t="inlineStr"/>
       <c r="AK26" t="inlineStr"/>
+      <c r="AL26" s="4" t="inlineStr"/>
+      <c r="AM26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2923,9 +3031,15 @@
       <c r="AJ27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK27" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="AK27" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AL27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM27" t="inlineStr">
+        <is>
+          <t>2516</t>
         </is>
       </c>
     </row>
@@ -2979,6 +3093,8 @@
       <c r="AI28" t="inlineStr"/>
       <c r="AJ28" s="4" t="inlineStr"/>
       <c r="AK28" t="inlineStr"/>
+      <c r="AL28" s="4" t="inlineStr"/>
+      <c r="AM28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -3095,9 +3211,15 @@
       <c r="AJ29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK29" t="inlineStr">
-        <is>
-          <t>3429</t>
+      <c r="AK29" t="n">
+        <v>3429</v>
+      </c>
+      <c r="AL29" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AM29" t="inlineStr">
+        <is>
+          <t>3796</t>
         </is>
       </c>
     </row>
@@ -3216,9 +3338,15 @@
       <c r="AJ30" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK30" t="inlineStr">
-        <is>
-          <t>3597</t>
+      <c r="AK30" t="n">
+        <v>3597</v>
+      </c>
+      <c r="AL30" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AM30" t="inlineStr">
+        <is>
+          <t>3738</t>
         </is>
       </c>
     </row>
@@ -3337,9 +3465,15 @@
       <c r="AJ31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AK31" t="inlineStr">
-        <is>
-          <t>5255</t>
+      <c r="AK31" t="n">
+        <v>5255</v>
+      </c>
+      <c r="AL31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM31" t="inlineStr">
+        <is>
+          <t>5410</t>
         </is>
       </c>
     </row>
@@ -3458,9 +3592,15 @@
       <c r="AJ32" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AK32" t="inlineStr">
-        <is>
-          <t>3687</t>
+      <c r="AK32" t="n">
+        <v>3687</v>
+      </c>
+      <c r="AL32" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM32" t="inlineStr">
+        <is>
+          <t>4186</t>
         </is>
       </c>
     </row>
@@ -3514,6 +3654,8 @@
       <c r="AI33" t="inlineStr"/>
       <c r="AJ33" s="4" t="inlineStr"/>
       <c r="AK33" t="inlineStr"/>
+      <c r="AL33" s="4" t="inlineStr"/>
+      <c r="AM33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3630,7 +3772,13 @@
       <c r="AJ34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK34" t="inlineStr">
+      <c r="AK34" t="n">
+        <v>2625</v>
+      </c>
+      <c r="AL34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM34" t="inlineStr">
         <is>
           <t>2625</t>
         </is>
@@ -3751,7 +3899,13 @@
       <c r="AJ35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK35" t="inlineStr">
+      <c r="AK35" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AL35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM35" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3872,9 +4026,15 @@
       <c r="AJ36" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AK36" t="inlineStr">
-        <is>
-          <t>4059</t>
+      <c r="AK36" t="n">
+        <v>4059</v>
+      </c>
+      <c r="AL36" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM36" t="inlineStr">
+        <is>
+          <t>4418</t>
         </is>
       </c>
     </row>
@@ -3993,9 +4153,15 @@
       <c r="AJ37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AK37" t="inlineStr">
-        <is>
-          <t>5008</t>
+      <c r="AK37" t="n">
+        <v>5008</v>
+      </c>
+      <c r="AL37" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM37" t="inlineStr">
+        <is>
+          <t>5098</t>
         </is>
       </c>
     </row>
@@ -4114,9 +4280,15 @@
       <c r="AJ38" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AK38" t="inlineStr">
-        <is>
-          <t>5802</t>
+      <c r="AK38" t="n">
+        <v>5802</v>
+      </c>
+      <c r="AL38" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AM38" t="inlineStr">
+        <is>
+          <t>5979</t>
         </is>
       </c>
     </row>
@@ -4235,9 +4407,15 @@
       <c r="AJ39" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="AK39" t="inlineStr">
-        <is>
-          <t>4859</t>
+      <c r="AK39" t="n">
+        <v>4859</v>
+      </c>
+      <c r="AL39" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="AM39" t="inlineStr">
+        <is>
+          <t>4841</t>
         </is>
       </c>
     </row>
@@ -4356,7 +4534,13 @@
       <c r="AJ40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK40" t="inlineStr">
+      <c r="AK40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4477,9 +4661,15 @@
       <c r="AJ41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK41" t="inlineStr">
-        <is>
-          <t>4506</t>
+      <c r="AK41" t="n">
+        <v>4506</v>
+      </c>
+      <c r="AL41" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AM41" t="inlineStr">
+        <is>
+          <t>4608</t>
         </is>
       </c>
     </row>
@@ -4598,9 +4788,15 @@
       <c r="AJ42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK42" t="inlineStr">
-        <is>
-          <t>3047</t>
+      <c r="AK42" t="n">
+        <v>3047</v>
+      </c>
+      <c r="AL42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM42" t="inlineStr">
+        <is>
+          <t>3146</t>
         </is>
       </c>
     </row>
@@ -4654,6 +4850,8 @@
       <c r="AI43" t="inlineStr"/>
       <c r="AJ43" s="4" t="inlineStr"/>
       <c r="AK43" t="inlineStr"/>
+      <c r="AL43" s="4" t="inlineStr"/>
+      <c r="AM43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -4705,6 +4903,8 @@
       <c r="AI44" t="inlineStr"/>
       <c r="AJ44" s="4" t="inlineStr"/>
       <c r="AK44" t="inlineStr"/>
+      <c r="AL44" s="4" t="inlineStr"/>
+      <c r="AM44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -4788,6 +4988,8 @@
       <c r="AI45" t="inlineStr"/>
       <c r="AJ45" s="4" t="inlineStr"/>
       <c r="AK45" t="inlineStr"/>
+      <c r="AL45" s="4" t="inlineStr"/>
+      <c r="AM45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -4904,9 +5106,15 @@
       <c r="AJ46" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="AK46" t="inlineStr">
-        <is>
-          <t>4394</t>
+      <c r="AK46" t="n">
+        <v>4394</v>
+      </c>
+      <c r="AL46" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="AM46" t="inlineStr">
+        <is>
+          <t>4566</t>
         </is>
       </c>
     </row>
@@ -5025,9 +5233,15 @@
       <c r="AJ47" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AK47" t="inlineStr">
-        <is>
-          <t>5881</t>
+      <c r="AK47" t="n">
+        <v>5881</v>
+      </c>
+      <c r="AL47" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AM47" t="inlineStr">
+        <is>
+          <t>6058</t>
         </is>
       </c>
     </row>
@@ -5146,7 +5360,13 @@
       <c r="AJ48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK48" t="inlineStr">
+      <c r="AK48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5267,9 +5487,15 @@
       <c r="AJ49" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AK49" t="inlineStr">
-        <is>
-          <t>5066</t>
+      <c r="AK49" t="n">
+        <v>5066</v>
+      </c>
+      <c r="AL49" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="AM49" t="inlineStr">
+        <is>
+          <t>5240</t>
         </is>
       </c>
     </row>
@@ -5388,9 +5614,15 @@
       <c r="AJ50" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AK50" t="inlineStr">
-        <is>
-          <t>5374</t>
+      <c r="AK50" t="n">
+        <v>5374</v>
+      </c>
+      <c r="AL50" s="4" t="n">
+        <v>24</v>
+      </c>
+      <c r="AM50" t="inlineStr">
+        <is>
+          <t>5529</t>
         </is>
       </c>
     </row>
@@ -5476,6 +5708,8 @@
       <c r="AI51" t="inlineStr"/>
       <c r="AJ51" s="4" t="inlineStr"/>
       <c r="AK51" t="inlineStr"/>
+      <c r="AL51" s="4" t="inlineStr"/>
+      <c r="AM51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -5592,9 +5826,15 @@
       <c r="AJ52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AK52" t="inlineStr">
-        <is>
-          <t>5361</t>
+      <c r="AK52" t="n">
+        <v>5361</v>
+      </c>
+      <c r="AL52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM52" t="inlineStr">
+        <is>
+          <t>5551</t>
         </is>
       </c>
     </row>
@@ -5713,9 +5953,15 @@
       <c r="AJ53" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="AK53" t="inlineStr">
-        <is>
-          <t>4366</t>
+      <c r="AK53" t="n">
+        <v>4366</v>
+      </c>
+      <c r="AL53" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AM53" t="inlineStr">
+        <is>
+          <t>4525</t>
         </is>
       </c>
     </row>
@@ -5801,6 +6047,8 @@
       <c r="AI54" t="inlineStr"/>
       <c r="AJ54" s="4" t="inlineStr"/>
       <c r="AK54" t="inlineStr"/>
+      <c r="AL54" s="4" t="inlineStr"/>
+      <c r="AM54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -5917,9 +6165,15 @@
       <c r="AJ55" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AK55" t="inlineStr">
-        <is>
-          <t>4639</t>
+      <c r="AK55" t="n">
+        <v>4639</v>
+      </c>
+      <c r="AL55" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM55" t="inlineStr">
+        <is>
+          <t>4807</t>
         </is>
       </c>
     </row>
@@ -6038,9 +6292,15 @@
       <c r="AJ56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AK56" t="inlineStr">
-        <is>
-          <t>5617</t>
+      <c r="AK56" t="n">
+        <v>5617</v>
+      </c>
+      <c r="AL56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM56" t="inlineStr">
+        <is>
+          <t>5868</t>
         </is>
       </c>
     </row>
@@ -6159,9 +6419,15 @@
       <c r="AJ57" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="AK57" t="inlineStr">
-        <is>
-          <t>4365</t>
+      <c r="AK57" t="n">
+        <v>4365</v>
+      </c>
+      <c r="AL57" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AM57" t="inlineStr">
+        <is>
+          <t>4388</t>
         </is>
       </c>
     </row>
@@ -6280,9 +6546,15 @@
       <c r="AJ58" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AK58" t="inlineStr">
-        <is>
-          <t>4514</t>
+      <c r="AK58" t="n">
+        <v>4514</v>
+      </c>
+      <c r="AL58" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AM58" t="inlineStr">
+        <is>
+          <t>4713</t>
         </is>
       </c>
     </row>
@@ -6401,9 +6673,15 @@
       <c r="AJ59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AK59" t="inlineStr">
-        <is>
-          <t>4229</t>
+      <c r="AK59" t="n">
+        <v>4229</v>
+      </c>
+      <c r="AL59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM59" t="inlineStr">
+        <is>
+          <t>4356</t>
         </is>
       </c>
     </row>
@@ -6522,9 +6800,15 @@
       <c r="AJ60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AK60" t="inlineStr">
-        <is>
-          <t>4596</t>
+      <c r="AK60" t="n">
+        <v>4596</v>
+      </c>
+      <c r="AL60" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM60" t="inlineStr">
+        <is>
+          <t>4666</t>
         </is>
       </c>
     </row>
@@ -6578,6 +6862,8 @@
       <c r="AI61" t="inlineStr"/>
       <c r="AJ61" s="4" t="inlineStr"/>
       <c r="AK61" t="inlineStr"/>
+      <c r="AL61" s="4" t="inlineStr"/>
+      <c r="AM61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -6694,9 +6980,15 @@
       <c r="AJ62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AK62" t="inlineStr">
-        <is>
-          <t>4183</t>
+      <c r="AK62" t="n">
+        <v>4183</v>
+      </c>
+      <c r="AL62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AM62" t="inlineStr">
+        <is>
+          <t>4213</t>
         </is>
       </c>
     </row>
@@ -6815,9 +7107,15 @@
       <c r="AJ63" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="AK63" t="inlineStr">
-        <is>
-          <t>4046</t>
+      <c r="AK63" t="n">
+        <v>4046</v>
+      </c>
+      <c r="AL63" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AM63" t="inlineStr">
+        <is>
+          <t>4119</t>
         </is>
       </c>
     </row>
@@ -6936,9 +7234,15 @@
       <c r="AJ64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AK64" t="inlineStr">
-        <is>
-          <t>4590</t>
+      <c r="AK64" t="n">
+        <v>4590</v>
+      </c>
+      <c r="AL64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM64" t="inlineStr">
+        <is>
+          <t>4550</t>
         </is>
       </c>
     </row>
@@ -7044,6 +7348,8 @@
       <c r="AI65" t="inlineStr"/>
       <c r="AJ65" s="4" t="inlineStr"/>
       <c r="AK65" t="inlineStr"/>
+      <c r="AL65" s="4" t="inlineStr"/>
+      <c r="AM65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -7160,7 +7466,13 @@
       <c r="AJ66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK66" t="inlineStr">
+      <c r="AK66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7281,7 +7593,13 @@
       <c r="AJ67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK67" t="inlineStr">
+      <c r="AK67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7402,7 +7720,13 @@
       <c r="AJ68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK68" t="inlineStr">
+      <c r="AK68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7458,6 +7782,8 @@
       <c r="AI69" t="inlineStr"/>
       <c r="AJ69" s="4" t="inlineStr"/>
       <c r="AK69" t="inlineStr"/>
+      <c r="AL69" s="4" t="inlineStr"/>
+      <c r="AM69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -7574,7 +7900,13 @@
       <c r="AJ70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK70" t="inlineStr">
+      <c r="AK70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7695,7 +8027,13 @@
       <c r="AJ71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK71" t="inlineStr">
+      <c r="AK71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7816,7 +8154,13 @@
       <c r="AJ72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK72" t="inlineStr">
+      <c r="AK72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7937,9 +8281,15 @@
       <c r="AJ73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK73" t="inlineStr">
-        <is>
-          <t>2934</t>
+      <c r="AK73" t="n">
+        <v>2934</v>
+      </c>
+      <c r="AL73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM73" t="inlineStr">
+        <is>
+          <t>2986</t>
         </is>
       </c>
     </row>
@@ -8058,7 +8408,13 @@
       <c r="AJ74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK74" t="inlineStr">
+      <c r="AK74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8179,7 +8535,13 @@
       <c r="AJ75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK75" t="inlineStr">
+      <c r="AK75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8300,9 +8662,15 @@
       <c r="AJ76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK76" t="inlineStr">
-        <is>
-          <t>3587</t>
+      <c r="AK76" t="n">
+        <v>3587</v>
+      </c>
+      <c r="AL76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM76" t="inlineStr">
+        <is>
+          <t>3598</t>
         </is>
       </c>
     </row>
@@ -8421,9 +8789,15 @@
       <c r="AJ77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK77" t="inlineStr">
-        <is>
-          <t>2778</t>
+      <c r="AK77" t="n">
+        <v>2778</v>
+      </c>
+      <c r="AL77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM77" t="inlineStr">
+        <is>
+          <t>2803</t>
         </is>
       </c>
     </row>
@@ -8542,7 +8916,13 @@
       <c r="AJ78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK78" t="inlineStr">
+      <c r="AK78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8663,7 +9043,13 @@
       <c r="AJ79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK79" t="inlineStr">
+      <c r="AK79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8784,7 +9170,13 @@
       <c r="AJ80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK80" t="inlineStr">
+      <c r="AK80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8905,7 +9297,13 @@
       <c r="AJ81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK81" t="inlineStr">
+      <c r="AK81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9026,7 +9424,13 @@
       <c r="AJ82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK82" t="inlineStr">
+      <c r="AK82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9147,7 +9551,13 @@
       <c r="AJ83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK83" t="inlineStr">
+      <c r="AK83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9268,7 +9678,13 @@
       <c r="AJ84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK84" t="inlineStr">
+      <c r="AK84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9389,7 +9805,13 @@
       <c r="AJ85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK85" t="inlineStr">
+      <c r="AK85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9510,9 +9932,15 @@
       <c r="AJ86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK86" t="inlineStr">
-        <is>
-          <t>0</t>
+      <c r="AK86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM86" t="inlineStr">
+        <is>
+          <t>1084</t>
         </is>
       </c>
     </row>
@@ -9631,7 +10059,13 @@
       <c r="AJ87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK87" t="inlineStr">
+      <c r="AK87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9752,7 +10186,13 @@
       <c r="AJ88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK88" t="inlineStr">
+      <c r="AK88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9873,7 +10313,13 @@
       <c r="AJ89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK89" t="inlineStr">
+      <c r="AK89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9994,7 +10440,13 @@
       <c r="AJ90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK90" t="inlineStr">
+      <c r="AK90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10115,7 +10567,13 @@
       <c r="AJ91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK91" t="inlineStr">
+      <c r="AK91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10236,7 +10694,13 @@
       <c r="AJ92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK92" t="inlineStr">
+      <c r="AK92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10357,7 +10821,13 @@
       <c r="AJ93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK93" t="inlineStr">
+      <c r="AK93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10478,7 +10948,13 @@
       <c r="AJ94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK94" t="inlineStr">
+      <c r="AK94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10599,7 +11075,13 @@
       <c r="AJ95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK95" t="inlineStr">
+      <c r="AK95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10720,9 +11202,15 @@
       <c r="AJ96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK96" t="inlineStr">
-        <is>
-          <t>2489</t>
+      <c r="AK96" t="n">
+        <v>2489</v>
+      </c>
+      <c r="AL96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM96" t="inlineStr">
+        <is>
+          <t>2487</t>
         </is>
       </c>
     </row>
@@ -10841,7 +11329,13 @@
       <c r="AJ97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK97" t="inlineStr">
+      <c r="AK97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10962,7 +11456,13 @@
       <c r="AJ98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK98" t="inlineStr">
+      <c r="AK98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11083,7 +11583,13 @@
       <c r="AJ99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK99" t="inlineStr">
+      <c r="AK99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11204,7 +11710,13 @@
       <c r="AJ100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK100" t="inlineStr">
+      <c r="AK100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11325,7 +11837,13 @@
       <c r="AJ101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK101" t="inlineStr">
+      <c r="AK101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11446,7 +11964,13 @@
       <c r="AJ102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK102" t="inlineStr">
+      <c r="AK102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11567,7 +12091,13 @@
       <c r="AJ103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK103" t="inlineStr">
+      <c r="AK103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11688,7 +12218,13 @@
       <c r="AJ104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK104" t="inlineStr">
+      <c r="AK104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11809,7 +12345,13 @@
       <c r="AJ105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK105" t="inlineStr">
+      <c r="AK105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11865,6 +12407,8 @@
       <c r="AI106" t="inlineStr"/>
       <c r="AJ106" s="4" t="inlineStr"/>
       <c r="AK106" t="inlineStr"/>
+      <c r="AL106" s="4" t="inlineStr"/>
+      <c r="AM106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -11916,6 +12460,8 @@
       <c r="AI107" t="inlineStr"/>
       <c r="AJ107" s="4" t="inlineStr"/>
       <c r="AK107" t="inlineStr"/>
+      <c r="AL107" s="4" t="inlineStr"/>
+      <c r="AM107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -11967,6 +12513,8 @@
       <c r="AI108" t="inlineStr"/>
       <c r="AJ108" s="4" t="inlineStr"/>
       <c r="AK108" t="inlineStr"/>
+      <c r="AL108" s="4" t="inlineStr"/>
+      <c r="AM108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -12018,6 +12566,8 @@
       <c r="AI109" t="inlineStr"/>
       <c r="AJ109" s="4" t="inlineStr"/>
       <c r="AK109" t="inlineStr"/>
+      <c r="AL109" s="4" t="inlineStr"/>
+      <c r="AM109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -12069,6 +12619,8 @@
       <c r="AI110" t="inlineStr"/>
       <c r="AJ110" s="4" t="inlineStr"/>
       <c r="AK110" t="inlineStr"/>
+      <c r="AL110" s="4" t="inlineStr"/>
+      <c r="AM110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -12120,6 +12672,8 @@
       <c r="AI111" t="inlineStr"/>
       <c r="AJ111" s="4" t="inlineStr"/>
       <c r="AK111" t="inlineStr"/>
+      <c r="AL111" s="4" t="inlineStr"/>
+      <c r="AM111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -12171,6 +12725,8 @@
       <c r="AI112" t="inlineStr"/>
       <c r="AJ112" s="4" t="inlineStr"/>
       <c r="AK112" t="inlineStr"/>
+      <c r="AL112" s="4" t="inlineStr"/>
+      <c r="AM112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -12222,6 +12778,8 @@
       <c r="AI113" t="inlineStr"/>
       <c r="AJ113" s="4" t="inlineStr"/>
       <c r="AK113" t="inlineStr"/>
+      <c r="AL113" s="4" t="inlineStr"/>
+      <c r="AM113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -12273,6 +12831,8 @@
       <c r="AI114" t="inlineStr"/>
       <c r="AJ114" s="4" t="inlineStr"/>
       <c r="AK114" t="inlineStr"/>
+      <c r="AL114" s="4" t="inlineStr"/>
+      <c r="AM114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -12367,9 +12927,15 @@
       <c r="AJ115" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="AK115" t="inlineStr">
-        <is>
-          <t>5887</t>
+      <c r="AK115" t="n">
+        <v>5887</v>
+      </c>
+      <c r="AL115" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AM115" t="inlineStr">
+        <is>
+          <t>6032</t>
         </is>
       </c>
     </row>
@@ -12482,7 +13048,13 @@
       <c r="AJ116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK116" t="inlineStr">
+      <c r="AK116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12572,6 +13144,8 @@
       <c r="AI117" t="inlineStr"/>
       <c r="AJ117" s="4" t="inlineStr"/>
       <c r="AK117" t="inlineStr"/>
+      <c r="AL117" s="4" t="inlineStr"/>
+      <c r="AM117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -12682,9 +13256,15 @@
       <c r="AJ118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK118" t="inlineStr">
-        <is>
-          <t>3318</t>
+      <c r="AK118" t="n">
+        <v>3318</v>
+      </c>
+      <c r="AL118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM118" t="inlineStr">
+        <is>
+          <t>3334</t>
         </is>
       </c>
     </row>
@@ -12797,9 +13377,15 @@
       <c r="AJ119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK119" t="inlineStr">
-        <is>
-          <t>1574</t>
+      <c r="AK119" t="n">
+        <v>1574</v>
+      </c>
+      <c r="AL119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM119" t="inlineStr">
+        <is>
+          <t>1586</t>
         </is>
       </c>
     </row>
@@ -12912,7 +13498,13 @@
       <c r="AJ120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK120" t="inlineStr">
+      <c r="AK120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM120" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13027,7 +13619,13 @@
       <c r="AJ121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK121" t="inlineStr">
+      <c r="AK121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13142,7 +13740,13 @@
       <c r="AJ122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK122" t="inlineStr">
+      <c r="AK122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AL122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13253,7 +13857,13 @@
       <c r="AJ123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK123" t="inlineStr">
+      <c r="AK123" t="n">
+        <v>2680</v>
+      </c>
+      <c r="AL123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM123" t="inlineStr">
         <is>
           <t>2680</t>
         </is>
@@ -13335,6 +13945,8 @@
       <c r="AI124" t="inlineStr"/>
       <c r="AJ124" s="4" t="inlineStr"/>
       <c r="AK124" t="inlineStr"/>
+      <c r="AL124" s="4" t="inlineStr"/>
+      <c r="AM124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -13437,9 +14049,15 @@
       <c r="AJ125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK125" t="inlineStr">
-        <is>
-          <t>2284</t>
+      <c r="AK125" t="n">
+        <v>2284</v>
+      </c>
+      <c r="AL125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM125" t="inlineStr">
+        <is>
+          <t>2277</t>
         </is>
       </c>
     </row>
@@ -13532,7 +14150,13 @@
       <c r="AJ126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK126" t="inlineStr">
+      <c r="AK126" t="n">
+        <v>1553</v>
+      </c>
+      <c r="AL126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM126" t="inlineStr">
         <is>
           <t>1553</t>
         </is>
@@ -13606,6 +14230,8 @@
       <c r="AI127" t="inlineStr"/>
       <c r="AJ127" s="4" t="inlineStr"/>
       <c r="AK127" t="inlineStr"/>
+      <c r="AL127" s="4" t="inlineStr"/>
+      <c r="AM127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -13687,6 +14313,8 @@
       </c>
       <c r="AJ128" s="4" t="inlineStr"/>
       <c r="AK128" t="inlineStr"/>
+      <c r="AL128" s="4" t="inlineStr"/>
+      <c r="AM128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -13769,9 +14397,15 @@
       <c r="AJ129" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="AK129" t="inlineStr">
-        <is>
-          <t>3568</t>
+      <c r="AK129" t="n">
+        <v>3568</v>
+      </c>
+      <c r="AL129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM129" t="inlineStr">
+        <is>
+          <t>3567</t>
         </is>
       </c>
     </row>
@@ -13855,6 +14489,8 @@
       </c>
       <c r="AJ130" s="4" t="inlineStr"/>
       <c r="AK130" t="inlineStr"/>
+      <c r="AL130" s="4" t="inlineStr"/>
+      <c r="AM130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -13933,7 +14569,13 @@
       <c r="AJ131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK131" t="inlineStr">
+      <c r="AK131" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AL131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM131" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -14004,9 +14646,15 @@
       <c r="AJ132" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="AK132" t="inlineStr">
-        <is>
-          <t>4253</t>
+      <c r="AK132" t="n">
+        <v>4253</v>
+      </c>
+      <c r="AL132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM132" t="inlineStr">
+        <is>
+          <t>4250</t>
         </is>
       </c>
     </row>
@@ -14075,9 +14723,15 @@
       <c r="AJ133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK133" t="inlineStr">
-        <is>
-          <t>3248</t>
+      <c r="AK133" t="n">
+        <v>3248</v>
+      </c>
+      <c r="AL133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM133" t="inlineStr">
+        <is>
+          <t>3241</t>
         </is>
       </c>
     </row>
@@ -14133,6 +14787,8 @@
       <c r="AI134" t="inlineStr"/>
       <c r="AJ134" s="4" t="inlineStr"/>
       <c r="AK134" t="inlineStr"/>
+      <c r="AL134" s="4" t="inlineStr"/>
+      <c r="AM134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -14190,6 +14846,8 @@
       <c r="AI135" t="inlineStr"/>
       <c r="AJ135" s="4" t="inlineStr"/>
       <c r="AK135" t="inlineStr"/>
+      <c r="AL135" s="4" t="inlineStr"/>
+      <c r="AM135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -14247,6 +14905,8 @@
       <c r="AI136" t="inlineStr"/>
       <c r="AJ136" s="4" t="inlineStr"/>
       <c r="AK136" t="inlineStr"/>
+      <c r="AL136" s="4" t="inlineStr"/>
+      <c r="AM136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -14304,6 +14964,8 @@
       <c r="AI137" t="inlineStr"/>
       <c r="AJ137" s="4" t="inlineStr"/>
       <c r="AK137" t="inlineStr"/>
+      <c r="AL137" s="4" t="inlineStr"/>
+      <c r="AM137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -14361,6 +15023,8 @@
       <c r="AI138" t="inlineStr"/>
       <c r="AJ138" s="4" t="inlineStr"/>
       <c r="AK138" t="inlineStr"/>
+      <c r="AL138" s="4" t="inlineStr"/>
+      <c r="AM138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -14418,6 +15082,8 @@
       <c r="AI139" t="inlineStr"/>
       <c r="AJ139" s="4" t="inlineStr"/>
       <c r="AK139" t="inlineStr"/>
+      <c r="AL139" s="4" t="inlineStr"/>
+      <c r="AM139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -14468,17 +15134,21 @@
       <c r="AJ140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AK140" t="inlineStr">
-        <is>
-          <t>2069</t>
+      <c r="AK140" t="n">
+        <v>2069</v>
+      </c>
+      <c r="AL140" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="AM140" t="inlineStr">
+        <is>
+          <t>2232</t>
         </is>
       </c>
     </row>
     <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>59437166</t>
-        </is>
+      <c r="A141" t="n">
+        <v>59437166</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
@@ -14525,9 +15195,127 @@
       <c r="AJ141" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="AK141" t="inlineStr">
-        <is>
-          <t>1750</t>
+      <c r="AK141" t="n">
+        <v>1750</v>
+      </c>
+      <c r="AL141" s="4" t="inlineStr"/>
+      <c r="AM141" t="inlineStr"/>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>59127877</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>yasin22999</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr"/>
+      <c r="D142" t="inlineStr"/>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F142" s="4" t="inlineStr"/>
+      <c r="G142" t="inlineStr"/>
+      <c r="H142" s="4" t="inlineStr"/>
+      <c r="I142" t="inlineStr"/>
+      <c r="J142" s="4" t="inlineStr"/>
+      <c r="K142" t="inlineStr"/>
+      <c r="L142" s="4" t="inlineStr"/>
+      <c r="M142" t="inlineStr"/>
+      <c r="N142" s="4" t="inlineStr"/>
+      <c r="O142" t="inlineStr"/>
+      <c r="P142" s="4" t="inlineStr"/>
+      <c r="Q142" t="inlineStr"/>
+      <c r="R142" s="4" t="inlineStr"/>
+      <c r="S142" t="inlineStr"/>
+      <c r="T142" s="4" t="inlineStr"/>
+      <c r="U142" t="inlineStr"/>
+      <c r="V142" s="4" t="inlineStr"/>
+      <c r="W142" t="inlineStr"/>
+      <c r="X142" s="4" t="inlineStr"/>
+      <c r="Y142" t="inlineStr"/>
+      <c r="Z142" s="4" t="inlineStr"/>
+      <c r="AA142" t="inlineStr"/>
+      <c r="AB142" s="4" t="inlineStr"/>
+      <c r="AC142" t="inlineStr"/>
+      <c r="AD142" s="4" t="inlineStr"/>
+      <c r="AE142" t="inlineStr"/>
+      <c r="AF142" s="4" t="inlineStr"/>
+      <c r="AG142" t="inlineStr"/>
+      <c r="AH142" s="4" t="inlineStr"/>
+      <c r="AI142" t="inlineStr"/>
+      <c r="AJ142" s="4" t="inlineStr"/>
+      <c r="AK142" t="inlineStr"/>
+      <c r="AL142" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM142" t="inlineStr">
+        <is>
+          <t>2648</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>59482456</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>DialecticalCommerce7</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr"/>
+      <c r="D143" t="inlineStr"/>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F143" s="4" t="inlineStr"/>
+      <c r="G143" t="inlineStr"/>
+      <c r="H143" s="4" t="inlineStr"/>
+      <c r="I143" t="inlineStr"/>
+      <c r="J143" s="4" t="inlineStr"/>
+      <c r="K143" t="inlineStr"/>
+      <c r="L143" s="4" t="inlineStr"/>
+      <c r="M143" t="inlineStr"/>
+      <c r="N143" s="4" t="inlineStr"/>
+      <c r="O143" t="inlineStr"/>
+      <c r="P143" s="4" t="inlineStr"/>
+      <c r="Q143" t="inlineStr"/>
+      <c r="R143" s="4" t="inlineStr"/>
+      <c r="S143" t="inlineStr"/>
+      <c r="T143" s="4" t="inlineStr"/>
+      <c r="U143" t="inlineStr"/>
+      <c r="V143" s="4" t="inlineStr"/>
+      <c r="W143" t="inlineStr"/>
+      <c r="X143" s="4" t="inlineStr"/>
+      <c r="Y143" t="inlineStr"/>
+      <c r="Z143" s="4" t="inlineStr"/>
+      <c r="AA143" t="inlineStr"/>
+      <c r="AB143" s="4" t="inlineStr"/>
+      <c r="AC143" t="inlineStr"/>
+      <c r="AD143" s="4" t="inlineStr"/>
+      <c r="AE143" t="inlineStr"/>
+      <c r="AF143" s="4" t="inlineStr"/>
+      <c r="AG143" t="inlineStr"/>
+      <c r="AH143" s="4" t="inlineStr"/>
+      <c r="AI143" t="inlineStr"/>
+      <c r="AJ143" s="4" t="inlineStr"/>
+      <c r="AK143" t="inlineStr"/>
+      <c r="AL143" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="AM143" t="inlineStr">
+        <is>
+          <t>1557</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-06-08 11:30:58
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AM143"/>
+  <dimension ref="A1:AO148"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -586,6 +586,16 @@
           <t>06-02_0</t>
         </is>
       </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>06-07_A</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>06-07_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -708,9 +718,15 @@
       <c r="AL2" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="AM2" t="inlineStr">
-        <is>
-          <t>5055</t>
+      <c r="AM2" t="n">
+        <v>5055</v>
+      </c>
+      <c r="AN2" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="AO2" t="inlineStr">
+        <is>
+          <t>3478</t>
         </is>
       </c>
     </row>
@@ -835,7 +851,13 @@
       <c r="AL3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM3" t="inlineStr">
+      <c r="AM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -962,9 +984,15 @@
       <c r="AL4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM4" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="AM4" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AN4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO4" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1089,9 +1117,15 @@
       <c r="AL5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM5" t="inlineStr">
-        <is>
-          <t>2834</t>
+      <c r="AM5" t="n">
+        <v>2834</v>
+      </c>
+      <c r="AN5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO5" t="inlineStr">
+        <is>
+          <t>2640</t>
         </is>
       </c>
     </row>
@@ -1216,7 +1250,13 @@
       <c r="AL6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM6" t="inlineStr">
+      <c r="AM6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1274,6 +1314,8 @@
       <c r="AK7" t="inlineStr"/>
       <c r="AL7" s="4" t="inlineStr"/>
       <c r="AM7" t="inlineStr"/>
+      <c r="AN7" s="4" t="inlineStr"/>
+      <c r="AO7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1327,6 +1369,8 @@
       <c r="AK8" t="inlineStr"/>
       <c r="AL8" s="4" t="inlineStr"/>
       <c r="AM8" t="inlineStr"/>
+      <c r="AN8" s="4" t="inlineStr"/>
+      <c r="AO8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1380,6 +1424,8 @@
       <c r="AK9" t="inlineStr"/>
       <c r="AL9" s="4" t="inlineStr"/>
       <c r="AM9" t="inlineStr"/>
+      <c r="AN9" s="4" t="inlineStr"/>
+      <c r="AO9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1433,6 +1479,8 @@
       <c r="AK10" t="inlineStr"/>
       <c r="AL10" s="4" t="inlineStr"/>
       <c r="AM10" t="inlineStr"/>
+      <c r="AN10" s="4" t="inlineStr"/>
+      <c r="AO10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1486,6 +1534,8 @@
       <c r="AK11" t="inlineStr"/>
       <c r="AL11" s="4" t="inlineStr"/>
       <c r="AM11" t="inlineStr"/>
+      <c r="AN11" s="4" t="inlineStr"/>
+      <c r="AO11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1539,6 +1589,8 @@
       <c r="AK12" t="inlineStr"/>
       <c r="AL12" s="4" t="inlineStr"/>
       <c r="AM12" t="inlineStr"/>
+      <c r="AN12" s="4" t="inlineStr"/>
+      <c r="AO12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1592,6 +1644,8 @@
       <c r="AK13" t="inlineStr"/>
       <c r="AL13" s="4" t="inlineStr"/>
       <c r="AM13" t="inlineStr"/>
+      <c r="AN13" s="4" t="inlineStr"/>
+      <c r="AO13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1645,6 +1699,8 @@
       <c r="AK14" t="inlineStr"/>
       <c r="AL14" s="4" t="inlineStr"/>
       <c r="AM14" t="inlineStr"/>
+      <c r="AN14" s="4" t="inlineStr"/>
+      <c r="AO14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1698,6 +1754,8 @@
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" s="4" t="inlineStr"/>
       <c r="AM15" t="inlineStr"/>
+      <c r="AN15" s="4" t="inlineStr"/>
+      <c r="AO15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1751,6 +1809,8 @@
       <c r="AK16" t="inlineStr"/>
       <c r="AL16" s="4" t="inlineStr"/>
       <c r="AM16" t="inlineStr"/>
+      <c r="AN16" s="4" t="inlineStr"/>
+      <c r="AO16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1804,6 +1864,8 @@
       <c r="AK17" t="inlineStr"/>
       <c r="AL17" s="4" t="inlineStr"/>
       <c r="AM17" t="inlineStr"/>
+      <c r="AN17" s="4" t="inlineStr"/>
+      <c r="AO17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1926,9 +1988,15 @@
       <c r="AL18" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="AM18" t="inlineStr">
-        <is>
-          <t>4112</t>
+      <c r="AM18" t="n">
+        <v>4112</v>
+      </c>
+      <c r="AN18" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO18" t="inlineStr">
+        <is>
+          <t>3348</t>
         </is>
       </c>
     </row>
@@ -2053,9 +2121,15 @@
       <c r="AL19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM19" t="inlineStr">
-        <is>
-          <t>2857</t>
+      <c r="AM19" t="n">
+        <v>2857</v>
+      </c>
+      <c r="AN19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO19" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2180,9 +2254,15 @@
       <c r="AL20" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AM20" t="inlineStr">
-        <is>
-          <t>4601</t>
+      <c r="AM20" t="n">
+        <v>4601</v>
+      </c>
+      <c r="AN20" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO20" t="inlineStr">
+        <is>
+          <t>3440</t>
         </is>
       </c>
     </row>
@@ -2307,9 +2387,15 @@
       <c r="AL21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM21" t="inlineStr">
-        <is>
-          <t>3002</t>
+      <c r="AM21" t="n">
+        <v>3002</v>
+      </c>
+      <c r="AN21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO21" t="inlineStr">
+        <is>
+          <t>2928</t>
         </is>
       </c>
     </row>
@@ -2434,9 +2520,15 @@
       <c r="AL22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AM22" t="inlineStr">
-        <is>
-          <t>5405</t>
+      <c r="AM22" t="n">
+        <v>5405</v>
+      </c>
+      <c r="AN22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO22" t="inlineStr">
+        <is>
+          <t>3782</t>
         </is>
       </c>
     </row>
@@ -2561,9 +2653,15 @@
       <c r="AL23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AM23" t="inlineStr">
-        <is>
-          <t>6176</t>
+      <c r="AM23" t="n">
+        <v>6176</v>
+      </c>
+      <c r="AN23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO23" t="inlineStr">
+        <is>
+          <t>3950</t>
         </is>
       </c>
     </row>
@@ -2688,9 +2786,15 @@
       <c r="AL24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AM24" t="inlineStr">
-        <is>
-          <t>5423</t>
+      <c r="AM24" t="n">
+        <v>5423</v>
+      </c>
+      <c r="AN24" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AO24" t="inlineStr">
+        <is>
+          <t>3969</t>
         </is>
       </c>
     </row>
@@ -2810,6 +2914,8 @@
       <c r="AK25" t="inlineStr"/>
       <c r="AL25" s="4" t="inlineStr"/>
       <c r="AM25" t="inlineStr"/>
+      <c r="AN25" s="4" t="inlineStr"/>
+      <c r="AO25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2915,6 +3021,8 @@
       <c r="AK26" t="inlineStr"/>
       <c r="AL26" s="4" t="inlineStr"/>
       <c r="AM26" t="inlineStr"/>
+      <c r="AN26" s="4" t="inlineStr"/>
+      <c r="AO26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -3037,9 +3145,15 @@
       <c r="AL27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM27" t="inlineStr">
-        <is>
-          <t>2516</t>
+      <c r="AM27" t="n">
+        <v>2516</v>
+      </c>
+      <c r="AN27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO27" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3095,6 +3209,8 @@
       <c r="AK28" t="inlineStr"/>
       <c r="AL28" s="4" t="inlineStr"/>
       <c r="AM28" t="inlineStr"/>
+      <c r="AN28" s="4" t="inlineStr"/>
+      <c r="AO28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -3217,9 +3333,15 @@
       <c r="AL29" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="AM29" t="inlineStr">
-        <is>
-          <t>3796</t>
+      <c r="AM29" t="n">
+        <v>3796</v>
+      </c>
+      <c r="AN29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO29" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -3344,9 +3466,15 @@
       <c r="AL30" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="AM30" t="inlineStr">
-        <is>
-          <t>3738</t>
+      <c r="AM30" t="n">
+        <v>3738</v>
+      </c>
+      <c r="AN30" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO30" t="inlineStr">
+        <is>
+          <t>2902</t>
         </is>
       </c>
     </row>
@@ -3471,9 +3599,15 @@
       <c r="AL31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AM31" t="inlineStr">
-        <is>
-          <t>5410</t>
+      <c r="AM31" t="n">
+        <v>5410</v>
+      </c>
+      <c r="AN31" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AO31" t="inlineStr">
+        <is>
+          <t>4032</t>
         </is>
       </c>
     </row>
@@ -3598,9 +3732,15 @@
       <c r="AL32" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AM32" t="inlineStr">
-        <is>
-          <t>4186</t>
+      <c r="AM32" t="n">
+        <v>4186</v>
+      </c>
+      <c r="AN32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO32" t="inlineStr">
+        <is>
+          <t>2551</t>
         </is>
       </c>
     </row>
@@ -3656,6 +3796,8 @@
       <c r="AK33" t="inlineStr"/>
       <c r="AL33" s="4" t="inlineStr"/>
       <c r="AM33" t="inlineStr"/>
+      <c r="AN33" s="4" t="inlineStr"/>
+      <c r="AO33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3778,9 +3920,15 @@
       <c r="AL34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM34" t="inlineStr">
-        <is>
-          <t>2625</t>
+      <c r="AM34" t="n">
+        <v>2625</v>
+      </c>
+      <c r="AN34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO34" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -3905,9 +4053,15 @@
       <c r="AL35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM35" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="AM35" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AN35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO35" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -4032,9 +4186,15 @@
       <c r="AL36" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AM36" t="inlineStr">
-        <is>
-          <t>4418</t>
+      <c r="AM36" t="n">
+        <v>4418</v>
+      </c>
+      <c r="AN36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO36" t="inlineStr">
+        <is>
+          <t>2704</t>
         </is>
       </c>
     </row>
@@ -4159,11 +4319,11 @@
       <c r="AL37" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AM37" t="inlineStr">
-        <is>
-          <t>5098</t>
-        </is>
-      </c>
+      <c r="AM37" t="n">
+        <v>5098</v>
+      </c>
+      <c r="AN37" s="4" t="inlineStr"/>
+      <c r="AO37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -4286,9 +4446,15 @@
       <c r="AL38" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AM38" t="inlineStr">
-        <is>
-          <t>5979</t>
+      <c r="AM38" t="n">
+        <v>5979</v>
+      </c>
+      <c r="AN38" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO38" t="inlineStr">
+        <is>
+          <t>3853</t>
         </is>
       </c>
     </row>
@@ -4413,9 +4579,15 @@
       <c r="AL39" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="AM39" t="inlineStr">
-        <is>
-          <t>4841</t>
+      <c r="AM39" t="n">
+        <v>4841</v>
+      </c>
+      <c r="AN39" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AO39" t="inlineStr">
+        <is>
+          <t>3756</t>
         </is>
       </c>
     </row>
@@ -4540,7 +4712,13 @@
       <c r="AL40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM40" t="inlineStr">
+      <c r="AM40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4667,9 +4845,15 @@
       <c r="AL41" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="AM41" t="inlineStr">
-        <is>
-          <t>4608</t>
+      <c r="AM41" t="n">
+        <v>4608</v>
+      </c>
+      <c r="AN41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO41" t="inlineStr">
+        <is>
+          <t>3517</t>
         </is>
       </c>
     </row>
@@ -4794,9 +4978,15 @@
       <c r="AL42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM42" t="inlineStr">
-        <is>
-          <t>3146</t>
+      <c r="AM42" t="n">
+        <v>3146</v>
+      </c>
+      <c r="AN42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO42" t="inlineStr">
+        <is>
+          <t>2725</t>
         </is>
       </c>
     </row>
@@ -4852,6 +5042,8 @@
       <c r="AK43" t="inlineStr"/>
       <c r="AL43" s="4" t="inlineStr"/>
       <c r="AM43" t="inlineStr"/>
+      <c r="AN43" s="4" t="inlineStr"/>
+      <c r="AO43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -4905,6 +5097,8 @@
       <c r="AK44" t="inlineStr"/>
       <c r="AL44" s="4" t="inlineStr"/>
       <c r="AM44" t="inlineStr"/>
+      <c r="AN44" s="4" t="inlineStr"/>
+      <c r="AO44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -4990,6 +5184,8 @@
       <c r="AK45" t="inlineStr"/>
       <c r="AL45" s="4" t="inlineStr"/>
       <c r="AM45" t="inlineStr"/>
+      <c r="AN45" s="4" t="inlineStr"/>
+      <c r="AO45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -4997,7 +5193,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>larios</t>
+          <t>senjie90</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -5112,9 +5308,15 @@
       <c r="AL46" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="AM46" t="inlineStr">
-        <is>
-          <t>4566</t>
+      <c r="AM46" t="n">
+        <v>4566</v>
+      </c>
+      <c r="AN46" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AO46" t="inlineStr">
+        <is>
+          <t>3582</t>
         </is>
       </c>
     </row>
@@ -5239,9 +5441,15 @@
       <c r="AL47" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AM47" t="inlineStr">
-        <is>
-          <t>6058</t>
+      <c r="AM47" t="n">
+        <v>6058</v>
+      </c>
+      <c r="AN47" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO47" t="inlineStr">
+        <is>
+          <t>4298</t>
         </is>
       </c>
     </row>
@@ -5366,7 +5574,13 @@
       <c r="AL48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM48" t="inlineStr">
+      <c r="AM48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5493,9 +5707,15 @@
       <c r="AL49" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="AM49" t="inlineStr">
-        <is>
-          <t>5240</t>
+      <c r="AM49" t="n">
+        <v>5240</v>
+      </c>
+      <c r="AN49" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AO49" t="inlineStr">
+        <is>
+          <t>4007</t>
         </is>
       </c>
     </row>
@@ -5620,9 +5840,15 @@
       <c r="AL50" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="AM50" t="inlineStr">
-        <is>
-          <t>5529</t>
+      <c r="AM50" t="n">
+        <v>5529</v>
+      </c>
+      <c r="AN50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO50" t="inlineStr">
+        <is>
+          <t>3996</t>
         </is>
       </c>
     </row>
@@ -5710,6 +5936,8 @@
       <c r="AK51" t="inlineStr"/>
       <c r="AL51" s="4" t="inlineStr"/>
       <c r="AM51" t="inlineStr"/>
+      <c r="AN51" s="4" t="inlineStr"/>
+      <c r="AO51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -5832,9 +6060,15 @@
       <c r="AL52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AM52" t="inlineStr">
-        <is>
-          <t>5551</t>
+      <c r="AM52" t="n">
+        <v>5551</v>
+      </c>
+      <c r="AN52" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="AO52" t="inlineStr">
+        <is>
+          <t>3985</t>
         </is>
       </c>
     </row>
@@ -5959,9 +6193,15 @@
       <c r="AL53" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="AM53" t="inlineStr">
-        <is>
-          <t>4525</t>
+      <c r="AM53" t="n">
+        <v>4525</v>
+      </c>
+      <c r="AN53" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AO53" t="inlineStr">
+        <is>
+          <t>2963</t>
         </is>
       </c>
     </row>
@@ -6049,6 +6289,8 @@
       <c r="AK54" t="inlineStr"/>
       <c r="AL54" s="4" t="inlineStr"/>
       <c r="AM54" t="inlineStr"/>
+      <c r="AN54" s="4" t="inlineStr"/>
+      <c r="AO54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -6171,9 +6413,15 @@
       <c r="AL55" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AM55" t="inlineStr">
-        <is>
-          <t>4807</t>
+      <c r="AM55" t="n">
+        <v>4807</v>
+      </c>
+      <c r="AN55" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AO55" t="inlineStr">
+        <is>
+          <t>2938</t>
         </is>
       </c>
     </row>
@@ -6298,9 +6546,15 @@
       <c r="AL56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AM56" t="inlineStr">
-        <is>
-          <t>5868</t>
+      <c r="AM56" t="n">
+        <v>5868</v>
+      </c>
+      <c r="AN56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO56" t="inlineStr">
+        <is>
+          <t>4172</t>
         </is>
       </c>
     </row>
@@ -6425,9 +6679,15 @@
       <c r="AL57" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="AM57" t="inlineStr">
-        <is>
-          <t>4388</t>
+      <c r="AM57" t="n">
+        <v>4388</v>
+      </c>
+      <c r="AN57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO57" t="inlineStr">
+        <is>
+          <t>3420</t>
         </is>
       </c>
     </row>
@@ -6552,9 +6812,15 @@
       <c r="AL58" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AM58" t="inlineStr">
-        <is>
-          <t>4713</t>
+      <c r="AM58" t="n">
+        <v>4713</v>
+      </c>
+      <c r="AN58" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AO58" t="inlineStr">
+        <is>
+          <t>3560</t>
         </is>
       </c>
     </row>
@@ -6679,9 +6945,15 @@
       <c r="AL59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AM59" t="inlineStr">
-        <is>
-          <t>4356</t>
+      <c r="AM59" t="n">
+        <v>4356</v>
+      </c>
+      <c r="AN59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO59" t="inlineStr">
+        <is>
+          <t>3391</t>
         </is>
       </c>
     </row>
@@ -6806,9 +7078,15 @@
       <c r="AL60" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AM60" t="inlineStr">
-        <is>
-          <t>4666</t>
+      <c r="AM60" t="n">
+        <v>4666</v>
+      </c>
+      <c r="AN60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AO60" t="inlineStr">
+        <is>
+          <t>3876</t>
         </is>
       </c>
     </row>
@@ -6864,6 +7142,8 @@
       <c r="AK61" t="inlineStr"/>
       <c r="AL61" s="4" t="inlineStr"/>
       <c r="AM61" t="inlineStr"/>
+      <c r="AN61" s="4" t="inlineStr"/>
+      <c r="AO61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -6986,9 +7266,15 @@
       <c r="AL62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AM62" t="inlineStr">
-        <is>
-          <t>4213</t>
+      <c r="AM62" t="n">
+        <v>4213</v>
+      </c>
+      <c r="AN62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO62" t="inlineStr">
+        <is>
+          <t>3262</t>
         </is>
       </c>
     </row>
@@ -7113,9 +7399,15 @@
       <c r="AL63" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="AM63" t="inlineStr">
-        <is>
-          <t>4119</t>
+      <c r="AM63" t="n">
+        <v>4119</v>
+      </c>
+      <c r="AN63" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO63" t="inlineStr">
+        <is>
+          <t>3255</t>
         </is>
       </c>
     </row>
@@ -7240,9 +7532,15 @@
       <c r="AL64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AM64" t="inlineStr">
-        <is>
-          <t>4550</t>
+      <c r="AM64" t="n">
+        <v>4550</v>
+      </c>
+      <c r="AN64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO64" t="inlineStr">
+        <is>
+          <t>3634</t>
         </is>
       </c>
     </row>
@@ -7350,6 +7648,8 @@
       <c r="AK65" t="inlineStr"/>
       <c r="AL65" s="4" t="inlineStr"/>
       <c r="AM65" t="inlineStr"/>
+      <c r="AN65" s="4" t="inlineStr"/>
+      <c r="AO65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -7472,7 +7772,13 @@
       <c r="AL66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM66" t="inlineStr">
+      <c r="AM66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7599,7 +7905,13 @@
       <c r="AL67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM67" t="inlineStr">
+      <c r="AM67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7726,7 +8038,13 @@
       <c r="AL68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM68" t="inlineStr">
+      <c r="AM68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7784,6 +8102,8 @@
       <c r="AK69" t="inlineStr"/>
       <c r="AL69" s="4" t="inlineStr"/>
       <c r="AM69" t="inlineStr"/>
+      <c r="AN69" s="4" t="inlineStr"/>
+      <c r="AO69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -7906,7 +8226,13 @@
       <c r="AL70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM70" t="inlineStr">
+      <c r="AM70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8033,7 +8359,13 @@
       <c r="AL71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM71" t="inlineStr">
+      <c r="AM71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8160,7 +8492,13 @@
       <c r="AL72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM72" t="inlineStr">
+      <c r="AM72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8287,9 +8625,15 @@
       <c r="AL73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM73" t="inlineStr">
-        <is>
-          <t>2986</t>
+      <c r="AM73" t="n">
+        <v>2986</v>
+      </c>
+      <c r="AN73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO73" t="inlineStr">
+        <is>
+          <t>2641</t>
         </is>
       </c>
     </row>
@@ -8414,7 +8758,13 @@
       <c r="AL74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM74" t="inlineStr">
+      <c r="AM74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8541,7 +8891,13 @@
       <c r="AL75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM75" t="inlineStr">
+      <c r="AM75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8668,9 +9024,15 @@
       <c r="AL76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM76" t="inlineStr">
-        <is>
-          <t>3598</t>
+      <c r="AM76" t="n">
+        <v>3598</v>
+      </c>
+      <c r="AN76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO76" t="inlineStr">
+        <is>
+          <t>2499</t>
         </is>
       </c>
     </row>
@@ -8795,9 +9157,15 @@
       <c r="AL77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM77" t="inlineStr">
-        <is>
-          <t>2803</t>
+      <c r="AM77" t="n">
+        <v>2803</v>
+      </c>
+      <c r="AN77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO77" t="inlineStr">
+        <is>
+          <t>2583</t>
         </is>
       </c>
     </row>
@@ -8922,7 +9290,13 @@
       <c r="AL78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM78" t="inlineStr">
+      <c r="AM78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9049,7 +9423,13 @@
       <c r="AL79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM79" t="inlineStr">
+      <c r="AM79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9176,7 +9556,13 @@
       <c r="AL80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM80" t="inlineStr">
+      <c r="AM80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9303,7 +9689,13 @@
       <c r="AL81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM81" t="inlineStr">
+      <c r="AM81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9430,7 +9822,13 @@
       <c r="AL82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM82" t="inlineStr">
+      <c r="AM82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9557,7 +9955,13 @@
       <c r="AL83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM83" t="inlineStr">
+      <c r="AM83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9684,7 +10088,13 @@
       <c r="AL84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM84" t="inlineStr">
+      <c r="AM84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9811,7 +10221,13 @@
       <c r="AL85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM85" t="inlineStr">
+      <c r="AM85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9938,9 +10354,15 @@
       <c r="AL86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM86" t="inlineStr">
-        <is>
-          <t>1084</t>
+      <c r="AM86" t="n">
+        <v>1084</v>
+      </c>
+      <c r="AN86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO86" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -10065,7 +10487,13 @@
       <c r="AL87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM87" t="inlineStr">
+      <c r="AM87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10192,7 +10620,13 @@
       <c r="AL88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM88" t="inlineStr">
+      <c r="AM88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10319,7 +10753,13 @@
       <c r="AL89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM89" t="inlineStr">
+      <c r="AM89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10446,7 +10886,13 @@
       <c r="AL90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM90" t="inlineStr">
+      <c r="AM90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10573,7 +11019,13 @@
       <c r="AL91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM91" t="inlineStr">
+      <c r="AM91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10700,7 +11152,13 @@
       <c r="AL92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM92" t="inlineStr">
+      <c r="AM92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10827,7 +11285,13 @@
       <c r="AL93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM93" t="inlineStr">
+      <c r="AM93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10954,7 +11418,13 @@
       <c r="AL94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM94" t="inlineStr">
+      <c r="AM94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11081,7 +11551,13 @@
       <c r="AL95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM95" t="inlineStr">
+      <c r="AM95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11208,9 +11684,15 @@
       <c r="AL96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM96" t="inlineStr">
-        <is>
-          <t>2487</t>
+      <c r="AM96" t="n">
+        <v>2487</v>
+      </c>
+      <c r="AN96" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AO96" t="inlineStr">
+        <is>
+          <t>2480</t>
         </is>
       </c>
     </row>
@@ -11335,7 +11817,13 @@
       <c r="AL97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM97" t="inlineStr">
+      <c r="AM97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11462,7 +11950,13 @@
       <c r="AL98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM98" t="inlineStr">
+      <c r="AM98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11589,7 +12083,13 @@
       <c r="AL99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM99" t="inlineStr">
+      <c r="AM99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11716,7 +12216,13 @@
       <c r="AL100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM100" t="inlineStr">
+      <c r="AM100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11843,7 +12349,13 @@
       <c r="AL101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM101" t="inlineStr">
+      <c r="AM101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11970,7 +12482,13 @@
       <c r="AL102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM102" t="inlineStr">
+      <c r="AM102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12097,7 +12615,13 @@
       <c r="AL103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM103" t="inlineStr">
+      <c r="AM103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12224,7 +12748,13 @@
       <c r="AL104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM104" t="inlineStr">
+      <c r="AM104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12351,7 +12881,13 @@
       <c r="AL105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM105" t="inlineStr">
+      <c r="AM105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12409,6 +12945,8 @@
       <c r="AK106" t="inlineStr"/>
       <c r="AL106" s="4" t="inlineStr"/>
       <c r="AM106" t="inlineStr"/>
+      <c r="AN106" s="4" t="inlineStr"/>
+      <c r="AO106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -12462,6 +13000,8 @@
       <c r="AK107" t="inlineStr"/>
       <c r="AL107" s="4" t="inlineStr"/>
       <c r="AM107" t="inlineStr"/>
+      <c r="AN107" s="4" t="inlineStr"/>
+      <c r="AO107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -12515,6 +13055,8 @@
       <c r="AK108" t="inlineStr"/>
       <c r="AL108" s="4" t="inlineStr"/>
       <c r="AM108" t="inlineStr"/>
+      <c r="AN108" s="4" t="inlineStr"/>
+      <c r="AO108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -12568,6 +13110,8 @@
       <c r="AK109" t="inlineStr"/>
       <c r="AL109" s="4" t="inlineStr"/>
       <c r="AM109" t="inlineStr"/>
+      <c r="AN109" s="4" t="inlineStr"/>
+      <c r="AO109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -12621,6 +13165,8 @@
       <c r="AK110" t="inlineStr"/>
       <c r="AL110" s="4" t="inlineStr"/>
       <c r="AM110" t="inlineStr"/>
+      <c r="AN110" s="4" t="inlineStr"/>
+      <c r="AO110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -12674,6 +13220,8 @@
       <c r="AK111" t="inlineStr"/>
       <c r="AL111" s="4" t="inlineStr"/>
       <c r="AM111" t="inlineStr"/>
+      <c r="AN111" s="4" t="inlineStr"/>
+      <c r="AO111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -12727,6 +13275,8 @@
       <c r="AK112" t="inlineStr"/>
       <c r="AL112" s="4" t="inlineStr"/>
       <c r="AM112" t="inlineStr"/>
+      <c r="AN112" s="4" t="inlineStr"/>
+      <c r="AO112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -12780,6 +13330,8 @@
       <c r="AK113" t="inlineStr"/>
       <c r="AL113" s="4" t="inlineStr"/>
       <c r="AM113" t="inlineStr"/>
+      <c r="AN113" s="4" t="inlineStr"/>
+      <c r="AO113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -12833,6 +13385,8 @@
       <c r="AK114" t="inlineStr"/>
       <c r="AL114" s="4" t="inlineStr"/>
       <c r="AM114" t="inlineStr"/>
+      <c r="AN114" s="4" t="inlineStr"/>
+      <c r="AO114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -12933,9 +13487,15 @@
       <c r="AL115" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AM115" t="inlineStr">
-        <is>
-          <t>6032</t>
+      <c r="AM115" t="n">
+        <v>6032</v>
+      </c>
+      <c r="AN115" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO115" t="inlineStr">
+        <is>
+          <t>3753</t>
         </is>
       </c>
     </row>
@@ -13054,7 +13614,13 @@
       <c r="AL116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM116" t="inlineStr">
+      <c r="AM116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13066,7 +13632,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>"Zephyr-5ky zgx"</t>
+          <t>Zephyr</t>
         </is>
       </c>
       <c r="C117" t="inlineStr"/>
@@ -13146,6 +13712,14 @@
       <c r="AK117" t="inlineStr"/>
       <c r="AL117" s="4" t="inlineStr"/>
       <c r="AM117" t="inlineStr"/>
+      <c r="AN117" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AO117" t="inlineStr">
+        <is>
+          <t>4718</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -13262,9 +13836,15 @@
       <c r="AL118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM118" t="inlineStr">
-        <is>
-          <t>3334</t>
+      <c r="AM118" t="n">
+        <v>3334</v>
+      </c>
+      <c r="AN118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO118" t="inlineStr">
+        <is>
+          <t>2749</t>
         </is>
       </c>
     </row>
@@ -13383,9 +13963,15 @@
       <c r="AL119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM119" t="inlineStr">
-        <is>
-          <t>1586</t>
+      <c r="AM119" t="n">
+        <v>1586</v>
+      </c>
+      <c r="AN119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO119" t="inlineStr">
+        <is>
+          <t>1498</t>
         </is>
       </c>
     </row>
@@ -13504,7 +14090,13 @@
       <c r="AL120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM120" t="inlineStr">
+      <c r="AM120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO120" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13625,7 +14217,13 @@
       <c r="AL121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM121" t="inlineStr">
+      <c r="AM121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13746,7 +14344,13 @@
       <c r="AL122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM122" t="inlineStr">
+      <c r="AM122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13863,9 +14467,15 @@
       <c r="AL123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM123" t="inlineStr">
-        <is>
-          <t>2680</t>
+      <c r="AM123" t="n">
+        <v>2680</v>
+      </c>
+      <c r="AN123" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO123" t="inlineStr">
+        <is>
+          <t>2580</t>
         </is>
       </c>
     </row>
@@ -13947,6 +14557,8 @@
       <c r="AK124" t="inlineStr"/>
       <c r="AL124" s="4" t="inlineStr"/>
       <c r="AM124" t="inlineStr"/>
+      <c r="AN124" s="4" t="inlineStr"/>
+      <c r="AO124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -14055,9 +14667,15 @@
       <c r="AL125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM125" t="inlineStr">
-        <is>
-          <t>2277</t>
+      <c r="AM125" t="n">
+        <v>2277</v>
+      </c>
+      <c r="AN125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO125" t="inlineStr">
+        <is>
+          <t>2113</t>
         </is>
       </c>
     </row>
@@ -14156,9 +14774,15 @@
       <c r="AL126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM126" t="inlineStr">
-        <is>
-          <t>1553</t>
+      <c r="AM126" t="n">
+        <v>1553</v>
+      </c>
+      <c r="AN126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO126" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -14232,6 +14856,8 @@
       <c r="AK127" t="inlineStr"/>
       <c r="AL127" s="4" t="inlineStr"/>
       <c r="AM127" t="inlineStr"/>
+      <c r="AN127" s="4" t="inlineStr"/>
+      <c r="AO127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -14315,6 +14941,8 @@
       <c r="AK128" t="inlineStr"/>
       <c r="AL128" s="4" t="inlineStr"/>
       <c r="AM128" t="inlineStr"/>
+      <c r="AN128" s="4" t="inlineStr"/>
+      <c r="AO128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -14403,9 +15031,15 @@
       <c r="AL129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM129" t="inlineStr">
-        <is>
-          <t>3567</t>
+      <c r="AM129" t="n">
+        <v>3567</v>
+      </c>
+      <c r="AN129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO129" t="inlineStr">
+        <is>
+          <t>2500</t>
         </is>
       </c>
     </row>
@@ -14491,6 +15125,8 @@
       <c r="AK130" t="inlineStr"/>
       <c r="AL130" s="4" t="inlineStr"/>
       <c r="AM130" t="inlineStr"/>
+      <c r="AN130" s="4" t="inlineStr"/>
+      <c r="AO130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -14575,9 +15211,15 @@
       <c r="AL131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM131" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="AM131" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AN131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO131" t="inlineStr">
+        <is>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -14652,9 +15294,15 @@
       <c r="AL132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM132" t="inlineStr">
-        <is>
-          <t>4250</t>
+      <c r="AM132" t="n">
+        <v>4250</v>
+      </c>
+      <c r="AN132" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO132" t="inlineStr">
+        <is>
+          <t>3511</t>
         </is>
       </c>
     </row>
@@ -14729,9 +15377,15 @@
       <c r="AL133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AM133" t="inlineStr">
-        <is>
-          <t>3241</t>
+      <c r="AM133" t="n">
+        <v>3241</v>
+      </c>
+      <c r="AN133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO133" t="inlineStr">
+        <is>
+          <t>2484</t>
         </is>
       </c>
     </row>
@@ -14789,6 +15443,8 @@
       <c r="AK134" t="inlineStr"/>
       <c r="AL134" s="4" t="inlineStr"/>
       <c r="AM134" t="inlineStr"/>
+      <c r="AN134" s="4" t="inlineStr"/>
+      <c r="AO134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -14848,6 +15504,8 @@
       <c r="AK135" t="inlineStr"/>
       <c r="AL135" s="4" t="inlineStr"/>
       <c r="AM135" t="inlineStr"/>
+      <c r="AN135" s="4" t="inlineStr"/>
+      <c r="AO135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -14907,6 +15565,14 @@
       <c r="AK136" t="inlineStr"/>
       <c r="AL136" s="4" t="inlineStr"/>
       <c r="AM136" t="inlineStr"/>
+      <c r="AN136" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AO136" t="inlineStr">
+        <is>
+          <t>4390</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -14966,6 +15632,14 @@
       <c r="AK137" t="inlineStr"/>
       <c r="AL137" s="4" t="inlineStr"/>
       <c r="AM137" t="inlineStr"/>
+      <c r="AN137" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AO137" t="inlineStr">
+        <is>
+          <t>4256</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -15025,6 +15699,8 @@
       <c r="AK138" t="inlineStr"/>
       <c r="AL138" s="4" t="inlineStr"/>
       <c r="AM138" t="inlineStr"/>
+      <c r="AN138" s="4" t="inlineStr"/>
+      <c r="AO138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -15084,6 +15760,14 @@
       <c r="AK139" t="inlineStr"/>
       <c r="AL139" s="4" t="inlineStr"/>
       <c r="AM139" t="inlineStr"/>
+      <c r="AN139" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="AO139" t="inlineStr">
+        <is>
+          <t>4378</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -15140,9 +15824,15 @@
       <c r="AL140" s="3" t="n">
         <v>18</v>
       </c>
-      <c r="AM140" t="inlineStr">
-        <is>
-          <t>2232</t>
+      <c r="AM140" t="n">
+        <v>2232</v>
+      </c>
+      <c r="AN140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO140" t="inlineStr">
+        <is>
+          <t>1995</t>
         </is>
       </c>
     </row>
@@ -15200,12 +15890,12 @@
       </c>
       <c r="AL141" s="4" t="inlineStr"/>
       <c r="AM141" t="inlineStr"/>
+      <c r="AN141" s="4" t="inlineStr"/>
+      <c r="AO141" t="inlineStr"/>
     </row>
     <row r="142">
-      <c r="A142" t="inlineStr">
-        <is>
-          <t>59127877</t>
-        </is>
+      <c r="A142" t="n">
+        <v>59127877</v>
       </c>
       <c r="B142" t="inlineStr">
         <is>
@@ -15254,17 +15944,21 @@
       <c r="AL142" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AM142" t="inlineStr">
-        <is>
-          <t>2648</t>
+      <c r="AM142" t="n">
+        <v>2648</v>
+      </c>
+      <c r="AN142" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO142" t="inlineStr">
+        <is>
+          <t>2765</t>
         </is>
       </c>
     </row>
     <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>59482456</t>
-        </is>
+      <c r="A143" t="n">
+        <v>59482456</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
@@ -15313,9 +16007,320 @@
       <c r="AL143" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="AM143" t="inlineStr">
-        <is>
-          <t>1557</t>
+      <c r="AM143" t="n">
+        <v>1557</v>
+      </c>
+      <c r="AN143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO143" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>37111401</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>noaekt</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr"/>
+      <c r="D144" t="inlineStr"/>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F144" s="4" t="inlineStr"/>
+      <c r="G144" t="inlineStr"/>
+      <c r="H144" s="4" t="inlineStr"/>
+      <c r="I144" t="inlineStr"/>
+      <c r="J144" s="4" t="inlineStr"/>
+      <c r="K144" t="inlineStr"/>
+      <c r="L144" s="4" t="inlineStr"/>
+      <c r="M144" t="inlineStr"/>
+      <c r="N144" s="4" t="inlineStr"/>
+      <c r="O144" t="inlineStr"/>
+      <c r="P144" s="4" t="inlineStr"/>
+      <c r="Q144" t="inlineStr"/>
+      <c r="R144" s="4" t="inlineStr"/>
+      <c r="S144" t="inlineStr"/>
+      <c r="T144" s="4" t="inlineStr"/>
+      <c r="U144" t="inlineStr"/>
+      <c r="V144" s="4" t="inlineStr"/>
+      <c r="W144" t="inlineStr"/>
+      <c r="X144" s="4" t="inlineStr"/>
+      <c r="Y144" t="inlineStr"/>
+      <c r="Z144" s="4" t="inlineStr"/>
+      <c r="AA144" t="inlineStr"/>
+      <c r="AB144" s="4" t="inlineStr"/>
+      <c r="AC144" t="inlineStr"/>
+      <c r="AD144" s="4" t="inlineStr"/>
+      <c r="AE144" t="inlineStr"/>
+      <c r="AF144" s="4" t="inlineStr"/>
+      <c r="AG144" t="inlineStr"/>
+      <c r="AH144" s="4" t="inlineStr"/>
+      <c r="AI144" t="inlineStr"/>
+      <c r="AJ144" s="4" t="inlineStr"/>
+      <c r="AK144" t="inlineStr"/>
+      <c r="AL144" s="4" t="inlineStr"/>
+      <c r="AM144" t="inlineStr"/>
+      <c r="AN144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO144" t="inlineStr">
+        <is>
+          <t>1511</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>56300923</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>"El matador"</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr"/>
+      <c r="D145" t="inlineStr"/>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F145" s="4" t="inlineStr"/>
+      <c r="G145" t="inlineStr"/>
+      <c r="H145" s="4" t="inlineStr"/>
+      <c r="I145" t="inlineStr"/>
+      <c r="J145" s="4" t="inlineStr"/>
+      <c r="K145" t="inlineStr"/>
+      <c r="L145" s="4" t="inlineStr"/>
+      <c r="M145" t="inlineStr"/>
+      <c r="N145" s="4" t="inlineStr"/>
+      <c r="O145" t="inlineStr"/>
+      <c r="P145" s="4" t="inlineStr"/>
+      <c r="Q145" t="inlineStr"/>
+      <c r="R145" s="4" t="inlineStr"/>
+      <c r="S145" t="inlineStr"/>
+      <c r="T145" s="4" t="inlineStr"/>
+      <c r="U145" t="inlineStr"/>
+      <c r="V145" s="4" t="inlineStr"/>
+      <c r="W145" t="inlineStr"/>
+      <c r="X145" s="4" t="inlineStr"/>
+      <c r="Y145" t="inlineStr"/>
+      <c r="Z145" s="4" t="inlineStr"/>
+      <c r="AA145" t="inlineStr"/>
+      <c r="AB145" s="4" t="inlineStr"/>
+      <c r="AC145" t="inlineStr"/>
+      <c r="AD145" s="4" t="inlineStr"/>
+      <c r="AE145" t="inlineStr"/>
+      <c r="AF145" s="4" t="inlineStr"/>
+      <c r="AG145" t="inlineStr"/>
+      <c r="AH145" s="4" t="inlineStr"/>
+      <c r="AI145" t="inlineStr"/>
+      <c r="AJ145" s="4" t="inlineStr"/>
+      <c r="AK145" t="inlineStr"/>
+      <c r="AL145" s="4" t="inlineStr"/>
+      <c r="AM145" t="inlineStr"/>
+      <c r="AN145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO145" t="inlineStr">
+        <is>
+          <t>1785</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>59242379</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Player-59242379</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr"/>
+      <c r="D146" t="inlineStr"/>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F146" s="4" t="inlineStr"/>
+      <c r="G146" t="inlineStr"/>
+      <c r="H146" s="4" t="inlineStr"/>
+      <c r="I146" t="inlineStr"/>
+      <c r="J146" s="4" t="inlineStr"/>
+      <c r="K146" t="inlineStr"/>
+      <c r="L146" s="4" t="inlineStr"/>
+      <c r="M146" t="inlineStr"/>
+      <c r="N146" s="4" t="inlineStr"/>
+      <c r="O146" t="inlineStr"/>
+      <c r="P146" s="4" t="inlineStr"/>
+      <c r="Q146" t="inlineStr"/>
+      <c r="R146" s="4" t="inlineStr"/>
+      <c r="S146" t="inlineStr"/>
+      <c r="T146" s="4" t="inlineStr"/>
+      <c r="U146" t="inlineStr"/>
+      <c r="V146" s="4" t="inlineStr"/>
+      <c r="W146" t="inlineStr"/>
+      <c r="X146" s="4" t="inlineStr"/>
+      <c r="Y146" t="inlineStr"/>
+      <c r="Z146" s="4" t="inlineStr"/>
+      <c r="AA146" t="inlineStr"/>
+      <c r="AB146" s="4" t="inlineStr"/>
+      <c r="AC146" t="inlineStr"/>
+      <c r="AD146" s="4" t="inlineStr"/>
+      <c r="AE146" t="inlineStr"/>
+      <c r="AF146" s="4" t="inlineStr"/>
+      <c r="AG146" t="inlineStr"/>
+      <c r="AH146" s="4" t="inlineStr"/>
+      <c r="AI146" t="inlineStr"/>
+      <c r="AJ146" s="4" t="inlineStr"/>
+      <c r="AK146" t="inlineStr"/>
+      <c r="AL146" s="4" t="inlineStr"/>
+      <c r="AM146" t="inlineStr"/>
+      <c r="AN146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AO146" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>56555218</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>muvee123</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr"/>
+      <c r="D147" t="inlineStr"/>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F147" s="4" t="inlineStr"/>
+      <c r="G147" t="inlineStr"/>
+      <c r="H147" s="4" t="inlineStr"/>
+      <c r="I147" t="inlineStr"/>
+      <c r="J147" s="4" t="inlineStr"/>
+      <c r="K147" t="inlineStr"/>
+      <c r="L147" s="4" t="inlineStr"/>
+      <c r="M147" t="inlineStr"/>
+      <c r="N147" s="4" t="inlineStr"/>
+      <c r="O147" t="inlineStr"/>
+      <c r="P147" s="4" t="inlineStr"/>
+      <c r="Q147" t="inlineStr"/>
+      <c r="R147" s="4" t="inlineStr"/>
+      <c r="S147" t="inlineStr"/>
+      <c r="T147" s="4" t="inlineStr"/>
+      <c r="U147" t="inlineStr"/>
+      <c r="V147" s="4" t="inlineStr"/>
+      <c r="W147" t="inlineStr"/>
+      <c r="X147" s="4" t="inlineStr"/>
+      <c r="Y147" t="inlineStr"/>
+      <c r="Z147" s="4" t="inlineStr"/>
+      <c r="AA147" t="inlineStr"/>
+      <c r="AB147" s="4" t="inlineStr"/>
+      <c r="AC147" t="inlineStr"/>
+      <c r="AD147" s="4" t="inlineStr"/>
+      <c r="AE147" t="inlineStr"/>
+      <c r="AF147" s="4" t="inlineStr"/>
+      <c r="AG147" t="inlineStr"/>
+      <c r="AH147" s="4" t="inlineStr"/>
+      <c r="AI147" t="inlineStr"/>
+      <c r="AJ147" s="4" t="inlineStr"/>
+      <c r="AK147" t="inlineStr"/>
+      <c r="AL147" s="4" t="inlineStr"/>
+      <c r="AM147" t="inlineStr"/>
+      <c r="AN147" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AO147" t="inlineStr">
+        <is>
+          <t>3968</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>59519348</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Player-59519348</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr"/>
+      <c r="D148" t="inlineStr"/>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F148" s="4" t="inlineStr"/>
+      <c r="G148" t="inlineStr"/>
+      <c r="H148" s="4" t="inlineStr"/>
+      <c r="I148" t="inlineStr"/>
+      <c r="J148" s="4" t="inlineStr"/>
+      <c r="K148" t="inlineStr"/>
+      <c r="L148" s="4" t="inlineStr"/>
+      <c r="M148" t="inlineStr"/>
+      <c r="N148" s="4" t="inlineStr"/>
+      <c r="O148" t="inlineStr"/>
+      <c r="P148" s="4" t="inlineStr"/>
+      <c r="Q148" t="inlineStr"/>
+      <c r="R148" s="4" t="inlineStr"/>
+      <c r="S148" t="inlineStr"/>
+      <c r="T148" s="4" t="inlineStr"/>
+      <c r="U148" t="inlineStr"/>
+      <c r="V148" s="4" t="inlineStr"/>
+      <c r="W148" t="inlineStr"/>
+      <c r="X148" s="4" t="inlineStr"/>
+      <c r="Y148" t="inlineStr"/>
+      <c r="Z148" s="4" t="inlineStr"/>
+      <c r="AA148" t="inlineStr"/>
+      <c r="AB148" s="4" t="inlineStr"/>
+      <c r="AC148" t="inlineStr"/>
+      <c r="AD148" s="4" t="inlineStr"/>
+      <c r="AE148" t="inlineStr"/>
+      <c r="AF148" s="4" t="inlineStr"/>
+      <c r="AG148" t="inlineStr"/>
+      <c r="AH148" s="4" t="inlineStr"/>
+      <c r="AI148" t="inlineStr"/>
+      <c r="AJ148" s="4" t="inlineStr"/>
+      <c r="AK148" t="inlineStr"/>
+      <c r="AL148" s="4" t="inlineStr"/>
+      <c r="AM148" t="inlineStr"/>
+      <c r="AN148" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="AO148" t="inlineStr">
+        <is>
+          <t>1632</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-06-09 10:42:00
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AO148"/>
+  <dimension ref="A1:AQ151"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -596,6 +596,16 @@
           <t>06-07_0</t>
         </is>
       </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>06-08_A</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>06-08_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -724,9 +734,15 @@
       <c r="AN2" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="AO2" t="inlineStr">
-        <is>
-          <t>3478</t>
+      <c r="AO2" t="n">
+        <v>3478</v>
+      </c>
+      <c r="AP2" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AQ2" t="inlineStr">
+        <is>
+          <t>3666</t>
         </is>
       </c>
     </row>
@@ -857,7 +873,13 @@
       <c r="AN3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO3" t="inlineStr">
+      <c r="AO3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -990,7 +1012,13 @@
       <c r="AN4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO4" t="inlineStr">
+      <c r="AO4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1123,9 +1151,15 @@
       <c r="AN5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO5" t="inlineStr">
-        <is>
-          <t>2640</t>
+      <c r="AO5" t="n">
+        <v>2640</v>
+      </c>
+      <c r="AP5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ5" t="inlineStr">
+        <is>
+          <t>2688</t>
         </is>
       </c>
     </row>
@@ -1256,7 +1290,13 @@
       <c r="AN6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO6" t="inlineStr">
+      <c r="AO6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1316,6 +1356,8 @@
       <c r="AM7" t="inlineStr"/>
       <c r="AN7" s="4" t="inlineStr"/>
       <c r="AO7" t="inlineStr"/>
+      <c r="AP7" s="4" t="inlineStr"/>
+      <c r="AQ7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1371,6 +1413,8 @@
       <c r="AM8" t="inlineStr"/>
       <c r="AN8" s="4" t="inlineStr"/>
       <c r="AO8" t="inlineStr"/>
+      <c r="AP8" s="4" t="inlineStr"/>
+      <c r="AQ8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1426,6 +1470,8 @@
       <c r="AM9" t="inlineStr"/>
       <c r="AN9" s="4" t="inlineStr"/>
       <c r="AO9" t="inlineStr"/>
+      <c r="AP9" s="4" t="inlineStr"/>
+      <c r="AQ9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1481,6 +1527,8 @@
       <c r="AM10" t="inlineStr"/>
       <c r="AN10" s="4" t="inlineStr"/>
       <c r="AO10" t="inlineStr"/>
+      <c r="AP10" s="4" t="inlineStr"/>
+      <c r="AQ10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1536,6 +1584,8 @@
       <c r="AM11" t="inlineStr"/>
       <c r="AN11" s="4" t="inlineStr"/>
       <c r="AO11" t="inlineStr"/>
+      <c r="AP11" s="4" t="inlineStr"/>
+      <c r="AQ11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1591,6 +1641,8 @@
       <c r="AM12" t="inlineStr"/>
       <c r="AN12" s="4" t="inlineStr"/>
       <c r="AO12" t="inlineStr"/>
+      <c r="AP12" s="4" t="inlineStr"/>
+      <c r="AQ12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1646,6 +1698,8 @@
       <c r="AM13" t="inlineStr"/>
       <c r="AN13" s="4" t="inlineStr"/>
       <c r="AO13" t="inlineStr"/>
+      <c r="AP13" s="4" t="inlineStr"/>
+      <c r="AQ13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1701,6 +1755,8 @@
       <c r="AM14" t="inlineStr"/>
       <c r="AN14" s="4" t="inlineStr"/>
       <c r="AO14" t="inlineStr"/>
+      <c r="AP14" s="4" t="inlineStr"/>
+      <c r="AQ14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1756,6 +1812,8 @@
       <c r="AM15" t="inlineStr"/>
       <c r="AN15" s="4" t="inlineStr"/>
       <c r="AO15" t="inlineStr"/>
+      <c r="AP15" s="4" t="inlineStr"/>
+      <c r="AQ15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1811,6 +1869,8 @@
       <c r="AM16" t="inlineStr"/>
       <c r="AN16" s="4" t="inlineStr"/>
       <c r="AO16" t="inlineStr"/>
+      <c r="AP16" s="4" t="inlineStr"/>
+      <c r="AQ16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1866,6 +1926,8 @@
       <c r="AM17" t="inlineStr"/>
       <c r="AN17" s="4" t="inlineStr"/>
       <c r="AO17" t="inlineStr"/>
+      <c r="AP17" s="4" t="inlineStr"/>
+      <c r="AQ17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1994,9 +2056,15 @@
       <c r="AN18" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AO18" t="inlineStr">
-        <is>
-          <t>3348</t>
+      <c r="AO18" t="n">
+        <v>3348</v>
+      </c>
+      <c r="AP18" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="AQ18" t="inlineStr">
+        <is>
+          <t>3505</t>
         </is>
       </c>
     </row>
@@ -2127,7 +2195,13 @@
       <c r="AN19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO19" t="inlineStr">
+      <c r="AO19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ19" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2260,9 +2334,15 @@
       <c r="AN20" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AO20" t="inlineStr">
-        <is>
-          <t>3440</t>
+      <c r="AO20" t="n">
+        <v>3440</v>
+      </c>
+      <c r="AP20" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AQ20" t="inlineStr">
+        <is>
+          <t>3719</t>
         </is>
       </c>
     </row>
@@ -2393,9 +2473,15 @@
       <c r="AN21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO21" t="inlineStr">
-        <is>
-          <t>2928</t>
+      <c r="AO21" t="n">
+        <v>2928</v>
+      </c>
+      <c r="AP21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ21" t="inlineStr">
+        <is>
+          <t>2926</t>
         </is>
       </c>
     </row>
@@ -2526,9 +2612,15 @@
       <c r="AN22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AO22" t="inlineStr">
-        <is>
-          <t>3782</t>
+      <c r="AO22" t="n">
+        <v>3782</v>
+      </c>
+      <c r="AP22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ22" t="inlineStr">
+        <is>
+          <t>4063</t>
         </is>
       </c>
     </row>
@@ -2659,9 +2751,15 @@
       <c r="AN23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AO23" t="inlineStr">
-        <is>
-          <t>3950</t>
+      <c r="AO23" t="n">
+        <v>3950</v>
+      </c>
+      <c r="AP23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AQ23" t="inlineStr">
+        <is>
+          <t>4303</t>
         </is>
       </c>
     </row>
@@ -2792,9 +2890,15 @@
       <c r="AN24" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AO24" t="inlineStr">
-        <is>
-          <t>3969</t>
+      <c r="AO24" t="n">
+        <v>3969</v>
+      </c>
+      <c r="AP24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AQ24" t="inlineStr">
+        <is>
+          <t>4014</t>
         </is>
       </c>
     </row>
@@ -2916,6 +3020,8 @@
       <c r="AM25" t="inlineStr"/>
       <c r="AN25" s="4" t="inlineStr"/>
       <c r="AO25" t="inlineStr"/>
+      <c r="AP25" s="4" t="inlineStr"/>
+      <c r="AQ25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -3023,6 +3129,8 @@
       <c r="AM26" t="inlineStr"/>
       <c r="AN26" s="4" t="inlineStr"/>
       <c r="AO26" t="inlineStr"/>
+      <c r="AP26" s="4" t="inlineStr"/>
+      <c r="AQ26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -3151,7 +3259,13 @@
       <c r="AN27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO27" t="inlineStr">
+      <c r="AO27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3211,6 +3325,8 @@
       <c r="AM28" t="inlineStr"/>
       <c r="AN28" s="4" t="inlineStr"/>
       <c r="AO28" t="inlineStr"/>
+      <c r="AP28" s="4" t="inlineStr"/>
+      <c r="AQ28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -3339,7 +3455,13 @@
       <c r="AN29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO29" t="inlineStr">
+      <c r="AO29" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AP29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ29" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3472,9 +3594,15 @@
       <c r="AN30" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AO30" t="inlineStr">
-        <is>
-          <t>2902</t>
+      <c r="AO30" t="n">
+        <v>2902</v>
+      </c>
+      <c r="AP30" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ30" t="inlineStr">
+        <is>
+          <t>3260</t>
         </is>
       </c>
     </row>
@@ -3605,9 +3733,15 @@
       <c r="AN31" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AO31" t="inlineStr">
-        <is>
-          <t>4032</t>
+      <c r="AO31" t="n">
+        <v>4032</v>
+      </c>
+      <c r="AP31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ31" t="inlineStr">
+        <is>
+          <t>4180</t>
         </is>
       </c>
     </row>
@@ -3738,9 +3872,15 @@
       <c r="AN32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO32" t="inlineStr">
-        <is>
-          <t>2551</t>
+      <c r="AO32" t="n">
+        <v>2551</v>
+      </c>
+      <c r="AP32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ32" t="inlineStr">
+        <is>
+          <t>2566</t>
         </is>
       </c>
     </row>
@@ -3798,6 +3938,8 @@
       <c r="AM33" t="inlineStr"/>
       <c r="AN33" s="4" t="inlineStr"/>
       <c r="AO33" t="inlineStr"/>
+      <c r="AP33" s="4" t="inlineStr"/>
+      <c r="AQ33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -3926,7 +4068,13 @@
       <c r="AN34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO34" t="inlineStr">
+      <c r="AO34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4059,7 +4207,13 @@
       <c r="AN35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO35" t="inlineStr">
+      <c r="AO35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ35" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4192,9 +4346,15 @@
       <c r="AN36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO36" t="inlineStr">
-        <is>
-          <t>2704</t>
+      <c r="AO36" t="n">
+        <v>2704</v>
+      </c>
+      <c r="AP36" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AQ36" t="inlineStr">
+        <is>
+          <t>2847</t>
         </is>
       </c>
     </row>
@@ -4324,6 +4484,8 @@
       </c>
       <c r="AN37" s="4" t="inlineStr"/>
       <c r="AO37" t="inlineStr"/>
+      <c r="AP37" s="4" t="inlineStr"/>
+      <c r="AQ37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -4452,9 +4614,15 @@
       <c r="AN38" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AO38" t="inlineStr">
-        <is>
-          <t>3853</t>
+      <c r="AO38" t="n">
+        <v>3853</v>
+      </c>
+      <c r="AP38" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AQ38" t="inlineStr">
+        <is>
+          <t>4136</t>
         </is>
       </c>
     </row>
@@ -4585,9 +4753,15 @@
       <c r="AN39" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AO39" t="inlineStr">
-        <is>
-          <t>3756</t>
+      <c r="AO39" t="n">
+        <v>3756</v>
+      </c>
+      <c r="AP39" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AQ39" t="inlineStr">
+        <is>
+          <t>3990</t>
         </is>
       </c>
     </row>
@@ -4718,7 +4892,13 @@
       <c r="AN40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO40" t="inlineStr">
+      <c r="AO40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4851,9 +5031,15 @@
       <c r="AN41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO41" t="inlineStr">
-        <is>
-          <t>3517</t>
+      <c r="AO41" t="n">
+        <v>3517</v>
+      </c>
+      <c r="AP41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ41" t="inlineStr">
+        <is>
+          <t>3908</t>
         </is>
       </c>
     </row>
@@ -4984,9 +5170,15 @@
       <c r="AN42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO42" t="inlineStr">
-        <is>
-          <t>2725</t>
+      <c r="AO42" t="n">
+        <v>2725</v>
+      </c>
+      <c r="AP42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ42" t="inlineStr">
+        <is>
+          <t>2773</t>
         </is>
       </c>
     </row>
@@ -5044,6 +5236,8 @@
       <c r="AM43" t="inlineStr"/>
       <c r="AN43" s="4" t="inlineStr"/>
       <c r="AO43" t="inlineStr"/>
+      <c r="AP43" s="4" t="inlineStr"/>
+      <c r="AQ43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -5099,6 +5293,8 @@
       <c r="AM44" t="inlineStr"/>
       <c r="AN44" s="4" t="inlineStr"/>
       <c r="AO44" t="inlineStr"/>
+      <c r="AP44" s="4" t="inlineStr"/>
+      <c r="AQ44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -5186,6 +5382,8 @@
       <c r="AM45" t="inlineStr"/>
       <c r="AN45" s="4" t="inlineStr"/>
       <c r="AO45" t="inlineStr"/>
+      <c r="AP45" s="4" t="inlineStr"/>
+      <c r="AQ45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -5314,9 +5512,15 @@
       <c r="AN46" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="AO46" t="inlineStr">
-        <is>
-          <t>3582</t>
+      <c r="AO46" t="n">
+        <v>3582</v>
+      </c>
+      <c r="AP46" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="AQ46" t="inlineStr">
+        <is>
+          <t>3797</t>
         </is>
       </c>
     </row>
@@ -5447,9 +5651,15 @@
       <c r="AN47" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AO47" t="inlineStr">
-        <is>
-          <t>4298</t>
+      <c r="AO47" t="n">
+        <v>4298</v>
+      </c>
+      <c r="AP47" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ47" t="inlineStr">
+        <is>
+          <t>4397</t>
         </is>
       </c>
     </row>
@@ -5580,7 +5790,13 @@
       <c r="AN48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO48" t="inlineStr">
+      <c r="AO48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5713,9 +5929,15 @@
       <c r="AN49" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AO49" t="inlineStr">
-        <is>
-          <t>4007</t>
+      <c r="AO49" t="n">
+        <v>4007</v>
+      </c>
+      <c r="AP49" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AQ49" t="inlineStr">
+        <is>
+          <t>4076</t>
         </is>
       </c>
     </row>
@@ -5846,9 +6068,15 @@
       <c r="AN50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AO50" t="inlineStr">
-        <is>
-          <t>3996</t>
+      <c r="AO50" t="n">
+        <v>3996</v>
+      </c>
+      <c r="AP50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AQ50" t="inlineStr">
+        <is>
+          <t>4132</t>
         </is>
       </c>
     </row>
@@ -5938,6 +6166,8 @@
       <c r="AM51" t="inlineStr"/>
       <c r="AN51" s="4" t="inlineStr"/>
       <c r="AO51" t="inlineStr"/>
+      <c r="AP51" s="4" t="inlineStr"/>
+      <c r="AQ51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -6066,9 +6296,15 @@
       <c r="AN52" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AO52" t="inlineStr">
-        <is>
-          <t>3985</t>
+      <c r="AO52" t="n">
+        <v>3985</v>
+      </c>
+      <c r="AP52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ52" t="inlineStr">
+        <is>
+          <t>4178</t>
         </is>
       </c>
     </row>
@@ -6199,9 +6435,15 @@
       <c r="AN53" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="AO53" t="inlineStr">
-        <is>
-          <t>2963</t>
+      <c r="AO53" t="n">
+        <v>2963</v>
+      </c>
+      <c r="AP53" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ53" t="inlineStr">
+        <is>
+          <t>3018</t>
         </is>
       </c>
     </row>
@@ -6291,6 +6533,8 @@
       <c r="AM54" t="inlineStr"/>
       <c r="AN54" s="4" t="inlineStr"/>
       <c r="AO54" t="inlineStr"/>
+      <c r="AP54" s="4" t="inlineStr"/>
+      <c r="AQ54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -6419,9 +6663,15 @@
       <c r="AN55" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="AO55" t="inlineStr">
-        <is>
-          <t>2938</t>
+      <c r="AO55" t="n">
+        <v>2938</v>
+      </c>
+      <c r="AP55" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ55" t="inlineStr">
+        <is>
+          <t>3399</t>
         </is>
       </c>
     </row>
@@ -6552,9 +6802,15 @@
       <c r="AN56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AO56" t="inlineStr">
-        <is>
-          <t>4172</t>
+      <c r="AO56" t="n">
+        <v>4172</v>
+      </c>
+      <c r="AP56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ56" t="inlineStr">
+        <is>
+          <t>4397</t>
         </is>
       </c>
     </row>
@@ -6685,9 +6941,15 @@
       <c r="AN57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AO57" t="inlineStr">
-        <is>
-          <t>3420</t>
+      <c r="AO57" t="n">
+        <v>3420</v>
+      </c>
+      <c r="AP57" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="AQ57" t="inlineStr">
+        <is>
+          <t>3572</t>
         </is>
       </c>
     </row>
@@ -6818,9 +7080,15 @@
       <c r="AN58" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AO58" t="inlineStr">
-        <is>
-          <t>3560</t>
+      <c r="AO58" t="n">
+        <v>3560</v>
+      </c>
+      <c r="AP58" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AQ58" t="inlineStr">
+        <is>
+          <t>3727</t>
         </is>
       </c>
     </row>
@@ -6951,9 +7219,15 @@
       <c r="AN59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AO59" t="inlineStr">
-        <is>
-          <t>3391</t>
+      <c r="AO59" t="n">
+        <v>3391</v>
+      </c>
+      <c r="AP59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ59" t="inlineStr">
+        <is>
+          <t>3623</t>
         </is>
       </c>
     </row>
@@ -7084,9 +7358,15 @@
       <c r="AN60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AO60" t="inlineStr">
-        <is>
-          <t>3876</t>
+      <c r="AO60" t="n">
+        <v>3876</v>
+      </c>
+      <c r="AP60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AQ60" t="inlineStr">
+        <is>
+          <t>3993</t>
         </is>
       </c>
     </row>
@@ -7144,6 +7424,8 @@
       <c r="AM61" t="inlineStr"/>
       <c r="AN61" s="4" t="inlineStr"/>
       <c r="AO61" t="inlineStr"/>
+      <c r="AP61" s="4" t="inlineStr"/>
+      <c r="AQ61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -7272,9 +7554,15 @@
       <c r="AN62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AO62" t="inlineStr">
-        <is>
-          <t>3262</t>
+      <c r="AO62" t="n">
+        <v>3262</v>
+      </c>
+      <c r="AP62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ62" t="inlineStr">
+        <is>
+          <t>3371</t>
         </is>
       </c>
     </row>
@@ -7405,9 +7693,15 @@
       <c r="AN63" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="AO63" t="inlineStr">
-        <is>
-          <t>3255</t>
+      <c r="AO63" t="n">
+        <v>3255</v>
+      </c>
+      <c r="AP63" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ63" t="inlineStr">
+        <is>
+          <t>3271</t>
         </is>
       </c>
     </row>
@@ -7538,9 +7832,15 @@
       <c r="AN64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO64" t="inlineStr">
-        <is>
-          <t>3634</t>
+      <c r="AO64" t="n">
+        <v>3634</v>
+      </c>
+      <c r="AP64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ64" t="inlineStr">
+        <is>
+          <t>3871</t>
         </is>
       </c>
     </row>
@@ -7650,6 +7950,8 @@
       <c r="AM65" t="inlineStr"/>
       <c r="AN65" s="4" t="inlineStr"/>
       <c r="AO65" t="inlineStr"/>
+      <c r="AP65" s="4" t="inlineStr"/>
+      <c r="AQ65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -7778,7 +8080,13 @@
       <c r="AN66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO66" t="inlineStr">
+      <c r="AO66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7911,7 +8219,13 @@
       <c r="AN67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO67" t="inlineStr">
+      <c r="AO67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8044,7 +8358,13 @@
       <c r="AN68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO68" t="inlineStr">
+      <c r="AO68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8104,6 +8424,8 @@
       <c r="AM69" t="inlineStr"/>
       <c r="AN69" s="4" t="inlineStr"/>
       <c r="AO69" t="inlineStr"/>
+      <c r="AP69" s="4" t="inlineStr"/>
+      <c r="AQ69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -8232,7 +8554,13 @@
       <c r="AN70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO70" t="inlineStr">
+      <c r="AO70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8365,7 +8693,13 @@
       <c r="AN71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO71" t="inlineStr">
+      <c r="AO71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8498,7 +8832,13 @@
       <c r="AN72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO72" t="inlineStr">
+      <c r="AO72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8631,9 +8971,15 @@
       <c r="AN73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO73" t="inlineStr">
-        <is>
-          <t>2641</t>
+      <c r="AO73" t="n">
+        <v>2641</v>
+      </c>
+      <c r="AP73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ73" t="inlineStr">
+        <is>
+          <t>2634</t>
         </is>
       </c>
     </row>
@@ -8764,7 +9110,13 @@
       <c r="AN74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO74" t="inlineStr">
+      <c r="AO74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8897,7 +9249,13 @@
       <c r="AN75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO75" t="inlineStr">
+      <c r="AO75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9030,9 +9388,15 @@
       <c r="AN76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO76" t="inlineStr">
-        <is>
-          <t>2499</t>
+      <c r="AO76" t="n">
+        <v>2499</v>
+      </c>
+      <c r="AP76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ76" t="inlineStr">
+        <is>
+          <t>2614</t>
         </is>
       </c>
     </row>
@@ -9163,9 +9527,15 @@
       <c r="AN77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO77" t="inlineStr">
-        <is>
-          <t>2583</t>
+      <c r="AO77" t="n">
+        <v>2583</v>
+      </c>
+      <c r="AP77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ77" t="inlineStr">
+        <is>
+          <t>2598</t>
         </is>
       </c>
     </row>
@@ -9296,7 +9666,13 @@
       <c r="AN78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO78" t="inlineStr">
+      <c r="AO78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9429,7 +9805,13 @@
       <c r="AN79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO79" t="inlineStr">
+      <c r="AO79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9562,7 +9944,13 @@
       <c r="AN80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO80" t="inlineStr">
+      <c r="AO80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9695,7 +10083,13 @@
       <c r="AN81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO81" t="inlineStr">
+      <c r="AO81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9828,7 +10222,13 @@
       <c r="AN82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO82" t="inlineStr">
+      <c r="AO82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9961,7 +10361,13 @@
       <c r="AN83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO83" t="inlineStr">
+      <c r="AO83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10094,7 +10500,13 @@
       <c r="AN84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO84" t="inlineStr">
+      <c r="AO84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10227,7 +10639,13 @@
       <c r="AN85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO85" t="inlineStr">
+      <c r="AO85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10360,7 +10778,13 @@
       <c r="AN86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO86" t="inlineStr">
+      <c r="AO86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10493,7 +10917,13 @@
       <c r="AN87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO87" t="inlineStr">
+      <c r="AO87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10626,7 +11056,13 @@
       <c r="AN88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO88" t="inlineStr">
+      <c r="AO88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10759,7 +11195,13 @@
       <c r="AN89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO89" t="inlineStr">
+      <c r="AO89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10892,7 +11334,13 @@
       <c r="AN90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO90" t="inlineStr">
+      <c r="AO90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11025,7 +11473,13 @@
       <c r="AN91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO91" t="inlineStr">
+      <c r="AO91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11158,7 +11612,13 @@
       <c r="AN92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO92" t="inlineStr">
+      <c r="AO92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11291,7 +11751,13 @@
       <c r="AN93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO93" t="inlineStr">
+      <c r="AO93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11424,7 +11890,13 @@
       <c r="AN94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO94" t="inlineStr">
+      <c r="AO94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11557,7 +12029,13 @@
       <c r="AN95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO95" t="inlineStr">
+      <c r="AO95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11690,9 +12168,15 @@
       <c r="AN96" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="AO96" t="inlineStr">
-        <is>
-          <t>2480</t>
+      <c r="AO96" t="n">
+        <v>2480</v>
+      </c>
+      <c r="AP96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ96" t="inlineStr">
+        <is>
+          <t>2479</t>
         </is>
       </c>
     </row>
@@ -11823,7 +12307,13 @@
       <c r="AN97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO97" t="inlineStr">
+      <c r="AO97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11956,7 +12446,13 @@
       <c r="AN98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO98" t="inlineStr">
+      <c r="AO98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12089,7 +12585,13 @@
       <c r="AN99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO99" t="inlineStr">
+      <c r="AO99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12222,7 +12724,13 @@
       <c r="AN100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO100" t="inlineStr">
+      <c r="AO100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12355,7 +12863,13 @@
       <c r="AN101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO101" t="inlineStr">
+      <c r="AO101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12488,7 +13002,13 @@
       <c r="AN102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO102" t="inlineStr">
+      <c r="AO102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12621,7 +13141,13 @@
       <c r="AN103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO103" t="inlineStr">
+      <c r="AO103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12754,7 +13280,13 @@
       <c r="AN104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO104" t="inlineStr">
+      <c r="AO104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12887,7 +13419,13 @@
       <c r="AN105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO105" t="inlineStr">
+      <c r="AO105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12947,6 +13485,8 @@
       <c r="AM106" t="inlineStr"/>
       <c r="AN106" s="4" t="inlineStr"/>
       <c r="AO106" t="inlineStr"/>
+      <c r="AP106" s="4" t="inlineStr"/>
+      <c r="AQ106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -13002,6 +13542,8 @@
       <c r="AM107" t="inlineStr"/>
       <c r="AN107" s="4" t="inlineStr"/>
       <c r="AO107" t="inlineStr"/>
+      <c r="AP107" s="4" t="inlineStr"/>
+      <c r="AQ107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -13057,6 +13599,8 @@
       <c r="AM108" t="inlineStr"/>
       <c r="AN108" s="4" t="inlineStr"/>
       <c r="AO108" t="inlineStr"/>
+      <c r="AP108" s="4" t="inlineStr"/>
+      <c r="AQ108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -13112,6 +13656,8 @@
       <c r="AM109" t="inlineStr"/>
       <c r="AN109" s="4" t="inlineStr"/>
       <c r="AO109" t="inlineStr"/>
+      <c r="AP109" s="4" t="inlineStr"/>
+      <c r="AQ109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -13167,6 +13713,8 @@
       <c r="AM110" t="inlineStr"/>
       <c r="AN110" s="4" t="inlineStr"/>
       <c r="AO110" t="inlineStr"/>
+      <c r="AP110" s="4" t="inlineStr"/>
+      <c r="AQ110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -13222,6 +13770,8 @@
       <c r="AM111" t="inlineStr"/>
       <c r="AN111" s="4" t="inlineStr"/>
       <c r="AO111" t="inlineStr"/>
+      <c r="AP111" s="4" t="inlineStr"/>
+      <c r="AQ111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -13277,6 +13827,8 @@
       <c r="AM112" t="inlineStr"/>
       <c r="AN112" s="4" t="inlineStr"/>
       <c r="AO112" t="inlineStr"/>
+      <c r="AP112" s="4" t="inlineStr"/>
+      <c r="AQ112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -13332,6 +13884,8 @@
       <c r="AM113" t="inlineStr"/>
       <c r="AN113" s="4" t="inlineStr"/>
       <c r="AO113" t="inlineStr"/>
+      <c r="AP113" s="4" t="inlineStr"/>
+      <c r="AQ113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -13387,6 +13941,8 @@
       <c r="AM114" t="inlineStr"/>
       <c r="AN114" s="4" t="inlineStr"/>
       <c r="AO114" t="inlineStr"/>
+      <c r="AP114" s="4" t="inlineStr"/>
+      <c r="AQ114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -13493,9 +14049,15 @@
       <c r="AN115" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AO115" t="inlineStr">
-        <is>
-          <t>3753</t>
+      <c r="AO115" t="n">
+        <v>3753</v>
+      </c>
+      <c r="AP115" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ115" t="inlineStr">
+        <is>
+          <t>4163</t>
         </is>
       </c>
     </row>
@@ -13620,7 +14182,13 @@
       <c r="AN116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO116" t="inlineStr">
+      <c r="AO116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13715,9 +14283,15 @@
       <c r="AN117" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AO117" t="inlineStr">
-        <is>
-          <t>4718</t>
+      <c r="AO117" t="n">
+        <v>4718</v>
+      </c>
+      <c r="AP117" s="5" t="n">
+        <v>37</v>
+      </c>
+      <c r="AQ117" t="inlineStr">
+        <is>
+          <t>4921</t>
         </is>
       </c>
     </row>
@@ -13842,9 +14416,15 @@
       <c r="AN118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO118" t="inlineStr">
-        <is>
-          <t>2749</t>
+      <c r="AO118" t="n">
+        <v>2749</v>
+      </c>
+      <c r="AP118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ118" t="inlineStr">
+        <is>
+          <t>2748</t>
         </is>
       </c>
     </row>
@@ -13969,9 +14549,15 @@
       <c r="AN119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO119" t="inlineStr">
-        <is>
-          <t>1498</t>
+      <c r="AO119" t="n">
+        <v>1498</v>
+      </c>
+      <c r="AP119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ119" t="inlineStr">
+        <is>
+          <t>1521</t>
         </is>
       </c>
     </row>
@@ -14096,7 +14682,13 @@
       <c r="AN120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO120" t="inlineStr">
+      <c r="AO120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ120" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14223,7 +14815,13 @@
       <c r="AN121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO121" t="inlineStr">
+      <c r="AO121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14350,7 +14948,13 @@
       <c r="AN122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO122" t="inlineStr">
+      <c r="AO122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14473,9 +15077,15 @@
       <c r="AN123" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="AO123" t="inlineStr">
-        <is>
-          <t>2580</t>
+      <c r="AO123" t="n">
+        <v>2580</v>
+      </c>
+      <c r="AP123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ123" t="inlineStr">
+        <is>
+          <t>2579</t>
         </is>
       </c>
     </row>
@@ -14559,6 +15169,8 @@
       <c r="AM124" t="inlineStr"/>
       <c r="AN124" s="4" t="inlineStr"/>
       <c r="AO124" t="inlineStr"/>
+      <c r="AP124" s="4" t="inlineStr"/>
+      <c r="AQ124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -14673,9 +15285,15 @@
       <c r="AN125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO125" t="inlineStr">
-        <is>
-          <t>2113</t>
+      <c r="AO125" t="n">
+        <v>2113</v>
+      </c>
+      <c r="AP125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ125" t="inlineStr">
+        <is>
+          <t>2122</t>
         </is>
       </c>
     </row>
@@ -14780,7 +15398,13 @@
       <c r="AN126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO126" t="inlineStr">
+      <c r="AO126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ126" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14858,6 +15482,8 @@
       <c r="AM127" t="inlineStr"/>
       <c r="AN127" s="4" t="inlineStr"/>
       <c r="AO127" t="inlineStr"/>
+      <c r="AP127" s="4" t="inlineStr"/>
+      <c r="AQ127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -14943,6 +15569,8 @@
       <c r="AM128" t="inlineStr"/>
       <c r="AN128" s="4" t="inlineStr"/>
       <c r="AO128" t="inlineStr"/>
+      <c r="AP128" s="4" t="inlineStr"/>
+      <c r="AQ128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -15037,9 +15665,15 @@
       <c r="AN129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO129" t="inlineStr">
-        <is>
-          <t>2500</t>
+      <c r="AO129" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AP129" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ129" t="inlineStr">
+        <is>
+          <t>2530</t>
         </is>
       </c>
     </row>
@@ -15127,6 +15761,8 @@
       <c r="AM130" t="inlineStr"/>
       <c r="AN130" s="4" t="inlineStr"/>
       <c r="AO130" t="inlineStr"/>
+      <c r="AP130" s="4" t="inlineStr"/>
+      <c r="AQ130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -15217,7 +15853,13 @@
       <c r="AN131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO131" t="inlineStr">
+      <c r="AO131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15300,9 +15942,15 @@
       <c r="AN132" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AO132" t="inlineStr">
-        <is>
-          <t>3511</t>
+      <c r="AO132" t="n">
+        <v>3511</v>
+      </c>
+      <c r="AP132" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ132" t="inlineStr">
+        <is>
+          <t>3785</t>
         </is>
       </c>
     </row>
@@ -15383,9 +16031,15 @@
       <c r="AN133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO133" t="inlineStr">
-        <is>
-          <t>2484</t>
+      <c r="AO133" t="n">
+        <v>2484</v>
+      </c>
+      <c r="AP133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ133" t="inlineStr">
+        <is>
+          <t>2479</t>
         </is>
       </c>
     </row>
@@ -15445,6 +16099,8 @@
       <c r="AM134" t="inlineStr"/>
       <c r="AN134" s="4" t="inlineStr"/>
       <c r="AO134" t="inlineStr"/>
+      <c r="AP134" s="4" t="inlineStr"/>
+      <c r="AQ134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -15506,6 +16162,8 @@
       <c r="AM135" t="inlineStr"/>
       <c r="AN135" s="4" t="inlineStr"/>
       <c r="AO135" t="inlineStr"/>
+      <c r="AP135" s="4" t="inlineStr"/>
+      <c r="AQ135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -15568,9 +16226,15 @@
       <c r="AN136" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AO136" t="inlineStr">
-        <is>
-          <t>4390</t>
+      <c r="AO136" t="n">
+        <v>4390</v>
+      </c>
+      <c r="AP136" s="5" t="n">
+        <v>39</v>
+      </c>
+      <c r="AQ136" t="inlineStr">
+        <is>
+          <t>4795</t>
         </is>
       </c>
     </row>
@@ -15635,9 +16299,15 @@
       <c r="AN137" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AO137" t="inlineStr">
-        <is>
-          <t>4256</t>
+      <c r="AO137" t="n">
+        <v>4256</v>
+      </c>
+      <c r="AP137" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AQ137" t="inlineStr">
+        <is>
+          <t>4653</t>
         </is>
       </c>
     </row>
@@ -15701,6 +16371,8 @@
       <c r="AM138" t="inlineStr"/>
       <c r="AN138" s="4" t="inlineStr"/>
       <c r="AO138" t="inlineStr"/>
+      <c r="AP138" s="4" t="inlineStr"/>
+      <c r="AQ138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -15763,9 +16435,15 @@
       <c r="AN139" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="AO139" t="inlineStr">
-        <is>
-          <t>4378</t>
+      <c r="AO139" t="n">
+        <v>4378</v>
+      </c>
+      <c r="AP139" s="5" t="n">
+        <v>36</v>
+      </c>
+      <c r="AQ139" t="inlineStr">
+        <is>
+          <t>4783</t>
         </is>
       </c>
     </row>
@@ -15830,9 +16508,15 @@
       <c r="AN140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO140" t="inlineStr">
-        <is>
-          <t>1995</t>
+      <c r="AO140" t="n">
+        <v>1995</v>
+      </c>
+      <c r="AP140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ140" t="inlineStr">
+        <is>
+          <t>2010</t>
         </is>
       </c>
     </row>
@@ -15892,6 +16576,8 @@
       <c r="AM141" t="inlineStr"/>
       <c r="AN141" s="4" t="inlineStr"/>
       <c r="AO141" t="inlineStr"/>
+      <c r="AP141" s="4" t="inlineStr"/>
+      <c r="AQ141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -15950,9 +16636,15 @@
       <c r="AN142" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AO142" t="inlineStr">
-        <is>
-          <t>2765</t>
+      <c r="AO142" t="n">
+        <v>2765</v>
+      </c>
+      <c r="AP142" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ142" t="inlineStr">
+        <is>
+          <t>2859</t>
         </is>
       </c>
     </row>
@@ -16013,17 +16705,21 @@
       <c r="AN143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO143" t="inlineStr">
+      <c r="AO143" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
     <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>37111401</t>
-        </is>
+      <c r="A144" t="n">
+        <v>37111401</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
@@ -16074,17 +16770,21 @@
       <c r="AN144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO144" t="inlineStr">
+      <c r="AO144" t="n">
+        <v>1511</v>
+      </c>
+      <c r="AP144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ144" t="inlineStr">
         <is>
           <t>1511</t>
         </is>
       </c>
     </row>
     <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>56300923</t>
-        </is>
+      <c r="A145" t="n">
+        <v>56300923</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
@@ -16135,17 +16835,21 @@
       <c r="AN145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO145" t="inlineStr">
-        <is>
-          <t>1785</t>
+      <c r="AO145" t="n">
+        <v>1785</v>
+      </c>
+      <c r="AP145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ145" t="inlineStr">
+        <is>
+          <t>1783</t>
         </is>
       </c>
     </row>
     <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>59242379</t>
-        </is>
+      <c r="A146" t="n">
+        <v>59242379</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
@@ -16196,17 +16900,21 @@
       <c r="AN146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AO146" t="inlineStr">
+      <c r="AO146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
       </c>
     </row>
     <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>56555218</t>
-        </is>
+      <c r="A147" t="n">
+        <v>56555218</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
@@ -16257,17 +16965,21 @@
       <c r="AN147" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AO147" t="inlineStr">
-        <is>
-          <t>3968</t>
+      <c r="AO147" t="n">
+        <v>3968</v>
+      </c>
+      <c r="AP147" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AQ147" t="inlineStr">
+        <is>
+          <t>4038</t>
         </is>
       </c>
     </row>
     <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>59519348</t>
-        </is>
+      <c r="A148" t="n">
+        <v>59519348</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
@@ -16318,9 +17030,204 @@
       <c r="AN148" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="AO148" t="inlineStr">
-        <is>
-          <t>1632</t>
+      <c r="AO148" t="n">
+        <v>1632</v>
+      </c>
+      <c r="AP148" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="AQ148" t="inlineStr">
+        <is>
+          <t>1864</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>21177139</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Baba_Serkan_Genç</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr"/>
+      <c r="D149" t="inlineStr"/>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F149" s="4" t="inlineStr"/>
+      <c r="G149" t="inlineStr"/>
+      <c r="H149" s="4" t="inlineStr"/>
+      <c r="I149" t="inlineStr"/>
+      <c r="J149" s="4" t="inlineStr"/>
+      <c r="K149" t="inlineStr"/>
+      <c r="L149" s="4" t="inlineStr"/>
+      <c r="M149" t="inlineStr"/>
+      <c r="N149" s="4" t="inlineStr"/>
+      <c r="O149" t="inlineStr"/>
+      <c r="P149" s="4" t="inlineStr"/>
+      <c r="Q149" t="inlineStr"/>
+      <c r="R149" s="4" t="inlineStr"/>
+      <c r="S149" t="inlineStr"/>
+      <c r="T149" s="4" t="inlineStr"/>
+      <c r="U149" t="inlineStr"/>
+      <c r="V149" s="4" t="inlineStr"/>
+      <c r="W149" t="inlineStr"/>
+      <c r="X149" s="4" t="inlineStr"/>
+      <c r="Y149" t="inlineStr"/>
+      <c r="Z149" s="4" t="inlineStr"/>
+      <c r="AA149" t="inlineStr"/>
+      <c r="AB149" s="4" t="inlineStr"/>
+      <c r="AC149" t="inlineStr"/>
+      <c r="AD149" s="4" t="inlineStr"/>
+      <c r="AE149" t="inlineStr"/>
+      <c r="AF149" s="4" t="inlineStr"/>
+      <c r="AG149" t="inlineStr"/>
+      <c r="AH149" s="4" t="inlineStr"/>
+      <c r="AI149" t="inlineStr"/>
+      <c r="AJ149" s="4" t="inlineStr"/>
+      <c r="AK149" t="inlineStr"/>
+      <c r="AL149" s="4" t="inlineStr"/>
+      <c r="AM149" t="inlineStr"/>
+      <c r="AN149" s="4" t="inlineStr"/>
+      <c r="AO149" t="inlineStr"/>
+      <c r="AP149" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="AQ149" t="inlineStr">
+        <is>
+          <t>4631</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>59210895</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>wormak21</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr"/>
+      <c r="D150" t="inlineStr"/>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F150" s="4" t="inlineStr"/>
+      <c r="G150" t="inlineStr"/>
+      <c r="H150" s="4" t="inlineStr"/>
+      <c r="I150" t="inlineStr"/>
+      <c r="J150" s="4" t="inlineStr"/>
+      <c r="K150" t="inlineStr"/>
+      <c r="L150" s="4" t="inlineStr"/>
+      <c r="M150" t="inlineStr"/>
+      <c r="N150" s="4" t="inlineStr"/>
+      <c r="O150" t="inlineStr"/>
+      <c r="P150" s="4" t="inlineStr"/>
+      <c r="Q150" t="inlineStr"/>
+      <c r="R150" s="4" t="inlineStr"/>
+      <c r="S150" t="inlineStr"/>
+      <c r="T150" s="4" t="inlineStr"/>
+      <c r="U150" t="inlineStr"/>
+      <c r="V150" s="4" t="inlineStr"/>
+      <c r="W150" t="inlineStr"/>
+      <c r="X150" s="4" t="inlineStr"/>
+      <c r="Y150" t="inlineStr"/>
+      <c r="Z150" s="4" t="inlineStr"/>
+      <c r="AA150" t="inlineStr"/>
+      <c r="AB150" s="4" t="inlineStr"/>
+      <c r="AC150" t="inlineStr"/>
+      <c r="AD150" s="4" t="inlineStr"/>
+      <c r="AE150" t="inlineStr"/>
+      <c r="AF150" s="4" t="inlineStr"/>
+      <c r="AG150" t="inlineStr"/>
+      <c r="AH150" s="4" t="inlineStr"/>
+      <c r="AI150" t="inlineStr"/>
+      <c r="AJ150" s="4" t="inlineStr"/>
+      <c r="AK150" t="inlineStr"/>
+      <c r="AL150" s="4" t="inlineStr"/>
+      <c r="AM150" t="inlineStr"/>
+      <c r="AN150" s="4" t="inlineStr"/>
+      <c r="AO150" t="inlineStr"/>
+      <c r="AP150" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AQ150" t="inlineStr">
+        <is>
+          <t>3188</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>59510744</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>AgilePromise57</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr"/>
+      <c r="D151" t="inlineStr"/>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F151" s="4" t="inlineStr"/>
+      <c r="G151" t="inlineStr"/>
+      <c r="H151" s="4" t="inlineStr"/>
+      <c r="I151" t="inlineStr"/>
+      <c r="J151" s="4" t="inlineStr"/>
+      <c r="K151" t="inlineStr"/>
+      <c r="L151" s="4" t="inlineStr"/>
+      <c r="M151" t="inlineStr"/>
+      <c r="N151" s="4" t="inlineStr"/>
+      <c r="O151" t="inlineStr"/>
+      <c r="P151" s="4" t="inlineStr"/>
+      <c r="Q151" t="inlineStr"/>
+      <c r="R151" s="4" t="inlineStr"/>
+      <c r="S151" t="inlineStr"/>
+      <c r="T151" s="4" t="inlineStr"/>
+      <c r="U151" t="inlineStr"/>
+      <c r="V151" s="4" t="inlineStr"/>
+      <c r="W151" t="inlineStr"/>
+      <c r="X151" s="4" t="inlineStr"/>
+      <c r="Y151" t="inlineStr"/>
+      <c r="Z151" s="4" t="inlineStr"/>
+      <c r="AA151" t="inlineStr"/>
+      <c r="AB151" s="4" t="inlineStr"/>
+      <c r="AC151" t="inlineStr"/>
+      <c r="AD151" s="4" t="inlineStr"/>
+      <c r="AE151" t="inlineStr"/>
+      <c r="AF151" s="4" t="inlineStr"/>
+      <c r="AG151" t="inlineStr"/>
+      <c r="AH151" s="4" t="inlineStr"/>
+      <c r="AI151" t="inlineStr"/>
+      <c r="AJ151" s="4" t="inlineStr"/>
+      <c r="AK151" t="inlineStr"/>
+      <c r="AL151" s="4" t="inlineStr"/>
+      <c r="AM151" t="inlineStr"/>
+      <c r="AN151" s="4" t="inlineStr"/>
+      <c r="AO151" t="inlineStr"/>
+      <c r="AP151" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AQ151" t="inlineStr">
+        <is>
+          <t>2159</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-06-09 11:30:54
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -17043,10 +17043,8 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>21177139</t>
-        </is>
+      <c r="A149" t="n">
+        <v>21177139</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
@@ -17106,10 +17104,8 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" t="inlineStr">
-        <is>
-          <t>59210895</t>
-        </is>
+      <c r="A150" t="n">
+        <v>59210895</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
@@ -17169,10 +17165,8 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" t="inlineStr">
-        <is>
-          <t>59510744</t>
-        </is>
+      <c r="A151" t="n">
+        <v>59510744</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-06-10 10:37:44
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AQ151"/>
+  <dimension ref="A1:AS152"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -606,6 +606,16 @@
           <t>06-08_0</t>
         </is>
       </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>06-09_A</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>06-09_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -740,9 +750,15 @@
       <c r="AP2" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="AQ2" t="inlineStr">
-        <is>
-          <t>3666</t>
+      <c r="AQ2" t="n">
+        <v>3666</v>
+      </c>
+      <c r="AR2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS2" t="inlineStr">
+        <is>
+          <t>3693</t>
         </is>
       </c>
     </row>
@@ -879,7 +895,13 @@
       <c r="AP3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ3" t="inlineStr">
+      <c r="AQ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1018,7 +1040,13 @@
       <c r="AP4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ4" t="inlineStr">
+      <c r="AQ4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1157,9 +1185,15 @@
       <c r="AP5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ5" t="inlineStr">
-        <is>
-          <t>2688</t>
+      <c r="AQ5" t="n">
+        <v>2688</v>
+      </c>
+      <c r="AR5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS5" t="inlineStr">
+        <is>
+          <t>2713</t>
         </is>
       </c>
     </row>
@@ -1296,7 +1330,13 @@
       <c r="AP6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ6" t="inlineStr">
+      <c r="AQ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1358,6 +1398,8 @@
       <c r="AO7" t="inlineStr"/>
       <c r="AP7" s="4" t="inlineStr"/>
       <c r="AQ7" t="inlineStr"/>
+      <c r="AR7" s="4" t="inlineStr"/>
+      <c r="AS7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1415,6 +1457,8 @@
       <c r="AO8" t="inlineStr"/>
       <c r="AP8" s="4" t="inlineStr"/>
       <c r="AQ8" t="inlineStr"/>
+      <c r="AR8" s="4" t="inlineStr"/>
+      <c r="AS8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1472,6 +1516,8 @@
       <c r="AO9" t="inlineStr"/>
       <c r="AP9" s="4" t="inlineStr"/>
       <c r="AQ9" t="inlineStr"/>
+      <c r="AR9" s="4" t="inlineStr"/>
+      <c r="AS9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1529,6 +1575,8 @@
       <c r="AO10" t="inlineStr"/>
       <c r="AP10" s="4" t="inlineStr"/>
       <c r="AQ10" t="inlineStr"/>
+      <c r="AR10" s="4" t="inlineStr"/>
+      <c r="AS10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1586,6 +1634,8 @@
       <c r="AO11" t="inlineStr"/>
       <c r="AP11" s="4" t="inlineStr"/>
       <c r="AQ11" t="inlineStr"/>
+      <c r="AR11" s="4" t="inlineStr"/>
+      <c r="AS11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1643,6 +1693,8 @@
       <c r="AO12" t="inlineStr"/>
       <c r="AP12" s="4" t="inlineStr"/>
       <c r="AQ12" t="inlineStr"/>
+      <c r="AR12" s="4" t="inlineStr"/>
+      <c r="AS12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1700,6 +1752,8 @@
       <c r="AO13" t="inlineStr"/>
       <c r="AP13" s="4" t="inlineStr"/>
       <c r="AQ13" t="inlineStr"/>
+      <c r="AR13" s="4" t="inlineStr"/>
+      <c r="AS13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1757,6 +1811,8 @@
       <c r="AO14" t="inlineStr"/>
       <c r="AP14" s="4" t="inlineStr"/>
       <c r="AQ14" t="inlineStr"/>
+      <c r="AR14" s="4" t="inlineStr"/>
+      <c r="AS14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1814,6 +1870,8 @@
       <c r="AO15" t="inlineStr"/>
       <c r="AP15" s="4" t="inlineStr"/>
       <c r="AQ15" t="inlineStr"/>
+      <c r="AR15" s="4" t="inlineStr"/>
+      <c r="AS15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1871,6 +1929,8 @@
       <c r="AO16" t="inlineStr"/>
       <c r="AP16" s="4" t="inlineStr"/>
       <c r="AQ16" t="inlineStr"/>
+      <c r="AR16" s="4" t="inlineStr"/>
+      <c r="AS16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1928,6 +1988,8 @@
       <c r="AO17" t="inlineStr"/>
       <c r="AP17" s="4" t="inlineStr"/>
       <c r="AQ17" t="inlineStr"/>
+      <c r="AR17" s="4" t="inlineStr"/>
+      <c r="AS17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -2062,9 +2124,15 @@
       <c r="AP18" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="AQ18" t="inlineStr">
-        <is>
-          <t>3505</t>
+      <c r="AQ18" t="n">
+        <v>3505</v>
+      </c>
+      <c r="AR18" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS18" t="inlineStr">
+        <is>
+          <t>3791</t>
         </is>
       </c>
     </row>
@@ -2201,7 +2269,13 @@
       <c r="AP19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ19" t="inlineStr">
+      <c r="AQ19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS19" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2340,9 +2414,15 @@
       <c r="AP20" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AQ20" t="inlineStr">
-        <is>
-          <t>3719</t>
+      <c r="AQ20" t="n">
+        <v>3719</v>
+      </c>
+      <c r="AR20" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS20" t="inlineStr">
+        <is>
+          <t>3955</t>
         </is>
       </c>
     </row>
@@ -2479,9 +2559,15 @@
       <c r="AP21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ21" t="inlineStr">
-        <is>
-          <t>2926</t>
+      <c r="AQ21" t="n">
+        <v>2926</v>
+      </c>
+      <c r="AR21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS21" t="inlineStr">
+        <is>
+          <t>2996</t>
         </is>
       </c>
     </row>
@@ -2618,9 +2704,15 @@
       <c r="AP22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AQ22" t="inlineStr">
-        <is>
-          <t>4063</t>
+      <c r="AQ22" t="n">
+        <v>4063</v>
+      </c>
+      <c r="AR22" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AS22" t="inlineStr">
+        <is>
+          <t>4281</t>
         </is>
       </c>
     </row>
@@ -2757,9 +2849,15 @@
       <c r="AP23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AQ23" t="inlineStr">
-        <is>
-          <t>4303</t>
+      <c r="AQ23" t="n">
+        <v>4303</v>
+      </c>
+      <c r="AR23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AS23" t="inlineStr">
+        <is>
+          <t>4600</t>
         </is>
       </c>
     </row>
@@ -2896,9 +2994,15 @@
       <c r="AP24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AQ24" t="inlineStr">
-        <is>
-          <t>4014</t>
+      <c r="AQ24" t="n">
+        <v>4014</v>
+      </c>
+      <c r="AR24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AS24" t="inlineStr">
+        <is>
+          <t>4260</t>
         </is>
       </c>
     </row>
@@ -3022,6 +3126,8 @@
       <c r="AO25" t="inlineStr"/>
       <c r="AP25" s="4" t="inlineStr"/>
       <c r="AQ25" t="inlineStr"/>
+      <c r="AR25" s="4" t="inlineStr"/>
+      <c r="AS25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -3131,6 +3237,8 @@
       <c r="AO26" t="inlineStr"/>
       <c r="AP26" s="4" t="inlineStr"/>
       <c r="AQ26" t="inlineStr"/>
+      <c r="AR26" s="4" t="inlineStr"/>
+      <c r="AS26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -3265,7 +3373,13 @@
       <c r="AP27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ27" t="inlineStr">
+      <c r="AQ27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3327,6 +3441,8 @@
       <c r="AO28" t="inlineStr"/>
       <c r="AP28" s="4" t="inlineStr"/>
       <c r="AQ28" t="inlineStr"/>
+      <c r="AR28" s="4" t="inlineStr"/>
+      <c r="AS28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -3461,7 +3577,13 @@
       <c r="AP29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ29" t="inlineStr">
+      <c r="AQ29" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AR29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS29" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3600,9 +3722,15 @@
       <c r="AP30" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AQ30" t="inlineStr">
-        <is>
-          <t>3260</t>
+      <c r="AQ30" t="n">
+        <v>3260</v>
+      </c>
+      <c r="AR30" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS30" t="inlineStr">
+        <is>
+          <t>3585</t>
         </is>
       </c>
     </row>
@@ -3739,9 +3867,15 @@
       <c r="AP31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AQ31" t="inlineStr">
-        <is>
-          <t>4180</t>
+      <c r="AQ31" t="n">
+        <v>4180</v>
+      </c>
+      <c r="AR31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS31" t="inlineStr">
+        <is>
+          <t>4298</t>
         </is>
       </c>
     </row>
@@ -3878,9 +4012,15 @@
       <c r="AP32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ32" t="inlineStr">
-        <is>
-          <t>2566</t>
+      <c r="AQ32" t="n">
+        <v>2566</v>
+      </c>
+      <c r="AR32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS32" t="inlineStr">
+        <is>
+          <t>2565</t>
         </is>
       </c>
     </row>
@@ -3940,6 +4080,8 @@
       <c r="AO33" t="inlineStr"/>
       <c r="AP33" s="4" t="inlineStr"/>
       <c r="AQ33" t="inlineStr"/>
+      <c r="AR33" s="4" t="inlineStr"/>
+      <c r="AS33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -4074,7 +4216,13 @@
       <c r="AP34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ34" t="inlineStr">
+      <c r="AQ34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4213,7 +4361,13 @@
       <c r="AP35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ35" t="inlineStr">
+      <c r="AQ35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS35" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4352,9 +4506,15 @@
       <c r="AP36" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="AQ36" t="inlineStr">
-        <is>
-          <t>2847</t>
+      <c r="AQ36" t="n">
+        <v>2847</v>
+      </c>
+      <c r="AR36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS36" t="inlineStr">
+        <is>
+          <t>2879</t>
         </is>
       </c>
     </row>
@@ -4486,6 +4646,8 @@
       <c r="AO37" t="inlineStr"/>
       <c r="AP37" s="4" t="inlineStr"/>
       <c r="AQ37" t="inlineStr"/>
+      <c r="AR37" s="4" t="inlineStr"/>
+      <c r="AS37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -4620,9 +4782,15 @@
       <c r="AP38" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AQ38" t="inlineStr">
-        <is>
-          <t>4136</t>
+      <c r="AQ38" t="n">
+        <v>4136</v>
+      </c>
+      <c r="AR38" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS38" t="inlineStr">
+        <is>
+          <t>4372</t>
         </is>
       </c>
     </row>
@@ -4759,9 +4927,15 @@
       <c r="AP39" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AQ39" t="inlineStr">
-        <is>
-          <t>3990</t>
+      <c r="AQ39" t="n">
+        <v>3990</v>
+      </c>
+      <c r="AR39" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="AS39" t="inlineStr">
+        <is>
+          <t>4143</t>
         </is>
       </c>
     </row>
@@ -4898,7 +5072,13 @@
       <c r="AP40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ40" t="inlineStr">
+      <c r="AQ40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5037,9 +5217,15 @@
       <c r="AP41" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="AQ41" t="inlineStr">
-        <is>
-          <t>3908</t>
+      <c r="AQ41" t="n">
+        <v>3908</v>
+      </c>
+      <c r="AR41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS41" t="inlineStr">
+        <is>
+          <t>3994</t>
         </is>
       </c>
     </row>
@@ -5176,9 +5362,15 @@
       <c r="AP42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ42" t="inlineStr">
-        <is>
-          <t>2773</t>
+      <c r="AQ42" t="n">
+        <v>2773</v>
+      </c>
+      <c r="AR42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS42" t="inlineStr">
+        <is>
+          <t>2770</t>
         </is>
       </c>
     </row>
@@ -5238,6 +5430,8 @@
       <c r="AO43" t="inlineStr"/>
       <c r="AP43" s="4" t="inlineStr"/>
       <c r="AQ43" t="inlineStr"/>
+      <c r="AR43" s="4" t="inlineStr"/>
+      <c r="AS43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -5295,6 +5489,8 @@
       <c r="AO44" t="inlineStr"/>
       <c r="AP44" s="4" t="inlineStr"/>
       <c r="AQ44" t="inlineStr"/>
+      <c r="AR44" s="4" t="inlineStr"/>
+      <c r="AS44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -5384,6 +5580,8 @@
       <c r="AO45" t="inlineStr"/>
       <c r="AP45" s="4" t="inlineStr"/>
       <c r="AQ45" t="inlineStr"/>
+      <c r="AR45" s="4" t="inlineStr"/>
+      <c r="AS45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -5518,9 +5716,15 @@
       <c r="AP46" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="AQ46" t="inlineStr">
-        <is>
-          <t>3797</t>
+      <c r="AQ46" t="n">
+        <v>3797</v>
+      </c>
+      <c r="AR46" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="AS46" t="inlineStr">
+        <is>
+          <t>3994</t>
         </is>
       </c>
     </row>
@@ -5657,9 +5861,15 @@
       <c r="AP47" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AQ47" t="inlineStr">
-        <is>
-          <t>4397</t>
+      <c r="AQ47" t="n">
+        <v>4397</v>
+      </c>
+      <c r="AR47" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AS47" t="inlineStr">
+        <is>
+          <t>4698</t>
         </is>
       </c>
     </row>
@@ -5796,7 +6006,13 @@
       <c r="AP48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ48" t="inlineStr">
+      <c r="AQ48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5935,9 +6151,15 @@
       <c r="AP49" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AQ49" t="inlineStr">
-        <is>
-          <t>4076</t>
+      <c r="AQ49" t="n">
+        <v>4076</v>
+      </c>
+      <c r="AR49" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AS49" t="inlineStr">
+        <is>
+          <t>4260</t>
         </is>
       </c>
     </row>
@@ -6074,9 +6296,15 @@
       <c r="AP50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AQ50" t="inlineStr">
-        <is>
-          <t>4132</t>
+      <c r="AQ50" t="n">
+        <v>4132</v>
+      </c>
+      <c r="AR50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AS50" t="inlineStr">
+        <is>
+          <t>4329</t>
         </is>
       </c>
     </row>
@@ -6168,6 +6396,8 @@
       <c r="AO51" t="inlineStr"/>
       <c r="AP51" s="4" t="inlineStr"/>
       <c r="AQ51" t="inlineStr"/>
+      <c r="AR51" s="4" t="inlineStr"/>
+      <c r="AS51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -6302,9 +6532,15 @@
       <c r="AP52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AQ52" t="inlineStr">
-        <is>
-          <t>4178</t>
+      <c r="AQ52" t="n">
+        <v>4178</v>
+      </c>
+      <c r="AR52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS52" t="inlineStr">
+        <is>
+          <t>4329</t>
         </is>
       </c>
     </row>
@@ -6441,9 +6677,15 @@
       <c r="AP53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ53" t="inlineStr">
-        <is>
-          <t>3018</t>
+      <c r="AQ53" t="n">
+        <v>3018</v>
+      </c>
+      <c r="AR53" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AS53" t="inlineStr">
+        <is>
+          <t>3152</t>
         </is>
       </c>
     </row>
@@ -6535,6 +6777,8 @@
       <c r="AO54" t="inlineStr"/>
       <c r="AP54" s="4" t="inlineStr"/>
       <c r="AQ54" t="inlineStr"/>
+      <c r="AR54" s="4" t="inlineStr"/>
+      <c r="AS54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -6669,9 +6913,15 @@
       <c r="AP55" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AQ55" t="inlineStr">
-        <is>
-          <t>3399</t>
+      <c r="AQ55" t="n">
+        <v>3399</v>
+      </c>
+      <c r="AR55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS55" t="inlineStr">
+        <is>
+          <t>3437</t>
         </is>
       </c>
     </row>
@@ -6808,9 +7058,15 @@
       <c r="AP56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AQ56" t="inlineStr">
-        <is>
-          <t>4397</t>
+      <c r="AQ56" t="n">
+        <v>4397</v>
+      </c>
+      <c r="AR56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS56" t="inlineStr">
+        <is>
+          <t>4482</t>
         </is>
       </c>
     </row>
@@ -6947,9 +7203,15 @@
       <c r="AP57" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="AQ57" t="inlineStr">
-        <is>
-          <t>3572</t>
+      <c r="AQ57" t="n">
+        <v>3572</v>
+      </c>
+      <c r="AR57" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="AS57" t="inlineStr">
+        <is>
+          <t>3786</t>
         </is>
       </c>
     </row>
@@ -7086,9 +7348,15 @@
       <c r="AP58" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AQ58" t="inlineStr">
-        <is>
-          <t>3727</t>
+      <c r="AQ58" t="n">
+        <v>3727</v>
+      </c>
+      <c r="AR58" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AS58" t="inlineStr">
+        <is>
+          <t>3936</t>
         </is>
       </c>
     </row>
@@ -7225,9 +7493,15 @@
       <c r="AP59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AQ59" t="inlineStr">
-        <is>
-          <t>3623</t>
+      <c r="AQ59" t="n">
+        <v>3623</v>
+      </c>
+      <c r="AR59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS59" t="inlineStr">
+        <is>
+          <t>3925</t>
         </is>
       </c>
     </row>
@@ -7364,9 +7638,15 @@
       <c r="AP60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AQ60" t="inlineStr">
-        <is>
-          <t>3993</t>
+      <c r="AQ60" t="n">
+        <v>3993</v>
+      </c>
+      <c r="AR60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AS60" t="inlineStr">
+        <is>
+          <t>4052</t>
         </is>
       </c>
     </row>
@@ -7426,6 +7706,8 @@
       <c r="AO61" t="inlineStr"/>
       <c r="AP61" s="4" t="inlineStr"/>
       <c r="AQ61" t="inlineStr"/>
+      <c r="AR61" s="4" t="inlineStr"/>
+      <c r="AS61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -7560,9 +7842,15 @@
       <c r="AP62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AQ62" t="inlineStr">
-        <is>
-          <t>3371</t>
+      <c r="AQ62" t="n">
+        <v>3371</v>
+      </c>
+      <c r="AR62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS62" t="inlineStr">
+        <is>
+          <t>3601</t>
         </is>
       </c>
     </row>
@@ -7699,9 +7987,15 @@
       <c r="AP63" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="AQ63" t="inlineStr">
-        <is>
-          <t>3271</t>
+      <c r="AQ63" t="n">
+        <v>3271</v>
+      </c>
+      <c r="AR63" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="AS63" t="inlineStr">
+        <is>
+          <t>3550</t>
         </is>
       </c>
     </row>
@@ -7838,9 +8132,15 @@
       <c r="AP64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ64" t="inlineStr">
-        <is>
-          <t>3871</t>
+      <c r="AQ64" t="n">
+        <v>3871</v>
+      </c>
+      <c r="AR64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AS64" t="inlineStr">
+        <is>
+          <t>3988</t>
         </is>
       </c>
     </row>
@@ -7952,6 +8252,8 @@
       <c r="AO65" t="inlineStr"/>
       <c r="AP65" s="4" t="inlineStr"/>
       <c r="AQ65" t="inlineStr"/>
+      <c r="AR65" s="4" t="inlineStr"/>
+      <c r="AS65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -8086,7 +8388,13 @@
       <c r="AP66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ66" t="inlineStr">
+      <c r="AQ66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8225,7 +8533,13 @@
       <c r="AP67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ67" t="inlineStr">
+      <c r="AQ67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8364,7 +8678,13 @@
       <c r="AP68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ68" t="inlineStr">
+      <c r="AQ68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8426,6 +8746,8 @@
       <c r="AO69" t="inlineStr"/>
       <c r="AP69" s="4" t="inlineStr"/>
       <c r="AQ69" t="inlineStr"/>
+      <c r="AR69" s="4" t="inlineStr"/>
+      <c r="AS69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -8560,7 +8882,13 @@
       <c r="AP70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ70" t="inlineStr">
+      <c r="AQ70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8699,7 +9027,13 @@
       <c r="AP71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ71" t="inlineStr">
+      <c r="AQ71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8838,7 +9172,13 @@
       <c r="AP72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ72" t="inlineStr">
+      <c r="AQ72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8977,9 +9317,15 @@
       <c r="AP73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ73" t="inlineStr">
-        <is>
-          <t>2634</t>
+      <c r="AQ73" t="n">
+        <v>2634</v>
+      </c>
+      <c r="AR73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS73" t="inlineStr">
+        <is>
+          <t>2627</t>
         </is>
       </c>
     </row>
@@ -9116,7 +9462,13 @@
       <c r="AP74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ74" t="inlineStr">
+      <c r="AQ74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9255,7 +9607,13 @@
       <c r="AP75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ75" t="inlineStr">
+      <c r="AQ75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9394,9 +9752,15 @@
       <c r="AP76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ76" t="inlineStr">
-        <is>
-          <t>2614</t>
+      <c r="AQ76" t="n">
+        <v>2614</v>
+      </c>
+      <c r="AR76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS76" t="inlineStr">
+        <is>
+          <t>2640</t>
         </is>
       </c>
     </row>
@@ -9533,9 +9897,15 @@
       <c r="AP77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ77" t="inlineStr">
-        <is>
-          <t>2598</t>
+      <c r="AQ77" t="n">
+        <v>2598</v>
+      </c>
+      <c r="AR77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS77" t="inlineStr">
+        <is>
+          <t>2621</t>
         </is>
       </c>
     </row>
@@ -9672,7 +10042,13 @@
       <c r="AP78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ78" t="inlineStr">
+      <c r="AQ78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9811,7 +10187,13 @@
       <c r="AP79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ79" t="inlineStr">
+      <c r="AQ79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9950,7 +10332,13 @@
       <c r="AP80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ80" t="inlineStr">
+      <c r="AQ80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10089,7 +10477,13 @@
       <c r="AP81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ81" t="inlineStr">
+      <c r="AQ81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10228,7 +10622,13 @@
       <c r="AP82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ82" t="inlineStr">
+      <c r="AQ82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10367,7 +10767,13 @@
       <c r="AP83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ83" t="inlineStr">
+      <c r="AQ83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10506,7 +10912,13 @@
       <c r="AP84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ84" t="inlineStr">
+      <c r="AQ84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10645,7 +11057,13 @@
       <c r="AP85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ85" t="inlineStr">
+      <c r="AQ85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10784,7 +11202,13 @@
       <c r="AP86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ86" t="inlineStr">
+      <c r="AQ86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10923,7 +11347,13 @@
       <c r="AP87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ87" t="inlineStr">
+      <c r="AQ87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11062,7 +11492,13 @@
       <c r="AP88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ88" t="inlineStr">
+      <c r="AQ88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11201,7 +11637,13 @@
       <c r="AP89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ89" t="inlineStr">
+      <c r="AQ89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11340,7 +11782,13 @@
       <c r="AP90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ90" t="inlineStr">
+      <c r="AQ90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11479,7 +11927,13 @@
       <c r="AP91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ91" t="inlineStr">
+      <c r="AQ91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11618,7 +12072,13 @@
       <c r="AP92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ92" t="inlineStr">
+      <c r="AQ92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11757,7 +12217,13 @@
       <c r="AP93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ93" t="inlineStr">
+      <c r="AQ93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11896,7 +12362,13 @@
       <c r="AP94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ94" t="inlineStr">
+      <c r="AQ94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12035,7 +12507,13 @@
       <c r="AP95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ95" t="inlineStr">
+      <c r="AQ95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12174,9 +12652,15 @@
       <c r="AP96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ96" t="inlineStr">
-        <is>
-          <t>2479</t>
+      <c r="AQ96" t="n">
+        <v>2479</v>
+      </c>
+      <c r="AR96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS96" t="inlineStr">
+        <is>
+          <t>2475</t>
         </is>
       </c>
     </row>
@@ -12313,7 +12797,13 @@
       <c r="AP97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ97" t="inlineStr">
+      <c r="AQ97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12452,7 +12942,13 @@
       <c r="AP98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ98" t="inlineStr">
+      <c r="AQ98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12591,7 +13087,13 @@
       <c r="AP99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ99" t="inlineStr">
+      <c r="AQ99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12730,7 +13232,13 @@
       <c r="AP100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ100" t="inlineStr">
+      <c r="AQ100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12869,7 +13377,13 @@
       <c r="AP101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ101" t="inlineStr">
+      <c r="AQ101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13008,7 +13522,13 @@
       <c r="AP102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ102" t="inlineStr">
+      <c r="AQ102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13147,7 +13667,13 @@
       <c r="AP103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ103" t="inlineStr">
+      <c r="AQ103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13286,7 +13812,13 @@
       <c r="AP104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ104" t="inlineStr">
+      <c r="AQ104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13425,7 +13957,13 @@
       <c r="AP105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ105" t="inlineStr">
+      <c r="AQ105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13487,6 +14025,8 @@
       <c r="AO106" t="inlineStr"/>
       <c r="AP106" s="4" t="inlineStr"/>
       <c r="AQ106" t="inlineStr"/>
+      <c r="AR106" s="4" t="inlineStr"/>
+      <c r="AS106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -13544,6 +14084,8 @@
       <c r="AO107" t="inlineStr"/>
       <c r="AP107" s="4" t="inlineStr"/>
       <c r="AQ107" t="inlineStr"/>
+      <c r="AR107" s="4" t="inlineStr"/>
+      <c r="AS107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -13601,6 +14143,8 @@
       <c r="AO108" t="inlineStr"/>
       <c r="AP108" s="4" t="inlineStr"/>
       <c r="AQ108" t="inlineStr"/>
+      <c r="AR108" s="4" t="inlineStr"/>
+      <c r="AS108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -13658,6 +14202,8 @@
       <c r="AO109" t="inlineStr"/>
       <c r="AP109" s="4" t="inlineStr"/>
       <c r="AQ109" t="inlineStr"/>
+      <c r="AR109" s="4" t="inlineStr"/>
+      <c r="AS109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -13715,6 +14261,8 @@
       <c r="AO110" t="inlineStr"/>
       <c r="AP110" s="4" t="inlineStr"/>
       <c r="AQ110" t="inlineStr"/>
+      <c r="AR110" s="4" t="inlineStr"/>
+      <c r="AS110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -13772,6 +14320,8 @@
       <c r="AO111" t="inlineStr"/>
       <c r="AP111" s="4" t="inlineStr"/>
       <c r="AQ111" t="inlineStr"/>
+      <c r="AR111" s="4" t="inlineStr"/>
+      <c r="AS111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -13829,6 +14379,8 @@
       <c r="AO112" t="inlineStr"/>
       <c r="AP112" s="4" t="inlineStr"/>
       <c r="AQ112" t="inlineStr"/>
+      <c r="AR112" s="4" t="inlineStr"/>
+      <c r="AS112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -13886,6 +14438,8 @@
       <c r="AO113" t="inlineStr"/>
       <c r="AP113" s="4" t="inlineStr"/>
       <c r="AQ113" t="inlineStr"/>
+      <c r="AR113" s="4" t="inlineStr"/>
+      <c r="AS113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -13943,6 +14497,8 @@
       <c r="AO114" t="inlineStr"/>
       <c r="AP114" s="4" t="inlineStr"/>
       <c r="AQ114" t="inlineStr"/>
+      <c r="AR114" s="4" t="inlineStr"/>
+      <c r="AS114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -14055,9 +14611,15 @@
       <c r="AP115" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AQ115" t="inlineStr">
-        <is>
-          <t>4163</t>
+      <c r="AQ115" t="n">
+        <v>4163</v>
+      </c>
+      <c r="AR115" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS115" t="inlineStr">
+        <is>
+          <t>4549</t>
         </is>
       </c>
     </row>
@@ -14188,7 +14750,13 @@
       <c r="AP116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ116" t="inlineStr">
+      <c r="AQ116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14289,9 +14857,15 @@
       <c r="AP117" s="5" t="n">
         <v>37</v>
       </c>
-      <c r="AQ117" t="inlineStr">
-        <is>
-          <t>4921</t>
+      <c r="AQ117" t="n">
+        <v>4921</v>
+      </c>
+      <c r="AR117" s="5" t="n">
+        <v>38</v>
+      </c>
+      <c r="AS117" t="inlineStr">
+        <is>
+          <t>5169</t>
         </is>
       </c>
     </row>
@@ -14422,9 +14996,15 @@
       <c r="AP118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ118" t="inlineStr">
-        <is>
-          <t>2748</t>
+      <c r="AQ118" t="n">
+        <v>2748</v>
+      </c>
+      <c r="AR118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS118" t="inlineStr">
+        <is>
+          <t>2747</t>
         </is>
       </c>
     </row>
@@ -14555,9 +15135,15 @@
       <c r="AP119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ119" t="inlineStr">
-        <is>
-          <t>1521</t>
+      <c r="AQ119" t="n">
+        <v>1521</v>
+      </c>
+      <c r="AR119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS119" t="inlineStr">
+        <is>
+          <t>1518</t>
         </is>
       </c>
     </row>
@@ -14688,7 +15274,13 @@
       <c r="AP120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ120" t="inlineStr">
+      <c r="AQ120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS120" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14821,7 +15413,13 @@
       <c r="AP121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ121" t="inlineStr">
+      <c r="AQ121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14954,7 +15552,13 @@
       <c r="AP122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ122" t="inlineStr">
+      <c r="AQ122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15083,7 +15687,13 @@
       <c r="AP123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ123" t="inlineStr">
+      <c r="AQ123" t="n">
+        <v>2579</v>
+      </c>
+      <c r="AR123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS123" t="inlineStr">
         <is>
           <t>2579</t>
         </is>
@@ -15171,6 +15781,8 @@
       <c r="AO124" t="inlineStr"/>
       <c r="AP124" s="4" t="inlineStr"/>
       <c r="AQ124" t="inlineStr"/>
+      <c r="AR124" s="4" t="inlineStr"/>
+      <c r="AS124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -15291,9 +15903,15 @@
       <c r="AP125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ125" t="inlineStr">
-        <is>
-          <t>2122</t>
+      <c r="AQ125" t="n">
+        <v>2122</v>
+      </c>
+      <c r="AR125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS125" t="inlineStr">
+        <is>
+          <t>2134</t>
         </is>
       </c>
     </row>
@@ -15404,7 +16022,13 @@
       <c r="AP126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ126" t="inlineStr">
+      <c r="AQ126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS126" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15484,6 +16108,8 @@
       <c r="AO127" t="inlineStr"/>
       <c r="AP127" s="4" t="inlineStr"/>
       <c r="AQ127" t="inlineStr"/>
+      <c r="AR127" s="4" t="inlineStr"/>
+      <c r="AS127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -15571,6 +16197,8 @@
       <c r="AO128" t="inlineStr"/>
       <c r="AP128" s="4" t="inlineStr"/>
       <c r="AQ128" t="inlineStr"/>
+      <c r="AR128" s="4" t="inlineStr"/>
+      <c r="AS128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -15671,9 +16299,15 @@
       <c r="AP129" s="3" t="n">
         <v>4</v>
       </c>
-      <c r="AQ129" t="inlineStr">
-        <is>
-          <t>2530</t>
+      <c r="AQ129" t="n">
+        <v>2530</v>
+      </c>
+      <c r="AR129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS129" t="inlineStr">
+        <is>
+          <t>2528</t>
         </is>
       </c>
     </row>
@@ -15763,6 +16397,8 @@
       <c r="AO130" t="inlineStr"/>
       <c r="AP130" s="4" t="inlineStr"/>
       <c r="AQ130" t="inlineStr"/>
+      <c r="AR130" s="4" t="inlineStr"/>
+      <c r="AS130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -15859,7 +16495,13 @@
       <c r="AP131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ131" t="inlineStr">
+      <c r="AQ131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15948,9 +16590,15 @@
       <c r="AP132" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AQ132" t="inlineStr">
-        <is>
-          <t>3785</t>
+      <c r="AQ132" t="n">
+        <v>3785</v>
+      </c>
+      <c r="AR132" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AS132" t="inlineStr">
+        <is>
+          <t>3945</t>
         </is>
       </c>
     </row>
@@ -16037,9 +16685,15 @@
       <c r="AP133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ133" t="inlineStr">
-        <is>
-          <t>2479</t>
+      <c r="AQ133" t="n">
+        <v>2479</v>
+      </c>
+      <c r="AR133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS133" t="inlineStr">
+        <is>
+          <t>2474</t>
         </is>
       </c>
     </row>
@@ -16101,6 +16755,8 @@
       <c r="AO134" t="inlineStr"/>
       <c r="AP134" s="4" t="inlineStr"/>
       <c r="AQ134" t="inlineStr"/>
+      <c r="AR134" s="4" t="inlineStr"/>
+      <c r="AS134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -16164,6 +16820,8 @@
       <c r="AO135" t="inlineStr"/>
       <c r="AP135" s="4" t="inlineStr"/>
       <c r="AQ135" t="inlineStr"/>
+      <c r="AR135" s="4" t="inlineStr"/>
+      <c r="AS135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -16232,9 +16890,15 @@
       <c r="AP136" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="AQ136" t="inlineStr">
-        <is>
-          <t>4795</t>
+      <c r="AQ136" t="n">
+        <v>4795</v>
+      </c>
+      <c r="AR136" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AS136" t="inlineStr">
+        <is>
+          <t>5055</t>
         </is>
       </c>
     </row>
@@ -16305,9 +16969,15 @@
       <c r="AP137" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AQ137" t="inlineStr">
-        <is>
-          <t>4653</t>
+      <c r="AQ137" t="n">
+        <v>4653</v>
+      </c>
+      <c r="AR137" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AS137" t="inlineStr">
+        <is>
+          <t>4918</t>
         </is>
       </c>
     </row>
@@ -16373,6 +17043,8 @@
       <c r="AO138" t="inlineStr"/>
       <c r="AP138" s="4" t="inlineStr"/>
       <c r="AQ138" t="inlineStr"/>
+      <c r="AR138" s="4" t="inlineStr"/>
+      <c r="AS138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -16380,7 +17052,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>"㊥ PhononDisperse"</t>
+          <t>"㊥ PRL"</t>
         </is>
       </c>
       <c r="C139" t="inlineStr"/>
@@ -16441,9 +17113,15 @@
       <c r="AP139" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="AQ139" t="inlineStr">
-        <is>
-          <t>4783</t>
+      <c r="AQ139" t="n">
+        <v>4783</v>
+      </c>
+      <c r="AR139" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AS139" t="inlineStr">
+        <is>
+          <t>5186</t>
         </is>
       </c>
     </row>
@@ -16514,9 +17192,15 @@
       <c r="AP140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ140" t="inlineStr">
-        <is>
-          <t>2010</t>
+      <c r="AQ140" t="n">
+        <v>2010</v>
+      </c>
+      <c r="AR140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS140" t="inlineStr">
+        <is>
+          <t>2007</t>
         </is>
       </c>
     </row>
@@ -16578,6 +17262,8 @@
       <c r="AO141" t="inlineStr"/>
       <c r="AP141" s="4" t="inlineStr"/>
       <c r="AQ141" t="inlineStr"/>
+      <c r="AR141" s="4" t="inlineStr"/>
+      <c r="AS141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -16642,9 +17328,15 @@
       <c r="AP142" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AQ142" t="inlineStr">
-        <is>
-          <t>2859</t>
+      <c r="AQ142" t="n">
+        <v>2859</v>
+      </c>
+      <c r="AR142" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AS142" t="inlineStr">
+        <is>
+          <t>2833</t>
         </is>
       </c>
     </row>
@@ -16711,7 +17403,13 @@
       <c r="AP143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ143" t="inlineStr">
+      <c r="AQ143" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16776,7 +17474,13 @@
       <c r="AP144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ144" t="inlineStr">
+      <c r="AQ144" t="n">
+        <v>1511</v>
+      </c>
+      <c r="AR144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS144" t="inlineStr">
         <is>
           <t>1511</t>
         </is>
@@ -16841,9 +17545,15 @@
       <c r="AP145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ145" t="inlineStr">
-        <is>
-          <t>1783</t>
+      <c r="AQ145" t="n">
+        <v>1783</v>
+      </c>
+      <c r="AR145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS145" t="inlineStr">
+        <is>
+          <t>1806</t>
         </is>
       </c>
     </row>
@@ -16906,7 +17616,13 @@
       <c r="AP146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AQ146" t="inlineStr">
+      <c r="AQ146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16971,9 +17687,15 @@
       <c r="AP147" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AQ147" t="inlineStr">
-        <is>
-          <t>4038</t>
+      <c r="AQ147" t="n">
+        <v>4038</v>
+      </c>
+      <c r="AR147" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AS147" t="inlineStr">
+        <is>
+          <t>4166</t>
         </is>
       </c>
     </row>
@@ -17036,9 +17758,15 @@
       <c r="AP148" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="AQ148" t="inlineStr">
-        <is>
-          <t>1864</t>
+      <c r="AQ148" t="n">
+        <v>1864</v>
+      </c>
+      <c r="AR148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS148" t="inlineStr">
+        <is>
+          <t>2001</t>
         </is>
       </c>
     </row>
@@ -17097,9 +17825,15 @@
       <c r="AP149" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="AQ149" t="inlineStr">
-        <is>
-          <t>4631</t>
+      <c r="AQ149" t="n">
+        <v>4631</v>
+      </c>
+      <c r="AR149" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="AS149" t="inlineStr">
+        <is>
+          <t>5105</t>
         </is>
       </c>
     </row>
@@ -17158,9 +17892,15 @@
       <c r="AP150" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="AQ150" t="inlineStr">
-        <is>
-          <t>3188</t>
+      <c r="AQ150" t="n">
+        <v>3188</v>
+      </c>
+      <c r="AR150" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AS150" t="inlineStr">
+        <is>
+          <t>3347</t>
         </is>
       </c>
     </row>
@@ -17219,9 +17959,80 @@
       <c r="AP151" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AQ151" t="inlineStr">
-        <is>
-          <t>2159</t>
+      <c r="AQ151" t="n">
+        <v>2159</v>
+      </c>
+      <c r="AR151" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AS151" t="inlineStr">
+        <is>
+          <t>2239</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>1342640</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>☠禕☸神☠</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr"/>
+      <c r="D152" t="inlineStr"/>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>一馆</t>
+        </is>
+      </c>
+      <c r="F152" s="4" t="inlineStr"/>
+      <c r="G152" t="inlineStr"/>
+      <c r="H152" s="4" t="inlineStr"/>
+      <c r="I152" t="inlineStr"/>
+      <c r="J152" s="4" t="inlineStr"/>
+      <c r="K152" t="inlineStr"/>
+      <c r="L152" s="4" t="inlineStr"/>
+      <c r="M152" t="inlineStr"/>
+      <c r="N152" s="4" t="inlineStr"/>
+      <c r="O152" t="inlineStr"/>
+      <c r="P152" s="4" t="inlineStr"/>
+      <c r="Q152" t="inlineStr"/>
+      <c r="R152" s="4" t="inlineStr"/>
+      <c r="S152" t="inlineStr"/>
+      <c r="T152" s="4" t="inlineStr"/>
+      <c r="U152" t="inlineStr"/>
+      <c r="V152" s="4" t="inlineStr"/>
+      <c r="W152" t="inlineStr"/>
+      <c r="X152" s="4" t="inlineStr"/>
+      <c r="Y152" t="inlineStr"/>
+      <c r="Z152" s="4" t="inlineStr"/>
+      <c r="AA152" t="inlineStr"/>
+      <c r="AB152" s="4" t="inlineStr"/>
+      <c r="AC152" t="inlineStr"/>
+      <c r="AD152" s="4" t="inlineStr"/>
+      <c r="AE152" t="inlineStr"/>
+      <c r="AF152" s="4" t="inlineStr"/>
+      <c r="AG152" t="inlineStr"/>
+      <c r="AH152" s="4" t="inlineStr"/>
+      <c r="AI152" t="inlineStr"/>
+      <c r="AJ152" s="4" t="inlineStr"/>
+      <c r="AK152" t="inlineStr"/>
+      <c r="AL152" s="4" t="inlineStr"/>
+      <c r="AM152" t="inlineStr"/>
+      <c r="AN152" s="4" t="inlineStr"/>
+      <c r="AO152" t="inlineStr"/>
+      <c r="AP152" s="4" t="inlineStr"/>
+      <c r="AQ152" t="inlineStr"/>
+      <c r="AR152" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AS152" t="inlineStr">
+        <is>
+          <t>3724</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-06-10 11:30:51
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -17972,10 +17972,8 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" t="inlineStr">
-        <is>
-          <t>1342640</t>
-        </is>
+      <c r="A152" t="n">
+        <v>1342640</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-06-11 10:51:05
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AS152"/>
+  <dimension ref="A1:AU153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -616,6 +616,16 @@
           <t>06-09_0</t>
         </is>
       </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>06-10_A</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>06-10_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -756,9 +766,15 @@
       <c r="AR2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="AS2" t="inlineStr">
-        <is>
-          <t>3693</t>
+      <c r="AS2" t="n">
+        <v>3693</v>
+      </c>
+      <c r="AT2" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU2" t="inlineStr">
+        <is>
+          <t>4156</t>
         </is>
       </c>
     </row>
@@ -901,7 +917,13 @@
       <c r="AR3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS3" t="inlineStr">
+      <c r="AS3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1046,7 +1068,13 @@
       <c r="AR4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS4" t="inlineStr">
+      <c r="AS4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1191,9 +1219,15 @@
       <c r="AR5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS5" t="inlineStr">
-        <is>
-          <t>2713</t>
+      <c r="AS5" t="n">
+        <v>2713</v>
+      </c>
+      <c r="AT5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU5" t="inlineStr">
+        <is>
+          <t>2736</t>
         </is>
       </c>
     </row>
@@ -1336,7 +1370,13 @@
       <c r="AR6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS6" t="inlineStr">
+      <c r="AS6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1400,6 +1440,8 @@
       <c r="AQ7" t="inlineStr"/>
       <c r="AR7" s="4" t="inlineStr"/>
       <c r="AS7" t="inlineStr"/>
+      <c r="AT7" s="4" t="inlineStr"/>
+      <c r="AU7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1459,6 +1501,8 @@
       <c r="AQ8" t="inlineStr"/>
       <c r="AR8" s="4" t="inlineStr"/>
       <c r="AS8" t="inlineStr"/>
+      <c r="AT8" s="4" t="inlineStr"/>
+      <c r="AU8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1518,6 +1562,8 @@
       <c r="AQ9" t="inlineStr"/>
       <c r="AR9" s="4" t="inlineStr"/>
       <c r="AS9" t="inlineStr"/>
+      <c r="AT9" s="4" t="inlineStr"/>
+      <c r="AU9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1577,6 +1623,8 @@
       <c r="AQ10" t="inlineStr"/>
       <c r="AR10" s="4" t="inlineStr"/>
       <c r="AS10" t="inlineStr"/>
+      <c r="AT10" s="4" t="inlineStr"/>
+      <c r="AU10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1636,6 +1684,8 @@
       <c r="AQ11" t="inlineStr"/>
       <c r="AR11" s="4" t="inlineStr"/>
       <c r="AS11" t="inlineStr"/>
+      <c r="AT11" s="4" t="inlineStr"/>
+      <c r="AU11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1695,6 +1745,8 @@
       <c r="AQ12" t="inlineStr"/>
       <c r="AR12" s="4" t="inlineStr"/>
       <c r="AS12" t="inlineStr"/>
+      <c r="AT12" s="4" t="inlineStr"/>
+      <c r="AU12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1754,6 +1806,8 @@
       <c r="AQ13" t="inlineStr"/>
       <c r="AR13" s="4" t="inlineStr"/>
       <c r="AS13" t="inlineStr"/>
+      <c r="AT13" s="4" t="inlineStr"/>
+      <c r="AU13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1813,6 +1867,8 @@
       <c r="AQ14" t="inlineStr"/>
       <c r="AR14" s="4" t="inlineStr"/>
       <c r="AS14" t="inlineStr"/>
+      <c r="AT14" s="4" t="inlineStr"/>
+      <c r="AU14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1872,6 +1928,8 @@
       <c r="AQ15" t="inlineStr"/>
       <c r="AR15" s="4" t="inlineStr"/>
       <c r="AS15" t="inlineStr"/>
+      <c r="AT15" s="4" t="inlineStr"/>
+      <c r="AU15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1931,6 +1989,8 @@
       <c r="AQ16" t="inlineStr"/>
       <c r="AR16" s="4" t="inlineStr"/>
       <c r="AS16" t="inlineStr"/>
+      <c r="AT16" s="4" t="inlineStr"/>
+      <c r="AU16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1990,6 +2050,8 @@
       <c r="AQ17" t="inlineStr"/>
       <c r="AR17" s="4" t="inlineStr"/>
       <c r="AS17" t="inlineStr"/>
+      <c r="AT17" s="4" t="inlineStr"/>
+      <c r="AU17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -2130,9 +2192,15 @@
       <c r="AR18" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AS18" t="inlineStr">
-        <is>
-          <t>3791</t>
+      <c r="AS18" t="n">
+        <v>3791</v>
+      </c>
+      <c r="AT18" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="AU18" t="inlineStr">
+        <is>
+          <t>3957</t>
         </is>
       </c>
     </row>
@@ -2275,7 +2343,13 @@
       <c r="AR19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS19" t="inlineStr">
+      <c r="AS19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU19" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2420,9 +2494,15 @@
       <c r="AR20" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AS20" t="inlineStr">
-        <is>
-          <t>3955</t>
+      <c r="AS20" t="n">
+        <v>3955</v>
+      </c>
+      <c r="AT20" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU20" t="inlineStr">
+        <is>
+          <t>4090</t>
         </is>
       </c>
     </row>
@@ -2565,9 +2645,15 @@
       <c r="AR21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS21" t="inlineStr">
-        <is>
-          <t>2996</t>
+      <c r="AS21" t="n">
+        <v>2996</v>
+      </c>
+      <c r="AT21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU21" t="inlineStr">
+        <is>
+          <t>3035</t>
         </is>
       </c>
     </row>
@@ -2710,9 +2796,15 @@
       <c r="AR22" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AS22" t="inlineStr">
-        <is>
-          <t>4281</t>
+      <c r="AS22" t="n">
+        <v>4281</v>
+      </c>
+      <c r="AT22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU22" t="inlineStr">
+        <is>
+          <t>4495</t>
         </is>
       </c>
     </row>
@@ -2855,9 +2947,15 @@
       <c r="AR23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AS23" t="inlineStr">
-        <is>
-          <t>4600</t>
+      <c r="AS23" t="n">
+        <v>4600</v>
+      </c>
+      <c r="AT23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AU23" t="inlineStr">
+        <is>
+          <t>4883</t>
         </is>
       </c>
     </row>
@@ -3000,9 +3098,15 @@
       <c r="AR24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AS24" t="inlineStr">
-        <is>
-          <t>4260</t>
+      <c r="AS24" t="n">
+        <v>4260</v>
+      </c>
+      <c r="AT24" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AU24" t="inlineStr">
+        <is>
+          <t>4376</t>
         </is>
       </c>
     </row>
@@ -3128,6 +3232,8 @@
       <c r="AQ25" t="inlineStr"/>
       <c r="AR25" s="4" t="inlineStr"/>
       <c r="AS25" t="inlineStr"/>
+      <c r="AT25" s="4" t="inlineStr"/>
+      <c r="AU25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -3239,6 +3345,8 @@
       <c r="AQ26" t="inlineStr"/>
       <c r="AR26" s="4" t="inlineStr"/>
       <c r="AS26" t="inlineStr"/>
+      <c r="AT26" s="4" t="inlineStr"/>
+      <c r="AU26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -3379,7 +3487,13 @@
       <c r="AR27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS27" t="inlineStr">
+      <c r="AS27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3443,6 +3557,8 @@
       <c r="AQ28" t="inlineStr"/>
       <c r="AR28" s="4" t="inlineStr"/>
       <c r="AS28" t="inlineStr"/>
+      <c r="AT28" s="4" t="inlineStr"/>
+      <c r="AU28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -3583,7 +3699,13 @@
       <c r="AR29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS29" t="inlineStr">
+      <c r="AS29" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AT29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU29" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3728,9 +3850,15 @@
       <c r="AR30" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AS30" t="inlineStr">
-        <is>
-          <t>3585</t>
+      <c r="AS30" t="n">
+        <v>3585</v>
+      </c>
+      <c r="AT30" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AU30" t="inlineStr">
+        <is>
+          <t>3939</t>
         </is>
       </c>
     </row>
@@ -3873,9 +4001,15 @@
       <c r="AR31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AS31" t="inlineStr">
-        <is>
-          <t>4298</t>
+      <c r="AS31" t="n">
+        <v>4298</v>
+      </c>
+      <c r="AT31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU31" t="inlineStr">
+        <is>
+          <t>4506</t>
         </is>
       </c>
     </row>
@@ -4018,9 +4152,15 @@
       <c r="AR32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS32" t="inlineStr">
-        <is>
-          <t>2565</t>
+      <c r="AS32" t="n">
+        <v>2565</v>
+      </c>
+      <c r="AT32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU32" t="inlineStr">
+        <is>
+          <t>2597</t>
         </is>
       </c>
     </row>
@@ -4082,6 +4222,8 @@
       <c r="AQ33" t="inlineStr"/>
       <c r="AR33" s="4" t="inlineStr"/>
       <c r="AS33" t="inlineStr"/>
+      <c r="AT33" s="4" t="inlineStr"/>
+      <c r="AU33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -4222,7 +4364,13 @@
       <c r="AR34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS34" t="inlineStr">
+      <c r="AS34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4367,7 +4515,13 @@
       <c r="AR35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS35" t="inlineStr">
+      <c r="AS35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU35" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4512,9 +4666,15 @@
       <c r="AR36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS36" t="inlineStr">
-        <is>
-          <t>2879</t>
+      <c r="AS36" t="n">
+        <v>2879</v>
+      </c>
+      <c r="AT36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU36" t="inlineStr">
+        <is>
+          <t>2932</t>
         </is>
       </c>
     </row>
@@ -4648,6 +4808,8 @@
       <c r="AQ37" t="inlineStr"/>
       <c r="AR37" s="4" t="inlineStr"/>
       <c r="AS37" t="inlineStr"/>
+      <c r="AT37" s="4" t="inlineStr"/>
+      <c r="AU37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -4788,9 +4950,15 @@
       <c r="AR38" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AS38" t="inlineStr">
-        <is>
-          <t>4372</t>
+      <c r="AS38" t="n">
+        <v>4372</v>
+      </c>
+      <c r="AT38" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AU38" t="inlineStr">
+        <is>
+          <t>4656</t>
         </is>
       </c>
     </row>
@@ -4933,9 +5101,15 @@
       <c r="AR39" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="AS39" t="inlineStr">
-        <is>
-          <t>4143</t>
+      <c r="AS39" t="n">
+        <v>4143</v>
+      </c>
+      <c r="AT39" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AU39" t="inlineStr">
+        <is>
+          <t>4226</t>
         </is>
       </c>
     </row>
@@ -5078,7 +5252,13 @@
       <c r="AR40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS40" t="inlineStr">
+      <c r="AS40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5223,7 +5403,13 @@
       <c r="AR41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS41" t="inlineStr">
+      <c r="AS41" t="n">
+        <v>3994</v>
+      </c>
+      <c r="AT41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU41" t="inlineStr">
         <is>
           <t>3994</t>
         </is>
@@ -5368,9 +5554,15 @@
       <c r="AR42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS42" t="inlineStr">
-        <is>
-          <t>2770</t>
+      <c r="AS42" t="n">
+        <v>2770</v>
+      </c>
+      <c r="AT42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU42" t="inlineStr">
+        <is>
+          <t>2768</t>
         </is>
       </c>
     </row>
@@ -5432,6 +5624,8 @@
       <c r="AQ43" t="inlineStr"/>
       <c r="AR43" s="4" t="inlineStr"/>
       <c r="AS43" t="inlineStr"/>
+      <c r="AT43" s="4" t="inlineStr"/>
+      <c r="AU43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -5491,6 +5685,8 @@
       <c r="AQ44" t="inlineStr"/>
       <c r="AR44" s="4" t="inlineStr"/>
       <c r="AS44" t="inlineStr"/>
+      <c r="AT44" s="4" t="inlineStr"/>
+      <c r="AU44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -5582,6 +5778,8 @@
       <c r="AQ45" t="inlineStr"/>
       <c r="AR45" s="4" t="inlineStr"/>
       <c r="AS45" t="inlineStr"/>
+      <c r="AT45" s="4" t="inlineStr"/>
+      <c r="AU45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -5722,9 +5920,15 @@
       <c r="AR46" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="AS46" t="inlineStr">
-        <is>
-          <t>3994</t>
+      <c r="AS46" t="n">
+        <v>3994</v>
+      </c>
+      <c r="AT46" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AU46" t="inlineStr">
+        <is>
+          <t>4126</t>
         </is>
       </c>
     </row>
@@ -5867,9 +6071,15 @@
       <c r="AR47" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AS47" t="inlineStr">
-        <is>
-          <t>4698</t>
+      <c r="AS47" t="n">
+        <v>4698</v>
+      </c>
+      <c r="AT47" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AU47" t="inlineStr">
+        <is>
+          <t>4919</t>
         </is>
       </c>
     </row>
@@ -6012,7 +6222,13 @@
       <c r="AR48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS48" t="inlineStr">
+      <c r="AS48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6157,9 +6373,15 @@
       <c r="AR49" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AS49" t="inlineStr">
-        <is>
-          <t>4260</t>
+      <c r="AS49" t="n">
+        <v>4260</v>
+      </c>
+      <c r="AT49" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="AU49" t="inlineStr">
+        <is>
+          <t>4375</t>
         </is>
       </c>
     </row>
@@ -6302,9 +6524,15 @@
       <c r="AR50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AS50" t="inlineStr">
-        <is>
-          <t>4329</t>
+      <c r="AS50" t="n">
+        <v>4329</v>
+      </c>
+      <c r="AT50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AU50" t="inlineStr">
+        <is>
+          <t>4489</t>
         </is>
       </c>
     </row>
@@ -6398,6 +6626,8 @@
       <c r="AQ51" t="inlineStr"/>
       <c r="AR51" s="4" t="inlineStr"/>
       <c r="AS51" t="inlineStr"/>
+      <c r="AT51" s="4" t="inlineStr"/>
+      <c r="AU51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -6538,9 +6768,15 @@
       <c r="AR52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AS52" t="inlineStr">
-        <is>
-          <t>4329</t>
+      <c r="AS52" t="n">
+        <v>4329</v>
+      </c>
+      <c r="AT52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU52" t="inlineStr">
+        <is>
+          <t>4627</t>
         </is>
       </c>
     </row>
@@ -6683,9 +6919,15 @@
       <c r="AR53" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="AS53" t="inlineStr">
-        <is>
-          <t>3152</t>
+      <c r="AS53" t="n">
+        <v>3152</v>
+      </c>
+      <c r="AT53" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AU53" t="inlineStr">
+        <is>
+          <t>3290</t>
         </is>
       </c>
     </row>
@@ -6779,6 +7021,8 @@
       <c r="AQ54" t="inlineStr"/>
       <c r="AR54" s="4" t="inlineStr"/>
       <c r="AS54" t="inlineStr"/>
+      <c r="AT54" s="4" t="inlineStr"/>
+      <c r="AU54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -6919,9 +7163,15 @@
       <c r="AR55" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS55" t="inlineStr">
-        <is>
-          <t>3437</t>
+      <c r="AS55" t="n">
+        <v>3437</v>
+      </c>
+      <c r="AT55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU55" t="inlineStr">
+        <is>
+          <t>3432</t>
         </is>
       </c>
     </row>
@@ -7064,9 +7314,15 @@
       <c r="AR56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AS56" t="inlineStr">
-        <is>
-          <t>4482</t>
+      <c r="AS56" t="n">
+        <v>4482</v>
+      </c>
+      <c r="AT56" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AU56" t="inlineStr">
+        <is>
+          <t>4735</t>
         </is>
       </c>
     </row>
@@ -7209,9 +7465,15 @@
       <c r="AR57" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="AS57" t="inlineStr">
-        <is>
-          <t>3786</t>
+      <c r="AS57" t="n">
+        <v>3786</v>
+      </c>
+      <c r="AT57" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="AU57" t="inlineStr">
+        <is>
+          <t>4050</t>
         </is>
       </c>
     </row>
@@ -7354,9 +7616,15 @@
       <c r="AR58" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AS58" t="inlineStr">
-        <is>
-          <t>3936</t>
+      <c r="AS58" t="n">
+        <v>3936</v>
+      </c>
+      <c r="AT58" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AU58" t="inlineStr">
+        <is>
+          <t>3995</t>
         </is>
       </c>
     </row>
@@ -7499,9 +7767,15 @@
       <c r="AR59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AS59" t="inlineStr">
-        <is>
-          <t>3925</t>
+      <c r="AS59" t="n">
+        <v>3925</v>
+      </c>
+      <c r="AT59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU59" t="inlineStr">
+        <is>
+          <t>3994</t>
         </is>
       </c>
     </row>
@@ -7644,9 +7918,15 @@
       <c r="AR60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AS60" t="inlineStr">
-        <is>
-          <t>4052</t>
+      <c r="AS60" t="n">
+        <v>4052</v>
+      </c>
+      <c r="AT60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AU60" t="inlineStr">
+        <is>
+          <t>4149</t>
         </is>
       </c>
     </row>
@@ -7708,6 +7988,8 @@
       <c r="AQ61" t="inlineStr"/>
       <c r="AR61" s="4" t="inlineStr"/>
       <c r="AS61" t="inlineStr"/>
+      <c r="AT61" s="4" t="inlineStr"/>
+      <c r="AU61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -7848,9 +8130,15 @@
       <c r="AR62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AS62" t="inlineStr">
-        <is>
-          <t>3601</t>
+      <c r="AS62" t="n">
+        <v>3601</v>
+      </c>
+      <c r="AT62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU62" t="inlineStr">
+        <is>
+          <t>3720</t>
         </is>
       </c>
     </row>
@@ -7993,9 +8281,15 @@
       <c r="AR63" s="3" t="n">
         <v>14</v>
       </c>
-      <c r="AS63" t="inlineStr">
-        <is>
-          <t>3550</t>
+      <c r="AS63" t="n">
+        <v>3550</v>
+      </c>
+      <c r="AT63" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU63" t="inlineStr">
+        <is>
+          <t>3885</t>
         </is>
       </c>
     </row>
@@ -8138,9 +8432,15 @@
       <c r="AR64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AS64" t="inlineStr">
-        <is>
-          <t>3988</t>
+      <c r="AS64" t="n">
+        <v>3988</v>
+      </c>
+      <c r="AT64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU64" t="inlineStr">
+        <is>
+          <t>4042</t>
         </is>
       </c>
     </row>
@@ -8254,6 +8554,8 @@
       <c r="AQ65" t="inlineStr"/>
       <c r="AR65" s="4" t="inlineStr"/>
       <c r="AS65" t="inlineStr"/>
+      <c r="AT65" s="4" t="inlineStr"/>
+      <c r="AU65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -8394,7 +8696,13 @@
       <c r="AR66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS66" t="inlineStr">
+      <c r="AS66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8539,7 +8847,13 @@
       <c r="AR67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS67" t="inlineStr">
+      <c r="AS67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8684,7 +8998,13 @@
       <c r="AR68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS68" t="inlineStr">
+      <c r="AS68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8748,6 +9068,8 @@
       <c r="AQ69" t="inlineStr"/>
       <c r="AR69" s="4" t="inlineStr"/>
       <c r="AS69" t="inlineStr"/>
+      <c r="AT69" s="4" t="inlineStr"/>
+      <c r="AU69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -8888,7 +9210,13 @@
       <c r="AR70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS70" t="inlineStr">
+      <c r="AS70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9033,7 +9361,13 @@
       <c r="AR71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS71" t="inlineStr">
+      <c r="AS71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9178,7 +9512,13 @@
       <c r="AR72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS72" t="inlineStr">
+      <c r="AS72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9323,9 +9663,15 @@
       <c r="AR73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS73" t="inlineStr">
-        <is>
-          <t>2627</t>
+      <c r="AS73" t="n">
+        <v>2627</v>
+      </c>
+      <c r="AT73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU73" t="inlineStr">
+        <is>
+          <t>2664</t>
         </is>
       </c>
     </row>
@@ -9468,7 +9814,13 @@
       <c r="AR74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS74" t="inlineStr">
+      <c r="AS74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9613,7 +9965,13 @@
       <c r="AR75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS75" t="inlineStr">
+      <c r="AS75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9758,9 +10116,15 @@
       <c r="AR76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS76" t="inlineStr">
-        <is>
-          <t>2640</t>
+      <c r="AS76" t="n">
+        <v>2640</v>
+      </c>
+      <c r="AT76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU76" t="inlineStr">
+        <is>
+          <t>2639</t>
         </is>
       </c>
     </row>
@@ -9903,9 +10267,15 @@
       <c r="AR77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS77" t="inlineStr">
-        <is>
-          <t>2621</t>
+      <c r="AS77" t="n">
+        <v>2621</v>
+      </c>
+      <c r="AT77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU77" t="inlineStr">
+        <is>
+          <t>2616</t>
         </is>
       </c>
     </row>
@@ -10048,7 +10418,13 @@
       <c r="AR78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS78" t="inlineStr">
+      <c r="AS78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10193,7 +10569,13 @@
       <c r="AR79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS79" t="inlineStr">
+      <c r="AS79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10338,7 +10720,13 @@
       <c r="AR80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS80" t="inlineStr">
+      <c r="AS80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10483,7 +10871,13 @@
       <c r="AR81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS81" t="inlineStr">
+      <c r="AS81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10628,7 +11022,13 @@
       <c r="AR82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS82" t="inlineStr">
+      <c r="AS82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10773,7 +11173,13 @@
       <c r="AR83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS83" t="inlineStr">
+      <c r="AS83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10918,7 +11324,13 @@
       <c r="AR84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS84" t="inlineStr">
+      <c r="AS84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11063,7 +11475,13 @@
       <c r="AR85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS85" t="inlineStr">
+      <c r="AS85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11208,7 +11626,13 @@
       <c r="AR86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS86" t="inlineStr">
+      <c r="AS86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11353,7 +11777,13 @@
       <c r="AR87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS87" t="inlineStr">
+      <c r="AS87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11498,7 +11928,13 @@
       <c r="AR88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS88" t="inlineStr">
+      <c r="AS88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11643,7 +12079,13 @@
       <c r="AR89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS89" t="inlineStr">
+      <c r="AS89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11788,7 +12230,13 @@
       <c r="AR90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS90" t="inlineStr">
+      <c r="AS90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11933,7 +12381,13 @@
       <c r="AR91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS91" t="inlineStr">
+      <c r="AS91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12078,7 +12532,13 @@
       <c r="AR92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS92" t="inlineStr">
+      <c r="AS92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12223,7 +12683,13 @@
       <c r="AR93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS93" t="inlineStr">
+      <c r="AS93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12368,7 +12834,13 @@
       <c r="AR94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS94" t="inlineStr">
+      <c r="AS94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12513,7 +12985,13 @@
       <c r="AR95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS95" t="inlineStr">
+      <c r="AS95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12658,9 +13136,15 @@
       <c r="AR96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS96" t="inlineStr">
-        <is>
-          <t>2475</t>
+      <c r="AS96" t="n">
+        <v>2475</v>
+      </c>
+      <c r="AT96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU96" t="inlineStr">
+        <is>
+          <t>2473</t>
         </is>
       </c>
     </row>
@@ -12803,7 +13287,13 @@
       <c r="AR97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS97" t="inlineStr">
+      <c r="AS97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12948,7 +13438,13 @@
       <c r="AR98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS98" t="inlineStr">
+      <c r="AS98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13093,7 +13589,13 @@
       <c r="AR99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS99" t="inlineStr">
+      <c r="AS99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13238,7 +13740,13 @@
       <c r="AR100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS100" t="inlineStr">
+      <c r="AS100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13383,7 +13891,13 @@
       <c r="AR101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS101" t="inlineStr">
+      <c r="AS101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13528,7 +14042,13 @@
       <c r="AR102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS102" t="inlineStr">
+      <c r="AS102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13673,7 +14193,13 @@
       <c r="AR103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS103" t="inlineStr">
+      <c r="AS103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13818,7 +14344,13 @@
       <c r="AR104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS104" t="inlineStr">
+      <c r="AS104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13963,7 +14495,13 @@
       <c r="AR105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS105" t="inlineStr">
+      <c r="AS105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14027,6 +14565,8 @@
       <c r="AQ106" t="inlineStr"/>
       <c r="AR106" s="4" t="inlineStr"/>
       <c r="AS106" t="inlineStr"/>
+      <c r="AT106" s="4" t="inlineStr"/>
+      <c r="AU106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -14086,6 +14626,8 @@
       <c r="AQ107" t="inlineStr"/>
       <c r="AR107" s="4" t="inlineStr"/>
       <c r="AS107" t="inlineStr"/>
+      <c r="AT107" s="4" t="inlineStr"/>
+      <c r="AU107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -14145,6 +14687,8 @@
       <c r="AQ108" t="inlineStr"/>
       <c r="AR108" s="4" t="inlineStr"/>
       <c r="AS108" t="inlineStr"/>
+      <c r="AT108" s="4" t="inlineStr"/>
+      <c r="AU108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -14204,6 +14748,8 @@
       <c r="AQ109" t="inlineStr"/>
       <c r="AR109" s="4" t="inlineStr"/>
       <c r="AS109" t="inlineStr"/>
+      <c r="AT109" s="4" t="inlineStr"/>
+      <c r="AU109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -14263,6 +14809,8 @@
       <c r="AQ110" t="inlineStr"/>
       <c r="AR110" s="4" t="inlineStr"/>
       <c r="AS110" t="inlineStr"/>
+      <c r="AT110" s="4" t="inlineStr"/>
+      <c r="AU110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -14322,6 +14870,8 @@
       <c r="AQ111" t="inlineStr"/>
       <c r="AR111" s="4" t="inlineStr"/>
       <c r="AS111" t="inlineStr"/>
+      <c r="AT111" s="4" t="inlineStr"/>
+      <c r="AU111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -14381,6 +14931,8 @@
       <c r="AQ112" t="inlineStr"/>
       <c r="AR112" s="4" t="inlineStr"/>
       <c r="AS112" t="inlineStr"/>
+      <c r="AT112" s="4" t="inlineStr"/>
+      <c r="AU112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -14440,6 +14992,8 @@
       <c r="AQ113" t="inlineStr"/>
       <c r="AR113" s="4" t="inlineStr"/>
       <c r="AS113" t="inlineStr"/>
+      <c r="AT113" s="4" t="inlineStr"/>
+      <c r="AU113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -14499,6 +15053,8 @@
       <c r="AQ114" t="inlineStr"/>
       <c r="AR114" s="4" t="inlineStr"/>
       <c r="AS114" t="inlineStr"/>
+      <c r="AT114" s="4" t="inlineStr"/>
+      <c r="AU114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -14617,9 +15173,15 @@
       <c r="AR115" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AS115" t="inlineStr">
-        <is>
-          <t>4549</t>
+      <c r="AS115" t="n">
+        <v>4549</v>
+      </c>
+      <c r="AT115" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AU115" t="inlineStr">
+        <is>
+          <t>4829</t>
         </is>
       </c>
     </row>
@@ -14756,7 +15318,13 @@
       <c r="AR116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS116" t="inlineStr">
+      <c r="AS116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14863,9 +15431,15 @@
       <c r="AR117" s="5" t="n">
         <v>38</v>
       </c>
-      <c r="AS117" t="inlineStr">
-        <is>
-          <t>5169</t>
+      <c r="AS117" t="n">
+        <v>5169</v>
+      </c>
+      <c r="AT117" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU117" t="inlineStr">
+        <is>
+          <t>5453</t>
         </is>
       </c>
     </row>
@@ -15002,7 +15576,13 @@
       <c r="AR118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS118" t="inlineStr">
+      <c r="AS118" t="n">
+        <v>2747</v>
+      </c>
+      <c r="AT118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU118" t="inlineStr">
         <is>
           <t>2747</t>
         </is>
@@ -15141,9 +15721,15 @@
       <c r="AR119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS119" t="inlineStr">
-        <is>
-          <t>1518</t>
+      <c r="AS119" t="n">
+        <v>1518</v>
+      </c>
+      <c r="AT119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU119" t="inlineStr">
+        <is>
+          <t>1516</t>
         </is>
       </c>
     </row>
@@ -15280,7 +15866,13 @@
       <c r="AR120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS120" t="inlineStr">
+      <c r="AS120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU120" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15419,7 +16011,13 @@
       <c r="AR121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS121" t="inlineStr">
+      <c r="AS121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15558,7 +16156,13 @@
       <c r="AR122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS122" t="inlineStr">
+      <c r="AS122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15693,7 +16297,13 @@
       <c r="AR123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS123" t="inlineStr">
+      <c r="AS123" t="n">
+        <v>2579</v>
+      </c>
+      <c r="AT123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU123" t="inlineStr">
         <is>
           <t>2579</t>
         </is>
@@ -15783,6 +16393,8 @@
       <c r="AQ124" t="inlineStr"/>
       <c r="AR124" s="4" t="inlineStr"/>
       <c r="AS124" t="inlineStr"/>
+      <c r="AT124" s="4" t="inlineStr"/>
+      <c r="AU124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -15909,9 +16521,15 @@
       <c r="AR125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS125" t="inlineStr">
-        <is>
-          <t>2134</t>
+      <c r="AS125" t="n">
+        <v>2134</v>
+      </c>
+      <c r="AT125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU125" t="inlineStr">
+        <is>
+          <t>2133</t>
         </is>
       </c>
     </row>
@@ -16028,7 +16646,13 @@
       <c r="AR126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS126" t="inlineStr">
+      <c r="AS126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU126" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16110,6 +16734,8 @@
       <c r="AQ127" t="inlineStr"/>
       <c r="AR127" s="4" t="inlineStr"/>
       <c r="AS127" t="inlineStr"/>
+      <c r="AT127" s="4" t="inlineStr"/>
+      <c r="AU127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -16199,6 +16825,8 @@
       <c r="AQ128" t="inlineStr"/>
       <c r="AR128" s="4" t="inlineStr"/>
       <c r="AS128" t="inlineStr"/>
+      <c r="AT128" s="4" t="inlineStr"/>
+      <c r="AU128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -16305,9 +16933,15 @@
       <c r="AR129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS129" t="inlineStr">
-        <is>
-          <t>2528</t>
+      <c r="AS129" t="n">
+        <v>2528</v>
+      </c>
+      <c r="AT129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU129" t="inlineStr">
+        <is>
+          <t>2525</t>
         </is>
       </c>
     </row>
@@ -16399,6 +17033,8 @@
       <c r="AQ130" t="inlineStr"/>
       <c r="AR130" s="4" t="inlineStr"/>
       <c r="AS130" t="inlineStr"/>
+      <c r="AT130" s="4" t="inlineStr"/>
+      <c r="AU130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -16501,7 +17137,13 @@
       <c r="AR131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS131" t="inlineStr">
+      <c r="AS131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16596,9 +17238,15 @@
       <c r="AR132" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="AS132" t="inlineStr">
-        <is>
-          <t>3945</t>
+      <c r="AS132" t="n">
+        <v>3945</v>
+      </c>
+      <c r="AT132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU132" t="inlineStr">
+        <is>
+          <t>3979</t>
         </is>
       </c>
     </row>
@@ -16691,9 +17339,15 @@
       <c r="AR133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS133" t="inlineStr">
-        <is>
-          <t>2474</t>
+      <c r="AS133" t="n">
+        <v>2474</v>
+      </c>
+      <c r="AT133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU133" t="inlineStr">
+        <is>
+          <t>2469</t>
         </is>
       </c>
     </row>
@@ -16757,6 +17411,8 @@
       <c r="AQ134" t="inlineStr"/>
       <c r="AR134" s="4" t="inlineStr"/>
       <c r="AS134" t="inlineStr"/>
+      <c r="AT134" s="4" t="inlineStr"/>
+      <c r="AU134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -16822,6 +17478,8 @@
       <c r="AQ135" t="inlineStr"/>
       <c r="AR135" s="4" t="inlineStr"/>
       <c r="AS135" t="inlineStr"/>
+      <c r="AT135" s="4" t="inlineStr"/>
+      <c r="AU135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -16896,9 +17554,15 @@
       <c r="AR136" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AS136" t="inlineStr">
-        <is>
-          <t>5055</t>
+      <c r="AS136" t="n">
+        <v>5055</v>
+      </c>
+      <c r="AT136" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AU136" t="inlineStr">
+        <is>
+          <t>5441</t>
         </is>
       </c>
     </row>
@@ -16975,9 +17639,15 @@
       <c r="AR137" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AS137" t="inlineStr">
-        <is>
-          <t>4918</t>
+      <c r="AS137" t="n">
+        <v>4918</v>
+      </c>
+      <c r="AT137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU137" t="inlineStr">
+        <is>
+          <t>4904</t>
         </is>
       </c>
     </row>
@@ -17045,6 +17715,8 @@
       <c r="AQ138" t="inlineStr"/>
       <c r="AR138" s="4" t="inlineStr"/>
       <c r="AS138" t="inlineStr"/>
+      <c r="AT138" s="4" t="inlineStr"/>
+      <c r="AU138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -17119,9 +17791,15 @@
       <c r="AR139" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AS139" t="inlineStr">
-        <is>
-          <t>5186</t>
+      <c r="AS139" t="n">
+        <v>5186</v>
+      </c>
+      <c r="AT139" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AU139" t="inlineStr">
+        <is>
+          <t>5504</t>
         </is>
       </c>
     </row>
@@ -17198,9 +17876,15 @@
       <c r="AR140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS140" t="inlineStr">
-        <is>
-          <t>2007</t>
+      <c r="AS140" t="n">
+        <v>2007</v>
+      </c>
+      <c r="AT140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU140" t="inlineStr">
+        <is>
+          <t>2023</t>
         </is>
       </c>
     </row>
@@ -17264,6 +17948,8 @@
       <c r="AQ141" t="inlineStr"/>
       <c r="AR141" s="4" t="inlineStr"/>
       <c r="AS141" t="inlineStr"/>
+      <c r="AT141" s="4" t="inlineStr"/>
+      <c r="AU141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -17334,9 +18020,15 @@
       <c r="AR142" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="AS142" t="inlineStr">
-        <is>
-          <t>2833</t>
+      <c r="AS142" t="n">
+        <v>2833</v>
+      </c>
+      <c r="AT142" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="AU142" t="inlineStr">
+        <is>
+          <t>2927</t>
         </is>
       </c>
     </row>
@@ -17409,7 +18101,13 @@
       <c r="AR143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS143" t="inlineStr">
+      <c r="AS143" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17480,7 +18178,13 @@
       <c r="AR144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS144" t="inlineStr">
+      <c r="AS144" t="n">
+        <v>1511</v>
+      </c>
+      <c r="AT144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU144" t="inlineStr">
         <is>
           <t>1511</t>
         </is>
@@ -17551,9 +18255,15 @@
       <c r="AR145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS145" t="inlineStr">
-        <is>
-          <t>1806</t>
+      <c r="AS145" t="n">
+        <v>1806</v>
+      </c>
+      <c r="AT145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU145" t="inlineStr">
+        <is>
+          <t>1803</t>
         </is>
       </c>
     </row>
@@ -17622,7 +18332,13 @@
       <c r="AR146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS146" t="inlineStr">
+      <c r="AS146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17693,9 +18409,15 @@
       <c r="AR147" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AS147" t="inlineStr">
-        <is>
-          <t>4166</t>
+      <c r="AS147" t="n">
+        <v>4166</v>
+      </c>
+      <c r="AT147" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AU147" t="inlineStr">
+        <is>
+          <t>4352</t>
         </is>
       </c>
     </row>
@@ -17764,9 +18486,15 @@
       <c r="AR148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AS148" t="inlineStr">
-        <is>
-          <t>2001</t>
+      <c r="AS148" t="n">
+        <v>2001</v>
+      </c>
+      <c r="AT148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU148" t="inlineStr">
+        <is>
+          <t>1996</t>
         </is>
       </c>
     </row>
@@ -17831,11 +18559,11 @@
       <c r="AR149" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="AS149" t="inlineStr">
-        <is>
-          <t>5105</t>
-        </is>
-      </c>
+      <c r="AS149" t="n">
+        <v>5105</v>
+      </c>
+      <c r="AT149" s="4" t="inlineStr"/>
+      <c r="AU149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -17898,9 +18626,15 @@
       <c r="AR150" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AS150" t="inlineStr">
-        <is>
-          <t>3347</t>
+      <c r="AS150" t="n">
+        <v>3347</v>
+      </c>
+      <c r="AT150" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="AU150" t="inlineStr">
+        <is>
+          <t>3473</t>
         </is>
       </c>
     </row>
@@ -17965,9 +18699,15 @@
       <c r="AR151" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="AS151" t="inlineStr">
-        <is>
-          <t>2239</t>
+      <c r="AS151" t="n">
+        <v>2239</v>
+      </c>
+      <c r="AT151" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="AU151" t="inlineStr">
+        <is>
+          <t>2307</t>
         </is>
       </c>
     </row>
@@ -18028,9 +18768,82 @@
       <c r="AR152" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AS152" t="inlineStr">
-        <is>
-          <t>3724</t>
+      <c r="AS152" t="n">
+        <v>3724</v>
+      </c>
+      <c r="AT152" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AU152" t="inlineStr">
+        <is>
+          <t>3931</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>59540953</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>PreventiveGlimpse27</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr"/>
+      <c r="D153" t="inlineStr"/>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>三馆</t>
+        </is>
+      </c>
+      <c r="F153" s="4" t="inlineStr"/>
+      <c r="G153" t="inlineStr"/>
+      <c r="H153" s="4" t="inlineStr"/>
+      <c r="I153" t="inlineStr"/>
+      <c r="J153" s="4" t="inlineStr"/>
+      <c r="K153" t="inlineStr"/>
+      <c r="L153" s="4" t="inlineStr"/>
+      <c r="M153" t="inlineStr"/>
+      <c r="N153" s="4" t="inlineStr"/>
+      <c r="O153" t="inlineStr"/>
+      <c r="P153" s="4" t="inlineStr"/>
+      <c r="Q153" t="inlineStr"/>
+      <c r="R153" s="4" t="inlineStr"/>
+      <c r="S153" t="inlineStr"/>
+      <c r="T153" s="4" t="inlineStr"/>
+      <c r="U153" t="inlineStr"/>
+      <c r="V153" s="4" t="inlineStr"/>
+      <c r="W153" t="inlineStr"/>
+      <c r="X153" s="4" t="inlineStr"/>
+      <c r="Y153" t="inlineStr"/>
+      <c r="Z153" s="4" t="inlineStr"/>
+      <c r="AA153" t="inlineStr"/>
+      <c r="AB153" s="4" t="inlineStr"/>
+      <c r="AC153" t="inlineStr"/>
+      <c r="AD153" s="4" t="inlineStr"/>
+      <c r="AE153" t="inlineStr"/>
+      <c r="AF153" s="4" t="inlineStr"/>
+      <c r="AG153" t="inlineStr"/>
+      <c r="AH153" s="4" t="inlineStr"/>
+      <c r="AI153" t="inlineStr"/>
+      <c r="AJ153" s="4" t="inlineStr"/>
+      <c r="AK153" t="inlineStr"/>
+      <c r="AL153" s="4" t="inlineStr"/>
+      <c r="AM153" t="inlineStr"/>
+      <c r="AN153" s="4" t="inlineStr"/>
+      <c r="AO153" t="inlineStr"/>
+      <c r="AP153" s="4" t="inlineStr"/>
+      <c r="AQ153" t="inlineStr"/>
+      <c r="AR153" s="4" t="inlineStr"/>
+      <c r="AS153" t="inlineStr"/>
+      <c r="AT153" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AU153" t="inlineStr">
+        <is>
+          <t>1565</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-06-11 11:30:57
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -18781,10 +18781,8 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" t="inlineStr">
-        <is>
-          <t>59540953</t>
-        </is>
+      <c r="A153" t="n">
+        <v>59540953</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Code updated 23-06-12 06:47:35
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AU153"/>
+  <dimension ref="A1:AW153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -626,6 +626,16 @@
           <t>06-10_0</t>
         </is>
       </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>06-11_A</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>06-11_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -772,7 +782,13 @@
       <c r="AT2" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AU2" t="inlineStr">
+      <c r="AU2" t="n">
+        <v>4156</v>
+      </c>
+      <c r="AV2" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW2" t="inlineStr">
         <is>
           <t>4156</t>
         </is>
@@ -923,7 +939,13 @@
       <c r="AT3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU3" t="inlineStr">
+      <c r="AU3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1074,7 +1096,13 @@
       <c r="AT4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU4" t="inlineStr">
+      <c r="AU4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1225,7 +1253,13 @@
       <c r="AT5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU5" t="inlineStr">
+      <c r="AU5" t="n">
+        <v>2736</v>
+      </c>
+      <c r="AV5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW5" t="inlineStr">
         <is>
           <t>2736</t>
         </is>
@@ -1376,7 +1410,13 @@
       <c r="AT6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU6" t="inlineStr">
+      <c r="AU6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1442,6 +1482,8 @@
       <c r="AS7" t="inlineStr"/>
       <c r="AT7" s="4" t="inlineStr"/>
       <c r="AU7" t="inlineStr"/>
+      <c r="AV7" s="4" t="inlineStr"/>
+      <c r="AW7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1503,6 +1545,8 @@
       <c r="AS8" t="inlineStr"/>
       <c r="AT8" s="4" t="inlineStr"/>
       <c r="AU8" t="inlineStr"/>
+      <c r="AV8" s="4" t="inlineStr"/>
+      <c r="AW8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1564,6 +1608,8 @@
       <c r="AS9" t="inlineStr"/>
       <c r="AT9" s="4" t="inlineStr"/>
       <c r="AU9" t="inlineStr"/>
+      <c r="AV9" s="4" t="inlineStr"/>
+      <c r="AW9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1625,6 +1671,8 @@
       <c r="AS10" t="inlineStr"/>
       <c r="AT10" s="4" t="inlineStr"/>
       <c r="AU10" t="inlineStr"/>
+      <c r="AV10" s="4" t="inlineStr"/>
+      <c r="AW10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1686,6 +1734,8 @@
       <c r="AS11" t="inlineStr"/>
       <c r="AT11" s="4" t="inlineStr"/>
       <c r="AU11" t="inlineStr"/>
+      <c r="AV11" s="4" t="inlineStr"/>
+      <c r="AW11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1747,6 +1797,8 @@
       <c r="AS12" t="inlineStr"/>
       <c r="AT12" s="4" t="inlineStr"/>
       <c r="AU12" t="inlineStr"/>
+      <c r="AV12" s="4" t="inlineStr"/>
+      <c r="AW12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1808,6 +1860,8 @@
       <c r="AS13" t="inlineStr"/>
       <c r="AT13" s="4" t="inlineStr"/>
       <c r="AU13" t="inlineStr"/>
+      <c r="AV13" s="4" t="inlineStr"/>
+      <c r="AW13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1869,6 +1923,8 @@
       <c r="AS14" t="inlineStr"/>
       <c r="AT14" s="4" t="inlineStr"/>
       <c r="AU14" t="inlineStr"/>
+      <c r="AV14" s="4" t="inlineStr"/>
+      <c r="AW14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1930,6 +1986,8 @@
       <c r="AS15" t="inlineStr"/>
       <c r="AT15" s="4" t="inlineStr"/>
       <c r="AU15" t="inlineStr"/>
+      <c r="AV15" s="4" t="inlineStr"/>
+      <c r="AW15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1991,6 +2049,8 @@
       <c r="AS16" t="inlineStr"/>
       <c r="AT16" s="4" t="inlineStr"/>
       <c r="AU16" t="inlineStr"/>
+      <c r="AV16" s="4" t="inlineStr"/>
+      <c r="AW16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -2052,6 +2112,8 @@
       <c r="AS17" t="inlineStr"/>
       <c r="AT17" s="4" t="inlineStr"/>
       <c r="AU17" t="inlineStr"/>
+      <c r="AV17" s="4" t="inlineStr"/>
+      <c r="AW17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -2198,7 +2260,13 @@
       <c r="AT18" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="AU18" t="inlineStr">
+      <c r="AU18" t="n">
+        <v>3957</v>
+      </c>
+      <c r="AV18" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="AW18" t="inlineStr">
         <is>
           <t>3957</t>
         </is>
@@ -2349,7 +2417,13 @@
       <c r="AT19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU19" t="inlineStr">
+      <c r="AU19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW19" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2500,7 +2574,13 @@
       <c r="AT20" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AU20" t="inlineStr">
+      <c r="AU20" t="n">
+        <v>4090</v>
+      </c>
+      <c r="AV20" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW20" t="inlineStr">
         <is>
           <t>4090</t>
         </is>
@@ -2651,7 +2731,13 @@
       <c r="AT21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU21" t="inlineStr">
+      <c r="AU21" t="n">
+        <v>3035</v>
+      </c>
+      <c r="AV21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW21" t="inlineStr">
         <is>
           <t>3035</t>
         </is>
@@ -2802,7 +2888,13 @@
       <c r="AT22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AU22" t="inlineStr">
+      <c r="AU22" t="n">
+        <v>4495</v>
+      </c>
+      <c r="AV22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW22" t="inlineStr">
         <is>
           <t>4495</t>
         </is>
@@ -2953,7 +3045,13 @@
       <c r="AT23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AU23" t="inlineStr">
+      <c r="AU23" t="n">
+        <v>4883</v>
+      </c>
+      <c r="AV23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AW23" t="inlineStr">
         <is>
           <t>4883</t>
         </is>
@@ -3104,7 +3202,13 @@
       <c r="AT24" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AU24" t="inlineStr">
+      <c r="AU24" t="n">
+        <v>4376</v>
+      </c>
+      <c r="AV24" s="5" t="n">
+        <v>34</v>
+      </c>
+      <c r="AW24" t="inlineStr">
         <is>
           <t>4376</t>
         </is>
@@ -3234,6 +3338,8 @@
       <c r="AS25" t="inlineStr"/>
       <c r="AT25" s="4" t="inlineStr"/>
       <c r="AU25" t="inlineStr"/>
+      <c r="AV25" s="4" t="inlineStr"/>
+      <c r="AW25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -3347,6 +3453,8 @@
       <c r="AS26" t="inlineStr"/>
       <c r="AT26" s="4" t="inlineStr"/>
       <c r="AU26" t="inlineStr"/>
+      <c r="AV26" s="4" t="inlineStr"/>
+      <c r="AW26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -3493,7 +3601,13 @@
       <c r="AT27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU27" t="inlineStr">
+      <c r="AU27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3559,6 +3673,8 @@
       <c r="AS28" t="inlineStr"/>
       <c r="AT28" s="4" t="inlineStr"/>
       <c r="AU28" t="inlineStr"/>
+      <c r="AV28" s="4" t="inlineStr"/>
+      <c r="AW28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -3705,7 +3821,13 @@
       <c r="AT29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU29" t="inlineStr">
+      <c r="AU29" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AV29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW29" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3856,7 +3978,13 @@
       <c r="AT30" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AU30" t="inlineStr">
+      <c r="AU30" t="n">
+        <v>3939</v>
+      </c>
+      <c r="AV30" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AW30" t="inlineStr">
         <is>
           <t>3939</t>
         </is>
@@ -4007,7 +4135,13 @@
       <c r="AT31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AU31" t="inlineStr">
+      <c r="AU31" t="n">
+        <v>4506</v>
+      </c>
+      <c r="AV31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW31" t="inlineStr">
         <is>
           <t>4506</t>
         </is>
@@ -4158,7 +4292,13 @@
       <c r="AT32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU32" t="inlineStr">
+      <c r="AU32" t="n">
+        <v>2597</v>
+      </c>
+      <c r="AV32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW32" t="inlineStr">
         <is>
           <t>2597</t>
         </is>
@@ -4224,6 +4364,8 @@
       <c r="AS33" t="inlineStr"/>
       <c r="AT33" s="4" t="inlineStr"/>
       <c r="AU33" t="inlineStr"/>
+      <c r="AV33" s="4" t="inlineStr"/>
+      <c r="AW33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -4370,7 +4512,13 @@
       <c r="AT34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU34" t="inlineStr">
+      <c r="AU34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4521,7 +4669,13 @@
       <c r="AT35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU35" t="inlineStr">
+      <c r="AU35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW35" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4672,7 +4826,13 @@
       <c r="AT36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU36" t="inlineStr">
+      <c r="AU36" t="n">
+        <v>2932</v>
+      </c>
+      <c r="AV36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW36" t="inlineStr">
         <is>
           <t>2932</t>
         </is>
@@ -4810,6 +4970,8 @@
       <c r="AS37" t="inlineStr"/>
       <c r="AT37" s="4" t="inlineStr"/>
       <c r="AU37" t="inlineStr"/>
+      <c r="AV37" s="4" t="inlineStr"/>
+      <c r="AW37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -4956,7 +5118,13 @@
       <c r="AT38" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="AU38" t="inlineStr">
+      <c r="AU38" t="n">
+        <v>4656</v>
+      </c>
+      <c r="AV38" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AW38" t="inlineStr">
         <is>
           <t>4656</t>
         </is>
@@ -5107,7 +5275,13 @@
       <c r="AT39" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AU39" t="inlineStr">
+      <c r="AU39" t="n">
+        <v>4226</v>
+      </c>
+      <c r="AV39" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AW39" t="inlineStr">
         <is>
           <t>4226</t>
         </is>
@@ -5258,7 +5432,13 @@
       <c r="AT40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU40" t="inlineStr">
+      <c r="AU40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5409,7 +5589,13 @@
       <c r="AT41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU41" t="inlineStr">
+      <c r="AU41" t="n">
+        <v>3994</v>
+      </c>
+      <c r="AV41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW41" t="inlineStr">
         <is>
           <t>3994</t>
         </is>
@@ -5560,7 +5746,13 @@
       <c r="AT42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU42" t="inlineStr">
+      <c r="AU42" t="n">
+        <v>2768</v>
+      </c>
+      <c r="AV42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW42" t="inlineStr">
         <is>
           <t>2768</t>
         </is>
@@ -5626,6 +5818,8 @@
       <c r="AS43" t="inlineStr"/>
       <c r="AT43" s="4" t="inlineStr"/>
       <c r="AU43" t="inlineStr"/>
+      <c r="AV43" s="4" t="inlineStr"/>
+      <c r="AW43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -5687,6 +5881,8 @@
       <c r="AS44" t="inlineStr"/>
       <c r="AT44" s="4" t="inlineStr"/>
       <c r="AU44" t="inlineStr"/>
+      <c r="AV44" s="4" t="inlineStr"/>
+      <c r="AW44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -5780,6 +5976,8 @@
       <c r="AS45" t="inlineStr"/>
       <c r="AT45" s="4" t="inlineStr"/>
       <c r="AU45" t="inlineStr"/>
+      <c r="AV45" s="4" t="inlineStr"/>
+      <c r="AW45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -5926,7 +6124,13 @@
       <c r="AT46" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="AU46" t="inlineStr">
+      <c r="AU46" t="n">
+        <v>4126</v>
+      </c>
+      <c r="AV46" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AW46" t="inlineStr">
         <is>
           <t>4126</t>
         </is>
@@ -6077,7 +6281,13 @@
       <c r="AT47" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AU47" t="inlineStr">
+      <c r="AU47" t="n">
+        <v>4919</v>
+      </c>
+      <c r="AV47" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AW47" t="inlineStr">
         <is>
           <t>4919</t>
         </is>
@@ -6228,7 +6438,13 @@
       <c r="AT48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU48" t="inlineStr">
+      <c r="AU48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6379,7 +6595,13 @@
       <c r="AT49" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="AU49" t="inlineStr">
+      <c r="AU49" t="n">
+        <v>4375</v>
+      </c>
+      <c r="AV49" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="AW49" t="inlineStr">
         <is>
           <t>4375</t>
         </is>
@@ -6530,7 +6752,13 @@
       <c r="AT50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AU50" t="inlineStr">
+      <c r="AU50" t="n">
+        <v>4489</v>
+      </c>
+      <c r="AV50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AW50" t="inlineStr">
         <is>
           <t>4489</t>
         </is>
@@ -6628,6 +6856,8 @@
       <c r="AS51" t="inlineStr"/>
       <c r="AT51" s="4" t="inlineStr"/>
       <c r="AU51" t="inlineStr"/>
+      <c r="AV51" s="4" t="inlineStr"/>
+      <c r="AW51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -6774,7 +7004,13 @@
       <c r="AT52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AU52" t="inlineStr">
+      <c r="AU52" t="n">
+        <v>4627</v>
+      </c>
+      <c r="AV52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW52" t="inlineStr">
         <is>
           <t>4627</t>
         </is>
@@ -6925,7 +7161,13 @@
       <c r="AT53" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="AU53" t="inlineStr">
+      <c r="AU53" t="n">
+        <v>3290</v>
+      </c>
+      <c r="AV53" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AW53" t="inlineStr">
         <is>
           <t>3290</t>
         </is>
@@ -7023,6 +7265,8 @@
       <c r="AS54" t="inlineStr"/>
       <c r="AT54" s="4" t="inlineStr"/>
       <c r="AU54" t="inlineStr"/>
+      <c r="AV54" s="4" t="inlineStr"/>
+      <c r="AW54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -7169,7 +7413,13 @@
       <c r="AT55" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU55" t="inlineStr">
+      <c r="AU55" t="n">
+        <v>3432</v>
+      </c>
+      <c r="AV55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW55" t="inlineStr">
         <is>
           <t>3432</t>
         </is>
@@ -7320,7 +7570,13 @@
       <c r="AT56" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AU56" t="inlineStr">
+      <c r="AU56" t="n">
+        <v>4735</v>
+      </c>
+      <c r="AV56" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AW56" t="inlineStr">
         <is>
           <t>4735</t>
         </is>
@@ -7471,7 +7727,13 @@
       <c r="AT57" s="3" t="n">
         <v>19</v>
       </c>
-      <c r="AU57" t="inlineStr">
+      <c r="AU57" t="n">
+        <v>4050</v>
+      </c>
+      <c r="AV57" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="AW57" t="inlineStr">
         <is>
           <t>4050</t>
         </is>
@@ -7622,7 +7884,13 @@
       <c r="AT58" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AU58" t="inlineStr">
+      <c r="AU58" t="n">
+        <v>3995</v>
+      </c>
+      <c r="AV58" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AW58" t="inlineStr">
         <is>
           <t>3995</t>
         </is>
@@ -7773,7 +8041,13 @@
       <c r="AT59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AU59" t="inlineStr">
+      <c r="AU59" t="n">
+        <v>3994</v>
+      </c>
+      <c r="AV59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW59" t="inlineStr">
         <is>
           <t>3994</t>
         </is>
@@ -7924,7 +8198,13 @@
       <c r="AT60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AU60" t="inlineStr">
+      <c r="AU60" t="n">
+        <v>4149</v>
+      </c>
+      <c r="AV60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AW60" t="inlineStr">
         <is>
           <t>4149</t>
         </is>
@@ -7990,6 +8270,8 @@
       <c r="AS61" t="inlineStr"/>
       <c r="AT61" s="4" t="inlineStr"/>
       <c r="AU61" t="inlineStr"/>
+      <c r="AV61" s="4" t="inlineStr"/>
+      <c r="AW61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -8136,7 +8418,13 @@
       <c r="AT62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AU62" t="inlineStr">
+      <c r="AU62" t="n">
+        <v>3720</v>
+      </c>
+      <c r="AV62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW62" t="inlineStr">
         <is>
           <t>3720</t>
         </is>
@@ -8287,7 +8575,13 @@
       <c r="AT63" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AU63" t="inlineStr">
+      <c r="AU63" t="n">
+        <v>3885</v>
+      </c>
+      <c r="AV63" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW63" t="inlineStr">
         <is>
           <t>3885</t>
         </is>
@@ -8438,7 +8732,13 @@
       <c r="AT64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AU64" t="inlineStr">
+      <c r="AU64" t="n">
+        <v>4042</v>
+      </c>
+      <c r="AV64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW64" t="inlineStr">
         <is>
           <t>4042</t>
         </is>
@@ -8556,6 +8856,8 @@
       <c r="AS65" t="inlineStr"/>
       <c r="AT65" s="4" t="inlineStr"/>
       <c r="AU65" t="inlineStr"/>
+      <c r="AV65" s="4" t="inlineStr"/>
+      <c r="AW65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -8702,7 +9004,13 @@
       <c r="AT66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU66" t="inlineStr">
+      <c r="AU66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -8853,7 +9161,13 @@
       <c r="AT67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU67" t="inlineStr">
+      <c r="AU67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9004,7 +9318,13 @@
       <c r="AT68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU68" t="inlineStr">
+      <c r="AU68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9070,6 +9390,8 @@
       <c r="AS69" t="inlineStr"/>
       <c r="AT69" s="4" t="inlineStr"/>
       <c r="AU69" t="inlineStr"/>
+      <c r="AV69" s="4" t="inlineStr"/>
+      <c r="AW69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -9216,7 +9538,13 @@
       <c r="AT70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU70" t="inlineStr">
+      <c r="AU70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9367,7 +9695,13 @@
       <c r="AT71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU71" t="inlineStr">
+      <c r="AU71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9518,7 +9852,13 @@
       <c r="AT72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU72" t="inlineStr">
+      <c r="AU72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9669,7 +10009,13 @@
       <c r="AT73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU73" t="inlineStr">
+      <c r="AU73" t="n">
+        <v>2664</v>
+      </c>
+      <c r="AV73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW73" t="inlineStr">
         <is>
           <t>2664</t>
         </is>
@@ -9820,7 +10166,13 @@
       <c r="AT74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU74" t="inlineStr">
+      <c r="AU74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9971,7 +10323,13 @@
       <c r="AT75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU75" t="inlineStr">
+      <c r="AU75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10122,7 +10480,13 @@
       <c r="AT76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU76" t="inlineStr">
+      <c r="AU76" t="n">
+        <v>2639</v>
+      </c>
+      <c r="AV76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW76" t="inlineStr">
         <is>
           <t>2639</t>
         </is>
@@ -10273,7 +10637,13 @@
       <c r="AT77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU77" t="inlineStr">
+      <c r="AU77" t="n">
+        <v>2616</v>
+      </c>
+      <c r="AV77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW77" t="inlineStr">
         <is>
           <t>2616</t>
         </is>
@@ -10424,7 +10794,13 @@
       <c r="AT78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU78" t="inlineStr">
+      <c r="AU78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10575,7 +10951,13 @@
       <c r="AT79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU79" t="inlineStr">
+      <c r="AU79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10726,7 +11108,13 @@
       <c r="AT80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU80" t="inlineStr">
+      <c r="AU80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10877,7 +11265,13 @@
       <c r="AT81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU81" t="inlineStr">
+      <c r="AU81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11028,7 +11422,13 @@
       <c r="AT82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU82" t="inlineStr">
+      <c r="AU82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11179,7 +11579,13 @@
       <c r="AT83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU83" t="inlineStr">
+      <c r="AU83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11330,7 +11736,13 @@
       <c r="AT84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU84" t="inlineStr">
+      <c r="AU84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11481,7 +11893,13 @@
       <c r="AT85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU85" t="inlineStr">
+      <c r="AU85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11632,7 +12050,13 @@
       <c r="AT86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU86" t="inlineStr">
+      <c r="AU86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11783,7 +12207,13 @@
       <c r="AT87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU87" t="inlineStr">
+      <c r="AU87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11934,7 +12364,13 @@
       <c r="AT88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU88" t="inlineStr">
+      <c r="AU88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12085,7 +12521,13 @@
       <c r="AT89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU89" t="inlineStr">
+      <c r="AU89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12236,7 +12678,13 @@
       <c r="AT90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU90" t="inlineStr">
+      <c r="AU90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12387,7 +12835,13 @@
       <c r="AT91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU91" t="inlineStr">
+      <c r="AU91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12538,7 +12992,13 @@
       <c r="AT92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU92" t="inlineStr">
+      <c r="AU92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12689,7 +13149,13 @@
       <c r="AT93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU93" t="inlineStr">
+      <c r="AU93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12840,7 +13306,13 @@
       <c r="AT94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU94" t="inlineStr">
+      <c r="AU94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12991,7 +13463,13 @@
       <c r="AT95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU95" t="inlineStr">
+      <c r="AU95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13142,7 +13620,13 @@
       <c r="AT96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU96" t="inlineStr">
+      <c r="AU96" t="n">
+        <v>2473</v>
+      </c>
+      <c r="AV96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW96" t="inlineStr">
         <is>
           <t>2473</t>
         </is>
@@ -13293,7 +13777,13 @@
       <c r="AT97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU97" t="inlineStr">
+      <c r="AU97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13444,7 +13934,13 @@
       <c r="AT98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU98" t="inlineStr">
+      <c r="AU98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13595,7 +14091,13 @@
       <c r="AT99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU99" t="inlineStr">
+      <c r="AU99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13746,7 +14248,13 @@
       <c r="AT100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU100" t="inlineStr">
+      <c r="AU100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13897,7 +14405,13 @@
       <c r="AT101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU101" t="inlineStr">
+      <c r="AU101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14048,7 +14562,13 @@
       <c r="AT102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU102" t="inlineStr">
+      <c r="AU102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14199,7 +14719,13 @@
       <c r="AT103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU103" t="inlineStr">
+      <c r="AU103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14350,7 +14876,13 @@
       <c r="AT104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU104" t="inlineStr">
+      <c r="AU104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14501,7 +15033,13 @@
       <c r="AT105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU105" t="inlineStr">
+      <c r="AU105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14567,6 +15105,8 @@
       <c r="AS106" t="inlineStr"/>
       <c r="AT106" s="4" t="inlineStr"/>
       <c r="AU106" t="inlineStr"/>
+      <c r="AV106" s="4" t="inlineStr"/>
+      <c r="AW106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -14628,6 +15168,8 @@
       <c r="AS107" t="inlineStr"/>
       <c r="AT107" s="4" t="inlineStr"/>
       <c r="AU107" t="inlineStr"/>
+      <c r="AV107" s="4" t="inlineStr"/>
+      <c r="AW107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -14689,6 +15231,8 @@
       <c r="AS108" t="inlineStr"/>
       <c r="AT108" s="4" t="inlineStr"/>
       <c r="AU108" t="inlineStr"/>
+      <c r="AV108" s="4" t="inlineStr"/>
+      <c r="AW108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -14750,6 +15294,8 @@
       <c r="AS109" t="inlineStr"/>
       <c r="AT109" s="4" t="inlineStr"/>
       <c r="AU109" t="inlineStr"/>
+      <c r="AV109" s="4" t="inlineStr"/>
+      <c r="AW109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -14811,6 +15357,8 @@
       <c r="AS110" t="inlineStr"/>
       <c r="AT110" s="4" t="inlineStr"/>
       <c r="AU110" t="inlineStr"/>
+      <c r="AV110" s="4" t="inlineStr"/>
+      <c r="AW110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -14872,6 +15420,8 @@
       <c r="AS111" t="inlineStr"/>
       <c r="AT111" s="4" t="inlineStr"/>
       <c r="AU111" t="inlineStr"/>
+      <c r="AV111" s="4" t="inlineStr"/>
+      <c r="AW111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -14933,6 +15483,8 @@
       <c r="AS112" t="inlineStr"/>
       <c r="AT112" s="4" t="inlineStr"/>
       <c r="AU112" t="inlineStr"/>
+      <c r="AV112" s="4" t="inlineStr"/>
+      <c r="AW112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -14994,6 +15546,8 @@
       <c r="AS113" t="inlineStr"/>
       <c r="AT113" s="4" t="inlineStr"/>
       <c r="AU113" t="inlineStr"/>
+      <c r="AV113" s="4" t="inlineStr"/>
+      <c r="AW113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -15055,6 +15609,8 @@
       <c r="AS114" t="inlineStr"/>
       <c r="AT114" s="4" t="inlineStr"/>
       <c r="AU114" t="inlineStr"/>
+      <c r="AV114" s="4" t="inlineStr"/>
+      <c r="AW114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -15179,7 +15735,13 @@
       <c r="AT115" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AU115" t="inlineStr">
+      <c r="AU115" t="n">
+        <v>4829</v>
+      </c>
+      <c r="AV115" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AW115" t="inlineStr">
         <is>
           <t>4829</t>
         </is>
@@ -15324,7 +15886,13 @@
       <c r="AT116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU116" t="inlineStr">
+      <c r="AU116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15437,7 +16005,13 @@
       <c r="AT117" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AU117" t="inlineStr">
+      <c r="AU117" t="n">
+        <v>5453</v>
+      </c>
+      <c r="AV117" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW117" t="inlineStr">
         <is>
           <t>5453</t>
         </is>
@@ -15582,7 +16156,13 @@
       <c r="AT118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU118" t="inlineStr">
+      <c r="AU118" t="n">
+        <v>2747</v>
+      </c>
+      <c r="AV118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW118" t="inlineStr">
         <is>
           <t>2747</t>
         </is>
@@ -15727,7 +16307,13 @@
       <c r="AT119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU119" t="inlineStr">
+      <c r="AU119" t="n">
+        <v>1516</v>
+      </c>
+      <c r="AV119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW119" t="inlineStr">
         <is>
           <t>1516</t>
         </is>
@@ -15872,7 +16458,13 @@
       <c r="AT120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU120" t="inlineStr">
+      <c r="AU120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW120" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16017,7 +16609,13 @@
       <c r="AT121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU121" t="inlineStr">
+      <c r="AU121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16162,7 +16760,13 @@
       <c r="AT122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU122" t="inlineStr">
+      <c r="AU122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16303,7 +16907,13 @@
       <c r="AT123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU123" t="inlineStr">
+      <c r="AU123" t="n">
+        <v>2579</v>
+      </c>
+      <c r="AV123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW123" t="inlineStr">
         <is>
           <t>2579</t>
         </is>
@@ -16395,6 +17005,8 @@
       <c r="AS124" t="inlineStr"/>
       <c r="AT124" s="4" t="inlineStr"/>
       <c r="AU124" t="inlineStr"/>
+      <c r="AV124" s="4" t="inlineStr"/>
+      <c r="AW124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -16527,7 +17139,13 @@
       <c r="AT125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU125" t="inlineStr">
+      <c r="AU125" t="n">
+        <v>2133</v>
+      </c>
+      <c r="AV125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW125" t="inlineStr">
         <is>
           <t>2133</t>
         </is>
@@ -16652,7 +17270,13 @@
       <c r="AT126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU126" t="inlineStr">
+      <c r="AU126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW126" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16736,6 +17360,8 @@
       <c r="AS127" t="inlineStr"/>
       <c r="AT127" s="4" t="inlineStr"/>
       <c r="AU127" t="inlineStr"/>
+      <c r="AV127" s="4" t="inlineStr"/>
+      <c r="AW127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -16827,6 +17453,8 @@
       <c r="AS128" t="inlineStr"/>
       <c r="AT128" s="4" t="inlineStr"/>
       <c r="AU128" t="inlineStr"/>
+      <c r="AV128" s="4" t="inlineStr"/>
+      <c r="AW128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -16939,7 +17567,13 @@
       <c r="AT129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU129" t="inlineStr">
+      <c r="AU129" t="n">
+        <v>2525</v>
+      </c>
+      <c r="AV129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW129" t="inlineStr">
         <is>
           <t>2525</t>
         </is>
@@ -17035,6 +17669,8 @@
       <c r="AS130" t="inlineStr"/>
       <c r="AT130" s="4" t="inlineStr"/>
       <c r="AU130" t="inlineStr"/>
+      <c r="AV130" s="4" t="inlineStr"/>
+      <c r="AW130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -17143,7 +17779,13 @@
       <c r="AT131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU131" t="inlineStr">
+      <c r="AU131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17244,7 +17886,13 @@
       <c r="AT132" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU132" t="inlineStr">
+      <c r="AU132" t="n">
+        <v>3979</v>
+      </c>
+      <c r="AV132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW132" t="inlineStr">
         <is>
           <t>3979</t>
         </is>
@@ -17345,7 +17993,13 @@
       <c r="AT133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU133" t="inlineStr">
+      <c r="AU133" t="n">
+        <v>2469</v>
+      </c>
+      <c r="AV133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW133" t="inlineStr">
         <is>
           <t>2469</t>
         </is>
@@ -17413,6 +18067,8 @@
       <c r="AS134" t="inlineStr"/>
       <c r="AT134" s="4" t="inlineStr"/>
       <c r="AU134" t="inlineStr"/>
+      <c r="AV134" s="4" t="inlineStr"/>
+      <c r="AW134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -17480,6 +18136,8 @@
       <c r="AS135" t="inlineStr"/>
       <c r="AT135" s="4" t="inlineStr"/>
       <c r="AU135" t="inlineStr"/>
+      <c r="AV135" s="4" t="inlineStr"/>
+      <c r="AW135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -17560,7 +18218,13 @@
       <c r="AT136" s="5" t="n">
         <v>35</v>
       </c>
-      <c r="AU136" t="inlineStr">
+      <c r="AU136" t="n">
+        <v>5441</v>
+      </c>
+      <c r="AV136" s="5" t="n">
+        <v>35</v>
+      </c>
+      <c r="AW136" t="inlineStr">
         <is>
           <t>5441</t>
         </is>
@@ -17645,7 +18309,13 @@
       <c r="AT137" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU137" t="inlineStr">
+      <c r="AU137" t="n">
+        <v>4904</v>
+      </c>
+      <c r="AV137" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW137" t="inlineStr">
         <is>
           <t>4904</t>
         </is>
@@ -17717,6 +18387,8 @@
       <c r="AS138" t="inlineStr"/>
       <c r="AT138" s="4" t="inlineStr"/>
       <c r="AU138" t="inlineStr"/>
+      <c r="AV138" s="4" t="inlineStr"/>
+      <c r="AW138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -17797,7 +18469,13 @@
       <c r="AT139" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AU139" t="inlineStr">
+      <c r="AU139" t="n">
+        <v>5504</v>
+      </c>
+      <c r="AV139" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AW139" t="inlineStr">
         <is>
           <t>5504</t>
         </is>
@@ -17882,7 +18560,13 @@
       <c r="AT140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU140" t="inlineStr">
+      <c r="AU140" t="n">
+        <v>2023</v>
+      </c>
+      <c r="AV140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW140" t="inlineStr">
         <is>
           <t>2023</t>
         </is>
@@ -17950,6 +18634,8 @@
       <c r="AS141" t="inlineStr"/>
       <c r="AT141" s="4" t="inlineStr"/>
       <c r="AU141" t="inlineStr"/>
+      <c r="AV141" s="4" t="inlineStr"/>
+      <c r="AW141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -18026,7 +18712,13 @@
       <c r="AT142" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="AU142" t="inlineStr">
+      <c r="AU142" t="n">
+        <v>2927</v>
+      </c>
+      <c r="AV142" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="AW142" t="inlineStr">
         <is>
           <t>2927</t>
         </is>
@@ -18107,7 +18799,13 @@
       <c r="AT143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU143" t="inlineStr">
+      <c r="AU143" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18184,7 +18882,13 @@
       <c r="AT144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU144" t="inlineStr">
+      <c r="AU144" t="n">
+        <v>1511</v>
+      </c>
+      <c r="AV144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW144" t="inlineStr">
         <is>
           <t>1511</t>
         </is>
@@ -18261,7 +18965,13 @@
       <c r="AT145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU145" t="inlineStr">
+      <c r="AU145" t="n">
+        <v>1803</v>
+      </c>
+      <c r="AV145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW145" t="inlineStr">
         <is>
           <t>1803</t>
         </is>
@@ -18338,7 +19048,13 @@
       <c r="AT146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU146" t="inlineStr">
+      <c r="AU146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18415,7 +19131,13 @@
       <c r="AT147" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AU147" t="inlineStr">
+      <c r="AU147" t="n">
+        <v>4352</v>
+      </c>
+      <c r="AV147" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AW147" t="inlineStr">
         <is>
           <t>4352</t>
         </is>
@@ -18492,7 +19214,13 @@
       <c r="AT148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AU148" t="inlineStr">
+      <c r="AU148" t="n">
+        <v>1996</v>
+      </c>
+      <c r="AV148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW148" t="inlineStr">
         <is>
           <t>1996</t>
         </is>
@@ -18564,6 +19292,8 @@
       </c>
       <c r="AT149" s="4" t="inlineStr"/>
       <c r="AU149" t="inlineStr"/>
+      <c r="AV149" s="4" t="inlineStr"/>
+      <c r="AW149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -18632,7 +19362,13 @@
       <c r="AT150" s="4" t="n">
         <v>26</v>
       </c>
-      <c r="AU150" t="inlineStr">
+      <c r="AU150" t="n">
+        <v>3473</v>
+      </c>
+      <c r="AV150" s="4" t="n">
+        <v>26</v>
+      </c>
+      <c r="AW150" t="inlineStr">
         <is>
           <t>3473</t>
         </is>
@@ -18705,7 +19441,13 @@
       <c r="AT151" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="AU151" t="inlineStr">
+      <c r="AU151" t="n">
+        <v>2307</v>
+      </c>
+      <c r="AV151" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="AW151" t="inlineStr">
         <is>
           <t>2307</t>
         </is>
@@ -18774,7 +19516,13 @@
       <c r="AT152" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AU152" t="inlineStr">
+      <c r="AU152" t="n">
+        <v>3931</v>
+      </c>
+      <c r="AV152" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AW152" t="inlineStr">
         <is>
           <t>3931</t>
         </is>
@@ -18839,7 +19587,13 @@
       <c r="AT153" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AU153" t="inlineStr">
+      <c r="AU153" t="n">
+        <v>1565</v>
+      </c>
+      <c r="AV153" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AW153" t="inlineStr">
         <is>
           <t>1565</t>
         </is>

</xml_diff>

<commit_message>
Code updated 23-06-12 11:30:49
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -785,12 +785,12 @@
       <c r="AU2" t="n">
         <v>4156</v>
       </c>
-      <c r="AV2" s="4" t="n">
-        <v>20</v>
+      <c r="AV2" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AW2" t="inlineStr">
         <is>
-          <t>4156</t>
+          <t>4152</t>
         </is>
       </c>
     </row>
@@ -1261,7 +1261,7 @@
       </c>
       <c r="AW5" t="inlineStr">
         <is>
-          <t>2736</t>
+          <t>2751</t>
         </is>
       </c>
     </row>
@@ -2264,11 +2264,11 @@
         <v>3957</v>
       </c>
       <c r="AV18" s="3" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AW18" t="inlineStr">
         <is>
-          <t>3957</t>
+          <t>3989</t>
         </is>
       </c>
     </row>
@@ -2577,12 +2577,12 @@
       <c r="AU20" t="n">
         <v>4090</v>
       </c>
-      <c r="AV20" s="4" t="n">
-        <v>20</v>
+      <c r="AV20" s="3" t="n">
+        <v>16</v>
       </c>
       <c r="AW20" t="inlineStr">
         <is>
-          <t>4090</t>
+          <t>4140</t>
         </is>
       </c>
     </row>
@@ -2739,7 +2739,7 @@
       </c>
       <c r="AW21" t="inlineStr">
         <is>
-          <t>3035</t>
+          <t>3137</t>
         </is>
       </c>
     </row>
@@ -2896,7 +2896,7 @@
       </c>
       <c r="AW22" t="inlineStr">
         <is>
-          <t>4495</t>
+          <t>4676</t>
         </is>
       </c>
     </row>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="AW23" t="inlineStr">
         <is>
-          <t>4883</t>
+          <t>5144</t>
         </is>
       </c>
     </row>
@@ -3206,11 +3206,11 @@
         <v>4376</v>
       </c>
       <c r="AV24" s="5" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AW24" t="inlineStr">
         <is>
-          <t>4376</t>
+          <t>4601</t>
         </is>
       </c>
     </row>
@@ -3982,11 +3982,11 @@
         <v>3939</v>
       </c>
       <c r="AV30" s="4" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AW30" t="inlineStr">
         <is>
-          <t>3939</t>
+          <t>4269</t>
         </is>
       </c>
     </row>
@@ -4138,12 +4138,12 @@
       <c r="AU31" t="n">
         <v>4506</v>
       </c>
-      <c r="AV31" s="4" t="n">
-        <v>30</v>
+      <c r="AV31" s="5" t="n">
+        <v>31</v>
       </c>
       <c r="AW31" t="inlineStr">
         <is>
-          <t>4506</t>
+          <t>4667</t>
         </is>
       </c>
     </row>
@@ -4300,7 +4300,7 @@
       </c>
       <c r="AW32" t="inlineStr">
         <is>
-          <t>2597</t>
+          <t>2624</t>
         </is>
       </c>
     </row>
@@ -4834,7 +4834,7 @@
       </c>
       <c r="AW36" t="inlineStr">
         <is>
-          <t>2932</t>
+          <t>3009</t>
         </is>
       </c>
     </row>
@@ -5121,12 +5121,12 @@
       <c r="AU38" t="n">
         <v>4656</v>
       </c>
-      <c r="AV38" s="4" t="n">
-        <v>22</v>
+      <c r="AV38" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AW38" t="inlineStr">
         <is>
-          <t>4656</t>
+          <t>4676</t>
         </is>
       </c>
     </row>
@@ -5283,7 +5283,7 @@
       </c>
       <c r="AW39" t="inlineStr">
         <is>
-          <t>4226</t>
+          <t>4383</t>
         </is>
       </c>
     </row>
@@ -5597,7 +5597,7 @@
       </c>
       <c r="AW41" t="inlineStr">
         <is>
-          <t>3994</t>
+          <t>4169</t>
         </is>
       </c>
     </row>
@@ -5754,7 +5754,7 @@
       </c>
       <c r="AW42" t="inlineStr">
         <is>
-          <t>2768</t>
+          <t>2819</t>
         </is>
       </c>
     </row>
@@ -6128,11 +6128,11 @@
         <v>4126</v>
       </c>
       <c r="AV46" s="3" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AW46" t="inlineStr">
         <is>
-          <t>4126</t>
+          <t>4170</t>
         </is>
       </c>
     </row>
@@ -6284,12 +6284,12 @@
       <c r="AU47" t="n">
         <v>4919</v>
       </c>
-      <c r="AV47" s="5" t="n">
-        <v>32</v>
+      <c r="AV47" s="4" t="n">
+        <v>30</v>
       </c>
       <c r="AW47" t="inlineStr">
         <is>
-          <t>4919</t>
+          <t>4994</t>
         </is>
       </c>
     </row>
@@ -6599,11 +6599,11 @@
         <v>4375</v>
       </c>
       <c r="AV49" s="4" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AW49" t="inlineStr">
         <is>
-          <t>4375</t>
+          <t>4612</t>
         </is>
       </c>
     </row>
@@ -6756,11 +6756,11 @@
         <v>4489</v>
       </c>
       <c r="AV50" s="4" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AW50" t="inlineStr">
         <is>
-          <t>4489</t>
+          <t>4712</t>
         </is>
       </c>
     </row>
@@ -7012,7 +7012,7 @@
       </c>
       <c r="AW52" t="inlineStr">
         <is>
-          <t>4627</t>
+          <t>4746</t>
         </is>
       </c>
     </row>
@@ -7164,12 +7164,12 @@
       <c r="AU53" t="n">
         <v>3290</v>
       </c>
-      <c r="AV53" s="3" t="n">
-        <v>8</v>
+      <c r="AV53" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AW53" t="inlineStr">
         <is>
-          <t>3290</t>
+          <t>3336</t>
         </is>
       </c>
     </row>
@@ -7421,7 +7421,7 @@
       </c>
       <c r="AW55" t="inlineStr">
         <is>
-          <t>3432</t>
+          <t>3458</t>
         </is>
       </c>
     </row>
@@ -7574,11 +7574,11 @@
         <v>4735</v>
       </c>
       <c r="AV56" s="4" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AW56" t="inlineStr">
         <is>
-          <t>4735</t>
+          <t>5008</t>
         </is>
       </c>
     </row>
@@ -7730,12 +7730,12 @@
       <c r="AU57" t="n">
         <v>4050</v>
       </c>
-      <c r="AV57" s="3" t="n">
-        <v>19</v>
+      <c r="AV57" s="4" t="n">
+        <v>20</v>
       </c>
       <c r="AW57" t="inlineStr">
         <is>
-          <t>4050</t>
+          <t>4098</t>
         </is>
       </c>
     </row>
@@ -7892,7 +7892,7 @@
       </c>
       <c r="AW58" t="inlineStr">
         <is>
-          <t>3995</t>
+          <t>4085</t>
         </is>
       </c>
     </row>
@@ -8044,12 +8044,12 @@
       <c r="AU59" t="n">
         <v>3994</v>
       </c>
-      <c r="AV59" s="4" t="n">
-        <v>20</v>
+      <c r="AV59" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AW59" t="inlineStr">
         <is>
-          <t>3994</t>
+          <t>3988</t>
         </is>
       </c>
     </row>
@@ -8206,7 +8206,7 @@
       </c>
       <c r="AW60" t="inlineStr">
         <is>
-          <t>4149</t>
+          <t>4193</t>
         </is>
       </c>
     </row>
@@ -8426,7 +8426,7 @@
       </c>
       <c r="AW62" t="inlineStr">
         <is>
-          <t>3720</t>
+          <t>3913</t>
         </is>
       </c>
     </row>
@@ -8578,12 +8578,12 @@
       <c r="AU63" t="n">
         <v>3885</v>
       </c>
-      <c r="AV63" s="4" t="n">
-        <v>20</v>
+      <c r="AV63" s="3" t="n">
+        <v>17</v>
       </c>
       <c r="AW63" t="inlineStr">
         <is>
-          <t>3885</t>
+          <t>3985</t>
         </is>
       </c>
     </row>
@@ -8740,7 +8740,7 @@
       </c>
       <c r="AW64" t="inlineStr">
         <is>
-          <t>4042</t>
+          <t>4181</t>
         </is>
       </c>
     </row>
@@ -10017,7 +10017,7 @@
       </c>
       <c r="AW73" t="inlineStr">
         <is>
-          <t>2664</t>
+          <t>2656</t>
         </is>
       </c>
     </row>
@@ -10488,7 +10488,7 @@
       </c>
       <c r="AW76" t="inlineStr">
         <is>
-          <t>2639</t>
+          <t>2636</t>
         </is>
       </c>
     </row>
@@ -10645,7 +10645,7 @@
       </c>
       <c r="AW77" t="inlineStr">
         <is>
-          <t>2616</t>
+          <t>2612</t>
         </is>
       </c>
     </row>
@@ -13628,7 +13628,7 @@
       </c>
       <c r="AW96" t="inlineStr">
         <is>
-          <t>2473</t>
+          <t>2470</t>
         </is>
       </c>
     </row>
@@ -15743,7 +15743,7 @@
       </c>
       <c r="AW115" t="inlineStr">
         <is>
-          <t>4829</t>
+          <t>5053</t>
         </is>
       </c>
     </row>
@@ -16008,12 +16008,12 @@
       <c r="AU117" t="n">
         <v>5453</v>
       </c>
-      <c r="AV117" s="4" t="n">
-        <v>20</v>
+      <c r="AV117" s="5" t="n">
+        <v>33</v>
       </c>
       <c r="AW117" t="inlineStr">
         <is>
-          <t>5453</t>
+          <t>5917</t>
         </is>
       </c>
     </row>
@@ -16159,12 +16159,12 @@
       <c r="AU118" t="n">
         <v>2747</v>
       </c>
-      <c r="AV118" s="2" t="n">
-        <v>0</v>
+      <c r="AV118" s="4" t="n">
+        <v>20</v>
       </c>
       <c r="AW118" t="inlineStr">
         <is>
-          <t>2747</t>
+          <t>3233</t>
         </is>
       </c>
     </row>
@@ -16315,7 +16315,7 @@
       </c>
       <c r="AW119" t="inlineStr">
         <is>
-          <t>1516</t>
+          <t>1530</t>
         </is>
       </c>
     </row>
@@ -17147,7 +17147,7 @@
       </c>
       <c r="AW125" t="inlineStr">
         <is>
-          <t>2133</t>
+          <t>2148</t>
         </is>
       </c>
     </row>
@@ -17575,7 +17575,7 @@
       </c>
       <c r="AW129" t="inlineStr">
         <is>
-          <t>2525</t>
+          <t>2538</t>
         </is>
       </c>
     </row>
@@ -17889,12 +17889,12 @@
       <c r="AU132" t="n">
         <v>3979</v>
       </c>
-      <c r="AV132" s="2" t="n">
-        <v>0</v>
+      <c r="AV132" s="3" t="n">
+        <v>8</v>
       </c>
       <c r="AW132" t="inlineStr">
         <is>
-          <t>3979</t>
+          <t>4095</t>
         </is>
       </c>
     </row>
@@ -18001,7 +18001,7 @@
       </c>
       <c r="AW133" t="inlineStr">
         <is>
-          <t>2469</t>
+          <t>2481</t>
         </is>
       </c>
     </row>
@@ -18222,11 +18222,11 @@
         <v>5441</v>
       </c>
       <c r="AV136" s="5" t="n">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="AW136" t="inlineStr">
         <is>
-          <t>5441</t>
+          <t>5865</t>
         </is>
       </c>
     </row>
@@ -18236,7 +18236,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>"Cry ab it林黛玉ᶻᵍˣ"</t>
+          <t>"L ᶻᵍˣ"</t>
         </is>
       </c>
       <c r="C137" t="inlineStr"/>
@@ -18312,12 +18312,12 @@
       <c r="AU137" t="n">
         <v>4904</v>
       </c>
-      <c r="AV137" s="2" t="n">
-        <v>0</v>
+      <c r="AV137" s="4" t="n">
+        <v>30</v>
       </c>
       <c r="AW137" t="inlineStr">
         <is>
-          <t>4904</t>
+          <t>5409</t>
         </is>
       </c>
     </row>
@@ -18473,11 +18473,11 @@
         <v>5504</v>
       </c>
       <c r="AV139" s="5" t="n">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AW139" t="inlineStr">
         <is>
-          <t>5504</t>
+          <t>5845</t>
         </is>
       </c>
     </row>
@@ -18568,7 +18568,7 @@
       </c>
       <c r="AW140" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>2038</t>
         </is>
       </c>
     </row>
@@ -18715,12 +18715,12 @@
       <c r="AU142" t="n">
         <v>2927</v>
       </c>
-      <c r="AV142" s="3" t="n">
-        <v>16</v>
+      <c r="AV142" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AW142" t="inlineStr">
         <is>
-          <t>2927</t>
+          <t>2924</t>
         </is>
       </c>
     </row>
@@ -18885,12 +18885,12 @@
       <c r="AU144" t="n">
         <v>1511</v>
       </c>
-      <c r="AV144" s="2" t="n">
-        <v>0</v>
+      <c r="AV144" s="3" t="n">
+        <v>6</v>
       </c>
       <c r="AW144" t="inlineStr">
         <is>
-          <t>1511</t>
+          <t>1621</t>
         </is>
       </c>
     </row>
@@ -18973,7 +18973,7 @@
       </c>
       <c r="AW145" t="inlineStr">
         <is>
-          <t>1803</t>
+          <t>1801</t>
         </is>
       </c>
     </row>
@@ -19139,7 +19139,7 @@
       </c>
       <c r="AW147" t="inlineStr">
         <is>
-          <t>4352</t>
+          <t>4483</t>
         </is>
       </c>
     </row>
@@ -19222,7 +19222,7 @@
       </c>
       <c r="AW148" t="inlineStr">
         <is>
-          <t>1996</t>
+          <t>2007</t>
         </is>
       </c>
     </row>
@@ -19365,12 +19365,12 @@
       <c r="AU150" t="n">
         <v>3473</v>
       </c>
-      <c r="AV150" s="4" t="n">
-        <v>26</v>
+      <c r="AV150" s="3" t="n">
+        <v>13</v>
       </c>
       <c r="AW150" t="inlineStr">
         <is>
-          <t>3473</t>
+          <t>3514</t>
         </is>
       </c>
     </row>
@@ -19444,12 +19444,12 @@
       <c r="AU151" t="n">
         <v>2307</v>
       </c>
-      <c r="AV151" s="3" t="n">
-        <v>12</v>
+      <c r="AV151" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="AW151" t="inlineStr">
         <is>
-          <t>2307</t>
+          <t>2296</t>
         </is>
       </c>
     </row>
@@ -19519,12 +19519,12 @@
       <c r="AU152" t="n">
         <v>3931</v>
       </c>
-      <c r="AV152" s="4" t="n">
-        <v>21</v>
+      <c r="AV152" s="3" t="n">
+        <v>7</v>
       </c>
       <c r="AW152" t="inlineStr">
         <is>
-          <t>3931</t>
+          <t>3975</t>
         </is>
       </c>
     </row>
@@ -19595,7 +19595,7 @@
       </c>
       <c r="AW153" t="inlineStr">
         <is>
-          <t>1565</t>
+          <t>1823</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-06-13 11:30:55
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AW153"/>
+  <dimension ref="A1:AY154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -636,6 +636,16 @@
           <t>06-11_0</t>
         </is>
       </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>06-12_A</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>06-12_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -788,9 +798,15 @@
       <c r="AV2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW2" t="inlineStr">
-        <is>
-          <t>4152</t>
+      <c r="AW2" t="n">
+        <v>4152</v>
+      </c>
+      <c r="AX2" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AY2" t="inlineStr">
+        <is>
+          <t>4580</t>
         </is>
       </c>
     </row>
@@ -945,7 +961,13 @@
       <c r="AV3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW3" t="inlineStr">
+      <c r="AW3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1102,7 +1124,13 @@
       <c r="AV4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW4" t="inlineStr">
+      <c r="AW4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1259,9 +1287,15 @@
       <c r="AV5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW5" t="inlineStr">
-        <is>
-          <t>2751</t>
+      <c r="AW5" t="n">
+        <v>2751</v>
+      </c>
+      <c r="AX5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY5" t="inlineStr">
+        <is>
+          <t>2775</t>
         </is>
       </c>
     </row>
@@ -1416,7 +1450,13 @@
       <c r="AV6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW6" t="inlineStr">
+      <c r="AW6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1484,6 +1524,8 @@
       <c r="AU7" t="inlineStr"/>
       <c r="AV7" s="4" t="inlineStr"/>
       <c r="AW7" t="inlineStr"/>
+      <c r="AX7" s="4" t="inlineStr"/>
+      <c r="AY7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1547,6 +1589,8 @@
       <c r="AU8" t="inlineStr"/>
       <c r="AV8" s="4" t="inlineStr"/>
       <c r="AW8" t="inlineStr"/>
+      <c r="AX8" s="4" t="inlineStr"/>
+      <c r="AY8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1610,6 +1654,8 @@
       <c r="AU9" t="inlineStr"/>
       <c r="AV9" s="4" t="inlineStr"/>
       <c r="AW9" t="inlineStr"/>
+      <c r="AX9" s="4" t="inlineStr"/>
+      <c r="AY9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1673,6 +1719,8 @@
       <c r="AU10" t="inlineStr"/>
       <c r="AV10" s="4" t="inlineStr"/>
       <c r="AW10" t="inlineStr"/>
+      <c r="AX10" s="4" t="inlineStr"/>
+      <c r="AY10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1736,6 +1784,8 @@
       <c r="AU11" t="inlineStr"/>
       <c r="AV11" s="4" t="inlineStr"/>
       <c r="AW11" t="inlineStr"/>
+      <c r="AX11" s="4" t="inlineStr"/>
+      <c r="AY11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1799,6 +1849,8 @@
       <c r="AU12" t="inlineStr"/>
       <c r="AV12" s="4" t="inlineStr"/>
       <c r="AW12" t="inlineStr"/>
+      <c r="AX12" s="4" t="inlineStr"/>
+      <c r="AY12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1862,6 +1914,8 @@
       <c r="AU13" t="inlineStr"/>
       <c r="AV13" s="4" t="inlineStr"/>
       <c r="AW13" t="inlineStr"/>
+      <c r="AX13" s="4" t="inlineStr"/>
+      <c r="AY13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1925,6 +1979,8 @@
       <c r="AU14" t="inlineStr"/>
       <c r="AV14" s="4" t="inlineStr"/>
       <c r="AW14" t="inlineStr"/>
+      <c r="AX14" s="4" t="inlineStr"/>
+      <c r="AY14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1988,6 +2044,8 @@
       <c r="AU15" t="inlineStr"/>
       <c r="AV15" s="4" t="inlineStr"/>
       <c r="AW15" t="inlineStr"/>
+      <c r="AX15" s="4" t="inlineStr"/>
+      <c r="AY15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -2051,6 +2109,8 @@
       <c r="AU16" t="inlineStr"/>
       <c r="AV16" s="4" t="inlineStr"/>
       <c r="AW16" t="inlineStr"/>
+      <c r="AX16" s="4" t="inlineStr"/>
+      <c r="AY16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -2114,6 +2174,8 @@
       <c r="AU17" t="inlineStr"/>
       <c r="AV17" s="4" t="inlineStr"/>
       <c r="AW17" t="inlineStr"/>
+      <c r="AX17" s="4" t="inlineStr"/>
+      <c r="AY17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -2266,9 +2328,15 @@
       <c r="AV18" s="3" t="n">
         <v>11</v>
       </c>
-      <c r="AW18" t="inlineStr">
-        <is>
-          <t>3989</t>
+      <c r="AW18" t="n">
+        <v>3989</v>
+      </c>
+      <c r="AX18" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AY18" t="inlineStr">
+        <is>
+          <t>3994</t>
         </is>
       </c>
     </row>
@@ -2423,7 +2491,13 @@
       <c r="AV19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW19" t="inlineStr">
+      <c r="AW19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY19" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2580,9 +2654,15 @@
       <c r="AV20" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="AW20" t="inlineStr">
-        <is>
-          <t>4140</t>
+      <c r="AW20" t="n">
+        <v>4140</v>
+      </c>
+      <c r="AX20" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="AY20" t="inlineStr">
+        <is>
+          <t>4225</t>
         </is>
       </c>
     </row>
@@ -2737,9 +2817,15 @@
       <c r="AV21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW21" t="inlineStr">
-        <is>
-          <t>3137</t>
+      <c r="AW21" t="n">
+        <v>3137</v>
+      </c>
+      <c r="AX21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY21" t="inlineStr">
+        <is>
+          <t>3193</t>
         </is>
       </c>
     </row>
@@ -2894,9 +2980,15 @@
       <c r="AV22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AW22" t="inlineStr">
-        <is>
-          <t>4676</t>
+      <c r="AW22" t="n">
+        <v>4676</v>
+      </c>
+      <c r="AX22" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="AY22" t="inlineStr">
+        <is>
+          <t>4809</t>
         </is>
       </c>
     </row>
@@ -3051,9 +3143,15 @@
       <c r="AV23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AW23" t="inlineStr">
-        <is>
-          <t>5144</t>
+      <c r="AW23" t="n">
+        <v>5144</v>
+      </c>
+      <c r="AX23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AY23" t="inlineStr">
+        <is>
+          <t>5360</t>
         </is>
       </c>
     </row>
@@ -3208,9 +3306,15 @@
       <c r="AV24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AW24" t="inlineStr">
-        <is>
-          <t>4601</t>
+      <c r="AW24" t="n">
+        <v>4601</v>
+      </c>
+      <c r="AX24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AY24" t="inlineStr">
+        <is>
+          <t>4694</t>
         </is>
       </c>
     </row>
@@ -3340,6 +3444,8 @@
       <c r="AU25" t="inlineStr"/>
       <c r="AV25" s="4" t="inlineStr"/>
       <c r="AW25" t="inlineStr"/>
+      <c r="AX25" s="4" t="inlineStr"/>
+      <c r="AY25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -3455,6 +3561,8 @@
       <c r="AU26" t="inlineStr"/>
       <c r="AV26" s="4" t="inlineStr"/>
       <c r="AW26" t="inlineStr"/>
+      <c r="AX26" s="4" t="inlineStr"/>
+      <c r="AY26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -3607,7 +3715,13 @@
       <c r="AV27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW27" t="inlineStr">
+      <c r="AW27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3675,6 +3789,8 @@
       <c r="AU28" t="inlineStr"/>
       <c r="AV28" s="4" t="inlineStr"/>
       <c r="AW28" t="inlineStr"/>
+      <c r="AX28" s="4" t="inlineStr"/>
+      <c r="AY28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -3827,7 +3943,13 @@
       <c r="AV29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW29" t="inlineStr">
+      <c r="AW29" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AX29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY29" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -3984,9 +4106,15 @@
       <c r="AV30" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AW30" t="inlineStr">
-        <is>
-          <t>4269</t>
+      <c r="AW30" t="n">
+        <v>4269</v>
+      </c>
+      <c r="AX30" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY30" t="inlineStr">
+        <is>
+          <t>4550</t>
         </is>
       </c>
     </row>
@@ -4141,9 +4269,15 @@
       <c r="AV31" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="AW31" t="inlineStr">
-        <is>
-          <t>4667</t>
+      <c r="AW31" t="n">
+        <v>4667</v>
+      </c>
+      <c r="AX31" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="AY31" t="inlineStr">
+        <is>
+          <t>4866</t>
         </is>
       </c>
     </row>
@@ -4298,7 +4432,13 @@
       <c r="AV32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW32" t="inlineStr">
+      <c r="AW32" t="n">
+        <v>2624</v>
+      </c>
+      <c r="AX32" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY32" t="inlineStr">
         <is>
           <t>2624</t>
         </is>
@@ -4366,6 +4506,8 @@
       <c r="AU33" t="inlineStr"/>
       <c r="AV33" s="4" t="inlineStr"/>
       <c r="AW33" t="inlineStr"/>
+      <c r="AX33" s="4" t="inlineStr"/>
+      <c r="AY33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -4518,7 +4660,13 @@
       <c r="AV34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW34" t="inlineStr">
+      <c r="AW34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4675,7 +4823,13 @@
       <c r="AV35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW35" t="inlineStr">
+      <c r="AW35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY35" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4832,9 +4986,15 @@
       <c r="AV36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW36" t="inlineStr">
-        <is>
-          <t>3009</t>
+      <c r="AW36" t="n">
+        <v>3009</v>
+      </c>
+      <c r="AX36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY36" t="inlineStr">
+        <is>
+          <t>3011</t>
         </is>
       </c>
     </row>
@@ -4972,6 +5132,8 @@
       <c r="AU37" t="inlineStr"/>
       <c r="AV37" s="4" t="inlineStr"/>
       <c r="AW37" t="inlineStr"/>
+      <c r="AX37" s="4" t="inlineStr"/>
+      <c r="AY37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -5124,9 +5286,15 @@
       <c r="AV38" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW38" t="inlineStr">
-        <is>
-          <t>4676</t>
+      <c r="AW38" t="n">
+        <v>4676</v>
+      </c>
+      <c r="AX38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY38" t="inlineStr">
+        <is>
+          <t>4696</t>
         </is>
       </c>
     </row>
@@ -5281,9 +5449,15 @@
       <c r="AV39" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AW39" t="inlineStr">
-        <is>
-          <t>4383</t>
+      <c r="AW39" t="n">
+        <v>4383</v>
+      </c>
+      <c r="AX39" s="4" t="n">
+        <v>29</v>
+      </c>
+      <c r="AY39" t="inlineStr">
+        <is>
+          <t>4505</t>
         </is>
       </c>
     </row>
@@ -5438,7 +5612,13 @@
       <c r="AV40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW40" t="inlineStr">
+      <c r="AW40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5595,9 +5775,15 @@
       <c r="AV41" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW41" t="inlineStr">
-        <is>
-          <t>4169</t>
+      <c r="AW41" t="n">
+        <v>4169</v>
+      </c>
+      <c r="AX41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY41" t="inlineStr">
+        <is>
+          <t>4318</t>
         </is>
       </c>
     </row>
@@ -5752,9 +5938,15 @@
       <c r="AV42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW42" t="inlineStr">
-        <is>
-          <t>2819</t>
+      <c r="AW42" t="n">
+        <v>2819</v>
+      </c>
+      <c r="AX42" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY42" t="inlineStr">
+        <is>
+          <t>2872</t>
         </is>
       </c>
     </row>
@@ -5820,6 +6012,8 @@
       <c r="AU43" t="inlineStr"/>
       <c r="AV43" s="4" t="inlineStr"/>
       <c r="AW43" t="inlineStr"/>
+      <c r="AX43" s="4" t="inlineStr"/>
+      <c r="AY43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -5883,6 +6077,8 @@
       <c r="AU44" t="inlineStr"/>
       <c r="AV44" s="4" t="inlineStr"/>
       <c r="AW44" t="inlineStr"/>
+      <c r="AX44" s="4" t="inlineStr"/>
+      <c r="AY44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -5978,6 +6174,8 @@
       <c r="AU45" t="inlineStr"/>
       <c r="AV45" s="4" t="inlineStr"/>
       <c r="AW45" t="inlineStr"/>
+      <c r="AX45" s="4" t="inlineStr"/>
+      <c r="AY45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -6130,9 +6328,15 @@
       <c r="AV46" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="AW46" t="inlineStr">
-        <is>
-          <t>4170</t>
+      <c r="AW46" t="n">
+        <v>4170</v>
+      </c>
+      <c r="AX46" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY46" t="inlineStr">
+        <is>
+          <t>4190</t>
         </is>
       </c>
     </row>
@@ -6287,9 +6491,15 @@
       <c r="AV47" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AW47" t="inlineStr">
-        <is>
-          <t>4994</t>
+      <c r="AW47" t="n">
+        <v>4994</v>
+      </c>
+      <c r="AX47" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="AY47" t="inlineStr">
+        <is>
+          <t>5223</t>
         </is>
       </c>
     </row>
@@ -6444,7 +6654,13 @@
       <c r="AV48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW48" t="inlineStr">
+      <c r="AW48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6601,9 +6817,15 @@
       <c r="AV49" s="4" t="n">
         <v>27</v>
       </c>
-      <c r="AW49" t="inlineStr">
-        <is>
-          <t>4612</t>
+      <c r="AW49" t="n">
+        <v>4612</v>
+      </c>
+      <c r="AX49" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="AY49" t="inlineStr">
+        <is>
+          <t>4763</t>
         </is>
       </c>
     </row>
@@ -6758,9 +6980,15 @@
       <c r="AV50" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="AW50" t="inlineStr">
-        <is>
-          <t>4712</t>
+      <c r="AW50" t="n">
+        <v>4712</v>
+      </c>
+      <c r="AX50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="AY50" t="inlineStr">
+        <is>
+          <t>4852</t>
         </is>
       </c>
     </row>
@@ -6858,6 +7086,8 @@
       <c r="AU51" t="inlineStr"/>
       <c r="AV51" s="4" t="inlineStr"/>
       <c r="AW51" t="inlineStr"/>
+      <c r="AX51" s="4" t="inlineStr"/>
+      <c r="AY51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -7010,9 +7240,15 @@
       <c r="AV52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AW52" t="inlineStr">
-        <is>
-          <t>4746</t>
+      <c r="AW52" t="n">
+        <v>4746</v>
+      </c>
+      <c r="AX52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AY52" t="inlineStr">
+        <is>
+          <t>4822</t>
         </is>
       </c>
     </row>
@@ -7167,9 +7403,15 @@
       <c r="AV53" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW53" t="inlineStr">
-        <is>
-          <t>3336</t>
+      <c r="AW53" t="n">
+        <v>3336</v>
+      </c>
+      <c r="AX53" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AY53" t="inlineStr">
+        <is>
+          <t>3521</t>
         </is>
       </c>
     </row>
@@ -7267,6 +7509,8 @@
       <c r="AU54" t="inlineStr"/>
       <c r="AV54" s="4" t="inlineStr"/>
       <c r="AW54" t="inlineStr"/>
+      <c r="AX54" s="4" t="inlineStr"/>
+      <c r="AY54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -7419,9 +7663,15 @@
       <c r="AV55" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW55" t="inlineStr">
-        <is>
-          <t>3458</t>
+      <c r="AW55" t="n">
+        <v>3458</v>
+      </c>
+      <c r="AX55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY55" t="inlineStr">
+        <is>
+          <t>3496</t>
         </is>
       </c>
     </row>
@@ -7576,9 +7826,15 @@
       <c r="AV56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AW56" t="inlineStr">
-        <is>
-          <t>5008</t>
+      <c r="AW56" t="n">
+        <v>5008</v>
+      </c>
+      <c r="AX56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AY56" t="inlineStr">
+        <is>
+          <t>5176</t>
         </is>
       </c>
     </row>
@@ -7733,9 +7989,15 @@
       <c r="AV57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AW57" t="inlineStr">
-        <is>
-          <t>4098</t>
+      <c r="AW57" t="n">
+        <v>4098</v>
+      </c>
+      <c r="AX57" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="AY57" t="inlineStr">
+        <is>
+          <t>4122</t>
         </is>
       </c>
     </row>
@@ -7890,9 +8152,15 @@
       <c r="AV58" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AW58" t="inlineStr">
-        <is>
-          <t>4085</t>
+      <c r="AW58" t="n">
+        <v>4085</v>
+      </c>
+      <c r="AX58" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AY58" t="inlineStr">
+        <is>
+          <t>4182</t>
         </is>
       </c>
     </row>
@@ -8047,9 +8315,15 @@
       <c r="AV59" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW59" t="inlineStr">
-        <is>
-          <t>3988</t>
+      <c r="AW59" t="n">
+        <v>3988</v>
+      </c>
+      <c r="AX59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY59" t="inlineStr">
+        <is>
+          <t>4039</t>
         </is>
       </c>
     </row>
@@ -8204,9 +8478,15 @@
       <c r="AV60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AW60" t="inlineStr">
-        <is>
-          <t>4193</t>
+      <c r="AW60" t="n">
+        <v>4193</v>
+      </c>
+      <c r="AX60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AY60" t="inlineStr">
+        <is>
+          <t>4287</t>
         </is>
       </c>
     </row>
@@ -8272,6 +8552,8 @@
       <c r="AU61" t="inlineStr"/>
       <c r="AV61" s="4" t="inlineStr"/>
       <c r="AW61" t="inlineStr"/>
+      <c r="AX61" s="4" t="inlineStr"/>
+      <c r="AY61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -8424,9 +8706,15 @@
       <c r="AV62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AW62" t="inlineStr">
-        <is>
-          <t>3913</t>
+      <c r="AW62" t="n">
+        <v>3913</v>
+      </c>
+      <c r="AX62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AY62" t="inlineStr">
+        <is>
+          <t>3986</t>
         </is>
       </c>
     </row>
@@ -8581,9 +8869,15 @@
       <c r="AV63" s="3" t="n">
         <v>17</v>
       </c>
-      <c r="AW63" t="inlineStr">
-        <is>
-          <t>3985</t>
+      <c r="AW63" t="n">
+        <v>3985</v>
+      </c>
+      <c r="AX63" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="AY63" t="inlineStr">
+        <is>
+          <t>4043</t>
         </is>
       </c>
     </row>
@@ -8738,9 +9032,15 @@
       <c r="AV64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AW64" t="inlineStr">
-        <is>
-          <t>4181</t>
+      <c r="AW64" t="n">
+        <v>4181</v>
+      </c>
+      <c r="AX64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY64" t="inlineStr">
+        <is>
+          <t>4271</t>
         </is>
       </c>
     </row>
@@ -8858,6 +9158,8 @@
       <c r="AU65" t="inlineStr"/>
       <c r="AV65" s="4" t="inlineStr"/>
       <c r="AW65" t="inlineStr"/>
+      <c r="AX65" s="4" t="inlineStr"/>
+      <c r="AY65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -9010,7 +9312,13 @@
       <c r="AV66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW66" t="inlineStr">
+      <c r="AW66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9167,7 +9475,13 @@
       <c r="AV67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW67" t="inlineStr">
+      <c r="AW67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9324,7 +9638,13 @@
       <c r="AV68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW68" t="inlineStr">
+      <c r="AW68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9392,6 +9712,8 @@
       <c r="AU69" t="inlineStr"/>
       <c r="AV69" s="4" t="inlineStr"/>
       <c r="AW69" t="inlineStr"/>
+      <c r="AX69" s="4" t="inlineStr"/>
+      <c r="AY69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -9544,7 +9866,13 @@
       <c r="AV70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW70" t="inlineStr">
+      <c r="AW70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9701,7 +10029,13 @@
       <c r="AV71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW71" t="inlineStr">
+      <c r="AW71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9858,7 +10192,13 @@
       <c r="AV72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW72" t="inlineStr">
+      <c r="AW72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10015,9 +10355,15 @@
       <c r="AV73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW73" t="inlineStr">
-        <is>
-          <t>2656</t>
+      <c r="AW73" t="n">
+        <v>2656</v>
+      </c>
+      <c r="AX73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY73" t="inlineStr">
+        <is>
+          <t>2678</t>
         </is>
       </c>
     </row>
@@ -10172,7 +10518,13 @@
       <c r="AV74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW74" t="inlineStr">
+      <c r="AW74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10329,7 +10681,13 @@
       <c r="AV75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW75" t="inlineStr">
+      <c r="AW75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10486,9 +10844,15 @@
       <c r="AV76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW76" t="inlineStr">
-        <is>
-          <t>2636</t>
+      <c r="AW76" t="n">
+        <v>2636</v>
+      </c>
+      <c r="AX76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY76" t="inlineStr">
+        <is>
+          <t>2651</t>
         </is>
       </c>
     </row>
@@ -10643,9 +11007,15 @@
       <c r="AV77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW77" t="inlineStr">
-        <is>
-          <t>2612</t>
+      <c r="AW77" t="n">
+        <v>2612</v>
+      </c>
+      <c r="AX77" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY77" t="inlineStr">
+        <is>
+          <t>2935</t>
         </is>
       </c>
     </row>
@@ -10800,7 +11170,13 @@
       <c r="AV78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW78" t="inlineStr">
+      <c r="AW78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10957,7 +11333,13 @@
       <c r="AV79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW79" t="inlineStr">
+      <c r="AW79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11114,7 +11496,13 @@
       <c r="AV80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW80" t="inlineStr">
+      <c r="AW80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11271,7 +11659,13 @@
       <c r="AV81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW81" t="inlineStr">
+      <c r="AW81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11428,7 +11822,13 @@
       <c r="AV82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW82" t="inlineStr">
+      <c r="AW82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11585,7 +11985,13 @@
       <c r="AV83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW83" t="inlineStr">
+      <c r="AW83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11742,7 +12148,13 @@
       <c r="AV84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW84" t="inlineStr">
+      <c r="AW84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11899,7 +12311,13 @@
       <c r="AV85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW85" t="inlineStr">
+      <c r="AW85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12056,7 +12474,13 @@
       <c r="AV86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW86" t="inlineStr">
+      <c r="AW86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12213,7 +12637,13 @@
       <c r="AV87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW87" t="inlineStr">
+      <c r="AW87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12370,7 +12800,13 @@
       <c r="AV88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW88" t="inlineStr">
+      <c r="AW88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12527,7 +12963,13 @@
       <c r="AV89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW89" t="inlineStr">
+      <c r="AW89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12684,7 +13126,13 @@
       <c r="AV90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW90" t="inlineStr">
+      <c r="AW90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12841,7 +13289,13 @@
       <c r="AV91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW91" t="inlineStr">
+      <c r="AW91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12998,7 +13452,13 @@
       <c r="AV92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW92" t="inlineStr">
+      <c r="AW92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13155,7 +13615,13 @@
       <c r="AV93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW93" t="inlineStr">
+      <c r="AW93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13312,7 +13778,13 @@
       <c r="AV94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW94" t="inlineStr">
+      <c r="AW94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13469,7 +13941,13 @@
       <c r="AV95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW95" t="inlineStr">
+      <c r="AW95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13626,11 +14104,11 @@
       <c r="AV96" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW96" t="inlineStr">
-        <is>
-          <t>2470</t>
-        </is>
-      </c>
+      <c r="AW96" t="n">
+        <v>2470</v>
+      </c>
+      <c r="AX96" s="4" t="inlineStr"/>
+      <c r="AY96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -13783,7 +14261,13 @@
       <c r="AV97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW97" t="inlineStr">
+      <c r="AW97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13940,7 +14424,13 @@
       <c r="AV98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW98" t="inlineStr">
+      <c r="AW98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14097,7 +14587,13 @@
       <c r="AV99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW99" t="inlineStr">
+      <c r="AW99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14254,7 +14750,13 @@
       <c r="AV100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW100" t="inlineStr">
+      <c r="AW100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14411,7 +14913,13 @@
       <c r="AV101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW101" t="inlineStr">
+      <c r="AW101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14568,7 +15076,13 @@
       <c r="AV102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW102" t="inlineStr">
+      <c r="AW102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14725,7 +15239,13 @@
       <c r="AV103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW103" t="inlineStr">
+      <c r="AW103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14882,7 +15402,13 @@
       <c r="AV104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW104" t="inlineStr">
+      <c r="AW104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15039,7 +15565,13 @@
       <c r="AV105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW105" t="inlineStr">
+      <c r="AW105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15107,6 +15639,8 @@
       <c r="AU106" t="inlineStr"/>
       <c r="AV106" s="4" t="inlineStr"/>
       <c r="AW106" t="inlineStr"/>
+      <c r="AX106" s="4" t="inlineStr"/>
+      <c r="AY106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -15170,6 +15704,8 @@
       <c r="AU107" t="inlineStr"/>
       <c r="AV107" s="4" t="inlineStr"/>
       <c r="AW107" t="inlineStr"/>
+      <c r="AX107" s="4" t="inlineStr"/>
+      <c r="AY107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -15233,6 +15769,8 @@
       <c r="AU108" t="inlineStr"/>
       <c r="AV108" s="4" t="inlineStr"/>
       <c r="AW108" t="inlineStr"/>
+      <c r="AX108" s="4" t="inlineStr"/>
+      <c r="AY108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -15296,6 +15834,8 @@
       <c r="AU109" t="inlineStr"/>
       <c r="AV109" s="4" t="inlineStr"/>
       <c r="AW109" t="inlineStr"/>
+      <c r="AX109" s="4" t="inlineStr"/>
+      <c r="AY109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -15359,6 +15899,8 @@
       <c r="AU110" t="inlineStr"/>
       <c r="AV110" s="4" t="inlineStr"/>
       <c r="AW110" t="inlineStr"/>
+      <c r="AX110" s="4" t="inlineStr"/>
+      <c r="AY110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -15422,6 +15964,8 @@
       <c r="AU111" t="inlineStr"/>
       <c r="AV111" s="4" t="inlineStr"/>
       <c r="AW111" t="inlineStr"/>
+      <c r="AX111" s="4" t="inlineStr"/>
+      <c r="AY111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -15485,6 +16029,8 @@
       <c r="AU112" t="inlineStr"/>
       <c r="AV112" s="4" t="inlineStr"/>
       <c r="AW112" t="inlineStr"/>
+      <c r="AX112" s="4" t="inlineStr"/>
+      <c r="AY112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -15548,6 +16094,8 @@
       <c r="AU113" t="inlineStr"/>
       <c r="AV113" s="4" t="inlineStr"/>
       <c r="AW113" t="inlineStr"/>
+      <c r="AX113" s="4" t="inlineStr"/>
+      <c r="AY113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -15611,6 +16159,8 @@
       <c r="AU114" t="inlineStr"/>
       <c r="AV114" s="4" t="inlineStr"/>
       <c r="AW114" t="inlineStr"/>
+      <c r="AX114" s="4" t="inlineStr"/>
+      <c r="AY114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -15741,9 +16291,15 @@
       <c r="AV115" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AW115" t="inlineStr">
-        <is>
-          <t>5053</t>
+      <c r="AW115" t="n">
+        <v>5053</v>
+      </c>
+      <c r="AX115" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="AY115" t="inlineStr">
+        <is>
+          <t>5257</t>
         </is>
       </c>
     </row>
@@ -15892,7 +16448,13 @@
       <c r="AV116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW116" t="inlineStr">
+      <c r="AW116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16011,11 +16573,11 @@
       <c r="AV117" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AW117" t="inlineStr">
-        <is>
-          <t>5917</t>
-        </is>
-      </c>
+      <c r="AW117" t="n">
+        <v>5917</v>
+      </c>
+      <c r="AX117" s="4" t="inlineStr"/>
+      <c r="AY117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -16162,9 +16724,15 @@
       <c r="AV118" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AW118" t="inlineStr">
-        <is>
-          <t>3233</t>
+      <c r="AW118" t="n">
+        <v>3233</v>
+      </c>
+      <c r="AX118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY118" t="inlineStr">
+        <is>
+          <t>3231</t>
         </is>
       </c>
     </row>
@@ -16313,9 +16881,15 @@
       <c r="AV119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW119" t="inlineStr">
-        <is>
-          <t>1530</t>
+      <c r="AW119" t="n">
+        <v>1530</v>
+      </c>
+      <c r="AX119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY119" t="inlineStr">
+        <is>
+          <t>1528</t>
         </is>
       </c>
     </row>
@@ -16464,7 +17038,13 @@
       <c r="AV120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW120" t="inlineStr">
+      <c r="AW120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY120" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16615,7 +17195,13 @@
       <c r="AV121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW121" t="inlineStr">
+      <c r="AW121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16766,7 +17352,13 @@
       <c r="AV122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW122" t="inlineStr">
+      <c r="AW122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16913,7 +17505,13 @@
       <c r="AV123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW123" t="inlineStr">
+      <c r="AW123" t="n">
+        <v>2579</v>
+      </c>
+      <c r="AX123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY123" t="inlineStr">
         <is>
           <t>2579</t>
         </is>
@@ -17007,6 +17605,8 @@
       <c r="AU124" t="inlineStr"/>
       <c r="AV124" s="4" t="inlineStr"/>
       <c r="AW124" t="inlineStr"/>
+      <c r="AX124" s="4" t="inlineStr"/>
+      <c r="AY124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -17145,9 +17745,15 @@
       <c r="AV125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW125" t="inlineStr">
-        <is>
-          <t>2148</t>
+      <c r="AW125" t="n">
+        <v>2148</v>
+      </c>
+      <c r="AX125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY125" t="inlineStr">
+        <is>
+          <t>2145</t>
         </is>
       </c>
     </row>
@@ -17276,7 +17882,13 @@
       <c r="AV126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW126" t="inlineStr">
+      <c r="AW126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY126" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17362,6 +17974,8 @@
       <c r="AU127" t="inlineStr"/>
       <c r="AV127" s="4" t="inlineStr"/>
       <c r="AW127" t="inlineStr"/>
+      <c r="AX127" s="4" t="inlineStr"/>
+      <c r="AY127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -17455,6 +18069,8 @@
       <c r="AU128" t="inlineStr"/>
       <c r="AV128" s="4" t="inlineStr"/>
       <c r="AW128" t="inlineStr"/>
+      <c r="AX128" s="4" t="inlineStr"/>
+      <c r="AY128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -17573,9 +18189,15 @@
       <c r="AV129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW129" t="inlineStr">
-        <is>
-          <t>2538</t>
+      <c r="AW129" t="n">
+        <v>2538</v>
+      </c>
+      <c r="AX129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY129" t="inlineStr">
+        <is>
+          <t>2552</t>
         </is>
       </c>
     </row>
@@ -17671,6 +18293,8 @@
       <c r="AU130" t="inlineStr"/>
       <c r="AV130" s="4" t="inlineStr"/>
       <c r="AW130" t="inlineStr"/>
+      <c r="AX130" s="4" t="inlineStr"/>
+      <c r="AY130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -17678,7 +18302,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>垃圾游戏草</t>
+          <t>Player-47928278</t>
         </is>
       </c>
       <c r="C131" t="inlineStr"/>
@@ -17785,7 +18409,13 @@
       <c r="AV131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW131" t="inlineStr">
+      <c r="AW131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17892,9 +18522,15 @@
       <c r="AV132" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="AW132" t="inlineStr">
-        <is>
-          <t>4095</t>
+      <c r="AW132" t="n">
+        <v>4095</v>
+      </c>
+      <c r="AX132" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AY132" t="inlineStr">
+        <is>
+          <t>4153</t>
         </is>
       </c>
     </row>
@@ -17999,9 +18635,15 @@
       <c r="AV133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW133" t="inlineStr">
-        <is>
-          <t>2481</t>
+      <c r="AW133" t="n">
+        <v>2481</v>
+      </c>
+      <c r="AX133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY133" t="inlineStr">
+        <is>
+          <t>2475</t>
         </is>
       </c>
     </row>
@@ -18069,6 +18711,8 @@
       <c r="AU134" t="inlineStr"/>
       <c r="AV134" s="4" t="inlineStr"/>
       <c r="AW134" t="inlineStr"/>
+      <c r="AX134" s="4" t="inlineStr"/>
+      <c r="AY134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -18138,6 +18782,8 @@
       <c r="AU135" t="inlineStr"/>
       <c r="AV135" s="4" t="inlineStr"/>
       <c r="AW135" t="inlineStr"/>
+      <c r="AX135" s="4" t="inlineStr"/>
+      <c r="AY135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -18224,11 +18870,11 @@
       <c r="AV136" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="AW136" t="inlineStr">
-        <is>
-          <t>5865</t>
-        </is>
-      </c>
+      <c r="AW136" t="n">
+        <v>5865</v>
+      </c>
+      <c r="AX136" s="4" t="inlineStr"/>
+      <c r="AY136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -18315,11 +18961,11 @@
       <c r="AV137" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AW137" t="inlineStr">
-        <is>
-          <t>5409</t>
-        </is>
-      </c>
+      <c r="AW137" t="n">
+        <v>5409</v>
+      </c>
+      <c r="AX137" s="4" t="inlineStr"/>
+      <c r="AY137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -18389,6 +19035,8 @@
       <c r="AU138" t="inlineStr"/>
       <c r="AV138" s="4" t="inlineStr"/>
       <c r="AW138" t="inlineStr"/>
+      <c r="AX138" s="4" t="inlineStr"/>
+      <c r="AY138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -18475,11 +19123,11 @@
       <c r="AV139" s="5" t="n">
         <v>34</v>
       </c>
-      <c r="AW139" t="inlineStr">
-        <is>
-          <t>5845</t>
-        </is>
-      </c>
+      <c r="AW139" t="n">
+        <v>5845</v>
+      </c>
+      <c r="AX139" s="4" t="inlineStr"/>
+      <c r="AY139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -18566,9 +19214,15 @@
       <c r="AV140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW140" t="inlineStr">
-        <is>
-          <t>2038</t>
+      <c r="AW140" t="n">
+        <v>2038</v>
+      </c>
+      <c r="AX140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY140" t="inlineStr">
+        <is>
+          <t>2037</t>
         </is>
       </c>
     </row>
@@ -18636,6 +19290,8 @@
       <c r="AU141" t="inlineStr"/>
       <c r="AV141" s="4" t="inlineStr"/>
       <c r="AW141" t="inlineStr"/>
+      <c r="AX141" s="4" t="inlineStr"/>
+      <c r="AY141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -18718,9 +19374,15 @@
       <c r="AV142" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW142" t="inlineStr">
-        <is>
-          <t>2924</t>
+      <c r="AW142" t="n">
+        <v>2924</v>
+      </c>
+      <c r="AX142" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AY142" t="inlineStr">
+        <is>
+          <t>2923</t>
         </is>
       </c>
     </row>
@@ -18805,7 +19467,13 @@
       <c r="AV143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW143" t="inlineStr">
+      <c r="AW143" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18888,7 +19556,13 @@
       <c r="AV144" s="3" t="n">
         <v>6</v>
       </c>
-      <c r="AW144" t="inlineStr">
+      <c r="AW144" t="n">
+        <v>1621</v>
+      </c>
+      <c r="AX144" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY144" t="inlineStr">
         <is>
           <t>1621</t>
         </is>
@@ -18971,9 +19645,15 @@
       <c r="AV145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW145" t="inlineStr">
-        <is>
-          <t>1801</t>
+      <c r="AW145" t="n">
+        <v>1801</v>
+      </c>
+      <c r="AX145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY145" t="inlineStr">
+        <is>
+          <t>1833</t>
         </is>
       </c>
     </row>
@@ -19054,7 +19734,13 @@
       <c r="AV146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW146" t="inlineStr">
+      <c r="AW146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19137,9 +19823,15 @@
       <c r="AV147" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AW147" t="inlineStr">
-        <is>
-          <t>4483</t>
+      <c r="AW147" t="n">
+        <v>4483</v>
+      </c>
+      <c r="AX147" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AY147" t="inlineStr">
+        <is>
+          <t>4615</t>
         </is>
       </c>
     </row>
@@ -19220,9 +19912,15 @@
       <c r="AV148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW148" t="inlineStr">
-        <is>
-          <t>2007</t>
+      <c r="AW148" t="n">
+        <v>2007</v>
+      </c>
+      <c r="AX148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY148" t="inlineStr">
+        <is>
+          <t>2030</t>
         </is>
       </c>
     </row>
@@ -19294,6 +19992,8 @@
       <c r="AU149" t="inlineStr"/>
       <c r="AV149" s="4" t="inlineStr"/>
       <c r="AW149" t="inlineStr"/>
+      <c r="AX149" s="4" t="inlineStr"/>
+      <c r="AY149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -19368,9 +20068,15 @@
       <c r="AV150" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="AW150" t="inlineStr">
-        <is>
-          <t>3514</t>
+      <c r="AW150" t="n">
+        <v>3514</v>
+      </c>
+      <c r="AX150" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY150" t="inlineStr">
+        <is>
+          <t>3603</t>
         </is>
       </c>
     </row>
@@ -19447,9 +20153,15 @@
       <c r="AV151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AW151" t="inlineStr">
-        <is>
-          <t>2296</t>
+      <c r="AW151" t="n">
+        <v>2296</v>
+      </c>
+      <c r="AX151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY151" t="inlineStr">
+        <is>
+          <t>2290</t>
         </is>
       </c>
     </row>
@@ -19522,9 +20234,15 @@
       <c r="AV152" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="AW152" t="inlineStr">
-        <is>
-          <t>3975</t>
+      <c r="AW152" t="n">
+        <v>3975</v>
+      </c>
+      <c r="AX152" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY152" t="inlineStr">
+        <is>
+          <t>3933</t>
         </is>
       </c>
     </row>
@@ -19593,9 +20311,86 @@
       <c r="AV153" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AW153" t="inlineStr">
-        <is>
-          <t>1823</t>
+      <c r="AW153" t="n">
+        <v>1823</v>
+      </c>
+      <c r="AX153" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AY153" t="inlineStr">
+        <is>
+          <t>1810</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>59552264</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>SPADGERCC</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr"/>
+      <c r="D154" t="inlineStr"/>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>总馆</t>
+        </is>
+      </c>
+      <c r="F154" s="4" t="inlineStr"/>
+      <c r="G154" t="inlineStr"/>
+      <c r="H154" s="4" t="inlineStr"/>
+      <c r="I154" t="inlineStr"/>
+      <c r="J154" s="4" t="inlineStr"/>
+      <c r="K154" t="inlineStr"/>
+      <c r="L154" s="4" t="inlineStr"/>
+      <c r="M154" t="inlineStr"/>
+      <c r="N154" s="4" t="inlineStr"/>
+      <c r="O154" t="inlineStr"/>
+      <c r="P154" s="4" t="inlineStr"/>
+      <c r="Q154" t="inlineStr"/>
+      <c r="R154" s="4" t="inlineStr"/>
+      <c r="S154" t="inlineStr"/>
+      <c r="T154" s="4" t="inlineStr"/>
+      <c r="U154" t="inlineStr"/>
+      <c r="V154" s="4" t="inlineStr"/>
+      <c r="W154" t="inlineStr"/>
+      <c r="X154" s="4" t="inlineStr"/>
+      <c r="Y154" t="inlineStr"/>
+      <c r="Z154" s="4" t="inlineStr"/>
+      <c r="AA154" t="inlineStr"/>
+      <c r="AB154" s="4" t="inlineStr"/>
+      <c r="AC154" t="inlineStr"/>
+      <c r="AD154" s="4" t="inlineStr"/>
+      <c r="AE154" t="inlineStr"/>
+      <c r="AF154" s="4" t="inlineStr"/>
+      <c r="AG154" t="inlineStr"/>
+      <c r="AH154" s="4" t="inlineStr"/>
+      <c r="AI154" t="inlineStr"/>
+      <c r="AJ154" s="4" t="inlineStr"/>
+      <c r="AK154" t="inlineStr"/>
+      <c r="AL154" s="4" t="inlineStr"/>
+      <c r="AM154" t="inlineStr"/>
+      <c r="AN154" s="4" t="inlineStr"/>
+      <c r="AO154" t="inlineStr"/>
+      <c r="AP154" s="4" t="inlineStr"/>
+      <c r="AQ154" t="inlineStr"/>
+      <c r="AR154" s="4" t="inlineStr"/>
+      <c r="AS154" t="inlineStr"/>
+      <c r="AT154" s="4" t="inlineStr"/>
+      <c r="AU154" t="inlineStr"/>
+      <c r="AV154" s="4" t="inlineStr"/>
+      <c r="AW154" t="inlineStr"/>
+      <c r="AX154" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="AY154" t="inlineStr">
+        <is>
+          <t>1876</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-06-14 10:24:49
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AY154"/>
+  <dimension ref="A1:BA154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -646,6 +646,16 @@
           <t>06-12_0</t>
         </is>
       </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>06-13_A</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>06-13_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -804,9 +814,15 @@
       <c r="AX2" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AY2" t="inlineStr">
-        <is>
-          <t>4580</t>
+      <c r="AY2" t="n">
+        <v>4580</v>
+      </c>
+      <c r="AZ2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA2" t="inlineStr">
+        <is>
+          <t>4598</t>
         </is>
       </c>
     </row>
@@ -967,7 +983,13 @@
       <c r="AX3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY3" t="inlineStr">
+      <c r="AY3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1130,7 +1152,13 @@
       <c r="AX4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY4" t="inlineStr">
+      <c r="AY4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1293,9 +1321,15 @@
       <c r="AX5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY5" t="inlineStr">
-        <is>
-          <t>2775</t>
+      <c r="AY5" t="n">
+        <v>2775</v>
+      </c>
+      <c r="AZ5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA5" t="inlineStr">
+        <is>
+          <t>2770</t>
         </is>
       </c>
     </row>
@@ -1456,7 +1490,13 @@
       <c r="AX6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY6" t="inlineStr">
+      <c r="AY6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1526,6 +1566,8 @@
       <c r="AW7" t="inlineStr"/>
       <c r="AX7" s="4" t="inlineStr"/>
       <c r="AY7" t="inlineStr"/>
+      <c r="AZ7" s="4" t="inlineStr"/>
+      <c r="BA7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1591,6 +1633,8 @@
       <c r="AW8" t="inlineStr"/>
       <c r="AX8" s="4" t="inlineStr"/>
       <c r="AY8" t="inlineStr"/>
+      <c r="AZ8" s="4" t="inlineStr"/>
+      <c r="BA8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1656,6 +1700,8 @@
       <c r="AW9" t="inlineStr"/>
       <c r="AX9" s="4" t="inlineStr"/>
       <c r="AY9" t="inlineStr"/>
+      <c r="AZ9" s="4" t="inlineStr"/>
+      <c r="BA9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1721,6 +1767,8 @@
       <c r="AW10" t="inlineStr"/>
       <c r="AX10" s="4" t="inlineStr"/>
       <c r="AY10" t="inlineStr"/>
+      <c r="AZ10" s="4" t="inlineStr"/>
+      <c r="BA10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1786,6 +1834,8 @@
       <c r="AW11" t="inlineStr"/>
       <c r="AX11" s="4" t="inlineStr"/>
       <c r="AY11" t="inlineStr"/>
+      <c r="AZ11" s="4" t="inlineStr"/>
+      <c r="BA11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1851,6 +1901,8 @@
       <c r="AW12" t="inlineStr"/>
       <c r="AX12" s="4" t="inlineStr"/>
       <c r="AY12" t="inlineStr"/>
+      <c r="AZ12" s="4" t="inlineStr"/>
+      <c r="BA12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1916,6 +1968,8 @@
       <c r="AW13" t="inlineStr"/>
       <c r="AX13" s="4" t="inlineStr"/>
       <c r="AY13" t="inlineStr"/>
+      <c r="AZ13" s="4" t="inlineStr"/>
+      <c r="BA13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1981,6 +2035,8 @@
       <c r="AW14" t="inlineStr"/>
       <c r="AX14" s="4" t="inlineStr"/>
       <c r="AY14" t="inlineStr"/>
+      <c r="AZ14" s="4" t="inlineStr"/>
+      <c r="BA14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -2046,6 +2102,8 @@
       <c r="AW15" t="inlineStr"/>
       <c r="AX15" s="4" t="inlineStr"/>
       <c r="AY15" t="inlineStr"/>
+      <c r="AZ15" s="4" t="inlineStr"/>
+      <c r="BA15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -2111,6 +2169,8 @@
       <c r="AW16" t="inlineStr"/>
       <c r="AX16" s="4" t="inlineStr"/>
       <c r="AY16" t="inlineStr"/>
+      <c r="AZ16" s="4" t="inlineStr"/>
+      <c r="BA16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -2176,6 +2236,8 @@
       <c r="AW17" t="inlineStr"/>
       <c r="AX17" s="4" t="inlineStr"/>
       <c r="AY17" t="inlineStr"/>
+      <c r="AZ17" s="4" t="inlineStr"/>
+      <c r="BA17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -2334,9 +2396,15 @@
       <c r="AX18" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="AY18" t="inlineStr">
-        <is>
-          <t>3994</t>
+      <c r="AY18" t="n">
+        <v>3994</v>
+      </c>
+      <c r="AZ18" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="BA18" t="inlineStr">
+        <is>
+          <t>4098</t>
         </is>
       </c>
     </row>
@@ -2497,7 +2565,13 @@
       <c r="AX19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY19" t="inlineStr">
+      <c r="AY19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA19" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2660,9 +2734,15 @@
       <c r="AX20" s="4" t="n">
         <v>22</v>
       </c>
-      <c r="AY20" t="inlineStr">
-        <is>
-          <t>4225</t>
+      <c r="AY20" t="n">
+        <v>4225</v>
+      </c>
+      <c r="AZ20" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA20" t="inlineStr">
+        <is>
+          <t>4354</t>
         </is>
       </c>
     </row>
@@ -2823,9 +2903,15 @@
       <c r="AX21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY21" t="inlineStr">
-        <is>
-          <t>3193</t>
+      <c r="AY21" t="n">
+        <v>3193</v>
+      </c>
+      <c r="AZ21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA21" t="inlineStr">
+        <is>
+          <t>3234</t>
         </is>
       </c>
     </row>
@@ -2986,9 +3072,15 @@
       <c r="AX22" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="AY22" t="inlineStr">
-        <is>
-          <t>4809</t>
+      <c r="AY22" t="n">
+        <v>4809</v>
+      </c>
+      <c r="AZ22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA22" t="inlineStr">
+        <is>
+          <t>4988</t>
         </is>
       </c>
     </row>
@@ -3149,9 +3241,15 @@
       <c r="AX23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AY23" t="inlineStr">
-        <is>
-          <t>5360</t>
+      <c r="AY23" t="n">
+        <v>5360</v>
+      </c>
+      <c r="AZ23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="BA23" t="inlineStr">
+        <is>
+          <t>5611</t>
         </is>
       </c>
     </row>
@@ -3312,9 +3410,15 @@
       <c r="AX24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AY24" t="inlineStr">
-        <is>
-          <t>4694</t>
+      <c r="AY24" t="n">
+        <v>4694</v>
+      </c>
+      <c r="AZ24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BA24" t="inlineStr">
+        <is>
+          <t>5052</t>
         </is>
       </c>
     </row>
@@ -3446,6 +3550,8 @@
       <c r="AW25" t="inlineStr"/>
       <c r="AX25" s="4" t="inlineStr"/>
       <c r="AY25" t="inlineStr"/>
+      <c r="AZ25" s="4" t="inlineStr"/>
+      <c r="BA25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -3563,6 +3669,8 @@
       <c r="AW26" t="inlineStr"/>
       <c r="AX26" s="4" t="inlineStr"/>
       <c r="AY26" t="inlineStr"/>
+      <c r="AZ26" s="4" t="inlineStr"/>
+      <c r="BA26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -3721,7 +3829,13 @@
       <c r="AX27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY27" t="inlineStr">
+      <c r="AY27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3791,6 +3905,8 @@
       <c r="AW28" t="inlineStr"/>
       <c r="AX28" s="4" t="inlineStr"/>
       <c r="AY28" t="inlineStr"/>
+      <c r="AZ28" s="4" t="inlineStr"/>
+      <c r="BA28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -3949,7 +4065,13 @@
       <c r="AX29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY29" t="inlineStr">
+      <c r="AY29" t="n">
+        <v>2500</v>
+      </c>
+      <c r="AZ29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA29" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -4112,9 +4234,15 @@
       <c r="AX30" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AY30" t="inlineStr">
-        <is>
-          <t>4550</t>
+      <c r="AY30" t="n">
+        <v>4550</v>
+      </c>
+      <c r="AZ30" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA30" t="inlineStr">
+        <is>
+          <t>4808</t>
         </is>
       </c>
     </row>
@@ -4275,9 +4403,15 @@
       <c r="AX31" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="AY31" t="inlineStr">
-        <is>
-          <t>4866</t>
+      <c r="AY31" t="n">
+        <v>4866</v>
+      </c>
+      <c r="AZ31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="BA31" t="inlineStr">
+        <is>
+          <t>4950</t>
         </is>
       </c>
     </row>
@@ -4438,9 +4572,15 @@
       <c r="AX32" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY32" t="inlineStr">
-        <is>
-          <t>2624</t>
+      <c r="AY32" t="n">
+        <v>2624</v>
+      </c>
+      <c r="AZ32" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA32" t="inlineStr">
+        <is>
+          <t>2985</t>
         </is>
       </c>
     </row>
@@ -4508,6 +4648,8 @@
       <c r="AW33" t="inlineStr"/>
       <c r="AX33" s="4" t="inlineStr"/>
       <c r="AY33" t="inlineStr"/>
+      <c r="AZ33" s="4" t="inlineStr"/>
+      <c r="BA33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -4666,7 +4808,13 @@
       <c r="AX34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY34" t="inlineStr">
+      <c r="AY34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4829,7 +4977,13 @@
       <c r="AX35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY35" t="inlineStr">
+      <c r="AY35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA35" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4992,9 +5146,15 @@
       <c r="AX36" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY36" t="inlineStr">
-        <is>
-          <t>3011</t>
+      <c r="AY36" t="n">
+        <v>3011</v>
+      </c>
+      <c r="AZ36" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA36" t="inlineStr">
+        <is>
+          <t>3372</t>
         </is>
       </c>
     </row>
@@ -5134,6 +5294,8 @@
       <c r="AW37" t="inlineStr"/>
       <c r="AX37" s="4" t="inlineStr"/>
       <c r="AY37" t="inlineStr"/>
+      <c r="AZ37" s="4" t="inlineStr"/>
+      <c r="BA37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -5292,7 +5454,13 @@
       <c r="AX38" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY38" t="inlineStr">
+      <c r="AY38" t="n">
+        <v>4696</v>
+      </c>
+      <c r="AZ38" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA38" t="inlineStr">
         <is>
           <t>4696</t>
         </is>
@@ -5455,9 +5623,15 @@
       <c r="AX39" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="AY39" t="inlineStr">
-        <is>
-          <t>4505</t>
+      <c r="AY39" t="n">
+        <v>4505</v>
+      </c>
+      <c r="AZ39" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="BA39" t="inlineStr">
+        <is>
+          <t>4560</t>
         </is>
       </c>
     </row>
@@ -5618,7 +5792,13 @@
       <c r="AX40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY40" t="inlineStr">
+      <c r="AY40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5781,9 +5961,15 @@
       <c r="AX41" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="AY41" t="inlineStr">
-        <is>
-          <t>4318</t>
+      <c r="AY41" t="n">
+        <v>4318</v>
+      </c>
+      <c r="AZ41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA41" t="inlineStr">
+        <is>
+          <t>4242</t>
         </is>
       </c>
     </row>
@@ -5944,7 +6130,13 @@
       <c r="AX42" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="AY42" t="inlineStr">
+      <c r="AY42" t="n">
+        <v>2872</v>
+      </c>
+      <c r="AZ42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA42" t="inlineStr">
         <is>
           <t>2872</t>
         </is>
@@ -6014,6 +6206,8 @@
       <c r="AW43" t="inlineStr"/>
       <c r="AX43" s="4" t="inlineStr"/>
       <c r="AY43" t="inlineStr"/>
+      <c r="AZ43" s="4" t="inlineStr"/>
+      <c r="BA43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -6079,6 +6273,8 @@
       <c r="AW44" t="inlineStr"/>
       <c r="AX44" s="4" t="inlineStr"/>
       <c r="AY44" t="inlineStr"/>
+      <c r="AZ44" s="4" t="inlineStr"/>
+      <c r="BA44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -6176,6 +6372,8 @@
       <c r="AW45" t="inlineStr"/>
       <c r="AX45" s="4" t="inlineStr"/>
       <c r="AY45" t="inlineStr"/>
+      <c r="AZ45" s="4" t="inlineStr"/>
+      <c r="BA45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -6334,9 +6532,15 @@
       <c r="AX46" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY46" t="inlineStr">
-        <is>
-          <t>4190</t>
+      <c r="AY46" t="n">
+        <v>4190</v>
+      </c>
+      <c r="AZ46" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="BA46" t="inlineStr">
+        <is>
+          <t>4465</t>
         </is>
       </c>
     </row>
@@ -6497,9 +6701,15 @@
       <c r="AX47" s="5" t="n">
         <v>32</v>
       </c>
-      <c r="AY47" t="inlineStr">
-        <is>
-          <t>5223</t>
+      <c r="AY47" t="n">
+        <v>5223</v>
+      </c>
+      <c r="AZ47" s="5" t="n">
+        <v>31</v>
+      </c>
+      <c r="BA47" t="inlineStr">
+        <is>
+          <t>5433</t>
         </is>
       </c>
     </row>
@@ -6660,7 +6870,13 @@
       <c r="AX48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY48" t="inlineStr">
+      <c r="AY48" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -6823,9 +7039,15 @@
       <c r="AX49" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="AY49" t="inlineStr">
-        <is>
-          <t>4763</t>
+      <c r="AY49" t="n">
+        <v>4763</v>
+      </c>
+      <c r="AZ49" s="4" t="n">
+        <v>28</v>
+      </c>
+      <c r="BA49" t="inlineStr">
+        <is>
+          <t>4790</t>
         </is>
       </c>
     </row>
@@ -6986,9 +7208,15 @@
       <c r="AX50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="AY50" t="inlineStr">
-        <is>
-          <t>4852</t>
+      <c r="AY50" t="n">
+        <v>4852</v>
+      </c>
+      <c r="AZ50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="BA50" t="inlineStr">
+        <is>
+          <t>5020</t>
         </is>
       </c>
     </row>
@@ -7088,6 +7316,8 @@
       <c r="AW51" t="inlineStr"/>
       <c r="AX51" s="4" t="inlineStr"/>
       <c r="AY51" t="inlineStr"/>
+      <c r="AZ51" s="4" t="inlineStr"/>
+      <c r="BA51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -7246,9 +7476,15 @@
       <c r="AX52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AY52" t="inlineStr">
-        <is>
-          <t>4822</t>
+      <c r="AY52" t="n">
+        <v>4822</v>
+      </c>
+      <c r="AZ52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="BA52" t="inlineStr">
+        <is>
+          <t>5056</t>
         </is>
       </c>
     </row>
@@ -7409,9 +7645,15 @@
       <c r="AX53" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="AY53" t="inlineStr">
-        <is>
-          <t>3521</t>
+      <c r="AY53" t="n">
+        <v>3521</v>
+      </c>
+      <c r="AZ53" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="BA53" t="inlineStr">
+        <is>
+          <t>3724</t>
         </is>
       </c>
     </row>
@@ -7511,6 +7753,8 @@
       <c r="AW54" t="inlineStr"/>
       <c r="AX54" s="4" t="inlineStr"/>
       <c r="AY54" t="inlineStr"/>
+      <c r="AZ54" s="4" t="inlineStr"/>
+      <c r="BA54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -7669,9 +7913,15 @@
       <c r="AX55" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY55" t="inlineStr">
-        <is>
-          <t>3496</t>
+      <c r="AY55" t="n">
+        <v>3496</v>
+      </c>
+      <c r="AZ55" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA55" t="inlineStr">
+        <is>
+          <t>3537</t>
         </is>
       </c>
     </row>
@@ -7832,9 +8082,15 @@
       <c r="AX56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AY56" t="inlineStr">
-        <is>
-          <t>5176</t>
+      <c r="AY56" t="n">
+        <v>5176</v>
+      </c>
+      <c r="AZ56" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="BA56" t="inlineStr">
+        <is>
+          <t>5377</t>
         </is>
       </c>
     </row>
@@ -7995,9 +8251,15 @@
       <c r="AX57" s="3" t="n">
         <v>13</v>
       </c>
-      <c r="AY57" t="inlineStr">
-        <is>
-          <t>4122</t>
+      <c r="AY57" t="n">
+        <v>4122</v>
+      </c>
+      <c r="AZ57" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="BA57" t="inlineStr">
+        <is>
+          <t>4275</t>
         </is>
       </c>
     </row>
@@ -8158,9 +8420,15 @@
       <c r="AX58" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AY58" t="inlineStr">
-        <is>
-          <t>4182</t>
+      <c r="AY58" t="n">
+        <v>4182</v>
+      </c>
+      <c r="AZ58" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="BA58" t="inlineStr">
+        <is>
+          <t>4233</t>
         </is>
       </c>
     </row>
@@ -8321,9 +8589,15 @@
       <c r="AX59" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AY59" t="inlineStr">
-        <is>
-          <t>4039</t>
+      <c r="AY59" t="n">
+        <v>4039</v>
+      </c>
+      <c r="AZ59" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="BA59" t="inlineStr">
+        <is>
+          <t>4157</t>
         </is>
       </c>
     </row>
@@ -8484,9 +8758,15 @@
       <c r="AX60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AY60" t="inlineStr">
-        <is>
-          <t>4287</t>
+      <c r="AY60" t="n">
+        <v>4287</v>
+      </c>
+      <c r="AZ60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="BA60" t="inlineStr">
+        <is>
+          <t>4333</t>
         </is>
       </c>
     </row>
@@ -8554,6 +8834,8 @@
       <c r="AW61" t="inlineStr"/>
       <c r="AX61" s="4" t="inlineStr"/>
       <c r="AY61" t="inlineStr"/>
+      <c r="AZ61" s="4" t="inlineStr"/>
+      <c r="BA61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -8712,9 +8994,15 @@
       <c r="AX62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AY62" t="inlineStr">
-        <is>
-          <t>3986</t>
+      <c r="AY62" t="n">
+        <v>3986</v>
+      </c>
+      <c r="AZ62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="BA62" t="inlineStr">
+        <is>
+          <t>4102</t>
         </is>
       </c>
     </row>
@@ -8875,9 +9163,15 @@
       <c r="AX63" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="AY63" t="inlineStr">
-        <is>
-          <t>4043</t>
+      <c r="AY63" t="n">
+        <v>4043</v>
+      </c>
+      <c r="AZ63" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="BA63" t="inlineStr">
+        <is>
+          <t>4111</t>
         </is>
       </c>
     </row>
@@ -9038,9 +9332,15 @@
       <c r="AX64" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AY64" t="inlineStr">
-        <is>
-          <t>4271</t>
+      <c r="AY64" t="n">
+        <v>4271</v>
+      </c>
+      <c r="AZ64" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA64" t="inlineStr">
+        <is>
+          <t>4362</t>
         </is>
       </c>
     </row>
@@ -9160,6 +9460,8 @@
       <c r="AW65" t="inlineStr"/>
       <c r="AX65" s="4" t="inlineStr"/>
       <c r="AY65" t="inlineStr"/>
+      <c r="AZ65" s="4" t="inlineStr"/>
+      <c r="BA65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -9318,7 +9620,13 @@
       <c r="AX66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY66" t="inlineStr">
+      <c r="AY66" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9481,7 +9789,13 @@
       <c r="AX67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY67" t="inlineStr">
+      <c r="AY67" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9644,7 +9958,13 @@
       <c r="AX68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY68" t="inlineStr">
+      <c r="AY68" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9714,6 +10034,8 @@
       <c r="AW69" t="inlineStr"/>
       <c r="AX69" s="4" t="inlineStr"/>
       <c r="AY69" t="inlineStr"/>
+      <c r="AZ69" s="4" t="inlineStr"/>
+      <c r="BA69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -9872,7 +10194,13 @@
       <c r="AX70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY70" t="inlineStr">
+      <c r="AY70" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10035,7 +10363,13 @@
       <c r="AX71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY71" t="inlineStr">
+      <c r="AY71" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10198,7 +10532,13 @@
       <c r="AX72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY72" t="inlineStr">
+      <c r="AY72" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10361,9 +10701,15 @@
       <c r="AX73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY73" t="inlineStr">
-        <is>
-          <t>2678</t>
+      <c r="AY73" t="n">
+        <v>2678</v>
+      </c>
+      <c r="AZ73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA73" t="inlineStr">
+        <is>
+          <t>2690</t>
         </is>
       </c>
     </row>
@@ -10524,7 +10870,13 @@
       <c r="AX74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY74" t="inlineStr">
+      <c r="AY74" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10687,7 +11039,13 @@
       <c r="AX75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY75" t="inlineStr">
+      <c r="AY75" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10850,9 +11208,15 @@
       <c r="AX76" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY76" t="inlineStr">
-        <is>
-          <t>2651</t>
+      <c r="AY76" t="n">
+        <v>2651</v>
+      </c>
+      <c r="AZ76" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="BA76" t="inlineStr">
+        <is>
+          <t>2839</t>
         </is>
       </c>
     </row>
@@ -11013,9 +11377,15 @@
       <c r="AX77" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AY77" t="inlineStr">
-        <is>
-          <t>2935</t>
+      <c r="AY77" t="n">
+        <v>2935</v>
+      </c>
+      <c r="AZ77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA77" t="inlineStr">
+        <is>
+          <t>2973</t>
         </is>
       </c>
     </row>
@@ -11176,7 +11546,13 @@
       <c r="AX78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY78" t="inlineStr">
+      <c r="AY78" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11339,7 +11715,13 @@
       <c r="AX79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY79" t="inlineStr">
+      <c r="AY79" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11502,7 +11884,13 @@
       <c r="AX80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY80" t="inlineStr">
+      <c r="AY80" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11665,7 +12053,13 @@
       <c r="AX81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY81" t="inlineStr">
+      <c r="AY81" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11828,7 +12222,13 @@
       <c r="AX82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY82" t="inlineStr">
+      <c r="AY82" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11991,7 +12391,13 @@
       <c r="AX83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY83" t="inlineStr">
+      <c r="AY83" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12154,7 +12560,13 @@
       <c r="AX84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY84" t="inlineStr">
+      <c r="AY84" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12317,7 +12729,13 @@
       <c r="AX85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY85" t="inlineStr">
+      <c r="AY85" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12480,7 +12898,13 @@
       <c r="AX86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY86" t="inlineStr">
+      <c r="AY86" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12643,7 +13067,13 @@
       <c r="AX87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY87" t="inlineStr">
+      <c r="AY87" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12806,7 +13236,13 @@
       <c r="AX88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY88" t="inlineStr">
+      <c r="AY88" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12969,7 +13405,13 @@
       <c r="AX89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY89" t="inlineStr">
+      <c r="AY89" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13132,7 +13574,13 @@
       <c r="AX90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY90" t="inlineStr">
+      <c r="AY90" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13295,7 +13743,13 @@
       <c r="AX91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY91" t="inlineStr">
+      <c r="AY91" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13458,7 +13912,13 @@
       <c r="AX92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY92" t="inlineStr">
+      <c r="AY92" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13621,7 +14081,13 @@
       <c r="AX93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY93" t="inlineStr">
+      <c r="AY93" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13784,7 +14250,13 @@
       <c r="AX94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY94" t="inlineStr">
+      <c r="AY94" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13947,7 +14419,13 @@
       <c r="AX95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY95" t="inlineStr">
+      <c r="AY95" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14109,6 +14587,8 @@
       </c>
       <c r="AX96" s="4" t="inlineStr"/>
       <c r="AY96" t="inlineStr"/>
+      <c r="AZ96" s="4" t="inlineStr"/>
+      <c r="BA96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -14267,7 +14747,13 @@
       <c r="AX97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY97" t="inlineStr">
+      <c r="AY97" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14430,7 +14916,13 @@
       <c r="AX98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY98" t="inlineStr">
+      <c r="AY98" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14593,7 +15085,13 @@
       <c r="AX99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY99" t="inlineStr">
+      <c r="AY99" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14756,7 +15254,13 @@
       <c r="AX100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY100" t="inlineStr">
+      <c r="AY100" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14919,7 +15423,13 @@
       <c r="AX101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY101" t="inlineStr">
+      <c r="AY101" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15082,7 +15592,13 @@
       <c r="AX102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY102" t="inlineStr">
+      <c r="AY102" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15245,7 +15761,13 @@
       <c r="AX103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY103" t="inlineStr">
+      <c r="AY103" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15408,7 +15930,13 @@
       <c r="AX104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY104" t="inlineStr">
+      <c r="AY104" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15571,7 +16099,13 @@
       <c r="AX105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY105" t="inlineStr">
+      <c r="AY105" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15641,6 +16175,8 @@
       <c r="AW106" t="inlineStr"/>
       <c r="AX106" s="4" t="inlineStr"/>
       <c r="AY106" t="inlineStr"/>
+      <c r="AZ106" s="4" t="inlineStr"/>
+      <c r="BA106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -15706,6 +16242,8 @@
       <c r="AW107" t="inlineStr"/>
       <c r="AX107" s="4" t="inlineStr"/>
       <c r="AY107" t="inlineStr"/>
+      <c r="AZ107" s="4" t="inlineStr"/>
+      <c r="BA107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -15771,6 +16309,8 @@
       <c r="AW108" t="inlineStr"/>
       <c r="AX108" s="4" t="inlineStr"/>
       <c r="AY108" t="inlineStr"/>
+      <c r="AZ108" s="4" t="inlineStr"/>
+      <c r="BA108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -15836,6 +16376,8 @@
       <c r="AW109" t="inlineStr"/>
       <c r="AX109" s="4" t="inlineStr"/>
       <c r="AY109" t="inlineStr"/>
+      <c r="AZ109" s="4" t="inlineStr"/>
+      <c r="BA109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -15901,6 +16443,8 @@
       <c r="AW110" t="inlineStr"/>
       <c r="AX110" s="4" t="inlineStr"/>
       <c r="AY110" t="inlineStr"/>
+      <c r="AZ110" s="4" t="inlineStr"/>
+      <c r="BA110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -15966,6 +16510,8 @@
       <c r="AW111" t="inlineStr"/>
       <c r="AX111" s="4" t="inlineStr"/>
       <c r="AY111" t="inlineStr"/>
+      <c r="AZ111" s="4" t="inlineStr"/>
+      <c r="BA111" t="inlineStr"/>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -16031,6 +16577,8 @@
       <c r="AW112" t="inlineStr"/>
       <c r="AX112" s="4" t="inlineStr"/>
       <c r="AY112" t="inlineStr"/>
+      <c r="AZ112" s="4" t="inlineStr"/>
+      <c r="BA112" t="inlineStr"/>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -16096,6 +16644,8 @@
       <c r="AW113" t="inlineStr"/>
       <c r="AX113" s="4" t="inlineStr"/>
       <c r="AY113" t="inlineStr"/>
+      <c r="AZ113" s="4" t="inlineStr"/>
+      <c r="BA113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -16161,6 +16711,8 @@
       <c r="AW114" t="inlineStr"/>
       <c r="AX114" s="4" t="inlineStr"/>
       <c r="AY114" t="inlineStr"/>
+      <c r="AZ114" s="4" t="inlineStr"/>
+      <c r="BA114" t="inlineStr"/>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -16297,9 +16849,15 @@
       <c r="AX115" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="AY115" t="inlineStr">
-        <is>
-          <t>5257</t>
+      <c r="AY115" t="n">
+        <v>5257</v>
+      </c>
+      <c r="AZ115" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="BA115" t="inlineStr">
+        <is>
+          <t>5552</t>
         </is>
       </c>
     </row>
@@ -16454,7 +17012,13 @@
       <c r="AX116" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY116" t="inlineStr">
+      <c r="AY116" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ116" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA116" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16578,6 +17142,8 @@
       </c>
       <c r="AX117" s="4" t="inlineStr"/>
       <c r="AY117" t="inlineStr"/>
+      <c r="AZ117" s="4" t="inlineStr"/>
+      <c r="BA117" t="inlineStr"/>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -16730,9 +17296,15 @@
       <c r="AX118" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY118" t="inlineStr">
-        <is>
-          <t>3231</t>
+      <c r="AY118" t="n">
+        <v>3231</v>
+      </c>
+      <c r="AZ118" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA118" t="inlineStr">
+        <is>
+          <t>3229</t>
         </is>
       </c>
     </row>
@@ -16887,9 +17459,15 @@
       <c r="AX119" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY119" t="inlineStr">
-        <is>
-          <t>1528</t>
+      <c r="AY119" t="n">
+        <v>1528</v>
+      </c>
+      <c r="AZ119" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA119" t="inlineStr">
+        <is>
+          <t>1556</t>
         </is>
       </c>
     </row>
@@ -17044,7 +17622,13 @@
       <c r="AX120" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY120" t="inlineStr">
+      <c r="AY120" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA120" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17201,7 +17785,13 @@
       <c r="AX121" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY121" t="inlineStr">
+      <c r="AY121" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ121" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA121" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17358,7 +17948,13 @@
       <c r="AX122" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY122" t="inlineStr">
+      <c r="AY122" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ122" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA122" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17511,7 +18107,13 @@
       <c r="AX123" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY123" t="inlineStr">
+      <c r="AY123" t="n">
+        <v>2579</v>
+      </c>
+      <c r="AZ123" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA123" t="inlineStr">
         <is>
           <t>2579</t>
         </is>
@@ -17607,6 +18209,8 @@
       <c r="AW124" t="inlineStr"/>
       <c r="AX124" s="4" t="inlineStr"/>
       <c r="AY124" t="inlineStr"/>
+      <c r="AZ124" s="4" t="inlineStr"/>
+      <c r="BA124" t="inlineStr"/>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -17751,9 +18355,15 @@
       <c r="AX125" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY125" t="inlineStr">
-        <is>
-          <t>2145</t>
+      <c r="AY125" t="n">
+        <v>2145</v>
+      </c>
+      <c r="AZ125" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA125" t="inlineStr">
+        <is>
+          <t>2162</t>
         </is>
       </c>
     </row>
@@ -17888,7 +18498,13 @@
       <c r="AX126" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY126" t="inlineStr">
+      <c r="AY126" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ126" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA126" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -17976,6 +18592,8 @@
       <c r="AW127" t="inlineStr"/>
       <c r="AX127" s="4" t="inlineStr"/>
       <c r="AY127" t="inlineStr"/>
+      <c r="AZ127" s="4" t="inlineStr"/>
+      <c r="BA127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -18071,6 +18689,8 @@
       <c r="AW128" t="inlineStr"/>
       <c r="AX128" s="4" t="inlineStr"/>
       <c r="AY128" t="inlineStr"/>
+      <c r="AZ128" s="4" t="inlineStr"/>
+      <c r="BA128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -18195,9 +18815,15 @@
       <c r="AX129" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY129" t="inlineStr">
-        <is>
-          <t>2552</t>
+      <c r="AY129" t="n">
+        <v>2552</v>
+      </c>
+      <c r="AZ129" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA129" t="inlineStr">
+        <is>
+          <t>2551</t>
         </is>
       </c>
     </row>
@@ -18295,6 +18921,8 @@
       <c r="AW130" t="inlineStr"/>
       <c r="AX130" s="4" t="inlineStr"/>
       <c r="AY130" t="inlineStr"/>
+      <c r="AZ130" s="4" t="inlineStr"/>
+      <c r="BA130" t="inlineStr"/>
     </row>
     <row r="131">
       <c r="A131" t="n">
@@ -18415,7 +19043,13 @@
       <c r="AX131" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY131" t="inlineStr">
+      <c r="AY131" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ131" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA131" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -18528,9 +19162,15 @@
       <c r="AX132" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="AY132" t="inlineStr">
-        <is>
-          <t>4153</t>
+      <c r="AY132" t="n">
+        <v>4153</v>
+      </c>
+      <c r="AZ132" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA132" t="inlineStr">
+        <is>
+          <t>4137</t>
         </is>
       </c>
     </row>
@@ -18641,9 +19281,15 @@
       <c r="AX133" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY133" t="inlineStr">
-        <is>
-          <t>2475</t>
+      <c r="AY133" t="n">
+        <v>2475</v>
+      </c>
+      <c r="AZ133" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA133" t="inlineStr">
+        <is>
+          <t>2469</t>
         </is>
       </c>
     </row>
@@ -18713,6 +19359,8 @@
       <c r="AW134" t="inlineStr"/>
       <c r="AX134" s="4" t="inlineStr"/>
       <c r="AY134" t="inlineStr"/>
+      <c r="AZ134" s="4" t="inlineStr"/>
+      <c r="BA134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -18784,6 +19432,8 @@
       <c r="AW135" t="inlineStr"/>
       <c r="AX135" s="4" t="inlineStr"/>
       <c r="AY135" t="inlineStr"/>
+      <c r="AZ135" s="4" t="inlineStr"/>
+      <c r="BA135" t="inlineStr"/>
     </row>
     <row r="136">
       <c r="A136" t="n">
@@ -18875,6 +19525,8 @@
       </c>
       <c r="AX136" s="4" t="inlineStr"/>
       <c r="AY136" t="inlineStr"/>
+      <c r="AZ136" s="4" t="inlineStr"/>
+      <c r="BA136" t="inlineStr"/>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -18966,6 +19618,8 @@
       </c>
       <c r="AX137" s="4" t="inlineStr"/>
       <c r="AY137" t="inlineStr"/>
+      <c r="AZ137" s="4" t="inlineStr"/>
+      <c r="BA137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -19037,6 +19691,8 @@
       <c r="AW138" t="inlineStr"/>
       <c r="AX138" s="4" t="inlineStr"/>
       <c r="AY138" t="inlineStr"/>
+      <c r="AZ138" s="4" t="inlineStr"/>
+      <c r="BA138" t="inlineStr"/>
     </row>
     <row r="139">
       <c r="A139" t="n">
@@ -19128,6 +19784,8 @@
       </c>
       <c r="AX139" s="4" t="inlineStr"/>
       <c r="AY139" t="inlineStr"/>
+      <c r="AZ139" s="4" t="inlineStr"/>
+      <c r="BA139" t="inlineStr"/>
     </row>
     <row r="140">
       <c r="A140" t="n">
@@ -19220,9 +19878,15 @@
       <c r="AX140" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY140" t="inlineStr">
-        <is>
-          <t>2037</t>
+      <c r="AY140" t="n">
+        <v>2037</v>
+      </c>
+      <c r="AZ140" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA140" t="inlineStr">
+        <is>
+          <t>2036</t>
         </is>
       </c>
     </row>
@@ -19292,6 +19956,8 @@
       <c r="AW141" t="inlineStr"/>
       <c r="AX141" s="4" t="inlineStr"/>
       <c r="AY141" t="inlineStr"/>
+      <c r="AZ141" s="4" t="inlineStr"/>
+      <c r="BA141" t="inlineStr"/>
     </row>
     <row r="142">
       <c r="A142" t="n">
@@ -19380,9 +20046,15 @@
       <c r="AX142" s="3" t="n">
         <v>7</v>
       </c>
-      <c r="AY142" t="inlineStr">
-        <is>
-          <t>2923</t>
+      <c r="AY142" t="n">
+        <v>2923</v>
+      </c>
+      <c r="AZ142" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA142" t="inlineStr">
+        <is>
+          <t>2915</t>
         </is>
       </c>
     </row>
@@ -19473,7 +20145,13 @@
       <c r="AX143" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY143" t="inlineStr">
+      <c r="AY143" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ143" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA143" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19562,9 +20240,15 @@
       <c r="AX144" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY144" t="inlineStr">
-        <is>
-          <t>1621</t>
+      <c r="AY144" t="n">
+        <v>1621</v>
+      </c>
+      <c r="AZ144" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="BA144" t="inlineStr">
+        <is>
+          <t>1657</t>
         </is>
       </c>
     </row>
@@ -19651,9 +20335,15 @@
       <c r="AX145" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY145" t="inlineStr">
-        <is>
-          <t>1833</t>
+      <c r="AY145" t="n">
+        <v>1833</v>
+      </c>
+      <c r="AZ145" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA145" t="inlineStr">
+        <is>
+          <t>1830</t>
         </is>
       </c>
     </row>
@@ -19740,7 +20430,13 @@
       <c r="AX146" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY146" t="inlineStr">
+      <c r="AY146" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ146" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA146" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -19829,9 +20525,15 @@
       <c r="AX147" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AY147" t="inlineStr">
-        <is>
-          <t>4615</t>
+      <c r="AY147" t="n">
+        <v>4615</v>
+      </c>
+      <c r="AZ147" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="BA147" t="inlineStr">
+        <is>
+          <t>4718</t>
         </is>
       </c>
     </row>
@@ -19918,9 +20620,15 @@
       <c r="AX148" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY148" t="inlineStr">
-        <is>
-          <t>2030</t>
+      <c r="AY148" t="n">
+        <v>2030</v>
+      </c>
+      <c r="AZ148" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA148" t="inlineStr">
+        <is>
+          <t>2043</t>
         </is>
       </c>
     </row>
@@ -19994,6 +20702,8 @@
       <c r="AW149" t="inlineStr"/>
       <c r="AX149" s="4" t="inlineStr"/>
       <c r="AY149" t="inlineStr"/>
+      <c r="AZ149" s="4" t="inlineStr"/>
+      <c r="BA149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -20074,9 +20784,15 @@
       <c r="AX150" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="AY150" t="inlineStr">
-        <is>
-          <t>3603</t>
+      <c r="AY150" t="n">
+        <v>3603</v>
+      </c>
+      <c r="AZ150" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="BA150" t="inlineStr">
+        <is>
+          <t>3772</t>
         </is>
       </c>
     </row>
@@ -20159,9 +20875,15 @@
       <c r="AX151" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY151" t="inlineStr">
-        <is>
-          <t>2290</t>
+      <c r="AY151" t="n">
+        <v>2290</v>
+      </c>
+      <c r="AZ151" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA151" t="inlineStr">
+        <is>
+          <t>2296</t>
         </is>
       </c>
     </row>
@@ -20240,9 +20962,15 @@
       <c r="AX152" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="AY152" t="inlineStr">
-        <is>
-          <t>3933</t>
+      <c r="AY152" t="n">
+        <v>3933</v>
+      </c>
+      <c r="AZ152" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="BA152" t="inlineStr">
+        <is>
+          <t>3991</t>
         </is>
       </c>
     </row>
@@ -20317,17 +21045,21 @@
       <c r="AX153" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="AY153" t="inlineStr">
-        <is>
-          <t>1810</t>
+      <c r="AY153" t="n">
+        <v>1810</v>
+      </c>
+      <c r="AZ153" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="BA153" t="inlineStr">
+        <is>
+          <t>2004</t>
         </is>
       </c>
     </row>
     <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>59552264</t>
-        </is>
+      <c r="A154" t="n">
+        <v>59552264</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
@@ -20388,9 +21120,15 @@
       <c r="AX154" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="AY154" t="inlineStr">
-        <is>
-          <t>1876</t>
+      <c r="AY154" t="n">
+        <v>1876</v>
+      </c>
+      <c r="AZ154" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="BA154" t="inlineStr">
+        <is>
+          <t>2264</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Code updated 23-06-15 10:44:25
</commit_message>
<xml_diff>
--- a/Season_Attack/89.xlsx
+++ b/Season_Attack/89.xlsx
@@ -382,7 +382,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA154"/>
+  <dimension ref="A1:BC155"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -656,6 +656,16 @@
           <t>06-13_0</t>
         </is>
       </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>06-14_A</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>06-14_0</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -820,9 +830,15 @@
       <c r="AZ2" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="BA2" t="inlineStr">
-        <is>
-          <t>4598</t>
+      <c r="BA2" t="n">
+        <v>4598</v>
+      </c>
+      <c r="BB2" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="BC2" t="inlineStr">
+        <is>
+          <t>4625</t>
         </is>
       </c>
     </row>
@@ -989,7 +1005,13 @@
       <c r="AZ3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA3" t="inlineStr">
+      <c r="BA3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC3" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1158,7 +1180,13 @@
       <c r="AZ4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA4" t="inlineStr">
+      <c r="BA4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC4" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1327,9 +1355,15 @@
       <c r="AZ5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA5" t="inlineStr">
-        <is>
-          <t>2770</t>
+      <c r="BA5" t="n">
+        <v>2770</v>
+      </c>
+      <c r="BB5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC5" t="inlineStr">
+        <is>
+          <t>2815</t>
         </is>
       </c>
     </row>
@@ -1496,7 +1530,13 @@
       <c r="AZ6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA6" t="inlineStr">
+      <c r="BA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC6" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -1568,6 +1608,8 @@
       <c r="AY7" t="inlineStr"/>
       <c r="AZ7" s="4" t="inlineStr"/>
       <c r="BA7" t="inlineStr"/>
+      <c r="BB7" s="4" t="inlineStr"/>
+      <c r="BC7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1635,6 +1677,8 @@
       <c r="AY8" t="inlineStr"/>
       <c r="AZ8" s="4" t="inlineStr"/>
       <c r="BA8" t="inlineStr"/>
+      <c r="BB8" s="4" t="inlineStr"/>
+      <c r="BC8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1702,6 +1746,8 @@
       <c r="AY9" t="inlineStr"/>
       <c r="AZ9" s="4" t="inlineStr"/>
       <c r="BA9" t="inlineStr"/>
+      <c r="BB9" s="4" t="inlineStr"/>
+      <c r="BC9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1769,6 +1815,8 @@
       <c r="AY10" t="inlineStr"/>
       <c r="AZ10" s="4" t="inlineStr"/>
       <c r="BA10" t="inlineStr"/>
+      <c r="BB10" s="4" t="inlineStr"/>
+      <c r="BC10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1836,6 +1884,8 @@
       <c r="AY11" t="inlineStr"/>
       <c r="AZ11" s="4" t="inlineStr"/>
       <c r="BA11" t="inlineStr"/>
+      <c r="BB11" s="4" t="inlineStr"/>
+      <c r="BC11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1903,6 +1953,8 @@
       <c r="AY12" t="inlineStr"/>
       <c r="AZ12" s="4" t="inlineStr"/>
       <c r="BA12" t="inlineStr"/>
+      <c r="BB12" s="4" t="inlineStr"/>
+      <c r="BC12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1970,6 +2022,8 @@
       <c r="AY13" t="inlineStr"/>
       <c r="AZ13" s="4" t="inlineStr"/>
       <c r="BA13" t="inlineStr"/>
+      <c r="BB13" s="4" t="inlineStr"/>
+      <c r="BC13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -2037,6 +2091,8 @@
       <c r="AY14" t="inlineStr"/>
       <c r="AZ14" s="4" t="inlineStr"/>
       <c r="BA14" t="inlineStr"/>
+      <c r="BB14" s="4" t="inlineStr"/>
+      <c r="BC14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -2104,6 +2160,8 @@
       <c r="AY15" t="inlineStr"/>
       <c r="AZ15" s="4" t="inlineStr"/>
       <c r="BA15" t="inlineStr"/>
+      <c r="BB15" s="4" t="inlineStr"/>
+      <c r="BC15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -2171,6 +2229,8 @@
       <c r="AY16" t="inlineStr"/>
       <c r="AZ16" s="4" t="inlineStr"/>
       <c r="BA16" t="inlineStr"/>
+      <c r="BB16" s="4" t="inlineStr"/>
+      <c r="BC16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -2238,6 +2298,8 @@
       <c r="AY17" t="inlineStr"/>
       <c r="AZ17" s="4" t="inlineStr"/>
       <c r="BA17" t="inlineStr"/>
+      <c r="BB17" s="4" t="inlineStr"/>
+      <c r="BC17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -2402,9 +2464,15 @@
       <c r="AZ18" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="BA18" t="inlineStr">
-        <is>
-          <t>4098</t>
+      <c r="BA18" t="n">
+        <v>4098</v>
+      </c>
+      <c r="BB18" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="BC18" t="inlineStr">
+        <is>
+          <t>4118</t>
         </is>
       </c>
     </row>
@@ -2571,7 +2639,13 @@
       <c r="AZ19" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA19" t="inlineStr">
+      <c r="BA19" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB19" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC19" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -2740,9 +2814,15 @@
       <c r="AZ20" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="BA20" t="inlineStr">
-        <is>
-          <t>4354</t>
+      <c r="BA20" t="n">
+        <v>4354</v>
+      </c>
+      <c r="BB20" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="BC20" t="inlineStr">
+        <is>
+          <t>4407</t>
         </is>
       </c>
     </row>
@@ -2909,9 +2989,15 @@
       <c r="AZ21" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA21" t="inlineStr">
-        <is>
-          <t>3234</t>
+      <c r="BA21" t="n">
+        <v>3234</v>
+      </c>
+      <c r="BB21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC21" t="inlineStr">
+        <is>
+          <t>3230</t>
         </is>
       </c>
     </row>
@@ -3078,9 +3164,15 @@
       <c r="AZ22" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="BA22" t="inlineStr">
-        <is>
-          <t>4988</t>
+      <c r="BA22" t="n">
+        <v>4988</v>
+      </c>
+      <c r="BB22" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC22" t="inlineStr">
+        <is>
+          <t>5064</t>
         </is>
       </c>
     </row>
@@ -3247,9 +3339,15 @@
       <c r="AZ23" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="BA23" t="inlineStr">
-        <is>
-          <t>5611</t>
+      <c r="BA23" t="n">
+        <v>5611</v>
+      </c>
+      <c r="BB23" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="BC23" t="inlineStr">
+        <is>
+          <t>5800</t>
         </is>
       </c>
     </row>
@@ -3416,9 +3514,15 @@
       <c r="AZ24" s="5" t="n">
         <v>33</v>
       </c>
-      <c r="BA24" t="inlineStr">
-        <is>
-          <t>5052</t>
+      <c r="BA24" t="n">
+        <v>5052</v>
+      </c>
+      <c r="BB24" s="5" t="n">
+        <v>33</v>
+      </c>
+      <c r="BC24" t="inlineStr">
+        <is>
+          <t>5141</t>
         </is>
       </c>
     </row>
@@ -3552,6 +3656,8 @@
       <c r="AY25" t="inlineStr"/>
       <c r="AZ25" s="4" t="inlineStr"/>
       <c r="BA25" t="inlineStr"/>
+      <c r="BB25" s="4" t="inlineStr"/>
+      <c r="BC25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -3671,6 +3777,8 @@
       <c r="AY26" t="inlineStr"/>
       <c r="AZ26" s="4" t="inlineStr"/>
       <c r="BA26" t="inlineStr"/>
+      <c r="BB26" s="4" t="inlineStr"/>
+      <c r="BC26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -3835,7 +3943,13 @@
       <c r="AZ27" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA27" t="inlineStr">
+      <c r="BA27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB27" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC27" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -3907,6 +4021,8 @@
       <c r="AY28" t="inlineStr"/>
       <c r="AZ28" s="4" t="inlineStr"/>
       <c r="BA28" t="inlineStr"/>
+      <c r="BB28" s="4" t="inlineStr"/>
+      <c r="BC28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -4071,7 +4187,13 @@
       <c r="AZ29" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA29" t="inlineStr">
+      <c r="BA29" t="n">
+        <v>2500</v>
+      </c>
+      <c r="BB29" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC29" t="inlineStr">
         <is>
           <t>2500</t>
         </is>
@@ -4240,9 +4362,15 @@
       <c r="AZ30" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="BA30" t="inlineStr">
-        <is>
-          <t>4808</t>
+      <c r="BA30" t="n">
+        <v>4808</v>
+      </c>
+      <c r="BB30" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC30" t="inlineStr">
+        <is>
+          <t>4988</t>
         </is>
       </c>
     </row>
@@ -4409,9 +4537,15 @@
       <c r="AZ31" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="BA31" t="inlineStr">
-        <is>
-          <t>4950</t>
+      <c r="BA31" t="n">
+        <v>4950</v>
+      </c>
+      <c r="BB31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="BC31" t="inlineStr">
+        <is>
+          <t>5060</t>
         </is>
       </c>
     </row>
@@ -4578,9 +4712,15 @@
       <c r="AZ32" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="BA32" t="inlineStr">
-        <is>
-          <t>2985</t>
+      <c r="BA32" t="n">
+        <v>2985</v>
+      </c>
+      <c r="BB32" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC32" t="inlineStr">
+        <is>
+          <t>3392</t>
         </is>
       </c>
     </row>
@@ -4650,6 +4790,8 @@
       <c r="AY33" t="inlineStr"/>
       <c r="AZ33" s="4" t="inlineStr"/>
       <c r="BA33" t="inlineStr"/>
+      <c r="BB33" s="4" t="inlineStr"/>
+      <c r="BC33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -4814,7 +4956,13 @@
       <c r="AZ34" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA34" t="inlineStr">
+      <c r="BA34" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB34" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC34" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -4983,7 +5131,13 @@
       <c r="AZ35" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA35" t="inlineStr">
+      <c r="BA35" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB35" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC35" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5152,9 +5306,15 @@
       <c r="AZ36" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="BA36" t="inlineStr">
-        <is>
-          <t>3372</t>
+      <c r="BA36" t="n">
+        <v>3372</v>
+      </c>
+      <c r="BB36" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC36" t="inlineStr">
+        <is>
+          <t>3824</t>
         </is>
       </c>
     </row>
@@ -5296,6 +5456,8 @@
       <c r="AY37" t="inlineStr"/>
       <c r="AZ37" s="4" t="inlineStr"/>
       <c r="BA37" t="inlineStr"/>
+      <c r="BB37" s="4" t="inlineStr"/>
+      <c r="BC37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -5460,9 +5622,15 @@
       <c r="AZ38" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA38" t="inlineStr">
-        <is>
-          <t>4696</t>
+      <c r="BA38" t="n">
+        <v>4696</v>
+      </c>
+      <c r="BB38" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="BC38" t="inlineStr">
+        <is>
+          <t>4754</t>
         </is>
       </c>
     </row>
@@ -5629,9 +5797,15 @@
       <c r="AZ39" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="BA39" t="inlineStr">
-        <is>
-          <t>4560</t>
+      <c r="BA39" t="n">
+        <v>4560</v>
+      </c>
+      <c r="BB39" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="BC39" t="inlineStr">
+        <is>
+          <t>4754</t>
         </is>
       </c>
     </row>
@@ -5798,7 +5972,13 @@
       <c r="AZ40" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA40" t="inlineStr">
+      <c r="BA40" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB40" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC40" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -5967,9 +6147,15 @@
       <c r="AZ41" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="BA41" t="inlineStr">
-        <is>
-          <t>4242</t>
+      <c r="BA41" t="n">
+        <v>4242</v>
+      </c>
+      <c r="BB41" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC41" t="inlineStr">
+        <is>
+          <t>4384</t>
         </is>
       </c>
     </row>
@@ -6136,9 +6322,15 @@
       <c r="AZ42" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA42" t="inlineStr">
-        <is>
-          <t>2872</t>
+      <c r="BA42" t="n">
+        <v>2872</v>
+      </c>
+      <c r="BB42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC42" t="inlineStr">
+        <is>
+          <t>2888</t>
         </is>
       </c>
     </row>
@@ -6208,6 +6400,8 @@
       <c r="AY43" t="inlineStr"/>
       <c r="AZ43" s="4" t="inlineStr"/>
       <c r="BA43" t="inlineStr"/>
+      <c r="BB43" s="4" t="inlineStr"/>
+      <c r="BC43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -6275,6 +6469,8 @@
       <c r="AY44" t="inlineStr"/>
       <c r="AZ44" s="4" t="inlineStr"/>
       <c r="BA44" t="inlineStr"/>
+      <c r="BB44" s="4" t="inlineStr"/>
+      <c r="BC44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -6374,6 +6570,8 @@
       <c r="AY45" t="inlineStr"/>
       <c r="AZ45" s="4" t="inlineStr"/>
       <c r="BA45" t="inlineStr"/>
+      <c r="BB45" s="4" t="inlineStr"/>
+      <c r="BC45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -6538,9 +6736,15 @@
       <c r="AZ46" s="3" t="n">
         <v>16</v>
       </c>
-      <c r="BA46" t="inlineStr">
-        <is>
-          <t>4465</t>
+      <c r="BA46" t="n">
+        <v>4465</v>
+      </c>
+      <c r="BB46" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC46" t="inlineStr">
+        <is>
+          <t>4556</t>
         </is>
       </c>
     </row>
@@ -6707,9 +6911,15 @@
       <c r="AZ47" s="5" t="n">
         <v>31</v>
       </c>
-      <c r="BA47" t="inlineStr">
-        <is>
-          <t>5433</t>
+      <c r="BA47" t="n">
+        <v>5433</v>
+      </c>
+      <c r="BB47" s="5" t="n">
+        <v>32</v>
+      </c>
+      <c r="BC47" t="inlineStr">
+        <is>
+          <t>5638</t>
         </is>
       </c>
     </row>
@@ -6876,7 +7086,13 @@
       <c r="AZ48" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA48" t="inlineStr">
+      <c r="BA48" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC48" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -7045,9 +7261,15 @@
       <c r="AZ49" s="4" t="n">
         <v>28</v>
       </c>
-      <c r="BA49" t="inlineStr">
-        <is>
-          <t>4790</t>
+      <c r="BA49" t="n">
+        <v>4790</v>
+      </c>
+      <c r="BB49" s="4" t="n">
+        <v>27</v>
+      </c>
+      <c r="BC49" t="inlineStr">
+        <is>
+          <t>4945</t>
         </is>
       </c>
     </row>
@@ -7214,9 +7436,15 @@
       <c r="AZ50" s="4" t="n">
         <v>23</v>
       </c>
-      <c r="BA50" t="inlineStr">
-        <is>
-          <t>5020</t>
+      <c r="BA50" t="n">
+        <v>5020</v>
+      </c>
+      <c r="BB50" s="4" t="n">
+        <v>23</v>
+      </c>
+      <c r="BC50" t="inlineStr">
+        <is>
+          <t>5154</t>
         </is>
       </c>
     </row>
@@ -7318,6 +7546,8 @@
       <c r="AY51" t="inlineStr"/>
       <c r="AZ51" s="4" t="inlineStr"/>
       <c r="BA51" t="inlineStr"/>
+      <c r="BB51" s="4" t="inlineStr"/>
+      <c r="BC51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -7482,9 +7712,15 @@
       <c r="AZ52" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="BA52" t="inlineStr">
-        <is>
-          <t>5056</t>
+      <c r="BA52" t="n">
+        <v>5056</v>
+      </c>
+      <c r="BB52" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="BC52" t="inlineStr">
+        <is>
+          <t>5316</t>
         </is>
       </c>
     </row>
@@ -7651,9 +7887,15 @@
       <c r="AZ53" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="BA53" t="inlineStr">
-        <is>
-          <t>3724</t>
+      <c r="BA53" t="n">
+        <v>3724</v>
+      </c>
+      <c r="BB53" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="BC53" t="inlineStr">
+        <is>
+          <t>3943</t>
         </is>
       </c>
     </row>
@@ -7755,6 +7997,8 @@
       <c r="AY54" t="inlineStr"/>
       <c r="AZ54" s="4" t="inlineStr"/>
       <c r="BA54" t="inlineStr"/>
+      <c r="BB54" s="4" t="inlineStr"/>
+      <c r="BC54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -7919,9 +8163,15 @@
       <c r="AZ55" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA55" t="inlineStr">
-        <is>
-          <t>3537</t>
+      <c r="BA55" t="n">
+        <v>3537</v>
+      </c>
+      <c r="BB55" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="BC55" t="inlineStr">
+        <is>
+          <t>3842</t>
         </is>
       </c>
     </row>
@@ -8088,9 +8338,15 @@
       <c r="AZ56" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="BA56" t="inlineStr">
-        <is>
-          <t>5377</t>
+      <c r="BA56" t="n">
+        <v>5377</v>
+      </c>
+      <c r="BB56" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="BC56" t="inlineStr">
+        <is>
+          <t>5356</t>
         </is>
       </c>
     </row>
@@ -8257,9 +8513,15 @@
       <c r="AZ57" s="4" t="n">
         <v>20</v>
       </c>
-      <c r="BA57" t="inlineStr">
-        <is>
-          <t>4275</t>
+      <c r="BA57" t="n">
+        <v>4275</v>
+      </c>
+      <c r="BB57" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="BC57" t="inlineStr">
+        <is>
+          <t>4257</t>
         </is>
       </c>
     </row>
@@ -8426,9 +8688,15 @@
       <c r="AZ58" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="BA58" t="inlineStr">
-        <is>
-          <t>4233</t>
+      <c r="BA58" t="n">
+        <v>4233</v>
+      </c>
+      <c r="BB58" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="BC58" t="inlineStr">
+        <is>
+          <t>4409</t>
         </is>
       </c>
     </row>
@@ -8595,9 +8863,15 @@
       <c r="AZ59" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="BA59" t="inlineStr">
-        <is>
-          <t>4157</t>
+      <c r="BA59" t="n">
+        <v>4157</v>
+      </c>
+      <c r="BB59" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC59" t="inlineStr">
+        <is>
+          <t>4204</t>
         </is>
       </c>
     </row>
@@ -8764,9 +9038,15 @@
       <c r="AZ60" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="BA60" t="inlineStr">
-        <is>
-          <t>4333</t>
+      <c r="BA60" t="n">
+        <v>4333</v>
+      </c>
+      <c r="BB60" s="4" t="n">
+        <v>25</v>
+      </c>
+      <c r="BC60" t="inlineStr">
+        <is>
+          <t>4512</t>
         </is>
       </c>
     </row>
@@ -8836,6 +9116,8 @@
       <c r="AY61" t="inlineStr"/>
       <c r="AZ61" s="4" t="inlineStr"/>
       <c r="BA61" t="inlineStr"/>
+      <c r="BB61" s="4" t="inlineStr"/>
+      <c r="BC61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -9000,9 +9282,15 @@
       <c r="AZ62" s="4" t="n">
         <v>30</v>
       </c>
-      <c r="BA62" t="inlineStr">
-        <is>
-          <t>4102</t>
+      <c r="BA62" t="n">
+        <v>4102</v>
+      </c>
+      <c r="BB62" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="BC62" t="inlineStr">
+        <is>
+          <t>4098</t>
         </is>
       </c>
     </row>
@@ -9169,9 +9457,15 @@
       <c r="AZ63" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="BA63" t="inlineStr">
-        <is>
-          <t>4111</t>
+      <c r="BA63" t="n">
+        <v>4111</v>
+      </c>
+      <c r="BB63" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC63" t="inlineStr">
+        <is>
+          <t>4131</t>
         </is>
       </c>
     </row>
@@ -9338,9 +9632,15 @@
       <c r="AZ64" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA64" t="inlineStr">
-        <is>
-          <t>4362</t>
+      <c r="BA64" t="n">
+        <v>4362</v>
+      </c>
+      <c r="BB64" s="4" t="n">
+        <v>20</v>
+      </c>
+      <c r="BC64" t="inlineStr">
+        <is>
+          <t>4419</t>
         </is>
       </c>
     </row>
@@ -9462,6 +9762,8 @@
       <c r="AY65" t="inlineStr"/>
       <c r="AZ65" s="4" t="inlineStr"/>
       <c r="BA65" t="inlineStr"/>
+      <c r="BB65" s="4" t="inlineStr"/>
+      <c r="BC65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -9626,7 +9928,13 @@
       <c r="AZ66" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA66" t="inlineStr">
+      <c r="BA66" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC66" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9795,7 +10103,13 @@
       <c r="AZ67" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA67" t="inlineStr">
+      <c r="BA67" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB67" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC67" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -9964,7 +10278,13 @@
       <c r="AZ68" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA68" t="inlineStr">
+      <c r="BA68" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB68" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC68" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10036,6 +10356,8 @@
       <c r="AY69" t="inlineStr"/>
       <c r="AZ69" s="4" t="inlineStr"/>
       <c r="BA69" t="inlineStr"/>
+      <c r="BB69" s="4" t="inlineStr"/>
+      <c r="BC69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -10200,7 +10522,13 @@
       <c r="AZ70" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA70" t="inlineStr">
+      <c r="BA70" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB70" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC70" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10369,7 +10697,13 @@
       <c r="AZ71" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA71" t="inlineStr">
+      <c r="BA71" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB71" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC71" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10538,7 +10872,13 @@
       <c r="AZ72" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA72" t="inlineStr">
+      <c r="BA72" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC72" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -10707,9 +11047,15 @@
       <c r="AZ73" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA73" t="inlineStr">
-        <is>
-          <t>2690</t>
+      <c r="BA73" t="n">
+        <v>2690</v>
+      </c>
+      <c r="BB73" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC73" t="inlineStr">
+        <is>
+          <t>2707</t>
         </is>
       </c>
     </row>
@@ -10876,7 +11222,13 @@
       <c r="AZ74" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA74" t="inlineStr">
+      <c r="BA74" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB74" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC74" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11045,7 +11397,13 @@
       <c r="AZ75" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA75" t="inlineStr">
+      <c r="BA75" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB75" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC75" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11214,9 +11572,15 @@
       <c r="AZ76" s="3" t="n">
         <v>5</v>
       </c>
-      <c r="BA76" t="inlineStr">
-        <is>
-          <t>2839</t>
+      <c r="BA76" t="n">
+        <v>2839</v>
+      </c>
+      <c r="BB76" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC76" t="inlineStr">
+        <is>
+          <t>2836</t>
         </is>
       </c>
     </row>
@@ -11383,9 +11747,15 @@
       <c r="AZ77" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA77" t="inlineStr">
-        <is>
-          <t>2973</t>
+      <c r="BA77" t="n">
+        <v>2973</v>
+      </c>
+      <c r="BB77" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC77" t="inlineStr">
+        <is>
+          <t>2987</t>
         </is>
       </c>
     </row>
@@ -11552,7 +11922,13 @@
       <c r="AZ78" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA78" t="inlineStr">
+      <c r="BA78" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC78" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11721,7 +12097,13 @@
       <c r="AZ79" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA79" t="inlineStr">
+      <c r="BA79" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB79" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC79" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -11890,7 +12272,13 @@
       <c r="AZ80" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA80" t="inlineStr">
+      <c r="BA80" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB80" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC80" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12059,7 +12447,13 @@
       <c r="AZ81" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA81" t="inlineStr">
+      <c r="BA81" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB81" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC81" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12228,7 +12622,13 @@
       <c r="AZ82" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA82" t="inlineStr">
+      <c r="BA82" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB82" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC82" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12397,7 +12797,13 @@
       <c r="AZ83" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA83" t="inlineStr">
+      <c r="BA83" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB83" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC83" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12566,7 +12972,13 @@
       <c r="AZ84" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA84" t="inlineStr">
+      <c r="BA84" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC84" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12735,7 +13147,13 @@
       <c r="AZ85" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA85" t="inlineStr">
+      <c r="BA85" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB85" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC85" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -12904,7 +13322,13 @@
       <c r="AZ86" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA86" t="inlineStr">
+      <c r="BA86" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB86" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC86" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13073,7 +13497,13 @@
       <c r="AZ87" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA87" t="inlineStr">
+      <c r="BA87" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB87" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC87" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13242,7 +13672,13 @@
       <c r="AZ88" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA88" t="inlineStr">
+      <c r="BA88" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB88" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC88" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13411,7 +13847,13 @@
       <c r="AZ89" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA89" t="inlineStr">
+      <c r="BA89" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB89" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC89" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13580,7 +14022,13 @@
       <c r="AZ90" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA90" t="inlineStr">
+      <c r="BA90" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC90" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13749,7 +14197,13 @@
       <c r="AZ91" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA91" t="inlineStr">
+      <c r="BA91" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB91" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC91" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -13918,7 +14372,13 @@
       <c r="AZ92" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA92" t="inlineStr">
+      <c r="BA92" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB92" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC92" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14087,7 +14547,13 @@
       <c r="AZ93" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA93" t="inlineStr">
+      <c r="BA93" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB93" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC93" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14256,7 +14722,13 @@
       <c r="AZ94" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA94" t="inlineStr">
+      <c r="BA94" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB94" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC94" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14425,7 +14897,13 @@
       <c r="AZ95" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA95" t="inlineStr">
+      <c r="BA95" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB95" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC95" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14589,6 +15067,8 @@
       <c r="AY96" t="inlineStr"/>
       <c r="AZ96" s="4" t="inlineStr"/>
       <c r="BA96" t="inlineStr"/>
+      <c r="BB96" s="4" t="inlineStr"/>
+      <c r="BC96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -14753,7 +15233,13 @@
       <c r="AZ97" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA97" t="inlineStr">
+      <c r="BA97" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB97" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC97" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -14922,7 +15408,13 @@
       <c r="AZ98" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA98" t="inlineStr">
+      <c r="BA98" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB98" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC98" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15091,7 +15583,13 @@
       <c r="AZ99" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA99" t="inlineStr">
+      <c r="BA99" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB99" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC99" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15260,7 +15758,13 @@
       <c r="AZ100" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA100" t="inlineStr">
+      <c r="BA100" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB100" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC100" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15429,7 +15933,13 @@
       <c r="AZ101" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA101" t="inlineStr">
+      <c r="BA101" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB101" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC101" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15598,7 +16108,13 @@
       <c r="AZ102" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA102" t="inlineStr">
+      <c r="BA102" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC102" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15767,7 +16283,13 @@
       <c r="AZ103" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA103" t="inlineStr">
+      <c r="BA103" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB103" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC103" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -15936,7 +16458,13 @@
       <c r="AZ104" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA104" t="inlineStr">
+      <c r="BA104" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB104" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC104" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16105,7 +16633,13 @@
       <c r="AZ105" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="BA105" t="inlineStr">
+      <c r="BA105" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB105" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC105" t="inlineStr">
         <is>
           <t>0</t>
         </is>
@@ -16177,6 +16711,8 @@
       <c r="AY106" t="inlineStr"/>
       <c r="AZ106" s="4" t="inlineStr"/>
       <c r="BA106" t="inlineStr"/>
+      <c r="BB106" s="4" t="inlineStr"/>
+      <c r="BC106" t="inlineStr"/>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -16244,6 +16780,8 @@
       <c r="AY107" t="inlineStr"/>
       <c r="AZ107" s="4" t="inlineStr"/>
       <c r="BA107" t="inlineStr"/>
+      <c r="BB107" s="4" t="inlineStr"/>
+      <c r="BC107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -16311,6 +16849,8 @@
       <c r="AY108" t="inlineStr"/>
       <c r="AZ108" s="4" t="inlineStr"/>
       <c r="BA108" t="inlineStr"/>
+      <c r="BB108" s="4" t="inlineStr"/>
+      <c r="BC108" t="inlineStr"/>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -16378,6 +16918,8 @@
       <c r="AY109" t="inlineStr"/>
       <c r="AZ109" s="4" t="inlineStr"/>
       <c r="BA109" t="inlineStr"/>
+      <c r="BB109" s="4" t="inlineStr"/>
+      <c r="BC109" t="inlineStr"/>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -16445,6 +16987,8 @@
       <c r="AY110